<commit_message>
Fix an error from previous commit
Former-commit-id: 01c49c1c01fc85b4130d3e45bad13788c94ee5be
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -1564,7 +1564,7 @@
     <t>SCORE MULTIPLIER DEFINITIONS</t>
   </si>
   <si>
-    <t>SP_Medieval_Final_Common;CO_Medieval_Final_Castle;CO_Medieval_Final_Dark_Caves;CO_Medieval_Final_Dark_Witch_Tree;CO_Medieval_Final_Village;ART_Medieval_Lighting;Art_Level_fog;ART_Levels_Background_Skies;SO_Medieval_Common</t>
+    <t>SP_Medieval_Final_Common;CO_Medieval_Final_Castle;CO_Medieval_Final_Dark_Caves;CO_Medieval_Final_Dark_Witch_Tree;CO_Medieval_Final_Village;ART_Medieval_Lighting;Art_Level_fog;SO_Medieval_Common;ART_Levels_Background_Skies</t>
   </si>
 </sst>
 </file>
@@ -6040,7 +6040,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -16346,7 +16346,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="255.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Removed table "LevelDefinitions". From now on, programmers will control that table
Former-commit-id: 1b8bda6e3c63841aab13422f12eeeba95f2b39a1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="2" r:id="rId1"/>
-    <sheet name="levels" sheetId="3" r:id="rId2"/>
-    <sheet name="score" sheetId="4" r:id="rId3"/>
+    <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$116:$O$117</definedName>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="461">
   <si>
     <t>tier_4</t>
   </si>
@@ -1242,160 +1241,6 @@
     <t>ENTITY CATEGORY DEFINITIONS</t>
   </si>
   <si>
-    <t>Profiler</t>
-  </si>
-  <si>
-    <t>area1</t>
-  </si>
-  <si>
-    <t>ART_Profiler</t>
-  </si>
-  <si>
-    <t>SP_Profiler;CO_Profiler;ART_Profiler</t>
-  </si>
-  <si>
-    <t>level_2_data</t>
-  </si>
-  <si>
-    <t>level_2</t>
-  </si>
-  <si>
-    <t>Barcelona</t>
-  </si>
-  <si>
-    <t>Test Spawners Toni</t>
-  </si>
-  <si>
-    <t>ART_Toni_SpawnersTest</t>
-  </si>
-  <si>
-    <t>SP_Toni_SpawnersTest;CO_Toni_SpawnersTest;ART_Toni_SpawnersTest</t>
-  </si>
-  <si>
-    <t>level_1_data</t>
-  </si>
-  <si>
-    <t>level_1</t>
-  </si>
-  <si>
-    <t>Medieval_Final</t>
-  </si>
-  <si>
-    <t>CO_Medieval_Gameplay_WIP</t>
-  </si>
-  <si>
-    <t>CO_LevelEditor_Gameplay</t>
-  </si>
-  <si>
-    <t>SP_Medieval_Final_Dark;SO_Medieval_Dark;ART_Particles_Dark;ART_L1_Background_Dark;ART_L1_Darkzone_Bigtree;ART_L1_loading_darkzone</t>
-  </si>
-  <si>
-    <t>SP_Medieval_Final_Castle;SO_Medieval_Castle;ART_L1_Castle_Air_Currents;ART_L1_Castle_Dungeon;ART_L1_Castle;ART_L1_Castle_Water_Caves;ART_Particles_Castle;ART_L1_Background_Castle;ART_L1_Castle_Goblins_Mines;ART_L1_Castle_Hazards;ART_L1_loading_castle</t>
-  </si>
-  <si>
-    <t>ART_Medieval_Lighting</t>
-  </si>
-  <si>
-    <t>SP_Medieval_Final_Village;SO_Medieval_Village;ART_L1_Village_Fortress;ART_L1_Village_Goblin_World;ART_L1_Village_Human_Village;ART_L1_Village_Witch_Forest;ART_Particles_Village;ART_L1_Village_Water_Caves;ART_L1_Left_Mini_Cave;ART_twister_cave;ART_L1_Village_Air_Cool;ART_L1_loading_castle;ART_L1_Background_Village;ART_L1_loading_darkzone</t>
-  </si>
-  <si>
-    <t>level_0_data</t>
-  </si>
-  <si>
-    <t>level_0</t>
-  </si>
-  <si>
-    <t>tidDesc</t>
-  </si>
-  <si>
-    <t>tidName</t>
-  </si>
-  <si>
-    <t>comingSoon</t>
-  </si>
-  <si>
-    <t>[gameplayWip]</t>
-  </si>
-  <si>
-    <t>[levelEditor]</t>
-  </si>
-  <si>
-    <t>[dragon_titan]</t>
-  </si>
-  <si>
-    <t>[dragon_devil]</t>
-  </si>
-  <si>
-    <t>[dragon_balrog]</t>
-  </si>
-  <si>
-    <t>[dragon_classic]</t>
-  </si>
-  <si>
-    <t>[dragon_bug]</t>
-  </si>
-  <si>
-    <t>[dragon_chinese]</t>
-  </si>
-  <si>
-    <t>[dragon_reptile]</t>
-  </si>
-  <si>
-    <t>[dragon_fat]</t>
-  </si>
-  <si>
-    <t>[dragon_crocodile]</t>
-  </si>
-  <si>
-    <t>[dragon_baby]</t>
-  </si>
-  <si>
-    <t>[area3]</t>
-  </si>
-  <si>
-    <t>[area2]</t>
-  </si>
-  <si>
-    <t>[area1Active]</t>
-  </si>
-  <si>
-    <t>[area1]</t>
-  </si>
-  <si>
-    <t>[common]</t>
-  </si>
-  <si>
-    <t>[dataFile]</t>
-  </si>
-  <si>
-    <t>dragonsToUnlock</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>{levelDefinitions}</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">WARNING: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Any new scene (spawners, collision or art) must be added to the project build settings (ask a programmer if you don't know how to do so)</t>
-    </r>
-  </si>
-  <si>
-    <t>LEVEL DEFINITIONS</t>
-  </si>
-  <si>
     <t>100;200;300;400;500;600</t>
   </si>
   <si>
@@ -1562,16 +1407,13 @@
   </si>
   <si>
     <t>SCORE MULTIPLIER DEFINITIONS</t>
-  </si>
-  <si>
-    <t>SP_Medieval_Final_Common;CO_Medieval_Final_Castle;CO_Medieval_Final_Dark_Caves;CO_Medieval_Final_Dark_Witch_Tree;CO_Medieval_Final_Village;ART_Medieval_Lighting;Art_Level_fog;SO_Medieval_Common;ART_Levels_Background_Skies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1667,25 +1509,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="21">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1794,20 +1619,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="24">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -2092,36 +1905,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2598,39 +2387,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2674,7 +2430,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="122">
+  <dxfs count="92">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3098,703 +2854,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5639,57 +4698,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE112" totalsRowShown="0" headerRowDxfId="121" dataDxfId="119" headerRowBorderDxfId="120" tableBorderDxfId="118" totalsRowBorderDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE112" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
   <autoFilter ref="A22:AE112"/>
   <sortState ref="A23:AE109">
     <sortCondition ref="B22:B109"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="116"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="115"/>
-    <tableColumn id="6" name="[category]" dataDxfId="114"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="113"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="112"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="111"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="110"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="109"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="108"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="107"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="106"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="105"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="104"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="103"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="102"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="101"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="100"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="99"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="98"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="97"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="96"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="95"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="94"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="93"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="92"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="91"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="90"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="89"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="88"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="87"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="86"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="86"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
+    <tableColumn id="6" name="[category]" dataDxfId="84"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="83"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="82"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="81"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="80"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="79"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B17" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="84" tableBorderDxfId="83" totalsRowBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B17" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B17"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="81"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="80"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5702,61 +4761,27 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="4" name="[category]" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="16" name="[size]" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="levelDefinitions" displayName="levelDefinitions" ref="A4:Y7" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
-  <autoFilter ref="A4:Y7"/>
-  <tableColumns count="25">
-    <tableColumn id="1" name="{levelDefinitions}" dataDxfId="42"/>
-    <tableColumn id="9" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" name="order" dataDxfId="40"/>
-    <tableColumn id="4" name="dragonsToUnlock" dataDxfId="39"/>
-    <tableColumn id="14" name="[dataFile]" dataDxfId="38"/>
-    <tableColumn id="5" name="[common]" dataDxfId="37"/>
-    <tableColumn id="2" name="[area1]" dataDxfId="36"/>
-    <tableColumn id="10" name="[area1Active]" dataDxfId="35"/>
-    <tableColumn id="22" name="[area2]" dataDxfId="34"/>
-    <tableColumn id="23" name="[area3]" dataDxfId="33"/>
-    <tableColumn id="7" name="[dragon_baby]" dataDxfId="32"/>
-    <tableColumn id="8" name="[dragon_crocodile]" dataDxfId="31"/>
-    <tableColumn id="13" name="[dragon_fat]" dataDxfId="30"/>
-    <tableColumn id="15" name="[dragon_reptile]" dataDxfId="29"/>
-    <tableColumn id="16" name="[dragon_chinese]" dataDxfId="28"/>
-    <tableColumn id="17" name="[dragon_bug]" dataDxfId="27"/>
-    <tableColumn id="18" name="[dragon_classic]" dataDxfId="26"/>
-    <tableColumn id="19" name="[dragon_balrog]" dataDxfId="25"/>
-    <tableColumn id="20" name="[dragon_devil]" dataDxfId="24"/>
-    <tableColumn id="21" name="[dragon_titan]" dataDxfId="23"/>
-    <tableColumn id="25" name="[levelEditor]"/>
-    <tableColumn id="24" name="[gameplayWip]"/>
-    <tableColumn id="6" name="comingSoon" dataDxfId="22"/>
-    <tableColumn id="11" name="tidName" dataDxfId="21"/>
-    <tableColumn id="12" name="tidDesc" dataDxfId="20"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
@@ -5772,7 +4797,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
@@ -6100,8 +5125,8 @@
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
-      <c r="E3" s="214"/>
-      <c r="F3" s="214"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
       <c r="G3" s="23"/>
       <c r="H3" s="22"/>
       <c r="I3" s="172"/>
@@ -6257,8 +5282,8 @@
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="214"/>
-      <c r="F21" s="214"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
       <c r="G21" s="23"/>
       <c r="H21" s="22"/>
       <c r="I21" s="23"/>
@@ -14789,8 +13814,8 @@
       <c r="C115" s="23"/>
       <c r="D115" s="23"/>
       <c r="E115" s="23"/>
-      <c r="F115" s="214"/>
-      <c r="G115" s="214"/>
+      <c r="F115" s="193"/>
+      <c r="G115" s="193"/>
       <c r="H115" s="22" t="s">
         <v>56</v>
       </c>
@@ -16341,385 +15366,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="6"/>
-  </sheetPr>
-  <dimension ref="A1:Y7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="255.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="135.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="179.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>451</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="194" t="s">
-        <v>450</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:25" ht="96" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="193" t="s">
-        <v>448</v>
-      </c>
-      <c r="D4" s="192" t="s">
-        <v>447</v>
-      </c>
-      <c r="E4" s="191" t="s">
-        <v>446</v>
-      </c>
-      <c r="F4" s="191" t="s">
-        <v>445</v>
-      </c>
-      <c r="G4" s="191" t="s">
-        <v>444</v>
-      </c>
-      <c r="H4" s="191" t="s">
-        <v>443</v>
-      </c>
-      <c r="I4" s="191" t="s">
-        <v>442</v>
-      </c>
-      <c r="J4" s="191" t="s">
-        <v>441</v>
-      </c>
-      <c r="K4" s="191" t="s">
-        <v>440</v>
-      </c>
-      <c r="L4" s="191" t="s">
-        <v>439</v>
-      </c>
-      <c r="M4" s="191" t="s">
-        <v>438</v>
-      </c>
-      <c r="N4" s="191" t="s">
-        <v>437</v>
-      </c>
-      <c r="O4" s="191" t="s">
-        <v>436</v>
-      </c>
-      <c r="P4" s="191" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q4" s="191" t="s">
-        <v>434</v>
-      </c>
-      <c r="R4" s="191" t="s">
-        <v>433</v>
-      </c>
-      <c r="S4" s="191" t="s">
-        <v>432</v>
-      </c>
-      <c r="T4" s="191" t="s">
-        <v>431</v>
-      </c>
-      <c r="U4" s="191" t="s">
-        <v>430</v>
-      </c>
-      <c r="V4" s="191" t="s">
-        <v>429</v>
-      </c>
-      <c r="W4" s="190" t="s">
-        <v>428</v>
-      </c>
-      <c r="X4" s="189" t="s">
-        <v>427</v>
-      </c>
-      <c r="Y4" s="188" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="187" t="s">
-        <v>425</v>
-      </c>
-      <c r="C5" s="186">
-        <v>0</v>
-      </c>
-      <c r="D5" s="185">
-        <v>0</v>
-      </c>
-      <c r="E5" s="179" t="s">
-        <v>424</v>
-      </c>
-      <c r="F5" s="179" t="s">
-        <v>508</v>
-      </c>
-      <c r="G5" s="179" t="s">
-        <v>423</v>
-      </c>
-      <c r="H5" s="179" t="s">
-        <v>422</v>
-      </c>
-      <c r="I5" s="179" t="s">
-        <v>421</v>
-      </c>
-      <c r="J5" s="179" t="s">
-        <v>420</v>
-      </c>
-      <c r="K5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="L5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="M5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="N5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="O5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="P5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="R5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="S5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="T5" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="U5" s="179" t="s">
-        <v>419</v>
-      </c>
-      <c r="V5" s="179" t="s">
-        <v>418</v>
-      </c>
-      <c r="W5" s="184" t="b">
-        <v>0</v>
-      </c>
-      <c r="X5" s="183" t="s">
-        <v>417</v>
-      </c>
-      <c r="Y5" s="182" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="171" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="187" t="s">
-        <v>416</v>
-      </c>
-      <c r="C6" s="186">
-        <v>1</v>
-      </c>
-      <c r="D6" s="185">
-        <v>0</v>
-      </c>
-      <c r="E6" s="179" t="s">
-        <v>415</v>
-      </c>
-      <c r="F6" s="179" t="s">
-        <v>414</v>
-      </c>
-      <c r="G6" s="179"/>
-      <c r="H6" s="179" t="s">
-        <v>413</v>
-      </c>
-      <c r="I6" s="179"/>
-      <c r="J6" s="179"/>
-      <c r="K6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="L6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="M6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="N6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="O6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="P6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="R6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="S6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="T6" s="179" t="s">
-        <v>406</v>
-      </c>
-      <c r="U6" s="179"/>
-      <c r="V6" s="179"/>
-      <c r="W6" s="184" t="b">
-        <v>0</v>
-      </c>
-      <c r="X6" s="183" t="s">
-        <v>412</v>
-      </c>
-      <c r="Y6" s="182" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="169" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="169" t="s">
-        <v>410</v>
-      </c>
-      <c r="C7" s="181">
-        <v>2</v>
-      </c>
-      <c r="D7" s="180">
-        <v>0</v>
-      </c>
-      <c r="E7" s="179" t="s">
-        <v>409</v>
-      </c>
-      <c r="F7" s="177" t="s">
-        <v>408</v>
-      </c>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178" t="s">
-        <v>407</v>
-      </c>
-      <c r="I7" s="178"/>
-      <c r="J7" s="178"/>
-      <c r="K7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="L7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="M7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="N7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="O7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="P7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="R7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="S7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="T7" s="177" t="s">
-        <v>406</v>
-      </c>
-      <c r="U7" s="177"/>
-      <c r="V7" s="177"/>
-      <c r="W7" s="176" t="b">
-        <v>0</v>
-      </c>
-      <c r="X7" s="175" t="s">
-        <v>405</v>
-      </c>
-      <c r="Y7" s="174" t="s">
-        <v>405</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="47" priority="3"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16736,7 +15387,7 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>507</v>
+        <v>460</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -16753,8 +15404,8 @@
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="214"/>
-      <c r="G3" s="214"/>
+      <c r="F3" s="193"/>
+      <c r="G3" s="193"/>
       <c r="H3" s="23"/>
       <c r="I3" s="22"/>
       <c r="J3" s="172"/>
@@ -16762,428 +15413,428 @@
     </row>
     <row r="4" spans="2:11" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>506</v>
+        <v>459</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>505</v>
+        <v>458</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>504</v>
+        <v>457</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>503</v>
+        <v>456</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>502</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="212" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="211" t="s">
-        <v>501</v>
-      </c>
-      <c r="D5" s="211">
-        <v>0</v>
-      </c>
-      <c r="E5" s="210">
-        <v>1</v>
-      </c>
-      <c r="F5" s="210">
-        <v>0</v>
-      </c>
-      <c r="G5" s="210">
+      <c r="B5" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="190" t="s">
+        <v>454</v>
+      </c>
+      <c r="D5" s="190">
+        <v>0</v>
+      </c>
+      <c r="E5" s="189">
+        <v>1</v>
+      </c>
+      <c r="F5" s="189">
+        <v>0</v>
+      </c>
+      <c r="G5" s="189">
         <v>-1</v>
       </c>
-      <c r="H5" s="209"/>
+      <c r="H5" s="188"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="212" t="s">
+      <c r="B6" s="191" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>500</v>
+        <v>453</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="213">
-        <v>2</v>
-      </c>
-      <c r="F6" s="213">
+      <c r="E6" s="192">
+        <v>2</v>
+      </c>
+      <c r="F6" s="192">
         <v>8</v>
       </c>
-      <c r="G6" s="213">
+      <c r="G6" s="192">
         <v>3</v>
       </c>
-      <c r="H6" s="209"/>
+      <c r="H6" s="188"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="208" t="s">
-        <v>477</v>
+      <c r="B7" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C7" s="170"/>
       <c r="D7" s="170"/>
-      <c r="E7" s="207"/>
-      <c r="F7" s="207"/>
-      <c r="G7" s="207"/>
-      <c r="H7" s="205" t="s">
-        <v>499</v>
+      <c r="E7" s="186"/>
+      <c r="F7" s="186"/>
+      <c r="G7" s="186"/>
+      <c r="H7" s="184" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="208" t="s">
-        <v>477</v>
+      <c r="B8" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C8" s="170"/>
       <c r="D8" s="170"/>
-      <c r="E8" s="207"/>
-      <c r="F8" s="207"/>
-      <c r="G8" s="207"/>
-      <c r="H8" s="205" t="s">
-        <v>498</v>
+      <c r="E8" s="186"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="186"/>
+      <c r="H8" s="184" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="208" t="s">
-        <v>477</v>
+      <c r="B9" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C9" s="170"/>
       <c r="D9" s="170"/>
-      <c r="E9" s="207"/>
-      <c r="F9" s="207"/>
-      <c r="G9" s="207"/>
-      <c r="H9" s="205" t="s">
-        <v>497</v>
+      <c r="E9" s="186"/>
+      <c r="F9" s="186"/>
+      <c r="G9" s="186"/>
+      <c r="H9" s="184" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="212" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="211" t="s">
-        <v>496</v>
-      </c>
-      <c r="D10" s="211">
-        <v>2</v>
-      </c>
-      <c r="E10" s="210">
+      <c r="B10" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="190" t="s">
+        <v>449</v>
+      </c>
+      <c r="D10" s="190">
+        <v>2</v>
+      </c>
+      <c r="E10" s="189">
         <v>4</v>
       </c>
-      <c r="F10" s="210">
+      <c r="F10" s="189">
         <v>22</v>
       </c>
-      <c r="G10" s="210">
+      <c r="G10" s="189">
         <v>2.5</v>
       </c>
-      <c r="H10" s="209"/>
+      <c r="H10" s="188"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="208" t="s">
-        <v>477</v>
+      <c r="B11" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C11" s="170"/>
       <c r="D11" s="170"/>
-      <c r="E11" s="207"/>
-      <c r="F11" s="207"/>
-      <c r="G11" s="207"/>
-      <c r="H11" s="205" t="s">
-        <v>495</v>
+      <c r="E11" s="186"/>
+      <c r="F11" s="186"/>
+      <c r="G11" s="186"/>
+      <c r="H11" s="184" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="208" t="s">
-        <v>477</v>
+      <c r="B12" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C12" s="170"/>
       <c r="D12" s="170"/>
-      <c r="E12" s="207"/>
-      <c r="F12" s="207"/>
-      <c r="G12" s="207"/>
-      <c r="H12" s="205" t="s">
-        <v>494</v>
+      <c r="E12" s="186"/>
+      <c r="F12" s="186"/>
+      <c r="G12" s="186"/>
+      <c r="H12" s="184" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="208" t="s">
-        <v>477</v>
+      <c r="B13" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C13" s="170"/>
       <c r="D13" s="170"/>
-      <c r="E13" s="207"/>
-      <c r="F13" s="207"/>
-      <c r="G13" s="207"/>
-      <c r="H13" s="205" t="s">
-        <v>493</v>
+      <c r="E13" s="186"/>
+      <c r="F13" s="186"/>
+      <c r="G13" s="186"/>
+      <c r="H13" s="184" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="212" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="211" t="s">
-        <v>492</v>
-      </c>
-      <c r="D14" s="211">
+      <c r="B14" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="190" t="s">
+        <v>445</v>
+      </c>
+      <c r="D14" s="190">
         <v>3</v>
       </c>
-      <c r="E14" s="210">
+      <c r="E14" s="189">
         <v>6</v>
       </c>
-      <c r="F14" s="210">
+      <c r="F14" s="189">
         <v>32</v>
       </c>
-      <c r="G14" s="210">
+      <c r="G14" s="189">
         <v>2.5</v>
       </c>
-      <c r="H14" s="209"/>
+      <c r="H14" s="188"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="208" t="s">
-        <v>477</v>
+      <c r="B15" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C15" s="170"/>
       <c r="D15" s="170"/>
-      <c r="E15" s="207"/>
-      <c r="F15" s="207"/>
-      <c r="G15" s="207"/>
-      <c r="H15" s="205" t="s">
-        <v>491</v>
+      <c r="E15" s="186"/>
+      <c r="F15" s="186"/>
+      <c r="G15" s="186"/>
+      <c r="H15" s="184" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="208" t="s">
-        <v>477</v>
+      <c r="B16" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C16" s="170"/>
       <c r="D16" s="170"/>
-      <c r="E16" s="207"/>
-      <c r="F16" s="207"/>
-      <c r="G16" s="207"/>
-      <c r="H16" s="205" t="s">
-        <v>490</v>
+      <c r="E16" s="186"/>
+      <c r="F16" s="186"/>
+      <c r="G16" s="186"/>
+      <c r="H16" s="184" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="208" t="s">
-        <v>477</v>
+      <c r="B17" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C17" s="170"/>
       <c r="D17" s="170"/>
-      <c r="E17" s="207"/>
-      <c r="F17" s="207"/>
-      <c r="G17" s="207"/>
-      <c r="H17" s="205" t="s">
-        <v>489</v>
+      <c r="E17" s="186"/>
+      <c r="F17" s="186"/>
+      <c r="G17" s="186"/>
+      <c r="H17" s="184" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="212" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="211" t="s">
-        <v>488</v>
-      </c>
-      <c r="D18" s="211">
+      <c r="B18" s="191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="190" t="s">
+        <v>441</v>
+      </c>
+      <c r="D18" s="190">
         <v>4</v>
       </c>
-      <c r="E18" s="210">
+      <c r="E18" s="189">
         <v>8</v>
       </c>
-      <c r="F18" s="210">
+      <c r="F18" s="189">
         <v>50</v>
       </c>
-      <c r="G18" s="210">
-        <v>2</v>
-      </c>
-      <c r="H18" s="209"/>
+      <c r="G18" s="189">
+        <v>2</v>
+      </c>
+      <c r="H18" s="188"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="208" t="s">
-        <v>477</v>
+      <c r="B19" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C19" s="170"/>
       <c r="D19" s="170"/>
-      <c r="E19" s="207"/>
-      <c r="F19" s="207"/>
-      <c r="G19" s="207"/>
-      <c r="H19" s="205" t="s">
-        <v>487</v>
+      <c r="E19" s="186"/>
+      <c r="F19" s="186"/>
+      <c r="G19" s="186"/>
+      <c r="H19" s="184" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="208" t="s">
-        <v>477</v>
+      <c r="B20" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C20" s="170"/>
       <c r="D20" s="170"/>
-      <c r="E20" s="207"/>
-      <c r="F20" s="207"/>
-      <c r="G20" s="207"/>
-      <c r="H20" s="205" t="s">
-        <v>486</v>
+      <c r="E20" s="186"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="186"/>
+      <c r="H20" s="184" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="208" t="s">
-        <v>477</v>
+      <c r="B21" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C21" s="170"/>
       <c r="D21" s="170"/>
-      <c r="E21" s="207"/>
-      <c r="F21" s="207"/>
-      <c r="G21" s="207"/>
-      <c r="H21" s="205" t="s">
-        <v>485</v>
+      <c r="E21" s="186"/>
+      <c r="F21" s="186"/>
+      <c r="G21" s="186"/>
+      <c r="H21" s="184" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="208" t="s">
+      <c r="B22" s="187" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="170" t="s">
-        <v>484</v>
+        <v>437</v>
       </c>
       <c r="D22" s="170">
         <v>5</v>
       </c>
-      <c r="E22" s="207">
+      <c r="E22" s="186">
         <v>10</v>
       </c>
-      <c r="F22" s="206">
+      <c r="F22" s="185">
         <v>75</v>
       </c>
-      <c r="G22" s="206">
-        <v>2</v>
-      </c>
-      <c r="H22" s="205"/>
+      <c r="G22" s="185">
+        <v>2</v>
+      </c>
+      <c r="H22" s="184"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="208" t="s">
-        <v>477</v>
+      <c r="B23" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C23" s="170"/>
       <c r="D23" s="170"/>
-      <c r="E23" s="207"/>
-      <c r="F23" s="206"/>
-      <c r="G23" s="206"/>
-      <c r="H23" s="205" t="s">
-        <v>483</v>
+      <c r="E23" s="186"/>
+      <c r="F23" s="185"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="184" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="208" t="s">
+      <c r="B24" s="187" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="170" t="s">
-        <v>482</v>
+        <v>435</v>
       </c>
       <c r="D24" s="170">
         <v>6</v>
       </c>
-      <c r="E24" s="207">
+      <c r="E24" s="186">
         <v>12</v>
       </c>
-      <c r="F24" s="206">
+      <c r="F24" s="185">
         <v>120</v>
       </c>
-      <c r="G24" s="206">
-        <v>2</v>
-      </c>
-      <c r="H24" s="205"/>
+      <c r="G24" s="185">
+        <v>2</v>
+      </c>
+      <c r="H24" s="184"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="208" t="s">
-        <v>477</v>
+      <c r="B25" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C25" s="170"/>
       <c r="D25" s="170"/>
-      <c r="E25" s="207"/>
-      <c r="F25" s="206"/>
-      <c r="G25" s="206"/>
-      <c r="H25" s="205" t="s">
-        <v>481</v>
+      <c r="E25" s="186"/>
+      <c r="F25" s="185"/>
+      <c r="G25" s="185"/>
+      <c r="H25" s="184" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="208" t="s">
+      <c r="B26" s="187" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="170" t="s">
-        <v>480</v>
+        <v>433</v>
       </c>
       <c r="D26" s="170">
         <v>7</v>
       </c>
-      <c r="E26" s="207">
+      <c r="E26" s="186">
         <v>14</v>
       </c>
-      <c r="F26" s="206">
+      <c r="F26" s="185">
         <v>5000</v>
       </c>
-      <c r="G26" s="206">
+      <c r="G26" s="185">
         <v>1.5</v>
       </c>
-      <c r="H26" s="205"/>
+      <c r="H26" s="184"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="208" t="s">
-        <v>477</v>
+      <c r="B27" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C27" s="170"/>
       <c r="D27" s="170"/>
-      <c r="E27" s="207"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="206"/>
-      <c r="H27" s="205" t="s">
-        <v>479</v>
+      <c r="E27" s="186"/>
+      <c r="F27" s="185"/>
+      <c r="G27" s="185"/>
+      <c r="H27" s="184" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="208" t="s">
+      <c r="B28" s="187" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="170" t="s">
-        <v>478</v>
+        <v>431</v>
       </c>
       <c r="D28" s="170">
         <v>8</v>
       </c>
-      <c r="E28" s="207">
+      <c r="E28" s="186">
         <v>16</v>
       </c>
-      <c r="F28" s="206">
+      <c r="F28" s="185">
         <v>5000</v>
       </c>
-      <c r="G28" s="206">
+      <c r="G28" s="185">
         <v>1.5</v>
       </c>
-      <c r="H28" s="205"/>
+      <c r="H28" s="184"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="208" t="s">
-        <v>477</v>
+      <c r="B29" s="187" t="s">
+        <v>430</v>
       </c>
       <c r="C29" s="170"/>
       <c r="D29" s="170"/>
-      <c r="E29" s="207"/>
-      <c r="F29" s="206"/>
-      <c r="G29" s="206"/>
-      <c r="H29" s="205" t="s">
-        <v>476</v>
+      <c r="E29" s="186"/>
+      <c r="F29" s="185"/>
+      <c r="G29" s="185"/>
+      <c r="H29" s="184" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B33" s="9" t="s">
-        <v>475</v>
+        <v>428</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -17193,163 +15844,163 @@
       <c r="H33" s="9"/>
     </row>
     <row r="35" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="204" t="s">
-        <v>474</v>
-      </c>
-      <c r="C35" s="203" t="s">
+      <c r="B35" s="183" t="s">
+        <v>427</v>
+      </c>
+      <c r="C35" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="203" t="s">
-        <v>473</v>
-      </c>
-      <c r="E35" s="203" t="s">
-        <v>472</v>
+      <c r="D35" s="182" t="s">
+        <v>426</v>
+      </c>
+      <c r="E35" s="182" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="201" t="s">
-        <v>471</v>
-      </c>
-      <c r="D36" s="201">
-        <v>1</v>
-      </c>
-      <c r="E36" s="200">
+      <c r="B36" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="180" t="s">
+        <v>424</v>
+      </c>
+      <c r="D36" s="180">
+        <v>1</v>
+      </c>
+      <c r="E36" s="179">
         <v>0.1</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="201" t="s">
-        <v>470</v>
-      </c>
-      <c r="D37" s="201">
-        <v>2</v>
-      </c>
-      <c r="E37" s="200">
+      <c r="B37" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="180" t="s">
+        <v>423</v>
+      </c>
+      <c r="D37" s="180">
+        <v>2</v>
+      </c>
+      <c r="E37" s="179">
         <v>8.7055056329612412E-2</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="201" t="s">
-        <v>469</v>
-      </c>
-      <c r="D38" s="201">
+      <c r="B38" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="180" t="s">
+        <v>422</v>
+      </c>
+      <c r="D38" s="180">
         <v>3</v>
       </c>
-      <c r="E38" s="200">
+      <c r="E38" s="179">
         <v>8.027415617602307E-2</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="201" t="s">
-        <v>468</v>
-      </c>
-      <c r="D39" s="201">
+      <c r="B39" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="180" t="s">
+        <v>421</v>
+      </c>
+      <c r="D39" s="180">
         <v>4</v>
       </c>
-      <c r="E39" s="200">
+      <c r="E39" s="179">
         <v>7.5785828325519916E-2</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="201" t="s">
-        <v>467</v>
-      </c>
-      <c r="D40" s="201">
-        <v>5</v>
-      </c>
-      <c r="E40" s="200">
+      <c r="B40" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="180" t="s">
+        <v>420</v>
+      </c>
+      <c r="D40" s="180">
+        <v>5</v>
+      </c>
+      <c r="E40" s="179">
         <v>7.2477966367769556E-2</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="201" t="s">
-        <v>466</v>
-      </c>
-      <c r="D41" s="201">
+      <c r="B41" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="180" t="s">
+        <v>419</v>
+      </c>
+      <c r="D41" s="180">
         <v>6</v>
       </c>
-      <c r="E41" s="200">
+      <c r="E41" s="179">
         <v>6.988271187715793E-2</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="201" t="s">
-        <v>465</v>
-      </c>
-      <c r="D42" s="201">
+      <c r="B42" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="180" t="s">
+        <v>418</v>
+      </c>
+      <c r="D42" s="180">
         <v>7</v>
       </c>
-      <c r="E42" s="200">
+      <c r="E42" s="179">
         <v>6.776109134004811E-2</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" s="201" t="s">
-        <v>464</v>
-      </c>
-      <c r="D43" s="201">
+      <c r="B43" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="180" t="s">
+        <v>417</v>
+      </c>
+      <c r="D43" s="180">
         <v>8</v>
       </c>
-      <c r="E43" s="200">
+      <c r="E43" s="179">
         <v>6.5975395538644718E-2</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="201" t="s">
-        <v>463</v>
-      </c>
-      <c r="D44" s="201">
+      <c r="B44" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="180" t="s">
+        <v>416</v>
+      </c>
+      <c r="D44" s="180">
         <v>9</v>
       </c>
-      <c r="E44" s="200">
+      <c r="E44" s="179">
         <v>6.4439401497725424E-2</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="202" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="201" t="s">
-        <v>462</v>
-      </c>
-      <c r="D45" s="201">
+      <c r="B45" s="181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="180" t="s">
+        <v>415</v>
+      </c>
+      <c r="D45" s="180">
         <v>10</v>
       </c>
-      <c r="E45" s="200">
+      <c r="E45" s="179">
         <v>6.3095734448019331E-2</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B47" s="9" t="s">
-        <v>461</v>
+        <v>414</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
@@ -17359,48 +16010,48 @@
       <c r="H47" s="9"/>
     </row>
     <row r="49" spans="2:8" ht="130.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="199" t="s">
-        <v>460</v>
-      </c>
-      <c r="C49" s="199" t="s">
+      <c r="B49" s="178" t="s">
+        <v>413</v>
+      </c>
+      <c r="C49" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="199" t="s">
-        <v>459</v>
-      </c>
-      <c r="E49" s="198" t="s">
-        <v>458</v>
-      </c>
-      <c r="F49" s="198" t="s">
-        <v>457</v>
-      </c>
-      <c r="G49" s="198" t="s">
-        <v>456</v>
-      </c>
-      <c r="H49" s="198" t="s">
-        <v>455</v>
+      <c r="D49" s="178" t="s">
+        <v>412</v>
+      </c>
+      <c r="E49" s="177" t="s">
+        <v>411</v>
+      </c>
+      <c r="F49" s="177" t="s">
+        <v>410</v>
+      </c>
+      <c r="G49" s="177" t="s">
+        <v>409</v>
+      </c>
+      <c r="H49" s="177" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="197" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" s="196" t="s">
-        <v>454</v>
-      </c>
-      <c r="D50" s="196" t="s">
-        <v>453</v>
-      </c>
-      <c r="E50" s="195" t="s">
-        <v>452</v>
-      </c>
-      <c r="F50" s="195">
+      <c r="B50" s="176" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="175" t="s">
+        <v>407</v>
+      </c>
+      <c r="D50" s="175" t="s">
+        <v>406</v>
+      </c>
+      <c r="E50" s="174" t="s">
+        <v>405</v>
+      </c>
+      <c r="F50" s="174">
         <v>50</v>
       </c>
-      <c r="G50" s="195">
+      <c r="G50" s="174">
         <v>30</v>
       </c>
-      <c r="H50" s="195">
+      <c r="H50" s="174">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[CONTENT] [FIX] [HDK-804] Soulmuncher pet gets stuck on trying to eat biggest (blue) ghost. Ghost03 wasn't edible. Parameter [isEdible] flagged as true, so now pets can eat them.
Former-commit-id: 44a39e6a371d9f119aa95024c4fb94ac980a0b6c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$116:$O$117</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5084,9 +5084,9 @@
   <dimension ref="A1:AE144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="C103" sqref="C103"/>
+      <selection pane="topRight" activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8977,7 +8977,7 @@
         <v>0</v>
       </c>
       <c r="L61" s="78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M61" s="81">
         <v>5</v>

</xml_diff>

<commit_message>
[CONTENT] [FIX] Pet MinerEater didn't eat medium and big mines, only small ones. Parameter [isEdible] flags as true for both mines.
Former-commit-id: 26179ff598d07a7abf03e03975291ec376ba3c5e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5086,7 +5086,7 @@
     <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A61" sqref="A61:XFD61"/>
+      <selection pane="topRight" activeCell="L78" sqref="L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10472,7 +10472,7 @@
         <v>0</v>
       </c>
       <c r="L77" s="78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M77" s="81">
         <v>5</v>
@@ -10568,7 +10568,7 @@
         <v>0</v>
       </c>
       <c r="L78" s="78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M78" s="81">
         <v>5</v>

</xml_diff>

<commit_message>
MineWagon is burnable from tier 0
Former-commit-id: 832a04f4c71fb294b5f70cd33c98d5b663ad440e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5083,10 +5083,10 @@
   </sheetPr>
   <dimension ref="A1:AE144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="L78" sqref="L78"/>
+      <selection pane="topRight" activeCell="P80" sqref="P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10770,7 +10770,7 @@
         <v>5</v>
       </c>
       <c r="P80" s="142">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q80" s="140" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
stunTime set to 0
Former-commit-id: c7977e67d87a2434935bfe74e36bc1ba8ee021ff
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5083,10 +5083,10 @@
   </sheetPr>
   <dimension ref="A1:AE144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="P80" sqref="P80"/>
+      <selection pane="topRight" activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14534,7 +14534,7 @@
         <v>2</v>
       </c>
       <c r="H133" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
@@ -14560,7 +14560,7 @@
         <v>2</v>
       </c>
       <c r="H134" s="2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
@@ -14586,7 +14586,7 @@
         <v>2</v>
       </c>
       <c r="H135" s="2">
-        <v>0.32500000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -14612,7 +14612,7 @@
         <v>2</v>
       </c>
       <c r="H136" s="2">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
@@ -14638,7 +14638,7 @@
         <v>2</v>
       </c>
       <c r="H137" s="2">
-        <v>0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
3 new rows in content for dark entities
Former-commit-id: 54423b518ac91be0a52b570b9e539bdd0bff7a43
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$117:$O$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$120:$O$121</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="465">
   <si>
     <t>tier_4</t>
   </si>
@@ -1415,6 +1415,15 @@
   </si>
   <si>
     <t>RazorbackBaby</t>
+  </si>
+  <si>
+    <t>HermitCrabBlueBig</t>
+  </si>
+  <si>
+    <t>HermitCrabBlueSmall</t>
+  </si>
+  <si>
+    <t>HermitCrabBlueSmallTurret</t>
   </si>
 </sst>
 </file>
@@ -1918,7 +1927,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2432,6 +2441,48 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4706,8 +4757,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE113" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
-  <autoFilter ref="A22:AE113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE116" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+  <autoFilter ref="A22:AE116"/>
   <sortState ref="A23:AE109">
     <sortCondition ref="B22:B109"/>
   </sortState>
@@ -4763,8 +4814,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A117:O128" totalsRowShown="0">
-  <autoFilter ref="A117:O128"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A120:O131" totalsRowShown="0">
+  <autoFilter ref="A120:O131"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
@@ -5084,12 +5135,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AE145"/>
+  <dimension ref="A1:AE148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A88" sqref="A88"/>
+      <selection pane="topRight" activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13879,281 +13930,410 @@
       <c r="AD113" s="26"/>
       <c r="AE113" s="25"/>
     </row>
-    <row r="114" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="115" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A115" s="9" t="s">
+    <row r="114" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A114" s="195" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="148" t="s">
+        <v>462</v>
+      </c>
+      <c r="C114" s="147" t="s">
+        <v>66</v>
+      </c>
+      <c r="D114" s="120">
+        <v>60</v>
+      </c>
+      <c r="E114" s="119">
+        <v>9</v>
+      </c>
+      <c r="F114" s="119">
+        <v>0</v>
+      </c>
+      <c r="G114" s="119">
+        <v>5</v>
+      </c>
+      <c r="H114" s="119">
+        <v>0</v>
+      </c>
+      <c r="I114" s="119">
+        <v>35</v>
+      </c>
+      <c r="J114" s="196">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K114" s="119">
+        <v>0</v>
+      </c>
+      <c r="L114" s="150" t="b">
+        <v>1</v>
+      </c>
+      <c r="M114" s="197">
+        <v>5</v>
+      </c>
+      <c r="N114" s="197">
+        <v>5</v>
+      </c>
+      <c r="O114" s="198">
+        <v>2</v>
+      </c>
+      <c r="P114" s="197">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>2</v>
+      </c>
+      <c r="Q114" s="149" t="b">
+        <v>1</v>
+      </c>
+      <c r="R114" s="199" t="b">
+        <v>0</v>
+      </c>
+      <c r="S114" s="149" t="b">
+        <v>0</v>
+      </c>
+      <c r="T114" s="149">
+        <v>1</v>
+      </c>
+      <c r="U114" s="199">
+        <v>2</v>
+      </c>
+      <c r="V114" s="149">
+        <v>0</v>
+      </c>
+      <c r="W114" s="116">
+        <v>0.1</v>
+      </c>
+      <c r="X114" s="116">
+        <v>0.1</v>
+      </c>
+      <c r="Y114" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z114" s="115">
+        <v>0</v>
+      </c>
+      <c r="AA114" s="145" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB114" s="130" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC114" s="125" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD114" s="125"/>
+      <c r="AE114" s="124"/>
+    </row>
+    <row r="115" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A115" s="207" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="88" t="s">
+        <v>463</v>
+      </c>
+      <c r="C115" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D115" s="194">
+        <v>60</v>
+      </c>
+      <c r="E115" s="71">
+        <v>9</v>
+      </c>
+      <c r="F115" s="71">
+        <v>0</v>
+      </c>
+      <c r="G115" s="71">
+        <v>5</v>
+      </c>
+      <c r="H115" s="71">
+        <v>0</v>
+      </c>
+      <c r="I115" s="71">
+        <v>35</v>
+      </c>
+      <c r="J115" s="42">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K115" s="71">
+        <v>0</v>
+      </c>
+      <c r="L115" s="200" t="b">
+        <v>1</v>
+      </c>
+      <c r="M115" s="38">
+        <v>5</v>
+      </c>
+      <c r="N115" s="38">
+        <v>5</v>
+      </c>
+      <c r="O115" s="201">
+        <v>2</v>
+      </c>
+      <c r="P115" s="38">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>2</v>
+      </c>
+      <c r="Q115" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="R115" s="202" t="b">
+        <v>0</v>
+      </c>
+      <c r="S115" s="202" t="b">
+        <v>0</v>
+      </c>
+      <c r="T115" s="203">
+        <v>1</v>
+      </c>
+      <c r="U115" s="204">
+        <v>2</v>
+      </c>
+      <c r="V115" s="205">
+        <v>0</v>
+      </c>
+      <c r="W115" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="X115" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="Y115" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z115" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA115" s="206" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB115" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC115" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD115" s="26"/>
+      <c r="AE115" s="25"/>
+    </row>
+    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A116" s="207" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="88" t="s">
+        <v>464</v>
+      </c>
+      <c r="C116" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D116" s="194">
+        <v>60</v>
+      </c>
+      <c r="E116" s="71">
+        <v>9</v>
+      </c>
+      <c r="F116" s="71">
+        <v>0</v>
+      </c>
+      <c r="G116" s="71">
+        <v>5</v>
+      </c>
+      <c r="H116" s="71">
+        <v>0</v>
+      </c>
+      <c r="I116" s="71">
+        <v>35</v>
+      </c>
+      <c r="J116" s="42">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K116" s="71">
+        <v>0</v>
+      </c>
+      <c r="L116" s="200" t="b">
+        <v>1</v>
+      </c>
+      <c r="M116" s="38">
+        <v>5</v>
+      </c>
+      <c r="N116" s="38">
+        <v>5</v>
+      </c>
+      <c r="O116" s="201">
+        <v>2</v>
+      </c>
+      <c r="P116" s="38">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>2</v>
+      </c>
+      <c r="Q116" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="R116" s="202" t="b">
+        <v>0</v>
+      </c>
+      <c r="S116" s="202" t="b">
+        <v>0</v>
+      </c>
+      <c r="T116" s="203">
+        <v>1</v>
+      </c>
+      <c r="U116" s="204">
+        <v>2</v>
+      </c>
+      <c r="V116" s="205">
+        <v>0</v>
+      </c>
+      <c r="W116" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="X116" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="Y116" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z116" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA116" s="206" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB116" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AC116" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD116" s="26"/>
+      <c r="AE116" s="25"/>
+    </row>
+    <row r="117" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A118" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B115" s="9"/>
-      <c r="C115" s="9"/>
-      <c r="D115" s="9"/>
-      <c r="E115" s="9"/>
-      <c r="F115" s="9"/>
-      <c r="G115" s="9"/>
-      <c r="H115" s="9"/>
-      <c r="I115" s="9"/>
-      <c r="J115" s="9"/>
-      <c r="K115" s="9"/>
-      <c r="L115" s="9"/>
-      <c r="M115" s="9"/>
-      <c r="N115" s="9"/>
-      <c r="O115" s="9"/>
-      <c r="P115" s="9"/>
-      <c r="Q115" s="9"/>
-      <c r="R115" s="9"/>
-      <c r="S115" s="9"/>
-      <c r="T115" s="9"/>
-      <c r="U115" s="9"/>
-      <c r="V115" s="9"/>
-      <c r="W115" s="9"/>
-      <c r="X115" s="9"/>
-      <c r="Y115" s="9"/>
-      <c r="Z115" s="9"/>
-      <c r="AA115" s="9"/>
-    </row>
-    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A116" s="23"/>
-      <c r="B116" s="23"/>
-      <c r="C116" s="23"/>
-      <c r="D116" s="23"/>
-      <c r="E116" s="23"/>
-      <c r="F116" s="193"/>
-      <c r="G116" s="193"/>
-      <c r="H116" s="22" t="s">
+      <c r="B118" s="9"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="9"/>
+      <c r="K118" s="9"/>
+      <c r="L118" s="9"/>
+      <c r="M118" s="9"/>
+      <c r="N118" s="9"/>
+      <c r="O118" s="9"/>
+      <c r="P118" s="9"/>
+      <c r="Q118" s="9"/>
+      <c r="R118" s="9"/>
+      <c r="S118" s="9"/>
+      <c r="T118" s="9"/>
+      <c r="U118" s="9"/>
+      <c r="V118" s="9"/>
+      <c r="W118" s="9"/>
+      <c r="X118" s="9"/>
+      <c r="Y118" s="9"/>
+      <c r="Z118" s="9"/>
+      <c r="AA118" s="9"/>
+    </row>
+    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A119" s="23"/>
+      <c r="B119" s="23"/>
+      <c r="C119" s="23"/>
+      <c r="D119" s="23"/>
+      <c r="E119" s="23"/>
+      <c r="F119" s="193"/>
+      <c r="G119" s="193"/>
+      <c r="H119" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I116" s="22"/>
-      <c r="J116" s="23"/>
-      <c r="K116" s="18"/>
-      <c r="L116" s="18"/>
-      <c r="M116" s="18" t="s">
+      <c r="I119" s="22"/>
+      <c r="J119" s="23"/>
+      <c r="K119" s="18"/>
+      <c r="L119" s="18"/>
+      <c r="M119" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="N116" s="18"/>
-      <c r="O116" s="18"/>
-      <c r="P116" s="18"/>
-      <c r="Q116" s="18"/>
-      <c r="R116" s="18"/>
-      <c r="S116" s="18"/>
-      <c r="T116" s="18"/>
-      <c r="U116" s="18"/>
-      <c r="V116" s="18"/>
-      <c r="W116" s="18"/>
-      <c r="X116" s="18"/>
-      <c r="Y116" s="18"/>
-      <c r="Z116" s="18"/>
-      <c r="AA116" s="22"/>
-      <c r="AB116" s="22"/>
-      <c r="AC116" s="22"/>
-      <c r="AD116" s="22"/>
-      <c r="AE116" s="18"/>
-    </row>
-    <row r="117" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D117" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E117" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F117" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="G117" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H117" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="I117" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="J117" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K117" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L117" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M117" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N117" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="O117" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A118" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B118" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C118" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D118" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E118" s="15">
-        <v>3</v>
-      </c>
-      <c r="F118" s="19">
-        <v>0</v>
-      </c>
-      <c r="G118" s="19">
-        <v>0</v>
-      </c>
-      <c r="H118" s="19">
-        <v>0</v>
-      </c>
-      <c r="I118" s="19">
-        <v>0</v>
-      </c>
-      <c r="J118" s="12">
-        <v>2</v>
-      </c>
-      <c r="K118" s="12">
-        <v>0</v>
-      </c>
-      <c r="L118" s="12">
-        <v>0</v>
-      </c>
-      <c r="M118" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N118" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O118" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P118" s="18"/>
-      <c r="Q118" s="18"/>
-    </row>
-    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B119" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C119" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D119" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E119" s="15">
-        <v>3</v>
-      </c>
-      <c r="F119" s="19">
-        <v>0</v>
-      </c>
-      <c r="G119" s="19">
-        <v>1</v>
-      </c>
-      <c r="H119" s="19">
-        <v>0</v>
-      </c>
-      <c r="I119" s="19">
-        <v>0</v>
-      </c>
-      <c r="J119" s="12">
-        <v>2</v>
-      </c>
-      <c r="K119" s="12">
-        <v>0</v>
-      </c>
-      <c r="L119" s="12">
-        <v>0</v>
-      </c>
-      <c r="M119" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N119" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O119" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N119" s="18"/>
+      <c r="O119" s="18"/>
       <c r="P119" s="18"/>
       <c r="Q119" s="18"/>
-    </row>
-    <row r="120" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A120" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B120" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C120" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D120" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E120" s="15">
-        <v>3</v>
-      </c>
-      <c r="F120" s="19">
-        <v>0</v>
-      </c>
-      <c r="G120" s="19">
-        <v>0</v>
-      </c>
-      <c r="H120" s="19">
-        <v>0</v>
-      </c>
-      <c r="I120" s="19">
-        <v>0</v>
-      </c>
-      <c r="J120" s="12">
-        <v>2</v>
-      </c>
-      <c r="K120" s="12">
-        <v>0</v>
-      </c>
-      <c r="L120" s="12">
-        <v>0</v>
-      </c>
-      <c r="M120" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N120" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O120" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P120" s="18"/>
-      <c r="Q120" s="18"/>
+      <c r="R119" s="18"/>
+      <c r="S119" s="18"/>
+      <c r="T119" s="18"/>
+      <c r="U119" s="18"/>
+      <c r="V119" s="18"/>
+      <c r="W119" s="18"/>
+      <c r="X119" s="18"/>
+      <c r="Y119" s="18"/>
+      <c r="Z119" s="18"/>
+      <c r="AA119" s="22"/>
+      <c r="AB119" s="22"/>
+      <c r="AC119" s="22"/>
+      <c r="AD119" s="22"/>
+      <c r="AE119" s="18"/>
+    </row>
+    <row r="120" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D120" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E120" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F120" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G120" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H120" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I120" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J120" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K120" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="L120" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="M120" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N120" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="O120" s="20" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="121" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A121" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D121" s="15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E121" s="15">
         <v>3</v>
@@ -14162,7 +14342,7 @@
         <v>0</v>
       </c>
       <c r="G121" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H121" s="19">
         <v>0</v>
@@ -14196,13 +14376,13 @@
         <v>2</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D122" s="15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E122" s="15">
         <v>3</v>
@@ -14211,7 +14391,7 @@
         <v>0</v>
       </c>
       <c r="G122" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H122" s="19">
         <v>0</v>
@@ -14245,13 +14425,13 @@
         <v>2</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C123" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D123" s="15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E123" s="15">
         <v>3</v>
@@ -14260,7 +14440,7 @@
         <v>0</v>
       </c>
       <c r="G123" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H123" s="19">
         <v>0</v>
@@ -14294,13 +14474,13 @@
         <v>2</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C124" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D124" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E124" s="15">
         <v>3</v>
@@ -14309,7 +14489,7 @@
         <v>0</v>
       </c>
       <c r="G124" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H124" s="19">
         <v>0</v>
@@ -14357,10 +14537,10 @@
         <v>2</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>30</v>
@@ -14406,10 +14586,10 @@
         <v>2</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D126" s="15" t="s">
         <v>23</v>
@@ -14455,10 +14635,10 @@
         <v>2</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D127" s="15" t="s">
         <v>26</v>
@@ -14504,27 +14684,27 @@
         <v>2</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D128" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E128" s="14">
-        <v>1</v>
-      </c>
-      <c r="F128" s="13">
-        <v>0</v>
-      </c>
-      <c r="G128" s="13">
-        <v>1</v>
-      </c>
-      <c r="H128" s="13">
-        <v>0</v>
-      </c>
-      <c r="I128" s="13">
+        <v>30</v>
+      </c>
+      <c r="E128" s="15">
+        <v>3</v>
+      </c>
+      <c r="F128" s="19">
+        <v>0</v>
+      </c>
+      <c r="G128" s="19">
+        <v>0</v>
+      </c>
+      <c r="H128" s="19">
+        <v>0</v>
+      </c>
+      <c r="I128" s="19">
         <v>0</v>
       </c>
       <c r="J128" s="12">
@@ -14545,146 +14725,215 @@
       <c r="O128" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P128" s="18"/>
+      <c r="Q128" s="18"/>
     </row>
     <row r="129" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N129" s="8"/>
-      <c r="O129" s="8"/>
-      <c r="P129" s="8"/>
-      <c r="Q129" s="8"/>
-      <c r="R129" s="8"/>
-      <c r="S129" s="8"/>
-      <c r="T129" s="8"/>
-      <c r="U129" s="8"/>
-      <c r="V129" s="8"/>
-      <c r="W129" s="8"/>
-      <c r="X129" s="8"/>
-      <c r="Y129" s="8"/>
-      <c r="Z129" s="8"/>
-      <c r="AA129" s="8"/>
-      <c r="AB129" s="8"/>
-      <c r="AC129" s="8"/>
-      <c r="AD129" s="8"/>
-      <c r="AE129" s="8"/>
-    </row>
-    <row r="130" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="131" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A131" s="9" t="s">
+      <c r="A129" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C129" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D129" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E129" s="15">
+        <v>3</v>
+      </c>
+      <c r="F129" s="19">
+        <v>0</v>
+      </c>
+      <c r="G129" s="19">
+        <v>1</v>
+      </c>
+      <c r="H129" s="19">
+        <v>0</v>
+      </c>
+      <c r="I129" s="19">
+        <v>0</v>
+      </c>
+      <c r="J129" s="12">
+        <v>2</v>
+      </c>
+      <c r="K129" s="12">
+        <v>0</v>
+      </c>
+      <c r="L129" s="12">
+        <v>0</v>
+      </c>
+      <c r="M129" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N129" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O129" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P129" s="18"/>
+      <c r="Q129" s="18"/>
+    </row>
+    <row r="130" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D130" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E130" s="15">
+        <v>3</v>
+      </c>
+      <c r="F130" s="19">
+        <v>0</v>
+      </c>
+      <c r="G130" s="19">
+        <v>2</v>
+      </c>
+      <c r="H130" s="19">
+        <v>0</v>
+      </c>
+      <c r="I130" s="19">
+        <v>0</v>
+      </c>
+      <c r="J130" s="12">
+        <v>2</v>
+      </c>
+      <c r="K130" s="12">
+        <v>0</v>
+      </c>
+      <c r="L130" s="12">
+        <v>0</v>
+      </c>
+      <c r="M130" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N130" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O130" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P130" s="18"/>
+      <c r="Q130" s="18"/>
+    </row>
+    <row r="131" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A131" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C131" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D131" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E131" s="14">
+        <v>1</v>
+      </c>
+      <c r="F131" s="13">
+        <v>0</v>
+      </c>
+      <c r="G131" s="13">
+        <v>1</v>
+      </c>
+      <c r="H131" s="13">
+        <v>0</v>
+      </c>
+      <c r="I131" s="13">
+        <v>0</v>
+      </c>
+      <c r="J131" s="12">
+        <v>2</v>
+      </c>
+      <c r="K131" s="12">
+        <v>0</v>
+      </c>
+      <c r="L131" s="12">
+        <v>0</v>
+      </c>
+      <c r="M131" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N131" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O131" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N132" s="8"/>
+      <c r="O132" s="8"/>
+      <c r="P132" s="8"/>
+      <c r="Q132" s="8"/>
+      <c r="R132" s="8"/>
+      <c r="S132" s="8"/>
+      <c r="T132" s="8"/>
+      <c r="U132" s="8"/>
+      <c r="V132" s="8"/>
+      <c r="W132" s="8"/>
+      <c r="X132" s="8"/>
+      <c r="Y132" s="8"/>
+      <c r="Z132" s="8"/>
+      <c r="AA132" s="8"/>
+      <c r="AB132" s="8"/>
+      <c r="AC132" s="8"/>
+      <c r="AD132" s="8"/>
+      <c r="AE132" s="8"/>
+    </row>
+    <row r="133" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="134" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A134" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B131" s="9"/>
-      <c r="C131" s="9"/>
-      <c r="D131" s="9"/>
-      <c r="E131" s="8"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
-      <c r="I131" s="8"/>
-      <c r="J131" s="8"/>
-      <c r="K131" s="8"/>
-      <c r="L131" s="8"/>
-    </row>
-    <row r="133" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="7" t="s">
+      <c r="B134" s="9"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="8"/>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
+      <c r="I134" s="8"/>
+      <c r="J134" s="8"/>
+      <c r="K134" s="8"/>
+      <c r="L134" s="8"/>
+    </row>
+    <row r="136" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A136" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B133" s="6" t="s">
+      <c r="B136" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C133" s="6" t="s">
+      <c r="C136" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D133" s="5" t="s">
+      <c r="D136" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E133" s="5" t="s">
+      <c r="E136" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F133" s="5" t="s">
+      <c r="F136" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G133" s="5" t="s">
+      <c r="G136" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H133" s="5" t="s">
+      <c r="H136" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="134" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A134" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D134" s="2">
-        <v>42</v>
-      </c>
-      <c r="E134" s="2">
-        <v>8</v>
-      </c>
-      <c r="F134" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G134" s="2">
-        <v>2</v>
-      </c>
-      <c r="H134" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A135" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D135" s="2">
-        <v>92</v>
-      </c>
-      <c r="E135" s="2">
-        <v>10</v>
-      </c>
-      <c r="F135" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G135" s="2">
-        <v>2</v>
-      </c>
-      <c r="H135" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A136" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D136" s="2">
-        <v>235</v>
-      </c>
-      <c r="E136" s="2">
-        <v>12</v>
-      </c>
-      <c r="F136" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="G136" s="2">
-        <v>2</v>
-      </c>
-      <c r="H136" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:31" x14ac:dyDescent="0.25">
@@ -14692,19 +14941,19 @@
         <v>2</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D137" s="2">
-        <v>686</v>
+        <v>42</v>
       </c>
       <c r="E137" s="2">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F137" s="2">
-        <v>0.7</v>
+        <v>1.3</v>
       </c>
       <c r="G137" s="2">
         <v>2</v>
@@ -14718,104 +14967,182 @@
         <v>2</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D138" s="2">
+        <v>92</v>
+      </c>
+      <c r="E138" s="2">
+        <v>10</v>
+      </c>
+      <c r="F138" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G138" s="2">
+        <v>2</v>
+      </c>
+      <c r="H138" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A139" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D139" s="2">
+        <v>235</v>
+      </c>
+      <c r="E139" s="2">
+        <v>12</v>
+      </c>
+      <c r="F139" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G139" s="2">
+        <v>2</v>
+      </c>
+      <c r="H139" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A140" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D140" s="2">
+        <v>686</v>
+      </c>
+      <c r="E140" s="2">
+        <v>14</v>
+      </c>
+      <c r="F140" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G140" s="2">
+        <v>2</v>
+      </c>
+      <c r="H140" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D141" s="2">
         <v>1040</v>
       </c>
-      <c r="E138" s="2">
+      <c r="E141" s="2">
         <v>14</v>
       </c>
-      <c r="F138" s="2">
+      <c r="F141" s="2">
         <v>0.5</v>
       </c>
-      <c r="G138" s="2">
-        <v>2</v>
-      </c>
-      <c r="H138" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D141" s="1">
-        <v>42</v>
-      </c>
-      <c r="F141" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G141">
-        <f>D134*F134</f>
-        <v>54.6</v>
-      </c>
-      <c r="I141">
-        <f>D141*F141</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="142" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D142" s="1">
-        <v>92</v>
-      </c>
-      <c r="F142" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G142">
-        <f>D135*F135</f>
-        <v>101.2</v>
-      </c>
-      <c r="I142">
-        <f>D142*F142</f>
-        <v>101.2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D143" s="1">
-        <v>235</v>
-      </c>
-      <c r="F143" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="G143">
-        <f>D136*F136</f>
-        <v>211.5</v>
-      </c>
-      <c r="I143">
-        <f>D143*F143</f>
-        <v>211.5</v>
+      <c r="G141" s="2">
+        <v>2</v>
+      </c>
+      <c r="H141" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D144" s="1">
-        <v>686</v>
+        <v>42</v>
       </c>
       <c r="F144" s="1">
-        <v>0.7</v>
+        <v>1.3</v>
       </c>
       <c r="G144">
         <f>D137*F137</f>
-        <v>480.2</v>
+        <v>54.6</v>
       </c>
       <c r="I144">
         <f>D144*F144</f>
-        <v>480.2</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="145" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D145" s="1">
-        <v>1040</v>
+        <v>92</v>
       </c>
       <c r="F145" s="1">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G145">
         <f>D138*F138</f>
-        <v>520</v>
+        <v>101.2</v>
       </c>
       <c r="I145">
         <f>D145*F145</f>
+        <v>101.2</v>
+      </c>
+    </row>
+    <row r="146" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D146" s="1">
+        <v>235</v>
+      </c>
+      <c r="F146" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G146">
+        <f>D139*F139</f>
+        <v>211.5</v>
+      </c>
+      <c r="I146">
+        <f>D146*F146</f>
+        <v>211.5</v>
+      </c>
+    </row>
+    <row r="147" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D147" s="1">
+        <v>686</v>
+      </c>
+      <c r="F147" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G147">
+        <f>D140*F140</f>
+        <v>480.2</v>
+      </c>
+      <c r="I147">
+        <f>D147*F147</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="148" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D148" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F148" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G148">
+        <f>D141*F141</f>
+        <v>520</v>
+      </c>
+      <c r="I148">
+        <f>D148*F148</f>
         <v>520</v>
       </c>
     </row>
@@ -14823,9 +15150,57 @@
   <mergeCells count="3">
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F119:G119"/>
   </mergeCells>
   <conditionalFormatting sqref="M97:P97">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M75:P77 M23:P24 M49:P59 M30:P47 M79:P84 M86:P87 M61:P70 M26:P27 M94:P97 M89:P92">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M71:P71">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M72:P72">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M48:P48">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -14837,19 +15212,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M75:P77 M23:P24 M49:P59 M30:P47 M79:P84 M86:P87 M61:P70 M26:P27 M94:P97 M89:P92">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M71:P71">
+  <conditionalFormatting sqref="M28:P28">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -14861,7 +15224,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M72:P72">
+  <conditionalFormatting sqref="M29:P29">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -14873,7 +15236,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M48:P48">
+  <conditionalFormatting sqref="M78:P78">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -14885,7 +15248,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:P28">
+  <conditionalFormatting sqref="M85:P85">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -14897,7 +15260,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M29:P29">
+  <conditionalFormatting sqref="M60:P60">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -14909,7 +15272,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M78:P78">
+  <conditionalFormatting sqref="M25:P25">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -14921,7 +15284,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M85:P85">
+  <conditionalFormatting sqref="M93:P93">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -14933,7 +15296,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M60:P60">
+  <conditionalFormatting sqref="M73:P73">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -14945,7 +15308,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25:P25">
+  <conditionalFormatting sqref="M74:P74">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -14957,7 +15320,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M93:P93">
+  <conditionalFormatting sqref="M98:P98">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -14969,7 +15332,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M73:P73">
+  <conditionalFormatting sqref="M99:P99">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -14981,7 +15344,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M74:P74">
+  <conditionalFormatting sqref="M100:P100">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -14993,7 +15356,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M98:P98">
+  <conditionalFormatting sqref="M101:P101">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -15005,7 +15368,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M99:P99">
+  <conditionalFormatting sqref="M102:P102">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -15017,7 +15380,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M100:P100">
+  <conditionalFormatting sqref="M103:P103">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -15029,7 +15392,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M101:P101">
+  <conditionalFormatting sqref="N104:P104">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -15041,7 +15404,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M102:P102">
+  <conditionalFormatting sqref="M105:P105">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -15053,7 +15416,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M103:P103">
+  <conditionalFormatting sqref="M104">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -15065,7 +15428,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N104:P104">
+  <conditionalFormatting sqref="O107">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -15077,7 +15440,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M105:P105">
+  <conditionalFormatting sqref="M107">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -15089,7 +15452,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M104">
+  <conditionalFormatting sqref="N107">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -15101,7 +15464,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O107">
+  <conditionalFormatting sqref="P107">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -15113,7 +15476,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M107">
+  <conditionalFormatting sqref="O108">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O108">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -15125,19 +15500,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N107">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P107">
+  <conditionalFormatting sqref="M108">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -15149,7 +15512,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108">
+  <conditionalFormatting sqref="N108">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -15161,7 +15524,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108">
+  <conditionalFormatting sqref="N108">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -15173,7 +15536,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M108">
+  <conditionalFormatting sqref="P108">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -15185,7 +15548,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N108">
+  <conditionalFormatting sqref="O109">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -15197,7 +15560,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N108">
+  <conditionalFormatting sqref="O109">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -15209,7 +15572,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P108">
+  <conditionalFormatting sqref="M109">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -15221,7 +15584,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109">
+  <conditionalFormatting sqref="N109">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -15233,7 +15596,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109">
+  <conditionalFormatting sqref="N109">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -15245,7 +15608,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M109">
+  <conditionalFormatting sqref="P109">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -15257,7 +15620,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N109">
+  <conditionalFormatting sqref="O110:P110">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M110">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -15269,8 +15644,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N109">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="N110">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15281,7 +15656,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P109">
+  <conditionalFormatting sqref="N110">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -15293,19 +15668,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O110:P110">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M110">
+  <conditionalFormatting sqref="M111:P111">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -15317,7 +15680,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N110">
+  <conditionalFormatting sqref="M112:P112">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O106">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -15329,19 +15704,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N110">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M111:P111">
+  <conditionalFormatting sqref="M106">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -15353,7 +15716,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M112:P112">
+  <conditionalFormatting sqref="N106">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -15365,7 +15728,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O106">
+  <conditionalFormatting sqref="P106">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -15377,7 +15740,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M106">
+  <conditionalFormatting sqref="M113:P113">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -15389,7 +15752,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N106">
+  <conditionalFormatting sqref="M88:P88">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -15401,19 +15764,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P106">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M113:P113">
+  <conditionalFormatting sqref="M114:P114">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -15425,8 +15776,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M88:P88">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="M115:P116">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15438,35 +15789,35 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="10">
-    <dataValidation type="list" sqref="O23:O113">
-      <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
+    <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G42"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I116">
+      <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K113">
+    <dataValidation type="decimal" allowBlank="1" sqref="D121:G131 P23:V116 M23:N116">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H121:L130 H131:I131 W23:Z116">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F113">
-      <formula1>0</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C121:C131 C23:C116">
+      <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="L23:L113">
-      <formula1>"true,false"</formula1>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="M121:O131 J131:L131 AA23:AA99 AA101:AA116 AB23:AE116"/>
+    <dataValidation type="list" sqref="O23:O116">
+      <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G42"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I113">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D118:G128 M23:N113 P23:V113">
-      <formula1>1</formula1>
-      <formula2>10</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H118:L127 H128:I128 W23:Z113">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K116">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C118:C128 C23:C113">
-      <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F116">
+      <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="M118:O128 J128:L128 AA101:AA113 AB23:AE113 AA23:AA99"/>
+    <dataValidation type="list" sqref="L23:L116">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Jellyfish01 and Jellyfish02 rows
Former-commit-id: 88de6dad40d0cb80c5b25c4cf9cbbd1f81fdfebc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$120:$O$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$122:$O$123</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="467">
   <si>
     <t>tier_4</t>
   </si>
@@ -1424,6 +1424,12 @@
   </si>
   <si>
     <t>HermitCrabBlueSmallTurret</t>
+  </si>
+  <si>
+    <t>Jellyfish01</t>
+  </si>
+  <si>
+    <t>Jellyfish02</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1933,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2439,49 +2445,70 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4757,8 +4784,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE116" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
-  <autoFilter ref="A22:AE116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE118" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+  <autoFilter ref="A22:AE118"/>
   <sortState ref="A23:AE109">
     <sortCondition ref="B22:B109"/>
   </sortState>
@@ -4814,8 +4841,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A120:O131" totalsRowShown="0">
-  <autoFilter ref="A120:O131"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A122:O133" totalsRowShown="0">
+  <autoFilter ref="A122:O133"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
@@ -5135,12 +5162,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AE148"/>
+  <dimension ref="A1:AE150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A116" sqref="A116"/>
+      <selection pane="topRight" activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5184,8 +5211,8 @@
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="193"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
       <c r="G3" s="23"/>
       <c r="H3" s="22"/>
       <c r="I3" s="172"/>
@@ -5341,8 +5368,8 @@
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
+      <c r="E21" s="207"/>
+      <c r="F21" s="207"/>
       <c r="G21" s="23"/>
       <c r="H21" s="22"/>
       <c r="I21" s="23"/>
@@ -13931,7 +13958,7 @@
       <c r="AE113" s="25"/>
     </row>
     <row r="114" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A114" s="195" t="s">
+      <c r="A114" s="194" t="s">
         <v>2</v>
       </c>
       <c r="B114" s="148" t="s">
@@ -13958,7 +13985,7 @@
       <c r="I114" s="119">
         <v>35</v>
       </c>
-      <c r="J114" s="196">
+      <c r="J114" s="195">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="K114" s="119">
@@ -13967,23 +13994,23 @@
       <c r="L114" s="150" t="b">
         <v>1</v>
       </c>
-      <c r="M114" s="197">
-        <v>5</v>
-      </c>
-      <c r="N114" s="197">
-        <v>5</v>
-      </c>
-      <c r="O114" s="198">
-        <v>2</v>
-      </c>
-      <c r="P114" s="197">
+      <c r="M114" s="196">
+        <v>5</v>
+      </c>
+      <c r="N114" s="196">
+        <v>5</v>
+      </c>
+      <c r="O114" s="197">
+        <v>2</v>
+      </c>
+      <c r="P114" s="196">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>2</v>
       </c>
       <c r="Q114" s="149" t="b">
         <v>1</v>
       </c>
-      <c r="R114" s="199" t="b">
+      <c r="R114" s="198" t="b">
         <v>0</v>
       </c>
       <c r="S114" s="149" t="b">
@@ -13992,7 +14019,7 @@
       <c r="T114" s="149">
         <v>1</v>
       </c>
-      <c r="U114" s="199">
+      <c r="U114" s="198">
         <v>2</v>
       </c>
       <c r="V114" s="149">
@@ -14023,7 +14050,7 @@
       <c r="AE114" s="124"/>
     </row>
     <row r="115" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A115" s="207" t="s">
+      <c r="A115" s="206" t="s">
         <v>2</v>
       </c>
       <c r="B115" s="88" t="s">
@@ -14032,7 +14059,7 @@
       <c r="C115" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="D115" s="194">
+      <c r="D115" s="193">
         <v>60</v>
       </c>
       <c r="E115" s="71">
@@ -14056,7 +14083,7 @@
       <c r="K115" s="71">
         <v>0</v>
       </c>
-      <c r="L115" s="200" t="b">
+      <c r="L115" s="199" t="b">
         <v>1</v>
       </c>
       <c r="M115" s="38">
@@ -14065,7 +14092,7 @@
       <c r="N115" s="38">
         <v>5</v>
       </c>
-      <c r="O115" s="201">
+      <c r="O115" s="200">
         <v>2</v>
       </c>
       <c r="P115" s="38">
@@ -14075,19 +14102,19 @@
       <c r="Q115" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="R115" s="202" t="b">
-        <v>0</v>
-      </c>
-      <c r="S115" s="202" t="b">
-        <v>0</v>
-      </c>
-      <c r="T115" s="203">
-        <v>1</v>
-      </c>
-      <c r="U115" s="204">
-        <v>2</v>
-      </c>
-      <c r="V115" s="205">
+      <c r="R115" s="201" t="b">
+        <v>0</v>
+      </c>
+      <c r="S115" s="201" t="b">
+        <v>0</v>
+      </c>
+      <c r="T115" s="202">
+        <v>1</v>
+      </c>
+      <c r="U115" s="203">
+        <v>2</v>
+      </c>
+      <c r="V115" s="204">
         <v>0</v>
       </c>
       <c r="W115" s="31">
@@ -14102,7 +14129,7 @@
       <c r="Z115" s="29">
         <v>0</v>
       </c>
-      <c r="AA115" s="206" t="s">
+      <c r="AA115" s="205" t="s">
         <v>144</v>
       </c>
       <c r="AB115" s="27" t="s">
@@ -14115,7 +14142,7 @@
       <c r="AE115" s="25"/>
     </row>
     <row r="116" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A116" s="207" t="s">
+      <c r="A116" s="206" t="s">
         <v>2</v>
       </c>
       <c r="B116" s="88" t="s">
@@ -14124,7 +14151,7 @@
       <c r="C116" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="D116" s="194">
+      <c r="D116" s="193">
         <v>60</v>
       </c>
       <c r="E116" s="71">
@@ -14148,7 +14175,7 @@
       <c r="K116" s="71">
         <v>0</v>
       </c>
-      <c r="L116" s="200" t="b">
+      <c r="L116" s="199" t="b">
         <v>1</v>
       </c>
       <c r="M116" s="38">
@@ -14157,7 +14184,7 @@
       <c r="N116" s="38">
         <v>5</v>
       </c>
-      <c r="O116" s="201">
+      <c r="O116" s="200">
         <v>2</v>
       </c>
       <c r="P116" s="38">
@@ -14167,19 +14194,19 @@
       <c r="Q116" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="R116" s="202" t="b">
-        <v>0</v>
-      </c>
-      <c r="S116" s="202" t="b">
-        <v>0</v>
-      </c>
-      <c r="T116" s="203">
-        <v>1</v>
-      </c>
-      <c r="U116" s="204">
-        <v>2</v>
-      </c>
-      <c r="V116" s="205">
+      <c r="R116" s="201" t="b">
+        <v>0</v>
+      </c>
+      <c r="S116" s="201" t="b">
+        <v>0</v>
+      </c>
+      <c r="T116" s="202">
+        <v>1</v>
+      </c>
+      <c r="U116" s="203">
+        <v>2</v>
+      </c>
+      <c r="V116" s="204">
         <v>0</v>
       </c>
       <c r="W116" s="31">
@@ -14194,7 +14221,7 @@
       <c r="Z116" s="29">
         <v>0</v>
       </c>
-      <c r="AA116" s="206" t="s">
+      <c r="AA116" s="205" t="s">
         <v>144</v>
       </c>
       <c r="AB116" s="27" t="s">
@@ -14206,229 +14233,323 @@
       <c r="AD116" s="26"/>
       <c r="AE116" s="25"/>
     </row>
-    <row r="117" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A118" s="9" t="s">
+    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A117" s="206" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="88" t="s">
+        <v>465</v>
+      </c>
+      <c r="C117" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D117" s="193">
+        <v>220</v>
+      </c>
+      <c r="E117" s="71">
+        <v>21</v>
+      </c>
+      <c r="F117" s="71">
+        <v>0</v>
+      </c>
+      <c r="G117" s="71">
+        <v>3</v>
+      </c>
+      <c r="H117" s="71">
+        <v>0</v>
+      </c>
+      <c r="I117" s="71">
+        <v>95</v>
+      </c>
+      <c r="J117" s="208">
+        <v>0.15</v>
+      </c>
+      <c r="K117" s="71">
+        <v>0</v>
+      </c>
+      <c r="L117" s="199" t="b">
+        <v>1</v>
+      </c>
+      <c r="M117" s="209">
+        <v>5</v>
+      </c>
+      <c r="N117" s="209">
+        <v>5</v>
+      </c>
+      <c r="O117" s="200">
+        <v>3</v>
+      </c>
+      <c r="P117" s="209">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>3</v>
+      </c>
+      <c r="Q117" s="210" t="b">
+        <v>1</v>
+      </c>
+      <c r="R117" s="211" t="b">
+        <v>0</v>
+      </c>
+      <c r="S117" s="211" t="b">
+        <v>0</v>
+      </c>
+      <c r="T117" s="212">
+        <v>1</v>
+      </c>
+      <c r="U117" s="203">
+        <v>1</v>
+      </c>
+      <c r="V117" s="204">
+        <v>0</v>
+      </c>
+      <c r="W117" s="213">
+        <v>0.25</v>
+      </c>
+      <c r="X117" s="214">
+        <v>0.25</v>
+      </c>
+      <c r="Y117" s="214">
+        <v>0</v>
+      </c>
+      <c r="Z117" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA117" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB117" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC117" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD117" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE117" s="25" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="118" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A118" s="206" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="88" t="s">
+        <v>466</v>
+      </c>
+      <c r="C118" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D118" s="193">
+        <v>220</v>
+      </c>
+      <c r="E118" s="71">
+        <v>21</v>
+      </c>
+      <c r="F118" s="71">
+        <v>0</v>
+      </c>
+      <c r="G118" s="71">
+        <v>3</v>
+      </c>
+      <c r="H118" s="71">
+        <v>0</v>
+      </c>
+      <c r="I118" s="71">
+        <v>95</v>
+      </c>
+      <c r="J118" s="208">
+        <v>0.15</v>
+      </c>
+      <c r="K118" s="71">
+        <v>0</v>
+      </c>
+      <c r="L118" s="199" t="b">
+        <v>1</v>
+      </c>
+      <c r="M118" s="209">
+        <v>5</v>
+      </c>
+      <c r="N118" s="209">
+        <v>5</v>
+      </c>
+      <c r="O118" s="200">
+        <v>3</v>
+      </c>
+      <c r="P118" s="209">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>3</v>
+      </c>
+      <c r="Q118" s="210" t="b">
+        <v>1</v>
+      </c>
+      <c r="R118" s="211" t="b">
+        <v>0</v>
+      </c>
+      <c r="S118" s="211" t="b">
+        <v>0</v>
+      </c>
+      <c r="T118" s="212">
+        <v>1</v>
+      </c>
+      <c r="U118" s="203">
+        <v>1</v>
+      </c>
+      <c r="V118" s="204">
+        <v>0</v>
+      </c>
+      <c r="W118" s="213">
+        <v>0.25</v>
+      </c>
+      <c r="X118" s="214">
+        <v>0.25</v>
+      </c>
+      <c r="Y118" s="214">
+        <v>0</v>
+      </c>
+      <c r="Z118" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA118" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB118" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC118" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD118" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE118" s="25" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="119" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A120" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B118" s="9"/>
-      <c r="C118" s="9"/>
-      <c r="D118" s="9"/>
-      <c r="E118" s="9"/>
-      <c r="F118" s="9"/>
-      <c r="G118" s="9"/>
-      <c r="H118" s="9"/>
-      <c r="I118" s="9"/>
-      <c r="J118" s="9"/>
-      <c r="K118" s="9"/>
-      <c r="L118" s="9"/>
-      <c r="M118" s="9"/>
-      <c r="N118" s="9"/>
-      <c r="O118" s="9"/>
-      <c r="P118" s="9"/>
-      <c r="Q118" s="9"/>
-      <c r="R118" s="9"/>
-      <c r="S118" s="9"/>
-      <c r="T118" s="9"/>
-      <c r="U118" s="9"/>
-      <c r="V118" s="9"/>
-      <c r="W118" s="9"/>
-      <c r="X118" s="9"/>
-      <c r="Y118" s="9"/>
-      <c r="Z118" s="9"/>
-      <c r="AA118" s="9"/>
-    </row>
-    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A119" s="23"/>
-      <c r="B119" s="23"/>
-      <c r="C119" s="23"/>
-      <c r="D119" s="23"/>
-      <c r="E119" s="23"/>
-      <c r="F119" s="193"/>
-      <c r="G119" s="193"/>
-      <c r="H119" s="22" t="s">
+      <c r="B120" s="9"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="9"/>
+      <c r="K120" s="9"/>
+      <c r="L120" s="9"/>
+      <c r="M120" s="9"/>
+      <c r="N120" s="9"/>
+      <c r="O120" s="9"/>
+      <c r="P120" s="9"/>
+      <c r="Q120" s="9"/>
+      <c r="R120" s="9"/>
+      <c r="S120" s="9"/>
+      <c r="T120" s="9"/>
+      <c r="U120" s="9"/>
+      <c r="V120" s="9"/>
+      <c r="W120" s="9"/>
+      <c r="X120" s="9"/>
+      <c r="Y120" s="9"/>
+      <c r="Z120" s="9"/>
+      <c r="AA120" s="9"/>
+    </row>
+    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A121" s="23"/>
+      <c r="B121" s="23"/>
+      <c r="C121" s="23"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23"/>
+      <c r="F121" s="207"/>
+      <c r="G121" s="207"/>
+      <c r="H121" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I119" s="22"/>
-      <c r="J119" s="23"/>
-      <c r="K119" s="18"/>
-      <c r="L119" s="18"/>
-      <c r="M119" s="18" t="s">
+      <c r="I121" s="22"/>
+      <c r="J121" s="23"/>
+      <c r="K121" s="18"/>
+      <c r="L121" s="18"/>
+      <c r="M121" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="N119" s="18"/>
-      <c r="O119" s="18"/>
-      <c r="P119" s="18"/>
-      <c r="Q119" s="18"/>
-      <c r="R119" s="18"/>
-      <c r="S119" s="18"/>
-      <c r="T119" s="18"/>
-      <c r="U119" s="18"/>
-      <c r="V119" s="18"/>
-      <c r="W119" s="18"/>
-      <c r="X119" s="18"/>
-      <c r="Y119" s="18"/>
-      <c r="Z119" s="18"/>
-      <c r="AA119" s="22"/>
-      <c r="AB119" s="22"/>
-      <c r="AC119" s="22"/>
-      <c r="AD119" s="22"/>
-      <c r="AE119" s="18"/>
-    </row>
-    <row r="120" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D120" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E120" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F120" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="G120" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H120" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="I120" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="J120" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K120" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L120" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M120" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N120" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="O120" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A121" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B121" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C121" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D121" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E121" s="15">
-        <v>3</v>
-      </c>
-      <c r="F121" s="19">
-        <v>0</v>
-      </c>
-      <c r="G121" s="19">
-        <v>0</v>
-      </c>
-      <c r="H121" s="19">
-        <v>0</v>
-      </c>
-      <c r="I121" s="19">
-        <v>0</v>
-      </c>
-      <c r="J121" s="12">
-        <v>2</v>
-      </c>
-      <c r="K121" s="12">
-        <v>0</v>
-      </c>
-      <c r="L121" s="12">
-        <v>0</v>
-      </c>
-      <c r="M121" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N121" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O121" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N121" s="18"/>
+      <c r="O121" s="18"/>
       <c r="P121" s="18"/>
       <c r="Q121" s="18"/>
-    </row>
-    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A122" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B122" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C122" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D122" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E122" s="15">
-        <v>3</v>
-      </c>
-      <c r="F122" s="19">
-        <v>0</v>
-      </c>
-      <c r="G122" s="19">
-        <v>1</v>
-      </c>
-      <c r="H122" s="19">
-        <v>0</v>
-      </c>
-      <c r="I122" s="19">
-        <v>0</v>
-      </c>
-      <c r="J122" s="12">
-        <v>2</v>
-      </c>
-      <c r="K122" s="12">
-        <v>0</v>
-      </c>
-      <c r="L122" s="12">
-        <v>0</v>
-      </c>
-      <c r="M122" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N122" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O122" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P122" s="18"/>
-      <c r="Q122" s="18"/>
+      <c r="R121" s="18"/>
+      <c r="S121" s="18"/>
+      <c r="T121" s="18"/>
+      <c r="U121" s="18"/>
+      <c r="V121" s="18"/>
+      <c r="W121" s="18"/>
+      <c r="X121" s="18"/>
+      <c r="Y121" s="18"/>
+      <c r="Z121" s="18"/>
+      <c r="AA121" s="22"/>
+      <c r="AB121" s="22"/>
+      <c r="AC121" s="22"/>
+      <c r="AD121" s="22"/>
+      <c r="AE121" s="18"/>
+    </row>
+    <row r="122" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D122" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E122" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F122" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G122" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H122" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I122" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J122" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K122" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="L122" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="M122" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N122" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="O122" s="20" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="123" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C123" s="16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D123" s="15" t="s">
         <v>30</v>
@@ -14469,15 +14590,15 @@
       <c r="P123" s="18"/>
       <c r="Q123" s="18"/>
     </row>
-    <row r="124" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A124" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C124" s="16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D124" s="15" t="s">
         <v>23</v>
@@ -14517,30 +14638,16 @@
       </c>
       <c r="P124" s="18"/>
       <c r="Q124" s="18"/>
-      <c r="R124"/>
-      <c r="S124"/>
-      <c r="T124"/>
-      <c r="U124"/>
-      <c r="V124"/>
-      <c r="W124"/>
-      <c r="X124"/>
-      <c r="Y124"/>
-      <c r="Z124"/>
-      <c r="AA124"/>
-      <c r="AB124"/>
-      <c r="AC124"/>
-      <c r="AD124"/>
-      <c r="AE124"/>
     </row>
     <row r="125" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>30</v>
@@ -14581,15 +14688,15 @@
       <c r="P125" s="18"/>
       <c r="Q125" s="18"/>
     </row>
-    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D126" s="15" t="s">
         <v>23</v>
@@ -14629,19 +14736,33 @@
       </c>
       <c r="P126" s="18"/>
       <c r="Q126" s="18"/>
+      <c r="R126"/>
+      <c r="S126"/>
+      <c r="T126"/>
+      <c r="U126"/>
+      <c r="V126"/>
+      <c r="W126"/>
+      <c r="X126"/>
+      <c r="Y126"/>
+      <c r="Z126"/>
+      <c r="AA126"/>
+      <c r="AB126"/>
+      <c r="AC126"/>
+      <c r="AD126"/>
+      <c r="AE126"/>
     </row>
     <row r="127" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A127" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C127" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D127" s="15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E127" s="15">
         <v>3</v>
@@ -14650,7 +14771,7 @@
         <v>0</v>
       </c>
       <c r="G127" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H127" s="19">
         <v>0</v>
@@ -14684,13 +14805,13 @@
         <v>2</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D128" s="15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E128" s="15">
         <v>3</v>
@@ -14699,7 +14820,7 @@
         <v>0</v>
       </c>
       <c r="G128" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H128" s="19">
         <v>0</v>
@@ -14733,13 +14854,13 @@
         <v>2</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C129" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D129" s="15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E129" s="15">
         <v>3</v>
@@ -14748,7 +14869,7 @@
         <v>0</v>
       </c>
       <c r="G129" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H129" s="19">
         <v>0</v>
@@ -14782,13 +14903,13 @@
         <v>2</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C130" s="16" t="s">
         <v>27</v>
       </c>
       <c r="D130" s="15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E130" s="15">
         <v>3</v>
@@ -14797,7 +14918,7 @@
         <v>0</v>
       </c>
       <c r="G130" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H130" s="19">
         <v>0</v>
@@ -14831,27 +14952,27 @@
         <v>2</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D131" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E131" s="14">
-        <v>1</v>
-      </c>
-      <c r="F131" s="13">
-        <v>0</v>
-      </c>
-      <c r="G131" s="13">
-        <v>1</v>
-      </c>
-      <c r="H131" s="13">
-        <v>0</v>
-      </c>
-      <c r="I131" s="13">
+      <c r="E131" s="15">
+        <v>3</v>
+      </c>
+      <c r="F131" s="19">
+        <v>0</v>
+      </c>
+      <c r="G131" s="19">
+        <v>1</v>
+      </c>
+      <c r="H131" s="19">
+        <v>0</v>
+      </c>
+      <c r="I131" s="19">
         <v>0</v>
       </c>
       <c r="J131" s="12">
@@ -14872,120 +14993,166 @@
       <c r="O131" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P131" s="18"/>
+      <c r="Q131" s="18"/>
     </row>
     <row r="132" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N132" s="8"/>
-      <c r="O132" s="8"/>
-      <c r="P132" s="8"/>
-      <c r="Q132" s="8"/>
-      <c r="R132" s="8"/>
-      <c r="S132" s="8"/>
-      <c r="T132" s="8"/>
-      <c r="U132" s="8"/>
-      <c r="V132" s="8"/>
-      <c r="W132" s="8"/>
-      <c r="X132" s="8"/>
-      <c r="Y132" s="8"/>
-      <c r="Z132" s="8"/>
-      <c r="AA132" s="8"/>
-      <c r="AB132" s="8"/>
-      <c r="AC132" s="8"/>
-      <c r="AD132" s="8"/>
-      <c r="AE132" s="8"/>
-    </row>
-    <row r="133" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="134" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A134" s="9" t="s">
+      <c r="A132" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C132" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D132" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E132" s="15">
+        <v>3</v>
+      </c>
+      <c r="F132" s="19">
+        <v>0</v>
+      </c>
+      <c r="G132" s="19">
+        <v>2</v>
+      </c>
+      <c r="H132" s="19">
+        <v>0</v>
+      </c>
+      <c r="I132" s="19">
+        <v>0</v>
+      </c>
+      <c r="J132" s="12">
+        <v>2</v>
+      </c>
+      <c r="K132" s="12">
+        <v>0</v>
+      </c>
+      <c r="L132" s="12">
+        <v>0</v>
+      </c>
+      <c r="M132" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N132" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O132" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P132" s="18"/>
+      <c r="Q132" s="18"/>
+    </row>
+    <row r="133" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A133" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B133" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C133" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D133" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E133" s="14">
+        <v>1</v>
+      </c>
+      <c r="F133" s="13">
+        <v>0</v>
+      </c>
+      <c r="G133" s="13">
+        <v>1</v>
+      </c>
+      <c r="H133" s="13">
+        <v>0</v>
+      </c>
+      <c r="I133" s="13">
+        <v>0</v>
+      </c>
+      <c r="J133" s="12">
+        <v>2</v>
+      </c>
+      <c r="K133" s="12">
+        <v>0</v>
+      </c>
+      <c r="L133" s="12">
+        <v>0</v>
+      </c>
+      <c r="M133" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N133" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O133" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N134" s="8"/>
+      <c r="O134" s="8"/>
+      <c r="P134" s="8"/>
+      <c r="Q134" s="8"/>
+      <c r="R134" s="8"/>
+      <c r="S134" s="8"/>
+      <c r="T134" s="8"/>
+      <c r="U134" s="8"/>
+      <c r="V134" s="8"/>
+      <c r="W134" s="8"/>
+      <c r="X134" s="8"/>
+      <c r="Y134" s="8"/>
+      <c r="Z134" s="8"/>
+      <c r="AA134" s="8"/>
+      <c r="AB134" s="8"/>
+      <c r="AC134" s="8"/>
+      <c r="AD134" s="8"/>
+      <c r="AE134" s="8"/>
+    </row>
+    <row r="135" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="136" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A136" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B134" s="9"/>
-      <c r="C134" s="9"/>
-      <c r="D134" s="9"/>
-      <c r="E134" s="8"/>
-      <c r="F134" s="8"/>
-      <c r="G134" s="8"/>
-      <c r="H134" s="8"/>
-      <c r="I134" s="8"/>
-      <c r="J134" s="8"/>
-      <c r="K134" s="8"/>
-      <c r="L134" s="8"/>
-    </row>
-    <row r="136" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="7" t="s">
+      <c r="B136" s="9"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="8"/>
+      <c r="F136" s="8"/>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
+      <c r="I136" s="8"/>
+      <c r="J136" s="8"/>
+      <c r="K136" s="8"/>
+      <c r="L136" s="8"/>
+    </row>
+    <row r="138" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A138" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="B138" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C138" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D136" s="5" t="s">
+      <c r="D138" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E136" s="5" t="s">
+      <c r="E138" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F136" s="5" t="s">
+      <c r="F138" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G136" s="5" t="s">
+      <c r="G138" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H136" s="5" t="s">
+      <c r="H138" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="137" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A137" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D137" s="2">
-        <v>42</v>
-      </c>
-      <c r="E137" s="2">
-        <v>8</v>
-      </c>
-      <c r="F137" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G137" s="2">
-        <v>2</v>
-      </c>
-      <c r="H137" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A138" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D138" s="2">
-        <v>92</v>
-      </c>
-      <c r="E138" s="2">
-        <v>10</v>
-      </c>
-      <c r="F138" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G138" s="2">
-        <v>2</v>
-      </c>
-      <c r="H138" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:31" x14ac:dyDescent="0.25">
@@ -14993,19 +15160,19 @@
         <v>2</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D139" s="2">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="E139" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F139" s="2">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="G139" s="2">
         <v>2</v>
@@ -15019,19 +15186,19 @@
         <v>2</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D140" s="2">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="E140" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F140" s="2">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G140" s="2">
         <v>2</v>
@@ -15045,104 +15212,156 @@
         <v>2</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D141" s="2">
+        <v>235</v>
+      </c>
+      <c r="E141" s="2">
+        <v>12</v>
+      </c>
+      <c r="F141" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G141" s="2">
+        <v>2</v>
+      </c>
+      <c r="H141" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D142" s="2">
+        <v>686</v>
+      </c>
+      <c r="E142" s="2">
+        <v>14</v>
+      </c>
+      <c r="F142" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G142" s="2">
+        <v>2</v>
+      </c>
+      <c r="H142" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D143" s="2">
         <v>1040</v>
       </c>
-      <c r="E141" s="2">
+      <c r="E143" s="2">
         <v>14</v>
       </c>
-      <c r="F141" s="2">
+      <c r="F143" s="2">
         <v>0.5</v>
       </c>
-      <c r="G141" s="2">
-        <v>2</v>
-      </c>
-      <c r="H141" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D144" s="1">
-        <v>42</v>
-      </c>
-      <c r="F144" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G144">
-        <f>D137*F137</f>
-        <v>54.6</v>
-      </c>
-      <c r="I144">
-        <f>D144*F144</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="145" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D145" s="1">
-        <v>92</v>
-      </c>
-      <c r="F145" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G145">
-        <f>D138*F138</f>
-        <v>101.2</v>
-      </c>
-      <c r="I145">
-        <f>D145*F145</f>
-        <v>101.2</v>
+      <c r="G143" s="2">
+        <v>2</v>
+      </c>
+      <c r="H143" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D146" s="1">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="F146" s="1">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="G146">
         <f>D139*F139</f>
-        <v>211.5</v>
+        <v>54.6</v>
       </c>
       <c r="I146">
         <f>D146*F146</f>
-        <v>211.5</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="147" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D147" s="1">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="F147" s="1">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G147">
         <f>D140*F140</f>
-        <v>480.2</v>
+        <v>101.2</v>
       </c>
       <c r="I147">
         <f>D147*F147</f>
-        <v>480.2</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="148" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D148" s="1">
-        <v>1040</v>
+        <v>235</v>
       </c>
       <c r="F148" s="1">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G148">
         <f>D141*F141</f>
-        <v>520</v>
+        <v>211.5</v>
       </c>
       <c r="I148">
         <f>D148*F148</f>
+        <v>211.5</v>
+      </c>
+    </row>
+    <row r="149" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D149" s="1">
+        <v>686</v>
+      </c>
+      <c r="F149" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G149">
+        <f>D142*F142</f>
+        <v>480.2</v>
+      </c>
+      <c r="I149">
+        <f>D149*F149</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="150" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D150" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F150" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G150">
+        <f>D143*F143</f>
+        <v>520</v>
+      </c>
+      <c r="I150">
+        <f>D150*F150</f>
         <v>520</v>
       </c>
     </row>
@@ -15150,9 +15369,45 @@
   <mergeCells count="3">
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F119:G119"/>
+    <mergeCell ref="F121:G121"/>
   </mergeCells>
   <conditionalFormatting sqref="M97:P97">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M75:P77 M23:P24 M49:P59 M30:P47 M79:P84 M86:P87 M61:P70 M26:P27 M94:P97 M89:P92">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M71:P71">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M72:P72">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -15164,19 +15419,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M75:P77 M23:P24 M49:P59 M30:P47 M79:P84 M86:P87 M61:P70 M26:P27 M94:P97 M89:P92">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M71:P71">
+  <conditionalFormatting sqref="M48:P48">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -15188,7 +15431,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M72:P72">
+  <conditionalFormatting sqref="M28:P28">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -15200,7 +15443,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M48:P48">
+  <conditionalFormatting sqref="M29:P29">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -15212,7 +15455,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:P28">
+  <conditionalFormatting sqref="M78:P78">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -15224,7 +15467,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M29:P29">
+  <conditionalFormatting sqref="M85:P85">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -15236,7 +15479,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M78:P78">
+  <conditionalFormatting sqref="M60:P60">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -15248,7 +15491,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M85:P85">
+  <conditionalFormatting sqref="M25:P25">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -15260,7 +15503,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M60:P60">
+  <conditionalFormatting sqref="M93:P93">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -15272,7 +15515,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25:P25">
+  <conditionalFormatting sqref="M73:P73">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -15284,7 +15527,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M93:P93">
+  <conditionalFormatting sqref="M74:P74">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -15296,7 +15539,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M73:P73">
+  <conditionalFormatting sqref="M98:P98">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -15308,7 +15551,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M74:P74">
+  <conditionalFormatting sqref="M99:P99">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -15320,7 +15563,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M98:P98">
+  <conditionalFormatting sqref="M100:P100">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -15332,7 +15575,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M99:P99">
+  <conditionalFormatting sqref="M101:P101">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -15344,7 +15587,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M100:P100">
+  <conditionalFormatting sqref="M102:P102">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -15356,7 +15599,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M101:P101">
+  <conditionalFormatting sqref="M103:P103">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -15368,7 +15611,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M102:P102">
+  <conditionalFormatting sqref="N104:P104">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -15380,7 +15623,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M103:P103">
+  <conditionalFormatting sqref="M105:P105">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -15392,7 +15635,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N104:P104">
+  <conditionalFormatting sqref="M104">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -15404,7 +15647,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M105:P105">
+  <conditionalFormatting sqref="O107">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -15416,7 +15659,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M104">
+  <conditionalFormatting sqref="M107">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -15428,7 +15671,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O107">
+  <conditionalFormatting sqref="N107">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -15440,7 +15683,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M107">
+  <conditionalFormatting sqref="P107">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -15452,19 +15695,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N107">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P107">
+  <conditionalFormatting sqref="O108">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -15477,7 +15708,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15488,7 +15719,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108">
+  <conditionalFormatting sqref="M108">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -15500,7 +15731,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M108">
+  <conditionalFormatting sqref="N108">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -15513,7 +15744,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N108">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15524,7 +15755,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N108">
+  <conditionalFormatting sqref="P108">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -15536,7 +15767,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P108">
+  <conditionalFormatting sqref="O109">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -15549,7 +15780,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15560,7 +15791,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109">
+  <conditionalFormatting sqref="M109">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -15572,7 +15803,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M109">
+  <conditionalFormatting sqref="N109">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -15585,6 +15816,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N109">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P109">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O110:P110">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -15596,19 +15851,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N109">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P109">
+  <conditionalFormatting sqref="M110">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -15620,19 +15863,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O110:P110">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M110">
+  <conditionalFormatting sqref="N110">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -15645,6 +15876,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N110">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M111:P111">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M112:P112">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -15656,19 +15911,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N110">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M111:P111">
+  <conditionalFormatting sqref="O106">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -15680,7 +15923,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M112:P112">
+  <conditionalFormatting sqref="M106">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -15692,7 +15935,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O106">
+  <conditionalFormatting sqref="N106">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -15704,7 +15947,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M106">
+  <conditionalFormatting sqref="P106">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -15716,7 +15959,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N106">
+  <conditionalFormatting sqref="M113:P113">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -15728,7 +15971,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P106">
+  <conditionalFormatting sqref="M88:P88">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -15740,19 +15983,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M113:P113">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M88:P88">
+  <conditionalFormatting sqref="M114:P114">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -15764,7 +15995,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M114:P114">
+  <conditionalFormatting sqref="M115:P116">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M117:P117">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -15776,8 +16019,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M115:P116">
-    <cfRule type="colorScale" priority="56">
+  <conditionalFormatting sqref="M118:P118">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15790,32 +16033,32 @@
   </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G42"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I116">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I118">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D121:G131 P23:V116 M23:N116">
+    <dataValidation type="decimal" allowBlank="1" sqref="D123:G133 P23:V118 M23:N118">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H121:L130 H131:I131 W23:Z116">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H123:L132 H133:I133 W23:Z118">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C121:C131 C23:C116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C123:C133 C23:C118">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="M121:O131 J131:L131 AA23:AA99 AA101:AA116 AB23:AE116"/>
-    <dataValidation type="list" sqref="O23:O116">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="M123:O133 J133:L133 AA23:AA99 AA101:AA118 AB23:AE118"/>
+    <dataValidation type="list" sqref="O23:O118">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K116">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K118">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F116">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F118">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="L23:L116">
+    <dataValidation type="list" sqref="L23:L118">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15870,8 +16113,8 @@
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
       <c r="H3" s="23"/>
       <c r="I3" s="22"/>
       <c r="J3" s="172"/>

</xml_diff>

<commit_message>
Fixing conflict with 1.3
Former-commit-id: e260aae742d3e97243366cd18281da8260d8b474
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -2487,29 +2487,29 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5164,10 +5164,10 @@
   </sheetPr>
   <dimension ref="A1:AE150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A117" sqref="A117"/>
+      <selection pane="topRight" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5211,8 +5211,8 @@
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
+      <c r="E3" s="214"/>
+      <c r="F3" s="214"/>
       <c r="G3" s="23"/>
       <c r="H3" s="22"/>
       <c r="I3" s="172"/>
@@ -5368,8 +5368,8 @@
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="207"/>
-      <c r="F21" s="207"/>
+      <c r="E21" s="214"/>
+      <c r="F21" s="214"/>
       <c r="G21" s="23"/>
       <c r="H21" s="22"/>
       <c r="I21" s="23"/>
@@ -5780,7 +5780,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="131">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" s="131">
         <v>0</v>
@@ -9413,7 +9413,7 @@
         <v>20</v>
       </c>
       <c r="E65" s="107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" s="107">
         <v>0</v>
@@ -14261,7 +14261,7 @@
       <c r="I117" s="71">
         <v>95</v>
       </c>
-      <c r="J117" s="208">
+      <c r="J117" s="207">
         <v>0.15</v>
       </c>
       <c r="K117" s="71">
@@ -14270,29 +14270,29 @@
       <c r="L117" s="199" t="b">
         <v>1</v>
       </c>
-      <c r="M117" s="209">
-        <v>5</v>
-      </c>
-      <c r="N117" s="209">
+      <c r="M117" s="208">
+        <v>5</v>
+      </c>
+      <c r="N117" s="208">
         <v>5</v>
       </c>
       <c r="O117" s="200">
         <v>3</v>
       </c>
-      <c r="P117" s="209">
+      <c r="P117" s="208">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>3</v>
       </c>
-      <c r="Q117" s="210" t="b">
-        <v>1</v>
-      </c>
-      <c r="R117" s="211" t="b">
-        <v>0</v>
-      </c>
-      <c r="S117" s="211" t="b">
-        <v>0</v>
-      </c>
-      <c r="T117" s="212">
+      <c r="Q117" s="209" t="b">
+        <v>1</v>
+      </c>
+      <c r="R117" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="S117" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="T117" s="211">
         <v>1</v>
       </c>
       <c r="U117" s="203">
@@ -14301,13 +14301,13 @@
       <c r="V117" s="204">
         <v>0</v>
       </c>
-      <c r="W117" s="213">
+      <c r="W117" s="212">
         <v>0.25</v>
       </c>
-      <c r="X117" s="214">
+      <c r="X117" s="213">
         <v>0.25</v>
       </c>
-      <c r="Y117" s="214">
+      <c r="Y117" s="213">
         <v>0</v>
       </c>
       <c r="Z117" s="29">
@@ -14357,7 +14357,7 @@
       <c r="I118" s="71">
         <v>95</v>
       </c>
-      <c r="J118" s="208">
+      <c r="J118" s="207">
         <v>0.15</v>
       </c>
       <c r="K118" s="71">
@@ -14366,29 +14366,29 @@
       <c r="L118" s="199" t="b">
         <v>1</v>
       </c>
-      <c r="M118" s="209">
-        <v>5</v>
-      </c>
-      <c r="N118" s="209">
+      <c r="M118" s="208">
+        <v>5</v>
+      </c>
+      <c r="N118" s="208">
         <v>5</v>
       </c>
       <c r="O118" s="200">
         <v>3</v>
       </c>
-      <c r="P118" s="209">
+      <c r="P118" s="208">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>3</v>
       </c>
-      <c r="Q118" s="210" t="b">
-        <v>1</v>
-      </c>
-      <c r="R118" s="211" t="b">
-        <v>0</v>
-      </c>
-      <c r="S118" s="211" t="b">
-        <v>0</v>
-      </c>
-      <c r="T118" s="212">
+      <c r="Q118" s="209" t="b">
+        <v>1</v>
+      </c>
+      <c r="R118" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="S118" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="T118" s="211">
         <v>1</v>
       </c>
       <c r="U118" s="203">
@@ -14397,13 +14397,13 @@
       <c r="V118" s="204">
         <v>0</v>
       </c>
-      <c r="W118" s="213">
+      <c r="W118" s="212">
         <v>0.25</v>
       </c>
-      <c r="X118" s="214">
+      <c r="X118" s="213">
         <v>0.25</v>
       </c>
-      <c r="Y118" s="214">
+      <c r="Y118" s="213">
         <v>0</v>
       </c>
       <c r="Z118" s="29">
@@ -14463,8 +14463,8 @@
       <c r="C121" s="23"/>
       <c r="D121" s="23"/>
       <c r="E121" s="23"/>
-      <c r="F121" s="207"/>
-      <c r="G121" s="207"/>
+      <c r="F121" s="214"/>
+      <c r="G121" s="214"/>
       <c r="H121" s="22" t="s">
         <v>56</v>
       </c>
@@ -16113,8 +16113,8 @@
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
+      <c r="F3" s="214"/>
+      <c r="G3" s="214"/>
       <c r="H3" s="23"/>
       <c r="I3" s="22"/>
       <c r="J3" s="172"/>

</xml_diff>

<commit_message>
GoodJunkScore rewardCoins = 1
Former-commit-id: 46eedd7e69c717f2ab50bb9542059d0f27025901
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5086,10 +5086,10 @@
   </sheetPr>
   <dimension ref="A1:AE145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A88" sqref="A88"/>
+      <selection pane="topRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5702,7 +5702,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="131">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" s="131">
         <v>0</v>
@@ -9335,7 +9335,7 @@
         <v>20</v>
       </c>
       <c r="E65" s="107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" s="107">
         <v>0</v>

</xml_diff>

<commit_message>
Adding 2 more new spawners to content (NOT BALANCING YET)
Former-commit-id: a965e4b1fdeb54fc5707129062ad7abac773e423
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$122:$O$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$124:$O$125</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="469">
   <si>
     <t>tier_4</t>
   </si>
@@ -1430,6 +1430,12 @@
   </si>
   <si>
     <t>Jellyfish02</t>
+  </si>
+  <si>
+    <t>SpiderEggs</t>
+  </si>
+  <si>
+    <t>Firefly</t>
   </si>
 </sst>
 </file>
@@ -4784,8 +4790,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE118" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
-  <autoFilter ref="A22:AE118"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE120" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+  <autoFilter ref="A22:AE120"/>
   <sortState ref="A23:AE109">
     <sortCondition ref="B22:B109"/>
   </sortState>
@@ -4841,8 +4847,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A122:O133" totalsRowShown="0">
-  <autoFilter ref="A122:O133"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A124:O135" totalsRowShown="0">
+  <autoFilter ref="A124:O135"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
@@ -5162,12 +5168,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AE150"/>
+  <dimension ref="A1:AE152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="E66" sqref="E66"/>
+      <selection pane="topRight" activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14425,229 +14431,315 @@
         <v>248</v>
       </c>
     </row>
-    <row r="119" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A120" s="9" t="s">
+    <row r="119" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A119" s="206" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="88" t="s">
+        <v>467</v>
+      </c>
+      <c r="C119" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D119" s="193">
+        <v>20</v>
+      </c>
+      <c r="E119" s="71">
+        <v>0</v>
+      </c>
+      <c r="F119" s="71">
+        <v>0</v>
+      </c>
+      <c r="G119" s="71">
+        <v>-10</v>
+      </c>
+      <c r="H119" s="71">
+        <v>0</v>
+      </c>
+      <c r="I119" s="71">
+        <v>25</v>
+      </c>
+      <c r="J119" s="207">
+        <v>0</v>
+      </c>
+      <c r="K119" s="71">
+        <v>0</v>
+      </c>
+      <c r="L119" s="199" t="b">
+        <v>1</v>
+      </c>
+      <c r="M119" s="208">
+        <v>5</v>
+      </c>
+      <c r="N119" s="208">
+        <v>5</v>
+      </c>
+      <c r="O119" s="200">
+        <v>0</v>
+      </c>
+      <c r="P119" s="208">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>0</v>
+      </c>
+      <c r="Q119" s="209" t="b">
+        <v>1</v>
+      </c>
+      <c r="R119" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="S119" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="T119" s="211">
+        <v>1</v>
+      </c>
+      <c r="U119" s="203">
+        <v>2</v>
+      </c>
+      <c r="V119" s="204">
+        <v>0</v>
+      </c>
+      <c r="W119" s="212">
+        <v>1</v>
+      </c>
+      <c r="X119" s="213">
+        <v>1</v>
+      </c>
+      <c r="Y119" s="213">
+        <v>0</v>
+      </c>
+      <c r="Z119" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA119" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB119" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="AC119" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD119" s="26"/>
+      <c r="AE119" s="25"/>
+    </row>
+    <row r="120" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A120" s="206" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="88" t="s">
+        <v>468</v>
+      </c>
+      <c r="C120" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D120" s="193">
+        <v>20</v>
+      </c>
+      <c r="E120" s="71">
+        <v>2</v>
+      </c>
+      <c r="F120" s="71">
+        <v>0</v>
+      </c>
+      <c r="G120" s="71">
+        <v>2</v>
+      </c>
+      <c r="H120" s="71">
+        <v>0</v>
+      </c>
+      <c r="I120" s="71">
+        <v>25</v>
+      </c>
+      <c r="J120" s="207">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K120" s="71">
+        <v>0</v>
+      </c>
+      <c r="L120" s="199" t="b">
+        <v>1</v>
+      </c>
+      <c r="M120" s="208">
+        <v>5</v>
+      </c>
+      <c r="N120" s="208">
+        <v>5</v>
+      </c>
+      <c r="O120" s="200">
+        <v>0</v>
+      </c>
+      <c r="P120" s="208">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>0</v>
+      </c>
+      <c r="Q120" s="209" t="b">
+        <v>1</v>
+      </c>
+      <c r="R120" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="S120" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="T120" s="211">
+        <v>1</v>
+      </c>
+      <c r="U120" s="203">
+        <v>2</v>
+      </c>
+      <c r="V120" s="204">
+        <v>0</v>
+      </c>
+      <c r="W120" s="212">
+        <v>0.1</v>
+      </c>
+      <c r="X120" s="213">
+        <v>0.1</v>
+      </c>
+      <c r="Y120" s="213">
+        <v>0</v>
+      </c>
+      <c r="Z120" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA120" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB120" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC120" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD120" s="26"/>
+      <c r="AE120" s="25"/>
+    </row>
+    <row r="121" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A122" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B120" s="9"/>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="9"/>
-      <c r="J120" s="9"/>
-      <c r="K120" s="9"/>
-      <c r="L120" s="9"/>
-      <c r="M120" s="9"/>
-      <c r="N120" s="9"/>
-      <c r="O120" s="9"/>
-      <c r="P120" s="9"/>
-      <c r="Q120" s="9"/>
-      <c r="R120" s="9"/>
-      <c r="S120" s="9"/>
-      <c r="T120" s="9"/>
-      <c r="U120" s="9"/>
-      <c r="V120" s="9"/>
-      <c r="W120" s="9"/>
-      <c r="X120" s="9"/>
-      <c r="Y120" s="9"/>
-      <c r="Z120" s="9"/>
-      <c r="AA120" s="9"/>
-    </row>
-    <row r="121" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A121" s="23"/>
-      <c r="B121" s="23"/>
-      <c r="C121" s="23"/>
-      <c r="D121" s="23"/>
-      <c r="E121" s="23"/>
-      <c r="F121" s="214"/>
-      <c r="G121" s="214"/>
-      <c r="H121" s="22" t="s">
+      <c r="B122" s="9"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="9"/>
+      <c r="G122" s="9"/>
+      <c r="H122" s="9"/>
+      <c r="I122" s="9"/>
+      <c r="J122" s="9"/>
+      <c r="K122" s="9"/>
+      <c r="L122" s="9"/>
+      <c r="M122" s="9"/>
+      <c r="N122" s="9"/>
+      <c r="O122" s="9"/>
+      <c r="P122" s="9"/>
+      <c r="Q122" s="9"/>
+      <c r="R122" s="9"/>
+      <c r="S122" s="9"/>
+      <c r="T122" s="9"/>
+      <c r="U122" s="9"/>
+      <c r="V122" s="9"/>
+      <c r="W122" s="9"/>
+      <c r="X122" s="9"/>
+      <c r="Y122" s="9"/>
+      <c r="Z122" s="9"/>
+      <c r="AA122" s="9"/>
+    </row>
+    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A123" s="23"/>
+      <c r="B123" s="23"/>
+      <c r="C123" s="23"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="23"/>
+      <c r="F123" s="214"/>
+      <c r="G123" s="214"/>
+      <c r="H123" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I121" s="22"/>
-      <c r="J121" s="23"/>
-      <c r="K121" s="18"/>
-      <c r="L121" s="18"/>
-      <c r="M121" s="18" t="s">
+      <c r="I123" s="22"/>
+      <c r="J123" s="23"/>
+      <c r="K123" s="18"/>
+      <c r="L123" s="18"/>
+      <c r="M123" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="N121" s="18"/>
-      <c r="O121" s="18"/>
-      <c r="P121" s="18"/>
-      <c r="Q121" s="18"/>
-      <c r="R121" s="18"/>
-      <c r="S121" s="18"/>
-      <c r="T121" s="18"/>
-      <c r="U121" s="18"/>
-      <c r="V121" s="18"/>
-      <c r="W121" s="18"/>
-      <c r="X121" s="18"/>
-      <c r="Y121" s="18"/>
-      <c r="Z121" s="18"/>
-      <c r="AA121" s="22"/>
-      <c r="AB121" s="22"/>
-      <c r="AC121" s="22"/>
-      <c r="AD121" s="22"/>
-      <c r="AE121" s="18"/>
-    </row>
-    <row r="122" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B122" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D122" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E122" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F122" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="G122" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H122" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="I122" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="J122" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K122" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L122" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M122" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N122" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="O122" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="123" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A123" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B123" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C123" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D123" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E123" s="15">
-        <v>3</v>
-      </c>
-      <c r="F123" s="19">
-        <v>0</v>
-      </c>
-      <c r="G123" s="19">
-        <v>0</v>
-      </c>
-      <c r="H123" s="19">
-        <v>0</v>
-      </c>
-      <c r="I123" s="19">
-        <v>0</v>
-      </c>
-      <c r="J123" s="12">
-        <v>2</v>
-      </c>
-      <c r="K123" s="12">
-        <v>0</v>
-      </c>
-      <c r="L123" s="12">
-        <v>0</v>
-      </c>
-      <c r="M123" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N123" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O123" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N123" s="18"/>
+      <c r="O123" s="18"/>
       <c r="P123" s="18"/>
       <c r="Q123" s="18"/>
-    </row>
-    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A124" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B124" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C124" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D124" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E124" s="15">
-        <v>3</v>
-      </c>
-      <c r="F124" s="19">
-        <v>0</v>
-      </c>
-      <c r="G124" s="19">
-        <v>1</v>
-      </c>
-      <c r="H124" s="19">
-        <v>0</v>
-      </c>
-      <c r="I124" s="19">
-        <v>0</v>
-      </c>
-      <c r="J124" s="12">
-        <v>2</v>
-      </c>
-      <c r="K124" s="12">
-        <v>0</v>
-      </c>
-      <c r="L124" s="12">
-        <v>0</v>
-      </c>
-      <c r="M124" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N124" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O124" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P124" s="18"/>
-      <c r="Q124" s="18"/>
+      <c r="R123" s="18"/>
+      <c r="S123" s="18"/>
+      <c r="T123" s="18"/>
+      <c r="U123" s="18"/>
+      <c r="V123" s="18"/>
+      <c r="W123" s="18"/>
+      <c r="X123" s="18"/>
+      <c r="Y123" s="18"/>
+      <c r="Z123" s="18"/>
+      <c r="AA123" s="22"/>
+      <c r="AB123" s="22"/>
+      <c r="AC123" s="22"/>
+      <c r="AD123" s="22"/>
+      <c r="AE123" s="18"/>
+    </row>
+    <row r="124" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D124" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E124" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F124" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G124" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H124" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I124" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J124" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K124" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="L124" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="M124" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N124" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="O124" s="20" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="125" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>30</v>
@@ -14688,15 +14780,15 @@
       <c r="P125" s="18"/>
       <c r="Q125" s="18"/>
     </row>
-    <row r="126" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D126" s="15" t="s">
         <v>23</v>
@@ -14736,30 +14828,16 @@
       </c>
       <c r="P126" s="18"/>
       <c r="Q126" s="18"/>
-      <c r="R126"/>
-      <c r="S126"/>
-      <c r="T126"/>
-      <c r="U126"/>
-      <c r="V126"/>
-      <c r="W126"/>
-      <c r="X126"/>
-      <c r="Y126"/>
-      <c r="Z126"/>
-      <c r="AA126"/>
-      <c r="AB126"/>
-      <c r="AC126"/>
-      <c r="AD126"/>
-      <c r="AE126"/>
     </row>
     <row r="127" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A127" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D127" s="15" t="s">
         <v>30</v>
@@ -14800,15 +14878,15 @@
       <c r="P127" s="18"/>
       <c r="Q127" s="18"/>
     </row>
-    <row r="128" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D128" s="15" t="s">
         <v>23</v>
@@ -14848,19 +14926,33 @@
       </c>
       <c r="P128" s="18"/>
       <c r="Q128" s="18"/>
+      <c r="R128"/>
+      <c r="S128"/>
+      <c r="T128"/>
+      <c r="U128"/>
+      <c r="V128"/>
+      <c r="W128"/>
+      <c r="X128"/>
+      <c r="Y128"/>
+      <c r="Z128"/>
+      <c r="AA128"/>
+      <c r="AB128"/>
+      <c r="AC128"/>
+      <c r="AD128"/>
+      <c r="AE128"/>
     </row>
     <row r="129" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C129" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D129" s="15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E129" s="15">
         <v>3</v>
@@ -14869,7 +14961,7 @@
         <v>0</v>
       </c>
       <c r="G129" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H129" s="19">
         <v>0</v>
@@ -14903,13 +14995,13 @@
         <v>2</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D130" s="15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E130" s="15">
         <v>3</v>
@@ -14918,7 +15010,7 @@
         <v>0</v>
       </c>
       <c r="G130" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H130" s="19">
         <v>0</v>
@@ -14952,13 +15044,13 @@
         <v>2</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D131" s="15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E131" s="15">
         <v>3</v>
@@ -14967,7 +15059,7 @@
         <v>0</v>
       </c>
       <c r="G131" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H131" s="19">
         <v>0</v>
@@ -15001,13 +15093,13 @@
         <v>2</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C132" s="16" t="s">
         <v>27</v>
       </c>
       <c r="D132" s="15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E132" s="15">
         <v>3</v>
@@ -15016,7 +15108,7 @@
         <v>0</v>
       </c>
       <c r="G132" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H132" s="19">
         <v>0</v>
@@ -15050,27 +15142,27 @@
         <v>2</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D133" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E133" s="14">
-        <v>1</v>
-      </c>
-      <c r="F133" s="13">
-        <v>0</v>
-      </c>
-      <c r="G133" s="13">
-        <v>1</v>
-      </c>
-      <c r="H133" s="13">
-        <v>0</v>
-      </c>
-      <c r="I133" s="13">
+      <c r="E133" s="15">
+        <v>3</v>
+      </c>
+      <c r="F133" s="19">
+        <v>0</v>
+      </c>
+      <c r="G133" s="19">
+        <v>1</v>
+      </c>
+      <c r="H133" s="19">
+        <v>0</v>
+      </c>
+      <c r="I133" s="19">
         <v>0</v>
       </c>
       <c r="J133" s="12">
@@ -15091,120 +15183,166 @@
       <c r="O133" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P133" s="18"/>
+      <c r="Q133" s="18"/>
     </row>
     <row r="134" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N134" s="8"/>
-      <c r="O134" s="8"/>
-      <c r="P134" s="8"/>
-      <c r="Q134" s="8"/>
-      <c r="R134" s="8"/>
-      <c r="S134" s="8"/>
-      <c r="T134" s="8"/>
-      <c r="U134" s="8"/>
-      <c r="V134" s="8"/>
-      <c r="W134" s="8"/>
-      <c r="X134" s="8"/>
-      <c r="Y134" s="8"/>
-      <c r="Z134" s="8"/>
-      <c r="AA134" s="8"/>
-      <c r="AB134" s="8"/>
-      <c r="AC134" s="8"/>
-      <c r="AD134" s="8"/>
-      <c r="AE134" s="8"/>
-    </row>
-    <row r="135" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="136" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A136" s="9" t="s">
+      <c r="A134" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B134" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C134" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D134" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E134" s="15">
+        <v>3</v>
+      </c>
+      <c r="F134" s="19">
+        <v>0</v>
+      </c>
+      <c r="G134" s="19">
+        <v>2</v>
+      </c>
+      <c r="H134" s="19">
+        <v>0</v>
+      </c>
+      <c r="I134" s="19">
+        <v>0</v>
+      </c>
+      <c r="J134" s="12">
+        <v>2</v>
+      </c>
+      <c r="K134" s="12">
+        <v>0</v>
+      </c>
+      <c r="L134" s="12">
+        <v>0</v>
+      </c>
+      <c r="M134" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N134" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O134" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P134" s="18"/>
+      <c r="Q134" s="18"/>
+    </row>
+    <row r="135" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A135" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C135" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D135" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E135" s="14">
+        <v>1</v>
+      </c>
+      <c r="F135" s="13">
+        <v>0</v>
+      </c>
+      <c r="G135" s="13">
+        <v>1</v>
+      </c>
+      <c r="H135" s="13">
+        <v>0</v>
+      </c>
+      <c r="I135" s="13">
+        <v>0</v>
+      </c>
+      <c r="J135" s="12">
+        <v>2</v>
+      </c>
+      <c r="K135" s="12">
+        <v>0</v>
+      </c>
+      <c r="L135" s="12">
+        <v>0</v>
+      </c>
+      <c r="M135" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N135" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O135" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N136" s="8"/>
+      <c r="O136" s="8"/>
+      <c r="P136" s="8"/>
+      <c r="Q136" s="8"/>
+      <c r="R136" s="8"/>
+      <c r="S136" s="8"/>
+      <c r="T136" s="8"/>
+      <c r="U136" s="8"/>
+      <c r="V136" s="8"/>
+      <c r="W136" s="8"/>
+      <c r="X136" s="8"/>
+      <c r="Y136" s="8"/>
+      <c r="Z136" s="8"/>
+      <c r="AA136" s="8"/>
+      <c r="AB136" s="8"/>
+      <c r="AC136" s="8"/>
+      <c r="AD136" s="8"/>
+      <c r="AE136" s="8"/>
+    </row>
+    <row r="137" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A138" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B136" s="9"/>
-      <c r="C136" s="9"/>
-      <c r="D136" s="9"/>
-      <c r="E136" s="8"/>
-      <c r="F136" s="8"/>
-      <c r="G136" s="8"/>
-      <c r="H136" s="8"/>
-      <c r="I136" s="8"/>
-      <c r="J136" s="8"/>
-      <c r="K136" s="8"/>
-      <c r="L136" s="8"/>
-    </row>
-    <row r="138" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A138" s="7" t="s">
+      <c r="B138" s="9"/>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="8"/>
+      <c r="F138" s="8"/>
+      <c r="G138" s="8"/>
+      <c r="H138" s="8"/>
+      <c r="I138" s="8"/>
+      <c r="J138" s="8"/>
+      <c r="K138" s="8"/>
+      <c r="L138" s="8"/>
+    </row>
+    <row r="140" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A140" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B138" s="6" t="s">
+      <c r="B140" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C138" s="6" t="s">
+      <c r="C140" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D138" s="5" t="s">
+      <c r="D140" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E138" s="5" t="s">
+      <c r="E140" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F138" s="5" t="s">
+      <c r="F140" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G138" s="5" t="s">
+      <c r="G140" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H138" s="5" t="s">
+      <c r="H140" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="139" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A139" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D139" s="2">
-        <v>42</v>
-      </c>
-      <c r="E139" s="2">
-        <v>8</v>
-      </c>
-      <c r="F139" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G139" s="2">
-        <v>2</v>
-      </c>
-      <c r="H139" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A140" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D140" s="2">
-        <v>92</v>
-      </c>
-      <c r="E140" s="2">
-        <v>10</v>
-      </c>
-      <c r="F140" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G140" s="2">
-        <v>2</v>
-      </c>
-      <c r="H140" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:31" x14ac:dyDescent="0.25">
@@ -15212,19 +15350,19 @@
         <v>2</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D141" s="2">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="E141" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F141" s="2">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="G141" s="2">
         <v>2</v>
@@ -15238,19 +15376,19 @@
         <v>2</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D142" s="2">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="E142" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F142" s="2">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G142" s="2">
         <v>2</v>
@@ -15264,104 +15402,156 @@
         <v>2</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D143" s="2">
+        <v>235</v>
+      </c>
+      <c r="E143" s="2">
+        <v>12</v>
+      </c>
+      <c r="F143" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G143" s="2">
+        <v>2</v>
+      </c>
+      <c r="H143" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D144" s="2">
+        <v>686</v>
+      </c>
+      <c r="E144" s="2">
+        <v>14</v>
+      </c>
+      <c r="F144" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G144" s="2">
+        <v>2</v>
+      </c>
+      <c r="H144" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D145" s="2">
         <v>1040</v>
       </c>
-      <c r="E143" s="2">
+      <c r="E145" s="2">
         <v>14</v>
       </c>
-      <c r="F143" s="2">
+      <c r="F145" s="2">
         <v>0.5</v>
       </c>
-      <c r="G143" s="2">
-        <v>2</v>
-      </c>
-      <c r="H143" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D146" s="1">
+      <c r="G145" s="2">
+        <v>2</v>
+      </c>
+      <c r="H145" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D148" s="1">
         <v>42</v>
       </c>
-      <c r="F146" s="1">
+      <c r="F148" s="1">
         <v>1.3</v>
-      </c>
-      <c r="G146">
-        <f>D139*F139</f>
-        <v>54.6</v>
-      </c>
-      <c r="I146">
-        <f>D146*F146</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="147" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D147" s="1">
-        <v>92</v>
-      </c>
-      <c r="F147" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G147">
-        <f>D140*F140</f>
-        <v>101.2</v>
-      </c>
-      <c r="I147">
-        <f>D147*F147</f>
-        <v>101.2</v>
-      </c>
-    </row>
-    <row r="148" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D148" s="1">
-        <v>235</v>
-      </c>
-      <c r="F148" s="1">
-        <v>0.9</v>
       </c>
       <c r="G148">
         <f>D141*F141</f>
-        <v>211.5</v>
+        <v>54.6</v>
       </c>
       <c r="I148">
         <f>D148*F148</f>
-        <v>211.5</v>
-      </c>
-    </row>
-    <row r="149" spans="4:9" x14ac:dyDescent="0.25">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D149" s="1">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="F149" s="1">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G149">
         <f>D142*F142</f>
-        <v>480.2</v>
+        <v>101.2</v>
       </c>
       <c r="I149">
         <f>D149*F149</f>
-        <v>480.2</v>
-      </c>
-    </row>
-    <row r="150" spans="4:9" x14ac:dyDescent="0.25">
+        <v>101.2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D150" s="1">
-        <v>1040</v>
+        <v>235</v>
       </c>
       <c r="F150" s="1">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G150">
         <f>D143*F143</f>
-        <v>520</v>
+        <v>211.5</v>
       </c>
       <c r="I150">
         <f>D150*F150</f>
+        <v>211.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D151" s="1">
+        <v>686</v>
+      </c>
+      <c r="F151" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G151">
+        <f>D144*F144</f>
+        <v>480.2</v>
+      </c>
+      <c r="I151">
+        <f>D151*F151</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D152" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F152" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G152">
+        <f>D145*F145</f>
+        <v>520</v>
+      </c>
+      <c r="I152">
+        <f>D152*F152</f>
         <v>520</v>
       </c>
     </row>
@@ -15369,9 +15559,45 @@
   <mergeCells count="3">
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="F123:G123"/>
   </mergeCells>
   <conditionalFormatting sqref="M97:P97">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M75:P77 M23:P24 M49:P59 M30:P47 M79:P84 M86:P87 M61:P70 M26:P27 M94:P97 M89:P92">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M71:P71">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M72:P72">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -15383,19 +15609,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M75:P77 M23:P24 M49:P59 M30:P47 M79:P84 M86:P87 M61:P70 M26:P27 M94:P97 M89:P92">
-    <cfRule type="colorScale" priority="56">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M71:P71">
+  <conditionalFormatting sqref="M48:P48">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -15407,7 +15621,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M72:P72">
+  <conditionalFormatting sqref="M28:P28">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -15419,7 +15633,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M48:P48">
+  <conditionalFormatting sqref="M29:P29">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -15431,7 +15645,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:P28">
+  <conditionalFormatting sqref="M78:P78">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -15443,7 +15657,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M29:P29">
+  <conditionalFormatting sqref="M85:P85">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -15455,7 +15669,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M78:P78">
+  <conditionalFormatting sqref="M60:P60">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -15467,7 +15681,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M85:P85">
+  <conditionalFormatting sqref="M25:P25">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -15479,7 +15693,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M60:P60">
+  <conditionalFormatting sqref="M93:P93">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -15491,7 +15705,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25:P25">
+  <conditionalFormatting sqref="M73:P73">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -15503,7 +15717,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M93:P93">
+  <conditionalFormatting sqref="M74:P74">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -15515,7 +15729,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M73:P73">
+  <conditionalFormatting sqref="M98:P98">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -15527,7 +15741,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M74:P74">
+  <conditionalFormatting sqref="M99:P99">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -15539,7 +15753,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M98:P98">
+  <conditionalFormatting sqref="M100:P100">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -15551,7 +15765,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M99:P99">
+  <conditionalFormatting sqref="M101:P101">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -15563,7 +15777,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M100:P100">
+  <conditionalFormatting sqref="M102:P102">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -15575,7 +15789,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M101:P101">
+  <conditionalFormatting sqref="M103:P103">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -15587,7 +15801,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M102:P102">
+  <conditionalFormatting sqref="N104:P104">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -15599,7 +15813,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M103:P103">
+  <conditionalFormatting sqref="M105:P105">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -15611,7 +15825,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N104:P104">
+  <conditionalFormatting sqref="M104">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -15623,7 +15837,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M105:P105">
+  <conditionalFormatting sqref="O107">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -15635,7 +15849,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M104">
+  <conditionalFormatting sqref="M107">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -15647,7 +15861,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O107">
+  <conditionalFormatting sqref="N107">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -15659,7 +15873,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M107">
+  <conditionalFormatting sqref="P107">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -15671,19 +15885,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N107">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P107">
+  <conditionalFormatting sqref="O108">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -15696,7 +15898,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15707,7 +15909,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108">
+  <conditionalFormatting sqref="M108">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -15719,7 +15921,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M108">
+  <conditionalFormatting sqref="N108">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -15732,7 +15934,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N108">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15743,7 +15945,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N108">
+  <conditionalFormatting sqref="P108">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -15755,7 +15957,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P108">
+  <conditionalFormatting sqref="O109">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -15768,7 +15970,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -15779,7 +15981,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109">
+  <conditionalFormatting sqref="M109">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -15791,7 +15993,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M109">
+  <conditionalFormatting sqref="N109">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -15804,6 +16006,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N109">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P109">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O110:P110">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -15815,19 +16041,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N109">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P109">
+  <conditionalFormatting sqref="M110">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -15839,19 +16053,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O110:P110">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M110">
+  <conditionalFormatting sqref="N110">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -15864,6 +16066,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N110">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M111:P111">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M112:P112">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -15875,19 +16101,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N110">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M111:P111">
+  <conditionalFormatting sqref="O106">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -15899,7 +16113,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M112:P112">
+  <conditionalFormatting sqref="M106">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -15911,7 +16125,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O106">
+  <conditionalFormatting sqref="N106">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -15923,7 +16137,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M106">
+  <conditionalFormatting sqref="P106">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -15935,7 +16149,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N106">
+  <conditionalFormatting sqref="M113:P113">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -15947,7 +16161,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P106">
+  <conditionalFormatting sqref="M88:P88">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -15959,19 +16173,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M113:P113">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M88:P88">
+  <conditionalFormatting sqref="M114:P114">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -15983,7 +16185,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M114:P114">
+  <conditionalFormatting sqref="M115:P116">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M117:P117">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -15995,8 +16209,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M115:P116">
-    <cfRule type="colorScale" priority="58">
+  <conditionalFormatting sqref="M118:P118">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16007,7 +16221,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M117:P117">
+  <conditionalFormatting sqref="M119:P119">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -16019,7 +16233,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M118:P118">
+  <conditionalFormatting sqref="M120:P120">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -16033,32 +16247,32 @@
   </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G42"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I118">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I120">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D123:G133 P23:V118 M23:N118">
+    <dataValidation type="decimal" allowBlank="1" sqref="D125:G135 P23:V120 M23:N120">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H123:L132 H133:I133 W23:Z118">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H125:L134 H135:I135 W23:Z120">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C123:C133 C23:C118">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C125:C135 C23:C120">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="M123:O133 J133:L133 AA23:AA99 AA101:AA118 AB23:AE118"/>
-    <dataValidation type="list" sqref="O23:O118">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="M125:O135 J135:L135 AA23:AA99 AA101:AA120 AB23:AE120"/>
+    <dataValidation type="list" sqref="O23:O120">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K118">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K120">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F118">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F120">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="L23:L118">
+    <dataValidation type="list" sqref="L23:L120">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
And last spawners added to content
Former-commit-id: d98665810854cbf8d8f19e700b8802200ce9602b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$125:$O$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$126:$O$127</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="470">
   <si>
     <t>tier_4</t>
   </si>
@@ -1436,6 +1436,9 @@
   </si>
   <si>
     <t>Fireball</t>
+  </si>
+  <si>
+    <t>PlantCreature</t>
   </si>
 </sst>
 </file>
@@ -4790,8 +4793,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE121" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
-  <autoFilter ref="A22:AE121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE122" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
+  <autoFilter ref="A22:AE122"/>
   <sortState ref="A23:AE109">
     <sortCondition ref="B22:B109"/>
   </sortState>
@@ -4847,8 +4850,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A125:O136" totalsRowShown="0">
-  <autoFilter ref="A125:O136"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A126:O137" totalsRowShown="0">
+  <autoFilter ref="A126:O137"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
@@ -5168,12 +5171,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AE153"/>
+  <dimension ref="A1:AE154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A121" sqref="A121"/>
+      <selection pane="topRight" activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14623,7 +14626,7 @@
         <v>468</v>
       </c>
       <c r="C121" s="87" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D121" s="193">
         <v>120</v>
@@ -14711,170 +14714,215 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A123" s="9" t="s">
+    <row r="122" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A122" s="206" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="88" t="s">
+        <v>469</v>
+      </c>
+      <c r="C122" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D122" s="193">
+        <v>60</v>
+      </c>
+      <c r="E122" s="71">
+        <v>9</v>
+      </c>
+      <c r="F122" s="71">
+        <v>0</v>
+      </c>
+      <c r="G122" s="71">
+        <v>5</v>
+      </c>
+      <c r="H122" s="71">
+        <v>0</v>
+      </c>
+      <c r="I122" s="71">
+        <v>35</v>
+      </c>
+      <c r="J122" s="207">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K122" s="71">
+        <v>0</v>
+      </c>
+      <c r="L122" s="199" t="b">
+        <v>1</v>
+      </c>
+      <c r="M122" s="208">
+        <v>5</v>
+      </c>
+      <c r="N122" s="208">
+        <v>5</v>
+      </c>
+      <c r="O122" s="200">
+        <v>2</v>
+      </c>
+      <c r="P122" s="208">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>2</v>
+      </c>
+      <c r="Q122" s="209" t="b">
+        <v>1</v>
+      </c>
+      <c r="R122" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="S122" s="210" t="b">
+        <v>0</v>
+      </c>
+      <c r="T122" s="211">
+        <v>1</v>
+      </c>
+      <c r="U122" s="203">
+        <v>2</v>
+      </c>
+      <c r="V122" s="204">
+        <v>0</v>
+      </c>
+      <c r="W122" s="212">
+        <v>0.1</v>
+      </c>
+      <c r="X122" s="213">
+        <v>0.1</v>
+      </c>
+      <c r="Y122" s="213">
+        <v>0</v>
+      </c>
+      <c r="Z122" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA122" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB122" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC122" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD122" s="26"/>
+      <c r="AE122" s="25"/>
+    </row>
+    <row r="123" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A124" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B123" s="9"/>
-      <c r="C123" s="9"/>
-      <c r="D123" s="9"/>
-      <c r="E123" s="9"/>
-      <c r="F123" s="9"/>
-      <c r="G123" s="9"/>
-      <c r="H123" s="9"/>
-      <c r="I123" s="9"/>
-      <c r="J123" s="9"/>
-      <c r="K123" s="9"/>
-      <c r="L123" s="9"/>
-      <c r="M123" s="9"/>
-      <c r="N123" s="9"/>
-      <c r="O123" s="9"/>
-      <c r="P123" s="9"/>
-      <c r="Q123" s="9"/>
-      <c r="R123" s="9"/>
-      <c r="S123" s="9"/>
-      <c r="T123" s="9"/>
-      <c r="U123" s="9"/>
-      <c r="V123" s="9"/>
-      <c r="W123" s="9"/>
-      <c r="X123" s="9"/>
-      <c r="Y123" s="9"/>
-      <c r="Z123" s="9"/>
-      <c r="AA123" s="9"/>
-    </row>
-    <row r="124" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A124" s="23"/>
-      <c r="B124" s="23"/>
-      <c r="C124" s="23"/>
-      <c r="D124" s="23"/>
-      <c r="E124" s="23"/>
-      <c r="F124" s="214"/>
-      <c r="G124" s="214"/>
-      <c r="H124" s="22" t="s">
+      <c r="B124" s="9"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
+      <c r="H124" s="9"/>
+      <c r="I124" s="9"/>
+      <c r="J124" s="9"/>
+      <c r="K124" s="9"/>
+      <c r="L124" s="9"/>
+      <c r="M124" s="9"/>
+      <c r="N124" s="9"/>
+      <c r="O124" s="9"/>
+      <c r="P124" s="9"/>
+      <c r="Q124" s="9"/>
+      <c r="R124" s="9"/>
+      <c r="S124" s="9"/>
+      <c r="T124" s="9"/>
+      <c r="U124" s="9"/>
+      <c r="V124" s="9"/>
+      <c r="W124" s="9"/>
+      <c r="X124" s="9"/>
+      <c r="Y124" s="9"/>
+      <c r="Z124" s="9"/>
+      <c r="AA124" s="9"/>
+    </row>
+    <row r="125" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A125" s="23"/>
+      <c r="B125" s="23"/>
+      <c r="C125" s="23"/>
+      <c r="D125" s="23"/>
+      <c r="E125" s="23"/>
+      <c r="F125" s="214"/>
+      <c r="G125" s="214"/>
+      <c r="H125" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I124" s="22"/>
-      <c r="J124" s="23"/>
-      <c r="K124" s="18"/>
-      <c r="L124" s="18"/>
-      <c r="M124" s="18" t="s">
+      <c r="I125" s="22"/>
+      <c r="J125" s="23"/>
+      <c r="K125" s="18"/>
+      <c r="L125" s="18"/>
+      <c r="M125" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="N124" s="18"/>
-      <c r="O124" s="18"/>
-      <c r="P124" s="18"/>
-      <c r="Q124" s="18"/>
-      <c r="R124" s="18"/>
-      <c r="S124" s="18"/>
-      <c r="T124" s="18"/>
-      <c r="U124" s="18"/>
-      <c r="V124" s="18"/>
-      <c r="W124" s="18"/>
-      <c r="X124" s="18"/>
-      <c r="Y124" s="18"/>
-      <c r="Z124" s="18"/>
-      <c r="AA124" s="22"/>
-      <c r="AB124" s="22"/>
-      <c r="AC124" s="22"/>
-      <c r="AD124" s="22"/>
-      <c r="AE124" s="18"/>
-    </row>
-    <row r="125" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="7" t="s">
+      <c r="N125" s="18"/>
+      <c r="O125" s="18"/>
+      <c r="P125" s="18"/>
+      <c r="Q125" s="18"/>
+      <c r="R125" s="18"/>
+      <c r="S125" s="18"/>
+      <c r="T125" s="18"/>
+      <c r="U125" s="18"/>
+      <c r="V125" s="18"/>
+      <c r="W125" s="18"/>
+      <c r="X125" s="18"/>
+      <c r="Y125" s="18"/>
+      <c r="Z125" s="18"/>
+      <c r="AA125" s="22"/>
+      <c r="AB125" s="22"/>
+      <c r="AC125" s="22"/>
+      <c r="AD125" s="22"/>
+      <c r="AE125" s="18"/>
+    </row>
+    <row r="126" spans="1:31" s="8" customFormat="1" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="B126" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="C126" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D125" s="21" t="s">
+      <c r="D126" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E125" s="21" t="s">
+      <c r="E126" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F125" s="21" t="s">
+      <c r="F126" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="G125" s="21" t="s">
+      <c r="G126" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H125" s="21" t="s">
+      <c r="H126" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I125" s="21" t="s">
+      <c r="I126" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="J125" s="21" t="s">
+      <c r="J126" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="K125" s="21" t="s">
+      <c r="K126" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="L125" s="21" t="s">
+      <c r="L126" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M125" s="20" t="s">
+      <c r="M126" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="N125" s="20" t="s">
+      <c r="N126" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="O125" s="20" t="s">
+      <c r="O126" s="20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="126" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B126" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C126" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D126" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E126" s="15">
-        <v>3</v>
-      </c>
-      <c r="F126" s="19">
-        <v>0</v>
-      </c>
-      <c r="G126" s="19">
-        <v>0</v>
-      </c>
-      <c r="H126" s="19">
-        <v>0</v>
-      </c>
-      <c r="I126" s="19">
-        <v>0</v>
-      </c>
-      <c r="J126" s="12">
-        <v>2</v>
-      </c>
-      <c r="K126" s="12">
-        <v>0</v>
-      </c>
-      <c r="L126" s="12">
-        <v>0</v>
-      </c>
-      <c r="M126" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N126" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O126" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P126" s="18"/>
-      <c r="Q126" s="18"/>
+      <c r="P126"/>
+      <c r="Q126"/>
       <c r="R126"/>
       <c r="S126"/>
       <c r="T126"/>
@@ -14895,13 +14943,13 @@
         <v>2</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C127" s="16" t="s">
         <v>38</v>
       </c>
       <c r="D127" s="15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E127" s="15">
         <v>3</v>
@@ -14910,7 +14958,7 @@
         <v>0</v>
       </c>
       <c r="G127" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H127" s="19">
         <v>0</v>
@@ -14944,13 +14992,13 @@
         <v>2</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D128" s="15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E128" s="15">
         <v>3</v>
@@ -14959,7 +15007,7 @@
         <v>0</v>
       </c>
       <c r="G128" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H128" s="19">
         <v>0</v>
@@ -14993,13 +15041,13 @@
         <v>2</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C129" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D129" s="15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E129" s="15">
         <v>3</v>
@@ -15008,7 +15056,7 @@
         <v>0</v>
       </c>
       <c r="G129" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H129" s="19">
         <v>0</v>
@@ -15042,13 +15090,13 @@
         <v>2</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D130" s="15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E130" s="15">
         <v>3</v>
@@ -15057,7 +15105,7 @@
         <v>0</v>
       </c>
       <c r="G130" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H130" s="19">
         <v>0</v>
@@ -15091,13 +15139,13 @@
         <v>2</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C131" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D131" s="15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E131" s="15">
         <v>3</v>
@@ -15106,7 +15154,7 @@
         <v>0</v>
       </c>
       <c r="G131" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H131" s="19">
         <v>0</v>
@@ -15140,13 +15188,13 @@
         <v>2</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C132" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D132" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E132" s="15">
         <v>3</v>
@@ -15155,7 +15203,7 @@
         <v>0</v>
       </c>
       <c r="G132" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H132" s="19">
         <v>0</v>
@@ -15189,13 +15237,13 @@
         <v>2</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D133" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E133" s="15">
         <v>3</v>
@@ -15204,7 +15252,7 @@
         <v>0</v>
       </c>
       <c r="G133" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H133" s="19">
         <v>0</v>
@@ -15238,13 +15286,13 @@
         <v>2</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C134" s="16" t="s">
         <v>27</v>
       </c>
       <c r="D134" s="15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E134" s="15">
         <v>3</v>
@@ -15253,7 +15301,7 @@
         <v>0</v>
       </c>
       <c r="G134" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H134" s="19">
         <v>0</v>
@@ -15287,13 +15335,13 @@
         <v>2</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C135" s="16" t="s">
         <v>27</v>
       </c>
       <c r="D135" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E135" s="15">
         <v>3</v>
@@ -15302,7 +15350,7 @@
         <v>0</v>
       </c>
       <c r="G135" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H135" s="19">
         <v>0</v>
@@ -15336,27 +15384,27 @@
         <v>2</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D136" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E136" s="14">
-        <v>1</v>
-      </c>
-      <c r="F136" s="13">
-        <v>0</v>
-      </c>
-      <c r="G136" s="13">
-        <v>1</v>
-      </c>
-      <c r="H136" s="13">
-        <v>0</v>
-      </c>
-      <c r="I136" s="13">
+        <v>26</v>
+      </c>
+      <c r="E136" s="15">
+        <v>3</v>
+      </c>
+      <c r="F136" s="19">
+        <v>0</v>
+      </c>
+      <c r="G136" s="19">
+        <v>2</v>
+      </c>
+      <c r="H136" s="19">
+        <v>0</v>
+      </c>
+      <c r="I136" s="19">
         <v>0</v>
       </c>
       <c r="J136" s="12">
@@ -15377,94 +15425,117 @@
       <c r="O136" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P136" s="18"/>
+      <c r="Q136" s="18"/>
     </row>
     <row r="137" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N137" s="8"/>
-      <c r="O137" s="8"/>
-      <c r="P137" s="8"/>
-      <c r="Q137" s="8"/>
-      <c r="R137" s="8"/>
-      <c r="S137" s="8"/>
-      <c r="T137" s="8"/>
-      <c r="U137" s="8"/>
-      <c r="V137" s="8"/>
-      <c r="W137" s="8"/>
-      <c r="X137" s="8"/>
-      <c r="Y137" s="8"/>
-      <c r="Z137" s="8"/>
-      <c r="AA137" s="8"/>
-      <c r="AB137" s="8"/>
-      <c r="AC137" s="8"/>
-      <c r="AD137" s="8"/>
-      <c r="AE137" s="8"/>
-    </row>
-    <row r="138" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="139" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A139" s="9" t="s">
+      <c r="A137" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C137" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E137" s="14">
+        <v>1</v>
+      </c>
+      <c r="F137" s="13">
+        <v>0</v>
+      </c>
+      <c r="G137" s="13">
+        <v>1</v>
+      </c>
+      <c r="H137" s="13">
+        <v>0</v>
+      </c>
+      <c r="I137" s="13">
+        <v>0</v>
+      </c>
+      <c r="J137" s="12">
+        <v>2</v>
+      </c>
+      <c r="K137" s="12">
+        <v>0</v>
+      </c>
+      <c r="L137" s="12">
+        <v>0</v>
+      </c>
+      <c r="M137" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N137" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O137" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N138" s="8"/>
+      <c r="O138" s="8"/>
+      <c r="P138" s="8"/>
+      <c r="Q138" s="8"/>
+      <c r="R138" s="8"/>
+      <c r="S138" s="8"/>
+      <c r="T138" s="8"/>
+      <c r="U138" s="8"/>
+      <c r="V138" s="8"/>
+      <c r="W138" s="8"/>
+      <c r="X138" s="8"/>
+      <c r="Y138" s="8"/>
+      <c r="Z138" s="8"/>
+      <c r="AA138" s="8"/>
+      <c r="AB138" s="8"/>
+      <c r="AC138" s="8"/>
+      <c r="AD138" s="8"/>
+      <c r="AE138" s="8"/>
+    </row>
+    <row r="139" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="140" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A140" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B139" s="9"/>
-      <c r="C139" s="9"/>
-      <c r="D139" s="9"/>
-      <c r="E139" s="8"/>
-      <c r="F139" s="8"/>
-      <c r="G139" s="8"/>
-      <c r="H139" s="8"/>
-      <c r="I139" s="8"/>
-      <c r="J139" s="8"/>
-      <c r="K139" s="8"/>
-      <c r="L139" s="8"/>
-    </row>
-    <row r="141" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="7" t="s">
+      <c r="B140" s="9"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="8"/>
+      <c r="I140" s="8"/>
+      <c r="J140" s="8"/>
+      <c r="K140" s="8"/>
+      <c r="L140" s="8"/>
+    </row>
+    <row r="142" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B141" s="6" t="s">
+      <c r="B142" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C141" s="6" t="s">
+      <c r="C142" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D142" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E141" s="5" t="s">
+      <c r="E142" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F141" s="5" t="s">
+      <c r="F142" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G141" s="5" t="s">
+      <c r="G142" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H141" s="5" t="s">
+      <c r="H142" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="142" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A142" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D142" s="2">
-        <v>42</v>
-      </c>
-      <c r="E142" s="2">
-        <v>8</v>
-      </c>
-      <c r="F142" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G142" s="2">
-        <v>2</v>
-      </c>
-      <c r="H142" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:31" x14ac:dyDescent="0.25">
@@ -15472,19 +15543,19 @@
         <v>2</v>
       </c>
       <c r="B143" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" s="2">
+        <v>42</v>
+      </c>
+      <c r="E143" s="2">
         <v>8</v>
       </c>
-      <c r="C143" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D143" s="2">
-        <v>92</v>
-      </c>
-      <c r="E143" s="2">
-        <v>10</v>
-      </c>
       <c r="F143" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G143" s="2">
         <v>2</v>
@@ -15498,19 +15569,19 @@
         <v>2</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D144" s="2">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="E144" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F144" s="2">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G144" s="2">
         <v>2</v>
@@ -15524,19 +15595,19 @@
         <v>2</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D145" s="2">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="E145" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F145" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G145" s="2">
         <v>2</v>
@@ -15550,104 +15621,130 @@
         <v>2</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D146" s="2">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="E146" s="2">
         <v>14</v>
       </c>
       <c r="F146" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G146" s="2">
+        <v>2</v>
+      </c>
+      <c r="H146" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D147" s="2">
+        <v>1040</v>
+      </c>
+      <c r="E147" s="2">
+        <v>14</v>
+      </c>
+      <c r="F147" s="2">
         <v>0.5</v>
       </c>
-      <c r="G146" s="2">
-        <v>2</v>
-      </c>
-      <c r="H146" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D149" s="1">
-        <v>42</v>
-      </c>
-      <c r="F149" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G149">
-        <f>D142*F142</f>
-        <v>54.6</v>
-      </c>
-      <c r="I149">
-        <f>D149*F149</f>
-        <v>54.6</v>
+      <c r="G147" s="2">
+        <v>2</v>
+      </c>
+      <c r="H147" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D150" s="1">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="F150" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G150">
         <f>D143*F143</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
       <c r="I150">
         <f>D150*F150</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D151" s="1">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="F151" s="1">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G151">
         <f>D144*F144</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
       <c r="I151">
         <f>D151*F151</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D152" s="1">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="F152" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G152">
         <f>D145*F145</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
       <c r="I152">
         <f>D152*F152</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D153" s="1">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="F153" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G153">
         <f>D146*F146</f>
-        <v>520</v>
+        <v>480.2</v>
       </c>
       <c r="I153">
         <f>D153*F153</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D154" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F154" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G154">
+        <f>D147*F147</f>
+        <v>520</v>
+      </c>
+      <c r="I154">
+        <f>D154*F154</f>
         <v>520</v>
       </c>
     </row>
@@ -15655,9 +15752,33 @@
   <mergeCells count="3">
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="F125:G125"/>
   </mergeCells>
   <conditionalFormatting sqref="M96:P96">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M93:P96 M75:P77 M23:P24 M49:P59 M30:P47 M79:P84 M86:P87 M61:P70 M26:P27 M89:P91">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M71:P71">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -15669,19 +15790,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M93:P96 M75:P77 M23:P24 M49:P59 M30:P47 M79:P84 M86:P87 M61:P70 M26:P27 M89:P91">
-    <cfRule type="colorScale" priority="61">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M71:P71">
+  <conditionalFormatting sqref="M72:P72">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
@@ -15693,7 +15802,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M72:P72">
+  <conditionalFormatting sqref="M48:P48">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -15705,7 +15814,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M48:P48">
+  <conditionalFormatting sqref="M28:P28">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -15717,7 +15826,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:P28">
+  <conditionalFormatting sqref="M29:P29">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -15729,7 +15838,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M29:P29">
+  <conditionalFormatting sqref="M78:P78">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -15741,7 +15850,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M78:P78">
+  <conditionalFormatting sqref="M85:P85">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -15753,7 +15862,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M85:P85">
+  <conditionalFormatting sqref="M60:P60">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -15765,7 +15874,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M60:P60">
+  <conditionalFormatting sqref="M25:P25">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -15777,7 +15886,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25:P25">
+  <conditionalFormatting sqref="M92:P92">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -15789,7 +15898,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M92:P92">
+  <conditionalFormatting sqref="M73:P73">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -15801,7 +15910,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M73:P73">
+  <conditionalFormatting sqref="M74:P74">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -15813,7 +15922,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M74:P74">
+  <conditionalFormatting sqref="M97:P97">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -15825,7 +15934,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M97:P97">
+  <conditionalFormatting sqref="M98:P98">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -15837,7 +15946,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M98:P98">
+  <conditionalFormatting sqref="M99:P99">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -15849,7 +15958,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M99:P99">
+  <conditionalFormatting sqref="M100:P100">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -15861,7 +15970,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M100:P100">
+  <conditionalFormatting sqref="M101:P101">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -15873,7 +15982,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M101:P101">
+  <conditionalFormatting sqref="M102:P102">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -15885,7 +15994,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M102:P102">
+  <conditionalFormatting sqref="N103:P103">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -15897,7 +16006,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N103:P103">
+  <conditionalFormatting sqref="M104:P104">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -15909,7 +16018,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M104:P104">
+  <conditionalFormatting sqref="M103">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -15921,7 +16030,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M103">
+  <conditionalFormatting sqref="O106">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -15933,7 +16042,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O106">
+  <conditionalFormatting sqref="M106">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -15945,7 +16054,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M106">
+  <conditionalFormatting sqref="N106">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -15957,32 +16066,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N106">
+  <conditionalFormatting sqref="P106">
     <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P106">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O107">
-    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16005,8 +16090,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M107">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="O107">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16017,8 +16102,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N107">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="M107">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16041,8 +16126,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P107">
-    <cfRule type="colorScale" priority="29">
+  <conditionalFormatting sqref="N107">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16053,8 +16138,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O108">
-    <cfRule type="colorScale" priority="27">
+  <conditionalFormatting sqref="P107">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16077,8 +16162,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M108">
-    <cfRule type="colorScale" priority="26">
+  <conditionalFormatting sqref="O108">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16089,8 +16174,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N108">
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="M108">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16113,7 +16198,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N108">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="P108">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O109:P109">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -16125,32 +16234,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O109:P109">
+  <conditionalFormatting sqref="M109">
     <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M109">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N109">
-    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16173,7 +16258,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N109">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M110:P110">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M111:P111">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -16185,7 +16294,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M111:P111">
+  <conditionalFormatting sqref="O105">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -16197,7 +16306,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O105">
+  <conditionalFormatting sqref="M105">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -16209,7 +16318,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M105">
+  <conditionalFormatting sqref="N105">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -16221,7 +16330,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N105">
+  <conditionalFormatting sqref="P105">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -16233,7 +16342,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P105">
+  <conditionalFormatting sqref="M112:P112">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -16245,7 +16354,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M112:P112">
+  <conditionalFormatting sqref="M88:P88">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -16257,20 +16366,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M88:P88">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M113:P113">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16282,7 +16379,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M114:P115">
-    <cfRule type="colorScale" priority="63">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16294,6 +16391,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:P116">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M117:P117">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -16305,7 +16414,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M117:P117">
+  <conditionalFormatting sqref="M118:P118">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -16317,7 +16426,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M118:P118">
+  <conditionalFormatting sqref="M119:P119">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -16329,7 +16438,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M119:P119">
+  <conditionalFormatting sqref="M120:P120">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -16341,8 +16450,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M120:P120">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="M121:P121">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16353,7 +16462,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M121:P121">
+  <conditionalFormatting sqref="M122:P122">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -16367,32 +16476,32 @@
   </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G42"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I121">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I122">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D126:G136 P23:V121 M23:N121">
+    <dataValidation type="decimal" allowBlank="1" sqref="D127:G137 M23:N122 P23:V122">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H126:L135 H136:I136 W23:Z121">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H127:L136 H137:I137 W23:Z122">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C126:C136 C23:C121">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C127:C137 C23:C122">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="M126:O136 J136:L136 AA100:AA121 AA23:AA98 AB23:AE121"/>
-    <dataValidation type="list" sqref="O23:O121">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="M127:O137 J137:L137 AA100:AA122 AA23:AA98 AB23:AE122"/>
+    <dataValidation type="list" sqref="O23:O122">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K121">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K122">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F121">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F122">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="L23:L121">
+    <dataValidation type="list" sqref="L23:L122">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Content updated. New entities changes
Former-commit-id: 2f42be7c70572c4e4eb7b8010faf23298317922c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -2514,56 +2514,56 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5221,7 +5221,7 @@
     <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="B123" sqref="B123"/>
+      <selection pane="topRight" activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5265,8 +5265,8 @@
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
-      <c r="E3" s="206"/>
-      <c r="F3" s="206"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
       <c r="G3" s="23"/>
       <c r="H3" s="22"/>
       <c r="I3" s="171"/>
@@ -5422,8 +5422,8 @@
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="206"/>
-      <c r="F21" s="206"/>
+      <c r="E21" s="222"/>
+      <c r="F21" s="222"/>
       <c r="G21" s="23"/>
       <c r="H21" s="22"/>
       <c r="I21" s="23"/>
@@ -13230,7 +13230,7 @@
       <c r="O105" s="38">
         <v>0</v>
       </c>
-      <c r="P105" s="37">
+      <c r="P105" s="47">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>0</v>
       </c>
@@ -13322,7 +13322,7 @@
       <c r="O106" s="38">
         <v>0</v>
       </c>
-      <c r="P106" s="37">
+      <c r="P106" s="47">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>0</v>
       </c>
@@ -13782,7 +13782,7 @@
       <c r="O111" s="38">
         <v>5</v>
       </c>
-      <c r="P111" s="37">
+      <c r="P111" s="47">
         <v>4</v>
       </c>
       <c r="Q111" s="57" t="b">
@@ -13873,7 +13873,7 @@
       <c r="O112" s="38">
         <v>0</v>
       </c>
-      <c r="P112" s="37">
+      <c r="P112" s="47">
         <v>0</v>
       </c>
       <c r="Q112" s="57" t="b">
@@ -13945,7 +13945,7 @@
         <v>1</v>
       </c>
       <c r="J113" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K113" s="118">
         <v>0</v>
@@ -14037,7 +14037,7 @@
         <v>1</v>
       </c>
       <c r="J114" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K114" s="70">
         <v>0</v>
@@ -14129,7 +14129,7 @@
         <v>1</v>
       </c>
       <c r="J115" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K115" s="70">
         <v>0</v>
@@ -14212,7 +14212,7 @@
         <v>0</v>
       </c>
       <c r="G116" s="70">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H116" s="70">
         <v>0</v>
@@ -14221,7 +14221,7 @@
         <v>1</v>
       </c>
       <c r="J116" s="193">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K116" s="70">
         <v>0</v>
@@ -14317,7 +14317,7 @@
         <v>1</v>
       </c>
       <c r="J117" s="193">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K117" s="70">
         <v>0</v>
@@ -14505,7 +14505,7 @@
         <v>1</v>
       </c>
       <c r="J119" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K119" s="70">
         <v>0</v>
@@ -14597,7 +14597,7 @@
         <v>1</v>
       </c>
       <c r="J120" s="193">
-        <v>0.22499999999999998</v>
+        <v>0</v>
       </c>
       <c r="K120" s="70">
         <v>0</v>
@@ -14692,7 +14692,7 @@
         <v>1</v>
       </c>
       <c r="J121" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K121" s="70">
         <v>0</v>
@@ -14784,7 +14784,7 @@
         <v>1</v>
       </c>
       <c r="J122" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K122" s="70">
         <v>0</v>
@@ -14875,7 +14875,7 @@
         <v>1</v>
       </c>
       <c r="J123" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K123" s="70">
         <v>0</v>
@@ -14966,7 +14966,7 @@
         <v>1</v>
       </c>
       <c r="J124" s="193">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K124" s="70">
         <v>0</v>
@@ -14981,11 +14981,11 @@
         <v>5</v>
       </c>
       <c r="O124" s="198">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P124" s="202">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q124" s="148" t="b">
         <v>1</v>
@@ -15062,7 +15062,7 @@
         <v>1</v>
       </c>
       <c r="J125" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K125" s="70">
         <v>0</v>
@@ -15153,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="J126" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K126" s="70">
         <v>0</v>
@@ -15244,7 +15244,7 @@
         <v>1</v>
       </c>
       <c r="J127" s="193">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="K127" s="70">
         <v>0</v>
@@ -15259,10 +15259,10 @@
         <v>5</v>
       </c>
       <c r="O127" s="198">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P127" s="202">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q127" s="148" t="b">
         <v>1</v>
@@ -15335,7 +15335,7 @@
         <v>1</v>
       </c>
       <c r="J128" s="193">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K128" s="70">
         <v>0</v>
@@ -15430,7 +15430,7 @@
         <v>1</v>
       </c>
       <c r="J129" s="193">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K129" s="70">
         <v>0</v>
@@ -15497,37 +15497,37 @@
       </c>
     </row>
     <row r="130" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A130" s="207"/>
-      <c r="B130" s="207"/>
-      <c r="C130" s="207"/>
-      <c r="D130" s="208"/>
-      <c r="E130" s="209"/>
-      <c r="F130" s="209"/>
-      <c r="G130" s="209"/>
-      <c r="H130" s="209"/>
-      <c r="I130" s="209"/>
-      <c r="J130" s="210"/>
-      <c r="K130" s="209"/>
-      <c r="L130" s="211"/>
-      <c r="M130" s="212"/>
-      <c r="N130" s="212"/>
-      <c r="O130" s="213"/>
-      <c r="P130" s="212"/>
-      <c r="Q130" s="214"/>
-      <c r="R130" s="215"/>
-      <c r="S130" s="215"/>
-      <c r="T130" s="214"/>
-      <c r="U130" s="215"/>
-      <c r="V130" s="216"/>
-      <c r="W130" s="217"/>
-      <c r="X130" s="218"/>
-      <c r="Y130" s="218"/>
-      <c r="Z130" s="219"/>
-      <c r="AA130" s="220"/>
-      <c r="AB130" s="220"/>
-      <c r="AC130" s="221"/>
-      <c r="AD130" s="221"/>
-      <c r="AE130" s="222"/>
+      <c r="A130" s="206"/>
+      <c r="B130" s="206"/>
+      <c r="C130" s="206"/>
+      <c r="D130" s="207"/>
+      <c r="E130" s="208"/>
+      <c r="F130" s="208"/>
+      <c r="G130" s="208"/>
+      <c r="H130" s="208"/>
+      <c r="I130" s="208"/>
+      <c r="J130" s="209"/>
+      <c r="K130" s="208"/>
+      <c r="L130" s="210"/>
+      <c r="M130" s="211"/>
+      <c r="N130" s="211"/>
+      <c r="O130" s="212"/>
+      <c r="P130" s="211"/>
+      <c r="Q130" s="213"/>
+      <c r="R130" s="214"/>
+      <c r="S130" s="214"/>
+      <c r="T130" s="213"/>
+      <c r="U130" s="214"/>
+      <c r="V130" s="215"/>
+      <c r="W130" s="216"/>
+      <c r="X130" s="217"/>
+      <c r="Y130" s="217"/>
+      <c r="Z130" s="218"/>
+      <c r="AA130" s="219"/>
+      <c r="AB130" s="219"/>
+      <c r="AC130" s="220"/>
+      <c r="AD130" s="220"/>
+      <c r="AE130" s="221"/>
     </row>
     <row r="131" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="132" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
@@ -15567,8 +15567,8 @@
       <c r="C133" s="23"/>
       <c r="D133" s="23"/>
       <c r="E133" s="23"/>
-      <c r="F133" s="206"/>
-      <c r="G133" s="206"/>
+      <c r="F133" s="222"/>
+      <c r="G133" s="222"/>
       <c r="H133" s="22" t="s">
         <v>56</v>
       </c>
@@ -17347,8 +17347,8 @@
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="206"/>
-      <c r="G3" s="206"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
       <c r="H3" s="23"/>
       <c r="I3" s="22"/>
       <c r="J3" s="171"/>

</xml_diff>

<commit_message>
FallingRock is an entity, and spiderweb a decoration
Former-commit-id: e82de2cca41dedfaa782e2d1b08bd059967aecc7
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$134:$O$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$135:$O$136</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="481">
   <si>
     <t>tier_4</t>
   </si>
@@ -1471,7 +1471,7 @@
     <t>spiderweb</t>
   </si>
   <si>
-    <t>fallingRock</t>
+    <t>FallingRock</t>
   </si>
 </sst>
 </file>
@@ -2009,7 +2009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="269">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2742,19 +2742,31 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="95">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5030,113 +5042,113 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE129" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A22:AE129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A22:AE130" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+  <autoFilter ref="A22:AE130"/>
   <sortState ref="A23:AE109">
     <sortCondition ref="B22:B109"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="78"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="77"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="76"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="75"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="74"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="73"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="72"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="71"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="70"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="69"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="68"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="67"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="66"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="65"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="61"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="60"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="59"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="58"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="57"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="89"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
+    <tableColumn id="6" name="[category]" dataDxfId="87"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="86"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="85"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="84"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="83"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="82"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="81"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="80"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="79"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="78"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="77"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="76"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="75"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="74"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="73"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="72"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="71"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="70"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="69"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="68"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="67"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="66"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="65"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="63"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="62"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="61"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="60"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B17" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B17" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <autoFilter ref="A4:B17"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="52"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="54"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A134:O147" totalsRowShown="0">
-  <autoFilter ref="A134:O147"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A135:O147" totalsRowShown="0">
+  <autoFilter ref="A135:O147"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="4" name="[category]" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="16" name="[size]" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="4" name="[category]" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="16" name="[size]" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="16"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="6" name="[order]" dataDxfId="14"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="13"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="12"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="11"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="10"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="18"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="6" name="[order]" dataDxfId="16"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="15"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="14"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="13"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="4"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="3"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="2"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="6"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="4"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="3" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5410,10 +5422,10 @@
   </sheetPr>
   <dimension ref="A1:AE164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="J148" sqref="J148"/>
+      <selection pane="topRight" activeCell="AA130" sqref="AA130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5457,8 +5469,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="266"/>
-      <c r="F3" s="266"/>
+      <c r="E3" s="268"/>
+      <c r="F3" s="268"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="126"/>
@@ -5614,8 +5626,8 @@
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="22"/>
-      <c r="E21" s="266"/>
-      <c r="F21" s="266"/>
+      <c r="E21" s="268"/>
+      <c r="F21" s="268"/>
       <c r="G21" s="22"/>
       <c r="H21" s="21"/>
       <c r="I21" s="22"/>
@@ -15689,215 +15701,251 @@
       </c>
     </row>
     <row r="130" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A130" s="157"/>
-      <c r="B130" s="157"/>
-      <c r="C130" s="157"/>
-      <c r="D130" s="158"/>
-      <c r="E130" s="159"/>
-      <c r="F130" s="159"/>
-      <c r="G130" s="159"/>
-      <c r="H130" s="159"/>
-      <c r="I130" s="159"/>
-      <c r="J130" s="160"/>
-      <c r="K130" s="159"/>
-      <c r="L130" s="161"/>
-      <c r="M130" s="162"/>
-      <c r="N130" s="162"/>
-      <c r="O130" s="163"/>
-      <c r="P130" s="162"/>
-      <c r="Q130" s="164"/>
-      <c r="R130" s="165"/>
-      <c r="S130" s="165"/>
-      <c r="T130" s="164"/>
-      <c r="U130" s="165"/>
-      <c r="V130" s="166"/>
-      <c r="W130" s="167"/>
-      <c r="X130" s="168"/>
-      <c r="Y130" s="168"/>
-      <c r="Z130" s="169"/>
-      <c r="AA130" s="170"/>
-      <c r="AB130" s="170"/>
-      <c r="AC130" s="171"/>
-      <c r="AD130" s="171"/>
-      <c r="AE130" s="172"/>
-    </row>
-    <row r="131" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="132" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A132" s="9" t="s">
+      <c r="A130" s="234" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" s="235" t="s">
+        <v>480</v>
+      </c>
+      <c r="C130" s="236" t="s">
+        <v>38</v>
+      </c>
+      <c r="D130" s="239">
+        <v>1</v>
+      </c>
+      <c r="E130" s="239">
+        <v>1</v>
+      </c>
+      <c r="F130" s="239">
+        <v>0</v>
+      </c>
+      <c r="G130" s="239">
+        <v>0</v>
+      </c>
+      <c r="H130" s="239">
+        <v>0</v>
+      </c>
+      <c r="I130" s="239">
+        <v>1</v>
+      </c>
+      <c r="J130" s="238">
+        <v>0</v>
+      </c>
+      <c r="K130" s="239">
+        <v>0</v>
+      </c>
+      <c r="L130" s="52" t="b">
+        <v>0</v>
+      </c>
+      <c r="M130" s="155">
+        <v>5</v>
+      </c>
+      <c r="N130" s="155">
+        <v>5</v>
+      </c>
+      <c r="O130" s="151">
+        <v>5</v>
+      </c>
+      <c r="P130" s="155">
+        <v>2</v>
+      </c>
+      <c r="Q130" s="76" t="b">
+        <v>1</v>
+      </c>
+      <c r="R130" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="S130" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="T130" s="110">
+        <v>1</v>
+      </c>
+      <c r="U130" s="152">
+        <v>1</v>
+      </c>
+      <c r="V130" s="153">
+        <v>0</v>
+      </c>
+      <c r="W130" s="253">
+        <v>0</v>
+      </c>
+      <c r="X130" s="255">
+        <v>0</v>
+      </c>
+      <c r="Y130" s="255">
+        <v>0</v>
+      </c>
+      <c r="Z130" s="255">
+        <v>0</v>
+      </c>
+      <c r="AA130" s="262"/>
+      <c r="AB130" s="25"/>
+      <c r="AC130" s="25"/>
+      <c r="AD130" s="25"/>
+      <c r="AE130" s="24"/>
+    </row>
+    <row r="131" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A131" s="157"/>
+      <c r="B131" s="157"/>
+      <c r="C131" s="157"/>
+      <c r="D131" s="158"/>
+      <c r="E131" s="159"/>
+      <c r="F131" s="159"/>
+      <c r="G131" s="159"/>
+      <c r="H131" s="159"/>
+      <c r="I131" s="159"/>
+      <c r="J131" s="160"/>
+      <c r="K131" s="159"/>
+      <c r="L131" s="161"/>
+      <c r="M131" s="162"/>
+      <c r="N131" s="162"/>
+      <c r="O131" s="163"/>
+      <c r="P131" s="162"/>
+      <c r="Q131" s="164"/>
+      <c r="R131" s="165"/>
+      <c r="S131" s="165"/>
+      <c r="T131" s="164"/>
+      <c r="U131" s="165"/>
+      <c r="V131" s="166"/>
+      <c r="W131" s="167"/>
+      <c r="X131" s="168"/>
+      <c r="Y131" s="168"/>
+      <c r="Z131" s="169"/>
+      <c r="AA131" s="170"/>
+      <c r="AB131" s="170"/>
+      <c r="AC131" s="171"/>
+      <c r="AD131" s="171"/>
+      <c r="AE131" s="172"/>
+    </row>
+    <row r="132" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="133" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A133" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B132" s="9"/>
-      <c r="C132" s="9"/>
-      <c r="D132" s="9"/>
-      <c r="E132" s="9"/>
-      <c r="F132" s="9"/>
-      <c r="G132" s="9"/>
-      <c r="H132" s="9"/>
-      <c r="I132" s="9"/>
-      <c r="J132" s="9"/>
-      <c r="K132" s="9"/>
-      <c r="L132" s="9"/>
-      <c r="M132" s="9"/>
-      <c r="N132" s="9"/>
-      <c r="O132" s="9"/>
-      <c r="P132" s="9"/>
-      <c r="Q132" s="9"/>
-      <c r="R132" s="9"/>
-      <c r="S132" s="9"/>
-      <c r="T132" s="9"/>
-      <c r="U132" s="9"/>
-      <c r="V132" s="9"/>
-      <c r="W132" s="9"/>
-      <c r="X132" s="9"/>
-      <c r="Y132" s="9"/>
-      <c r="Z132" s="9"/>
-      <c r="AA132" s="9"/>
-    </row>
-    <row r="133" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="22"/>
-      <c r="B133" s="22"/>
-      <c r="C133" s="22"/>
-      <c r="D133" s="22"/>
-      <c r="E133" s="22"/>
-      <c r="F133" s="266"/>
-      <c r="G133" s="266"/>
-      <c r="H133" s="21" t="s">
+      <c r="B133" s="9"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="9"/>
+      <c r="K133" s="9"/>
+      <c r="L133" s="9"/>
+      <c r="M133" s="9"/>
+      <c r="N133" s="9"/>
+      <c r="O133" s="9"/>
+      <c r="P133" s="9"/>
+      <c r="Q133" s="9"/>
+      <c r="R133" s="9"/>
+      <c r="S133" s="9"/>
+      <c r="T133" s="9"/>
+      <c r="U133" s="9"/>
+      <c r="V133" s="9"/>
+      <c r="W133" s="9"/>
+      <c r="X133" s="9"/>
+      <c r="Y133" s="9"/>
+      <c r="Z133" s="9"/>
+      <c r="AA133" s="9"/>
+    </row>
+    <row r="134" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="22"/>
+      <c r="B134" s="22"/>
+      <c r="C134" s="22"/>
+      <c r="D134" s="22"/>
+      <c r="E134" s="22"/>
+      <c r="F134" s="268"/>
+      <c r="G134" s="268"/>
+      <c r="H134" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I133" s="21"/>
-      <c r="J133" s="22"/>
-      <c r="K133" s="17"/>
-      <c r="L133" s="17"/>
-      <c r="M133" s="17" t="s">
+      <c r="I134" s="21"/>
+      <c r="J134" s="22"/>
+      <c r="K134" s="17"/>
+      <c r="L134" s="17"/>
+      <c r="M134" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N133" s="17"/>
-      <c r="O133" s="17"/>
-      <c r="P133" s="17"/>
-      <c r="Q133" s="17"/>
-      <c r="R133" s="17"/>
-      <c r="S133" s="17"/>
-      <c r="T133" s="17"/>
-      <c r="U133" s="17"/>
-      <c r="V133" s="17"/>
-      <c r="W133" s="17"/>
-      <c r="X133" s="17"/>
-      <c r="Y133" s="17"/>
-      <c r="Z133" s="17"/>
-      <c r="AA133" s="21"/>
-      <c r="AB133" s="21"/>
-      <c r="AC133" s="21"/>
-      <c r="AD133" s="21"/>
-      <c r="AE133" s="17"/>
-    </row>
-    <row r="134" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="7" t="s">
+      <c r="N134" s="17"/>
+      <c r="O134" s="17"/>
+      <c r="P134" s="17"/>
+      <c r="Q134" s="17"/>
+      <c r="R134" s="17"/>
+      <c r="S134" s="17"/>
+      <c r="T134" s="17"/>
+      <c r="U134" s="17"/>
+      <c r="V134" s="17"/>
+      <c r="W134" s="17"/>
+      <c r="X134" s="17"/>
+      <c r="Y134" s="17"/>
+      <c r="Z134" s="17"/>
+      <c r="AA134" s="21"/>
+      <c r="AB134" s="21"/>
+      <c r="AC134" s="21"/>
+      <c r="AD134" s="21"/>
+      <c r="AE134" s="17"/>
+    </row>
+    <row r="135" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B134" s="7" t="s">
+      <c r="B135" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C135" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D134" s="20" t="s">
+      <c r="D135" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E134" s="20" t="s">
+      <c r="E135" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F134" s="20" t="s">
+      <c r="F135" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G134" s="20" t="s">
+      <c r="G135" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H134" s="20" t="s">
+      <c r="H135" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I134" s="20" t="s">
+      <c r="I135" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J134" s="20" t="s">
+      <c r="J135" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K134" s="20" t="s">
+      <c r="K135" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="L134" s="20" t="s">
+      <c r="L135" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M134" s="19" t="s">
+      <c r="M135" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N134" s="19" t="s">
+      <c r="N135" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O134" s="19" t="s">
+      <c r="O135" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="135" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A135" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B135" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C135" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D135" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E135" s="14">
-        <v>3</v>
-      </c>
-      <c r="F135" s="18">
-        <v>0</v>
-      </c>
-      <c r="G135" s="18">
-        <v>0</v>
-      </c>
-      <c r="H135" s="18">
-        <v>0</v>
-      </c>
-      <c r="I135" s="18">
-        <v>0</v>
-      </c>
-      <c r="J135" s="12">
-        <v>2</v>
-      </c>
-      <c r="K135" s="12">
-        <v>0</v>
-      </c>
-      <c r="L135" s="12">
-        <v>0</v>
-      </c>
-      <c r="M135" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N135" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O135" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P135" s="17"/>
-      <c r="Q135" s="17"/>
     </row>
     <row r="136" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A136" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B136" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C136" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E136" s="14">
         <v>3</v>
@@ -15906,7 +15954,7 @@
         <v>0</v>
       </c>
       <c r="G136" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H136" s="18">
         <v>0</v>
@@ -15940,13 +15988,13 @@
         <v>2</v>
       </c>
       <c r="B137" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E137" s="14">
         <v>3</v>
@@ -15955,7 +16003,7 @@
         <v>0</v>
       </c>
       <c r="G137" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H137" s="18">
         <v>0</v>
@@ -15989,13 +16037,13 @@
         <v>2</v>
       </c>
       <c r="B138" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C138" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E138" s="14">
         <v>3</v>
@@ -16004,7 +16052,7 @@
         <v>0</v>
       </c>
       <c r="G138" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H138" s="18">
         <v>0</v>
@@ -16038,13 +16086,13 @@
         <v>2</v>
       </c>
       <c r="B139" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E139" s="14">
         <v>3</v>
@@ -16053,7 +16101,7 @@
         <v>0</v>
       </c>
       <c r="G139" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H139" s="18">
         <v>0</v>
@@ -16087,13 +16135,13 @@
         <v>2</v>
       </c>
       <c r="B140" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C140" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E140" s="14">
         <v>3</v>
@@ -16102,7 +16150,7 @@
         <v>0</v>
       </c>
       <c r="G140" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H140" s="18">
         <v>0</v>
@@ -16136,13 +16184,13 @@
         <v>2</v>
       </c>
       <c r="B141" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C141" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E141" s="14">
         <v>3</v>
@@ -16151,7 +16199,7 @@
         <v>0</v>
       </c>
       <c r="G141" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H141" s="18">
         <v>0</v>
@@ -16185,13 +16233,13 @@
         <v>2</v>
       </c>
       <c r="B142" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E142" s="14">
         <v>3</v>
@@ -16200,7 +16248,7 @@
         <v>0</v>
       </c>
       <c r="G142" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H142" s="18">
         <v>0</v>
@@ -16234,13 +16282,13 @@
         <v>2</v>
       </c>
       <c r="B143" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C143" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E143" s="14">
         <v>3</v>
@@ -16249,7 +16297,7 @@
         <v>0</v>
       </c>
       <c r="G143" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H143" s="18">
         <v>0</v>
@@ -16283,13 +16331,13 @@
         <v>2</v>
       </c>
       <c r="B144" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C144" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E144" s="14">
         <v>3</v>
@@ -16298,7 +16346,7 @@
         <v>0</v>
       </c>
       <c r="G144" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H144" s="18">
         <v>0</v>
@@ -16332,27 +16380,27 @@
         <v>2</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E145" s="14">
-        <v>1</v>
-      </c>
-      <c r="F145" s="13">
-        <v>0</v>
-      </c>
-      <c r="G145" s="13">
-        <v>1</v>
-      </c>
-      <c r="H145" s="13">
-        <v>0</v>
-      </c>
-      <c r="I145" s="13">
+        <v>3</v>
+      </c>
+      <c r="F145" s="18">
+        <v>0</v>
+      </c>
+      <c r="G145" s="18">
+        <v>2</v>
+      </c>
+      <c r="H145" s="18">
+        <v>0</v>
+      </c>
+      <c r="I145" s="18">
         <v>0</v>
       </c>
       <c r="J145" s="12">
@@ -16373,33 +16421,35 @@
       <c r="O145" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P145" s="17"/>
+      <c r="Q145" s="17"/>
     </row>
     <row r="146" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A146" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B146" s="124" t="s">
-        <v>479</v>
-      </c>
-      <c r="C146" s="124" t="s">
-        <v>38</v>
-      </c>
-      <c r="D146" s="267" t="s">
-        <v>30</v>
+      <c r="B146" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C146" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D146" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E146" s="14">
         <v>1</v>
       </c>
-      <c r="F146" s="268">
-        <v>0</v>
-      </c>
-      <c r="G146" s="268">
-        <v>0</v>
-      </c>
-      <c r="H146" s="268">
-        <v>0</v>
-      </c>
-      <c r="I146" s="268">
+      <c r="F146" s="13">
+        <v>0</v>
+      </c>
+      <c r="G146" s="13">
+        <v>1</v>
+      </c>
+      <c r="H146" s="13">
+        <v>0</v>
+      </c>
+      <c r="I146" s="13">
         <v>0</v>
       </c>
       <c r="J146" s="12">
@@ -16420,53 +16470,37 @@
       <c r="O146" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P146" s="8"/>
-      <c r="Q146" s="8"/>
-      <c r="R146" s="8"/>
-      <c r="S146" s="8"/>
-      <c r="T146" s="8"/>
-      <c r="U146" s="8"/>
-      <c r="V146" s="8"/>
-      <c r="W146" s="8"/>
-      <c r="X146" s="8"/>
-      <c r="Y146" s="8"/>
-      <c r="Z146" s="8"/>
-      <c r="AA146" s="8"/>
-      <c r="AB146" s="8"/>
-      <c r="AC146" s="8"/>
-      <c r="AD146" s="8"/>
-      <c r="AE146" s="8"/>
     </row>
     <row r="147" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A147" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B147" s="15" t="s">
-        <v>480</v>
-      </c>
-      <c r="C147" s="15" t="s">
+      <c r="B147" s="124" t="s">
+        <v>479</v>
+      </c>
+      <c r="C147" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="D147" s="269" t="s">
-        <v>23</v>
+      <c r="D147" s="266" t="s">
+        <v>30</v>
       </c>
       <c r="E147" s="14">
-        <v>4</v>
-      </c>
-      <c r="F147" s="270">
-        <v>0</v>
-      </c>
-      <c r="G147" s="270">
-        <v>2</v>
-      </c>
-      <c r="H147" s="270">
-        <v>0</v>
-      </c>
-      <c r="I147" s="270">
+        <v>1</v>
+      </c>
+      <c r="F147" s="267">
+        <v>0</v>
+      </c>
+      <c r="G147" s="267">
+        <v>0</v>
+      </c>
+      <c r="H147" s="267">
+        <v>0</v>
+      </c>
+      <c r="I147" s="267">
         <v>0</v>
       </c>
       <c r="J147" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K147" s="12">
         <v>0</v>
@@ -16777,15 +16811,32 @@
   <mergeCells count="3">
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F133:G133"/>
+    <mergeCell ref="F134:G134"/>
   </mergeCells>
-  <conditionalFormatting sqref="L23:L129 Q23:Q129 R23:S129">
-    <cfRule type="expression" dxfId="0" priority="7">
+  <conditionalFormatting sqref="L23:L129 Q23:S129">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>L23=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23:P129">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L130 Q130:S130">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>L130=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M130:P130">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16798,32 +16849,32 @@
   </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G42"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I130">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G23:I40 G43:I131">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D135:G147 M23:N130 P23:V130">
+    <dataValidation type="decimal" allowBlank="1" sqref="D136:G147 M23:N131 P23:V131">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H135:L144 H145:I145 W23:Z130 J146:L146">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H136:L145 H146:I146 W23:Z131 J147:L147">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C135:C147 C23:C130">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C136:C147 C23:C131">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J147:L147 J145:L145 AA23:AA98 AA100:AA130 AB23:AE130 M135:O147"/>
-    <dataValidation type="list" sqref="O23:O130">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J146:L146 AA23:AA98 AA100:AA131 AB23:AE131 M136:O147"/>
+    <dataValidation type="list" sqref="O23:O131">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K130">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J23:K131">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F130">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D23:F131">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="L23:L130">
+    <dataValidation type="list" sqref="L23:L131">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16878,8 +16929,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="266"/>
-      <c r="G3" s="266"/>
+      <c r="F3" s="268"/>
+      <c r="G3" s="268"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="126"/>

</xml_diff>

<commit_message>
Added latch to HermitCrabBlue and Butterfly
Former-commit-id: 8dda4fec92996769de36e642a07f6d3cfe2bba44
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -2755,28 +2755,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="95">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="94">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5031,6 +5010,20 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5045,57 +5038,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AE131" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AE131" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
   <autoFilter ref="A23:AE131"/>
   <sortState ref="A23:AE109">
     <sortCondition ref="B22:B109"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="89"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
-    <tableColumn id="6" name="[category]" dataDxfId="87"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="86"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="85"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="84"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="83"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="82"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="81"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="80"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="79"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="78"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="77"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="76"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="75"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="74"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="73"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="72"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="71"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="70"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="69"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="68"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="67"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="66"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="65"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="63"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="62"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="61"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="60"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="59"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="86"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
+    <tableColumn id="6" name="[category]" dataDxfId="84"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="83"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="82"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="81"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="80"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="79"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="54"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="53"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5108,50 +5101,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="4" name="[category]" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="16" name="[size]" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="18"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
-    <tableColumn id="6" name="[order]" dataDxfId="16"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="15"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="14"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="13"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="12"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="6"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="4"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5425,10 +5418,10 @@
   </sheetPr>
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="C133" sqref="C133"/>
+      <selection pane="topRight" activeCell="M114" sqref="M114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14169,17 +14162,17 @@
         <v>1</v>
       </c>
       <c r="M114" s="148">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N114" s="148">
         <v>5</v>
       </c>
       <c r="O114" s="149">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P114" s="148">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q114" s="76" t="b">
         <v>1</v>
@@ -14188,7 +14181,7 @@
         <v>0</v>
       </c>
       <c r="S114" s="76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T114" s="110">
         <v>1</v>
@@ -14821,13 +14814,13 @@
         <v>1</v>
       </c>
       <c r="M121" s="155">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N121" s="155">
         <v>5</v>
       </c>
       <c r="O121" s="151">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P121" s="155">
         <v>0</v>
@@ -16825,7 +16818,7 @@
     <mergeCell ref="F135:G135"/>
   </mergeCells>
   <conditionalFormatting sqref="L24:L130 Q24:S130">
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="93" priority="9">
       <formula>L24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16842,7 +16835,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L131 Q131:S131">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="92" priority="2">
       <formula>L131=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Setting HP values to Butterfly and GrabBigBlue
Former-commit-id: bb109080706e4df09133b65fd147295307ef07e0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5418,10 +5418,10 @@
   </sheetPr>
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="M114" sqref="M114"/>
+      <selection pane="topRight" activeCell="T122" sqref="T122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14171,8 +14171,7 @@
         <v>4</v>
       </c>
       <c r="P114" s="148">
-        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q114" s="76" t="b">
         <v>1</v>
@@ -14184,7 +14183,7 @@
         <v>1</v>
       </c>
       <c r="T114" s="110">
-        <v>1</v>
+        <v>600</v>
       </c>
       <c r="U114" s="150">
         <v>14</v>
@@ -14835,7 +14834,7 @@
         <v>1</v>
       </c>
       <c r="T121" s="110">
-        <v>1</v>
+        <v>600</v>
       </c>
       <c r="U121" s="152">
         <v>12</v>

</xml_diff>

<commit_message>
[TEXTS] Adding TIDs to the table
Former-commit-id: ba56eb6cd0a8ac1a50a1f1af5f0c70071f3a6201
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="2" r:id="rId1"/>
@@ -1312,78 +1312,30 @@
     <t>SURVIVAL BONUS DEFINITIONS</t>
   </si>
   <si>
-    <t>God!</t>
-  </si>
-  <si>
     <t>&lt;FeedbackMessage&gt;</t>
   </si>
   <si>
     <t>multiplier_8</t>
   </si>
   <si>
-    <t>You've got the power!</t>
-  </si>
-  <si>
     <t>multiplier_7</t>
   </si>
   <si>
-    <t>It's over 9000!</t>
-  </si>
-  <si>
     <t>multiplier_6</t>
   </si>
   <si>
-    <t>Amazing!</t>
-  </si>
-  <si>
     <t>multiplier_5</t>
   </si>
   <si>
-    <t>Annihilator!</t>
-  </si>
-  <si>
-    <t>Legendary!</t>
-  </si>
-  <si>
-    <t>Terror of the Skies!</t>
-  </si>
-  <si>
     <t>multiplier_4</t>
   </si>
   <si>
-    <t>Kill'em'all!</t>
-  </si>
-  <si>
-    <t>Infamous!</t>
-  </si>
-  <si>
-    <t>Killing Beast!</t>
-  </si>
-  <si>
     <t>multiplier_3</t>
   </si>
   <si>
-    <t>Causing Panic!</t>
-  </si>
-  <si>
-    <t>Hungry Dragon!</t>
-  </si>
-  <si>
-    <t>Run you fools!</t>
-  </si>
-  <si>
     <t>multiplier_2</t>
   </si>
   <si>
-    <t>Serious Stuff!</t>
-  </si>
-  <si>
-    <t>Kill Streak!</t>
-  </si>
-  <si>
-    <t>Bird Killer!</t>
-  </si>
-  <si>
     <t>multiplier_1</t>
   </si>
   <si>
@@ -1475,6 +1427,54 @@
   </si>
   <si>
     <t>hazards</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X1_01</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X1_02</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X1_03</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X2_01</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X2_02</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X2_03</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X3_01</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X3_02</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X3_03</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X4_01</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X4_02</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X4_03</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X5_01</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X7_01</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X6_01</t>
+  </si>
+  <si>
+    <t>TID_FEEDBACK_SCORE_X8_01</t>
   </si>
 </sst>
 </file>
@@ -5418,8 +5418,8 @@
   </sheetPr>
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
       <selection pane="topRight" activeCell="T122" sqref="T122"/>
     </sheetView>
@@ -5588,7 +5588,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -11814,7 +11814,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="215" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="C89" s="216" t="s">
         <v>84</v>
@@ -13565,7 +13565,7 @@
         <v>0</v>
       </c>
       <c r="AA107" s="47" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="AB107" s="46" t="s">
         <v>82</v>
@@ -14024,13 +14024,13 @@
         <v>0</v>
       </c>
       <c r="AA112" s="47" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
       <c r="AB112" s="46" t="s">
         <v>143</v>
       </c>
       <c r="AC112" s="46" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
       <c r="AD112" s="25"/>
       <c r="AE112" s="24"/>
@@ -14129,7 +14129,7 @@
         <v>2</v>
       </c>
       <c r="B114" s="232" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="C114" s="233" t="s">
         <v>84</v>
@@ -14220,7 +14220,7 @@
         <v>2</v>
       </c>
       <c r="B115" s="235" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="C115" s="236" t="s">
         <v>84</v>
@@ -14312,7 +14312,7 @@
         <v>2</v>
       </c>
       <c r="B116" s="67" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="C116" s="66" t="s">
         <v>84</v>
@@ -14404,7 +14404,7 @@
         <v>2</v>
       </c>
       <c r="B117" s="67" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="C117" s="66" t="s">
         <v>84</v>
@@ -14500,7 +14500,7 @@
         <v>2</v>
       </c>
       <c r="B118" s="67" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="C118" s="66" t="s">
         <v>84</v>
@@ -14596,7 +14596,7 @@
         <v>2</v>
       </c>
       <c r="B119" s="67" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="C119" s="66" t="s">
         <v>84</v>
@@ -14688,7 +14688,7 @@
         <v>2</v>
       </c>
       <c r="B120" s="235" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="C120" s="236" t="s">
         <v>84</v>
@@ -14780,7 +14780,7 @@
         <v>2</v>
       </c>
       <c r="B121" s="235" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="C121" s="236" t="s">
         <v>84</v>
@@ -14875,7 +14875,7 @@
         <v>2</v>
       </c>
       <c r="B122" s="235" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="C122" s="236" t="s">
         <v>84</v>
@@ -14967,7 +14967,7 @@
         <v>2</v>
       </c>
       <c r="B123" s="235" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
       <c r="C123" s="236" t="s">
         <v>66</v>
@@ -15058,7 +15058,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="67" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="C124" s="66" t="s">
         <v>84</v>
@@ -15149,7 +15149,7 @@
         <v>2</v>
       </c>
       <c r="B125" s="67" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
       <c r="C125" s="66" t="s">
         <v>66</v>
@@ -15245,7 +15245,7 @@
         <v>2</v>
       </c>
       <c r="B126" s="67" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="C126" s="66" t="s">
         <v>84</v>
@@ -15427,7 +15427,7 @@
         <v>2</v>
       </c>
       <c r="B128" s="235" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="C128" s="236" t="s">
         <v>84</v>
@@ -15518,7 +15518,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="235" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="C129" s="236" t="s">
         <v>66</v>
@@ -15613,7 +15613,7 @@
         <v>2</v>
       </c>
       <c r="B130" s="235" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="C130" s="236" t="s">
         <v>66</v>
@@ -15708,10 +15708,10 @@
         <v>2</v>
       </c>
       <c r="B131" s="235" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
       <c r="C131" s="236" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
       <c r="D131" s="239">
         <v>1</v>
@@ -16479,7 +16479,7 @@
         <v>2</v>
       </c>
       <c r="B148" s="124" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
       <c r="C148" s="124" t="s">
         <v>38</v>
@@ -16898,7 +16898,9 @@
   </sheetPr>
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16915,7 +16917,7 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -16941,25 +16943,25 @@
     </row>
     <row r="4" spans="2:11" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -16967,7 +16969,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
       <c r="D5" s="144">
         <v>0</v>
@@ -16988,7 +16990,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>451</v>
+        <v>435</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -17006,7 +17008,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C7" s="124"/>
       <c r="D7" s="124"/>
@@ -17014,12 +17016,12 @@
       <c r="F7" s="140"/>
       <c r="G7" s="140"/>
       <c r="H7" s="138" t="s">
-        <v>450</v>
+        <v>466</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C8" s="124"/>
       <c r="D8" s="124"/>
@@ -17027,12 +17029,12 @@
       <c r="F8" s="140"/>
       <c r="G8" s="140"/>
       <c r="H8" s="138" t="s">
-        <v>449</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C9" s="124"/>
       <c r="D9" s="124"/>
@@ -17040,7 +17042,7 @@
       <c r="F9" s="140"/>
       <c r="G9" s="140"/>
       <c r="H9" s="138" t="s">
-        <v>448</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -17048,7 +17050,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="144" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="D10" s="144">
         <v>2</v>
@@ -17066,7 +17068,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C11" s="124"/>
       <c r="D11" s="124"/>
@@ -17074,12 +17076,12 @@
       <c r="F11" s="140"/>
       <c r="G11" s="140"/>
       <c r="H11" s="138" t="s">
-        <v>446</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C12" s="124"/>
       <c r="D12" s="124"/>
@@ -17087,12 +17089,12 @@
       <c r="F12" s="140"/>
       <c r="G12" s="140"/>
       <c r="H12" s="138" t="s">
-        <v>445</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C13" s="124"/>
       <c r="D13" s="124"/>
@@ -17100,7 +17102,7 @@
       <c r="F13" s="140"/>
       <c r="G13" s="140"/>
       <c r="H13" s="138" t="s">
-        <v>444</v>
+        <v>471</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -17108,7 +17110,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="144" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D14" s="144">
         <v>3</v>
@@ -17126,7 +17128,7 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C15" s="124"/>
       <c r="D15" s="124"/>
@@ -17134,12 +17136,12 @@
       <c r="F15" s="140"/>
       <c r="G15" s="140"/>
       <c r="H15" s="138" t="s">
-        <v>442</v>
+        <v>472</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C16" s="124"/>
       <c r="D16" s="124"/>
@@ -17147,12 +17149,12 @@
       <c r="F16" s="140"/>
       <c r="G16" s="140"/>
       <c r="H16" s="138" t="s">
-        <v>441</v>
+        <v>473</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C17" s="124"/>
       <c r="D17" s="124"/>
@@ -17160,7 +17162,7 @@
       <c r="F17" s="140"/>
       <c r="G17" s="140"/>
       <c r="H17" s="138" t="s">
-        <v>440</v>
+        <v>474</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -17168,7 +17170,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="144" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="D18" s="144">
         <v>4</v>
@@ -17186,7 +17188,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C19" s="124"/>
       <c r="D19" s="124"/>
@@ -17194,12 +17196,12 @@
       <c r="F19" s="140"/>
       <c r="G19" s="140"/>
       <c r="H19" s="138" t="s">
-        <v>438</v>
+        <v>475</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C20" s="124"/>
       <c r="D20" s="124"/>
@@ -17207,12 +17209,12 @@
       <c r="F20" s="140"/>
       <c r="G20" s="140"/>
       <c r="H20" s="138" t="s">
-        <v>437</v>
+        <v>476</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C21" s="124"/>
       <c r="D21" s="124"/>
@@ -17220,7 +17222,7 @@
       <c r="F21" s="140"/>
       <c r="G21" s="140"/>
       <c r="H21" s="138" t="s">
-        <v>436</v>
+        <v>477</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -17228,7 +17230,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="124" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D22" s="124">
         <v>5</v>
@@ -17246,7 +17248,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C23" s="124"/>
       <c r="D23" s="124"/>
@@ -17254,7 +17256,7 @@
       <c r="F23" s="139"/>
       <c r="G23" s="139"/>
       <c r="H23" s="138" t="s">
-        <v>434</v>
+        <v>478</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -17262,7 +17264,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="124" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D24" s="124">
         <v>6</v>
@@ -17280,7 +17282,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C25" s="124"/>
       <c r="D25" s="124"/>
@@ -17288,7 +17290,7 @@
       <c r="F25" s="139"/>
       <c r="G25" s="139"/>
       <c r="H25" s="138" t="s">
-        <v>432</v>
+        <v>479</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -17296,7 +17298,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="124" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D26" s="124">
         <v>7</v>
@@ -17314,7 +17316,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C27" s="124"/>
       <c r="D27" s="124"/>
@@ -17322,7 +17324,7 @@
       <c r="F27" s="139"/>
       <c r="G27" s="139"/>
       <c r="H27" s="138" t="s">
-        <v>430</v>
+        <v>480</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -17330,7 +17332,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="124" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D28" s="124">
         <v>8</v>
@@ -17348,7 +17350,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C29" s="124"/>
       <c r="D29" s="124"/>
@@ -17356,7 +17358,7 @@
       <c r="F29" s="139"/>
       <c r="G29" s="139"/>
       <c r="H29" s="138" t="s">
-        <v>427</v>
+        <v>481</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Setting some spawners values
Former-commit-id: 8658247be031880fa9795518ecbe8cdf40a0fedb
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="2" r:id="rId1"/>
@@ -5418,10 +5418,10 @@
   </sheetPr>
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="T122" sqref="T122"/>
+      <selection pane="topRight" activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14183,7 +14183,7 @@
         <v>1</v>
       </c>
       <c r="T114" s="110">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="U114" s="150">
         <v>14</v>
@@ -14443,11 +14443,11 @@
         <v>5</v>
       </c>
       <c r="O117" s="151">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P117" s="155">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q117" s="76" t="b">
         <v>1</v>
@@ -14539,11 +14539,11 @@
         <v>5</v>
       </c>
       <c r="O118" s="151">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P118" s="155">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q118" s="76" t="b">
         <v>1</v>
@@ -14635,11 +14635,11 @@
         <v>5</v>
       </c>
       <c r="O119" s="151">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P119" s="155">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q119" s="76" t="b">
         <v>1</v>
@@ -14727,11 +14727,11 @@
         <v>5</v>
       </c>
       <c r="O120" s="151">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P120" s="155">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q120" s="76" t="b">
         <v>1</v>
@@ -14813,7 +14813,7 @@
         <v>1</v>
       </c>
       <c r="M121" s="155">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N121" s="155">
         <v>5</v>
@@ -14822,7 +14822,7 @@
         <v>4</v>
       </c>
       <c r="P121" s="155">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q121" s="76" t="b">
         <v>1</v>
@@ -14834,7 +14834,7 @@
         <v>1</v>
       </c>
       <c r="T121" s="110">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="U121" s="152">
         <v>12</v>
@@ -14914,11 +14914,11 @@
         <v>5</v>
       </c>
       <c r="O122" s="151">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P122" s="155">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q122" s="76" t="b">
         <v>1</v>
@@ -15006,7 +15006,7 @@
         <v>5</v>
       </c>
       <c r="O123" s="151">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P123" s="155">
         <v>0</v>
@@ -15097,10 +15097,10 @@
         <v>5</v>
       </c>
       <c r="O124" s="151">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P124" s="155">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q124" s="76" t="b">
         <v>1</v>
@@ -15188,11 +15188,11 @@
         <v>5</v>
       </c>
       <c r="O125" s="151">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P125" s="155">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q125" s="76" t="b">
         <v>1</v>
@@ -15390,7 +15390,7 @@
         <v>1</v>
       </c>
       <c r="T127" s="241">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="U127" s="151">
         <v>14</v>
@@ -15753,7 +15753,7 @@
         <v>2</v>
       </c>
       <c r="Q131" s="76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R131" s="32" t="b">
         <v>0</v>
@@ -16898,7 +16898,7 @@
   </sheetPr>
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Content - Balancing again
Former-commit-id: aa9f3829a4d4176b0a377d6b55bc0cda601fb0b2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -1590,6 +1590,7 @@
       <sz val="11"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2687,86 +2688,86 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5436,10 +5437,10 @@
   </sheetPr>
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="C29" sqref="C29"/>
+      <selection pane="topRight" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5483,8 +5484,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="248"/>
-      <c r="F3" s="248"/>
+      <c r="E3" s="274"/>
+      <c r="F3" s="274"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="122"/>
@@ -5648,8 +5649,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="248"/>
-      <c r="F22" s="248"/>
+      <c r="E22" s="274"/>
+      <c r="F22" s="274"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -6803,7 +6804,7 @@
       <c r="C35" s="219" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="252">
+      <c r="D35" s="251">
         <v>220</v>
       </c>
       <c r="E35" s="223">
@@ -6860,7 +6861,7 @@
       <c r="V35" s="106">
         <v>0</v>
       </c>
-      <c r="W35" s="265">
+      <c r="W35" s="264">
         <v>0.1</v>
       </c>
       <c r="X35" s="237">
@@ -6885,37 +6886,37 @@
       <c r="AE35" s="92"/>
     </row>
     <row r="36" spans="1:31" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="249" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="250" t="s">
+      <c r="A36" s="248" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="249" t="s">
         <v>473</v>
       </c>
-      <c r="C36" s="251" t="s">
+      <c r="C36" s="250" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="253">
+      <c r="D36" s="252">
         <v>20</v>
       </c>
-      <c r="E36" s="257">
-        <v>2</v>
-      </c>
-      <c r="F36" s="257">
-        <v>0</v>
-      </c>
-      <c r="G36" s="257">
+      <c r="E36" s="256">
+        <v>2</v>
+      </c>
+      <c r="F36" s="256">
+        <v>0</v>
+      </c>
+      <c r="G36" s="256">
         <v>15</v>
       </c>
-      <c r="H36" s="257">
-        <v>0</v>
-      </c>
-      <c r="I36" s="257">
+      <c r="H36" s="256">
+        <v>0</v>
+      </c>
+      <c r="I36" s="256">
         <v>25</v>
       </c>
       <c r="J36" s="143">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="K36" s="257">
+      <c r="K36" s="256">
         <v>0</v>
       </c>
       <c r="L36" s="106" t="b">
@@ -6952,19 +6953,19 @@
       <c r="V36" s="226">
         <v>0</v>
       </c>
-      <c r="W36" s="267">
+      <c r="W36" s="266">
         <v>0.25</v>
       </c>
-      <c r="X36" s="269">
+      <c r="X36" s="268">
         <v>0.25</v>
       </c>
-      <c r="Y36" s="269">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="269">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="270" t="s">
+      <c r="Y36" s="268">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="268">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="269" t="s">
         <v>255</v>
       </c>
       <c r="AB36" s="96" t="s">
@@ -7449,7 +7450,7 @@
       <c r="C42" s="219" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="252">
+      <c r="D42" s="251">
         <v>60</v>
       </c>
       <c r="E42" s="223">
@@ -7506,7 +7507,7 @@
       <c r="V42" s="106">
         <v>0</v>
       </c>
-      <c r="W42" s="265">
+      <c r="W42" s="264">
         <v>0.1</v>
       </c>
       <c r="X42" s="237">
@@ -7622,37 +7623,37 @@
       <c r="AE43" s="95"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A44" s="249" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="250" t="s">
+      <c r="A44" s="248" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="249" t="s">
         <v>466</v>
       </c>
-      <c r="C44" s="251" t="s">
+      <c r="C44" s="250" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="253">
+      <c r="D44" s="252">
         <v>330</v>
       </c>
-      <c r="E44" s="257">
+      <c r="E44" s="256">
         <v>20</v>
       </c>
-      <c r="F44" s="257">
-        <v>0</v>
-      </c>
-      <c r="G44" s="257">
+      <c r="F44" s="256">
+        <v>0</v>
+      </c>
+      <c r="G44" s="256">
         <v>12</v>
       </c>
-      <c r="H44" s="257">
-        <v>0</v>
-      </c>
-      <c r="I44" s="257">
+      <c r="H44" s="256">
+        <v>0</v>
+      </c>
+      <c r="I44" s="256">
         <v>143</v>
       </c>
       <c r="J44" s="143">
         <v>0.22499999999999998</v>
       </c>
-      <c r="K44" s="257">
+      <c r="K44" s="256">
         <v>0</v>
       </c>
       <c r="L44" s="106" t="b">
@@ -7689,19 +7690,19 @@
       <c r="V44" s="226">
         <v>0</v>
       </c>
-      <c r="W44" s="267">
+      <c r="W44" s="266">
         <v>0.25</v>
       </c>
-      <c r="X44" s="269">
+      <c r="X44" s="268">
         <v>0.25</v>
       </c>
-      <c r="Y44" s="269">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="269">
-        <v>0</v>
-      </c>
-      <c r="AA44" s="270" t="s">
+      <c r="Y44" s="268">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="268">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="269" t="s">
         <v>255</v>
       </c>
       <c r="AB44" s="96" t="s">
@@ -7718,37 +7719,37 @@
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A45" s="249" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="250" t="s">
+      <c r="A45" s="248" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="249" t="s">
         <v>469</v>
       </c>
-      <c r="C45" s="251" t="s">
+      <c r="C45" s="250" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="253">
+      <c r="D45" s="252">
         <v>360</v>
       </c>
-      <c r="E45" s="257">
+      <c r="E45" s="256">
         <v>49</v>
       </c>
-      <c r="F45" s="257">
-        <v>0</v>
-      </c>
-      <c r="G45" s="257">
+      <c r="F45" s="256">
+        <v>0</v>
+      </c>
+      <c r="G45" s="256">
         <v>15</v>
       </c>
-      <c r="H45" s="257">
-        <v>0</v>
-      </c>
-      <c r="I45" s="257">
+      <c r="H45" s="256">
+        <v>0</v>
+      </c>
+      <c r="I45" s="256">
         <v>130</v>
       </c>
       <c r="J45" s="143">
         <v>0.15</v>
       </c>
-      <c r="K45" s="257">
+      <c r="K45" s="256">
         <v>0</v>
       </c>
       <c r="L45" s="106" t="b">
@@ -7784,19 +7785,19 @@
       <c r="V45" s="226">
         <v>0</v>
       </c>
-      <c r="W45" s="267">
+      <c r="W45" s="266">
         <v>0.1</v>
       </c>
-      <c r="X45" s="269">
+      <c r="X45" s="268">
         <v>0.1</v>
       </c>
-      <c r="Y45" s="269">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="269">
-        <v>0</v>
-      </c>
-      <c r="AA45" s="270" t="s">
+      <c r="Y45" s="268">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="268">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="269" t="s">
         <v>144</v>
       </c>
       <c r="AB45" s="96" t="s">
@@ -9033,7 +9034,7 @@
       <c r="C59" s="219" t="s">
         <v>481</v>
       </c>
-      <c r="D59" s="252">
+      <c r="D59" s="251">
         <v>270</v>
       </c>
       <c r="E59" s="223">
@@ -9090,7 +9091,7 @@
       <c r="V59" s="106">
         <v>0</v>
       </c>
-      <c r="W59" s="265">
+      <c r="W59" s="264">
         <v>0</v>
       </c>
       <c r="X59" s="237">
@@ -9118,7 +9119,7 @@
       <c r="C60" s="219" t="s">
         <v>84</v>
       </c>
-      <c r="D60" s="252">
+      <c r="D60" s="251">
         <v>60</v>
       </c>
       <c r="E60" s="223">
@@ -9176,7 +9177,7 @@
       <c r="V60" s="106">
         <v>0</v>
       </c>
-      <c r="W60" s="265">
+      <c r="W60" s="264">
         <v>0.1</v>
       </c>
       <c r="X60" s="237">
@@ -9485,7 +9486,7 @@
       <c r="C64" s="219" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="252">
+      <c r="D64" s="251">
         <v>40</v>
       </c>
       <c r="E64" s="223">
@@ -9543,7 +9544,7 @@
       <c r="V64" s="106">
         <v>0</v>
       </c>
-      <c r="W64" s="265">
+      <c r="W64" s="264">
         <v>0.1</v>
       </c>
       <c r="X64" s="237">
@@ -11074,7 +11075,7 @@
       <c r="C81" s="219" t="s">
         <v>84</v>
       </c>
-      <c r="D81" s="252">
+      <c r="D81" s="251">
         <v>20</v>
       </c>
       <c r="E81" s="223">
@@ -11131,7 +11132,7 @@
       <c r="V81" s="106">
         <v>0</v>
       </c>
-      <c r="W81" s="265">
+      <c r="W81" s="264">
         <v>0.05</v>
       </c>
       <c r="X81" s="237">
@@ -11160,37 +11161,37 @@
       </c>
     </row>
     <row r="82" spans="1:31" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="249" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82" s="250" t="s">
+      <c r="A82" s="248" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="249" t="s">
         <v>461</v>
       </c>
-      <c r="C82" s="251" t="s">
+      <c r="C82" s="250" t="s">
         <v>84</v>
       </c>
-      <c r="D82" s="253">
+      <c r="D82" s="252">
         <v>20</v>
       </c>
-      <c r="E82" s="257">
-        <v>2</v>
-      </c>
-      <c r="F82" s="257">
-        <v>0</v>
-      </c>
-      <c r="G82" s="257">
+      <c r="E82" s="256">
+        <v>2</v>
+      </c>
+      <c r="F82" s="256">
+        <v>0</v>
+      </c>
+      <c r="G82" s="256">
         <v>10</v>
       </c>
-      <c r="H82" s="257">
-        <v>0</v>
-      </c>
-      <c r="I82" s="257">
+      <c r="H82" s="256">
+        <v>0</v>
+      </c>
+      <c r="I82" s="256">
         <v>25</v>
       </c>
       <c r="J82" s="143">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="K82" s="257">
+      <c r="K82" s="256">
         <v>0</v>
       </c>
       <c r="L82" s="106" t="b">
@@ -11227,19 +11228,19 @@
       <c r="V82" s="226">
         <v>0</v>
       </c>
-      <c r="W82" s="267">
-        <v>1</v>
-      </c>
-      <c r="X82" s="269">
-        <v>1</v>
-      </c>
-      <c r="Y82" s="269">
-        <v>0</v>
-      </c>
-      <c r="Z82" s="269">
-        <v>0</v>
-      </c>
-      <c r="AA82" s="270" t="s">
+      <c r="W82" s="266">
+        <v>1</v>
+      </c>
+      <c r="X82" s="268">
+        <v>1</v>
+      </c>
+      <c r="Y82" s="268">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="268">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="269" t="s">
         <v>354</v>
       </c>
       <c r="AB82" s="96" t="s">
@@ -11261,7 +11262,7 @@
       <c r="C83" s="219" t="s">
         <v>84</v>
       </c>
-      <c r="D83" s="252">
+      <c r="D83" s="251">
         <v>20</v>
       </c>
       <c r="E83" s="223">
@@ -11319,7 +11320,7 @@
       <c r="V83" s="106">
         <v>0</v>
       </c>
-      <c r="W83" s="265">
+      <c r="W83" s="264">
         <v>0.1</v>
       </c>
       <c r="X83" s="237">
@@ -11344,37 +11345,37 @@
       <c r="AE83" s="104"/>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A84" s="249" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" s="250" t="s">
+      <c r="A84" s="248" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" s="249" t="s">
         <v>468</v>
       </c>
-      <c r="C84" s="251" t="s">
+      <c r="C84" s="250" t="s">
         <v>84</v>
       </c>
-      <c r="D84" s="253">
+      <c r="D84" s="252">
         <v>60</v>
       </c>
-      <c r="E84" s="257">
+      <c r="E84" s="256">
         <v>4</v>
       </c>
-      <c r="F84" s="257">
-        <v>0</v>
-      </c>
-      <c r="G84" s="257">
+      <c r="F84" s="256">
+        <v>0</v>
+      </c>
+      <c r="G84" s="256">
         <v>15</v>
       </c>
-      <c r="H84" s="257">
-        <v>0</v>
-      </c>
-      <c r="I84" s="257">
+      <c r="H84" s="256">
+        <v>0</v>
+      </c>
+      <c r="I84" s="256">
         <v>55</v>
       </c>
       <c r="J84" s="143">
         <v>0.15</v>
       </c>
-      <c r="K84" s="257">
+      <c r="K84" s="256">
         <v>0</v>
       </c>
       <c r="L84" s="106" t="b">
@@ -11410,19 +11411,19 @@
       <c r="V84" s="226">
         <v>0</v>
       </c>
-      <c r="W84" s="267">
+      <c r="W84" s="266">
         <v>0.1</v>
       </c>
-      <c r="X84" s="269">
+      <c r="X84" s="268">
         <v>0.1</v>
       </c>
-      <c r="Y84" s="269">
-        <v>0</v>
-      </c>
-      <c r="Z84" s="269">
-        <v>0</v>
-      </c>
-      <c r="AA84" s="270" t="s">
+      <c r="Y84" s="268">
+        <v>0</v>
+      </c>
+      <c r="Z84" s="268">
+        <v>0</v>
+      </c>
+      <c r="AA84" s="269" t="s">
         <v>144</v>
       </c>
       <c r="AB84" s="96" t="s">
@@ -11535,7 +11536,7 @@
       <c r="C86" s="219" t="s">
         <v>66</v>
       </c>
-      <c r="D86" s="252">
+      <c r="D86" s="251">
         <v>360</v>
       </c>
       <c r="E86" s="223">
@@ -11592,7 +11593,7 @@
       <c r="V86" s="106">
         <v>0</v>
       </c>
-      <c r="W86" s="265">
+      <c r="W86" s="264">
         <v>0.1</v>
       </c>
       <c r="X86" s="237">
@@ -11630,7 +11631,7 @@
       <c r="C87" s="219" t="s">
         <v>66</v>
       </c>
-      <c r="D87" s="252">
+      <c r="D87" s="251">
         <v>810</v>
       </c>
       <c r="E87" s="223">
@@ -11687,7 +11688,7 @@
       <c r="V87" s="106">
         <v>0</v>
       </c>
-      <c r="W87" s="265">
+      <c r="W87" s="264">
         <v>0.1</v>
       </c>
       <c r="X87" s="237">
@@ -11901,7 +11902,7 @@
         <v>81</v>
       </c>
       <c r="AD89" s="184"/>
-      <c r="AE89" s="274"/>
+      <c r="AE89" s="273"/>
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A90" s="211" t="s">
@@ -12087,7 +12088,7 @@
         <v>202</v>
       </c>
       <c r="AD91" s="183"/>
-      <c r="AE91" s="273"/>
+      <c r="AE91" s="272"/>
     </row>
     <row r="92" spans="1:31" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="170" t="s">
@@ -12180,7 +12181,7 @@
       <c r="AD92" s="183" t="s">
         <v>197</v>
       </c>
-      <c r="AE92" s="272" t="s">
+      <c r="AE92" s="271" t="s">
         <v>196</v>
       </c>
     </row>
@@ -12608,7 +12609,7 @@
       <c r="N97" s="50">
         <v>5</v>
       </c>
-      <c r="O97" s="261">
+      <c r="O97" s="260">
         <v>4</v>
       </c>
       <c r="P97" s="50">
@@ -12632,16 +12633,16 @@
       <c r="V97" s="46">
         <v>0</v>
       </c>
-      <c r="W97" s="268">
+      <c r="W97" s="267">
         <v>0.1</v>
       </c>
-      <c r="X97" s="268">
+      <c r="X97" s="267">
         <v>0.1</v>
       </c>
-      <c r="Y97" s="268">
-        <v>0</v>
-      </c>
-      <c r="Z97" s="268">
+      <c r="Y97" s="267">
+        <v>0</v>
+      </c>
+      <c r="Z97" s="267">
         <v>0</v>
       </c>
       <c r="AA97" s="44" t="s">
@@ -12654,7 +12655,7 @@
         <v>81</v>
       </c>
       <c r="AD97" s="43"/>
-      <c r="AE97" s="271"/>
+      <c r="AE97" s="270"/>
     </row>
     <row r="98" spans="1:31" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="150" t="s">
@@ -12666,28 +12667,28 @@
       <c r="C98" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="D98" s="253">
+      <c r="D98" s="252">
         <v>40</v>
       </c>
-      <c r="E98" s="257">
-        <v>2</v>
-      </c>
-      <c r="F98" s="257">
-        <v>0</v>
-      </c>
-      <c r="G98" s="257">
+      <c r="E98" s="256">
+        <v>2</v>
+      </c>
+      <c r="F98" s="256">
+        <v>0</v>
+      </c>
+      <c r="G98" s="256">
         <v>15</v>
       </c>
-      <c r="H98" s="257">
-        <v>0</v>
-      </c>
-      <c r="I98" s="257">
+      <c r="H98" s="256">
+        <v>0</v>
+      </c>
+      <c r="I98" s="256">
         <v>50</v>
       </c>
       <c r="J98" s="143">
         <v>0.15</v>
       </c>
-      <c r="K98" s="257">
+      <c r="K98" s="256">
         <v>0</v>
       </c>
       <c r="L98" s="149" t="b">
@@ -12724,10 +12725,10 @@
       <c r="V98" s="226">
         <v>0</v>
       </c>
-      <c r="W98" s="267">
+      <c r="W98" s="266">
         <v>0.1</v>
       </c>
-      <c r="X98" s="269">
+      <c r="X98" s="268">
         <v>0.1</v>
       </c>
       <c r="Y98" s="152">
@@ -12841,7 +12842,7 @@
         <v>173</v>
       </c>
       <c r="AD99" s="43"/>
-      <c r="AE99" s="271"/>
+      <c r="AE99" s="270"/>
     </row>
     <row r="100" spans="1:31" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="38" t="s">
@@ -13097,7 +13098,7 @@
       <c r="V102" s="149">
         <v>0</v>
       </c>
-      <c r="W102" s="265">
+      <c r="W102" s="264">
         <v>0.1</v>
       </c>
       <c r="X102" s="238">
@@ -13590,7 +13591,7 @@
       <c r="A108" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="B108" s="250" t="s">
+      <c r="B108" s="249" t="s">
         <v>465</v>
       </c>
       <c r="C108" s="63" t="s">
@@ -13688,7 +13689,7 @@
       <c r="C109" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="D109" s="256">
+      <c r="D109" s="255">
         <v>540</v>
       </c>
       <c r="E109" s="52">
@@ -13715,7 +13716,7 @@
       <c r="L109" s="149" t="b">
         <v>1</v>
       </c>
-      <c r="M109" s="260">
+      <c r="M109" s="259">
         <v>4</v>
       </c>
       <c r="N109" s="144">
@@ -13779,7 +13780,7 @@
       <c r="C110" s="214" t="s">
         <v>84</v>
       </c>
-      <c r="D110" s="255">
+      <c r="D110" s="254">
         <v>60</v>
       </c>
       <c r="E110" s="48">
@@ -13797,7 +13798,7 @@
       <c r="I110" s="48">
         <v>75</v>
       </c>
-      <c r="J110" s="259">
+      <c r="J110" s="258">
         <v>0.22499999999999998</v>
       </c>
       <c r="K110" s="48">
@@ -13870,7 +13871,7 @@
       <c r="C111" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D111" s="254">
+      <c r="D111" s="253">
         <v>180</v>
       </c>
       <c r="E111" s="74">
@@ -13888,7 +13889,7 @@
       <c r="I111" s="74">
         <v>105</v>
       </c>
-      <c r="J111" s="258">
+      <c r="J111" s="257">
         <v>0.22499999999999998</v>
       </c>
       <c r="K111" s="74">
@@ -13994,7 +13995,7 @@
       <c r="N112" s="40">
         <v>5</v>
       </c>
-      <c r="O112" s="261">
+      <c r="O112" s="260">
         <v>2</v>
       </c>
       <c r="P112" s="40">
@@ -14007,10 +14008,10 @@
       <c r="R112" s="32" t="b">
         <v>0</v>
       </c>
-      <c r="S112" s="262" t="b">
-        <v>0</v>
-      </c>
-      <c r="T112" s="263">
+      <c r="S112" s="261" t="b">
+        <v>0</v>
+      </c>
+      <c r="T112" s="262">
         <v>1</v>
       </c>
       <c r="U112" s="34">
@@ -14019,16 +14020,16 @@
       <c r="V112" s="34">
         <v>0</v>
       </c>
-      <c r="W112" s="266">
+      <c r="W112" s="265">
         <v>0.1</v>
       </c>
-      <c r="X112" s="266">
+      <c r="X112" s="265">
         <v>0.1</v>
       </c>
-      <c r="Y112" s="266">
-        <v>0</v>
-      </c>
-      <c r="Z112" s="266">
+      <c r="Y112" s="265">
+        <v>0</v>
+      </c>
+      <c r="Z112" s="265">
         <v>0</v>
       </c>
       <c r="AA112" s="68" t="s">
@@ -14086,7 +14087,7 @@
       <c r="N113" s="40">
         <v>5</v>
       </c>
-      <c r="O113" s="261">
+      <c r="O113" s="260">
         <v>4</v>
       </c>
       <c r="P113" s="40">
@@ -14099,10 +14100,10 @@
       <c r="R113" s="32" t="b">
         <v>0</v>
       </c>
-      <c r="S113" s="262" t="b">
-        <v>0</v>
-      </c>
-      <c r="T113" s="263">
+      <c r="S113" s="261" t="b">
+        <v>0</v>
+      </c>
+      <c r="T113" s="262">
         <v>1</v>
       </c>
       <c r="U113" s="34">
@@ -14111,16 +14112,16 @@
       <c r="V113" s="34">
         <v>0</v>
       </c>
-      <c r="W113" s="266">
+      <c r="W113" s="265">
         <v>0.15</v>
       </c>
-      <c r="X113" s="266">
+      <c r="X113" s="265">
         <v>0.15</v>
       </c>
-      <c r="Y113" s="266">
-        <v>1</v>
-      </c>
-      <c r="Z113" s="266">
+      <c r="Y113" s="265">
+        <v>1</v>
+      </c>
+      <c r="Z113" s="265">
         <v>0</v>
       </c>
       <c r="AA113" s="68" t="s">
@@ -14206,7 +14207,7 @@
       <c r="V114" s="58">
         <v>0</v>
       </c>
-      <c r="W114" s="266">
+      <c r="W114" s="265">
         <v>0.1</v>
       </c>
       <c r="X114" s="230">
@@ -15508,7 +15509,7 @@
       <c r="U128" s="198">
         <v>9</v>
       </c>
-      <c r="V128" s="264">
+      <c r="V128" s="263">
         <v>0</v>
       </c>
       <c r="W128" s="200">
@@ -15877,8 +15878,8 @@
       <c r="C135" s="22"/>
       <c r="D135" s="22"/>
       <c r="E135" s="22"/>
-      <c r="F135" s="248"/>
-      <c r="G135" s="248"/>
+      <c r="F135" s="274"/>
+      <c r="G135" s="274"/>
       <c r="H135" s="21" t="s">
         <v>56</v>
       </c>
@@ -16950,8 +16951,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="248"/>
-      <c r="G3" s="248"/>
+      <c r="F3" s="274"/>
+      <c r="G3" s="274"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="122"/>

</xml_diff>

<commit_message>
HP balanced for some entitites
Former-commit-id: 86a6440a09afe990b371041acea07179c8550051
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5197,10 +5197,10 @@
   </sheetPr>
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="AD41" sqref="AD41"/>
+      <selection pane="topRight" activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6574,7 +6574,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="66">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H35" s="66">
         <v>0</v>
@@ -8702,7 +8702,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="66">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H58" s="66">
         <v>0</v>
@@ -9069,7 +9069,7 @@
         <v>0</v>
       </c>
       <c r="G62" s="77">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H62" s="77">
         <v>0</v>
@@ -10563,7 +10563,7 @@
         <v>0</v>
       </c>
       <c r="G78" s="77">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H78" s="77">
         <v>0</v>
@@ -10655,7 +10655,7 @@
         <v>0</v>
       </c>
       <c r="G79" s="77">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H79" s="77">
         <v>0</v>
@@ -10747,7 +10747,7 @@
         <v>0</v>
       </c>
       <c r="G80" s="66">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H80" s="66">
         <v>0</v>
@@ -12715,7 +12715,7 @@
         <v>0</v>
       </c>
       <c r="G101" s="77">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H101" s="77">
         <v>0</v>

</xml_diff>

<commit_message>
Falling rocks are burnable from tier 3
Former-commit-id: 6a381cc604f73b8207f1b1fb28787153b566038a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5197,10 +5197,10 @@
   </sheetPr>
   <dimension ref="A1:AE165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="G115" sqref="G115"/>
+      <selection pane="topRight" activeCell="T57" sqref="T57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8644,7 +8644,7 @@
         <v>5</v>
       </c>
       <c r="P57" s="41">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q57" s="59" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Added seasonal entity to content
Former-commit-id: 3985363fdac22a43eabb4c774d443e9b98469fdf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$136:$O$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$137:$O$138</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="500">
   <si>
     <t>tier_4</t>
   </si>
@@ -1526,6 +1526,9 @@
   </si>
   <si>
     <t>TID_QUIP_DRG_KILL_ENT_07</t>
+  </si>
+  <si>
+    <t>seasonal</t>
   </si>
 </sst>
 </file>
@@ -2534,7 +2537,28 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="94">
+  <dxfs count="95">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4789,20 +4813,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4817,113 +4827,113 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AE131" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88" totalsRowBorderDxfId="87">
-  <autoFilter ref="A23:AE131"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AE132" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+  <autoFilter ref="A23:AE132"/>
   <sortState ref="A24:AE131">
     <sortCondition ref="B23:B131"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="86"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="85"/>
-    <tableColumn id="6" name="[category]" dataDxfId="84"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="83"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="82"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="81"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="80"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="79"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="89"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
+    <tableColumn id="6" name="[category]" dataDxfId="87"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="86"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="85"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="84"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="83"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="82"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="81"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="80"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="79"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="78"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="77"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="76"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="75"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="74"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="73"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="72"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="71"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="70"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="69"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="68"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="67"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="66"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="65"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="63"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="62"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="61"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="60"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="54"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A136:O148" totalsRowShown="0">
-  <autoFilter ref="A136:O148"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A137:O149" totalsRowShown="0">
+  <autoFilter ref="A137:O149"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="4" name="[category]" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="16" name="[size]" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="18"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="6" name="[order]" dataDxfId="16"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="15"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="14"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="13"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="6"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="5"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="4"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="3" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5195,12 +5205,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AE165"/>
+  <dimension ref="A1:AE166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="T57" sqref="T57"/>
+      <selection pane="topRight" activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14831,126 +14841,126 @@
       <c r="AE123" s="24"/>
     </row>
     <row r="124" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A124" s="152" t="s">
-        <v>2</v>
-      </c>
-      <c r="B124" s="153" t="s">
-        <v>205</v>
-      </c>
-      <c r="C124" s="154" t="s">
-        <v>66</v>
-      </c>
-      <c r="D124" s="155">
-        <v>220</v>
-      </c>
-      <c r="E124" s="156">
-        <v>21</v>
-      </c>
-      <c r="F124" s="156">
-        <v>0</v>
-      </c>
-      <c r="G124" s="156">
-        <v>50</v>
-      </c>
-      <c r="H124" s="156">
-        <v>0</v>
-      </c>
-      <c r="I124" s="156">
-        <v>95</v>
-      </c>
-      <c r="J124" s="157">
-        <v>0.15</v>
-      </c>
-      <c r="K124" s="156">
-        <v>0</v>
-      </c>
-      <c r="L124" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="M124" s="171">
-        <v>3</v>
-      </c>
-      <c r="N124" s="171">
-        <v>5</v>
-      </c>
-      <c r="O124" s="172">
-        <v>4</v>
-      </c>
-      <c r="P124" s="171">
-        <v>3</v>
-      </c>
-      <c r="Q124" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="R124" s="158" t="b">
-        <v>0</v>
-      </c>
-      <c r="S124" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="T124" s="158">
-        <v>800</v>
-      </c>
-      <c r="U124" s="156">
-        <v>12</v>
-      </c>
-      <c r="V124" s="158">
-        <v>0</v>
-      </c>
-      <c r="W124" s="160">
-        <v>0.25</v>
-      </c>
-      <c r="X124" s="160">
-        <v>0.25</v>
-      </c>
-      <c r="Y124" s="160">
-        <v>0</v>
-      </c>
-      <c r="Z124" s="160">
-        <v>0</v>
-      </c>
-      <c r="AA124" s="155" t="s">
-        <v>204</v>
-      </c>
-      <c r="AB124" s="156" t="s">
-        <v>203</v>
-      </c>
-      <c r="AC124" s="156" t="s">
-        <v>202</v>
-      </c>
-      <c r="AD124" s="156"/>
-      <c r="AE124" s="161"/>
+      <c r="A124" s="141" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="143" t="s">
+        <v>499</v>
+      </c>
+      <c r="C124" s="142" t="s">
+        <v>61</v>
+      </c>
+      <c r="D124" s="39">
+        <v>20</v>
+      </c>
+      <c r="E124" s="39">
+        <v>2</v>
+      </c>
+      <c r="F124" s="39">
+        <v>0</v>
+      </c>
+      <c r="G124" s="39">
+        <v>5</v>
+      </c>
+      <c r="H124" s="39">
+        <v>0</v>
+      </c>
+      <c r="I124" s="39">
+        <v>25</v>
+      </c>
+      <c r="J124" s="54">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K124" s="39">
+        <v>0</v>
+      </c>
+      <c r="L124" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M124" s="33">
+        <v>5</v>
+      </c>
+      <c r="N124" s="33">
+        <v>5</v>
+      </c>
+      <c r="O124" s="30">
+        <v>0</v>
+      </c>
+      <c r="P124" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="R124" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="S124" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="T124" s="37">
+        <v>1</v>
+      </c>
+      <c r="U124" s="37">
+        <v>1</v>
+      </c>
+      <c r="V124" s="37">
+        <v>0</v>
+      </c>
+      <c r="W124" s="53">
+        <v>0</v>
+      </c>
+      <c r="X124" s="53">
+        <v>0</v>
+      </c>
+      <c r="Y124" s="53">
+        <v>0</v>
+      </c>
+      <c r="Z124" s="53">
+        <v>0</v>
+      </c>
+      <c r="AA124" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB124" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC124" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD124" s="25"/>
+      <c r="AE124" s="24"/>
     </row>
     <row r="125" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A125" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B125" s="153" t="s">
-        <v>86</v>
+        <v>205</v>
       </c>
       <c r="C125" s="154" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D125" s="155">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="E125" s="156">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F125" s="156">
         <v>0</v>
       </c>
       <c r="G125" s="156">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="H125" s="156">
         <v>0</v>
       </c>
       <c r="I125" s="156">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="J125" s="157">
-        <v>7.4999999999999997E-2</v>
+        <v>0.15</v>
       </c>
       <c r="K125" s="156">
         <v>0</v>
@@ -14959,17 +14969,16 @@
         <v>1</v>
       </c>
       <c r="M125" s="171">
-        <v>5</v>
-      </c>
-      <c r="N125" s="173">
+        <v>3</v>
+      </c>
+      <c r="N125" s="171">
         <v>5</v>
       </c>
       <c r="O125" s="172">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P125" s="171">
-        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q125" s="158" t="b">
         <v>1</v>
@@ -14977,23 +14986,23 @@
       <c r="R125" s="158" t="b">
         <v>0</v>
       </c>
-      <c r="S125" s="156" t="b">
-        <v>0</v>
+      <c r="S125" s="158" t="b">
+        <v>1</v>
       </c>
       <c r="T125" s="158">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="U125" s="156">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="V125" s="158">
         <v>0</v>
       </c>
-      <c r="W125" s="159">
-        <v>0.05</v>
+      <c r="W125" s="160">
+        <v>0.25</v>
       </c>
       <c r="X125" s="160">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Y125" s="160">
         <v>0</v>
@@ -15002,29 +15011,29 @@
         <v>0</v>
       </c>
       <c r="AA125" s="155" t="s">
-        <v>83</v>
+        <v>204</v>
       </c>
       <c r="AB125" s="156" t="s">
-        <v>82</v>
+        <v>203</v>
       </c>
       <c r="AC125" s="156" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="AD125" s="156"/>
-      <c r="AE125" s="159"/>
+      <c r="AE125" s="161"/>
     </row>
     <row r="126" spans="1:31" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B126" s="153" t="s">
-        <v>305</v>
+        <v>86</v>
       </c>
       <c r="C126" s="154" t="s">
         <v>84</v>
       </c>
       <c r="D126" s="155">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E126" s="156">
         <v>2</v>
@@ -15039,10 +15048,10 @@
         <v>0</v>
       </c>
       <c r="I126" s="156">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="J126" s="157">
-        <v>0.22499999999999998</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="K126" s="156">
         <v>0</v>
@@ -15050,7 +15059,7 @@
       <c r="L126" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="M126" s="173">
+      <c r="M126" s="171">
         <v>5</v>
       </c>
       <c r="N126" s="173">
@@ -15059,7 +15068,7 @@
       <c r="O126" s="172">
         <v>0</v>
       </c>
-      <c r="P126" s="173">
+      <c r="P126" s="171">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>0</v>
       </c>
@@ -15069,7 +15078,7 @@
       <c r="R126" s="158" t="b">
         <v>0</v>
       </c>
-      <c r="S126" s="158" t="b">
+      <c r="S126" s="156" t="b">
         <v>0</v>
       </c>
       <c r="T126" s="158">
@@ -15103,38 +15112,38 @@
         <v>81</v>
       </c>
       <c r="AD126" s="156"/>
-      <c r="AE126" s="161"/>
+      <c r="AE126" s="159"/>
     </row>
     <row r="127" spans="1:31" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B127" s="153" t="s">
-        <v>260</v>
+        <v>305</v>
       </c>
       <c r="C127" s="154" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="D127" s="155">
         <v>60</v>
       </c>
       <c r="E127" s="156">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F127" s="156">
         <v>0</v>
       </c>
       <c r="G127" s="156">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H127" s="156">
         <v>0</v>
       </c>
       <c r="I127" s="156">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="J127" s="157">
-        <v>0.15</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="K127" s="156">
         <v>0</v>
@@ -15148,11 +15157,12 @@
       <c r="N127" s="173">
         <v>5</v>
       </c>
-      <c r="O127" s="174">
-        <v>1</v>
+      <c r="O127" s="172">
+        <v>0</v>
       </c>
       <c r="P127" s="173">
-        <v>1</v>
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>0</v>
       </c>
       <c r="Q127" s="158" t="b">
         <v>1</v>
@@ -15167,66 +15177,62 @@
         <v>1</v>
       </c>
       <c r="U127" s="156">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V127" s="158">
         <v>0</v>
       </c>
-      <c r="W127" s="160">
-        <v>0.1</v>
+      <c r="W127" s="159">
+        <v>0.05</v>
       </c>
       <c r="X127" s="160">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="Y127" s="160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z127" s="160">
         <v>0</v>
       </c>
       <c r="AA127" s="155" t="s">
-        <v>259</v>
+        <v>83</v>
       </c>
       <c r="AB127" s="156" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
       <c r="AC127" s="156" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD127" s="156" t="s">
-        <v>258</v>
-      </c>
-      <c r="AE127" s="156" t="s">
-        <v>257</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="AD127" s="156"/>
+      <c r="AE127" s="161"/>
     </row>
     <row r="128" spans="1:31" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B128" s="153" t="s">
-        <v>337</v>
+        <v>260</v>
       </c>
       <c r="C128" s="154" t="s">
         <v>66</v>
       </c>
       <c r="D128" s="155">
-        <v>360</v>
+        <v>60</v>
       </c>
       <c r="E128" s="156">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="F128" s="156">
         <v>0</v>
       </c>
       <c r="G128" s="156">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H128" s="156">
         <v>0</v>
       </c>
       <c r="I128" s="156">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="J128" s="157">
         <v>0.15</v>
@@ -15237,87 +15243,91 @@
       <c r="L128" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="M128" s="171">
+      <c r="M128" s="173">
+        <v>5</v>
+      </c>
+      <c r="N128" s="173">
+        <v>5</v>
+      </c>
+      <c r="O128" s="174">
+        <v>1</v>
+      </c>
+      <c r="P128" s="173">
+        <v>1</v>
+      </c>
+      <c r="Q128" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="R128" s="158" t="b">
+        <v>0</v>
+      </c>
+      <c r="S128" s="158" t="b">
+        <v>0</v>
+      </c>
+      <c r="T128" s="158">
+        <v>1</v>
+      </c>
+      <c r="U128" s="156">
         <v>4</v>
       </c>
-      <c r="N128" s="171">
-        <v>5</v>
-      </c>
-      <c r="O128" s="172">
-        <v>5</v>
-      </c>
-      <c r="P128" s="171">
-        <v>4</v>
-      </c>
-      <c r="Q128" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="R128" s="158" t="b">
-        <v>0</v>
-      </c>
-      <c r="S128" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="T128" s="158">
-        <v>1000</v>
-      </c>
-      <c r="U128" s="156">
-        <v>17</v>
-      </c>
       <c r="V128" s="158">
         <v>0</v>
       </c>
       <c r="W128" s="160">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="X128" s="160">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="Y128" s="160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z128" s="160">
         <v>0</v>
       </c>
       <c r="AA128" s="155" t="s">
-        <v>204</v>
+        <v>259</v>
       </c>
       <c r="AB128" s="156" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="AC128" s="156" t="s">
-        <v>202</v>
-      </c>
-      <c r="AD128" s="156"/>
-      <c r="AE128" s="161"/>
+        <v>21</v>
+      </c>
+      <c r="AD128" s="156" t="s">
+        <v>258</v>
+      </c>
+      <c r="AE128" s="156" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="129" spans="1:31" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B129" s="153" t="s">
-        <v>228</v>
+        <v>337</v>
       </c>
       <c r="C129" s="154" t="s">
         <v>66</v>
       </c>
       <c r="D129" s="155">
-        <v>220</v>
+        <v>360</v>
       </c>
       <c r="E129" s="156">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F129" s="156">
         <v>0</v>
       </c>
       <c r="G129" s="156">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="H129" s="156">
         <v>0</v>
       </c>
       <c r="I129" s="156">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="J129" s="157">
         <v>0.15</v>
@@ -15329,16 +15339,16 @@
         <v>1</v>
       </c>
       <c r="M129" s="171">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N129" s="171">
         <v>5</v>
       </c>
       <c r="O129" s="172">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P129" s="171">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q129" s="158" t="b">
         <v>1</v>
@@ -15346,14 +15356,14 @@
       <c r="R129" s="158" t="b">
         <v>0</v>
       </c>
-      <c r="S129" s="156" t="b">
-        <v>0</v>
+      <c r="S129" s="158" t="b">
+        <v>1</v>
       </c>
       <c r="T129" s="158">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="U129" s="156">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="V129" s="158">
         <v>0</v>
@@ -15380,38 +15390,38 @@
         <v>202</v>
       </c>
       <c r="AD129" s="156"/>
-      <c r="AE129" s="159"/>
+      <c r="AE129" s="161"/>
     </row>
     <row r="130" spans="1:31" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B130" s="153" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="C130" s="154" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="D130" s="155">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="E130" s="156">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F130" s="156">
         <v>0</v>
       </c>
       <c r="G130" s="156">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H130" s="156">
         <v>0</v>
       </c>
       <c r="I130" s="156">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="J130" s="157">
-        <v>0.22499999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="K130" s="156">
         <v>0</v>
@@ -15419,32 +15429,32 @@
       <c r="L130" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="M130" s="173">
-        <v>5</v>
-      </c>
-      <c r="N130" s="173">
-        <v>0</v>
-      </c>
-      <c r="O130" s="174">
-        <v>1</v>
-      </c>
-      <c r="P130" s="173">
-        <v>0</v>
+      <c r="M130" s="171">
+        <v>5</v>
+      </c>
+      <c r="N130" s="171">
+        <v>5</v>
+      </c>
+      <c r="O130" s="172">
+        <v>3</v>
+      </c>
+      <c r="P130" s="171">
+        <v>3</v>
       </c>
       <c r="Q130" s="158" t="b">
         <v>1</v>
       </c>
       <c r="R130" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="S130" s="158" t="b">
+        <v>0</v>
+      </c>
+      <c r="S130" s="156" t="b">
         <v>0</v>
       </c>
       <c r="T130" s="158">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="U130" s="156">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="V130" s="158">
         <v>0</v>
@@ -15456,328 +15466,374 @@
         <v>0.25</v>
       </c>
       <c r="Y130" s="160">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="Z130" s="160">
         <v>0</v>
       </c>
       <c r="AA130" s="155" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="AB130" s="156" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="AC130" s="156" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD130" s="156" t="s">
-        <v>197</v>
-      </c>
-      <c r="AE130" s="162" t="s">
-        <v>196</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="AD130" s="156"/>
+      <c r="AE130" s="159"/>
     </row>
     <row r="131" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A131" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B131" s="153" t="s">
+        <v>201</v>
+      </c>
+      <c r="C131" s="154" t="s">
+        <v>90</v>
+      </c>
+      <c r="D131" s="155">
+        <v>60</v>
+      </c>
+      <c r="E131" s="156">
+        <v>2</v>
+      </c>
+      <c r="F131" s="156">
+        <v>0</v>
+      </c>
+      <c r="G131" s="156">
+        <v>20</v>
+      </c>
+      <c r="H131" s="156">
+        <v>0</v>
+      </c>
+      <c r="I131" s="156">
+        <v>75</v>
+      </c>
+      <c r="J131" s="157">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="K131" s="156">
+        <v>0</v>
+      </c>
+      <c r="L131" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="M131" s="173">
+        <v>5</v>
+      </c>
+      <c r="N131" s="173">
+        <v>0</v>
+      </c>
+      <c r="O131" s="174">
+        <v>1</v>
+      </c>
+      <c r="P131" s="173">
+        <v>0</v>
+      </c>
+      <c r="Q131" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="R131" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="S131" s="158" t="b">
+        <v>0</v>
+      </c>
+      <c r="T131" s="158">
+        <v>75</v>
+      </c>
+      <c r="U131" s="156">
+        <v>7</v>
+      </c>
+      <c r="V131" s="158">
+        <v>0</v>
+      </c>
+      <c r="W131" s="160">
+        <v>0.25</v>
+      </c>
+      <c r="X131" s="160">
+        <v>0.25</v>
+      </c>
+      <c r="Y131" s="160">
+        <v>0.7</v>
+      </c>
+      <c r="Z131" s="160">
+        <v>0</v>
+      </c>
+      <c r="AA131" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB131" s="156" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC131" s="156" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD131" s="156" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE131" s="162" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A132" s="152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="C131" s="154" t="s">
+      <c r="C132" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="D131" s="155">
+      <c r="D132" s="155">
         <v>40</v>
       </c>
-      <c r="E131" s="156">
-        <v>2</v>
-      </c>
-      <c r="F131" s="156">
-        <v>0</v>
-      </c>
-      <c r="G131" s="156">
+      <c r="E132" s="156">
+        <v>2</v>
+      </c>
+      <c r="F132" s="156">
+        <v>0</v>
+      </c>
+      <c r="G132" s="156">
         <v>30</v>
       </c>
-      <c r="H131" s="156">
-        <v>0</v>
-      </c>
-      <c r="I131" s="156">
+      <c r="H132" s="156">
+        <v>0</v>
+      </c>
+      <c r="I132" s="156">
         <v>50</v>
       </c>
-      <c r="J131" s="157">
+      <c r="J132" s="157">
         <v>0.15</v>
       </c>
-      <c r="K131" s="156">
-        <v>0</v>
-      </c>
-      <c r="L131" s="163" t="b">
-        <v>1</v>
-      </c>
-      <c r="M131" s="175">
-        <v>5</v>
-      </c>
-      <c r="N131" s="175">
-        <v>5</v>
-      </c>
-      <c r="O131" s="176">
-        <v>0</v>
-      </c>
-      <c r="P131" s="175">
-        <v>0</v>
-      </c>
-      <c r="Q131" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="R131" s="165" t="b">
-        <v>0</v>
-      </c>
-      <c r="S131" s="165" t="b">
-        <v>0</v>
-      </c>
-      <c r="T131" s="158">
+      <c r="K132" s="156">
+        <v>0</v>
+      </c>
+      <c r="L132" s="163" t="b">
+        <v>1</v>
+      </c>
+      <c r="M132" s="175">
+        <v>5</v>
+      </c>
+      <c r="N132" s="175">
+        <v>5</v>
+      </c>
+      <c r="O132" s="176">
+        <v>0</v>
+      </c>
+      <c r="P132" s="175">
+        <v>0</v>
+      </c>
+      <c r="Q132" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="R132" s="165" t="b">
+        <v>0</v>
+      </c>
+      <c r="S132" s="165" t="b">
+        <v>0</v>
+      </c>
+      <c r="T132" s="158">
         <v>85</v>
       </c>
-      <c r="U131" s="164">
+      <c r="U132" s="164">
         <v>9</v>
       </c>
-      <c r="V131" s="163">
-        <v>0</v>
-      </c>
-      <c r="W131" s="166">
+      <c r="V132" s="163">
+        <v>0</v>
+      </c>
+      <c r="W132" s="166">
         <v>0.25</v>
       </c>
-      <c r="X131" s="166">
+      <c r="X132" s="166">
         <v>0.25</v>
       </c>
-      <c r="Y131" s="166">
+      <c r="Y132" s="166">
         <v>0.75</v>
       </c>
-      <c r="Z131" s="166">
-        <v>0</v>
-      </c>
-      <c r="AA131" s="167" t="s">
+      <c r="Z132" s="166">
+        <v>0</v>
+      </c>
+      <c r="AA132" s="167" t="s">
         <v>73</v>
       </c>
-      <c r="AB131" s="164" t="s">
+      <c r="AB132" s="164" t="s">
         <v>72</v>
       </c>
-      <c r="AC131" s="164" t="s">
+      <c r="AC132" s="164" t="s">
         <v>71</v>
       </c>
-      <c r="AD131" s="164"/>
-      <c r="AE131" s="168"/>
-    </row>
-    <row r="132" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A132" s="119"/>
-      <c r="B132" s="119"/>
-      <c r="C132" s="119"/>
-      <c r="D132" s="120"/>
-      <c r="E132" s="121"/>
-      <c r="F132" s="121"/>
-      <c r="G132" s="121"/>
-      <c r="H132" s="121"/>
-      <c r="I132" s="121"/>
-      <c r="J132" s="122"/>
-      <c r="K132" s="121"/>
-      <c r="L132" s="123"/>
-      <c r="M132" s="124"/>
-      <c r="N132" s="124"/>
-      <c r="O132" s="125"/>
-      <c r="P132" s="124"/>
-      <c r="Q132" s="126"/>
-      <c r="R132" s="127"/>
-      <c r="S132" s="127"/>
-      <c r="T132" s="126"/>
-      <c r="U132" s="127"/>
-      <c r="V132" s="128"/>
-      <c r="W132" s="129"/>
-      <c r="X132" s="130"/>
-      <c r="Y132" s="130"/>
-      <c r="Z132" s="131"/>
-      <c r="AA132" s="132"/>
-      <c r="AB132" s="132"/>
-      <c r="AC132" s="133"/>
-      <c r="AD132" s="133"/>
-      <c r="AE132" s="134"/>
-    </row>
-    <row r="133" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="134" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A134" s="9" t="s">
+      <c r="AD132" s="164"/>
+      <c r="AE132" s="168"/>
+    </row>
+    <row r="133" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A133" s="119"/>
+      <c r="B133" s="119"/>
+      <c r="C133" s="119"/>
+      <c r="D133" s="120"/>
+      <c r="E133" s="121"/>
+      <c r="F133" s="121"/>
+      <c r="G133" s="121"/>
+      <c r="H133" s="121"/>
+      <c r="I133" s="121"/>
+      <c r="J133" s="122"/>
+      <c r="K133" s="121"/>
+      <c r="L133" s="123"/>
+      <c r="M133" s="124"/>
+      <c r="N133" s="124"/>
+      <c r="O133" s="125"/>
+      <c r="P133" s="124"/>
+      <c r="Q133" s="126"/>
+      <c r="R133" s="127"/>
+      <c r="S133" s="127"/>
+      <c r="T133" s="126"/>
+      <c r="U133" s="127"/>
+      <c r="V133" s="128"/>
+      <c r="W133" s="129"/>
+      <c r="X133" s="130"/>
+      <c r="Y133" s="130"/>
+      <c r="Z133" s="131"/>
+      <c r="AA133" s="132"/>
+      <c r="AB133" s="132"/>
+      <c r="AC133" s="133"/>
+      <c r="AD133" s="133"/>
+      <c r="AE133" s="134"/>
+    </row>
+    <row r="134" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="135" spans="1:31" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A135" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B134" s="9"/>
-      <c r="C134" s="9"/>
-      <c r="D134" s="9"/>
-      <c r="E134" s="9"/>
-      <c r="F134" s="9"/>
-      <c r="G134" s="9"/>
-      <c r="H134" s="9"/>
-      <c r="I134" s="9"/>
-      <c r="J134" s="9"/>
-      <c r="K134" s="9"/>
-      <c r="L134" s="9"/>
-      <c r="M134" s="9"/>
-      <c r="N134" s="9"/>
-      <c r="O134" s="9"/>
-      <c r="P134" s="9"/>
-      <c r="Q134" s="9"/>
-      <c r="R134" s="9"/>
-      <c r="S134" s="9"/>
-      <c r="T134" s="9"/>
-      <c r="U134" s="9"/>
-      <c r="V134" s="9"/>
-      <c r="W134" s="9"/>
-      <c r="X134" s="9"/>
-      <c r="Y134" s="9"/>
-      <c r="Z134" s="9"/>
-      <c r="AA134" s="9"/>
-    </row>
-    <row r="135" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="22"/>
-      <c r="B135" s="22"/>
-      <c r="C135" s="22"/>
-      <c r="D135" s="22"/>
-      <c r="E135" s="22"/>
-      <c r="F135" s="178"/>
-      <c r="G135" s="178"/>
-      <c r="H135" s="21" t="s">
+      <c r="B135" s="9"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="9"/>
+      <c r="K135" s="9"/>
+      <c r="L135" s="9"/>
+      <c r="M135" s="9"/>
+      <c r="N135" s="9"/>
+      <c r="O135" s="9"/>
+      <c r="P135" s="9"/>
+      <c r="Q135" s="9"/>
+      <c r="R135" s="9"/>
+      <c r="S135" s="9"/>
+      <c r="T135" s="9"/>
+      <c r="U135" s="9"/>
+      <c r="V135" s="9"/>
+      <c r="W135" s="9"/>
+      <c r="X135" s="9"/>
+      <c r="Y135" s="9"/>
+      <c r="Z135" s="9"/>
+      <c r="AA135" s="9"/>
+      <c r="AB135"/>
+      <c r="AC135"/>
+      <c r="AD135"/>
+      <c r="AE135"/>
+    </row>
+    <row r="136" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A136" s="22"/>
+      <c r="B136" s="22"/>
+      <c r="C136" s="22"/>
+      <c r="D136" s="22"/>
+      <c r="E136" s="22"/>
+      <c r="F136" s="178"/>
+      <c r="G136" s="178"/>
+      <c r="H136" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I135" s="21"/>
-      <c r="J135" s="22"/>
-      <c r="K135" s="17"/>
-      <c r="L135" s="17"/>
-      <c r="M135" s="17" t="s">
+      <c r="I136" s="21"/>
+      <c r="J136" s="22"/>
+      <c r="K136" s="17"/>
+      <c r="L136" s="17"/>
+      <c r="M136" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N135" s="17"/>
-      <c r="O135" s="17"/>
-      <c r="P135" s="17"/>
-      <c r="Q135" s="17"/>
-      <c r="R135" s="17"/>
-      <c r="S135" s="17"/>
-      <c r="T135" s="17"/>
-      <c r="U135" s="17"/>
-      <c r="V135" s="17"/>
-      <c r="W135" s="17"/>
-      <c r="X135" s="17"/>
-      <c r="Y135" s="17"/>
-      <c r="Z135" s="17"/>
-      <c r="AA135" s="21"/>
-      <c r="AB135" s="21"/>
-      <c r="AC135" s="21"/>
-      <c r="AD135" s="21"/>
-      <c r="AE135" s="17"/>
-    </row>
-    <row r="136" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="7" t="s">
+      <c r="N136" s="17"/>
+      <c r="O136" s="17"/>
+      <c r="P136" s="17"/>
+      <c r="Q136" s="17"/>
+      <c r="R136" s="17"/>
+      <c r="S136" s="17"/>
+      <c r="T136" s="17"/>
+      <c r="U136" s="17"/>
+      <c r="V136" s="17"/>
+      <c r="W136" s="17"/>
+      <c r="X136" s="17"/>
+      <c r="Y136" s="17"/>
+      <c r="Z136" s="17"/>
+      <c r="AA136" s="21"/>
+      <c r="AB136" s="21"/>
+      <c r="AC136" s="21"/>
+      <c r="AD136" s="21"/>
+      <c r="AE136" s="17"/>
+    </row>
+    <row r="137" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A137" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B136" s="7" t="s">
+      <c r="B137" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C136" s="7" t="s">
+      <c r="C137" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D136" s="20" t="s">
+      <c r="D137" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E136" s="20" t="s">
+      <c r="E137" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F136" s="20" t="s">
+      <c r="F137" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G136" s="20" t="s">
+      <c r="G137" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H136" s="20" t="s">
+      <c r="H137" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I136" s="20" t="s">
+      <c r="I137" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J136" s="20" t="s">
+      <c r="J137" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K136" s="20" t="s">
+      <c r="K137" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="L136" s="20" t="s">
+      <c r="L137" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M136" s="19" t="s">
+      <c r="M137" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N136" s="19" t="s">
+      <c r="N137" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O136" s="19" t="s">
+      <c r="O137" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="137" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A137" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B137" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C137" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D137" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E137" s="14">
-        <v>3</v>
-      </c>
-      <c r="F137" s="18">
-        <v>0</v>
-      </c>
-      <c r="G137" s="18">
-        <v>0</v>
-      </c>
-      <c r="H137" s="18">
-        <v>0</v>
-      </c>
-      <c r="I137" s="18">
-        <v>0</v>
-      </c>
-      <c r="J137" s="12">
-        <v>2</v>
-      </c>
-      <c r="K137" s="12">
-        <v>0</v>
-      </c>
-      <c r="L137" s="12">
-        <v>0</v>
-      </c>
-      <c r="M137" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N137" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O137" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P137" s="17"/>
-      <c r="Q137" s="17"/>
     </row>
     <row r="138" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A138" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B138" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C138" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E138" s="14">
         <v>3</v>
@@ -15786,7 +15842,7 @@
         <v>0</v>
       </c>
       <c r="G138" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H138" s="18">
         <v>0</v>
@@ -15820,13 +15876,13 @@
         <v>2</v>
       </c>
       <c r="B139" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E139" s="14">
         <v>3</v>
@@ -15835,7 +15891,7 @@
         <v>0</v>
       </c>
       <c r="G139" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H139" s="18">
         <v>0</v>
@@ -15869,13 +15925,13 @@
         <v>2</v>
       </c>
       <c r="B140" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C140" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E140" s="14">
         <v>3</v>
@@ -15884,7 +15940,7 @@
         <v>0</v>
       </c>
       <c r="G140" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H140" s="18">
         <v>0</v>
@@ -15918,13 +15974,13 @@
         <v>2</v>
       </c>
       <c r="B141" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E141" s="14">
         <v>3</v>
@@ -15933,7 +15989,7 @@
         <v>0</v>
       </c>
       <c r="G141" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H141" s="18">
         <v>0</v>
@@ -15967,13 +16023,13 @@
         <v>2</v>
       </c>
       <c r="B142" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C142" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E142" s="14">
         <v>3</v>
@@ -15982,7 +16038,7 @@
         <v>0</v>
       </c>
       <c r="G142" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H142" s="18">
         <v>0</v>
@@ -16016,13 +16072,13 @@
         <v>2</v>
       </c>
       <c r="B143" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C143" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E143" s="14">
         <v>3</v>
@@ -16031,7 +16087,7 @@
         <v>0</v>
       </c>
       <c r="G143" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H143" s="18">
         <v>0</v>
@@ -16065,13 +16121,13 @@
         <v>2</v>
       </c>
       <c r="B144" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E144" s="14">
         <v>3</v>
@@ -16080,7 +16136,7 @@
         <v>0</v>
       </c>
       <c r="G144" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H144" s="18">
         <v>0</v>
@@ -16114,13 +16170,13 @@
         <v>2</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C145" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E145" s="14">
         <v>3</v>
@@ -16129,7 +16185,7 @@
         <v>0</v>
       </c>
       <c r="G145" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H145" s="18">
         <v>0</v>
@@ -16163,13 +16219,13 @@
         <v>2</v>
       </c>
       <c r="B146" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C146" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E146" s="14">
         <v>3</v>
@@ -16178,7 +16234,7 @@
         <v>0</v>
       </c>
       <c r="G146" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H146" s="18">
         <v>0</v>
@@ -16212,27 +16268,27 @@
         <v>2</v>
       </c>
       <c r="B147" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E147" s="14">
-        <v>1</v>
-      </c>
-      <c r="F147" s="13">
-        <v>0</v>
-      </c>
-      <c r="G147" s="13">
-        <v>1</v>
-      </c>
-      <c r="H147" s="13">
-        <v>0</v>
-      </c>
-      <c r="I147" s="13">
+        <v>3</v>
+      </c>
+      <c r="F147" s="18">
+        <v>0</v>
+      </c>
+      <c r="G147" s="18">
+        <v>2</v>
+      </c>
+      <c r="H147" s="18">
+        <v>0</v>
+      </c>
+      <c r="I147" s="18">
         <v>0</v>
       </c>
       <c r="J147" s="12">
@@ -16253,33 +16309,35 @@
       <c r="O147" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P147" s="17"/>
+      <c r="Q147" s="17"/>
     </row>
     <row r="148" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A148" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B148" s="96" t="s">
-        <v>463</v>
-      </c>
-      <c r="C148" s="96" t="s">
-        <v>38</v>
-      </c>
-      <c r="D148" s="146" t="s">
-        <v>30</v>
+      <c r="B148" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C148" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D148" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E148" s="14">
         <v>1</v>
       </c>
-      <c r="F148" s="147">
-        <v>0</v>
-      </c>
-      <c r="G148" s="147">
-        <v>0</v>
-      </c>
-      <c r="H148" s="147">
-        <v>0</v>
-      </c>
-      <c r="I148" s="147">
+      <c r="F148" s="13">
+        <v>0</v>
+      </c>
+      <c r="G148" s="13">
+        <v>1</v>
+      </c>
+      <c r="H148" s="13">
+        <v>0</v>
+      </c>
+      <c r="I148" s="13">
         <v>0</v>
       </c>
       <c r="J148" s="12">
@@ -16300,26 +16358,53 @@
       <c r="O148" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P148" s="8"/>
-      <c r="Q148" s="8"/>
-      <c r="R148" s="8"/>
-      <c r="S148" s="8"/>
-      <c r="T148" s="8"/>
-      <c r="U148" s="8"/>
-      <c r="V148" s="8"/>
-      <c r="W148" s="8"/>
-      <c r="X148" s="8"/>
-      <c r="Y148" s="8"/>
-      <c r="Z148" s="8"/>
-      <c r="AA148" s="8"/>
-      <c r="AB148" s="8"/>
-      <c r="AC148" s="8"/>
-      <c r="AD148" s="8"/>
-      <c r="AE148" s="8"/>
     </row>
     <row r="149" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N149" s="8"/>
-      <c r="O149" s="8"/>
+      <c r="A149" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B149" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C149" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="D149" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="E149" s="14">
+        <v>1</v>
+      </c>
+      <c r="F149" s="147">
+        <v>0</v>
+      </c>
+      <c r="G149" s="147">
+        <v>0</v>
+      </c>
+      <c r="H149" s="147">
+        <v>0</v>
+      </c>
+      <c r="I149" s="147">
+        <v>0</v>
+      </c>
+      <c r="J149" s="12">
+        <v>2</v>
+      </c>
+      <c r="K149" s="12">
+        <v>0</v>
+      </c>
+      <c r="L149" s="12">
+        <v>0</v>
+      </c>
+      <c r="M149" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N149" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O149" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="P149" s="8"/>
       <c r="Q149" s="8"/>
       <c r="R149" s="8"/>
@@ -16337,73 +16422,67 @@
       <c r="AD149" s="8"/>
       <c r="AE149" s="8"/>
     </row>
-    <row r="150" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="151" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A151" s="9" t="s">
+    <row r="150" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N150" s="8"/>
+      <c r="O150" s="8"/>
+      <c r="P150" s="8"/>
+      <c r="Q150" s="8"/>
+      <c r="R150" s="8"/>
+      <c r="S150" s="8"/>
+      <c r="T150" s="8"/>
+      <c r="U150" s="8"/>
+      <c r="V150" s="8"/>
+      <c r="W150" s="8"/>
+      <c r="X150" s="8"/>
+      <c r="Y150" s="8"/>
+      <c r="Z150" s="8"/>
+      <c r="AA150" s="8"/>
+      <c r="AB150" s="8"/>
+      <c r="AC150" s="8"/>
+      <c r="AD150" s="8"/>
+      <c r="AE150" s="8"/>
+    </row>
+    <row r="151" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A152" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B151" s="9"/>
-      <c r="C151" s="9"/>
-      <c r="D151" s="9"/>
-      <c r="E151" s="8"/>
-      <c r="F151" s="8"/>
-      <c r="G151" s="8"/>
-      <c r="H151" s="8"/>
-      <c r="I151" s="8"/>
-      <c r="J151" s="8"/>
-      <c r="K151" s="8"/>
-      <c r="L151" s="8"/>
-    </row>
-    <row r="153" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="7" t="s">
+      <c r="B152" s="9"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="8"/>
+      <c r="F152" s="8"/>
+      <c r="G152" s="8"/>
+      <c r="H152" s="8"/>
+      <c r="I152" s="8"/>
+      <c r="J152" s="8"/>
+      <c r="K152" s="8"/>
+      <c r="L152" s="8"/>
+    </row>
+    <row r="154" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A154" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B153" s="6" t="s">
+      <c r="B154" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C153" s="6" t="s">
+      <c r="C154" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D153" s="5" t="s">
+      <c r="D154" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E153" s="5" t="s">
+      <c r="E154" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F153" s="5" t="s">
+      <c r="F154" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G153" s="5" t="s">
+      <c r="G154" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H153" s="5" t="s">
+      <c r="H154" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="154" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A154" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D154" s="2">
-        <v>42</v>
-      </c>
-      <c r="E154" s="2">
-        <v>8</v>
-      </c>
-      <c r="F154" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G154" s="2">
-        <v>2</v>
-      </c>
-      <c r="H154" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:31" x14ac:dyDescent="0.25">
@@ -16411,19 +16490,19 @@
         <v>2</v>
       </c>
       <c r="B155" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D155" s="2">
+        <v>42</v>
+      </c>
+      <c r="E155" s="2">
         <v>8</v>
       </c>
-      <c r="C155" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D155" s="2">
-        <v>92</v>
-      </c>
-      <c r="E155" s="2">
-        <v>10</v>
-      </c>
       <c r="F155" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G155" s="2">
         <v>2</v>
@@ -16437,19 +16516,19 @@
         <v>2</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D156" s="2">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="E156" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F156" s="2">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G156" s="2">
         <v>2</v>
@@ -16463,19 +16542,19 @@
         <v>2</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D157" s="2">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="E157" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F157" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G157" s="2">
         <v>2</v>
@@ -16489,104 +16568,130 @@
         <v>2</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D158" s="2">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="E158" s="2">
         <v>14</v>
       </c>
       <c r="F158" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G158" s="2">
+        <v>2</v>
+      </c>
+      <c r="H158" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D159" s="2">
+        <v>1040</v>
+      </c>
+      <c r="E159" s="2">
+        <v>14</v>
+      </c>
+      <c r="F159" s="2">
         <v>0.5</v>
       </c>
-      <c r="G158" s="2">
-        <v>2</v>
-      </c>
-      <c r="H158" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D161" s="1">
-        <v>42</v>
-      </c>
-      <c r="F161" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G161">
-        <f>D154*F154</f>
-        <v>54.6</v>
-      </c>
-      <c r="I161">
-        <f>D161*F161</f>
-        <v>54.6</v>
+      <c r="G159" s="2">
+        <v>2</v>
+      </c>
+      <c r="H159" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D162" s="1">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="F162" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G162">
         <f>D155*F155</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
       <c r="I162">
         <f>D162*F162</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="163" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D163" s="1">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="F163" s="1">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G163">
         <f>D156*F156</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
       <c r="I163">
         <f>D163*F163</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="164" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D164" s="1">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="F164" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G164">
         <f>D157*F157</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
       <c r="I164">
         <f>D164*F164</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
     </row>
     <row r="165" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D165" s="1">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="F165" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G165">
         <f>D158*F158</f>
-        <v>520</v>
+        <v>480.2</v>
       </c>
       <c r="I165">
         <f>D165*F165</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="166" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D166" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F166" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G166">
+        <f>D159*F159</f>
+        <v>520</v>
+      </c>
+      <c r="I166">
+        <f>D166*F166</f>
         <v>520</v>
       </c>
     </row>
@@ -16594,15 +16699,15 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F135:G135"/>
+    <mergeCell ref="F136:G136"/>
   </mergeCells>
-  <conditionalFormatting sqref="L24:L122 L124:L131 Q24:S122 Q124:S131">
-    <cfRule type="expression" dxfId="93" priority="9">
+  <conditionalFormatting sqref="L24:L122 Q24:S122 L125:L132 Q125:S132">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>L24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:P122 M124:P131">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="M125:P132 M24:P122">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -16614,11 +16719,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L123 Q123:S123">
-    <cfRule type="expression" dxfId="92" priority="2">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>L123=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M123:P123">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L124 Q124:S124">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>L124=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M124:P124">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -16632,32 +16754,32 @@
   </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G42"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G43:I132 G24:I40">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G24:I40 G43:I133">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D137:G148 P24:V132 M24:N132">
+    <dataValidation type="decimal" allowBlank="1" sqref="D138:G149 P24:V133 M24:N133">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H137:L146 H147:I147 J148:L148 W24:Z132">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H138:L147 H148:I148 J149:L149 W24:Z133">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C137:C148 C24:C132">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C138:C149 C24:C133">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J147:L147 M137:O148 AA94:AA120 AA86:AA92 AA121:AE132 AA24:AE85 AB86:AE120"/>
-    <dataValidation type="list" sqref="O24:O132">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J148:L148 M138:O149 AA94:AA120 AA86:AA92 AA24:AE85 AB86:AE120 AA121:AE133"/>
+    <dataValidation type="list" sqref="O24:O133">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J24:K132">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J24:K133">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F132">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F133">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="L24:L132">
+    <dataValidation type="list" sqref="L24:L133">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Feedback dmg, reduced for jellyfishes
Former-commit-id: 4d89a8f7818444982003d6d62a8ed6380adfa391
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -2541,68 +2541,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="96">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4570,6 +4508,47 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -4857,6 +4836,27 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4871,58 +4871,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF132" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94" tableBorderDxfId="92" totalsRowBorderDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF132" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF132"/>
   <sortState ref="A24:AE131">
     <sortCondition ref="B23:B131"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="90"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="89"/>
-    <tableColumn id="6" name="[category]" dataDxfId="88"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="87"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="86"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="85"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="84"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="83"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="82"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="0"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="81"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="80"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="79"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="78"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="77"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="76"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="75"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="74"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="73"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="72"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="71"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="70"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="69"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="68"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="67"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="66"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="65"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="64"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="63"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="62"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="61"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="60"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="55"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="54"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4935,50 +4935,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="4" name="[category]" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="16" name="[size]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="19"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="18"/>
-    <tableColumn id="6" name="[order]" dataDxfId="17"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="16"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="15"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="14"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="13"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="7"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="6"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="5"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5252,10 +5252,10 @@
   </sheetPr>
   <dimension ref="A1:AF166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="Y1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="J125" sqref="J125"/>
+      <selection pane="topRight" activeCell="Z82" sqref="Z82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11222,7 +11222,7 @@
         <v>0.1</v>
       </c>
       <c r="Z82" s="53">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA82" s="53">
         <v>0</v>
@@ -11320,7 +11320,7 @@
         <v>0.1</v>
       </c>
       <c r="Z83" s="53">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA83" s="53">
         <v>0</v>
@@ -17061,7 +17061,7 @@
     <mergeCell ref="F136:G136"/>
   </mergeCells>
   <conditionalFormatting sqref="M24:M122 R24:T122 M125:M132 R125:T132">
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="95" priority="11">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17078,7 +17078,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M123 R123:T123">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="94" priority="4">
       <formula>M123=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17095,7 +17095,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M124 R124:T124">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="93" priority="2">
       <formula>M124=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Content and texts for drones
Former-commit-id: 017b6dbf01c7e8033e91fcaa1791d677443695de
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$137:$O$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$139:$O$140</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="505">
   <si>
     <t>tier_4</t>
   </si>
@@ -1532,6 +1532,18 @@
   </si>
   <si>
     <t>[rewardFury]</t>
+  </si>
+  <si>
+    <t>GoblinDroneFood</t>
+  </si>
+  <si>
+    <t>GoblinDrone</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_DRONE_FOOD</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_DRONE</t>
   </si>
 </sst>
 </file>
@@ -2540,7 +2552,42 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="98">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4836,27 +4883,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4871,114 +4897,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF132" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF132"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF134" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+  <autoFilter ref="A23:AF134"/>
   <sortState ref="A24:AE131">
     <sortCondition ref="B23:B131"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="92"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="91"/>
+    <tableColumn id="6" name="[category]" dataDxfId="90"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="89"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="88"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="87"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="86"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="85"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="84"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="83"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="82"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="81"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="80"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="79"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="78"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="77"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="76"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="75"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="74"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="73"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="72"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="71"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="70"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="69"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="68"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="67"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="66"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="65"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="64"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="63"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="62"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A137:O149" totalsRowShown="0">
-  <autoFilter ref="A137:O149"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A139:O151" totalsRowShown="0">
+  <autoFilter ref="A139:O151"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="4" name="[category]" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="16" name="[size]" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="26" totalsRowDxfId="25"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="20"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="19"/>
+    <tableColumn id="6" name="[order]" dataDxfId="18"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="17"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="16"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="15"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="8"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="7"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="6"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="5" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5250,12 +5276,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF166"/>
+  <dimension ref="A1:AF168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="Z82" sqref="Z82"/>
+      <selection pane="topRight" activeCell="AB125" sqref="AB125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15189,55 +15215,55 @@
       <c r="AF123" s="24"/>
     </row>
     <row r="124" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A124" s="141" t="s">
-        <v>2</v>
-      </c>
-      <c r="B124" s="143" t="s">
+      <c r="A124" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="50" t="s">
         <v>499</v>
       </c>
-      <c r="C124" s="142" t="s">
+      <c r="C124" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="D124" s="39">
+      <c r="D124" s="62">
         <v>20</v>
       </c>
-      <c r="E124" s="39">
-        <v>2</v>
-      </c>
-      <c r="F124" s="39">
-        <v>0</v>
-      </c>
-      <c r="G124" s="39">
-        <v>5</v>
-      </c>
-      <c r="H124" s="39">
-        <v>0</v>
-      </c>
-      <c r="I124" s="39">
+      <c r="E124" s="77">
+        <v>2</v>
+      </c>
+      <c r="F124" s="77">
+        <v>0</v>
+      </c>
+      <c r="G124" s="77">
+        <v>5</v>
+      </c>
+      <c r="H124" s="77">
+        <v>0</v>
+      </c>
+      <c r="I124" s="77">
         <v>25</v>
       </c>
-      <c r="J124" s="39">
+      <c r="J124" s="77">
         <v>2500</v>
       </c>
-      <c r="K124" s="54">
+      <c r="K124" s="43">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="L124" s="39">
+      <c r="L124" s="77">
         <v>0</v>
       </c>
       <c r="M124" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="N124" s="33">
-        <v>5</v>
-      </c>
-      <c r="O124" s="33">
-        <v>5</v>
-      </c>
-      <c r="P124" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q124" s="33">
+      <c r="N124" s="34">
+        <v>5</v>
+      </c>
+      <c r="O124" s="34">
+        <v>5</v>
+      </c>
+      <c r="P124" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="34">
         <v>0</v>
       </c>
       <c r="R124" s="37" t="b">
@@ -15246,258 +15272,263 @@
       <c r="S124" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="T124" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="U124" s="37">
-        <v>1</v>
-      </c>
-      <c r="V124" s="37">
-        <v>1</v>
-      </c>
-      <c r="W124" s="37">
-        <v>0</v>
-      </c>
-      <c r="X124" s="53">
-        <v>0</v>
-      </c>
-      <c r="Y124" s="53">
-        <v>0</v>
-      </c>
-      <c r="Z124" s="53">
-        <v>0</v>
-      </c>
-      <c r="AA124" s="53">
-        <v>0</v>
-      </c>
-      <c r="AB124" s="36" t="s">
+      <c r="T124" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="U124" s="47">
+        <v>1</v>
+      </c>
+      <c r="V124" s="47">
+        <v>1</v>
+      </c>
+      <c r="W124" s="47">
+        <v>0</v>
+      </c>
+      <c r="X124" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y124" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z124" s="56">
+        <v>0</v>
+      </c>
+      <c r="AA124" s="56">
+        <v>0</v>
+      </c>
+      <c r="AB124" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="AC124" s="35" t="s">
+      <c r="AC124" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="AD124" s="35" t="s">
+      <c r="AD124" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="AE124" s="25"/>
-      <c r="AF124" s="24"/>
+      <c r="AE124" s="26"/>
+      <c r="AF124" s="60"/>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A125" s="152" t="s">
-        <v>2</v>
-      </c>
-      <c r="B125" s="153" t="s">
+      <c r="A125" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B125" s="50" t="s">
+        <v>501</v>
+      </c>
+      <c r="C125" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D125" s="62">
+        <v>60</v>
+      </c>
+      <c r="E125" s="77">
+        <v>9</v>
+      </c>
+      <c r="F125" s="77">
+        <v>0</v>
+      </c>
+      <c r="G125" s="77">
+        <v>35</v>
+      </c>
+      <c r="H125" s="77">
+        <v>0</v>
+      </c>
+      <c r="I125" s="77">
+        <v>35</v>
+      </c>
+      <c r="J125" s="77">
+        <v>0</v>
+      </c>
+      <c r="K125" s="43">
+        <v>0.15</v>
+      </c>
+      <c r="L125" s="77">
+        <v>0</v>
+      </c>
+      <c r="M125" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N125" s="34">
+        <v>5</v>
+      </c>
+      <c r="O125" s="34">
+        <v>5</v>
+      </c>
+      <c r="P125" s="27">
+        <v>2</v>
+      </c>
+      <c r="Q125" s="34">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>2</v>
+      </c>
+      <c r="R125" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="S125" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T125" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="U125" s="47">
+        <v>1</v>
+      </c>
+      <c r="V125" s="47">
+        <v>8</v>
+      </c>
+      <c r="W125" s="47">
+        <v>0</v>
+      </c>
+      <c r="X125" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="Y125" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="Z125" s="56">
+        <v>0.5</v>
+      </c>
+      <c r="AA125" s="56">
+        <v>0</v>
+      </c>
+      <c r="AB125" s="46" t="s">
+        <v>503</v>
+      </c>
+      <c r="AC125" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD125" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE125" s="26"/>
+      <c r="AF125" s="60"/>
+    </row>
+    <row r="126" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A126" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="50" t="s">
+        <v>502</v>
+      </c>
+      <c r="C126" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D126" s="62">
+        <v>220</v>
+      </c>
+      <c r="E126" s="77">
+        <v>21</v>
+      </c>
+      <c r="F126" s="77">
+        <v>0</v>
+      </c>
+      <c r="G126" s="77">
+        <v>100</v>
+      </c>
+      <c r="H126" s="77">
+        <v>0</v>
+      </c>
+      <c r="I126" s="77">
+        <v>95</v>
+      </c>
+      <c r="J126" s="77">
+        <v>0</v>
+      </c>
+      <c r="K126" s="43">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L126" s="77">
+        <v>0</v>
+      </c>
+      <c r="M126" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N126" s="33">
+        <v>5</v>
+      </c>
+      <c r="O126" s="34">
+        <v>5</v>
+      </c>
+      <c r="P126" s="30">
+        <v>3</v>
+      </c>
+      <c r="Q126" s="33">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>3</v>
+      </c>
+      <c r="R126" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="S126" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T126" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U126" s="47">
+        <v>1</v>
+      </c>
+      <c r="V126" s="47">
+        <v>12</v>
+      </c>
+      <c r="W126" s="47">
+        <v>0</v>
+      </c>
+      <c r="X126" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="Y126" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="Z126" s="56">
+        <v>0</v>
+      </c>
+      <c r="AA126" s="56">
+        <v>0</v>
+      </c>
+      <c r="AB126" s="55" t="s">
+        <v>504</v>
+      </c>
+      <c r="AC126" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD126" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE126" s="26"/>
+      <c r="AF126" s="60"/>
+    </row>
+    <row r="127" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A127" s="152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B127" s="153" t="s">
         <v>205</v>
       </c>
-      <c r="C125" s="154" t="s">
+      <c r="C127" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="D125" s="155">
+      <c r="D127" s="155">
         <v>220</v>
       </c>
-      <c r="E125" s="156">
+      <c r="E127" s="156">
         <v>21</v>
       </c>
-      <c r="F125" s="156">
-        <v>0</v>
-      </c>
-      <c r="G125" s="156">
+      <c r="F127" s="156">
+        <v>0</v>
+      </c>
+      <c r="G127" s="156">
         <v>50</v>
       </c>
-      <c r="H125" s="156">
-        <v>0</v>
-      </c>
-      <c r="I125" s="156">
+      <c r="H127" s="156">
+        <v>0</v>
+      </c>
+      <c r="I127" s="156">
         <v>95</v>
-      </c>
-      <c r="J125" s="156"/>
-      <c r="K125" s="157">
-        <v>0.15</v>
-      </c>
-      <c r="L125" s="156">
-        <v>0</v>
-      </c>
-      <c r="M125" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="N125" s="171">
-        <v>3</v>
-      </c>
-      <c r="O125" s="171">
-        <v>5</v>
-      </c>
-      <c r="P125" s="172">
-        <v>4</v>
-      </c>
-      <c r="Q125" s="171">
-        <v>3</v>
-      </c>
-      <c r="R125" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="S125" s="158" t="b">
-        <v>0</v>
-      </c>
-      <c r="T125" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="U125" s="158">
-        <v>800</v>
-      </c>
-      <c r="V125" s="156">
-        <v>12</v>
-      </c>
-      <c r="W125" s="158">
-        <v>0</v>
-      </c>
-      <c r="X125" s="160">
-        <v>0.25</v>
-      </c>
-      <c r="Y125" s="160">
-        <v>0.25</v>
-      </c>
-      <c r="Z125" s="160">
-        <v>0</v>
-      </c>
-      <c r="AA125" s="160">
-        <v>0</v>
-      </c>
-      <c r="AB125" s="155" t="s">
-        <v>204</v>
-      </c>
-      <c r="AC125" s="156" t="s">
-        <v>203</v>
-      </c>
-      <c r="AD125" s="156" t="s">
-        <v>202</v>
-      </c>
-      <c r="AE125" s="156"/>
-      <c r="AF125" s="161"/>
-    </row>
-    <row r="126" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="152" t="s">
-        <v>2</v>
-      </c>
-      <c r="B126" s="153" t="s">
-        <v>86</v>
-      </c>
-      <c r="C126" s="154" t="s">
-        <v>84</v>
-      </c>
-      <c r="D126" s="155">
-        <v>20</v>
-      </c>
-      <c r="E126" s="156">
-        <v>2</v>
-      </c>
-      <c r="F126" s="156">
-        <v>0</v>
-      </c>
-      <c r="G126" s="156">
-        <v>15</v>
-      </c>
-      <c r="H126" s="156">
-        <v>0</v>
-      </c>
-      <c r="I126" s="156">
-        <v>25</v>
-      </c>
-      <c r="J126" s="156"/>
-      <c r="K126" s="157">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="L126" s="156">
-        <v>0</v>
-      </c>
-      <c r="M126" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="N126" s="171">
-        <v>5</v>
-      </c>
-      <c r="O126" s="173">
-        <v>5</v>
-      </c>
-      <c r="P126" s="172">
-        <v>0</v>
-      </c>
-      <c r="Q126" s="171">
-        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>0</v>
-      </c>
-      <c r="R126" s="158" t="b">
-        <v>1</v>
-      </c>
-      <c r="S126" s="158" t="b">
-        <v>0</v>
-      </c>
-      <c r="T126" s="156" t="b">
-        <v>0</v>
-      </c>
-      <c r="U126" s="158">
-        <v>1</v>
-      </c>
-      <c r="V126" s="156">
-        <v>9</v>
-      </c>
-      <c r="W126" s="158">
-        <v>0</v>
-      </c>
-      <c r="X126" s="159">
-        <v>0.05</v>
-      </c>
-      <c r="Y126" s="160">
-        <v>0.05</v>
-      </c>
-      <c r="Z126" s="160">
-        <v>0</v>
-      </c>
-      <c r="AA126" s="160">
-        <v>0</v>
-      </c>
-      <c r="AB126" s="155" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC126" s="156" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD126" s="156" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE126" s="156"/>
-      <c r="AF126" s="159"/>
-    </row>
-    <row r="127" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="152" t="s">
-        <v>2</v>
-      </c>
-      <c r="B127" s="153" t="s">
-        <v>305</v>
-      </c>
-      <c r="C127" s="154" t="s">
-        <v>84</v>
-      </c>
-      <c r="D127" s="155">
-        <v>60</v>
-      </c>
-      <c r="E127" s="156">
-        <v>2</v>
-      </c>
-      <c r="F127" s="156">
-        <v>0</v>
-      </c>
-      <c r="G127" s="156">
-        <v>15</v>
-      </c>
-      <c r="H127" s="156">
-        <v>0</v>
-      </c>
-      <c r="I127" s="156">
-        <v>75</v>
       </c>
       <c r="J127" s="156"/>
       <c r="K127" s="157">
-        <v>0.22499999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="L127" s="156">
         <v>0</v>
@@ -15505,18 +15536,17 @@
       <c r="M127" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="N127" s="173">
-        <v>5</v>
-      </c>
-      <c r="O127" s="173">
+      <c r="N127" s="171">
+        <v>3</v>
+      </c>
+      <c r="O127" s="171">
         <v>5</v>
       </c>
       <c r="P127" s="172">
-        <v>0</v>
-      </c>
-      <c r="Q127" s="173">
-        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="Q127" s="171">
+        <v>3</v>
       </c>
       <c r="R127" s="158" t="b">
         <v>1</v>
@@ -15525,22 +15555,22 @@
         <v>0</v>
       </c>
       <c r="T127" s="158" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U127" s="158">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="V127" s="156">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="W127" s="158">
         <v>0</v>
       </c>
-      <c r="X127" s="159">
-        <v>0.05</v>
+      <c r="X127" s="160">
+        <v>0.25</v>
       </c>
       <c r="Y127" s="160">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Z127" s="160">
         <v>0</v>
@@ -15549,13 +15579,13 @@
         <v>0</v>
       </c>
       <c r="AB127" s="155" t="s">
-        <v>83</v>
+        <v>204</v>
       </c>
       <c r="AC127" s="156" t="s">
-        <v>82</v>
+        <v>203</v>
       </c>
       <c r="AD127" s="156" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="AE127" s="156"/>
       <c r="AF127" s="161"/>
@@ -15565,32 +15595,32 @@
         <v>2</v>
       </c>
       <c r="B128" s="153" t="s">
-        <v>260</v>
+        <v>86</v>
       </c>
       <c r="C128" s="154" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="D128" s="155">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E128" s="156">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F128" s="156">
         <v>0</v>
       </c>
       <c r="G128" s="156">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H128" s="156">
         <v>0</v>
       </c>
       <c r="I128" s="156">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="J128" s="156"/>
       <c r="K128" s="157">
-        <v>0.15</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L128" s="156">
         <v>0</v>
@@ -15598,17 +15628,18 @@
       <c r="M128" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="N128" s="173">
+      <c r="N128" s="171">
         <v>5</v>
       </c>
       <c r="O128" s="173">
         <v>5</v>
       </c>
-      <c r="P128" s="174">
-        <v>1</v>
-      </c>
-      <c r="Q128" s="173">
-        <v>1</v>
+      <c r="P128" s="172">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="171">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>0</v>
       </c>
       <c r="R128" s="158" t="b">
         <v>1</v>
@@ -15616,77 +15647,73 @@
       <c r="S128" s="158" t="b">
         <v>0</v>
       </c>
-      <c r="T128" s="158" t="b">
+      <c r="T128" s="156" t="b">
         <v>0</v>
       </c>
       <c r="U128" s="158">
         <v>1</v>
       </c>
       <c r="V128" s="156">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="W128" s="158">
         <v>0</v>
       </c>
-      <c r="X128" s="160">
-        <v>0.1</v>
+      <c r="X128" s="159">
+        <v>0.05</v>
       </c>
       <c r="Y128" s="160">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="Z128" s="160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA128" s="160">
         <v>0</v>
       </c>
       <c r="AB128" s="155" t="s">
-        <v>259</v>
+        <v>83</v>
       </c>
       <c r="AC128" s="156" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
       <c r="AD128" s="156" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE128" s="156" t="s">
-        <v>258</v>
-      </c>
-      <c r="AF128" s="156" t="s">
-        <v>257</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="AE128" s="156"/>
+      <c r="AF128" s="159"/>
     </row>
     <row r="129" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B129" s="153" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="C129" s="154" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="D129" s="155">
-        <v>360</v>
+        <v>60</v>
       </c>
       <c r="E129" s="156">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="F129" s="156">
         <v>0</v>
       </c>
       <c r="G129" s="156">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="H129" s="156">
         <v>0</v>
       </c>
       <c r="I129" s="156">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="J129" s="156"/>
       <c r="K129" s="157">
-        <v>0.15</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="L129" s="156">
         <v>0</v>
@@ -15694,17 +15721,18 @@
       <c r="M129" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="N129" s="171">
-        <v>4</v>
-      </c>
-      <c r="O129" s="171">
+      <c r="N129" s="173">
+        <v>5</v>
+      </c>
+      <c r="O129" s="173">
         <v>5</v>
       </c>
       <c r="P129" s="172">
-        <v>5</v>
-      </c>
-      <c r="Q129" s="171">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="Q129" s="173">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>0</v>
       </c>
       <c r="R129" s="158" t="b">
         <v>1</v>
@@ -15713,22 +15741,22 @@
         <v>0</v>
       </c>
       <c r="T129" s="158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U129" s="158">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="V129" s="156">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="W129" s="158">
         <v>0</v>
       </c>
-      <c r="X129" s="160">
-        <v>0.25</v>
+      <c r="X129" s="159">
+        <v>0.05</v>
       </c>
       <c r="Y129" s="160">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="Z129" s="160">
         <v>0</v>
@@ -15737,13 +15765,13 @@
         <v>0</v>
       </c>
       <c r="AB129" s="155" t="s">
-        <v>204</v>
+        <v>83</v>
       </c>
       <c r="AC129" s="156" t="s">
-        <v>203</v>
+        <v>82</v>
       </c>
       <c r="AD129" s="156" t="s">
-        <v>202</v>
+        <v>81</v>
       </c>
       <c r="AE129" s="156"/>
       <c r="AF129" s="161"/>
@@ -15753,28 +15781,28 @@
         <v>2</v>
       </c>
       <c r="B130" s="153" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="C130" s="154" t="s">
         <v>66</v>
       </c>
       <c r="D130" s="155">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="E130" s="156">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F130" s="156">
         <v>0</v>
       </c>
       <c r="G130" s="156">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H130" s="156">
         <v>0</v>
       </c>
       <c r="I130" s="156">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="J130" s="156"/>
       <c r="K130" s="157">
@@ -15786,17 +15814,17 @@
       <c r="M130" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="N130" s="171">
-        <v>5</v>
-      </c>
-      <c r="O130" s="171">
-        <v>5</v>
-      </c>
-      <c r="P130" s="172">
-        <v>3</v>
-      </c>
-      <c r="Q130" s="171">
-        <v>3</v>
+      <c r="N130" s="173">
+        <v>5</v>
+      </c>
+      <c r="O130" s="173">
+        <v>5</v>
+      </c>
+      <c r="P130" s="174">
+        <v>1</v>
+      </c>
+      <c r="Q130" s="173">
+        <v>1</v>
       </c>
       <c r="R130" s="158" t="b">
         <v>1</v>
@@ -15804,73 +15832,77 @@
       <c r="S130" s="158" t="b">
         <v>0</v>
       </c>
-      <c r="T130" s="156" t="b">
+      <c r="T130" s="158" t="b">
         <v>0</v>
       </c>
       <c r="U130" s="158">
         <v>1</v>
       </c>
       <c r="V130" s="156">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="W130" s="158">
         <v>0</v>
       </c>
       <c r="X130" s="160">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="Y130" s="160">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="Z130" s="160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA130" s="160">
         <v>0</v>
       </c>
       <c r="AB130" s="155" t="s">
-        <v>204</v>
+        <v>259</v>
       </c>
       <c r="AC130" s="156" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="AD130" s="156" t="s">
-        <v>202</v>
-      </c>
-      <c r="AE130" s="156"/>
-      <c r="AF130" s="159"/>
-    </row>
-    <row r="131" spans="1:32" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="AE130" s="156" t="s">
+        <v>258</v>
+      </c>
+      <c r="AF130" s="156" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="131" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B131" s="153" t="s">
-        <v>201</v>
+        <v>337</v>
       </c>
       <c r="C131" s="154" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="D131" s="155">
-        <v>60</v>
+        <v>360</v>
       </c>
       <c r="E131" s="156">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="F131" s="156">
         <v>0</v>
       </c>
       <c r="G131" s="156">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="H131" s="156">
         <v>0</v>
       </c>
       <c r="I131" s="156">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="J131" s="156"/>
       <c r="K131" s="157">
-        <v>0.22499999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="L131" s="156">
         <v>0</v>
@@ -15878,32 +15910,32 @@
       <c r="M131" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="N131" s="173">
-        <v>5</v>
-      </c>
-      <c r="O131" s="173">
-        <v>0</v>
-      </c>
-      <c r="P131" s="174">
-        <v>1</v>
-      </c>
-      <c r="Q131" s="173">
-        <v>0</v>
+      <c r="N131" s="171">
+        <v>4</v>
+      </c>
+      <c r="O131" s="171">
+        <v>5</v>
+      </c>
+      <c r="P131" s="172">
+        <v>5</v>
+      </c>
+      <c r="Q131" s="171">
+        <v>4</v>
       </c>
       <c r="R131" s="158" t="b">
         <v>1</v>
       </c>
       <c r="S131" s="158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T131" s="158" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U131" s="158">
-        <v>75</v>
+        <v>1000</v>
       </c>
       <c r="V131" s="156">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="W131" s="158">
         <v>0</v>
@@ -15915,54 +15947,50 @@
         <v>0.25</v>
       </c>
       <c r="Z131" s="160">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AA131" s="160">
         <v>0</v>
       </c>
       <c r="AB131" s="155" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="AC131" s="156" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="AD131" s="156" t="s">
-        <v>198</v>
-      </c>
-      <c r="AE131" s="156" t="s">
-        <v>197</v>
-      </c>
-      <c r="AF131" s="162" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="AE131" s="156"/>
+      <c r="AF131" s="161"/>
+    </row>
+    <row r="132" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B132" s="153" t="s">
-        <v>74</v>
+        <v>228</v>
       </c>
       <c r="C132" s="154" t="s">
         <v>66</v>
       </c>
       <c r="D132" s="155">
-        <v>40</v>
+        <v>220</v>
       </c>
       <c r="E132" s="156">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F132" s="156">
         <v>0</v>
       </c>
       <c r="G132" s="156">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H132" s="156">
         <v>0</v>
       </c>
       <c r="I132" s="156">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="J132" s="156"/>
       <c r="K132" s="157">
@@ -15971,323 +15999,413 @@
       <c r="L132" s="156">
         <v>0</v>
       </c>
-      <c r="M132" s="163" t="b">
-        <v>1</v>
-      </c>
-      <c r="N132" s="175">
-        <v>5</v>
-      </c>
-      <c r="O132" s="175">
-        <v>5</v>
-      </c>
-      <c r="P132" s="176">
-        <v>0</v>
-      </c>
-      <c r="Q132" s="175">
-        <v>0</v>
+      <c r="M132" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="N132" s="171">
+        <v>5</v>
+      </c>
+      <c r="O132" s="171">
+        <v>5</v>
+      </c>
+      <c r="P132" s="172">
+        <v>3</v>
+      </c>
+      <c r="Q132" s="171">
+        <v>3</v>
       </c>
       <c r="R132" s="158" t="b">
         <v>1</v>
       </c>
-      <c r="S132" s="165" t="b">
-        <v>0</v>
-      </c>
-      <c r="T132" s="165" t="b">
+      <c r="S132" s="158" t="b">
+        <v>0</v>
+      </c>
+      <c r="T132" s="156" t="b">
         <v>0</v>
       </c>
       <c r="U132" s="158">
+        <v>1</v>
+      </c>
+      <c r="V132" s="156">
+        <v>9</v>
+      </c>
+      <c r="W132" s="158">
+        <v>0</v>
+      </c>
+      <c r="X132" s="160">
+        <v>0.25</v>
+      </c>
+      <c r="Y132" s="160">
+        <v>0.25</v>
+      </c>
+      <c r="Z132" s="160">
+        <v>0</v>
+      </c>
+      <c r="AA132" s="160">
+        <v>0</v>
+      </c>
+      <c r="AB132" s="155" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC132" s="156" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD132" s="156" t="s">
+        <v>202</v>
+      </c>
+      <c r="AE132" s="156"/>
+      <c r="AF132" s="159"/>
+    </row>
+    <row r="133" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A133" s="152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B133" s="153" t="s">
+        <v>201</v>
+      </c>
+      <c r="C133" s="154" t="s">
+        <v>90</v>
+      </c>
+      <c r="D133" s="155">
+        <v>60</v>
+      </c>
+      <c r="E133" s="156">
+        <v>2</v>
+      </c>
+      <c r="F133" s="156">
+        <v>0</v>
+      </c>
+      <c r="G133" s="156">
+        <v>20</v>
+      </c>
+      <c r="H133" s="156">
+        <v>0</v>
+      </c>
+      <c r="I133" s="156">
+        <v>75</v>
+      </c>
+      <c r="J133" s="156"/>
+      <c r="K133" s="157">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="L133" s="156">
+        <v>0</v>
+      </c>
+      <c r="M133" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="N133" s="173">
+        <v>5</v>
+      </c>
+      <c r="O133" s="173">
+        <v>0</v>
+      </c>
+      <c r="P133" s="174">
+        <v>1</v>
+      </c>
+      <c r="Q133" s="173">
+        <v>0</v>
+      </c>
+      <c r="R133" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="S133" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="T133" s="158" t="b">
+        <v>0</v>
+      </c>
+      <c r="U133" s="158">
+        <v>75</v>
+      </c>
+      <c r="V133" s="156">
+        <v>7</v>
+      </c>
+      <c r="W133" s="158">
+        <v>0</v>
+      </c>
+      <c r="X133" s="160">
+        <v>0.25</v>
+      </c>
+      <c r="Y133" s="160">
+        <v>0.25</v>
+      </c>
+      <c r="Z133" s="160">
+        <v>0.7</v>
+      </c>
+      <c r="AA133" s="160">
+        <v>0</v>
+      </c>
+      <c r="AB133" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC133" s="156" t="s">
+        <v>199</v>
+      </c>
+      <c r="AD133" s="156" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE133" s="156" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF133" s="162" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="134" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A134" s="152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B134" s="153" t="s">
+        <v>74</v>
+      </c>
+      <c r="C134" s="154" t="s">
+        <v>66</v>
+      </c>
+      <c r="D134" s="155">
+        <v>40</v>
+      </c>
+      <c r="E134" s="156">
+        <v>2</v>
+      </c>
+      <c r="F134" s="156">
+        <v>0</v>
+      </c>
+      <c r="G134" s="156">
+        <v>30</v>
+      </c>
+      <c r="H134" s="156">
+        <v>0</v>
+      </c>
+      <c r="I134" s="156">
+        <v>50</v>
+      </c>
+      <c r="J134" s="156"/>
+      <c r="K134" s="157">
+        <v>0.15</v>
+      </c>
+      <c r="L134" s="156">
+        <v>0</v>
+      </c>
+      <c r="M134" s="163" t="b">
+        <v>1</v>
+      </c>
+      <c r="N134" s="175">
+        <v>5</v>
+      </c>
+      <c r="O134" s="175">
+        <v>5</v>
+      </c>
+      <c r="P134" s="176">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="175">
+        <v>0</v>
+      </c>
+      <c r="R134" s="158" t="b">
+        <v>1</v>
+      </c>
+      <c r="S134" s="165" t="b">
+        <v>0</v>
+      </c>
+      <c r="T134" s="165" t="b">
+        <v>0</v>
+      </c>
+      <c r="U134" s="158">
         <v>85</v>
       </c>
-      <c r="V132" s="164">
+      <c r="V134" s="164">
         <v>9</v>
       </c>
-      <c r="W132" s="163">
-        <v>0</v>
-      </c>
-      <c r="X132" s="166">
+      <c r="W134" s="163">
+        <v>0</v>
+      </c>
+      <c r="X134" s="166">
         <v>0.25</v>
       </c>
-      <c r="Y132" s="166">
+      <c r="Y134" s="166">
         <v>0.25</v>
       </c>
-      <c r="Z132" s="166">
+      <c r="Z134" s="166">
         <v>0.75</v>
       </c>
-      <c r="AA132" s="166">
-        <v>0</v>
-      </c>
-      <c r="AB132" s="167" t="s">
+      <c r="AA134" s="166">
+        <v>0</v>
+      </c>
+      <c r="AB134" s="167" t="s">
         <v>73</v>
       </c>
-      <c r="AC132" s="164" t="s">
+      <c r="AC134" s="164" t="s">
         <v>72</v>
       </c>
-      <c r="AD132" s="164" t="s">
+      <c r="AD134" s="164" t="s">
         <v>71</v>
       </c>
-      <c r="AE132" s="164"/>
-      <c r="AF132" s="168"/>
-    </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A133" s="119"/>
-      <c r="B133" s="119"/>
-      <c r="C133" s="119"/>
-      <c r="D133" s="120"/>
-      <c r="E133" s="121"/>
-      <c r="F133" s="121"/>
-      <c r="G133" s="121"/>
-      <c r="H133" s="121"/>
-      <c r="I133" s="121"/>
-      <c r="J133" s="122"/>
-      <c r="K133" s="121"/>
-      <c r="L133" s="123"/>
-      <c r="M133" s="124"/>
-      <c r="N133" s="124"/>
-      <c r="O133" s="125"/>
-      <c r="P133" s="124"/>
-      <c r="Q133" s="126"/>
-      <c r="R133" s="127"/>
-      <c r="S133" s="127"/>
-      <c r="T133" s="126"/>
-      <c r="U133" s="127"/>
-      <c r="V133" s="128"/>
-      <c r="W133" s="129"/>
-      <c r="X133" s="130"/>
-      <c r="Y133" s="130"/>
-      <c r="Z133" s="131"/>
-      <c r="AA133" s="132"/>
-      <c r="AB133" s="132"/>
-      <c r="AC133" s="133"/>
-      <c r="AD133" s="133"/>
-      <c r="AE133" s="134"/>
-    </row>
-    <row r="134" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="135" spans="1:32" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A135" s="9" t="s">
+      <c r="AE134" s="164"/>
+      <c r="AF134" s="168"/>
+    </row>
+    <row r="135" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A135" s="119"/>
+      <c r="B135" s="119"/>
+      <c r="C135" s="119"/>
+      <c r="D135" s="120"/>
+      <c r="E135" s="121"/>
+      <c r="F135" s="121"/>
+      <c r="G135" s="121"/>
+      <c r="H135" s="121"/>
+      <c r="I135" s="121"/>
+      <c r="J135" s="122"/>
+      <c r="K135" s="121"/>
+      <c r="L135" s="123"/>
+      <c r="M135" s="124"/>
+      <c r="N135" s="124"/>
+      <c r="O135" s="125"/>
+      <c r="P135" s="124"/>
+      <c r="Q135" s="126"/>
+      <c r="R135" s="127"/>
+      <c r="S135" s="127"/>
+      <c r="T135" s="126"/>
+      <c r="U135" s="127"/>
+      <c r="V135" s="128"/>
+      <c r="W135" s="129"/>
+      <c r="X135" s="130"/>
+      <c r="Y135" s="130"/>
+      <c r="Z135" s="131"/>
+      <c r="AA135" s="132"/>
+      <c r="AB135" s="132"/>
+      <c r="AC135" s="133"/>
+      <c r="AD135" s="133"/>
+      <c r="AE135" s="134"/>
+    </row>
+    <row r="136" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="137" spans="1:32" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A137" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B135" s="9"/>
-      <c r="C135" s="9"/>
-      <c r="D135" s="9"/>
-      <c r="E135" s="9"/>
-      <c r="F135" s="9"/>
-      <c r="G135" s="9"/>
-      <c r="H135" s="9"/>
-      <c r="I135" s="9"/>
-      <c r="J135" s="9"/>
-      <c r="K135" s="9"/>
-      <c r="L135" s="9"/>
-      <c r="M135" s="9"/>
-      <c r="N135" s="9"/>
-      <c r="O135" s="9"/>
-      <c r="P135" s="9"/>
-      <c r="Q135" s="9"/>
-      <c r="R135" s="9"/>
-      <c r="S135" s="9"/>
-      <c r="T135" s="9"/>
-      <c r="U135" s="9"/>
-      <c r="V135" s="9"/>
-      <c r="W135" s="9"/>
-      <c r="X135" s="9"/>
-      <c r="Y135" s="9"/>
-      <c r="Z135" s="9"/>
-      <c r="AA135" s="9"/>
-      <c r="AB135"/>
-      <c r="AC135"/>
-      <c r="AD135"/>
-      <c r="AE135"/>
-    </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A136" s="22"/>
-      <c r="B136" s="22"/>
-      <c r="C136" s="22"/>
-      <c r="D136" s="22"/>
-      <c r="E136" s="22"/>
-      <c r="F136" s="178"/>
-      <c r="G136" s="178"/>
-      <c r="H136" s="21" t="s">
+      <c r="B137" s="9"/>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+      <c r="H137" s="9"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="9"/>
+      <c r="K137" s="9"/>
+      <c r="L137" s="9"/>
+      <c r="M137" s="9"/>
+      <c r="N137" s="9"/>
+      <c r="O137" s="9"/>
+      <c r="P137" s="9"/>
+      <c r="Q137" s="9"/>
+      <c r="R137" s="9"/>
+      <c r="S137" s="9"/>
+      <c r="T137" s="9"/>
+      <c r="U137" s="9"/>
+      <c r="V137" s="9"/>
+      <c r="W137" s="9"/>
+      <c r="X137" s="9"/>
+      <c r="Y137" s="9"/>
+      <c r="Z137" s="9"/>
+      <c r="AA137" s="9"/>
+      <c r="AB137"/>
+      <c r="AC137"/>
+      <c r="AD137"/>
+      <c r="AE137"/>
+    </row>
+    <row r="138" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A138" s="22"/>
+      <c r="B138" s="22"/>
+      <c r="C138" s="22"/>
+      <c r="D138" s="22"/>
+      <c r="E138" s="22"/>
+      <c r="F138" s="178"/>
+      <c r="G138" s="178"/>
+      <c r="H138" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I136" s="21"/>
-      <c r="J136" s="22"/>
-      <c r="K136" s="17"/>
-      <c r="L136" s="17"/>
-      <c r="M136" s="17" t="s">
+      <c r="I138" s="21"/>
+      <c r="J138" s="22"/>
+      <c r="K138" s="17"/>
+      <c r="L138" s="17"/>
+      <c r="M138" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N136" s="17"/>
-      <c r="O136" s="17"/>
-      <c r="P136" s="17"/>
-      <c r="Q136" s="17"/>
-      <c r="R136" s="17"/>
-      <c r="S136" s="17"/>
-      <c r="T136" s="17"/>
-      <c r="U136" s="17"/>
-      <c r="V136" s="17"/>
-      <c r="W136" s="17"/>
-      <c r="X136" s="17"/>
-      <c r="Y136" s="17"/>
-      <c r="Z136" s="17"/>
-      <c r="AA136" s="21"/>
-      <c r="AB136" s="21"/>
-      <c r="AC136" s="21"/>
-      <c r="AD136" s="21"/>
-      <c r="AE136" s="17"/>
-    </row>
-    <row r="137" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D137" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E137" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F137" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G137" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H137" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I137" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="J137" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="K137" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="L137" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="M137" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="N137" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O137" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A138" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B138" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C138" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D138" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E138" s="14">
-        <v>3</v>
-      </c>
-      <c r="F138" s="18">
-        <v>0</v>
-      </c>
-      <c r="G138" s="18">
-        <v>0</v>
-      </c>
-      <c r="H138" s="18">
-        <v>0</v>
-      </c>
-      <c r="I138" s="18">
-        <v>0</v>
-      </c>
-      <c r="J138" s="12">
-        <v>2</v>
-      </c>
-      <c r="K138" s="12">
-        <v>0</v>
-      </c>
-      <c r="L138" s="12">
-        <v>0</v>
-      </c>
-      <c r="M138" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N138" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O138" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N138" s="17"/>
+      <c r="O138" s="17"/>
       <c r="P138" s="17"/>
       <c r="Q138" s="17"/>
-    </row>
-    <row r="139" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A139" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B139" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C139" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D139" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E139" s="14">
-        <v>3</v>
-      </c>
-      <c r="F139" s="18">
-        <v>0</v>
-      </c>
-      <c r="G139" s="18">
-        <v>1</v>
-      </c>
-      <c r="H139" s="18">
-        <v>0</v>
-      </c>
-      <c r="I139" s="18">
-        <v>0</v>
-      </c>
-      <c r="J139" s="12">
-        <v>2</v>
-      </c>
-      <c r="K139" s="12">
-        <v>0</v>
-      </c>
-      <c r="L139" s="12">
-        <v>0</v>
-      </c>
-      <c r="M139" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N139" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O139" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P139" s="17"/>
-      <c r="Q139" s="17"/>
+      <c r="R138" s="17"/>
+      <c r="S138" s="17"/>
+      <c r="T138" s="17"/>
+      <c r="U138" s="17"/>
+      <c r="V138" s="17"/>
+      <c r="W138" s="17"/>
+      <c r="X138" s="17"/>
+      <c r="Y138" s="17"/>
+      <c r="Z138" s="17"/>
+      <c r="AA138" s="21"/>
+      <c r="AB138" s="21"/>
+      <c r="AC138" s="21"/>
+      <c r="AD138" s="21"/>
+      <c r="AE138" s="17"/>
+    </row>
+    <row r="139" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D139" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E139" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F139" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G139" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H139" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I139" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J139" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="K139" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L139" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M139" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N139" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="O139" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="140" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A140" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B140" s="15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D140" s="14" t="s">
         <v>30</v>
@@ -16333,10 +16451,10 @@
         <v>2</v>
       </c>
       <c r="B141" s="15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D141" s="14" t="s">
         <v>23</v>
@@ -16382,10 +16500,10 @@
         <v>2</v>
       </c>
       <c r="B142" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D142" s="14" t="s">
         <v>30</v>
@@ -16431,10 +16549,10 @@
         <v>2</v>
       </c>
       <c r="B143" s="15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D143" s="14" t="s">
         <v>23</v>
@@ -16480,13 +16598,13 @@
         <v>2</v>
       </c>
       <c r="B144" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C144" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E144" s="14">
         <v>3</v>
@@ -16495,7 +16613,7 @@
         <v>0</v>
       </c>
       <c r="G144" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H144" s="18">
         <v>0</v>
@@ -16529,13 +16647,13 @@
         <v>2</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E145" s="14">
         <v>3</v>
@@ -16544,7 +16662,7 @@
         <v>0</v>
       </c>
       <c r="G145" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H145" s="18">
         <v>0</v>
@@ -16578,13 +16696,13 @@
         <v>2</v>
       </c>
       <c r="B146" s="15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E146" s="14">
         <v>3</v>
@@ -16593,7 +16711,7 @@
         <v>0</v>
       </c>
       <c r="G146" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H146" s="18">
         <v>0</v>
@@ -16627,13 +16745,13 @@
         <v>2</v>
       </c>
       <c r="B147" s="15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C147" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E147" s="14">
         <v>3</v>
@@ -16642,7 +16760,7 @@
         <v>0</v>
       </c>
       <c r="G147" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H147" s="18">
         <v>0</v>
@@ -16676,27 +16794,27 @@
         <v>2</v>
       </c>
       <c r="B148" s="15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D148" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E148" s="14">
-        <v>1</v>
-      </c>
-      <c r="F148" s="13">
-        <v>0</v>
-      </c>
-      <c r="G148" s="13">
-        <v>1</v>
-      </c>
-      <c r="H148" s="13">
-        <v>0</v>
-      </c>
-      <c r="I148" s="13">
+        <v>3</v>
+      </c>
+      <c r="F148" s="18">
+        <v>0</v>
+      </c>
+      <c r="G148" s="18">
+        <v>1</v>
+      </c>
+      <c r="H148" s="18">
+        <v>0</v>
+      </c>
+      <c r="I148" s="18">
         <v>0</v>
       </c>
       <c r="J148" s="12">
@@ -16717,33 +16835,35 @@
       <c r="O148" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P148" s="17"/>
+      <c r="Q148" s="17"/>
     </row>
     <row r="149" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A149" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B149" s="96" t="s">
-        <v>463</v>
-      </c>
-      <c r="C149" s="96" t="s">
-        <v>38</v>
-      </c>
-      <c r="D149" s="146" t="s">
-        <v>30</v>
+      <c r="B149" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D149" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E149" s="14">
-        <v>1</v>
-      </c>
-      <c r="F149" s="147">
-        <v>0</v>
-      </c>
-      <c r="G149" s="147">
-        <v>0</v>
-      </c>
-      <c r="H149" s="147">
-        <v>0</v>
-      </c>
-      <c r="I149" s="147">
+        <v>3</v>
+      </c>
+      <c r="F149" s="18">
+        <v>0</v>
+      </c>
+      <c r="G149" s="18">
+        <v>2</v>
+      </c>
+      <c r="H149" s="18">
+        <v>0</v>
+      </c>
+      <c r="I149" s="18">
         <v>0</v>
       </c>
       <c r="J149" s="12">
@@ -16764,136 +16884,180 @@
       <c r="O149" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P149" s="8"/>
-      <c r="Q149" s="8"/>
-      <c r="R149" s="8"/>
-      <c r="S149" s="8"/>
-      <c r="T149" s="8"/>
-      <c r="U149" s="8"/>
-      <c r="V149" s="8"/>
-      <c r="W149" s="8"/>
-      <c r="X149" s="8"/>
-      <c r="Y149" s="8"/>
-      <c r="Z149" s="8"/>
-      <c r="AA149" s="8"/>
-      <c r="AB149" s="8"/>
-      <c r="AC149" s="8"/>
-      <c r="AD149" s="8"/>
-      <c r="AE149" s="8"/>
+      <c r="P149" s="17"/>
+      <c r="Q149" s="17"/>
     </row>
     <row r="150" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N150" s="8"/>
-      <c r="O150" s="8"/>
-      <c r="P150" s="8"/>
-      <c r="Q150" s="8"/>
-      <c r="R150" s="8"/>
-      <c r="S150" s="8"/>
-      <c r="T150" s="8"/>
-      <c r="U150" s="8"/>
-      <c r="V150" s="8"/>
-      <c r="W150" s="8"/>
-      <c r="X150" s="8"/>
-      <c r="Y150" s="8"/>
-      <c r="Z150" s="8"/>
-      <c r="AA150" s="8"/>
-      <c r="AB150" s="8"/>
-      <c r="AC150" s="8"/>
-      <c r="AD150" s="8"/>
-      <c r="AE150" s="8"/>
-    </row>
-    <row r="151" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="152" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A152" s="9" t="s">
+      <c r="A150" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D150" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E150" s="14">
+        <v>1</v>
+      </c>
+      <c r="F150" s="13">
+        <v>0</v>
+      </c>
+      <c r="G150" s="13">
+        <v>1</v>
+      </c>
+      <c r="H150" s="13">
+        <v>0</v>
+      </c>
+      <c r="I150" s="13">
+        <v>0</v>
+      </c>
+      <c r="J150" s="12">
+        <v>2</v>
+      </c>
+      <c r="K150" s="12">
+        <v>0</v>
+      </c>
+      <c r="L150" s="12">
+        <v>0</v>
+      </c>
+      <c r="M150" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N150" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O150" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A151" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B151" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C151" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="D151" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="E151" s="14">
+        <v>1</v>
+      </c>
+      <c r="F151" s="147">
+        <v>0</v>
+      </c>
+      <c r="G151" s="147">
+        <v>0</v>
+      </c>
+      <c r="H151" s="147">
+        <v>0</v>
+      </c>
+      <c r="I151" s="147">
+        <v>0</v>
+      </c>
+      <c r="J151" s="12">
+        <v>2</v>
+      </c>
+      <c r="K151" s="12">
+        <v>0</v>
+      </c>
+      <c r="L151" s="12">
+        <v>0</v>
+      </c>
+      <c r="M151" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N151" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O151" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P151" s="8"/>
+      <c r="Q151" s="8"/>
+      <c r="R151" s="8"/>
+      <c r="S151" s="8"/>
+      <c r="T151" s="8"/>
+      <c r="U151" s="8"/>
+      <c r="V151" s="8"/>
+      <c r="W151" s="8"/>
+      <c r="X151" s="8"/>
+      <c r="Y151" s="8"/>
+      <c r="Z151" s="8"/>
+      <c r="AA151" s="8"/>
+      <c r="AB151" s="8"/>
+      <c r="AC151" s="8"/>
+      <c r="AD151" s="8"/>
+      <c r="AE151" s="8"/>
+    </row>
+    <row r="152" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N152" s="8"/>
+      <c r="O152" s="8"/>
+      <c r="P152" s="8"/>
+      <c r="Q152" s="8"/>
+      <c r="R152" s="8"/>
+      <c r="S152" s="8"/>
+      <c r="T152" s="8"/>
+      <c r="U152" s="8"/>
+      <c r="V152" s="8"/>
+      <c r="W152" s="8"/>
+      <c r="X152" s="8"/>
+      <c r="Y152" s="8"/>
+      <c r="Z152" s="8"/>
+      <c r="AA152" s="8"/>
+      <c r="AB152" s="8"/>
+      <c r="AC152" s="8"/>
+      <c r="AD152" s="8"/>
+      <c r="AE152" s="8"/>
+    </row>
+    <row r="153" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A154" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B152" s="9"/>
-      <c r="C152" s="9"/>
-      <c r="D152" s="9"/>
-      <c r="E152" s="8"/>
-      <c r="F152" s="8"/>
-      <c r="G152" s="8"/>
-      <c r="H152" s="8"/>
-      <c r="I152" s="8"/>
-      <c r="J152" s="8"/>
-      <c r="K152" s="8"/>
-      <c r="L152" s="8"/>
-    </row>
-    <row r="154" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="7" t="s">
+      <c r="B154" s="9"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="8"/>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="8"/>
+      <c r="I154" s="8"/>
+      <c r="J154" s="8"/>
+      <c r="K154" s="8"/>
+      <c r="L154" s="8"/>
+    </row>
+    <row r="156" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B154" s="6" t="s">
+      <c r="B156" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C154" s="6" t="s">
+      <c r="C156" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D154" s="5" t="s">
+      <c r="D156" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E154" s="5" t="s">
+      <c r="E156" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F154" s="5" t="s">
+      <c r="F156" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G154" s="5" t="s">
+      <c r="G156" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H154" s="5" t="s">
+      <c r="H156" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="155" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A155" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D155" s="2">
-        <v>42</v>
-      </c>
-      <c r="E155" s="2">
-        <v>8</v>
-      </c>
-      <c r="F155" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G155" s="2">
-        <v>2</v>
-      </c>
-      <c r="H155" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A156" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D156" s="2">
-        <v>92</v>
-      </c>
-      <c r="E156" s="2">
-        <v>10</v>
-      </c>
-      <c r="F156" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G156" s="2">
-        <v>2</v>
-      </c>
-      <c r="H156" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:31" x14ac:dyDescent="0.25">
@@ -16901,19 +17065,19 @@
         <v>2</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D157" s="2">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="E157" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F157" s="2">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="G157" s="2">
         <v>2</v>
@@ -16927,19 +17091,19 @@
         <v>2</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D158" s="2">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="E158" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F158" s="2">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G158" s="2">
         <v>2</v>
@@ -16953,104 +17117,156 @@
         <v>2</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D159" s="2">
+        <v>235</v>
+      </c>
+      <c r="E159" s="2">
+        <v>12</v>
+      </c>
+      <c r="F159" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G159" s="2">
+        <v>2</v>
+      </c>
+      <c r="H159" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D160" s="2">
+        <v>686</v>
+      </c>
+      <c r="E160" s="2">
+        <v>14</v>
+      </c>
+      <c r="F160" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G160" s="2">
+        <v>2</v>
+      </c>
+      <c r="H160" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D161" s="2">
         <v>1040</v>
       </c>
-      <c r="E159" s="2">
+      <c r="E161" s="2">
         <v>14</v>
       </c>
-      <c r="F159" s="2">
+      <c r="F161" s="2">
         <v>0.5</v>
       </c>
-      <c r="G159" s="2">
-        <v>2</v>
-      </c>
-      <c r="H159" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D162" s="1">
+      <c r="G161" s="2">
+        <v>2</v>
+      </c>
+      <c r="H161" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D164" s="1">
         <v>42</v>
       </c>
-      <c r="F162" s="1">
+      <c r="F164" s="1">
         <v>1.3</v>
-      </c>
-      <c r="G162">
-        <f>D155*F155</f>
-        <v>54.6</v>
-      </c>
-      <c r="I162">
-        <f>D162*F162</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="163" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D163" s="1">
-        <v>92</v>
-      </c>
-      <c r="F163" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G163">
-        <f>D156*F156</f>
-        <v>101.2</v>
-      </c>
-      <c r="I163">
-        <f>D163*F163</f>
-        <v>101.2</v>
-      </c>
-    </row>
-    <row r="164" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D164" s="1">
-        <v>235</v>
-      </c>
-      <c r="F164" s="1">
-        <v>0.9</v>
       </c>
       <c r="G164">
         <f>D157*F157</f>
-        <v>211.5</v>
+        <v>54.6</v>
       </c>
       <c r="I164">
         <f>D164*F164</f>
-        <v>211.5</v>
-      </c>
-    </row>
-    <row r="165" spans="4:9" x14ac:dyDescent="0.25">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D165" s="1">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="F165" s="1">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G165">
         <f>D158*F158</f>
-        <v>480.2</v>
+        <v>101.2</v>
       </c>
       <c r="I165">
         <f>D165*F165</f>
-        <v>480.2</v>
-      </c>
-    </row>
-    <row r="166" spans="4:9" x14ac:dyDescent="0.25">
+        <v>101.2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D166" s="1">
-        <v>1040</v>
+        <v>235</v>
       </c>
       <c r="F166" s="1">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G166">
         <f>D159*F159</f>
-        <v>520</v>
+        <v>211.5</v>
       </c>
       <c r="I166">
         <f>D166*F166</f>
+        <v>211.5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D167" s="1">
+        <v>686</v>
+      </c>
+      <c r="F167" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G167">
+        <f>D160*F160</f>
+        <v>480.2</v>
+      </c>
+      <c r="I167">
+        <f>D167*F167</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D168" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F168" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G168">
+        <f>D161*F161</f>
+        <v>520</v>
+      </c>
+      <c r="I168">
+        <f>D168*F168</f>
         <v>520</v>
       </c>
     </row>
@@ -17058,15 +17274,15 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F136:G136"/>
+    <mergeCell ref="F138:G138"/>
   </mergeCells>
-  <conditionalFormatting sqref="M24:M122 R24:T122 M125:M132 R125:T132">
-    <cfRule type="expression" dxfId="95" priority="11">
+  <conditionalFormatting sqref="M24:M122 R24:T122 M127:M134 R127:T134">
+    <cfRule type="expression" dxfId="4" priority="15">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N125:Q132 N24:Q122">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="N127:Q134 N24:Q122">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17078,12 +17294,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M123 R123:T123">
-    <cfRule type="expression" dxfId="94" priority="4">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>M123=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N123:Q123">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17094,12 +17310,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M124 R124:T124">
-    <cfRule type="expression" dxfId="93" priority="2">
+  <conditionalFormatting sqref="M124:M126 R124:T126">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>M124=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N124:Q124">
+  <conditionalFormatting sqref="N124:Q126">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -17113,32 +17329,32 @@
   </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G42"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G24:I40 G43:I133 J24:J132">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H41:I42 G41 G24:I40 J24:J134 G43:I135">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D138:G149 N24:O132 M133:N133 Q24:W132 P133:V133">
+    <dataValidation type="decimal" allowBlank="1" sqref="D140:G151 M135:N135 P135:V135 Q24:W134 N24:O134">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H138:L147 H148:I148 J149:L149 X24:AA132 W133:Z133">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H140:L149 H150:I150 J151:L151 W135:Z135 X24:AA134">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C138:C149 C24:C133">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C140:C151 C24:C135">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J148:L148 M138:O149 AB94:AB120 AB86:AB92 AB24:AF85 AC86:AF120 AB121:AF132 AA133:AE133"/>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F133">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J150:L150 M140:O151 AB94:AB120 AB86:AB92 AB24:AF85 AC86:AF120 AA135:AE135 AB121:AF134"/>
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F135">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="O133 P24:P132">
+    <dataValidation type="list" sqref="O135 P24:P134">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J133:K133 K24:L132">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J135:K135 K24:L134">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="L133 M24:M132">
+    <dataValidation type="list" sqref="L135 M24:M134">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Content - Fix bad values in EntitiyDef
Former-commit-id: 91cbd08336b8f67a880520db4b5820fbaccac5d7
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5282,10 +5282,10 @@
   </sheetPr>
   <dimension ref="A1:AF168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="F40" sqref="F40"/>
+      <selection pane="topRight" activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9640,7 +9640,7 @@
         <v>60</v>
       </c>
       <c r="E66" s="65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F66" s="65">
         <v>1</v>
@@ -9658,7 +9658,7 @@
         <v>0</v>
       </c>
       <c r="K66" s="53">
-        <v>0.22499999999999998</v>
+        <v>0</v>
       </c>
       <c r="L66" s="65">
         <v>1</v>
@@ -10432,7 +10432,7 @@
         <v>0</v>
       </c>
       <c r="K74" s="42">
-        <v>1</v>
+        <v>0.23</v>
       </c>
       <c r="L74" s="76">
         <v>0</v>
@@ -10625,7 +10625,7 @@
         <v>0</v>
       </c>
       <c r="K76" s="42">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="L76" s="76">
         <v>0</v>
@@ -10718,7 +10718,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="53">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="L77" s="65">
         <v>0</v>

</xml_diff>

<commit_message>
Mark some entities maybe are not used
Former-commit-id: 74a0d9c0f9c010fa2a90c032e3d4bcb2047d6581
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -1641,7 +1641,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1753,6 +1753,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2071,7 +2077,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2435,9 +2441,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2485,9 +2488,6 @@
     <xf numFmtId="0" fontId="7" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2510,145 +2510,58 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="112">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4944,6 +4857,139 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4958,58 +5004,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF137" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF137" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF137"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="106"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="105"/>
-    <tableColumn id="6" name="[category]" dataDxfId="104"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="103"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="102"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="101"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="100"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="99"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="98"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="97"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="96"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="95"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="94"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="93"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="92"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="91"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="90"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="89"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="88"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="87"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="86"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="85"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="84"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="83"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="82"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="81"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="80"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="79"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="78"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="77"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="76"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="75"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="74" headerRowBorderDxfId="73" tableBorderDxfId="72" totalsRowBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="70"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="69"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5022,50 +5068,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="4" name="[category]" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="16" name="[size]" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="34"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
-    <tableColumn id="6" name="[order]" dataDxfId="32"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="31"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="30"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="29"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="28"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="22"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="21"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="20"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5339,10 +5385,10 @@
   </sheetPr>
   <dimension ref="A1:AF171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A135" sqref="A135"/>
+      <selection pane="topRight" activeCell="B128" sqref="B128:B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5386,8 +5432,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5551,8 +5597,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="161"/>
-      <c r="F22" s="161"/>
+      <c r="E22" s="167"/>
+      <c r="F22" s="167"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -7113,7 +7159,7 @@
       <c r="AF38" s="79"/>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A39" s="153" t="s">
+      <c r="A39" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="49" t="s">
@@ -7678,7 +7724,7 @@
       <c r="AE44" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF44" s="152" t="s">
+      <c r="AF44" s="151" t="s">
         <v>288</v>
       </c>
     </row>
@@ -7875,7 +7921,7 @@
       </c>
     </row>
     <row r="47" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="153" t="s">
+      <c r="A47" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="49" t="s">
@@ -8554,7 +8600,7 @@
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A54" s="153" t="s">
+      <c r="A54" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="49" t="s">
@@ -8652,7 +8698,7 @@
       </c>
     </row>
     <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="153" t="s">
+      <c r="A55" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="49" t="s">
@@ -8841,93 +8887,93 @@
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
     </row>
-    <row r="57" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="135" t="s">
+    <row r="57" spans="1:32" s="182" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="168" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="169" t="s">
         <v>449</v>
       </c>
-      <c r="C57" s="136" t="s">
+      <c r="C57" s="170" t="s">
         <v>450</v>
       </c>
-      <c r="D57" s="66">
+      <c r="D57" s="171">
         <v>270</v>
       </c>
-      <c r="E57" s="65">
+      <c r="E57" s="172">
         <v>3</v>
       </c>
-      <c r="F57" s="65">
-        <v>0</v>
-      </c>
-      <c r="G57" s="65">
-        <v>0</v>
-      </c>
-      <c r="H57" s="65">
-        <v>0</v>
-      </c>
-      <c r="I57" s="65">
+      <c r="F57" s="172">
+        <v>0</v>
+      </c>
+      <c r="G57" s="172">
+        <v>0</v>
+      </c>
+      <c r="H57" s="172">
+        <v>0</v>
+      </c>
+      <c r="I57" s="172">
         <v>88</v>
       </c>
-      <c r="J57" s="65">
-        <v>0</v>
-      </c>
-      <c r="K57" s="53">
+      <c r="J57" s="172">
+        <v>0</v>
+      </c>
+      <c r="K57" s="173">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="L57" s="65">
-        <v>0</v>
-      </c>
-      <c r="M57" s="58" t="b">
-        <v>0</v>
-      </c>
-      <c r="N57" s="40">
-        <v>5</v>
-      </c>
-      <c r="O57" s="40">
-        <v>5</v>
-      </c>
-      <c r="P57" s="70">
-        <v>5</v>
-      </c>
-      <c r="Q57" s="40">
+      <c r="L57" s="172">
+        <v>0</v>
+      </c>
+      <c r="M57" s="174" t="b">
+        <v>0</v>
+      </c>
+      <c r="N57" s="175">
+        <v>5</v>
+      </c>
+      <c r="O57" s="175">
+        <v>5</v>
+      </c>
+      <c r="P57" s="176">
+        <v>5</v>
+      </c>
+      <c r="Q57" s="175">
         <v>3</v>
       </c>
-      <c r="R57" s="58" t="b">
-        <v>1</v>
-      </c>
-      <c r="S57" s="73" t="b">
-        <v>0</v>
-      </c>
-      <c r="T57" s="73" t="b">
-        <v>0</v>
-      </c>
-      <c r="U57" s="36">
-        <v>1</v>
-      </c>
-      <c r="V57" s="36">
-        <v>1</v>
-      </c>
-      <c r="W57" s="36">
-        <v>0</v>
-      </c>
-      <c r="X57" s="52">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="52">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="52">
-        <v>0</v>
-      </c>
-      <c r="AA57" s="52">
-        <v>0</v>
-      </c>
-      <c r="AB57" s="143"/>
-      <c r="AC57" s="72"/>
-      <c r="AD57" s="72"/>
-      <c r="AE57" s="72"/>
-      <c r="AF57" s="71"/>
+      <c r="R57" s="174" t="b">
+        <v>1</v>
+      </c>
+      <c r="S57" s="176" t="b">
+        <v>0</v>
+      </c>
+      <c r="T57" s="176" t="b">
+        <v>0</v>
+      </c>
+      <c r="U57" s="177">
+        <v>1</v>
+      </c>
+      <c r="V57" s="177">
+        <v>1</v>
+      </c>
+      <c r="W57" s="177">
+        <v>0</v>
+      </c>
+      <c r="X57" s="178">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="178">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="178">
+        <v>0</v>
+      </c>
+      <c r="AA57" s="178">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="179"/>
+      <c r="AC57" s="180"/>
+      <c r="AD57" s="180"/>
+      <c r="AE57" s="180"/>
+      <c r="AF57" s="181"/>
     </row>
     <row r="58" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="137" t="s">
@@ -9309,7 +9355,7 @@
       <c r="AF61" s="74"/>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A62" s="153" t="s">
+      <c r="A62" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B62" s="49" t="s">
@@ -9404,7 +9450,7 @@
       <c r="AF62" s="74"/>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A63" s="153" t="s">
+      <c r="A63" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B63" s="49" t="s">
@@ -9684,7 +9730,7 @@
         <v>150</v>
       </c>
       <c r="AE65" s="63"/>
-      <c r="AF65" s="150"/>
+      <c r="AF65" s="149"/>
     </row>
     <row r="66" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="137" t="s">
@@ -9984,7 +10030,7 @@
       </c>
     </row>
     <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="153" t="s">
+      <c r="A69" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B69" s="49" t="s">
@@ -10082,7 +10128,7 @@
       </c>
     </row>
     <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="153" t="s">
+      <c r="A70" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B70" s="49" t="s">
@@ -10177,7 +10223,7 @@
       <c r="AF70" s="79"/>
     </row>
     <row r="71" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="153" t="s">
+      <c r="A71" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B71" s="49" t="s">
@@ -10553,7 +10599,7 @@
         <v>58</v>
       </c>
       <c r="AE74" s="63"/>
-      <c r="AF74" s="150"/>
+      <c r="AF74" s="149"/>
     </row>
     <row r="75" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="139" t="s">
@@ -10654,7 +10700,7 @@
       </c>
     </row>
     <row r="76" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="153" t="s">
+      <c r="A76" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B76" s="49" t="s">
@@ -10750,7 +10796,7 @@
       <c r="AF76" s="68"/>
     </row>
     <row r="77" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="153" t="s">
+      <c r="A77" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B77" s="49" t="s">
@@ -11423,7 +11469,7 @@
       <c r="AF83" s="134"/>
     </row>
     <row r="84" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="153" t="s">
+      <c r="A84" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B84" s="49" t="s">
@@ -11718,7 +11764,7 @@
       </c>
     </row>
     <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="153" t="s">
+      <c r="A87" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B87" s="49" t="s">
@@ -11960,7 +12006,7 @@
       <c r="O89" s="32">
         <v>5</v>
       </c>
-      <c r="P89" s="146">
+      <c r="P89" s="145">
         <v>5</v>
       </c>
       <c r="Q89" s="32">
@@ -12008,7 +12054,7 @@
       <c r="AE89" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="AF89" s="148" t="s">
+      <c r="AF89" s="147" t="s">
         <v>179</v>
       </c>
     </row>
@@ -12058,7 +12104,7 @@
       <c r="O90" s="32">
         <v>5</v>
       </c>
-      <c r="P90" s="146">
+      <c r="P90" s="145">
         <v>4</v>
       </c>
       <c r="Q90" s="32">
@@ -12106,7 +12152,7 @@
       <c r="AE90" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="AF90" s="148" t="s">
+      <c r="AF90" s="147" t="s">
         <v>185</v>
       </c>
     </row>
@@ -12156,7 +12202,7 @@
       <c r="O91" s="32">
         <v>5</v>
       </c>
-      <c r="P91" s="146">
+      <c r="P91" s="145">
         <v>5</v>
       </c>
       <c r="Q91" s="32">
@@ -12491,7 +12537,7 @@
       <c r="AF94" s="43"/>
     </row>
     <row r="95" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="153" t="s">
+      <c r="A95" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B95" s="49" t="s">
@@ -12536,14 +12582,14 @@
       <c r="O95" s="32">
         <v>5</v>
       </c>
-      <c r="P95" s="146">
+      <c r="P95" s="145">
         <v>0</v>
       </c>
       <c r="Q95" s="32">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>0</v>
       </c>
-      <c r="R95" s="159" t="b">
+      <c r="R95" s="158" t="b">
         <v>1</v>
       </c>
       <c r="S95" s="28" t="b">
@@ -13115,7 +13161,7 @@
       <c r="O101" s="32">
         <v>5</v>
       </c>
-      <c r="P101" s="146">
+      <c r="P101" s="145">
         <v>0</v>
       </c>
       <c r="Q101" s="32">
@@ -13262,7 +13308,7 @@
       <c r="AF102" s="59"/>
     </row>
     <row r="103" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="153" t="s">
+      <c r="A103" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B103" s="49" t="s">
@@ -13301,13 +13347,13 @@
       <c r="M103" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="N103" s="149">
+      <c r="N103" s="148">
         <v>5</v>
       </c>
       <c r="O103" s="32">
         <v>5</v>
       </c>
-      <c r="P103" s="146">
+      <c r="P103" s="145">
         <v>2</v>
       </c>
       <c r="Q103" s="32">
@@ -13357,7 +13403,7 @@
       <c r="AF103" s="56"/>
     </row>
     <row r="104" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="153" t="s">
+      <c r="A104" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B104" s="49" t="s">
@@ -13544,7 +13590,7 @@
       <c r="AE105" s="25" t="s">
         <v>471</v>
       </c>
-      <c r="AF105" s="151" t="s">
+      <c r="AF105" s="150" t="s">
         <v>288</v>
       </c>
     </row>
@@ -13594,7 +13640,7 @@
       <c r="O106" s="32">
         <v>0</v>
       </c>
-      <c r="P106" s="146">
+      <c r="P106" s="145">
         <v>1</v>
       </c>
       <c r="Q106" s="32">
@@ -13606,7 +13652,7 @@
       <c r="S106" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="T106" s="147" t="b">
+      <c r="T106" s="146" t="b">
         <v>0</v>
       </c>
       <c r="U106" s="36">
@@ -13640,7 +13686,7 @@
         <v>144</v>
       </c>
       <c r="AE106" s="34"/>
-      <c r="AF106" s="148"/>
+      <c r="AF106" s="147"/>
     </row>
     <row r="107" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A107" s="137" t="s">
@@ -13688,7 +13734,7 @@
       <c r="O107" s="32">
         <v>2</v>
       </c>
-      <c r="P107" s="146">
+      <c r="P107" s="145">
         <v>3</v>
       </c>
       <c r="Q107" s="32">
@@ -13700,7 +13746,7 @@
       <c r="S107" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="T107" s="147" t="b">
+      <c r="T107" s="146" t="b">
         <v>0</v>
       </c>
       <c r="U107" s="36">
@@ -13782,7 +13828,7 @@
       <c r="O108" s="32">
         <v>5</v>
       </c>
-      <c r="P108" s="146">
+      <c r="P108" s="145">
         <v>2</v>
       </c>
       <c r="Q108" s="32">
@@ -13829,7 +13875,7 @@
         <v>21</v>
       </c>
       <c r="AE108" s="34"/>
-      <c r="AF108" s="148"/>
+      <c r="AF108" s="147"/>
     </row>
     <row r="109" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A109" s="49" t="s">
@@ -14025,40 +14071,40 @@
       <c r="AF110" s="43"/>
     </row>
     <row r="111" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A111" s="154" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" s="156" t="s">
+      <c r="A111" s="153" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="155" t="s">
         <v>135</v>
       </c>
-      <c r="C111" s="157" t="s">
+      <c r="C111" s="156" t="s">
         <v>87</v>
       </c>
-      <c r="D111" s="158">
+      <c r="D111" s="157">
         <v>120</v>
       </c>
-      <c r="E111" s="158">
+      <c r="E111" s="157">
         <v>17</v>
       </c>
-      <c r="F111" s="158">
-        <v>0</v>
-      </c>
-      <c r="G111" s="158">
+      <c r="F111" s="157">
+        <v>0</v>
+      </c>
+      <c r="G111" s="157">
         <v>50</v>
       </c>
-      <c r="H111" s="158">
-        <v>0</v>
-      </c>
-      <c r="I111" s="158">
+      <c r="H111" s="157">
+        <v>0</v>
+      </c>
+      <c r="I111" s="157">
         <v>70</v>
       </c>
-      <c r="J111" s="158">
+      <c r="J111" s="157">
         <v>0</v>
       </c>
       <c r="K111" s="42">
         <v>0.15</v>
       </c>
-      <c r="L111" s="158">
+      <c r="L111" s="157">
         <v>0</v>
       </c>
       <c r="M111" s="27" t="b">
@@ -14123,40 +14169,40 @@
       </c>
     </row>
     <row r="112" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A112" s="154" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="156" t="s">
+      <c r="A112" s="153" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="155" t="s">
         <v>129</v>
       </c>
-      <c r="C112" s="157" t="s">
+      <c r="C112" s="156" t="s">
         <v>68</v>
       </c>
-      <c r="D112" s="158">
+      <c r="D112" s="157">
         <v>60</v>
       </c>
-      <c r="E112" s="158">
+      <c r="E112" s="157">
         <v>17</v>
       </c>
-      <c r="F112" s="158">
-        <v>0</v>
-      </c>
-      <c r="G112" s="158">
+      <c r="F112" s="157">
+        <v>0</v>
+      </c>
+      <c r="G112" s="157">
         <v>30</v>
       </c>
-      <c r="H112" s="158">
-        <v>0</v>
-      </c>
-      <c r="I112" s="158">
+      <c r="H112" s="157">
+        <v>0</v>
+      </c>
+      <c r="I112" s="157">
         <v>75</v>
       </c>
-      <c r="J112" s="158">
+      <c r="J112" s="157">
         <v>0</v>
       </c>
       <c r="K112" s="42">
         <v>0.15</v>
       </c>
-      <c r="L112" s="158">
+      <c r="L112" s="157">
         <v>0</v>
       </c>
       <c r="M112" s="27" t="b">
@@ -14224,7 +14270,7 @@
       <c r="A113" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B113" s="155" t="s">
+      <c r="B113" s="154" t="s">
         <v>123</v>
       </c>
       <c r="C113" s="141" t="s">
@@ -14323,7 +14369,7 @@
       <c r="A114" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B114" s="155" t="s">
+      <c r="B114" s="154" t="s">
         <v>118</v>
       </c>
       <c r="C114" s="141" t="s">
@@ -14511,7 +14557,7 @@
         <v>109</v>
       </c>
       <c r="AE115" s="34"/>
-      <c r="AF115" s="148"/>
+      <c r="AF115" s="147"/>
     </row>
     <row r="116" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A116" s="137" t="s">
@@ -14606,7 +14652,7 @@
         <v>105</v>
       </c>
       <c r="AE116" s="34"/>
-      <c r="AF116" s="148"/>
+      <c r="AF116" s="147"/>
     </row>
     <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" s="49" t="s">
@@ -14704,7 +14750,7 @@
       <c r="AF117" s="43"/>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A118" s="153" t="s">
+      <c r="A118" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B118" s="49" t="s">
@@ -14799,7 +14845,7 @@
       <c r="AF118" s="74"/>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A119" s="153" t="s">
+      <c r="A119" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B119" s="49" t="s">
@@ -14897,7 +14943,7 @@
       </c>
     </row>
     <row r="120" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A120" s="153" t="s">
+      <c r="A120" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B120" s="49" t="s">
@@ -15347,16 +15393,16 @@
       <c r="W124" s="27">
         <v>0</v>
       </c>
-      <c r="X124" s="160">
+      <c r="X124" s="159">
         <v>0.25</v>
       </c>
-      <c r="Y124" s="160">
+      <c r="Y124" s="159">
         <v>0.25</v>
       </c>
-      <c r="Z124" s="160">
+      <c r="Z124" s="159">
         <v>0.8</v>
       </c>
-      <c r="AA124" s="160">
+      <c r="AA124" s="159">
         <v>0</v>
       </c>
       <c r="AB124" s="35" t="s">
@@ -15372,7 +15418,7 @@
       <c r="AF124" s="24"/>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A125" s="153" t="s">
+      <c r="A125" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B125" s="49" t="s">
@@ -15466,7 +15512,7 @@
       <c r="AF125" s="79"/>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A126" s="153" t="s">
+      <c r="A126" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B126" s="49" t="s">
@@ -15560,7 +15606,7 @@
       <c r="AF126" s="74"/>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A127" s="153" t="s">
+      <c r="A127" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B127" s="49" t="s">
@@ -15614,32 +15660,32 @@
       <c r="R127" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S127" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="T127" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="U127" s="162">
-        <v>1</v>
-      </c>
-      <c r="V127" s="162"/>
-      <c r="W127" s="162">
+      <c r="S127" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="T127" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="U127" s="160">
+        <v>1</v>
+      </c>
+      <c r="V127" s="160"/>
+      <c r="W127" s="160">
         <v>0</v>
       </c>
       <c r="X127" s="55">
         <v>0</v>
       </c>
-      <c r="Y127" s="163">
-        <v>0</v>
-      </c>
-      <c r="Z127" s="163">
+      <c r="Y127" s="161">
+        <v>0</v>
+      </c>
+      <c r="Z127" s="161">
         <v>0</v>
       </c>
       <c r="AA127" s="55">
         <v>0</v>
       </c>
-      <c r="AB127" s="167" t="s">
+      <c r="AB127" s="165" t="s">
         <v>225</v>
       </c>
       <c r="AC127" s="72" t="s">
@@ -15648,11 +15694,11 @@
       <c r="AD127" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE127" s="164"/>
-      <c r="AF127" s="165"/>
+      <c r="AE127" s="162"/>
+      <c r="AF127" s="163"/>
     </row>
     <row r="128" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="153" t="s">
+      <c r="A128" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B128" s="49" t="s">
@@ -15706,32 +15752,32 @@
       <c r="R128" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S128" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="T128" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="U128" s="162">
-        <v>1</v>
-      </c>
-      <c r="V128" s="162"/>
-      <c r="W128" s="162">
+      <c r="S128" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="T128" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="U128" s="160">
+        <v>1</v>
+      </c>
+      <c r="V128" s="160"/>
+      <c r="W128" s="160">
         <v>0</v>
       </c>
       <c r="X128" s="55">
         <v>0</v>
       </c>
-      <c r="Y128" s="163">
-        <v>0</v>
-      </c>
-      <c r="Z128" s="163">
+      <c r="Y128" s="161">
+        <v>0</v>
+      </c>
+      <c r="Z128" s="161">
         <v>0</v>
       </c>
       <c r="AA128" s="55">
         <v>0</v>
       </c>
-      <c r="AB128" s="167" t="s">
+      <c r="AB128" s="165" t="s">
         <v>225</v>
       </c>
       <c r="AC128" s="72" t="s">
@@ -15740,8 +15786,8 @@
       <c r="AD128" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE128" s="164"/>
-      <c r="AF128" s="165"/>
+      <c r="AE128" s="162"/>
+      <c r="AF128" s="163"/>
     </row>
     <row r="129" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A129" s="139" t="s">
@@ -16087,16 +16133,16 @@
       <c r="W132" s="27">
         <v>0</v>
       </c>
-      <c r="X132" s="160">
-        <v>0</v>
-      </c>
-      <c r="Y132" s="160">
-        <v>0</v>
-      </c>
-      <c r="Z132" s="160">
-        <v>0</v>
-      </c>
-      <c r="AA132" s="160">
+      <c r="X132" s="159">
+        <v>0</v>
+      </c>
+      <c r="Y132" s="159">
+        <v>0</v>
+      </c>
+      <c r="Z132" s="159">
+        <v>0</v>
+      </c>
+      <c r="AA132" s="159">
         <v>0</v>
       </c>
       <c r="AB132" s="35" t="s">
@@ -16112,7 +16158,7 @@
       <c r="AF132" s="24"/>
     </row>
     <row r="133" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A133" s="153" t="s">
+      <c r="A133" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B133" s="49" t="s">
@@ -16166,32 +16212,32 @@
       <c r="R133" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S133" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="T133" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="U133" s="162">
-        <v>1</v>
-      </c>
-      <c r="V133" s="162"/>
-      <c r="W133" s="162">
+      <c r="S133" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="T133" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="U133" s="160">
+        <v>1</v>
+      </c>
+      <c r="V133" s="160"/>
+      <c r="W133" s="160">
         <v>0</v>
       </c>
       <c r="X133" s="55">
         <v>0</v>
       </c>
-      <c r="Y133" s="163">
-        <v>0</v>
-      </c>
-      <c r="Z133" s="163">
+      <c r="Y133" s="161">
+        <v>0</v>
+      </c>
+      <c r="Z133" s="161">
         <v>0</v>
       </c>
       <c r="AA133" s="55">
         <v>0</v>
       </c>
-      <c r="AB133" s="167" t="s">
+      <c r="AB133" s="165" t="s">
         <v>225</v>
       </c>
       <c r="AC133" s="72" t="s">
@@ -16200,11 +16246,11 @@
       <c r="AD133" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE133" s="164"/>
-      <c r="AF133" s="165"/>
+      <c r="AE133" s="162"/>
+      <c r="AF133" s="163"/>
     </row>
     <row r="134" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A134" s="153" t="s">
+      <c r="A134" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B134" s="49" t="s">
@@ -16222,7 +16268,7 @@
       <c r="F134" s="76">
         <v>0</v>
       </c>
-      <c r="G134" s="168">
+      <c r="G134" s="166">
         <v>-20</v>
       </c>
       <c r="H134" s="76">
@@ -16259,34 +16305,34 @@
       <c r="R134" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S134" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="T134" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="U134" s="162">
-        <v>1</v>
-      </c>
-      <c r="V134" s="162">
-        <v>2</v>
-      </c>
-      <c r="W134" s="162">
+      <c r="S134" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="T134" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="U134" s="160">
+        <v>1</v>
+      </c>
+      <c r="V134" s="160">
+        <v>2</v>
+      </c>
+      <c r="W134" s="160">
         <v>0</v>
       </c>
       <c r="X134" s="55">
         <v>1</v>
       </c>
-      <c r="Y134" s="163">
-        <v>1</v>
-      </c>
-      <c r="Z134" s="163">
+      <c r="Y134" s="161">
+        <v>1</v>
+      </c>
+      <c r="Z134" s="161">
         <v>0</v>
       </c>
       <c r="AA134" s="55">
         <v>0</v>
       </c>
-      <c r="AB134" s="167" t="s">
+      <c r="AB134" s="165" t="s">
         <v>339</v>
       </c>
       <c r="AC134" s="72" t="s">
@@ -16295,11 +16341,11 @@
       <c r="AD134" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="AE134" s="164"/>
-      <c r="AF134" s="165"/>
+      <c r="AE134" s="162"/>
+      <c r="AF134" s="163"/>
     </row>
     <row r="135" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A135" s="153" t="s">
+      <c r="A135" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B135" s="49" t="s">
@@ -16317,7 +16363,7 @@
       <c r="F135" s="76">
         <v>1</v>
       </c>
-      <c r="G135" s="168">
+      <c r="G135" s="166">
         <v>0</v>
       </c>
       <c r="H135" s="76">
@@ -16353,32 +16399,32 @@
       <c r="R135" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S135" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="T135" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="U135" s="162">
-        <v>1</v>
-      </c>
-      <c r="V135" s="162"/>
-      <c r="W135" s="162">
+      <c r="S135" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="T135" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="U135" s="160">
+        <v>1</v>
+      </c>
+      <c r="V135" s="160"/>
+      <c r="W135" s="160">
         <v>0</v>
       </c>
       <c r="X135" s="55">
         <v>0</v>
       </c>
-      <c r="Y135" s="163">
-        <v>0</v>
-      </c>
-      <c r="Z135" s="163">
+      <c r="Y135" s="161">
+        <v>0</v>
+      </c>
+      <c r="Z135" s="161">
         <v>0</v>
       </c>
       <c r="AA135" s="55">
         <v>0</v>
       </c>
-      <c r="AB135" s="167" t="s">
+      <c r="AB135" s="165" t="s">
         <v>225</v>
       </c>
       <c r="AC135" s="72" t="s">
@@ -16387,11 +16433,11 @@
       <c r="AD135" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE135" s="164"/>
-      <c r="AF135" s="165"/>
+      <c r="AE135" s="162"/>
+      <c r="AF135" s="163"/>
     </row>
     <row r="136" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A136" s="153" t="s">
+      <c r="A136" s="152" t="s">
         <v>2</v>
       </c>
       <c r="B136" s="49" t="s">
@@ -16409,7 +16455,7 @@
       <c r="F136" s="76">
         <v>0</v>
       </c>
-      <c r="G136" s="168">
+      <c r="G136" s="166">
         <v>0</v>
       </c>
       <c r="H136" s="76">
@@ -16445,32 +16491,32 @@
       <c r="R136" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S136" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="T136" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="U136" s="162">
-        <v>1</v>
-      </c>
-      <c r="V136" s="162"/>
-      <c r="W136" s="162">
+      <c r="S136" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="T136" s="164" t="b">
+        <v>0</v>
+      </c>
+      <c r="U136" s="160">
+        <v>1</v>
+      </c>
+      <c r="V136" s="160"/>
+      <c r="W136" s="160">
         <v>0</v>
       </c>
       <c r="X136" s="55">
         <v>0</v>
       </c>
-      <c r="Y136" s="163">
-        <v>0</v>
-      </c>
-      <c r="Z136" s="163">
+      <c r="Y136" s="161">
+        <v>0</v>
+      </c>
+      <c r="Z136" s="161">
         <v>0</v>
       </c>
       <c r="AA136" s="55">
         <v>0</v>
       </c>
-      <c r="AB136" s="167" t="s">
+      <c r="AB136" s="165" t="s">
         <v>225</v>
       </c>
       <c r="AC136" s="72" t="s">
@@ -16479,8 +16525,8 @@
       <c r="AD136" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE136" s="164"/>
-      <c r="AF136" s="165"/>
+      <c r="AE136" s="162"/>
+      <c r="AF136" s="163"/>
     </row>
     <row r="137" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="139" t="s">
@@ -16646,8 +16692,8 @@
       <c r="C141" s="22"/>
       <c r="D141" s="22"/>
       <c r="E141" s="22"/>
-      <c r="F141" s="161"/>
-      <c r="G141" s="161"/>
+      <c r="F141" s="167"/>
+      <c r="G141" s="167"/>
       <c r="H141" s="21" t="s">
         <v>56</v>
       </c>
@@ -17271,22 +17317,22 @@
       <c r="C154" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="D154" s="144" t="s">
+      <c r="D154" s="143" t="s">
         <v>30</v>
       </c>
       <c r="E154" s="14">
         <v>1</v>
       </c>
-      <c r="F154" s="145">
-        <v>0</v>
-      </c>
-      <c r="G154" s="145">
-        <v>0</v>
-      </c>
-      <c r="H154" s="145">
-        <v>0</v>
-      </c>
-      <c r="I154" s="145">
+      <c r="F154" s="144">
+        <v>0</v>
+      </c>
+      <c r="G154" s="144">
+        <v>0</v>
+      </c>
+      <c r="H154" s="144">
+        <v>0</v>
+      </c>
+      <c r="I154" s="144">
         <v>0</v>
       </c>
       <c r="J154" s="12">
@@ -17604,12 +17650,12 @@
     <mergeCell ref="F141:G141"/>
   </mergeCells>
   <conditionalFormatting sqref="M118:M124 R118:T124 M24:M115 R24:T115 S127:T127 M127">
-    <cfRule type="expression" dxfId="18" priority="59">
+    <cfRule type="expression" dxfId="111" priority="59">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="17" priority="52">
+    <cfRule type="expression" dxfId="110" priority="52">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17626,7 +17672,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="16" priority="46">
+    <cfRule type="expression" dxfId="109" priority="46">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17655,7 +17701,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="15" priority="44">
+    <cfRule type="expression" dxfId="108" priority="44">
       <formula>M114=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17672,12 +17718,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="14" priority="41">
+    <cfRule type="expression" dxfId="107" priority="41">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="13" priority="40">
+    <cfRule type="expression" dxfId="106" priority="40">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17706,12 +17752,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="12" priority="38">
+    <cfRule type="expression" dxfId="105" priority="38">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="11" priority="37">
+    <cfRule type="expression" dxfId="104" priority="37">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17728,17 +17774,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="10" priority="35">
+    <cfRule type="expression" dxfId="103" priority="35">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="9" priority="20">
+    <cfRule type="expression" dxfId="102" priority="20">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="8" priority="22">
+    <cfRule type="expression" dxfId="101" priority="22">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17755,12 +17801,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="100" priority="15">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="6" priority="16">
+    <cfRule type="expression" dxfId="99" priority="16">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17789,12 +17835,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="5" priority="13">
+    <cfRule type="expression" dxfId="98" priority="13">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="97" priority="8">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17811,12 +17857,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="96" priority="10">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="95" priority="3">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17833,12 +17879,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="94" priority="5">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="93" priority="1">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17938,8 +17984,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
Just some cells format changed
Former-commit-id: ccfeaa30c1cc1325d4820940d5681b1c77fe68ff
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$142:$O$143</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2077,7 +2077,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2510,58 +2510,23 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="112">
+  <dxfs count="113">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5004,58 +4969,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF137" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF137" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90" totalsRowBorderDxfId="89">
   <autoFilter ref="A23:AF137"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="88"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
+    <tableColumn id="6" name="[category]" dataDxfId="86"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="85"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="84"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="83"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="82"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="81"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="80"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="79"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="78"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="77"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="76"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="75"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="74"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="73"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="72"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="71"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="70"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="69"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="68"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="67"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="66"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="65"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="61"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="60"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="59"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="58"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="52"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5068,50 +5033,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="4" name="[category]" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="16" name="[size]" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="22" totalsRowDxfId="21"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="16"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="6" name="[order]" dataDxfId="14"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="13"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="12"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="11"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="4"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="3"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="2"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="1" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5385,10 +5350,10 @@
   </sheetPr>
   <dimension ref="A1:AF171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="B128" sqref="B128:B137"/>
+      <selection pane="topRight" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5432,8 +5397,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="168"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5597,8 +5562,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="167"/>
-      <c r="F22" s="167"/>
+      <c r="E22" s="168"/>
+      <c r="F22" s="168"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -8887,93 +8852,93 @@
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
     </row>
-    <row r="57" spans="1:32" s="182" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="168" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="169" t="s">
+    <row r="57" spans="1:32" s="167" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="139" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="135" t="s">
         <v>449</v>
       </c>
-      <c r="C57" s="170" t="s">
+      <c r="C57" s="136" t="s">
         <v>450</v>
       </c>
-      <c r="D57" s="171">
+      <c r="D57" s="66">
         <v>270</v>
       </c>
-      <c r="E57" s="172">
+      <c r="E57" s="65">
         <v>3</v>
       </c>
-      <c r="F57" s="172">
-        <v>0</v>
-      </c>
-      <c r="G57" s="172">
-        <v>0</v>
-      </c>
-      <c r="H57" s="172">
-        <v>0</v>
-      </c>
-      <c r="I57" s="172">
+      <c r="F57" s="65">
+        <v>0</v>
+      </c>
+      <c r="G57" s="65">
+        <v>0</v>
+      </c>
+      <c r="H57" s="65">
+        <v>0</v>
+      </c>
+      <c r="I57" s="65">
         <v>88</v>
       </c>
-      <c r="J57" s="172">
-        <v>0</v>
-      </c>
-      <c r="K57" s="173">
+      <c r="J57" s="65">
+        <v>0</v>
+      </c>
+      <c r="K57" s="53">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="L57" s="172">
-        <v>0</v>
-      </c>
-      <c r="M57" s="174" t="b">
-        <v>0</v>
-      </c>
-      <c r="N57" s="175">
-        <v>5</v>
-      </c>
-      <c r="O57" s="175">
-        <v>5</v>
-      </c>
-      <c r="P57" s="176">
-        <v>5</v>
-      </c>
-      <c r="Q57" s="175">
+      <c r="L57" s="65">
+        <v>0</v>
+      </c>
+      <c r="M57" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N57" s="48">
+        <v>5</v>
+      </c>
+      <c r="O57" s="48">
+        <v>5</v>
+      </c>
+      <c r="P57" s="46">
+        <v>5</v>
+      </c>
+      <c r="Q57" s="48">
         <v>3</v>
       </c>
-      <c r="R57" s="174" t="b">
-        <v>1</v>
-      </c>
-      <c r="S57" s="176" t="b">
-        <v>0</v>
-      </c>
-      <c r="T57" s="176" t="b">
-        <v>0</v>
-      </c>
-      <c r="U57" s="177">
-        <v>1</v>
-      </c>
-      <c r="V57" s="177">
-        <v>1</v>
-      </c>
-      <c r="W57" s="177">
-        <v>0</v>
-      </c>
-      <c r="X57" s="178">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="178">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="178">
-        <v>0</v>
-      </c>
-      <c r="AA57" s="178">
-        <v>0</v>
-      </c>
-      <c r="AB57" s="179"/>
-      <c r="AC57" s="180"/>
-      <c r="AD57" s="180"/>
-      <c r="AE57" s="180"/>
-      <c r="AF57" s="181"/>
+      <c r="R57" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S57" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="T57" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="U57" s="36">
+        <v>1</v>
+      </c>
+      <c r="V57" s="36">
+        <v>1</v>
+      </c>
+      <c r="W57" s="36">
+        <v>0</v>
+      </c>
+      <c r="X57" s="52">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="52">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="52">
+        <v>0</v>
+      </c>
+      <c r="AA57" s="52">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="67"/>
+      <c r="AC57" s="63"/>
+      <c r="AD57" s="63"/>
+      <c r="AE57" s="72"/>
+      <c r="AF57" s="71"/>
     </row>
     <row r="58" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="137" t="s">
@@ -16692,8 +16657,8 @@
       <c r="C141" s="22"/>
       <c r="D141" s="22"/>
       <c r="E141" s="22"/>
-      <c r="F141" s="167"/>
-      <c r="G141" s="167"/>
+      <c r="F141" s="168"/>
+      <c r="G141" s="168"/>
       <c r="H141" s="21" t="s">
         <v>56</v>
       </c>
@@ -17649,18 +17614,18 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="F141:G141"/>
   </mergeCells>
-  <conditionalFormatting sqref="M118:M124 R118:T124 M24:M115 R24:T115 S127:T127 M127">
-    <cfRule type="expression" dxfId="111" priority="59">
+  <conditionalFormatting sqref="M118:M124 R118:T124 M24:M56 R24:T56 S127:T127 M127 R58:T115 M58:M115">
+    <cfRule type="expression" dxfId="112" priority="61">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="110" priority="52">
+    <cfRule type="expression" dxfId="111" priority="54">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116:Q116">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17672,11 +17637,40 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="109" priority="46">
+    <cfRule type="expression" dxfId="110" priority="48">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N115:Q119">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N118:Q124 N24:Q56 N58:Q115">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M114 R114:T114">
+    <cfRule type="expression" dxfId="109" priority="46">
+      <formula>M114=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N114:Q114">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -17688,47 +17682,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N118:Q124 N24:Q115">
-    <cfRule type="colorScale" priority="64">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="108" priority="44">
-      <formula>M114=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N114:Q114">
-    <cfRule type="colorScale" priority="43">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="107" priority="41">
+    <cfRule type="expression" dxfId="108" priority="43">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="106" priority="40">
+    <cfRule type="expression" dxfId="107" priority="42">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q125">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17740,7 +17705,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q127">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17752,17 +17717,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="105" priority="38">
+    <cfRule type="expression" dxfId="106" priority="40">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="104" priority="37">
+    <cfRule type="expression" dxfId="105" priority="39">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:Q128">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17774,22 +17739,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="103" priority="35">
+    <cfRule type="expression" dxfId="104" priority="37">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="102" priority="20">
+    <cfRule type="expression" dxfId="103" priority="22">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="101" priority="22">
+    <cfRule type="expression" dxfId="102" priority="24">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N133:Q133">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17801,17 +17766,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="100" priority="15">
+    <cfRule type="expression" dxfId="101" priority="17">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="99" priority="16">
+    <cfRule type="expression" dxfId="100" priority="18">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N129:Q132">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17823,7 +17788,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:Q134">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17835,17 +17800,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="98" priority="13">
+    <cfRule type="expression" dxfId="99" priority="15">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="97" priority="8">
+    <cfRule type="expression" dxfId="98" priority="10">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N135:Q135">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17857,16 +17822,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="96" priority="10">
+    <cfRule type="expression" dxfId="97" priority="12">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="95" priority="3">
+    <cfRule type="expression" dxfId="96" priority="5">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N136:Q136">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S136:T136 M136">
+    <cfRule type="expression" dxfId="95" priority="7">
+      <formula>M136=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M137 R137:T137">
+    <cfRule type="expression" dxfId="94" priority="3">
+      <formula>M137=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N137:Q137">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -17878,17 +17865,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="94" priority="5">
-      <formula>M136=FALSE</formula>
+  <conditionalFormatting sqref="M57 R57:T57">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="93" priority="1">
-      <formula>M137=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N137:Q137">
+  <conditionalFormatting sqref="N57:Q57">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -17984,8 +17966,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
Minor fixes in texts also in tids related to entities
Former-commit-id: 4618876f0068ff4015ac2e8aa020f0de07211cc8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="502">
   <si>
     <t>tier_4</t>
   </si>
@@ -1532,6 +1532,21 @@
   </si>
   <si>
     <t>Star</t>
+  </si>
+  <si>
+    <r>
+      <t>TID_QUIP_ENT_DMG_DRG_MINEBIG_01;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TID_QUIP_ENT_DMG_DRG_01</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2077,7 +2092,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2458,9 +2473,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2514,19 +2526,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="113">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4955,6 +4969,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4969,58 +4990,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF137" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90" totalsRowBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF137" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF137"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="88"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="87"/>
-    <tableColumn id="6" name="[category]" dataDxfId="86"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="85"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="84"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="83"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="82"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="81"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="80"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="79"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="78"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="77"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="76"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="75"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="74"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="73"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="72"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="71"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="70"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="69"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="68"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="67"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="66"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="65"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="61"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="60"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="59"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="58"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="57"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="52"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5033,50 +5054,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="4" name="[category]" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="16" name="[size]" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="16"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="6" name="[order]" dataDxfId="14"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="13"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="12"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="11"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="10"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="4"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="3"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="2"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5350,15 +5371,15 @@
   </sheetPr>
   <dimension ref="A1:AF171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AB1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A61" sqref="A61"/>
+      <selection pane="topRight" activeCell="AB75" sqref="AB75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="28" max="28" width="162.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5397,8 +5418,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5562,8 +5583,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="168"/>
-      <c r="F22" s="168"/>
+      <c r="E22" s="167"/>
+      <c r="F22" s="167"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -7124,7 +7145,7 @@
       <c r="AF38" s="79"/>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A39" s="152" t="s">
+      <c r="A39" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="49" t="s">
@@ -7689,7 +7710,7 @@
       <c r="AE44" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF44" s="151" t="s">
+      <c r="AF44" s="150" t="s">
         <v>288</v>
       </c>
     </row>
@@ -7886,7 +7907,7 @@
       </c>
     </row>
     <row r="47" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="152" t="s">
+      <c r="A47" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="49" t="s">
@@ -8565,7 +8586,7 @@
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A54" s="152" t="s">
+      <c r="A54" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="49" t="s">
@@ -8663,7 +8684,7 @@
       </c>
     </row>
     <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="152" t="s">
+      <c r="A55" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="49" t="s">
@@ -8852,7 +8873,7 @@
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
     </row>
-    <row r="57" spans="1:32" s="167" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" s="166" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="139" t="s">
         <v>2</v>
       </c>
@@ -9320,7 +9341,7 @@
       <c r="AF61" s="74"/>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A62" s="152" t="s">
+      <c r="A62" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B62" s="49" t="s">
@@ -9415,7 +9436,7 @@
       <c r="AF62" s="74"/>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A63" s="152" t="s">
+      <c r="A63" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B63" s="49" t="s">
@@ -9995,7 +10016,7 @@
       </c>
     </row>
     <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="152" t="s">
+      <c r="A69" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B69" s="49" t="s">
@@ -10093,7 +10114,7 @@
       </c>
     </row>
     <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="152" t="s">
+      <c r="A70" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B70" s="49" t="s">
@@ -10188,7 +10209,7 @@
       <c r="AF70" s="79"/>
     </row>
     <row r="71" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="152" t="s">
+      <c r="A71" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B71" s="49" t="s">
@@ -10373,10 +10394,10 @@
       <c r="AD72" s="63" t="s">
         <v>228</v>
       </c>
-      <c r="AE72" s="72" t="s">
+      <c r="AE72" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="AF72" s="80" t="s">
+      <c r="AF72" s="149" t="s">
         <v>227</v>
       </c>
     </row>
@@ -10665,7 +10686,7 @@
       </c>
     </row>
     <row r="76" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="152" t="s">
+      <c r="A76" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B76" s="49" t="s">
@@ -10761,7 +10782,7 @@
       <c r="AF76" s="68"/>
     </row>
     <row r="77" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="152" t="s">
+      <c r="A77" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B77" s="49" t="s">
@@ -10851,10 +10872,10 @@
       <c r="AD77" s="68" t="s">
         <v>215</v>
       </c>
-      <c r="AE77" s="75" t="s">
+      <c r="AE77" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF77" s="79" t="s">
+      <c r="AF77" s="170" t="s">
         <v>214</v>
       </c>
     </row>
@@ -10950,10 +10971,10 @@
       <c r="AD78" s="68" t="s">
         <v>209</v>
       </c>
-      <c r="AE78" s="75" t="s">
+      <c r="AE78" s="68" t="s">
         <v>208</v>
       </c>
-      <c r="AF78" s="79" t="s">
+      <c r="AF78" s="170" t="s">
         <v>207</v>
       </c>
     </row>
@@ -11434,7 +11455,7 @@
       <c r="AF83" s="134"/>
     </row>
     <row r="84" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="152" t="s">
+      <c r="A84" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B84" s="49" t="s">
@@ -11729,7 +11750,7 @@
       </c>
     </row>
     <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="152" t="s">
+      <c r="A87" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B87" s="49" t="s">
@@ -12212,10 +12233,10 @@
       <c r="AD91" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="AE91" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF91" s="24" t="s">
+      <c r="AE91" s="34" t="s">
+        <v>501</v>
+      </c>
+      <c r="AF91" s="147" t="s">
         <v>179</v>
       </c>
     </row>
@@ -12502,7 +12523,7 @@
       <c r="AF94" s="43"/>
     </row>
     <row r="95" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="152" t="s">
+      <c r="A95" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B95" s="49" t="s">
@@ -12554,7 +12575,7 @@
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>0</v>
       </c>
-      <c r="R95" s="158" t="b">
+      <c r="R95" s="157" t="b">
         <v>1</v>
       </c>
       <c r="S95" s="28" t="b">
@@ -12687,10 +12708,10 @@
       <c r="AD96" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="AE96" s="25" t="s">
+      <c r="AE96" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="AF96" s="24" t="s">
+      <c r="AF96" s="147" t="s">
         <v>148</v>
       </c>
     </row>
@@ -12785,10 +12806,10 @@
       <c r="AD97" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="AE97" s="25" t="s">
+      <c r="AE97" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="AF97" s="24" t="s">
+      <c r="AF97" s="147" t="s">
         <v>148</v>
       </c>
     </row>
@@ -13073,10 +13094,10 @@
       <c r="AD100" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="AE100" s="26" t="s">
+      <c r="AE100" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="AF100" s="59" t="s">
+      <c r="AF100" s="56" t="s">
         <v>136</v>
       </c>
     </row>
@@ -13171,12 +13192,8 @@
       <c r="AD101" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="AE101" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="AF101" s="59" t="s">
-        <v>136</v>
-      </c>
+      <c r="AE101" s="26"/>
+      <c r="AF101" s="59"/>
     </row>
     <row r="102" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="49" t="s">
@@ -13273,7 +13290,7 @@
       <c r="AF102" s="59"/>
     </row>
     <row r="103" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="152" t="s">
+      <c r="A103" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B103" s="49" t="s">
@@ -13368,7 +13385,7 @@
       <c r="AF103" s="56"/>
     </row>
     <row r="104" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="152" t="s">
+      <c r="A104" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B104" s="49" t="s">
@@ -13552,10 +13569,10 @@
       <c r="AD105" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="AE105" s="25" t="s">
+      <c r="AE105" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="AF105" s="150" t="s">
+      <c r="AF105" s="142" t="s">
         <v>288</v>
       </c>
     </row>
@@ -14036,40 +14053,40 @@
       <c r="AF110" s="43"/>
     </row>
     <row r="111" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A111" s="153" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" s="155" t="s">
+      <c r="A111" s="152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="154" t="s">
         <v>135</v>
       </c>
-      <c r="C111" s="156" t="s">
+      <c r="C111" s="155" t="s">
         <v>87</v>
       </c>
-      <c r="D111" s="157">
+      <c r="D111" s="156">
         <v>120</v>
       </c>
-      <c r="E111" s="157">
+      <c r="E111" s="156">
         <v>17</v>
       </c>
-      <c r="F111" s="157">
-        <v>0</v>
-      </c>
-      <c r="G111" s="157">
+      <c r="F111" s="156">
+        <v>0</v>
+      </c>
+      <c r="G111" s="156">
         <v>50</v>
       </c>
-      <c r="H111" s="157">
-        <v>0</v>
-      </c>
-      <c r="I111" s="157">
+      <c r="H111" s="156">
+        <v>0</v>
+      </c>
+      <c r="I111" s="156">
         <v>70</v>
       </c>
-      <c r="J111" s="157">
+      <c r="J111" s="156">
         <v>0</v>
       </c>
       <c r="K111" s="42">
         <v>0.15</v>
       </c>
-      <c r="L111" s="157">
+      <c r="L111" s="156">
         <v>0</v>
       </c>
       <c r="M111" s="27" t="b">
@@ -14134,40 +14151,40 @@
       </c>
     </row>
     <row r="112" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A112" s="153" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="155" t="s">
+      <c r="A112" s="152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="154" t="s">
         <v>129</v>
       </c>
-      <c r="C112" s="156" t="s">
+      <c r="C112" s="155" t="s">
         <v>68</v>
       </c>
-      <c r="D112" s="157">
+      <c r="D112" s="156">
         <v>60</v>
       </c>
-      <c r="E112" s="157">
+      <c r="E112" s="156">
         <v>17</v>
       </c>
-      <c r="F112" s="157">
-        <v>0</v>
-      </c>
-      <c r="G112" s="157">
+      <c r="F112" s="156">
+        <v>0</v>
+      </c>
+      <c r="G112" s="156">
         <v>30</v>
       </c>
-      <c r="H112" s="157">
-        <v>0</v>
-      </c>
-      <c r="I112" s="157">
+      <c r="H112" s="156">
+        <v>0</v>
+      </c>
+      <c r="I112" s="156">
         <v>75</v>
       </c>
-      <c r="J112" s="157">
+      <c r="J112" s="156">
         <v>0</v>
       </c>
       <c r="K112" s="42">
         <v>0.15</v>
       </c>
-      <c r="L112" s="157">
+      <c r="L112" s="156">
         <v>0</v>
       </c>
       <c r="M112" s="27" t="b">
@@ -14235,7 +14252,7 @@
       <c r="A113" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B113" s="154" t="s">
+      <c r="B113" s="153" t="s">
         <v>123</v>
       </c>
       <c r="C113" s="141" t="s">
@@ -14323,10 +14340,10 @@
       <c r="AD113" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="AE113" s="25" t="s">
+      <c r="AE113" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="AF113" s="24" t="s">
+      <c r="AF113" s="147" t="s">
         <v>119</v>
       </c>
     </row>
@@ -14334,7 +14351,7 @@
       <c r="A114" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B114" s="154" t="s">
+      <c r="B114" s="153" t="s">
         <v>118</v>
       </c>
       <c r="C114" s="141" t="s">
@@ -14422,10 +14439,10 @@
       <c r="AD114" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="AE114" s="25" t="s">
+      <c r="AE114" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="AF114" s="24" t="s">
+      <c r="AF114" s="147" t="s">
         <v>113</v>
       </c>
     </row>
@@ -14715,7 +14732,7 @@
       <c r="AF117" s="43"/>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A118" s="152" t="s">
+      <c r="A118" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B118" s="49" t="s">
@@ -14810,7 +14827,7 @@
       <c r="AF118" s="74"/>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A119" s="152" t="s">
+      <c r="A119" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B119" s="49" t="s">
@@ -14900,15 +14917,15 @@
       <c r="AD119" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="AE119" s="75" t="s">
+      <c r="AE119" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="AF119" s="79" t="s">
+      <c r="AF119" s="170" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="120" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A120" s="152" t="s">
+      <c r="A120" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B120" s="49" t="s">
@@ -15281,10 +15298,10 @@
       <c r="AD123" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="AE123" s="72" t="s">
+      <c r="AE123" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="AF123" s="71" t="s">
+      <c r="AF123" s="134" t="s">
         <v>74</v>
       </c>
     </row>
@@ -15358,16 +15375,16 @@
       <c r="W124" s="27">
         <v>0</v>
       </c>
-      <c r="X124" s="159">
+      <c r="X124" s="158">
         <v>0.25</v>
       </c>
-      <c r="Y124" s="159">
+      <c r="Y124" s="158">
         <v>0.25</v>
       </c>
-      <c r="Z124" s="159">
+      <c r="Z124" s="158">
         <v>0.8</v>
       </c>
-      <c r="AA124" s="159">
+      <c r="AA124" s="158">
         <v>0</v>
       </c>
       <c r="AB124" s="35" t="s">
@@ -15383,7 +15400,7 @@
       <c r="AF124" s="24"/>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A125" s="152" t="s">
+      <c r="A125" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B125" s="49" t="s">
@@ -15477,7 +15494,7 @@
       <c r="AF125" s="79"/>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A126" s="152" t="s">
+      <c r="A126" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B126" s="49" t="s">
@@ -15571,7 +15588,7 @@
       <c r="AF126" s="74"/>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A127" s="152" t="s">
+      <c r="A127" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B127" s="49" t="s">
@@ -15625,32 +15642,32 @@
       <c r="R127" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S127" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="T127" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="U127" s="160">
-        <v>1</v>
-      </c>
-      <c r="V127" s="160"/>
-      <c r="W127" s="160">
+      <c r="S127" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="T127" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="U127" s="159">
+        <v>1</v>
+      </c>
+      <c r="V127" s="159"/>
+      <c r="W127" s="159">
         <v>0</v>
       </c>
       <c r="X127" s="55">
         <v>0</v>
       </c>
-      <c r="Y127" s="161">
-        <v>0</v>
-      </c>
-      <c r="Z127" s="161">
+      <c r="Y127" s="160">
+        <v>0</v>
+      </c>
+      <c r="Z127" s="160">
         <v>0</v>
       </c>
       <c r="AA127" s="55">
         <v>0</v>
       </c>
-      <c r="AB127" s="165" t="s">
+      <c r="AB127" s="164" t="s">
         <v>225</v>
       </c>
       <c r="AC127" s="72" t="s">
@@ -15659,11 +15676,11 @@
       <c r="AD127" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE127" s="162"/>
-      <c r="AF127" s="163"/>
+      <c r="AE127" s="161"/>
+      <c r="AF127" s="162"/>
     </row>
     <row r="128" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="152" t="s">
+      <c r="A128" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B128" s="49" t="s">
@@ -15717,32 +15734,32 @@
       <c r="R128" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S128" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="T128" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="U128" s="160">
-        <v>1</v>
-      </c>
-      <c r="V128" s="160"/>
-      <c r="W128" s="160">
+      <c r="S128" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="T128" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="U128" s="159">
+        <v>1</v>
+      </c>
+      <c r="V128" s="159"/>
+      <c r="W128" s="159">
         <v>0</v>
       </c>
       <c r="X128" s="55">
         <v>0</v>
       </c>
-      <c r="Y128" s="161">
-        <v>0</v>
-      </c>
-      <c r="Z128" s="161">
+      <c r="Y128" s="160">
+        <v>0</v>
+      </c>
+      <c r="Z128" s="160">
         <v>0</v>
       </c>
       <c r="AA128" s="55">
         <v>0</v>
       </c>
-      <c r="AB128" s="165" t="s">
+      <c r="AB128" s="164" t="s">
         <v>225</v>
       </c>
       <c r="AC128" s="72" t="s">
@@ -15751,8 +15768,8 @@
       <c r="AD128" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE128" s="162"/>
-      <c r="AF128" s="163"/>
+      <c r="AE128" s="161"/>
+      <c r="AF128" s="162"/>
     </row>
     <row r="129" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A129" s="139" t="s">
@@ -15834,13 +15851,13 @@
       <c r="AA129" s="52">
         <v>0</v>
       </c>
-      <c r="AB129" s="67" t="s">
+      <c r="AB129" s="168" t="s">
         <v>225</v>
       </c>
-      <c r="AC129" s="63" t="s">
+      <c r="AC129" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="AD129" s="63" t="s">
+      <c r="AD129" s="72" t="s">
         <v>58</v>
       </c>
       <c r="AE129" s="63"/>
@@ -15926,13 +15943,13 @@
       <c r="AA130" s="52">
         <v>0</v>
       </c>
-      <c r="AB130" s="64" t="s">
+      <c r="AB130" s="168" t="s">
         <v>225</v>
       </c>
-      <c r="AC130" s="63" t="s">
+      <c r="AC130" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="AD130" s="63" t="s">
+      <c r="AD130" s="72" t="s">
         <v>58</v>
       </c>
       <c r="AE130" s="72"/>
@@ -16018,13 +16035,13 @@
       <c r="AA131" s="52">
         <v>0</v>
       </c>
-      <c r="AB131" s="64" t="s">
+      <c r="AB131" s="168" t="s">
         <v>225</v>
       </c>
-      <c r="AC131" s="63" t="s">
+      <c r="AC131" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="AD131" s="63" t="s">
+      <c r="AD131" s="72" t="s">
         <v>58</v>
       </c>
       <c r="AE131" s="72"/>
@@ -16098,32 +16115,32 @@
       <c r="W132" s="27">
         <v>0</v>
       </c>
-      <c r="X132" s="159">
-        <v>0</v>
-      </c>
-      <c r="Y132" s="159">
-        <v>0</v>
-      </c>
-      <c r="Z132" s="159">
-        <v>0</v>
-      </c>
-      <c r="AA132" s="159">
-        <v>0</v>
-      </c>
-      <c r="AB132" s="35" t="s">
+      <c r="X132" s="158">
+        <v>0</v>
+      </c>
+      <c r="Y132" s="158">
+        <v>0</v>
+      </c>
+      <c r="Z132" s="158">
+        <v>0</v>
+      </c>
+      <c r="AA132" s="158">
+        <v>0</v>
+      </c>
+      <c r="AB132" s="169" t="s">
         <v>225</v>
       </c>
-      <c r="AC132" s="34" t="s">
+      <c r="AC132" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="AD132" s="34" t="s">
+      <c r="AD132" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AE132" s="25"/>
       <c r="AF132" s="24"/>
     </row>
     <row r="133" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A133" s="152" t="s">
+      <c r="A133" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B133" s="49" t="s">
@@ -16177,32 +16194,32 @@
       <c r="R133" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S133" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="T133" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="U133" s="160">
-        <v>1</v>
-      </c>
-      <c r="V133" s="160"/>
-      <c r="W133" s="160">
+      <c r="S133" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="T133" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="U133" s="159">
+        <v>1</v>
+      </c>
+      <c r="V133" s="159"/>
+      <c r="W133" s="159">
         <v>0</v>
       </c>
       <c r="X133" s="55">
         <v>0</v>
       </c>
-      <c r="Y133" s="161">
-        <v>0</v>
-      </c>
-      <c r="Z133" s="161">
+      <c r="Y133" s="160">
+        <v>0</v>
+      </c>
+      <c r="Z133" s="160">
         <v>0</v>
       </c>
       <c r="AA133" s="55">
         <v>0</v>
       </c>
-      <c r="AB133" s="165" t="s">
+      <c r="AB133" s="164" t="s">
         <v>225</v>
       </c>
       <c r="AC133" s="72" t="s">
@@ -16211,11 +16228,11 @@
       <c r="AD133" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE133" s="162"/>
-      <c r="AF133" s="163"/>
+      <c r="AE133" s="161"/>
+      <c r="AF133" s="162"/>
     </row>
     <row r="134" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A134" s="152" t="s">
+      <c r="A134" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B134" s="49" t="s">
@@ -16233,7 +16250,7 @@
       <c r="F134" s="76">
         <v>0</v>
       </c>
-      <c r="G134" s="166">
+      <c r="G134" s="165">
         <v>-20</v>
       </c>
       <c r="H134" s="76">
@@ -16270,34 +16287,34 @@
       <c r="R134" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S134" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="T134" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="U134" s="160">
-        <v>1</v>
-      </c>
-      <c r="V134" s="160">
-        <v>2</v>
-      </c>
-      <c r="W134" s="160">
+      <c r="S134" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="T134" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="U134" s="159">
+        <v>1</v>
+      </c>
+      <c r="V134" s="159">
+        <v>2</v>
+      </c>
+      <c r="W134" s="159">
         <v>0</v>
       </c>
       <c r="X134" s="55">
         <v>1</v>
       </c>
-      <c r="Y134" s="161">
-        <v>1</v>
-      </c>
-      <c r="Z134" s="161">
+      <c r="Y134" s="160">
+        <v>1</v>
+      </c>
+      <c r="Z134" s="160">
         <v>0</v>
       </c>
       <c r="AA134" s="55">
         <v>0</v>
       </c>
-      <c r="AB134" s="165" t="s">
+      <c r="AB134" s="164" t="s">
         <v>339</v>
       </c>
       <c r="AC134" s="72" t="s">
@@ -16306,11 +16323,11 @@
       <c r="AD134" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="AE134" s="162"/>
-      <c r="AF134" s="163"/>
+      <c r="AE134" s="161"/>
+      <c r="AF134" s="162"/>
     </row>
     <row r="135" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A135" s="152" t="s">
+      <c r="A135" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B135" s="49" t="s">
@@ -16328,7 +16345,7 @@
       <c r="F135" s="76">
         <v>1</v>
       </c>
-      <c r="G135" s="166">
+      <c r="G135" s="165">
         <v>0</v>
       </c>
       <c r="H135" s="76">
@@ -16364,32 +16381,32 @@
       <c r="R135" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S135" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="T135" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="U135" s="160">
-        <v>1</v>
-      </c>
-      <c r="V135" s="160"/>
-      <c r="W135" s="160">
+      <c r="S135" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="T135" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="U135" s="159">
+        <v>1</v>
+      </c>
+      <c r="V135" s="159"/>
+      <c r="W135" s="159">
         <v>0</v>
       </c>
       <c r="X135" s="55">
         <v>0</v>
       </c>
-      <c r="Y135" s="161">
-        <v>0</v>
-      </c>
-      <c r="Z135" s="161">
+      <c r="Y135" s="160">
+        <v>0</v>
+      </c>
+      <c r="Z135" s="160">
         <v>0</v>
       </c>
       <c r="AA135" s="55">
         <v>0</v>
       </c>
-      <c r="AB135" s="165" t="s">
+      <c r="AB135" s="164" t="s">
         <v>225</v>
       </c>
       <c r="AC135" s="72" t="s">
@@ -16398,11 +16415,11 @@
       <c r="AD135" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE135" s="162"/>
-      <c r="AF135" s="163"/>
+      <c r="AE135" s="161"/>
+      <c r="AF135" s="162"/>
     </row>
     <row r="136" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A136" s="152" t="s">
+      <c r="A136" s="151" t="s">
         <v>2</v>
       </c>
       <c r="B136" s="49" t="s">
@@ -16420,7 +16437,7 @@
       <c r="F136" s="76">
         <v>0</v>
       </c>
-      <c r="G136" s="166">
+      <c r="G136" s="165">
         <v>0</v>
       </c>
       <c r="H136" s="76">
@@ -16456,32 +16473,32 @@
       <c r="R136" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S136" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="T136" s="164" t="b">
-        <v>0</v>
-      </c>
-      <c r="U136" s="160">
-        <v>1</v>
-      </c>
-      <c r="V136" s="160"/>
-      <c r="W136" s="160">
+      <c r="S136" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="T136" s="163" t="b">
+        <v>0</v>
+      </c>
+      <c r="U136" s="159">
+        <v>1</v>
+      </c>
+      <c r="V136" s="159"/>
+      <c r="W136" s="159">
         <v>0</v>
       </c>
       <c r="X136" s="55">
         <v>0</v>
       </c>
-      <c r="Y136" s="161">
-        <v>0</v>
-      </c>
-      <c r="Z136" s="161">
+      <c r="Y136" s="160">
+        <v>0</v>
+      </c>
+      <c r="Z136" s="160">
         <v>0</v>
       </c>
       <c r="AA136" s="55">
         <v>0</v>
       </c>
-      <c r="AB136" s="165" t="s">
+      <c r="AB136" s="164" t="s">
         <v>225</v>
       </c>
       <c r="AC136" s="72" t="s">
@@ -16490,8 +16507,8 @@
       <c r="AD136" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE136" s="162"/>
-      <c r="AF136" s="163"/>
+      <c r="AE136" s="161"/>
+      <c r="AF136" s="162"/>
     </row>
     <row r="137" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="139" t="s">
@@ -16573,13 +16590,13 @@
       <c r="AA137" s="52">
         <v>0</v>
       </c>
-      <c r="AB137" s="64" t="s">
+      <c r="AB137" s="168" t="s">
         <v>225</v>
       </c>
-      <c r="AC137" s="63" t="s">
+      <c r="AC137" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="AD137" s="63" t="s">
+      <c r="AD137" s="72" t="s">
         <v>58</v>
       </c>
       <c r="AE137" s="72"/>
@@ -16657,8 +16674,8 @@
       <c r="C141" s="22"/>
       <c r="D141" s="22"/>
       <c r="E141" s="22"/>
-      <c r="F141" s="168"/>
-      <c r="G141" s="168"/>
+      <c r="F141" s="167"/>
+      <c r="G141" s="167"/>
       <c r="H141" s="21" t="s">
         <v>56</v>
       </c>
@@ -17866,7 +17883,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="93" priority="1">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17966,8 +17983,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
OwlWhite has his own sku
Former-commit-id: 6dae12cc2dc203dd5db257de2ca5d8c19d73a7c8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -549,9 +549,6 @@
     <t>TID_EDIBLE_OWL_SMALL</t>
   </si>
   <si>
-    <t>OwlSmall</t>
-  </si>
-  <si>
     <t>TID_EDIBLE_OWL_LARGE</t>
   </si>
   <si>
@@ -1547,6 +1544,9 @@
       </rPr>
       <t>TID_QUIP_ENT_DMG_DRG_01</t>
     </r>
+  </si>
+  <si>
+    <t>OwlWhite</t>
   </si>
 </sst>
 </file>
@@ -2523,9 +2523,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2534,6 +2531,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5371,10 +5371,10 @@
   </sheetPr>
   <dimension ref="A1:AF171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="AB75" sqref="AB75"/>
+      <selection pane="topRight" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5385,7 +5385,7 @@
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -5413,20 +5413,20 @@
     </row>
     <row r="3" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="98" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
     </row>
     <row r="4" spans="1:24" ht="134.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
@@ -5469,7 +5469,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="95" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -5493,7 +5493,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="95" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -5501,7 +5501,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="95" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -5533,7 +5533,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
@@ -5541,13 +5541,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -5579,17 +5579,17 @@
     <row r="22" spans="1:32" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="167"/>
-      <c r="F22" s="167"/>
+      <c r="E22" s="170"/>
+      <c r="F22" s="170"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
       <c r="N22" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="Q22" s="17" t="s">
         <v>56</v>
@@ -5603,7 +5603,7 @@
     </row>
     <row r="23" spans="1:32" ht="126" x14ac:dyDescent="0.25">
       <c r="A23" s="93" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B23" s="92" t="s">
         <v>17</v>
@@ -5615,88 +5615,88 @@
         <v>44</v>
       </c>
       <c r="E23" s="89" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F23" s="89" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G23" s="89" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H23" s="89" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I23" s="89" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J23" s="89" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K23" s="89" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L23" s="89" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M23" s="88" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N23" s="88" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="O23" s="88" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P23" s="88" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q23" s="88" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R23" s="88" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S23" s="88" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="T23" s="88" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U23" s="88" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="V23" s="88" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="W23" s="88" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="X23" s="87" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Y23" s="87" t="s">
         <v>48</v>
       </c>
       <c r="Z23" s="87" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AA23" s="86" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AB23" s="85" t="s">
         <v>43</v>
       </c>
       <c r="AC23" s="84" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AD23" s="83" t="s">
         <v>42</v>
       </c>
       <c r="AE23" s="83" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AF23" s="82" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
@@ -5704,7 +5704,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="135" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C24" s="136" t="s">
         <v>87</v>
@@ -5782,19 +5782,19 @@
         <v>0</v>
       </c>
       <c r="AB24" s="67" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AC24" s="63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AD24" s="63" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AE24" s="63" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AF24" s="63" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
@@ -5802,13 +5802,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="135" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C25" s="136" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="66">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E25" s="65">
         <v>3</v>
@@ -5817,13 +5817,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="65">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H25" s="65">
         <v>0</v>
       </c>
       <c r="I25" s="65">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J25" s="65">
         <v>0</v>
@@ -5880,19 +5880,19 @@
         <v>0</v>
       </c>
       <c r="AB25" s="67" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AC25" s="63" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AD25" s="63" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AE25" s="63" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AF25" s="63" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
@@ -5900,7 +5900,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="135" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C26" s="136" t="s">
         <v>87</v>
@@ -5978,10 +5978,10 @@
         <v>0</v>
       </c>
       <c r="AB26" s="64" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AC26" s="63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AD26" s="63" t="s">
         <v>150</v>
@@ -5998,7 +5998,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="135" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C27" s="136" t="s">
         <v>82</v>
@@ -6077,10 +6077,10 @@
         <v>0</v>
       </c>
       <c r="AB27" s="64" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AC27" s="63" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AD27" s="63" t="s">
         <v>137</v>
@@ -6093,7 +6093,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C28" s="77" t="s">
         <v>66</v>
@@ -6191,7 +6191,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C29" s="77" t="s">
         <v>87</v>
@@ -6269,19 +6269,19 @@
         <v>0</v>
       </c>
       <c r="AB29" s="69" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AC29" s="68" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AD29" s="68" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE29" s="68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AF29" s="78" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -6289,7 +6289,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C30" s="77" t="s">
         <v>82</v>
@@ -6367,19 +6367,19 @@
         <v>0</v>
       </c>
       <c r="AB30" s="60" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AC30" s="68" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AD30" s="68" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AE30" s="68" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AF30" s="78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -6387,7 +6387,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C31" s="77" t="s">
         <v>82</v>
@@ -6466,13 +6466,13 @@
         <v>0</v>
       </c>
       <c r="AB31" s="60" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AC31" s="68" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AD31" s="68" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AE31" s="75"/>
       <c r="AF31" s="79"/>
@@ -6482,7 +6482,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="135" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C32" s="136" t="s">
         <v>87</v>
@@ -6576,7 +6576,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="135" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C33" s="136" t="s">
         <v>68</v>
@@ -6655,19 +6655,19 @@
         <v>0</v>
       </c>
       <c r="AB33" s="64" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AC33" s="63" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AD33" s="63" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AE33" s="63" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AF33" s="62" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -6675,7 +6675,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="137" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C34" s="138" t="s">
         <v>82</v>
@@ -6753,7 +6753,7 @@
         <v>0</v>
       </c>
       <c r="AB34" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AC34" s="63" t="s">
         <v>140</v>
@@ -6769,7 +6769,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="137" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C35" s="138" t="s">
         <v>82</v>
@@ -6848,10 +6848,10 @@
         <v>0</v>
       </c>
       <c r="AB35" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AC35" s="63" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AD35" s="63" t="s">
         <v>162</v>
@@ -6864,7 +6864,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C36" s="77" t="s">
         <v>82</v>
@@ -6943,13 +6943,13 @@
         <v>0</v>
       </c>
       <c r="AB36" s="60" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AC36" s="68" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AD36" s="68" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AE36" s="75"/>
       <c r="AF36" s="74"/>
@@ -6959,7 +6959,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C37" s="77" t="s">
         <v>82</v>
@@ -7038,13 +7038,13 @@
         <v>0</v>
       </c>
       <c r="AB37" s="60" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AC37" s="68" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AD37" s="68" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AE37" s="75"/>
       <c r="AF37" s="79"/>
@@ -7054,7 +7054,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="49" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C38" s="77" t="s">
         <v>82</v>
@@ -7133,13 +7133,13 @@
         <v>0</v>
       </c>
       <c r="AB38" s="60" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AC38" s="68" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AD38" s="68" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AE38" s="75"/>
       <c r="AF38" s="79"/>
@@ -7149,7 +7149,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="49" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C39" s="77" t="s">
         <v>82</v>
@@ -7228,13 +7228,13 @@
         <v>0</v>
       </c>
       <c r="AB39" s="60" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AC39" s="68" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AD39" s="68" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE39" s="75"/>
       <c r="AF39" s="79"/>
@@ -7322,13 +7322,13 @@
         <v>0</v>
       </c>
       <c r="AB40" s="64" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AC40" s="63" t="s">
         <v>140</v>
       </c>
       <c r="AD40" s="63" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AE40" s="72"/>
       <c r="AF40" s="71"/>
@@ -7338,7 +7338,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="135" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C41" s="136" t="s">
         <v>66</v>
@@ -7416,10 +7416,10 @@
         <v>0</v>
       </c>
       <c r="AB41" s="64" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AC41" s="63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD41" s="63" t="s">
         <v>137</v>
@@ -7432,7 +7432,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="137" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C42" s="138" t="s">
         <v>87</v>
@@ -7510,7 +7510,7 @@
         <v>0</v>
       </c>
       <c r="AB42" s="64" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AC42" s="63" t="s">
         <v>20</v>
@@ -7526,7 +7526,7 @@
         <v>2</v>
       </c>
       <c r="B43" s="137" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C43" s="138" t="s">
         <v>82</v>
@@ -7605,7 +7605,7 @@
         <v>0</v>
       </c>
       <c r="AB43" s="64" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AC43" s="63" t="s">
         <v>102</v>
@@ -7621,7 +7621,7 @@
         <v>2</v>
       </c>
       <c r="B44" s="49" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C44" s="77" t="s">
         <v>82</v>
@@ -7699,7 +7699,7 @@
         <v>0</v>
       </c>
       <c r="AB44" s="69" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AC44" s="68" t="s">
         <v>140</v>
@@ -7711,7 +7711,7 @@
         <v>114</v>
       </c>
       <c r="AF44" s="150" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
@@ -7719,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="49" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C45" s="77" t="s">
         <v>82</v>
@@ -7797,13 +7797,13 @@
         <v>0</v>
       </c>
       <c r="AB45" s="60" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AC45" s="68" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AD45" s="68" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AE45" s="75"/>
       <c r="AF45" s="74"/>
@@ -7813,7 +7813,7 @@
         <v>2</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C46" s="77" t="s">
         <v>82</v>
@@ -7891,13 +7891,13 @@
         <v>0</v>
       </c>
       <c r="AB46" s="69" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AC46" s="68" t="s">
         <v>20</v>
       </c>
       <c r="AD46" s="68" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AE46" s="68" t="s">
         <v>149</v>
@@ -7911,7 +7911,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C47" s="77" t="s">
         <v>82</v>
@@ -7990,13 +7990,13 @@
         <v>0</v>
       </c>
       <c r="AB47" s="69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AC47" s="68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AD47" s="68" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AE47" s="75"/>
       <c r="AF47" s="74"/>
@@ -8006,7 +8006,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="135" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C48" s="136" t="s">
         <v>68</v>
@@ -8084,10 +8084,10 @@
         <v>0</v>
       </c>
       <c r="AB48" s="64" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AC48" s="63" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AD48" s="63" t="s">
         <v>137</v>
@@ -8096,7 +8096,7 @@
         <v>114</v>
       </c>
       <c r="AF48" s="62" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -8104,7 +8104,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="135" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C49" s="136" t="s">
         <v>87</v>
@@ -8182,13 +8182,13 @@
         <v>0</v>
       </c>
       <c r="AB49" s="64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AC49" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AD49" s="63" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AE49" s="72"/>
       <c r="AF49" s="71"/>
@@ -8198,10 +8198,10 @@
         <v>2</v>
       </c>
       <c r="B50" s="137" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C50" s="138" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D50" s="66">
         <v>40</v>
@@ -8276,19 +8276,19 @@
         <v>0</v>
       </c>
       <c r="AB50" s="64" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AC50" s="63" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD50" s="63" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AE50" s="63" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF50" s="62" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="51" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -8296,10 +8296,10 @@
         <v>2</v>
       </c>
       <c r="B51" s="137" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C51" s="138" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D51" s="66">
         <v>90</v>
@@ -8374,19 +8374,19 @@
         <v>0</v>
       </c>
       <c r="AB51" s="64" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AC51" s="63" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD51" s="63" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AE51" s="63" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF51" s="63" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="52" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -8394,10 +8394,10 @@
         <v>2</v>
       </c>
       <c r="B52" s="49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C52" s="77" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D52" s="61">
         <v>180</v>
@@ -8472,19 +8472,19 @@
         <v>0</v>
       </c>
       <c r="AB52" s="69" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AC52" s="68" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD52" s="68" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AE52" s="68" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF52" s="68" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="53" spans="1:32" x14ac:dyDescent="0.25">
@@ -8492,10 +8492,10 @@
         <v>2</v>
       </c>
       <c r="B53" s="49" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C53" s="77" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D53" s="61">
         <v>330</v>
@@ -8570,19 +8570,19 @@
         <v>0</v>
       </c>
       <c r="AB53" s="69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AC53" s="68" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD53" s="68" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AE53" s="68" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF53" s="78" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
@@ -8590,10 +8590,10 @@
         <v>2</v>
       </c>
       <c r="B54" s="49" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C54" s="77" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D54" s="61">
         <v>360</v>
@@ -8668,19 +8668,19 @@
         <v>0</v>
       </c>
       <c r="AB54" s="69" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AC54" s="68" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD54" s="68" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AE54" s="68" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF54" s="78" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -8688,7 +8688,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C55" s="77" t="s">
         <v>82</v>
@@ -8767,13 +8767,13 @@
         <v>0</v>
       </c>
       <c r="AB55" s="60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AC55" s="68" t="s">
         <v>140</v>
       </c>
       <c r="AD55" s="68" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AE55" s="75"/>
       <c r="AF55" s="74"/>
@@ -8783,7 +8783,7 @@
         <v>2</v>
       </c>
       <c r="B56" s="135" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C56" s="136" t="s">
         <v>82</v>
@@ -8862,13 +8862,13 @@
         <v>0</v>
       </c>
       <c r="AB56" s="67" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AC56" s="63" t="s">
         <v>140</v>
       </c>
       <c r="AD56" s="63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
@@ -8878,10 +8878,10 @@
         <v>2</v>
       </c>
       <c r="B57" s="135" t="s">
+        <v>448</v>
+      </c>
+      <c r="C57" s="136" t="s">
         <v>449</v>
-      </c>
-      <c r="C57" s="136" t="s">
-        <v>450</v>
       </c>
       <c r="D57" s="66">
         <v>270</v>
@@ -8966,7 +8966,7 @@
         <v>2</v>
       </c>
       <c r="B58" s="137" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C58" s="138" t="s">
         <v>82</v>
@@ -9045,13 +9045,13 @@
         <v>0</v>
       </c>
       <c r="AB58" s="64" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AC58" s="63" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AD58" s="63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AE58" s="72"/>
       <c r="AF58" s="80"/>
@@ -9061,7 +9061,7 @@
         <v>2</v>
       </c>
       <c r="B59" s="137" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C59" s="138" t="s">
         <v>82</v>
@@ -9070,7 +9070,7 @@
         <v>20</v>
       </c>
       <c r="E59" s="65">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F59" s="65">
         <v>0</v>
@@ -9140,13 +9140,13 @@
         <v>0</v>
       </c>
       <c r="AB59" s="67" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AC59" s="63" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AD59" s="63" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AE59" s="72"/>
       <c r="AF59" s="80"/>
@@ -9156,7 +9156,7 @@
         <v>2</v>
       </c>
       <c r="B60" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C60" s="77" t="s">
         <v>82</v>
@@ -9235,13 +9235,13 @@
         <v>0</v>
       </c>
       <c r="AB60" s="60" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AC60" s="68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AD60" s="68" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AE60" s="75"/>
       <c r="AF60" s="79"/>
@@ -9251,7 +9251,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C61" s="77" t="s">
         <v>82</v>
@@ -9329,13 +9329,13 @@
         <v>0</v>
       </c>
       <c r="AB61" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AC61" s="68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AD61" s="68" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AE61" s="75"/>
       <c r="AF61" s="74"/>
@@ -9345,7 +9345,7 @@
         <v>2</v>
       </c>
       <c r="B62" s="49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C62" s="77" t="s">
         <v>82</v>
@@ -9424,13 +9424,13 @@
         <v>0</v>
       </c>
       <c r="AB62" s="69" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AC62" s="68" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AD62" s="68" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE62" s="75"/>
       <c r="AF62" s="74"/>
@@ -9440,7 +9440,7 @@
         <v>2</v>
       </c>
       <c r="B63" s="49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C63" s="77" t="s">
         <v>82</v>
@@ -9519,7 +9519,7 @@
         <v>0</v>
       </c>
       <c r="AB63" s="60" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AC63" s="68" t="s">
         <v>140</v>
@@ -9535,7 +9535,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="135" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C64" s="136" t="s">
         <v>61</v>
@@ -9614,13 +9614,13 @@
         <v>0</v>
       </c>
       <c r="AB64" s="67" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AC64" s="63" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AD64" s="63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AE64" s="72"/>
       <c r="AF64" s="80"/>
@@ -9630,7 +9630,7 @@
         <v>2</v>
       </c>
       <c r="B65" s="135" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C65" s="136" t="s">
         <v>61</v>
@@ -9707,10 +9707,10 @@
         <v>0</v>
       </c>
       <c r="AB65" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AC65" s="63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AD65" s="63" t="s">
         <v>150</v>
@@ -9723,7 +9723,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="137" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C66" s="138" t="s">
         <v>66</v>
@@ -9802,19 +9802,19 @@
         <v>0</v>
       </c>
       <c r="AB66" s="64" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AC66" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD66" s="63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AE66" s="63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF66" s="63" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
@@ -9822,7 +9822,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="137" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C67" s="138" t="s">
         <v>66</v>
@@ -9901,19 +9901,19 @@
         <v>0</v>
       </c>
       <c r="AB67" s="64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AC67" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD67" s="63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AE67" s="63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF67" s="63" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.25">
@@ -9921,7 +9921,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C68" s="77" t="s">
         <v>66</v>
@@ -10000,19 +10000,19 @@
         <v>0</v>
       </c>
       <c r="AB68" s="69" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AC68" s="68" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD68" s="68" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AE68" s="68" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF68" s="68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -10020,10 +10020,10 @@
         <v>2</v>
       </c>
       <c r="B69" s="49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C69" s="77" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D69" s="61">
         <v>90</v>
@@ -10098,19 +10098,19 @@
         <v>0</v>
       </c>
       <c r="AB69" s="69" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AC69" s="68" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AD69" s="68" t="s">
         <v>150</v>
       </c>
       <c r="AE69" s="68" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AF69" s="68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -10118,7 +10118,7 @@
         <v>2</v>
       </c>
       <c r="B70" s="49" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C70" s="77" t="s">
         <v>24</v>
@@ -10197,7 +10197,7 @@
         <v>0</v>
       </c>
       <c r="AB70" s="69" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AC70" s="68" t="s">
         <v>99</v>
@@ -10213,7 +10213,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="49" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C71" s="77" t="s">
         <v>24</v>
@@ -10292,7 +10292,7 @@
         <v>0</v>
       </c>
       <c r="AB71" s="60" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AC71" s="68" t="s">
         <v>102</v>
@@ -10308,10 +10308,10 @@
         <v>2</v>
       </c>
       <c r="B72" s="135" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C72" s="136" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D72" s="66">
         <v>90</v>
@@ -10386,19 +10386,19 @@
         <v>0</v>
       </c>
       <c r="AB72" s="64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AC72" s="63" t="s">
         <v>102</v>
       </c>
       <c r="AD72" s="63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AE72" s="63" t="s">
         <v>114</v>
       </c>
       <c r="AF72" s="149" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -10406,7 +10406,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="135" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C73" s="136" t="s">
         <v>61</v>
@@ -10483,7 +10483,7 @@
         <v>0</v>
       </c>
       <c r="AB73" s="67" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AC73" s="63" t="s">
         <v>59</v>
@@ -10499,7 +10499,7 @@
         <v>2</v>
       </c>
       <c r="B74" s="137" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C74" s="138" t="s">
         <v>61</v>
@@ -10576,7 +10576,7 @@
         <v>0</v>
       </c>
       <c r="AB74" s="64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AC74" s="63" t="s">
         <v>59</v>
@@ -10592,7 +10592,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="137" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C75" s="138" t="s">
         <v>66</v>
@@ -10690,7 +10690,7 @@
         <v>2</v>
       </c>
       <c r="B76" s="49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C76" s="77" t="s">
         <v>66</v>
@@ -10768,10 +10768,10 @@
         <v>0</v>
       </c>
       <c r="AB76" s="69" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AC76" s="68" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD76" s="68" t="s">
         <v>162</v>
@@ -10786,7 +10786,7 @@
         <v>2</v>
       </c>
       <c r="B77" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C77" s="77" t="s">
         <v>68</v>
@@ -10864,19 +10864,19 @@
         <v>0</v>
       </c>
       <c r="AB77" s="69" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AC77" s="68" t="s">
         <v>99</v>
       </c>
       <c r="AD77" s="68" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE77" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF77" s="170" t="s">
-        <v>214</v>
+      <c r="AF77" s="169" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.25">
@@ -10884,7 +10884,7 @@
         <v>2</v>
       </c>
       <c r="B78" s="49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C78" s="77" t="s">
         <v>82</v>
@@ -10951,7 +10951,7 @@
         <v>0</v>
       </c>
       <c r="X78" s="55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y78" s="55">
         <v>0.2</v>
@@ -10963,19 +10963,19 @@
         <v>0</v>
       </c>
       <c r="AB78" s="69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AC78" s="68" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AD78" s="68" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE78" s="68" t="s">
-        <v>208</v>
-      </c>
-      <c r="AF78" s="170" t="s">
         <v>207</v>
+      </c>
+      <c r="AF78" s="169" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="79" spans="1:32" x14ac:dyDescent="0.25">
@@ -10983,7 +10983,7 @@
         <v>2</v>
       </c>
       <c r="B79" s="49" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C79" s="77" t="s">
         <v>82</v>
@@ -11061,13 +11061,13 @@
         <v>0</v>
       </c>
       <c r="AB79" s="69" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AC79" s="68" t="s">
         <v>20</v>
       </c>
       <c r="AD79" s="68" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE79" s="75"/>
       <c r="AF79" s="74"/>
@@ -11077,7 +11077,7 @@
         <v>2</v>
       </c>
       <c r="B80" s="135" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C80" s="136" t="s">
         <v>82</v>
@@ -11156,10 +11156,10 @@
         <v>0</v>
       </c>
       <c r="AB80" s="64" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AC80" s="63" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AD80" s="63" t="s">
         <v>98</v>
@@ -11172,7 +11172,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="135" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C81" s="136" t="s">
         <v>82</v>
@@ -11251,13 +11251,13 @@
         <v>0</v>
       </c>
       <c r="AB81" s="67" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AC81" s="63" t="s">
         <v>20</v>
       </c>
       <c r="AD81" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AE81" s="72"/>
       <c r="AF81" s="71"/>
@@ -11267,7 +11267,7 @@
         <v>2</v>
       </c>
       <c r="B82" s="137" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C82" s="138" t="s">
         <v>82</v>
@@ -11345,7 +11345,7 @@
         <v>0</v>
       </c>
       <c r="AB82" s="64" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AC82" s="63" t="s">
         <v>140</v>
@@ -11357,7 +11357,7 @@
         <v>114</v>
       </c>
       <c r="AF82" s="134" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:32" x14ac:dyDescent="0.25">
@@ -11365,7 +11365,7 @@
         <v>2</v>
       </c>
       <c r="B83" s="137" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C83" s="138" t="s">
         <v>82</v>
@@ -11443,13 +11443,13 @@
         <v>0</v>
       </c>
       <c r="AB83" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AC83" s="63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AD83" s="63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AE83" s="63"/>
       <c r="AF83" s="134"/>
@@ -11459,7 +11459,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="49" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C84" s="77" t="s">
         <v>66</v>
@@ -11537,7 +11537,7 @@
         <v>0</v>
       </c>
       <c r="AB84" s="54" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AC84" s="44" t="s">
         <v>99</v>
@@ -11549,7 +11549,7 @@
         <v>114</v>
       </c>
       <c r="AF84" s="43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:32" x14ac:dyDescent="0.25">
@@ -11557,7 +11557,7 @@
         <v>2</v>
       </c>
       <c r="B85" s="49" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C85" s="77" t="s">
         <v>66</v>
@@ -11635,7 +11635,7 @@
         <v>0</v>
       </c>
       <c r="AB85" s="54" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AC85" s="44" t="s">
         <v>99</v>
@@ -11647,7 +11647,7 @@
         <v>114</v>
       </c>
       <c r="AF85" s="43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="86" spans="1:32" x14ac:dyDescent="0.25">
@@ -11655,7 +11655,7 @@
         <v>2</v>
       </c>
       <c r="B86" s="49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C86" s="77" t="s">
         <v>68</v>
@@ -11734,19 +11734,19 @@
         <v>0</v>
       </c>
       <c r="AB86" s="45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AC86" s="44" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AD86" s="44" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AE86" s="44" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF86" s="43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -11754,7 +11754,7 @@
         <v>2</v>
       </c>
       <c r="B87" s="49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C87" s="77" t="s">
         <v>82</v>
@@ -11832,13 +11832,13 @@
         <v>0</v>
       </c>
       <c r="AB87" s="54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AC87" s="44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AD87" s="44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AE87" s="44" t="s">
         <v>114</v>
@@ -11852,7 +11852,7 @@
         <v>2</v>
       </c>
       <c r="B88" s="135" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C88" s="136" t="s">
         <v>24</v>
@@ -11931,19 +11931,19 @@
         <v>1</v>
       </c>
       <c r="AB88" s="51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC88" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD88" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AE88" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AF88" s="142" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="135" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C89" s="136" t="s">
         <v>24</v>
@@ -12029,19 +12029,19 @@
         <v>1</v>
       </c>
       <c r="AB89" s="35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AC89" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD89" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AE89" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AF89" s="147" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="90" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -12049,7 +12049,7 @@
         <v>2</v>
       </c>
       <c r="B90" s="137" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C90" s="138" t="s">
         <v>24</v>
@@ -12127,19 +12127,19 @@
         <v>1</v>
       </c>
       <c r="AB90" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AC90" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD90" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AE90" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF90" s="147" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -12147,7 +12147,7 @@
         <v>2</v>
       </c>
       <c r="B91" s="137" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C91" s="138" t="s">
         <v>24</v>
@@ -12225,19 +12225,19 @@
         <v>0.25</v>
       </c>
       <c r="AB91" s="35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AC91" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD91" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AE91" s="34" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AF91" s="147" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="92" spans="1:32" x14ac:dyDescent="0.25">
@@ -12245,7 +12245,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C92" s="77" t="s">
         <v>66</v>
@@ -12323,10 +12323,10 @@
         <v>0</v>
       </c>
       <c r="AB92" s="54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AC92" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AD92" s="44" t="s">
         <v>80</v>
@@ -12339,7 +12339,7 @@
         <v>2</v>
       </c>
       <c r="B93" s="49" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C93" s="77" t="s">
         <v>66</v>
@@ -12417,7 +12417,7 @@
         <v>0</v>
       </c>
       <c r="AB93" s="54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AC93" s="44" t="s">
         <v>99</v>
@@ -12433,7 +12433,7 @@
         <v>2</v>
       </c>
       <c r="B94" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C94" s="77" t="s">
         <v>82</v>
@@ -12511,7 +12511,7 @@
         <v>0</v>
       </c>
       <c r="AB94" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC94" s="44" t="s">
         <v>171</v>
@@ -12527,7 +12527,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="49" t="s">
-        <v>173</v>
+        <v>501</v>
       </c>
       <c r="C95" s="77" t="s">
         <v>82</v>
@@ -12542,7 +12542,7 @@
         <v>0</v>
       </c>
       <c r="G95" s="76">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H95" s="76">
         <v>0</v>
@@ -12588,7 +12588,7 @@
         <v>1</v>
       </c>
       <c r="V95" s="46">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="W95" s="46">
         <v>0</v>
@@ -12720,7 +12720,7 @@
         <v>2</v>
       </c>
       <c r="B97" s="135" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C97" s="136" t="s">
         <v>82</v>
@@ -12798,7 +12798,7 @@
         <v>0</v>
       </c>
       <c r="AB97" s="35" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AC97" s="34" t="s">
         <v>140</v>
@@ -13106,7 +13106,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="49" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C101" s="77" t="s">
         <v>82</v>
@@ -13294,7 +13294,7 @@
         <v>2</v>
       </c>
       <c r="B103" s="49" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C103" s="77" t="s">
         <v>82</v>
@@ -13373,10 +13373,10 @@
         <v>0</v>
       </c>
       <c r="AB103" s="54" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AC103" s="44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AD103" s="44" t="s">
         <v>137</v>
@@ -13389,7 +13389,7 @@
         <v>2</v>
       </c>
       <c r="B104" s="49" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C104" s="77" t="s">
         <v>61</v>
@@ -13561,19 +13561,19 @@
         <v>0</v>
       </c>
       <c r="AB105" s="35" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AC105" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AD105" s="34" t="s">
         <v>80</v>
       </c>
       <c r="AE105" s="34" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AF105" s="142" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.25">
@@ -13963,7 +13963,7 @@
         <v>2</v>
       </c>
       <c r="B110" s="49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C110" s="77" t="s">
         <v>66</v>
@@ -14041,13 +14041,13 @@
         <v>0</v>
       </c>
       <c r="AB110" s="54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AC110" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AD110" s="44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AE110" s="44"/>
       <c r="AF110" s="43"/>
@@ -14920,7 +14920,7 @@
       <c r="AE119" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="AF119" s="170" t="s">
+      <c r="AF119" s="169" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15196,7 +15196,7 @@
         <v>0</v>
       </c>
       <c r="AB122" s="64" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AC122" s="63" t="s">
         <v>81</v>
@@ -15592,7 +15592,7 @@
         <v>2</v>
       </c>
       <c r="B127" s="49" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C127" s="77" t="s">
         <v>61</v>
@@ -15668,7 +15668,7 @@
         <v>0</v>
       </c>
       <c r="AB127" s="164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AC127" s="72" t="s">
         <v>59</v>
@@ -15684,7 +15684,7 @@
         <v>2</v>
       </c>
       <c r="B128" s="49" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C128" s="77" t="s">
         <v>61</v>
@@ -15760,7 +15760,7 @@
         <v>0</v>
       </c>
       <c r="AB128" s="164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AC128" s="72" t="s">
         <v>59</v>
@@ -15776,7 +15776,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="137" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C129" s="136" t="s">
         <v>61</v>
@@ -15851,8 +15851,8 @@
       <c r="AA129" s="52">
         <v>0</v>
       </c>
-      <c r="AB129" s="168" t="s">
-        <v>225</v>
+      <c r="AB129" s="167" t="s">
+        <v>224</v>
       </c>
       <c r="AC129" s="72" t="s">
         <v>59</v>
@@ -15868,7 +15868,7 @@
         <v>2</v>
       </c>
       <c r="B130" s="137" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C130" s="136" t="s">
         <v>61</v>
@@ -15943,8 +15943,8 @@
       <c r="AA130" s="52">
         <v>0</v>
       </c>
-      <c r="AB130" s="168" t="s">
-        <v>225</v>
+      <c r="AB130" s="167" t="s">
+        <v>224</v>
       </c>
       <c r="AC130" s="72" t="s">
         <v>59</v>
@@ -15960,7 +15960,7 @@
         <v>2</v>
       </c>
       <c r="B131" s="137" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C131" s="136" t="s">
         <v>61</v>
@@ -16035,8 +16035,8 @@
       <c r="AA131" s="52">
         <v>0</v>
       </c>
-      <c r="AB131" s="168" t="s">
-        <v>225</v>
+      <c r="AB131" s="167" t="s">
+        <v>224</v>
       </c>
       <c r="AC131" s="72" t="s">
         <v>59</v>
@@ -16052,7 +16052,7 @@
         <v>2</v>
       </c>
       <c r="B132" s="137" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C132" s="136" t="s">
         <v>61</v>
@@ -16127,8 +16127,8 @@
       <c r="AA132" s="158">
         <v>0</v>
       </c>
-      <c r="AB132" s="169" t="s">
-        <v>225</v>
+      <c r="AB132" s="168" t="s">
+        <v>224</v>
       </c>
       <c r="AC132" s="25" t="s">
         <v>59</v>
@@ -16144,7 +16144,7 @@
         <v>2</v>
       </c>
       <c r="B133" s="49" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C133" s="77" t="s">
         <v>61</v>
@@ -16220,7 +16220,7 @@
         <v>0</v>
       </c>
       <c r="AB133" s="164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AC133" s="72" t="s">
         <v>59</v>
@@ -16236,7 +16236,7 @@
         <v>2</v>
       </c>
       <c r="B134" s="49" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C134" s="77" t="s">
         <v>82</v>
@@ -16315,10 +16315,10 @@
         <v>0</v>
       </c>
       <c r="AB134" s="164" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AC134" s="72" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AD134" s="72" t="s">
         <v>137</v>
@@ -16331,7 +16331,7 @@
         <v>2</v>
       </c>
       <c r="B135" s="49" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C135" s="77" t="s">
         <v>61</v>
@@ -16407,7 +16407,7 @@
         <v>0</v>
       </c>
       <c r="AB135" s="164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AC135" s="72" t="s">
         <v>59</v>
@@ -16423,7 +16423,7 @@
         <v>2</v>
       </c>
       <c r="B136" s="49" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C136" s="77" t="s">
         <v>61</v>
@@ -16499,7 +16499,7 @@
         <v>0</v>
       </c>
       <c r="AB136" s="164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AC136" s="72" t="s">
         <v>59</v>
@@ -16515,7 +16515,7 @@
         <v>2</v>
       </c>
       <c r="B137" s="137" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C137" s="136" t="s">
         <v>61</v>
@@ -16590,8 +16590,8 @@
       <c r="AA137" s="52">
         <v>0</v>
       </c>
-      <c r="AB137" s="168" t="s">
-        <v>225</v>
+      <c r="AB137" s="167" t="s">
+        <v>224</v>
       </c>
       <c r="AC137" s="72" t="s">
         <v>59</v>
@@ -16674,8 +16674,8 @@
       <c r="C141" s="22"/>
       <c r="D141" s="22"/>
       <c r="E141" s="22"/>
-      <c r="F141" s="167"/>
-      <c r="G141" s="167"/>
+      <c r="F141" s="170"/>
+      <c r="G141" s="170"/>
       <c r="H141" s="21" t="s">
         <v>56</v>
       </c>
@@ -17294,7 +17294,7 @@
         <v>2</v>
       </c>
       <c r="B154" s="95" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C154" s="95" t="s">
         <v>38</v>
@@ -17966,7 +17966,7 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -17983,8 +17983,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="170"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>
@@ -17992,25 +17992,25 @@
     </row>
     <row r="4" spans="2:11" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -18018,7 +18018,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D5" s="115">
         <v>0</v>
@@ -18039,7 +18039,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -18057,7 +18057,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C7" s="95"/>
       <c r="D7" s="95"/>
@@ -18065,12 +18065,12 @@
       <c r="F7" s="111"/>
       <c r="G7" s="111"/>
       <c r="H7" s="109" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C8" s="95"/>
       <c r="D8" s="95"/>
@@ -18078,12 +18078,12 @@
       <c r="F8" s="111"/>
       <c r="G8" s="111"/>
       <c r="H8" s="109" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C9" s="95"/>
       <c r="D9" s="95"/>
@@ -18091,7 +18091,7 @@
       <c r="F9" s="111"/>
       <c r="G9" s="111"/>
       <c r="H9" s="109" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -18099,7 +18099,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D10" s="115">
         <v>2</v>
@@ -18117,7 +18117,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C11" s="95"/>
       <c r="D11" s="95"/>
@@ -18125,12 +18125,12 @@
       <c r="F11" s="111"/>
       <c r="G11" s="111"/>
       <c r="H11" s="109" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C12" s="95"/>
       <c r="D12" s="95"/>
@@ -18138,12 +18138,12 @@
       <c r="F12" s="111"/>
       <c r="G12" s="111"/>
       <c r="H12" s="109" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C13" s="95"/>
       <c r="D13" s="95"/>
@@ -18151,7 +18151,7 @@
       <c r="F13" s="111"/>
       <c r="G13" s="111"/>
       <c r="H13" s="109" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -18159,7 +18159,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="115" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D14" s="115">
         <v>3</v>
@@ -18177,7 +18177,7 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C15" s="95"/>
       <c r="D15" s="95"/>
@@ -18185,12 +18185,12 @@
       <c r="F15" s="111"/>
       <c r="G15" s="111"/>
       <c r="H15" s="109" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C16" s="95"/>
       <c r="D16" s="95"/>
@@ -18198,12 +18198,12 @@
       <c r="F16" s="111"/>
       <c r="G16" s="111"/>
       <c r="H16" s="109" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C17" s="95"/>
       <c r="D17" s="95"/>
@@ -18211,7 +18211,7 @@
       <c r="F17" s="111"/>
       <c r="G17" s="111"/>
       <c r="H17" s="109" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -18219,7 +18219,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="115" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D18" s="115">
         <v>4</v>
@@ -18237,7 +18237,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C19" s="95"/>
       <c r="D19" s="95"/>
@@ -18245,12 +18245,12 @@
       <c r="F19" s="111"/>
       <c r="G19" s="111"/>
       <c r="H19" s="109" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C20" s="95"/>
       <c r="D20" s="95"/>
@@ -18258,12 +18258,12 @@
       <c r="F20" s="111"/>
       <c r="G20" s="111"/>
       <c r="H20" s="109" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C21" s="95"/>
       <c r="D21" s="95"/>
@@ -18271,7 +18271,7 @@
       <c r="F21" s="111"/>
       <c r="G21" s="111"/>
       <c r="H21" s="109" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -18279,7 +18279,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="95" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D22" s="95">
         <v>5</v>
@@ -18297,7 +18297,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C23" s="95"/>
       <c r="D23" s="95"/>
@@ -18305,7 +18305,7 @@
       <c r="F23" s="110"/>
       <c r="G23" s="110"/>
       <c r="H23" s="109" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -18313,7 +18313,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="95" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D24" s="95">
         <v>6</v>
@@ -18331,7 +18331,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C25" s="95"/>
       <c r="D25" s="95"/>
@@ -18339,7 +18339,7 @@
       <c r="F25" s="110"/>
       <c r="G25" s="110"/>
       <c r="H25" s="109" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -18347,7 +18347,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="95" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D26" s="95">
         <v>7</v>
@@ -18365,7 +18365,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C27" s="95"/>
       <c r="D27" s="95"/>
@@ -18373,7 +18373,7 @@
       <c r="F27" s="110"/>
       <c r="G27" s="110"/>
       <c r="H27" s="109" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -18381,7 +18381,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="95" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D28" s="95">
         <v>8</v>
@@ -18399,7 +18399,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="112" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C29" s="95"/>
       <c r="D29" s="95"/>
@@ -18407,13 +18407,13 @@
       <c r="F29" s="110"/>
       <c r="G29" s="110"/>
       <c r="H29" s="109" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B33" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -18424,16 +18424,16 @@
     </row>
     <row r="35" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
       <c r="B35" s="108" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C35" s="107" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E35" s="107" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -18441,7 +18441,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="105" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D36" s="105">
         <v>1</v>
@@ -18455,7 +18455,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="105" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D37" s="105">
         <v>2</v>
@@ -18469,7 +18469,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="105" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D38" s="105">
         <v>3</v>
@@ -18483,7 +18483,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="105" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D39" s="105">
         <v>4</v>
@@ -18497,7 +18497,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="105" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D40" s="105">
         <v>5</v>
@@ -18511,7 +18511,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="105" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D41" s="105">
         <v>6</v>
@@ -18525,7 +18525,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="105" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D42" s="105">
         <v>7</v>
@@ -18539,7 +18539,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="105" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D43" s="105">
         <v>8</v>
@@ -18553,7 +18553,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="105" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D44" s="105">
         <v>9</v>
@@ -18567,7 +18567,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="105" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D45" s="105">
         <v>10</v>
@@ -18579,7 +18579,7 @@
     <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B47" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
@@ -18590,25 +18590,25 @@
     </row>
     <row r="49" spans="2:8" ht="130.5" x14ac:dyDescent="0.25">
       <c r="B49" s="103" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C49" s="103" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="103" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E49" s="102" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F49" s="102" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G49" s="102" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H49" s="102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -18616,13 +18616,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="100" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D50" s="100" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E50" s="99" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F50" s="99">
         <v>50</v>

</xml_diff>

<commit_message>
Unkas has their own sku in content
Former-commit-id: f5da2109b9c32dba74a59b7005c6e128ace5a3ce
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$142:$O$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$143:$O$144</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="503">
   <si>
     <t>tier_4</t>
   </si>
@@ -1547,6 +1547,9 @@
   </si>
   <si>
     <t>OwlWhite</t>
+  </si>
+  <si>
+    <t>Unka</t>
   </si>
 </sst>
 </file>
@@ -2540,7 +2543,154 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="113">
+  <dxfs count="114">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4836,146 +4986,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4990,114 +5000,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF137" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF137"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF138" totalsRowShown="0" headerRowDxfId="113" dataDxfId="111" headerRowBorderDxfId="112" tableBorderDxfId="110" totalsRowBorderDxfId="109">
+  <autoFilter ref="A23:AF138"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="108"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="107"/>
+    <tableColumn id="6" name="[category]" dataDxfId="106"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="105"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="104"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="103"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="102"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="101"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="100"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="99"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="98"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="97"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="96"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="95"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="94"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="93"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="92"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="91"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="90"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="89"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="88"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="87"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="86"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="85"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="84"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="83"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="82"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="81"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="80"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="79"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="78"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="76" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="72"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A142:O154" totalsRowShown="0">
-  <autoFilter ref="A142:O154"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A143:O155" totalsRowShown="0">
+  <autoFilter ref="A143:O155"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="4" name="[category]" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="16" name="[size]" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="42" totalsRowDxfId="41"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="36"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
+    <tableColumn id="6" name="[order]" dataDxfId="34"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="33"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="32"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="31"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="22"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="21" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5369,12 +5379,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF171"/>
+  <dimension ref="A1:AF172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A95" sqref="A95"/>
+      <selection pane="topRight" activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16510,309 +16520,354 @@
       <c r="AE136" s="161"/>
       <c r="AF136" s="162"/>
     </row>
-    <row r="137" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A137" s="139" t="s">
         <v>2</v>
       </c>
       <c r="B137" s="137" t="s">
+        <v>502</v>
+      </c>
+      <c r="C137" s="136" t="s">
+        <v>68</v>
+      </c>
+      <c r="D137" s="66">
+        <v>85</v>
+      </c>
+      <c r="E137" s="65">
+        <v>4</v>
+      </c>
+      <c r="F137" s="65">
+        <v>0</v>
+      </c>
+      <c r="G137" s="65">
+        <v>16</v>
+      </c>
+      <c r="H137" s="65">
+        <v>0</v>
+      </c>
+      <c r="I137" s="65">
+        <v>95</v>
+      </c>
+      <c r="J137" s="65">
+        <v>0</v>
+      </c>
+      <c r="K137" s="53">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L137" s="65">
+        <v>0</v>
+      </c>
+      <c r="M137" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N137" s="32">
+        <v>5</v>
+      </c>
+      <c r="O137" s="32">
+        <v>0</v>
+      </c>
+      <c r="P137" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q137" s="32">
+        <v>0</v>
+      </c>
+      <c r="R137" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S137" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="T137" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U137" s="36">
+        <v>30</v>
+      </c>
+      <c r="V137" s="27">
+        <v>8</v>
+      </c>
+      <c r="W137" s="27">
+        <v>0</v>
+      </c>
+      <c r="X137" s="158">
+        <v>0.25</v>
+      </c>
+      <c r="Y137" s="158">
+        <v>0.25</v>
+      </c>
+      <c r="Z137" s="158">
+        <v>0.8</v>
+      </c>
+      <c r="AA137" s="158">
+        <v>0</v>
+      </c>
+      <c r="AB137" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC137" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD137" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE137" s="25"/>
+      <c r="AF137" s="24"/>
+    </row>
+    <row r="138" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="139" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="137" t="s">
         <v>499</v>
       </c>
-      <c r="C137" s="136" t="s">
+      <c r="C138" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="D137" s="66">
+      <c r="D138" s="66">
         <v>100</v>
       </c>
-      <c r="E137" s="65">
-        <v>0</v>
-      </c>
-      <c r="F137" s="65">
-        <v>0</v>
-      </c>
-      <c r="G137" s="65">
-        <v>0</v>
-      </c>
-      <c r="H137" s="65">
-        <v>0</v>
-      </c>
-      <c r="I137" s="65">
+      <c r="E138" s="65">
+        <v>0</v>
+      </c>
+      <c r="F138" s="65">
+        <v>0</v>
+      </c>
+      <c r="G138" s="65">
+        <v>0</v>
+      </c>
+      <c r="H138" s="65">
+        <v>0</v>
+      </c>
+      <c r="I138" s="65">
         <v>50</v>
       </c>
-      <c r="J137" s="65">
-        <v>0</v>
-      </c>
-      <c r="K137" s="53">
-        <v>0</v>
-      </c>
-      <c r="L137" s="65">
-        <v>0</v>
-      </c>
-      <c r="M137" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="N137" s="40">
-        <v>5</v>
-      </c>
-      <c r="O137" s="37">
-        <v>5</v>
-      </c>
-      <c r="P137" s="81">
-        <v>0</v>
-      </c>
-      <c r="Q137" s="40">
-        <v>0</v>
-      </c>
-      <c r="R137" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="S137" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="T137" s="73" t="b">
-        <v>0</v>
-      </c>
-      <c r="U137" s="36">
-        <v>1</v>
-      </c>
-      <c r="V137" s="36"/>
-      <c r="W137" s="36">
-        <v>0</v>
-      </c>
-      <c r="X137" s="52">
-        <v>0</v>
-      </c>
-      <c r="Y137" s="52">
-        <v>0</v>
-      </c>
-      <c r="Z137" s="52">
-        <v>0</v>
-      </c>
-      <c r="AA137" s="52">
-        <v>0</v>
-      </c>
-      <c r="AB137" s="167" t="s">
+      <c r="J138" s="65">
+        <v>0</v>
+      </c>
+      <c r="K138" s="53">
+        <v>0</v>
+      </c>
+      <c r="L138" s="65">
+        <v>0</v>
+      </c>
+      <c r="M138" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N138" s="40">
+        <v>5</v>
+      </c>
+      <c r="O138" s="37">
+        <v>5</v>
+      </c>
+      <c r="P138" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="40">
+        <v>0</v>
+      </c>
+      <c r="R138" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S138" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="T138" s="73" t="b">
+        <v>0</v>
+      </c>
+      <c r="U138" s="36">
+        <v>1</v>
+      </c>
+      <c r="V138" s="36"/>
+      <c r="W138" s="36">
+        <v>0</v>
+      </c>
+      <c r="X138" s="52">
+        <v>0</v>
+      </c>
+      <c r="Y138" s="52">
+        <v>0</v>
+      </c>
+      <c r="Z138" s="52">
+        <v>0</v>
+      </c>
+      <c r="AA138" s="52">
+        <v>0</v>
+      </c>
+      <c r="AB138" s="167" t="s">
         <v>224</v>
       </c>
-      <c r="AC137" s="72" t="s">
+      <c r="AC138" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="AD137" s="72" t="s">
+      <c r="AD138" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE137" s="72"/>
-      <c r="AF137" s="71"/>
-    </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A138" s="118"/>
-      <c r="B138" s="118"/>
-      <c r="C138" s="118"/>
-      <c r="D138" s="119"/>
-      <c r="E138" s="120"/>
-      <c r="F138" s="120"/>
-      <c r="G138" s="120"/>
-      <c r="H138" s="120"/>
-      <c r="I138" s="120"/>
-      <c r="J138" s="121"/>
-      <c r="K138" s="120"/>
-      <c r="L138" s="122"/>
-      <c r="M138" s="123"/>
-      <c r="N138" s="123"/>
-      <c r="O138" s="124"/>
-      <c r="P138" s="123"/>
-      <c r="Q138" s="125"/>
-      <c r="R138" s="126"/>
-      <c r="S138" s="126"/>
-      <c r="T138" s="125"/>
-      <c r="U138" s="126"/>
-      <c r="V138" s="127"/>
-      <c r="W138" s="128"/>
-      <c r="X138" s="129"/>
-      <c r="Y138" s="129"/>
-      <c r="Z138" s="130"/>
-      <c r="AA138" s="131"/>
-      <c r="AB138" s="131"/>
-      <c r="AC138" s="132"/>
-      <c r="AD138" s="132"/>
-      <c r="AE138" s="133"/>
-    </row>
-    <row r="139" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="140" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A140" s="9" t="s">
+      <c r="AE138" s="72"/>
+      <c r="AF138" s="71"/>
+    </row>
+    <row r="139" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A139" s="118"/>
+      <c r="B139" s="118"/>
+      <c r="C139" s="118"/>
+      <c r="D139" s="119"/>
+      <c r="E139" s="120"/>
+      <c r="F139" s="120"/>
+      <c r="G139" s="120"/>
+      <c r="H139" s="120"/>
+      <c r="I139" s="120"/>
+      <c r="J139" s="121"/>
+      <c r="K139" s="120"/>
+      <c r="L139" s="122"/>
+      <c r="M139" s="123"/>
+      <c r="N139" s="123"/>
+      <c r="O139" s="124"/>
+      <c r="P139" s="123"/>
+      <c r="Q139" s="125"/>
+      <c r="R139" s="126"/>
+      <c r="S139" s="126"/>
+      <c r="T139" s="125"/>
+      <c r="U139" s="126"/>
+      <c r="V139" s="127"/>
+      <c r="W139" s="128"/>
+      <c r="X139" s="129"/>
+      <c r="Y139" s="129"/>
+      <c r="Z139" s="130"/>
+      <c r="AA139" s="131"/>
+      <c r="AB139" s="131"/>
+      <c r="AC139" s="132"/>
+      <c r="AD139" s="132"/>
+      <c r="AE139" s="133"/>
+    </row>
+    <row r="140" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="141" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A141" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B140" s="9"/>
-      <c r="C140" s="9"/>
-      <c r="D140" s="9"/>
-      <c r="E140" s="9"/>
-      <c r="F140" s="9"/>
-      <c r="G140" s="9"/>
-      <c r="H140" s="9"/>
-      <c r="I140" s="9"/>
-      <c r="J140" s="9"/>
-      <c r="K140" s="9"/>
-      <c r="L140" s="9"/>
-      <c r="M140" s="9"/>
-      <c r="N140" s="9"/>
-      <c r="O140" s="9"/>
-      <c r="P140" s="9"/>
-      <c r="Q140" s="9"/>
-      <c r="R140" s="9"/>
-      <c r="S140" s="9"/>
-      <c r="T140" s="9"/>
-      <c r="U140" s="9"/>
-      <c r="V140" s="9"/>
-      <c r="W140" s="9"/>
-      <c r="X140" s="9"/>
-      <c r="Y140" s="9"/>
-      <c r="Z140" s="9"/>
-      <c r="AA140" s="9"/>
-      <c r="AF140" s="8"/>
-    </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A141" s="22"/>
-      <c r="B141" s="22"/>
-      <c r="C141" s="22"/>
-      <c r="D141" s="22"/>
-      <c r="E141" s="22"/>
-      <c r="F141" s="170"/>
-      <c r="G141" s="170"/>
-      <c r="H141" s="21" t="s">
+      <c r="B141" s="9"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
+      <c r="I141" s="9"/>
+      <c r="J141" s="9"/>
+      <c r="K141" s="9"/>
+      <c r="L141" s="9"/>
+      <c r="M141" s="9"/>
+      <c r="N141" s="9"/>
+      <c r="O141" s="9"/>
+      <c r="P141" s="9"/>
+      <c r="Q141" s="9"/>
+      <c r="R141" s="9"/>
+      <c r="S141" s="9"/>
+      <c r="T141" s="9"/>
+      <c r="U141" s="9"/>
+      <c r="V141" s="9"/>
+      <c r="W141" s="9"/>
+      <c r="X141" s="9"/>
+      <c r="Y141" s="9"/>
+      <c r="Z141" s="9"/>
+      <c r="AA141" s="9"/>
+      <c r="AF141" s="8"/>
+    </row>
+    <row r="142" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A142" s="22"/>
+      <c r="B142" s="22"/>
+      <c r="C142" s="22"/>
+      <c r="D142" s="22"/>
+      <c r="E142" s="22"/>
+      <c r="F142" s="170"/>
+      <c r="G142" s="170"/>
+      <c r="H142" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I141" s="21"/>
-      <c r="J141" s="22"/>
-      <c r="K141" s="17"/>
-      <c r="L141" s="17"/>
-      <c r="M141" s="17" t="s">
+      <c r="I142" s="21"/>
+      <c r="J142" s="22"/>
+      <c r="K142" s="17"/>
+      <c r="L142" s="17"/>
+      <c r="M142" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N141" s="17"/>
-      <c r="O141" s="17"/>
-      <c r="P141" s="17"/>
-      <c r="Q141" s="17"/>
-      <c r="R141" s="17"/>
-      <c r="S141" s="17"/>
-      <c r="T141" s="17"/>
-      <c r="U141" s="17"/>
-      <c r="V141" s="17"/>
-      <c r="W141" s="17"/>
-      <c r="X141" s="17"/>
-      <c r="Y141" s="17"/>
-      <c r="Z141" s="17"/>
-      <c r="AA141" s="21"/>
-      <c r="AB141" s="21"/>
-      <c r="AC141" s="21"/>
-      <c r="AD141" s="21"/>
-      <c r="AE141" s="17"/>
-    </row>
-    <row r="142" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="7" t="s">
+      <c r="N142" s="17"/>
+      <c r="O142" s="17"/>
+      <c r="P142" s="17"/>
+      <c r="Q142" s="17"/>
+      <c r="R142" s="17"/>
+      <c r="S142" s="17"/>
+      <c r="T142" s="17"/>
+      <c r="U142" s="17"/>
+      <c r="V142" s="17"/>
+      <c r="W142" s="17"/>
+      <c r="X142" s="17"/>
+      <c r="Y142" s="17"/>
+      <c r="Z142" s="17"/>
+      <c r="AA142" s="21"/>
+      <c r="AB142" s="21"/>
+      <c r="AC142" s="21"/>
+      <c r="AD142" s="21"/>
+      <c r="AE142" s="17"/>
+    </row>
+    <row r="143" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A143" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B142" s="7" t="s">
+      <c r="B143" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C142" s="7" t="s">
+      <c r="C143" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D142" s="20" t="s">
+      <c r="D143" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E142" s="20" t="s">
+      <c r="E143" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F142" s="20" t="s">
+      <c r="F143" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G142" s="20" t="s">
+      <c r="G143" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H142" s="20" t="s">
+      <c r="H143" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I142" s="20" t="s">
+      <c r="I143" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J142" s="20" t="s">
+      <c r="J143" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K142" s="20" t="s">
+      <c r="K143" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="L142" s="20" t="s">
+      <c r="L143" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M142" s="19" t="s">
+      <c r="M143" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N142" s="19" t="s">
+      <c r="N143" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O142" s="19" t="s">
+      <c r="O143" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A143" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B143" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C143" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D143" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E143" s="14">
-        <v>3</v>
-      </c>
-      <c r="F143" s="18">
-        <v>0</v>
-      </c>
-      <c r="G143" s="18">
-        <v>0</v>
-      </c>
-      <c r="H143" s="18">
-        <v>0</v>
-      </c>
-      <c r="I143" s="18">
-        <v>0</v>
-      </c>
-      <c r="J143" s="12">
-        <v>2</v>
-      </c>
-      <c r="K143" s="12">
-        <v>0</v>
-      </c>
-      <c r="L143" s="12">
-        <v>0</v>
-      </c>
-      <c r="M143" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N143" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O143" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P143" s="17"/>
-      <c r="Q143" s="17"/>
     </row>
     <row r="144" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A144" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B144" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C144" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E144" s="14">
         <v>3</v>
@@ -16821,7 +16876,7 @@
         <v>0</v>
       </c>
       <c r="G144" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H144" s="18">
         <v>0</v>
@@ -16855,13 +16910,13 @@
         <v>2</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E145" s="14">
         <v>3</v>
@@ -16870,7 +16925,7 @@
         <v>0</v>
       </c>
       <c r="G145" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H145" s="18">
         <v>0</v>
@@ -16904,13 +16959,13 @@
         <v>2</v>
       </c>
       <c r="B146" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C146" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E146" s="14">
         <v>3</v>
@@ -16919,7 +16974,7 @@
         <v>0</v>
       </c>
       <c r="G146" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H146" s="18">
         <v>0</v>
@@ -16953,13 +17008,13 @@
         <v>2</v>
       </c>
       <c r="B147" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E147" s="14">
         <v>3</v>
@@ -16968,7 +17023,7 @@
         <v>0</v>
       </c>
       <c r="G147" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H147" s="18">
         <v>0</v>
@@ -17002,13 +17057,13 @@
         <v>2</v>
       </c>
       <c r="B148" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C148" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E148" s="14">
         <v>3</v>
@@ -17017,7 +17072,7 @@
         <v>0</v>
       </c>
       <c r="G148" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H148" s="18">
         <v>0</v>
@@ -17051,13 +17106,13 @@
         <v>2</v>
       </c>
       <c r="B149" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C149" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D149" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E149" s="14">
         <v>3</v>
@@ -17066,7 +17121,7 @@
         <v>0</v>
       </c>
       <c r="G149" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H149" s="18">
         <v>0</v>
@@ -17100,13 +17155,13 @@
         <v>2</v>
       </c>
       <c r="B150" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D150" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E150" s="14">
         <v>3</v>
@@ -17115,7 +17170,7 @@
         <v>0</v>
       </c>
       <c r="G150" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H150" s="18">
         <v>0</v>
@@ -17149,13 +17204,13 @@
         <v>2</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C151" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E151" s="14">
         <v>3</v>
@@ -17164,7 +17219,7 @@
         <v>0</v>
       </c>
       <c r="G151" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H151" s="18">
         <v>0</v>
@@ -17198,13 +17253,13 @@
         <v>2</v>
       </c>
       <c r="B152" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C152" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E152" s="14">
         <v>3</v>
@@ -17213,7 +17268,7 @@
         <v>0</v>
       </c>
       <c r="G152" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H152" s="18">
         <v>0</v>
@@ -17247,27 +17302,27 @@
         <v>2</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E153" s="14">
-        <v>1</v>
-      </c>
-      <c r="F153" s="13">
-        <v>0</v>
-      </c>
-      <c r="G153" s="13">
-        <v>1</v>
-      </c>
-      <c r="H153" s="13">
-        <v>0</v>
-      </c>
-      <c r="I153" s="13">
+        <v>3</v>
+      </c>
+      <c r="F153" s="18">
+        <v>0</v>
+      </c>
+      <c r="G153" s="18">
+        <v>2</v>
+      </c>
+      <c r="H153" s="18">
+        <v>0</v>
+      </c>
+      <c r="I153" s="18">
         <v>0</v>
       </c>
       <c r="J153" s="12">
@@ -17288,33 +17343,35 @@
       <c r="O153" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P153" s="17"/>
+      <c r="Q153" s="17"/>
     </row>
     <row r="154" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A154" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B154" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="C154" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="D154" s="143" t="s">
-        <v>30</v>
+      <c r="B154" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C154" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D154" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E154" s="14">
         <v>1</v>
       </c>
-      <c r="F154" s="144">
-        <v>0</v>
-      </c>
-      <c r="G154" s="144">
-        <v>0</v>
-      </c>
-      <c r="H154" s="144">
-        <v>0</v>
-      </c>
-      <c r="I154" s="144">
+      <c r="F154" s="13">
+        <v>0</v>
+      </c>
+      <c r="G154" s="13">
+        <v>1</v>
+      </c>
+      <c r="H154" s="13">
+        <v>0</v>
+      </c>
+      <c r="I154" s="13">
         <v>0</v>
       </c>
       <c r="J154" s="12">
@@ -17335,26 +17392,53 @@
       <c r="O154" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P154" s="8"/>
-      <c r="Q154" s="8"/>
-      <c r="R154" s="8"/>
-      <c r="S154" s="8"/>
-      <c r="T154" s="8"/>
-      <c r="U154" s="8"/>
-      <c r="V154" s="8"/>
-      <c r="W154" s="8"/>
-      <c r="X154" s="8"/>
-      <c r="Y154" s="8"/>
-      <c r="Z154" s="8"/>
-      <c r="AA154" s="8"/>
-      <c r="AB154" s="8"/>
-      <c r="AC154" s="8"/>
-      <c r="AD154" s="8"/>
-      <c r="AE154" s="8"/>
     </row>
     <row r="155" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N155" s="8"/>
-      <c r="O155" s="8"/>
+      <c r="A155" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B155" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="C155" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D155" s="143" t="s">
+        <v>30</v>
+      </c>
+      <c r="E155" s="14">
+        <v>1</v>
+      </c>
+      <c r="F155" s="144">
+        <v>0</v>
+      </c>
+      <c r="G155" s="144">
+        <v>0</v>
+      </c>
+      <c r="H155" s="144">
+        <v>0</v>
+      </c>
+      <c r="I155" s="144">
+        <v>0</v>
+      </c>
+      <c r="J155" s="12">
+        <v>2</v>
+      </c>
+      <c r="K155" s="12">
+        <v>0</v>
+      </c>
+      <c r="L155" s="12">
+        <v>0</v>
+      </c>
+      <c r="M155" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N155" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O155" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="P155" s="8"/>
       <c r="Q155" s="8"/>
       <c r="R155" s="8"/>
@@ -17372,73 +17456,67 @@
       <c r="AD155" s="8"/>
       <c r="AE155" s="8"/>
     </row>
-    <row r="156" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="157" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A157" s="9" t="s">
+    <row r="156" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N156" s="8"/>
+      <c r="O156" s="8"/>
+      <c r="P156" s="8"/>
+      <c r="Q156" s="8"/>
+      <c r="R156" s="8"/>
+      <c r="S156" s="8"/>
+      <c r="T156" s="8"/>
+      <c r="U156" s="8"/>
+      <c r="V156" s="8"/>
+      <c r="W156" s="8"/>
+      <c r="X156" s="8"/>
+      <c r="Y156" s="8"/>
+      <c r="Z156" s="8"/>
+      <c r="AA156" s="8"/>
+      <c r="AB156" s="8"/>
+      <c r="AC156" s="8"/>
+      <c r="AD156" s="8"/>
+      <c r="AE156" s="8"/>
+    </row>
+    <row r="157" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="158" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A158" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B157" s="9"/>
-      <c r="C157" s="9"/>
-      <c r="D157" s="9"/>
-      <c r="E157" s="8"/>
-      <c r="F157" s="8"/>
-      <c r="G157" s="8"/>
-      <c r="H157" s="8"/>
-      <c r="I157" s="8"/>
-      <c r="J157" s="8"/>
-      <c r="K157" s="8"/>
-      <c r="L157" s="8"/>
-    </row>
-    <row r="159" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="7" t="s">
+      <c r="B158" s="9"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="8"/>
+      <c r="F158" s="8"/>
+      <c r="G158" s="8"/>
+      <c r="H158" s="8"/>
+      <c r="I158" s="8"/>
+      <c r="J158" s="8"/>
+      <c r="K158" s="8"/>
+      <c r="L158" s="8"/>
+    </row>
+    <row r="160" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A160" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B159" s="6" t="s">
+      <c r="B160" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C159" s="6" t="s">
+      <c r="C160" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D159" s="5" t="s">
+      <c r="D160" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E159" s="5" t="s">
+      <c r="E160" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F159" s="5" t="s">
+      <c r="F160" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G159" s="5" t="s">
+      <c r="G160" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H159" s="5" t="s">
+      <c r="H160" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="160" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A160" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D160" s="2">
-        <v>42</v>
-      </c>
-      <c r="E160" s="2">
-        <v>8</v>
-      </c>
-      <c r="F160" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G160" s="2">
-        <v>2</v>
-      </c>
-      <c r="H160" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -17446,19 +17524,19 @@
         <v>2</v>
       </c>
       <c r="B161" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D161" s="2">
+        <v>42</v>
+      </c>
+      <c r="E161" s="2">
         <v>8</v>
       </c>
-      <c r="C161" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D161" s="2">
-        <v>92</v>
-      </c>
-      <c r="E161" s="2">
-        <v>10</v>
-      </c>
       <c r="F161" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G161" s="2">
         <v>2</v>
@@ -17472,19 +17550,19 @@
         <v>2</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D162" s="2">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="E162" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F162" s="2">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G162" s="2">
         <v>2</v>
@@ -17498,19 +17576,19 @@
         <v>2</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D163" s="2">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="E163" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F163" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G163" s="2">
         <v>2</v>
@@ -17524,104 +17602,130 @@
         <v>2</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D164" s="2">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="E164" s="2">
         <v>14</v>
       </c>
       <c r="F164" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G164" s="2">
+        <v>2</v>
+      </c>
+      <c r="H164" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D165" s="2">
+        <v>1040</v>
+      </c>
+      <c r="E165" s="2">
+        <v>14</v>
+      </c>
+      <c r="F165" s="2">
         <v>0.5</v>
       </c>
-      <c r="G164" s="2">
-        <v>2</v>
-      </c>
-      <c r="H164" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D167" s="1">
-        <v>42</v>
-      </c>
-      <c r="F167" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G167">
-        <f>D160*F160</f>
-        <v>54.6</v>
-      </c>
-      <c r="I167">
-        <f>D167*F167</f>
-        <v>54.6</v>
+      <c r="G165" s="2">
+        <v>2</v>
+      </c>
+      <c r="H165" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D168" s="1">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="F168" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G168">
         <f>D161*F161</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
       <c r="I168">
         <f>D168*F168</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D169" s="1">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="F169" s="1">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G169">
         <f>D162*F162</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
       <c r="I169">
         <f>D169*F169</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D170" s="1">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="F170" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G170">
         <f>D163*F163</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
       <c r="I170">
         <f>D170*F170</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D171" s="1">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="F171" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G171">
         <f>D164*F164</f>
-        <v>520</v>
+        <v>480.2</v>
       </c>
       <c r="I171">
         <f>D171*F171</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D172" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F172" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G172">
+        <f>D165*F165</f>
+        <v>520</v>
+      </c>
+      <c r="I172">
+        <f>D172*F172</f>
         <v>520</v>
       </c>
     </row>
@@ -17629,20 +17733,20 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="F142:G142"/>
   </mergeCells>
   <conditionalFormatting sqref="M118:M124 R118:T124 M24:M56 R24:T56 S127:T127 M127 R58:T115 M58:M115">
-    <cfRule type="expression" dxfId="112" priority="61">
+    <cfRule type="expression" dxfId="20" priority="63">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="111" priority="54">
+    <cfRule type="expression" dxfId="19" priority="56">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116:Q116">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17654,11 +17758,40 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="110" priority="48">
+    <cfRule type="expression" dxfId="18" priority="50">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N115:Q119">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N118:Q124 N24:Q56 N58:Q115">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M114 R114:T114">
+    <cfRule type="expression" dxfId="17" priority="48">
+      <formula>M114=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N114:Q114">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -17670,47 +17803,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N118:Q124 N24:Q56 N58:Q115">
-    <cfRule type="colorScale" priority="66">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="109" priority="46">
-      <formula>M114=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N114:Q114">
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="108" priority="43">
+    <cfRule type="expression" dxfId="16" priority="45">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="107" priority="42">
+    <cfRule type="expression" dxfId="15" priority="44">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q125">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17722,7 +17826,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q127">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17734,17 +17838,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="106" priority="40">
+    <cfRule type="expression" dxfId="14" priority="42">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="105" priority="39">
+    <cfRule type="expression" dxfId="13" priority="41">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:Q128">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17756,22 +17860,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="104" priority="37">
+    <cfRule type="expression" dxfId="12" priority="39">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="103" priority="22">
+    <cfRule type="expression" dxfId="11" priority="24">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="102" priority="24">
+    <cfRule type="expression" dxfId="10" priority="26">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N133:Q133">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17783,17 +17887,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="101" priority="17">
+    <cfRule type="expression" dxfId="9" priority="19">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="100" priority="18">
+    <cfRule type="expression" dxfId="8" priority="20">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N129:Q132">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17805,7 +17909,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:Q134">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17817,17 +17921,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="99" priority="15">
+    <cfRule type="expression" dxfId="7" priority="17">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="98" priority="10">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N135:Q135">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17839,16 +17943,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="97" priority="12">
+    <cfRule type="expression" dxfId="5" priority="14">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="96" priority="5">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N136:Q136">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S136:T136 M136">
+    <cfRule type="expression" dxfId="3" priority="9">
+      <formula>M136=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M138 R138:T138">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>M138=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N138:Q138">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -17860,17 +17986,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="95" priority="7">
-      <formula>M136=FALSE</formula>
+  <conditionalFormatting sqref="M57 R57:T57">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="94" priority="3">
-      <formula>M137=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N137:Q137">
+  <conditionalFormatting sqref="N57:Q57">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -17882,12 +18003,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="93" priority="1">
-      <formula>M57=FALSE</formula>
+  <conditionalFormatting sqref="M137 R137:T137">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57:Q57">
+  <conditionalFormatting sqref="N137:Q137">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -17901,32 +18022,32 @@
   </conditionalFormatting>
   <dataValidations count="10">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G134"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G133 G135:G138 H40:I138 J24:J137">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G133 J24:J138 H40:I139 G135:G139">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D143:G154 M138:N138 P138:V138 Q24:W137 N24:O137">
+    <dataValidation type="decimal" allowBlank="1" sqref="D144:G155 M139:N139 P139:V139 N24:O138 Q24:W138">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H143:L152 H153:I153 J154:L154 W138:Z138 X24:AA137">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H144:L153 H154:I154 J155:L155 W139:Z139 X24:AA138">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C143:C154 C24:C138">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C144:C155 C24:C139">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J153:L153 M143:O154 AA138:AE138 AB24:AF137"/>
-    <dataValidation type="list" sqref="O138 P24:P137">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J154:L154 M144:O155 AA139:AE139 AB24:AF138"/>
+    <dataValidation type="list" sqref="O139 P24:P138">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J138:K138 K24:L137">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J139:K139 K24:L138">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="L138 M24:M137">
+    <dataValidation type="list" sqref="L139 M24:M138">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F138">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F139">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changed 'star' content sku name. Also, 'coins' gives 2 coins instead of 3
Former-commit-id: 271b635c7eb7cec43ed29de33da40628a9aa684d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -1528,9 +1528,6 @@
     <t>RouletteStar</t>
   </si>
   <si>
-    <t>Star</t>
-  </si>
-  <si>
     <r>
       <t>TID_QUIP_ENT_DMG_DRG_MINEBIG_01;</t>
     </r>
@@ -1550,6 +1547,9 @@
   </si>
   <si>
     <t>Unka</t>
+  </si>
+  <si>
+    <t>StarSky</t>
   </si>
 </sst>
 </file>
@@ -2544,153 +2544,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="114">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4986,6 +4839,153 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5000,58 +5000,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF138" totalsRowShown="0" headerRowDxfId="113" dataDxfId="111" headerRowBorderDxfId="112" tableBorderDxfId="110" totalsRowBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF138" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF138"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="108"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="107"/>
-    <tableColumn id="6" name="[category]" dataDxfId="106"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="105"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="104"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="103"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="102"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="101"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="100"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="99"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="98"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="97"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="96"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="95"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="94"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="93"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="92"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="91"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="90"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="89"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="88"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="87"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="86"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="85"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="84"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="83"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="82"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="81"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="80"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="79"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="78"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="77"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="76" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="72"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="71"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5064,50 +5064,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="4" name="[category]" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="16" name="[size]" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="36"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="35"/>
-    <tableColumn id="6" name="[order]" dataDxfId="34"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="33"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="32"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="31"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="30"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="22"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="21" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5381,10 +5381,10 @@
   </sheetPr>
   <dimension ref="A1:AF172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="B137" sqref="B137"/>
+      <selection pane="topRight" activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10518,7 +10518,7 @@
         <v>40</v>
       </c>
       <c r="E74" s="65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" s="65">
         <v>0</v>
@@ -12244,7 +12244,7 @@
         <v>180</v>
       </c>
       <c r="AE91" s="34" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AF91" s="147" t="s">
         <v>178</v>
@@ -12537,7 +12537,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="49" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C95" s="77" t="s">
         <v>82</v>
@@ -16525,7 +16525,7 @@
         <v>2</v>
       </c>
       <c r="B137" s="137" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C137" s="136" t="s">
         <v>68</v>
@@ -16619,7 +16619,7 @@
         <v>2</v>
       </c>
       <c r="B138" s="137" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C138" s="136" t="s">
         <v>61</v>
@@ -17736,12 +17736,12 @@
     <mergeCell ref="F142:G142"/>
   </mergeCells>
   <conditionalFormatting sqref="M118:M124 R118:T124 M24:M56 R24:T56 S127:T127 M127 R58:T115 M58:M115">
-    <cfRule type="expression" dxfId="20" priority="63">
+    <cfRule type="expression" dxfId="113" priority="63">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="19" priority="56">
+    <cfRule type="expression" dxfId="112" priority="56">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17758,7 +17758,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="18" priority="50">
+    <cfRule type="expression" dxfId="111" priority="50">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17787,7 +17787,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="17" priority="48">
+    <cfRule type="expression" dxfId="110" priority="48">
       <formula>M114=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17804,12 +17804,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="16" priority="45">
+    <cfRule type="expression" dxfId="109" priority="45">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="15" priority="44">
+    <cfRule type="expression" dxfId="108" priority="44">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17838,12 +17838,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="14" priority="42">
+    <cfRule type="expression" dxfId="107" priority="42">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="13" priority="41">
+    <cfRule type="expression" dxfId="106" priority="41">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17860,17 +17860,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="12" priority="39">
+    <cfRule type="expression" dxfId="105" priority="39">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="11" priority="24">
+    <cfRule type="expression" dxfId="104" priority="24">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="10" priority="26">
+    <cfRule type="expression" dxfId="103" priority="26">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17887,12 +17887,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="9" priority="19">
+    <cfRule type="expression" dxfId="102" priority="19">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="8" priority="20">
+    <cfRule type="expression" dxfId="101" priority="20">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17921,12 +17921,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="7" priority="17">
+    <cfRule type="expression" dxfId="100" priority="17">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="99" priority="12">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17943,12 +17943,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="5" priority="14">
+    <cfRule type="expression" dxfId="98" priority="14">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="97" priority="7">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17965,12 +17965,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="96" priority="9">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="95" priority="5">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17987,7 +17987,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="94" priority="3">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18004,7 +18004,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="93" priority="1">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added an sku for MexicanPepper collectible
Former-commit-id: 7825649bfe50423d970e612f892db12aa287a592
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$143:$O$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$144:$O$145</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="504">
   <si>
     <t>tier_4</t>
   </si>
@@ -1551,12 +1551,15 @@
   <si>
     <t>StarSky</t>
   </si>
+  <si>
+    <t>MexicanPepper</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1658,8 +1661,46 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1777,6 +1818,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2095,7 +2142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2393,43 +2440,10 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2538,12 +2552,212 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="114">
+  <dxfs count="115">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4839,153 +5053,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5000,114 +5067,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF138" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF138"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF139" totalsRowShown="0" headerRowDxfId="114" dataDxfId="112" headerRowBorderDxfId="113" tableBorderDxfId="111" totalsRowBorderDxfId="110">
+  <autoFilter ref="A23:AF139"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="109"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="108"/>
+    <tableColumn id="6" name="[category]" dataDxfId="107"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="106"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="105"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="104"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="103"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="102"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="101"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="100"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="99"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="98"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="97"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="96"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="95"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="94"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="93"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="92"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="91"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="90"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="89"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="88"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="87"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="86"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="85"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="84"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="83"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="82"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="81"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="80"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="79"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75" totalsRowBorderDxfId="74">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="73"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A143:O155" totalsRowShown="0">
-  <autoFilter ref="A143:O155"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A144:O156" totalsRowShown="0">
+  <autoFilter ref="A144:O156"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="4" name="[category]" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="16" name="[size]" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="43" totalsRowDxfId="42"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="37"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="36"/>
+    <tableColumn id="6" name="[order]" dataDxfId="35"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="34"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="33"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="32"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="23"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="22" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5379,12 +5446,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF172"/>
+  <dimension ref="A1:AF173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="B138" sqref="B138"/>
+      <selection pane="topRight" activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5428,8 +5495,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5593,8 +5660,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="170"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="159"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -5710,13 +5777,13 @@
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A24" s="135" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="135" t="s">
+      <c r="A24" s="124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="124" t="s">
         <v>353</v>
       </c>
-      <c r="C24" s="136" t="s">
+      <c r="C24" s="125" t="s">
         <v>87</v>
       </c>
       <c r="D24" s="66">
@@ -5808,13 +5875,13 @@
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A25" s="135" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="135" t="s">
+      <c r="A25" s="124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="124" t="s">
         <v>347</v>
       </c>
-      <c r="C25" s="136" t="s">
+      <c r="C25" s="125" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="66">
@@ -5906,13 +5973,13 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A26" s="135" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="135" t="s">
+      <c r="A26" s="124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="124" t="s">
         <v>342</v>
       </c>
-      <c r="C26" s="136" t="s">
+      <c r="C26" s="125" t="s">
         <v>87</v>
       </c>
       <c r="D26" s="66">
@@ -6004,13 +6071,13 @@
       </c>
     </row>
     <row r="27" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="135" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="135" t="s">
+      <c r="A27" s="124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="124" t="s">
         <v>339</v>
       </c>
-      <c r="C27" s="136" t="s">
+      <c r="C27" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D27" s="66">
@@ -6488,13 +6555,13 @@
       <c r="AF31" s="79"/>
     </row>
     <row r="32" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="135" t="s">
+      <c r="A32" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="124" t="s">
         <v>321</v>
       </c>
-      <c r="C32" s="136" t="s">
+      <c r="C32" s="125" t="s">
         <v>87</v>
       </c>
       <c r="D32" s="66">
@@ -6582,13 +6649,13 @@
       <c r="AF32" s="71"/>
     </row>
     <row r="33" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="135" t="s">
+      <c r="A33" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="124" t="s">
         <v>320</v>
       </c>
-      <c r="C33" s="136" t="s">
+      <c r="C33" s="125" t="s">
         <v>68</v>
       </c>
       <c r="D33" s="66">
@@ -6681,13 +6748,13 @@
       </c>
     </row>
     <row r="34" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="137" t="s">
+      <c r="A34" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="126" t="s">
         <v>432</v>
       </c>
-      <c r="C34" s="138" t="s">
+      <c r="C34" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D34" s="66">
@@ -6775,13 +6842,13 @@
       <c r="AF34" s="71"/>
     </row>
     <row r="35" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="137" t="s">
+      <c r="A35" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="126" t="s">
         <v>441</v>
       </c>
-      <c r="C35" s="138" t="s">
+      <c r="C35" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D35" s="66">
@@ -7155,7 +7222,7 @@
       <c r="AF38" s="79"/>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A39" s="151" t="s">
+      <c r="A39" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="49" t="s">
@@ -7250,13 +7317,13 @@
       <c r="AF39" s="79"/>
     </row>
     <row r="40" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="135" t="s">
+      <c r="A40" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="136" t="s">
+      <c r="C40" s="125" t="s">
         <v>66</v>
       </c>
       <c r="D40" s="66">
@@ -7344,13 +7411,13 @@
       <c r="AF40" s="71"/>
     </row>
     <row r="41" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="135" t="s">
+      <c r="A41" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="124" t="s">
         <v>443</v>
       </c>
-      <c r="C41" s="136" t="s">
+      <c r="C41" s="125" t="s">
         <v>66</v>
       </c>
       <c r="D41" s="66">
@@ -7438,13 +7505,13 @@
       <c r="AF41" s="71"/>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A42" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="137" t="s">
+      <c r="A42" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="126" t="s">
         <v>302</v>
       </c>
-      <c r="C42" s="138" t="s">
+      <c r="C42" s="127" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="66">
@@ -7532,13 +7599,13 @@
       <c r="AF42" s="71"/>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A43" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="137" t="s">
+      <c r="A43" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="126" t="s">
         <v>434</v>
       </c>
-      <c r="C43" s="138" t="s">
+      <c r="C43" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D43" s="66">
@@ -7720,7 +7787,7 @@
       <c r="AE44" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF44" s="150" t="s">
+      <c r="AF44" s="139" t="s">
         <v>287</v>
       </c>
     </row>
@@ -7917,7 +7984,7 @@
       </c>
     </row>
     <row r="47" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="151" t="s">
+      <c r="A47" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="49" t="s">
@@ -8012,13 +8079,13 @@
       <c r="AF47" s="74"/>
     </row>
     <row r="48" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="135" t="s">
+      <c r="A48" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="124" t="s">
         <v>290</v>
       </c>
-      <c r="C48" s="136" t="s">
+      <c r="C48" s="125" t="s">
         <v>68</v>
       </c>
       <c r="D48" s="66">
@@ -8110,13 +8177,13 @@
       </c>
     </row>
     <row r="49" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="135" t="s">
+      <c r="A49" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="124" t="s">
         <v>286</v>
       </c>
-      <c r="C49" s="136" t="s">
+      <c r="C49" s="125" t="s">
         <v>87</v>
       </c>
       <c r="D49" s="66">
@@ -8204,13 +8271,13 @@
       <c r="AF49" s="71"/>
     </row>
     <row r="50" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" s="137" t="s">
+      <c r="A50" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="126" t="s">
         <v>282</v>
       </c>
-      <c r="C50" s="138" t="s">
+      <c r="C50" s="127" t="s">
         <v>273</v>
       </c>
       <c r="D50" s="66">
@@ -8302,13 +8369,13 @@
       </c>
     </row>
     <row r="51" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="137" t="s">
+      <c r="A51" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="126" t="s">
         <v>280</v>
       </c>
-      <c r="C51" s="138" t="s">
+      <c r="C51" s="127" t="s">
         <v>273</v>
       </c>
       <c r="D51" s="66">
@@ -8596,7 +8663,7 @@
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A54" s="151" t="s">
+      <c r="A54" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="49" t="s">
@@ -8694,7 +8761,7 @@
       </c>
     </row>
     <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="151" t="s">
+      <c r="A55" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="49" t="s">
@@ -8789,13 +8856,13 @@
       <c r="AF55" s="74"/>
     </row>
     <row r="56" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="135" t="s">
+      <c r="A56" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="124" t="s">
         <v>265</v>
       </c>
-      <c r="C56" s="136" t="s">
+      <c r="C56" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D56" s="66">
@@ -8883,14 +8950,14 @@
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
     </row>
-    <row r="57" spans="1:32" s="166" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="135" t="s">
+    <row r="57" spans="1:32" s="155" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="124" t="s">
         <v>448</v>
       </c>
-      <c r="C57" s="136" t="s">
+      <c r="C57" s="125" t="s">
         <v>449</v>
       </c>
       <c r="D57" s="66">
@@ -8972,13 +9039,13 @@
       <c r="AF57" s="71"/>
     </row>
     <row r="58" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" s="137" t="s">
+      <c r="A58" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="126" t="s">
         <v>431</v>
       </c>
-      <c r="C58" s="138" t="s">
+      <c r="C58" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D58" s="66">
@@ -9067,13 +9134,13 @@
       <c r="AF58" s="80"/>
     </row>
     <row r="59" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" s="137" t="s">
+      <c r="A59" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="126" t="s">
         <v>263</v>
       </c>
-      <c r="C59" s="138" t="s">
+      <c r="C59" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D59" s="66">
@@ -9351,7 +9418,7 @@
       <c r="AF61" s="74"/>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A62" s="151" t="s">
+      <c r="A62" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B62" s="49" t="s">
@@ -9446,7 +9513,7 @@
       <c r="AF62" s="74"/>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A63" s="151" t="s">
+      <c r="A63" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B63" s="49" t="s">
@@ -9541,13 +9608,13 @@
       <c r="AF63" s="74"/>
     </row>
     <row r="64" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B64" s="135" t="s">
+      <c r="A64" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="124" t="s">
         <v>253</v>
       </c>
-      <c r="C64" s="136" t="s">
+      <c r="C64" s="125" t="s">
         <v>61</v>
       </c>
       <c r="D64" s="66">
@@ -9636,13 +9703,13 @@
       <c r="AF64" s="80"/>
     </row>
     <row r="65" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B65" s="135" t="s">
+      <c r="A65" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="124" t="s">
         <v>249</v>
       </c>
-      <c r="C65" s="136" t="s">
+      <c r="C65" s="125" t="s">
         <v>61</v>
       </c>
       <c r="D65" s="66">
@@ -9726,16 +9793,16 @@
         <v>150</v>
       </c>
       <c r="AE65" s="63"/>
-      <c r="AF65" s="149"/>
+      <c r="AF65" s="138"/>
     </row>
     <row r="66" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="137" t="s">
+      <c r="A66" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="126" t="s">
         <v>244</v>
       </c>
-      <c r="C66" s="138" t="s">
+      <c r="C66" s="127" t="s">
         <v>66</v>
       </c>
       <c r="D66" s="66">
@@ -9828,13 +9895,13 @@
       </c>
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A67" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="137" t="s">
+      <c r="A67" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="126" t="s">
         <v>242</v>
       </c>
-      <c r="C67" s="138" t="s">
+      <c r="C67" s="127" t="s">
         <v>66</v>
       </c>
       <c r="D67" s="66">
@@ -10026,7 +10093,7 @@
       </c>
     </row>
     <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="151" t="s">
+      <c r="A69" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B69" s="49" t="s">
@@ -10124,7 +10191,7 @@
       </c>
     </row>
     <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="151" t="s">
+      <c r="A70" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B70" s="49" t="s">
@@ -10219,7 +10286,7 @@
       <c r="AF70" s="79"/>
     </row>
     <row r="71" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="151" t="s">
+      <c r="A71" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B71" s="49" t="s">
@@ -10314,13 +10381,13 @@
       <c r="AF71" s="79"/>
     </row>
     <row r="72" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" s="135" t="s">
+      <c r="A72" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="124" t="s">
         <v>230</v>
       </c>
-      <c r="C72" s="136" t="s">
+      <c r="C72" s="125" t="s">
         <v>229</v>
       </c>
       <c r="D72" s="66">
@@ -10407,18 +10474,18 @@
       <c r="AE72" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="AF72" s="149" t="s">
+      <c r="AF72" s="138" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="135" t="s">
+      <c r="A73" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="124" t="s">
         <v>225</v>
       </c>
-      <c r="C73" s="136" t="s">
+      <c r="C73" s="125" t="s">
         <v>61</v>
       </c>
       <c r="D73" s="66">
@@ -10505,13 +10572,13 @@
       <c r="AF73" s="63"/>
     </row>
     <row r="74" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="137" t="s">
+      <c r="A74" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="126" t="s">
         <v>223</v>
       </c>
-      <c r="C74" s="138" t="s">
+      <c r="C74" s="127" t="s">
         <v>61</v>
       </c>
       <c r="D74" s="66">
@@ -10595,16 +10662,16 @@
         <v>58</v>
       </c>
       <c r="AE74" s="63"/>
-      <c r="AF74" s="149"/>
+      <c r="AF74" s="138"/>
     </row>
     <row r="75" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="137" t="s">
+      <c r="A75" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="126" t="s">
         <v>221</v>
       </c>
-      <c r="C75" s="138" t="s">
+      <c r="C75" s="127" t="s">
         <v>66</v>
       </c>
       <c r="D75" s="66">
@@ -10696,7 +10763,7 @@
       </c>
     </row>
     <row r="76" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="151" t="s">
+      <c r="A76" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B76" s="49" t="s">
@@ -10792,7 +10859,7 @@
       <c r="AF76" s="68"/>
     </row>
     <row r="77" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="151" t="s">
+      <c r="A77" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B77" s="49" t="s">
@@ -10885,7 +10952,7 @@
       <c r="AE77" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF77" s="169" t="s">
+      <c r="AF77" s="158" t="s">
         <v>213</v>
       </c>
     </row>
@@ -10984,7 +11051,7 @@
       <c r="AE78" s="68" t="s">
         <v>207</v>
       </c>
-      <c r="AF78" s="169" t="s">
+      <c r="AF78" s="158" t="s">
         <v>206</v>
       </c>
     </row>
@@ -11083,13 +11150,13 @@
       <c r="AF79" s="74"/>
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A80" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="135" t="s">
+      <c r="A80" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="124" t="s">
         <v>429</v>
       </c>
-      <c r="C80" s="136" t="s">
+      <c r="C80" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D80" s="66">
@@ -11175,16 +11242,16 @@
         <v>98</v>
       </c>
       <c r="AE80" s="63"/>
-      <c r="AF80" s="134"/>
+      <c r="AF80" s="123"/>
     </row>
     <row r="81" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A81" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81" s="135" t="s">
+      <c r="A81" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="124" t="s">
         <v>430</v>
       </c>
-      <c r="C81" s="136" t="s">
+      <c r="C81" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D81" s="66">
@@ -11273,13 +11340,13 @@
       <c r="AF81" s="71"/>
     </row>
     <row r="82" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A82" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82" s="137" t="s">
+      <c r="A82" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="126" t="s">
         <v>436</v>
       </c>
-      <c r="C82" s="138" t="s">
+      <c r="C82" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D82" s="66">
@@ -11366,18 +11433,18 @@
       <c r="AE82" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="AF82" s="134" t="s">
+      <c r="AF82" s="123" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A83" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" s="137" t="s">
+      <c r="A83" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="126" t="s">
         <v>205</v>
       </c>
-      <c r="C83" s="138" t="s">
+      <c r="C83" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D83" s="66">
@@ -11462,10 +11529,10 @@
         <v>192</v>
       </c>
       <c r="AE83" s="63"/>
-      <c r="AF83" s="134"/>
+      <c r="AF83" s="123"/>
     </row>
     <row r="84" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="151" t="s">
+      <c r="A84" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B84" s="49" t="s">
@@ -11760,7 +11827,7 @@
       </c>
     </row>
     <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="151" t="s">
+      <c r="A87" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B87" s="49" t="s">
@@ -11858,13 +11925,13 @@
       </c>
     </row>
     <row r="88" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A88" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88" s="135" t="s">
+      <c r="A88" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="124" t="s">
         <v>191</v>
       </c>
-      <c r="C88" s="136" t="s">
+      <c r="C88" s="125" t="s">
         <v>24</v>
       </c>
       <c r="D88" s="66">
@@ -11952,18 +12019,18 @@
       <c r="AE88" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="AF88" s="142" t="s">
+      <c r="AF88" s="131" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="135" t="s">
+      <c r="A89" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="124" t="s">
         <v>189</v>
       </c>
-      <c r="C89" s="136" t="s">
+      <c r="C89" s="125" t="s">
         <v>24</v>
       </c>
       <c r="D89" s="66">
@@ -12002,7 +12069,7 @@
       <c r="O89" s="32">
         <v>5</v>
       </c>
-      <c r="P89" s="145">
+      <c r="P89" s="134">
         <v>5</v>
       </c>
       <c r="Q89" s="32">
@@ -12050,18 +12117,18 @@
       <c r="AE89" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="AF89" s="147" t="s">
+      <c r="AF89" s="136" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="90" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="137" t="s">
+      <c r="A90" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="126" t="s">
         <v>188</v>
       </c>
-      <c r="C90" s="138" t="s">
+      <c r="C90" s="127" t="s">
         <v>24</v>
       </c>
       <c r="D90" s="66">
@@ -12100,7 +12167,7 @@
       <c r="O90" s="32">
         <v>5</v>
       </c>
-      <c r="P90" s="145">
+      <c r="P90" s="134">
         <v>4</v>
       </c>
       <c r="Q90" s="32">
@@ -12148,18 +12215,18 @@
       <c r="AE90" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="AF90" s="147" t="s">
+      <c r="AF90" s="136" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" s="137" t="s">
+      <c r="A91" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="126" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="138" t="s">
+      <c r="C91" s="127" t="s">
         <v>24</v>
       </c>
       <c r="D91" s="66">
@@ -12198,7 +12265,7 @@
       <c r="O91" s="32">
         <v>5</v>
       </c>
-      <c r="P91" s="145">
+      <c r="P91" s="134">
         <v>5</v>
       </c>
       <c r="Q91" s="32">
@@ -12246,7 +12313,7 @@
       <c r="AE91" s="34" t="s">
         <v>499</v>
       </c>
-      <c r="AF91" s="147" t="s">
+      <c r="AF91" s="136" t="s">
         <v>178</v>
       </c>
     </row>
@@ -12533,7 +12600,7 @@
       <c r="AF94" s="43"/>
     </row>
     <row r="95" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="151" t="s">
+      <c r="A95" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B95" s="49" t="s">
@@ -12578,14 +12645,14 @@
       <c r="O95" s="32">
         <v>5</v>
       </c>
-      <c r="P95" s="145">
+      <c r="P95" s="134">
         <v>0</v>
       </c>
       <c r="Q95" s="32">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>0</v>
       </c>
-      <c r="R95" s="157" t="b">
+      <c r="R95" s="146" t="b">
         <v>1</v>
       </c>
       <c r="S95" s="28" t="b">
@@ -12628,13 +12695,13 @@
       <c r="AF95" s="43"/>
     </row>
     <row r="96" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B96" s="135" t="s">
+      <c r="A96" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="124" t="s">
         <v>169</v>
       </c>
-      <c r="C96" s="136" t="s">
+      <c r="C96" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D96" s="66">
@@ -12721,18 +12788,18 @@
       <c r="AE96" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="AF96" s="147" t="s">
+      <c r="AF96" s="136" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B97" s="135" t="s">
+      <c r="A97" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="124" t="s">
         <v>438</v>
       </c>
-      <c r="C97" s="136" t="s">
+      <c r="C97" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D97" s="66">
@@ -12819,18 +12886,18 @@
       <c r="AE97" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="AF97" s="147" t="s">
+      <c r="AF97" s="136" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="98" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B98" s="137" t="s">
+      <c r="A98" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="126" t="s">
         <v>165</v>
       </c>
-      <c r="C98" s="138" t="s">
+      <c r="C98" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D98" s="66">
@@ -12918,13 +12985,13 @@
       <c r="AF98" s="62"/>
     </row>
     <row r="99" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A99" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B99" s="137" t="s">
+      <c r="A99" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="126" t="s">
         <v>161</v>
       </c>
-      <c r="C99" s="138" t="s">
+      <c r="C99" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D99" s="66">
@@ -13010,7 +13077,7 @@
         <v>158</v>
       </c>
       <c r="AE99" s="34"/>
-      <c r="AF99" s="142"/>
+      <c r="AF99" s="131"/>
     </row>
     <row r="100" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A100" s="49" t="s">
@@ -13157,7 +13224,7 @@
       <c r="O101" s="32">
         <v>5</v>
       </c>
-      <c r="P101" s="145">
+      <c r="P101" s="134">
         <v>0</v>
       </c>
       <c r="Q101" s="32">
@@ -13300,7 +13367,7 @@
       <c r="AF102" s="59"/>
     </row>
     <row r="103" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="151" t="s">
+      <c r="A103" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B103" s="49" t="s">
@@ -13339,13 +13406,13 @@
       <c r="M103" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="N103" s="148">
+      <c r="N103" s="137">
         <v>5</v>
       </c>
       <c r="O103" s="32">
         <v>5</v>
       </c>
-      <c r="P103" s="145">
+      <c r="P103" s="134">
         <v>2</v>
       </c>
       <c r="Q103" s="32">
@@ -13395,7 +13462,7 @@
       <c r="AF103" s="56"/>
     </row>
     <row r="104" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="151" t="s">
+      <c r="A104" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B104" s="49" t="s">
@@ -13489,13 +13556,13 @@
       <c r="AF104" s="59"/>
     </row>
     <row r="105" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A105" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="135" t="s">
+      <c r="A105" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="C105" s="136" t="s">
+      <c r="C105" s="125" t="s">
         <v>66</v>
       </c>
       <c r="D105" s="66">
@@ -13582,18 +13649,18 @@
       <c r="AE105" s="34" t="s">
         <v>470</v>
       </c>
-      <c r="AF105" s="142" t="s">
+      <c r="AF105" s="131" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A106" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="135" t="s">
+      <c r="A106" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="124" t="s">
         <v>147</v>
       </c>
-      <c r="C106" s="136" t="s">
+      <c r="C106" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D106" s="66">
@@ -13632,7 +13699,7 @@
       <c r="O106" s="32">
         <v>0</v>
       </c>
-      <c r="P106" s="145">
+      <c r="P106" s="134">
         <v>1</v>
       </c>
       <c r="Q106" s="32">
@@ -13644,7 +13711,7 @@
       <c r="S106" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="T106" s="146" t="b">
+      <c r="T106" s="135" t="b">
         <v>0</v>
       </c>
       <c r="U106" s="36">
@@ -13678,16 +13745,16 @@
         <v>144</v>
       </c>
       <c r="AE106" s="34"/>
-      <c r="AF106" s="147"/>
+      <c r="AF106" s="136"/>
     </row>
     <row r="107" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A107" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="137" t="s">
+      <c r="A107" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="126" t="s">
         <v>143</v>
       </c>
-      <c r="C107" s="138" t="s">
+      <c r="C107" s="127" t="s">
         <v>87</v>
       </c>
       <c r="D107" s="66">
@@ -13726,7 +13793,7 @@
       <c r="O107" s="32">
         <v>2</v>
       </c>
-      <c r="P107" s="145">
+      <c r="P107" s="134">
         <v>3</v>
       </c>
       <c r="Q107" s="32">
@@ -13738,7 +13805,7 @@
       <c r="S107" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="T107" s="146" t="b">
+      <c r="T107" s="135" t="b">
         <v>0</v>
       </c>
       <c r="U107" s="36">
@@ -13772,16 +13839,16 @@
         <v>71</v>
       </c>
       <c r="AE107" s="34"/>
-      <c r="AF107" s="142"/>
+      <c r="AF107" s="131"/>
     </row>
     <row r="108" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A108" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B108" s="137" t="s">
+      <c r="A108" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="126" t="s">
         <v>142</v>
       </c>
-      <c r="C108" s="138" t="s">
+      <c r="C108" s="127" t="s">
         <v>66</v>
       </c>
       <c r="D108" s="66">
@@ -13820,7 +13887,7 @@
       <c r="O108" s="32">
         <v>5</v>
       </c>
-      <c r="P108" s="145">
+      <c r="P108" s="134">
         <v>2</v>
       </c>
       <c r="Q108" s="32">
@@ -13867,7 +13934,7 @@
         <v>21</v>
       </c>
       <c r="AE108" s="34"/>
-      <c r="AF108" s="147"/>
+      <c r="AF108" s="136"/>
     </row>
     <row r="109" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A109" s="49" t="s">
@@ -14063,40 +14130,40 @@
       <c r="AF110" s="43"/>
     </row>
     <row r="111" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A111" s="152" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" s="154" t="s">
+      <c r="A111" s="141" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="143" t="s">
         <v>135</v>
       </c>
-      <c r="C111" s="155" t="s">
+      <c r="C111" s="144" t="s">
         <v>87</v>
       </c>
-      <c r="D111" s="156">
+      <c r="D111" s="145">
         <v>120</v>
       </c>
-      <c r="E111" s="156">
+      <c r="E111" s="145">
         <v>17</v>
       </c>
-      <c r="F111" s="156">
-        <v>0</v>
-      </c>
-      <c r="G111" s="156">
+      <c r="F111" s="145">
+        <v>0</v>
+      </c>
+      <c r="G111" s="145">
         <v>50</v>
       </c>
-      <c r="H111" s="156">
-        <v>0</v>
-      </c>
-      <c r="I111" s="156">
+      <c r="H111" s="145">
+        <v>0</v>
+      </c>
+      <c r="I111" s="145">
         <v>70</v>
       </c>
-      <c r="J111" s="156">
+      <c r="J111" s="145">
         <v>0</v>
       </c>
       <c r="K111" s="42">
         <v>0.15</v>
       </c>
-      <c r="L111" s="156">
+      <c r="L111" s="145">
         <v>0</v>
       </c>
       <c r="M111" s="27" t="b">
@@ -14161,40 +14228,40 @@
       </c>
     </row>
     <row r="112" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A112" s="152" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="154" t="s">
+      <c r="A112" s="141" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="143" t="s">
         <v>129</v>
       </c>
-      <c r="C112" s="155" t="s">
+      <c r="C112" s="144" t="s">
         <v>68</v>
       </c>
-      <c r="D112" s="156">
+      <c r="D112" s="145">
         <v>60</v>
       </c>
-      <c r="E112" s="156">
+      <c r="E112" s="145">
         <v>17</v>
       </c>
-      <c r="F112" s="156">
-        <v>0</v>
-      </c>
-      <c r="G112" s="156">
+      <c r="F112" s="145">
+        <v>0</v>
+      </c>
+      <c r="G112" s="145">
         <v>30</v>
       </c>
-      <c r="H112" s="156">
-        <v>0</v>
-      </c>
-      <c r="I112" s="156">
+      <c r="H112" s="145">
+        <v>0</v>
+      </c>
+      <c r="I112" s="145">
         <v>75</v>
       </c>
-      <c r="J112" s="156">
+      <c r="J112" s="145">
         <v>0</v>
       </c>
       <c r="K112" s="42">
         <v>0.15</v>
       </c>
-      <c r="L112" s="156">
+      <c r="L112" s="145">
         <v>0</v>
       </c>
       <c r="M112" s="27" t="b">
@@ -14259,13 +14326,13 @@
       </c>
     </row>
     <row r="113" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A113" s="140" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" s="153" t="s">
+      <c r="A113" s="129" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="C113" s="141" t="s">
+      <c r="C113" s="130" t="s">
         <v>82</v>
       </c>
       <c r="D113" s="66">
@@ -14353,18 +14420,18 @@
       <c r="AE113" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="AF113" s="147" t="s">
+      <c r="AF113" s="136" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A114" s="140" t="s">
-        <v>2</v>
-      </c>
-      <c r="B114" s="153" t="s">
+      <c r="A114" s="129" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="142" t="s">
         <v>118</v>
       </c>
-      <c r="C114" s="141" t="s">
+      <c r="C114" s="130" t="s">
         <v>82</v>
       </c>
       <c r="D114" s="38">
@@ -14452,18 +14519,18 @@
       <c r="AE114" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="AF114" s="147" t="s">
+      <c r="AF114" s="136" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A115" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" s="137" t="s">
+      <c r="A115" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="138" t="s">
+      <c r="C115" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D115" s="66">
@@ -14549,16 +14616,16 @@
         <v>109</v>
       </c>
       <c r="AE115" s="34"/>
-      <c r="AF115" s="147"/>
+      <c r="AF115" s="136"/>
     </row>
     <row r="116" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A116" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="B116" s="137" t="s">
+      <c r="A116" s="126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="126" t="s">
         <v>108</v>
       </c>
-      <c r="C116" s="138" t="s">
+      <c r="C116" s="127" t="s">
         <v>82</v>
       </c>
       <c r="D116" s="66">
@@ -14644,7 +14711,7 @@
         <v>105</v>
       </c>
       <c r="AE116" s="34"/>
-      <c r="AF116" s="147"/>
+      <c r="AF116" s="136"/>
     </row>
     <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" s="49" t="s">
@@ -14742,7 +14809,7 @@
       <c r="AF117" s="43"/>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A118" s="151" t="s">
+      <c r="A118" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B118" s="49" t="s">
@@ -14837,7 +14904,7 @@
       <c r="AF118" s="74"/>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A119" s="151" t="s">
+      <c r="A119" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B119" s="49" t="s">
@@ -14930,12 +14997,12 @@
       <c r="AE119" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="AF119" s="169" t="s">
+      <c r="AF119" s="158" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="120" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A120" s="151" t="s">
+      <c r="A120" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B120" s="49" t="s">
@@ -15029,13 +15096,13 @@
       <c r="AF120" s="74"/>
     </row>
     <row r="121" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A121" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B121" s="137" t="s">
+      <c r="A121" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="126" t="s">
         <v>88</v>
       </c>
-      <c r="C121" s="136" t="s">
+      <c r="C121" s="125" t="s">
         <v>87</v>
       </c>
       <c r="D121" s="66">
@@ -15123,13 +15190,13 @@
       <c r="AF121" s="63"/>
     </row>
     <row r="122" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A122" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B122" s="137" t="s">
+      <c r="A122" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="126" t="s">
         <v>83</v>
       </c>
-      <c r="C122" s="136" t="s">
+      <c r="C122" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D122" s="66">
@@ -15218,13 +15285,13 @@
       <c r="AF122" s="72"/>
     </row>
     <row r="123" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A123" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B123" s="137" t="s">
+      <c r="A123" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="126" t="s">
         <v>79</v>
       </c>
-      <c r="C123" s="136" t="s">
+      <c r="C123" s="125" t="s">
         <v>66</v>
       </c>
       <c r="D123" s="66">
@@ -15311,18 +15378,18 @@
       <c r="AE123" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="AF123" s="134" t="s">
+      <c r="AF123" s="123" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="124" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A124" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B124" s="137" t="s">
+      <c r="A124" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="126" t="s">
         <v>70</v>
       </c>
-      <c r="C124" s="136" t="s">
+      <c r="C124" s="125" t="s">
         <v>68</v>
       </c>
       <c r="D124" s="66">
@@ -15385,16 +15452,16 @@
       <c r="W124" s="27">
         <v>0</v>
       </c>
-      <c r="X124" s="158">
+      <c r="X124" s="147">
         <v>0.25</v>
       </c>
-      <c r="Y124" s="158">
+      <c r="Y124" s="147">
         <v>0.25</v>
       </c>
-      <c r="Z124" s="158">
+      <c r="Z124" s="147">
         <v>0.8</v>
       </c>
-      <c r="AA124" s="158">
+      <c r="AA124" s="147">
         <v>0</v>
       </c>
       <c r="AB124" s="35" t="s">
@@ -15410,7 +15477,7 @@
       <c r="AF124" s="24"/>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A125" s="151" t="s">
+      <c r="A125" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B125" s="49" t="s">
@@ -15504,7 +15571,7 @@
       <c r="AF125" s="79"/>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A126" s="151" t="s">
+      <c r="A126" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B126" s="49" t="s">
@@ -15598,7 +15665,7 @@
       <c r="AF126" s="74"/>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A127" s="151" t="s">
+      <c r="A127" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B127" s="49" t="s">
@@ -15652,32 +15719,32 @@
       <c r="R127" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S127" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="T127" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="U127" s="159">
-        <v>1</v>
-      </c>
-      <c r="V127" s="159"/>
-      <c r="W127" s="159">
+      <c r="S127" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="T127" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="U127" s="148">
+        <v>1</v>
+      </c>
+      <c r="V127" s="148"/>
+      <c r="W127" s="148">
         <v>0</v>
       </c>
       <c r="X127" s="55">
         <v>0</v>
       </c>
-      <c r="Y127" s="160">
-        <v>0</v>
-      </c>
-      <c r="Z127" s="160">
+      <c r="Y127" s="149">
+        <v>0</v>
+      </c>
+      <c r="Z127" s="149">
         <v>0</v>
       </c>
       <c r="AA127" s="55">
         <v>0</v>
       </c>
-      <c r="AB127" s="164" t="s">
+      <c r="AB127" s="153" t="s">
         <v>224</v>
       </c>
       <c r="AC127" s="72" t="s">
@@ -15686,11 +15753,11 @@
       <c r="AD127" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE127" s="161"/>
-      <c r="AF127" s="162"/>
+      <c r="AE127" s="150"/>
+      <c r="AF127" s="151"/>
     </row>
     <row r="128" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="151" t="s">
+      <c r="A128" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B128" s="49" t="s">
@@ -15744,32 +15811,32 @@
       <c r="R128" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S128" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="T128" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="U128" s="159">
-        <v>1</v>
-      </c>
-      <c r="V128" s="159"/>
-      <c r="W128" s="159">
+      <c r="S128" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="T128" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="U128" s="148">
+        <v>1</v>
+      </c>
+      <c r="V128" s="148"/>
+      <c r="W128" s="148">
         <v>0</v>
       </c>
       <c r="X128" s="55">
         <v>0</v>
       </c>
-      <c r="Y128" s="160">
-        <v>0</v>
-      </c>
-      <c r="Z128" s="160">
+      <c r="Y128" s="149">
+        <v>0</v>
+      </c>
+      <c r="Z128" s="149">
         <v>0</v>
       </c>
       <c r="AA128" s="55">
         <v>0</v>
       </c>
-      <c r="AB128" s="164" t="s">
+      <c r="AB128" s="153" t="s">
         <v>224</v>
       </c>
       <c r="AC128" s="72" t="s">
@@ -15778,17 +15845,17 @@
       <c r="AD128" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE128" s="161"/>
-      <c r="AF128" s="162"/>
+      <c r="AE128" s="150"/>
+      <c r="AF128" s="151"/>
     </row>
     <row r="129" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A129" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B129" s="137" t="s">
+      <c r="A129" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="126" t="s">
         <v>491</v>
       </c>
-      <c r="C129" s="136" t="s">
+      <c r="C129" s="125" t="s">
         <v>61</v>
       </c>
       <c r="D129" s="66">
@@ -15861,7 +15928,7 @@
       <c r="AA129" s="52">
         <v>0</v>
       </c>
-      <c r="AB129" s="167" t="s">
+      <c r="AB129" s="156" t="s">
         <v>224</v>
       </c>
       <c r="AC129" s="72" t="s">
@@ -15874,13 +15941,13 @@
       <c r="AF129" s="63"/>
     </row>
     <row r="130" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A130" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B130" s="137" t="s">
+      <c r="A130" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" s="126" t="s">
         <v>492</v>
       </c>
-      <c r="C130" s="136" t="s">
+      <c r="C130" s="125" t="s">
         <v>61</v>
       </c>
       <c r="D130" s="66">
@@ -15953,7 +16020,7 @@
       <c r="AA130" s="52">
         <v>0</v>
       </c>
-      <c r="AB130" s="167" t="s">
+      <c r="AB130" s="156" t="s">
         <v>224</v>
       </c>
       <c r="AC130" s="72" t="s">
@@ -15966,13 +16033,13 @@
       <c r="AF130" s="72"/>
     </row>
     <row r="131" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A131" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B131" s="137" t="s">
+      <c r="A131" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="126" t="s">
         <v>493</v>
       </c>
-      <c r="C131" s="136" t="s">
+      <c r="C131" s="125" t="s">
         <v>61</v>
       </c>
       <c r="D131" s="66">
@@ -16045,7 +16112,7 @@
       <c r="AA131" s="52">
         <v>0</v>
       </c>
-      <c r="AB131" s="167" t="s">
+      <c r="AB131" s="156" t="s">
         <v>224</v>
       </c>
       <c r="AC131" s="72" t="s">
@@ -16058,13 +16125,13 @@
       <c r="AF131" s="71"/>
     </row>
     <row r="132" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A132" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B132" s="137" t="s">
+      <c r="A132" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="126" t="s">
         <v>494</v>
       </c>
-      <c r="C132" s="136" t="s">
+      <c r="C132" s="125" t="s">
         <v>61</v>
       </c>
       <c r="D132" s="66">
@@ -16125,19 +16192,19 @@
       <c r="W132" s="27">
         <v>0</v>
       </c>
-      <c r="X132" s="158">
-        <v>0</v>
-      </c>
-      <c r="Y132" s="158">
-        <v>0</v>
-      </c>
-      <c r="Z132" s="158">
-        <v>0</v>
-      </c>
-      <c r="AA132" s="158">
-        <v>0</v>
-      </c>
-      <c r="AB132" s="168" t="s">
+      <c r="X132" s="147">
+        <v>0</v>
+      </c>
+      <c r="Y132" s="147">
+        <v>0</v>
+      </c>
+      <c r="Z132" s="147">
+        <v>0</v>
+      </c>
+      <c r="AA132" s="147">
+        <v>0</v>
+      </c>
+      <c r="AB132" s="157" t="s">
         <v>224</v>
       </c>
       <c r="AC132" s="25" t="s">
@@ -16150,7 +16217,7 @@
       <c r="AF132" s="24"/>
     </row>
     <row r="133" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A133" s="151" t="s">
+      <c r="A133" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B133" s="49" t="s">
@@ -16204,32 +16271,32 @@
       <c r="R133" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S133" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="T133" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="U133" s="159">
-        <v>1</v>
-      </c>
-      <c r="V133" s="159"/>
-      <c r="W133" s="159">
+      <c r="S133" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="T133" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="U133" s="148">
+        <v>1</v>
+      </c>
+      <c r="V133" s="148"/>
+      <c r="W133" s="148">
         <v>0</v>
       </c>
       <c r="X133" s="55">
         <v>0</v>
       </c>
-      <c r="Y133" s="160">
-        <v>0</v>
-      </c>
-      <c r="Z133" s="160">
+      <c r="Y133" s="149">
+        <v>0</v>
+      </c>
+      <c r="Z133" s="149">
         <v>0</v>
       </c>
       <c r="AA133" s="55">
         <v>0</v>
       </c>
-      <c r="AB133" s="164" t="s">
+      <c r="AB133" s="153" t="s">
         <v>224</v>
       </c>
       <c r="AC133" s="72" t="s">
@@ -16238,11 +16305,11 @@
       <c r="AD133" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE133" s="161"/>
-      <c r="AF133" s="162"/>
+      <c r="AE133" s="150"/>
+      <c r="AF133" s="151"/>
     </row>
     <row r="134" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A134" s="151" t="s">
+      <c r="A134" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B134" s="49" t="s">
@@ -16260,7 +16327,7 @@
       <c r="F134" s="76">
         <v>0</v>
       </c>
-      <c r="G134" s="165">
+      <c r="G134" s="154">
         <v>-20</v>
       </c>
       <c r="H134" s="76">
@@ -16297,34 +16364,34 @@
       <c r="R134" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S134" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="T134" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="U134" s="159">
-        <v>1</v>
-      </c>
-      <c r="V134" s="159">
-        <v>2</v>
-      </c>
-      <c r="W134" s="159">
+      <c r="S134" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="T134" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="U134" s="148">
+        <v>1</v>
+      </c>
+      <c r="V134" s="148">
+        <v>2</v>
+      </c>
+      <c r="W134" s="148">
         <v>0</v>
       </c>
       <c r="X134" s="55">
         <v>1</v>
       </c>
-      <c r="Y134" s="160">
-        <v>1</v>
-      </c>
-      <c r="Z134" s="160">
+      <c r="Y134" s="149">
+        <v>1</v>
+      </c>
+      <c r="Z134" s="149">
         <v>0</v>
       </c>
       <c r="AA134" s="55">
         <v>0</v>
       </c>
-      <c r="AB134" s="164" t="s">
+      <c r="AB134" s="153" t="s">
         <v>338</v>
       </c>
       <c r="AC134" s="72" t="s">
@@ -16333,11 +16400,11 @@
       <c r="AD134" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="AE134" s="161"/>
-      <c r="AF134" s="162"/>
+      <c r="AE134" s="150"/>
+      <c r="AF134" s="151"/>
     </row>
     <row r="135" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A135" s="151" t="s">
+      <c r="A135" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B135" s="49" t="s">
@@ -16355,7 +16422,7 @@
       <c r="F135" s="76">
         <v>1</v>
       </c>
-      <c r="G135" s="165">
+      <c r="G135" s="154">
         <v>0</v>
       </c>
       <c r="H135" s="76">
@@ -16391,32 +16458,32 @@
       <c r="R135" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S135" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="T135" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="U135" s="159">
-        <v>1</v>
-      </c>
-      <c r="V135" s="159"/>
-      <c r="W135" s="159">
+      <c r="S135" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="T135" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="U135" s="148">
+        <v>1</v>
+      </c>
+      <c r="V135" s="148"/>
+      <c r="W135" s="148">
         <v>0</v>
       </c>
       <c r="X135" s="55">
         <v>0</v>
       </c>
-      <c r="Y135" s="160">
-        <v>0</v>
-      </c>
-      <c r="Z135" s="160">
+      <c r="Y135" s="149">
+        <v>0</v>
+      </c>
+      <c r="Z135" s="149">
         <v>0</v>
       </c>
       <c r="AA135" s="55">
         <v>0</v>
       </c>
-      <c r="AB135" s="164" t="s">
+      <c r="AB135" s="153" t="s">
         <v>224</v>
       </c>
       <c r="AC135" s="72" t="s">
@@ -16425,11 +16492,11 @@
       <c r="AD135" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE135" s="161"/>
-      <c r="AF135" s="162"/>
+      <c r="AE135" s="150"/>
+      <c r="AF135" s="151"/>
     </row>
     <row r="136" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A136" s="151" t="s">
+      <c r="A136" s="140" t="s">
         <v>2</v>
       </c>
       <c r="B136" s="49" t="s">
@@ -16447,7 +16514,7 @@
       <c r="F136" s="76">
         <v>0</v>
       </c>
-      <c r="G136" s="165">
+      <c r="G136" s="154">
         <v>0</v>
       </c>
       <c r="H136" s="76">
@@ -16483,32 +16550,32 @@
       <c r="R136" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S136" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="T136" s="163" t="b">
-        <v>0</v>
-      </c>
-      <c r="U136" s="159">
-        <v>1</v>
-      </c>
-      <c r="V136" s="159"/>
-      <c r="W136" s="159">
+      <c r="S136" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="T136" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="U136" s="148">
+        <v>1</v>
+      </c>
+      <c r="V136" s="148"/>
+      <c r="W136" s="148">
         <v>0</v>
       </c>
       <c r="X136" s="55">
         <v>0</v>
       </c>
-      <c r="Y136" s="160">
-        <v>0</v>
-      </c>
-      <c r="Z136" s="160">
+      <c r="Y136" s="149">
+        <v>0</v>
+      </c>
+      <c r="Z136" s="149">
         <v>0</v>
       </c>
       <c r="AA136" s="55">
         <v>0</v>
       </c>
-      <c r="AB136" s="164" t="s">
+      <c r="AB136" s="153" t="s">
         <v>224</v>
       </c>
       <c r="AC136" s="72" t="s">
@@ -16517,17 +16584,17 @@
       <c r="AD136" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE136" s="161"/>
-      <c r="AF136" s="162"/>
+      <c r="AE136" s="150"/>
+      <c r="AF136" s="151"/>
     </row>
     <row r="137" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A137" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B137" s="137" t="s">
+      <c r="A137" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" s="126" t="s">
         <v>501</v>
       </c>
-      <c r="C137" s="136" t="s">
+      <c r="C137" s="125" t="s">
         <v>68</v>
       </c>
       <c r="D137" s="66">
@@ -16590,16 +16657,16 @@
       <c r="W137" s="27">
         <v>0</v>
       </c>
-      <c r="X137" s="158">
+      <c r="X137" s="147">
         <v>0.25</v>
       </c>
-      <c r="Y137" s="158">
+      <c r="Y137" s="147">
         <v>0.25</v>
       </c>
-      <c r="Z137" s="158">
+      <c r="Z137" s="147">
         <v>0.8</v>
       </c>
-      <c r="AA137" s="158">
+      <c r="AA137" s="147">
         <v>0</v>
       </c>
       <c r="AB137" s="35" t="s">
@@ -16615,13 +16682,13 @@
       <c r="AF137" s="24"/>
     </row>
     <row r="138" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="B138" s="137" t="s">
+      <c r="A138" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="126" t="s">
         <v>502</v>
       </c>
-      <c r="C138" s="136" t="s">
+      <c r="C138" s="125" t="s">
         <v>61</v>
       </c>
       <c r="D138" s="66">
@@ -16694,7 +16761,7 @@
       <c r="AA138" s="52">
         <v>0</v>
       </c>
-      <c r="AB138" s="167" t="s">
+      <c r="AB138" s="156" t="s">
         <v>224</v>
       </c>
       <c r="AC138" s="72" t="s">
@@ -16707,216 +16774,262 @@
       <c r="AF138" s="71"/>
     </row>
     <row r="139" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A139" s="118"/>
-      <c r="B139" s="118"/>
-      <c r="C139" s="118"/>
-      <c r="D139" s="119"/>
-      <c r="E139" s="120"/>
-      <c r="F139" s="120"/>
-      <c r="G139" s="120"/>
-      <c r="H139" s="120"/>
-      <c r="I139" s="120"/>
-      <c r="J139" s="121"/>
-      <c r="K139" s="120"/>
-      <c r="L139" s="122"/>
-      <c r="M139" s="123"/>
-      <c r="N139" s="123"/>
-      <c r="O139" s="124"/>
-      <c r="P139" s="123"/>
-      <c r="Q139" s="125"/>
-      <c r="R139" s="126"/>
-      <c r="S139" s="126"/>
-      <c r="T139" s="125"/>
-      <c r="U139" s="126"/>
-      <c r="V139" s="127"/>
-      <c r="W139" s="128"/>
-      <c r="X139" s="129"/>
-      <c r="Y139" s="129"/>
-      <c r="Z139" s="130"/>
-      <c r="AA139" s="131"/>
-      <c r="AB139" s="131"/>
-      <c r="AC139" s="132"/>
-      <c r="AD139" s="132"/>
-      <c r="AE139" s="133"/>
-    </row>
-    <row r="140" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="141" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A141" s="9" t="s">
+      <c r="A139" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="126" t="s">
+        <v>503</v>
+      </c>
+      <c r="C139" s="125" t="s">
+        <v>61</v>
+      </c>
+      <c r="D139" s="66">
+        <v>20</v>
+      </c>
+      <c r="E139" s="65">
+        <v>3</v>
+      </c>
+      <c r="F139" s="65">
+        <v>0</v>
+      </c>
+      <c r="G139" s="65">
+        <v>1</v>
+      </c>
+      <c r="H139" s="65">
+        <v>0</v>
+      </c>
+      <c r="I139" s="65">
+        <v>25</v>
+      </c>
+      <c r="J139" s="174">
+        <v>2500</v>
+      </c>
+      <c r="K139" s="53">
+        <v>0.23</v>
+      </c>
+      <c r="L139" s="65">
+        <v>0</v>
+      </c>
+      <c r="M139" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N139" s="40">
+        <v>5</v>
+      </c>
+      <c r="O139" s="37">
+        <v>5</v>
+      </c>
+      <c r="P139" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="40">
+        <v>0</v>
+      </c>
+      <c r="R139" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S139" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="T139" s="73" t="b">
+        <v>0</v>
+      </c>
+      <c r="U139" s="36">
+        <v>1</v>
+      </c>
+      <c r="V139" s="36">
+        <v>1</v>
+      </c>
+      <c r="W139" s="36">
+        <v>0</v>
+      </c>
+      <c r="X139" s="52">
+        <v>0</v>
+      </c>
+      <c r="Y139" s="52">
+        <v>0</v>
+      </c>
+      <c r="Z139" s="52">
+        <v>0</v>
+      </c>
+      <c r="AA139" s="52">
+        <v>0</v>
+      </c>
+      <c r="AB139" s="156" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC139" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD139" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE139" s="72"/>
+      <c r="AF139" s="71"/>
+    </row>
+    <row r="140" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A140" s="160"/>
+      <c r="B140" s="118"/>
+      <c r="C140" s="118"/>
+      <c r="D140" s="119"/>
+      <c r="E140" s="120"/>
+      <c r="F140" s="120"/>
+      <c r="G140" s="120"/>
+      <c r="H140" s="120"/>
+      <c r="I140" s="120"/>
+      <c r="J140" s="161"/>
+      <c r="K140" s="162"/>
+      <c r="L140" s="120"/>
+      <c r="M140" s="121"/>
+      <c r="N140" s="163"/>
+      <c r="O140" s="163"/>
+      <c r="P140" s="164"/>
+      <c r="Q140" s="163"/>
+      <c r="R140" s="165"/>
+      <c r="S140" s="166"/>
+      <c r="T140" s="166"/>
+      <c r="U140" s="165"/>
+      <c r="V140" s="122"/>
+      <c r="W140" s="121"/>
+      <c r="X140" s="167"/>
+      <c r="Y140" s="168"/>
+      <c r="Z140" s="168"/>
+      <c r="AA140" s="169"/>
+      <c r="AB140" s="170"/>
+      <c r="AC140" s="171"/>
+      <c r="AD140" s="172"/>
+      <c r="AE140" s="172"/>
+      <c r="AF140" s="173"/>
+    </row>
+    <row r="141" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="142" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A142" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B141" s="9"/>
-      <c r="C141" s="9"/>
-      <c r="D141" s="9"/>
-      <c r="E141" s="9"/>
-      <c r="F141" s="9"/>
-      <c r="G141" s="9"/>
-      <c r="H141" s="9"/>
-      <c r="I141" s="9"/>
-      <c r="J141" s="9"/>
-      <c r="K141" s="9"/>
-      <c r="L141" s="9"/>
-      <c r="M141" s="9"/>
-      <c r="N141" s="9"/>
-      <c r="O141" s="9"/>
-      <c r="P141" s="9"/>
-      <c r="Q141" s="9"/>
-      <c r="R141" s="9"/>
-      <c r="S141" s="9"/>
-      <c r="T141" s="9"/>
-      <c r="U141" s="9"/>
-      <c r="V141" s="9"/>
-      <c r="W141" s="9"/>
-      <c r="X141" s="9"/>
-      <c r="Y141" s="9"/>
-      <c r="Z141" s="9"/>
-      <c r="AA141" s="9"/>
-      <c r="AF141" s="8"/>
-    </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A142" s="22"/>
-      <c r="B142" s="22"/>
-      <c r="C142" s="22"/>
-      <c r="D142" s="22"/>
-      <c r="E142" s="22"/>
-      <c r="F142" s="170"/>
-      <c r="G142" s="170"/>
-      <c r="H142" s="21" t="s">
+      <c r="B142" s="9"/>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="9"/>
+      <c r="H142" s="9"/>
+      <c r="I142" s="9"/>
+      <c r="J142" s="9"/>
+      <c r="K142" s="9"/>
+      <c r="L142" s="9"/>
+      <c r="M142" s="9"/>
+      <c r="N142" s="9"/>
+      <c r="O142" s="9"/>
+      <c r="P142" s="9"/>
+      <c r="Q142" s="9"/>
+      <c r="R142" s="9"/>
+      <c r="S142" s="9"/>
+      <c r="T142" s="9"/>
+      <c r="U142" s="9"/>
+      <c r="V142" s="9"/>
+      <c r="W142" s="9"/>
+      <c r="X142" s="9"/>
+      <c r="Y142" s="9"/>
+      <c r="Z142" s="9"/>
+      <c r="AA142" s="9"/>
+      <c r="AF142" s="8"/>
+    </row>
+    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A143" s="22"/>
+      <c r="B143" s="22"/>
+      <c r="C143" s="22"/>
+      <c r="D143" s="22"/>
+      <c r="E143" s="22"/>
+      <c r="F143" s="159"/>
+      <c r="G143" s="159"/>
+      <c r="H143" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I142" s="21"/>
-      <c r="J142" s="22"/>
-      <c r="K142" s="17"/>
-      <c r="L142" s="17"/>
-      <c r="M142" s="17" t="s">
+      <c r="I143" s="21"/>
+      <c r="J143" s="22"/>
+      <c r="K143" s="17"/>
+      <c r="L143" s="17"/>
+      <c r="M143" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N142" s="17"/>
-      <c r="O142" s="17"/>
-      <c r="P142" s="17"/>
-      <c r="Q142" s="17"/>
-      <c r="R142" s="17"/>
-      <c r="S142" s="17"/>
-      <c r="T142" s="17"/>
-      <c r="U142" s="17"/>
-      <c r="V142" s="17"/>
-      <c r="W142" s="17"/>
-      <c r="X142" s="17"/>
-      <c r="Y142" s="17"/>
-      <c r="Z142" s="17"/>
-      <c r="AA142" s="21"/>
-      <c r="AB142" s="21"/>
-      <c r="AC142" s="21"/>
-      <c r="AD142" s="21"/>
-      <c r="AE142" s="17"/>
-    </row>
-    <row r="143" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A143" s="7" t="s">
+      <c r="N143" s="17"/>
+      <c r="O143" s="17"/>
+      <c r="P143" s="17"/>
+      <c r="Q143" s="17"/>
+      <c r="R143" s="17"/>
+      <c r="S143" s="17"/>
+      <c r="T143" s="17"/>
+      <c r="U143" s="17"/>
+      <c r="V143" s="17"/>
+      <c r="W143" s="17"/>
+      <c r="X143" s="17"/>
+      <c r="Y143" s="17"/>
+      <c r="Z143" s="17"/>
+      <c r="AA143" s="21"/>
+      <c r="AB143" s="21"/>
+      <c r="AC143" s="21"/>
+      <c r="AD143" s="21"/>
+      <c r="AE143" s="17"/>
+    </row>
+    <row r="144" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B143" s="7" t="s">
+      <c r="B144" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C143" s="7" t="s">
+      <c r="C144" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D143" s="20" t="s">
+      <c r="D144" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E143" s="20" t="s">
+      <c r="E144" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F143" s="20" t="s">
+      <c r="F144" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G143" s="20" t="s">
+      <c r="G144" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H143" s="20" t="s">
+      <c r="H144" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I143" s="20" t="s">
+      <c r="I144" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J143" s="20" t="s">
+      <c r="J144" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K143" s="20" t="s">
+      <c r="K144" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="L143" s="20" t="s">
+      <c r="L144" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M143" s="19" t="s">
+      <c r="M144" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N143" s="19" t="s">
+      <c r="N144" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O143" s="19" t="s">
+      <c r="O144" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A144" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B144" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C144" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D144" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E144" s="14">
-        <v>3</v>
-      </c>
-      <c r="F144" s="18">
-        <v>0</v>
-      </c>
-      <c r="G144" s="18">
-        <v>0</v>
-      </c>
-      <c r="H144" s="18">
-        <v>0</v>
-      </c>
-      <c r="I144" s="18">
-        <v>0</v>
-      </c>
-      <c r="J144" s="12">
-        <v>2</v>
-      </c>
-      <c r="K144" s="12">
-        <v>0</v>
-      </c>
-      <c r="L144" s="12">
-        <v>0</v>
-      </c>
-      <c r="M144" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N144" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O144" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P144" s="17"/>
-      <c r="Q144" s="17"/>
     </row>
     <row r="145" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A145" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C145" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E145" s="14">
         <v>3</v>
@@ -16925,7 +17038,7 @@
         <v>0</v>
       </c>
       <c r="G145" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H145" s="18">
         <v>0</v>
@@ -16959,13 +17072,13 @@
         <v>2</v>
       </c>
       <c r="B146" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E146" s="14">
         <v>3</v>
@@ -16974,7 +17087,7 @@
         <v>0</v>
       </c>
       <c r="G146" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H146" s="18">
         <v>0</v>
@@ -17008,13 +17121,13 @@
         <v>2</v>
       </c>
       <c r="B147" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C147" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E147" s="14">
         <v>3</v>
@@ -17023,7 +17136,7 @@
         <v>0</v>
       </c>
       <c r="G147" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H147" s="18">
         <v>0</v>
@@ -17057,13 +17170,13 @@
         <v>2</v>
       </c>
       <c r="B148" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E148" s="14">
         <v>3</v>
@@ -17072,7 +17185,7 @@
         <v>0</v>
       </c>
       <c r="G148" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H148" s="18">
         <v>0</v>
@@ -17106,13 +17219,13 @@
         <v>2</v>
       </c>
       <c r="B149" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C149" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D149" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E149" s="14">
         <v>3</v>
@@ -17121,7 +17234,7 @@
         <v>0</v>
       </c>
       <c r="G149" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H149" s="18">
         <v>0</v>
@@ -17155,13 +17268,13 @@
         <v>2</v>
       </c>
       <c r="B150" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C150" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D150" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E150" s="14">
         <v>3</v>
@@ -17170,7 +17283,7 @@
         <v>0</v>
       </c>
       <c r="G150" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H150" s="18">
         <v>0</v>
@@ -17204,13 +17317,13 @@
         <v>2</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E151" s="14">
         <v>3</v>
@@ -17219,7 +17332,7 @@
         <v>0</v>
       </c>
       <c r="G151" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H151" s="18">
         <v>0</v>
@@ -17253,13 +17366,13 @@
         <v>2</v>
       </c>
       <c r="B152" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C152" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E152" s="14">
         <v>3</v>
@@ -17268,7 +17381,7 @@
         <v>0</v>
       </c>
       <c r="G152" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H152" s="18">
         <v>0</v>
@@ -17302,13 +17415,13 @@
         <v>2</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C153" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E153" s="14">
         <v>3</v>
@@ -17317,7 +17430,7 @@
         <v>0</v>
       </c>
       <c r="G153" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H153" s="18">
         <v>0</v>
@@ -17351,27 +17464,27 @@
         <v>2</v>
       </c>
       <c r="B154" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E154" s="14">
-        <v>1</v>
-      </c>
-      <c r="F154" s="13">
-        <v>0</v>
-      </c>
-      <c r="G154" s="13">
-        <v>1</v>
-      </c>
-      <c r="H154" s="13">
-        <v>0</v>
-      </c>
-      <c r="I154" s="13">
+        <v>3</v>
+      </c>
+      <c r="F154" s="18">
+        <v>0</v>
+      </c>
+      <c r="G154" s="18">
+        <v>2</v>
+      </c>
+      <c r="H154" s="18">
+        <v>0</v>
+      </c>
+      <c r="I154" s="18">
         <v>0</v>
       </c>
       <c r="J154" s="12">
@@ -17392,33 +17505,35 @@
       <c r="O154" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P154" s="17"/>
+      <c r="Q154" s="17"/>
     </row>
     <row r="155" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B155" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="C155" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="D155" s="143" t="s">
-        <v>30</v>
+      <c r="B155" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C155" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D155" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E155" s="14">
         <v>1</v>
       </c>
-      <c r="F155" s="144">
-        <v>0</v>
-      </c>
-      <c r="G155" s="144">
-        <v>0</v>
-      </c>
-      <c r="H155" s="144">
-        <v>0</v>
-      </c>
-      <c r="I155" s="144">
+      <c r="F155" s="13">
+        <v>0</v>
+      </c>
+      <c r="G155" s="13">
+        <v>1</v>
+      </c>
+      <c r="H155" s="13">
+        <v>0</v>
+      </c>
+      <c r="I155" s="13">
         <v>0</v>
       </c>
       <c r="J155" s="12">
@@ -17439,26 +17554,53 @@
       <c r="O155" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P155" s="8"/>
-      <c r="Q155" s="8"/>
-      <c r="R155" s="8"/>
-      <c r="S155" s="8"/>
-      <c r="T155" s="8"/>
-      <c r="U155" s="8"/>
-      <c r="V155" s="8"/>
-      <c r="W155" s="8"/>
-      <c r="X155" s="8"/>
-      <c r="Y155" s="8"/>
-      <c r="Z155" s="8"/>
-      <c r="AA155" s="8"/>
-      <c r="AB155" s="8"/>
-      <c r="AC155" s="8"/>
-      <c r="AD155" s="8"/>
-      <c r="AE155" s="8"/>
     </row>
     <row r="156" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N156" s="8"/>
-      <c r="O156" s="8"/>
+      <c r="A156" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B156" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="C156" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D156" s="132" t="s">
+        <v>30</v>
+      </c>
+      <c r="E156" s="14">
+        <v>1</v>
+      </c>
+      <c r="F156" s="133">
+        <v>0</v>
+      </c>
+      <c r="G156" s="133">
+        <v>0</v>
+      </c>
+      <c r="H156" s="133">
+        <v>0</v>
+      </c>
+      <c r="I156" s="133">
+        <v>0</v>
+      </c>
+      <c r="J156" s="12">
+        <v>2</v>
+      </c>
+      <c r="K156" s="12">
+        <v>0</v>
+      </c>
+      <c r="L156" s="12">
+        <v>0</v>
+      </c>
+      <c r="M156" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N156" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O156" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="P156" s="8"/>
       <c r="Q156" s="8"/>
       <c r="R156" s="8"/>
@@ -17476,73 +17618,67 @@
       <c r="AD156" s="8"/>
       <c r="AE156" s="8"/>
     </row>
-    <row r="157" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="158" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A158" s="9" t="s">
+    <row r="157" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N157" s="8"/>
+      <c r="O157" s="8"/>
+      <c r="P157" s="8"/>
+      <c r="Q157" s="8"/>
+      <c r="R157" s="8"/>
+      <c r="S157" s="8"/>
+      <c r="T157" s="8"/>
+      <c r="U157" s="8"/>
+      <c r="V157" s="8"/>
+      <c r="W157" s="8"/>
+      <c r="X157" s="8"/>
+      <c r="Y157" s="8"/>
+      <c r="Z157" s="8"/>
+      <c r="AA157" s="8"/>
+      <c r="AB157" s="8"/>
+      <c r="AC157" s="8"/>
+      <c r="AD157" s="8"/>
+      <c r="AE157" s="8"/>
+    </row>
+    <row r="158" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="159" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A159" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B158" s="9"/>
-      <c r="C158" s="9"/>
-      <c r="D158" s="9"/>
-      <c r="E158" s="8"/>
-      <c r="F158" s="8"/>
-      <c r="G158" s="8"/>
-      <c r="H158" s="8"/>
-      <c r="I158" s="8"/>
-      <c r="J158" s="8"/>
-      <c r="K158" s="8"/>
-      <c r="L158" s="8"/>
-    </row>
-    <row r="160" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="7" t="s">
+      <c r="B159" s="9"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="8"/>
+      <c r="F159" s="8"/>
+      <c r="G159" s="8"/>
+      <c r="H159" s="8"/>
+      <c r="I159" s="8"/>
+      <c r="J159" s="8"/>
+      <c r="K159" s="8"/>
+      <c r="L159" s="8"/>
+    </row>
+    <row r="161" spans="1:9" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A161" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B160" s="6" t="s">
+      <c r="B161" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C160" s="6" t="s">
+      <c r="C161" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D160" s="5" t="s">
+      <c r="D161" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E160" s="5" t="s">
+      <c r="E161" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F160" s="5" t="s">
+      <c r="F161" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G160" s="5" t="s">
+      <c r="G161" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H160" s="5" t="s">
+      <c r="H161" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D161" s="2">
-        <v>42</v>
-      </c>
-      <c r="E161" s="2">
-        <v>8</v>
-      </c>
-      <c r="F161" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G161" s="2">
-        <v>2</v>
-      </c>
-      <c r="H161" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -17550,19 +17686,19 @@
         <v>2</v>
       </c>
       <c r="B162" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D162" s="2">
+        <v>42</v>
+      </c>
+      <c r="E162" s="2">
         <v>8</v>
       </c>
-      <c r="C162" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D162" s="2">
-        <v>92</v>
-      </c>
-      <c r="E162" s="2">
-        <v>10</v>
-      </c>
       <c r="F162" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G162" s="2">
         <v>2</v>
@@ -17576,19 +17712,19 @@
         <v>2</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D163" s="2">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="E163" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F163" s="2">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G163" s="2">
         <v>2</v>
@@ -17602,19 +17738,19 @@
         <v>2</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D164" s="2">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="E164" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F164" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G164" s="2">
         <v>2</v>
@@ -17628,104 +17764,130 @@
         <v>2</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D165" s="2">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="E165" s="2">
         <v>14</v>
       </c>
       <c r="F165" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G165" s="2">
+        <v>2</v>
+      </c>
+      <c r="H165" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D166" s="2">
+        <v>1040</v>
+      </c>
+      <c r="E166" s="2">
+        <v>14</v>
+      </c>
+      <c r="F166" s="2">
         <v>0.5</v>
       </c>
-      <c r="G165" s="2">
-        <v>2</v>
-      </c>
-      <c r="H165" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D168" s="1">
-        <v>42</v>
-      </c>
-      <c r="F168" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G168">
-        <f>D161*F161</f>
-        <v>54.6</v>
-      </c>
-      <c r="I168">
-        <f>D168*F168</f>
-        <v>54.6</v>
+      <c r="G166" s="2">
+        <v>2</v>
+      </c>
+      <c r="H166" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D169" s="1">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="F169" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G169">
         <f>D162*F162</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
       <c r="I169">
         <f>D169*F169</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D170" s="1">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="F170" s="1">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G170">
         <f>D163*F163</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
       <c r="I170">
         <f>D170*F170</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D171" s="1">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="F171" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G171">
         <f>D164*F164</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
       <c r="I171">
         <f>D171*F171</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D172" s="1">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="F172" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G172">
         <f>D165*F165</f>
-        <v>520</v>
+        <v>480.2</v>
       </c>
       <c r="I172">
         <f>D172*F172</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D173" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F173" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G173">
+        <f>D166*F166</f>
+        <v>520</v>
+      </c>
+      <c r="I173">
+        <f>D173*F173</f>
         <v>520</v>
       </c>
     </row>
@@ -17733,20 +17895,20 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F142:G142"/>
+    <mergeCell ref="F143:G143"/>
   </mergeCells>
   <conditionalFormatting sqref="M118:M124 R118:T124 M24:M56 R24:T56 S127:T127 M127 R58:T115 M58:M115">
-    <cfRule type="expression" dxfId="113" priority="63">
+    <cfRule type="expression" dxfId="21" priority="65">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="112" priority="56">
+    <cfRule type="expression" dxfId="20" priority="58">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116:Q116">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17758,11 +17920,40 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="111" priority="50">
+    <cfRule type="expression" dxfId="19" priority="52">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N115:Q119">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N118:Q124 N24:Q56 N58:Q115">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M114 R114:T114">
+    <cfRule type="expression" dxfId="18" priority="50">
+      <formula>M114=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N114:Q114">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -17774,47 +17965,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N118:Q124 N24:Q56 N58:Q115">
-    <cfRule type="colorScale" priority="68">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="110" priority="48">
-      <formula>M114=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N114:Q114">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="109" priority="45">
+    <cfRule type="expression" dxfId="17" priority="47">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="108" priority="44">
+    <cfRule type="expression" dxfId="16" priority="46">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q125">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17826,7 +17988,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q127">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17838,17 +18000,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="107" priority="42">
+    <cfRule type="expression" dxfId="15" priority="44">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="106" priority="41">
+    <cfRule type="expression" dxfId="14" priority="43">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:Q128">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17860,22 +18022,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="105" priority="39">
+    <cfRule type="expression" dxfId="13" priority="41">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="104" priority="24">
+    <cfRule type="expression" dxfId="12" priority="26">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="103" priority="26">
+    <cfRule type="expression" dxfId="11" priority="28">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N133:Q133">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17887,17 +18049,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="102" priority="19">
+    <cfRule type="expression" dxfId="10" priority="21">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="101" priority="20">
+    <cfRule type="expression" dxfId="9" priority="22">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N129:Q132">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17909,7 +18071,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:Q134">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17921,17 +18083,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="100" priority="17">
+    <cfRule type="expression" dxfId="8" priority="19">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="99" priority="12">
+    <cfRule type="expression" dxfId="7" priority="14">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N135:Q135">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17943,16 +18105,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="98" priority="14">
+    <cfRule type="expression" dxfId="6" priority="16">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="97" priority="7">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N136:Q136">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S136:T136 M136">
+    <cfRule type="expression" dxfId="4" priority="11">
+      <formula>M136=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M138 R138:T138">
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>M138=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N138:Q138">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -17964,17 +18148,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="96" priority="9">
-      <formula>M136=FALSE</formula>
+  <conditionalFormatting sqref="M57 R57:T57">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="95" priority="5">
-      <formula>M138=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N138:Q138">
+  <conditionalFormatting sqref="N57:Q57">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -17986,12 +18165,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="94" priority="3">
-      <formula>M57=FALSE</formula>
+  <conditionalFormatting sqref="M137 R137:T137">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57:Q57">
+  <conditionalFormatting sqref="N137:Q137">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -18003,12 +18182,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="93" priority="1">
-      <formula>M137=FALSE</formula>
+  <conditionalFormatting sqref="M139 R139:T139">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N137:Q137">
+  <conditionalFormatting sqref="N139:Q139">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -18020,35 +18199,39 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="10">
+  <dataValidations count="11">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G134"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G133 J24:J138 H40:I139 G135:G139">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G133 J24:J138 H40:I140 G135:G140">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D144:G155 M139:N139 P139:V139 N24:O138 Q24:W138">
+    <dataValidation type="decimal" allowBlank="1" sqref="D145:G156 M139:N140 P139:V140 N24:O138 Q24:W138">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H144:L153 H154:I154 J155:L155 W139:Z139 X24:AA138">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H145:L154 H155:I155 J156:L156 W139:Z140 X24:AA138">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C144:C155 C24:C139">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C145:C156 C24:C140">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J154:L154 M144:O155 AA139:AE139 AB24:AF138"/>
-    <dataValidation type="list" sqref="O139 P24:P138">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J155:L155 M145:O156 AB24:AB140 AC24:AC138 AA139:AC140 AD24:AF140"/>
+    <dataValidation type="list" sqref="O139:O140 P24:P138">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J139:K139 K24:L138">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L138 K139:K140 J140">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="L139 M24:M138">
+    <dataValidation type="list" sqref="L139:L140 M24:M138">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F139">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F140">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J139">
+      <formula1>0</formula1>
+      <formula2>10000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18104,8 +18287,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="170"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
DrunkenMan doesn't make the dragon drunk anymore, until we solve/decide how to finish the feature
Former-commit-id: 41d5b0a981a5433bb0852ccb46986d3ecfa8986a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -2549,9 +2549,6 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2598,166 +2595,15 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="115">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5053,6 +4899,160 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5067,58 +5067,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF139" totalsRowShown="0" headerRowDxfId="114" dataDxfId="112" headerRowBorderDxfId="113" tableBorderDxfId="111" totalsRowBorderDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF139" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF139"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="109"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="108"/>
-    <tableColumn id="6" name="[category]" dataDxfId="107"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="106"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="105"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="104"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="103"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="102"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="101"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="100"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="99"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="98"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="97"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="96"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="95"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="94"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="93"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="92"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="91"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="90"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="89"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="88"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="87"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="86"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="85"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="84"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="83"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="82"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="81"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="80"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="79"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="78"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75" totalsRowBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="73"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="72"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5131,50 +5131,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="4" name="[category]" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="16" name="[size]" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="37"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="36"/>
-    <tableColumn id="6" name="[order]" dataDxfId="35"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="34"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="33"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="32"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="31"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="23"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="22" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5448,10 +5448,10 @@
   </sheetPr>
   <dimension ref="A1:AF173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A139" sqref="A139"/>
+      <selection pane="topRight" activeCell="W50" sqref="W50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5495,8 +5495,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="159"/>
-      <c r="F3" s="159"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5660,8 +5660,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="159"/>
-      <c r="F22" s="159"/>
+      <c r="E22" s="174"/>
+      <c r="F22" s="174"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -8244,7 +8244,7 @@
         <v>9</v>
       </c>
       <c r="W49" s="36">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="X49" s="52">
         <v>0.25</v>
@@ -16801,7 +16801,7 @@
       <c r="I139" s="65">
         <v>25</v>
       </c>
-      <c r="J139" s="174">
+      <c r="J139" s="173">
         <v>2500</v>
       </c>
       <c r="K139" s="53">
@@ -16868,7 +16868,7 @@
       <c r="AF139" s="71"/>
     </row>
     <row r="140" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A140" s="160"/>
+      <c r="A140" s="159"/>
       <c r="B140" s="118"/>
       <c r="C140" s="118"/>
       <c r="D140" s="119"/>
@@ -16877,29 +16877,29 @@
       <c r="G140" s="120"/>
       <c r="H140" s="120"/>
       <c r="I140" s="120"/>
-      <c r="J140" s="161"/>
-      <c r="K140" s="162"/>
+      <c r="J140" s="160"/>
+      <c r="K140" s="161"/>
       <c r="L140" s="120"/>
       <c r="M140" s="121"/>
-      <c r="N140" s="163"/>
-      <c r="O140" s="163"/>
-      <c r="P140" s="164"/>
-      <c r="Q140" s="163"/>
-      <c r="R140" s="165"/>
-      <c r="S140" s="166"/>
-      <c r="T140" s="166"/>
-      <c r="U140" s="165"/>
+      <c r="N140" s="162"/>
+      <c r="O140" s="162"/>
+      <c r="P140" s="163"/>
+      <c r="Q140" s="162"/>
+      <c r="R140" s="164"/>
+      <c r="S140" s="165"/>
+      <c r="T140" s="165"/>
+      <c r="U140" s="164"/>
       <c r="V140" s="122"/>
       <c r="W140" s="121"/>
-      <c r="X140" s="167"/>
-      <c r="Y140" s="168"/>
-      <c r="Z140" s="168"/>
-      <c r="AA140" s="169"/>
-      <c r="AB140" s="170"/>
-      <c r="AC140" s="171"/>
-      <c r="AD140" s="172"/>
-      <c r="AE140" s="172"/>
-      <c r="AF140" s="173"/>
+      <c r="X140" s="166"/>
+      <c r="Y140" s="167"/>
+      <c r="Z140" s="167"/>
+      <c r="AA140" s="168"/>
+      <c r="AB140" s="169"/>
+      <c r="AC140" s="170"/>
+      <c r="AD140" s="171"/>
+      <c r="AE140" s="171"/>
+      <c r="AF140" s="172"/>
     </row>
     <row r="141" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="142" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
@@ -16940,8 +16940,8 @@
       <c r="C143" s="22"/>
       <c r="D143" s="22"/>
       <c r="E143" s="22"/>
-      <c r="F143" s="159"/>
-      <c r="G143" s="159"/>
+      <c r="F143" s="174"/>
+      <c r="G143" s="174"/>
       <c r="H143" s="21" t="s">
         <v>56</v>
       </c>
@@ -17898,12 +17898,12 @@
     <mergeCell ref="F143:G143"/>
   </mergeCells>
   <conditionalFormatting sqref="M118:M124 R118:T124 M24:M56 R24:T56 S127:T127 M127 R58:T115 M58:M115">
-    <cfRule type="expression" dxfId="21" priority="65">
+    <cfRule type="expression" dxfId="114" priority="65">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="20" priority="58">
+    <cfRule type="expression" dxfId="113" priority="58">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17920,7 +17920,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="19" priority="52">
+    <cfRule type="expression" dxfId="112" priority="52">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17949,7 +17949,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="18" priority="50">
+    <cfRule type="expression" dxfId="111" priority="50">
       <formula>M114=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17966,12 +17966,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="17" priority="47">
+    <cfRule type="expression" dxfId="110" priority="47">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="16" priority="46">
+    <cfRule type="expression" dxfId="109" priority="46">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18000,12 +18000,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="15" priority="44">
+    <cfRule type="expression" dxfId="108" priority="44">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="14" priority="43">
+    <cfRule type="expression" dxfId="107" priority="43">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18022,17 +18022,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="13" priority="41">
+    <cfRule type="expression" dxfId="106" priority="41">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="12" priority="26">
+    <cfRule type="expression" dxfId="105" priority="26">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="11" priority="28">
+    <cfRule type="expression" dxfId="104" priority="28">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18049,12 +18049,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="10" priority="21">
+    <cfRule type="expression" dxfId="103" priority="21">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="102" priority="22">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18083,12 +18083,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="8" priority="19">
+    <cfRule type="expression" dxfId="101" priority="19">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="100" priority="14">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18105,12 +18105,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="6" priority="16">
+    <cfRule type="expression" dxfId="99" priority="16">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="98" priority="9">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18127,12 +18127,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="4" priority="11">
+    <cfRule type="expression" dxfId="97" priority="11">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="96" priority="7">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18149,7 +18149,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="95" priority="5">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18166,7 +18166,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="94" priority="3">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18183,7 +18183,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="93" priority="1">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18287,8 +18287,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="159"/>
-      <c r="G3" s="159"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
Added 'RatGrey' to content
Former-commit-id: 38448682f7468b1ffd8505fc0d464d1b347bb993
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="505">
   <si>
     <t>tier_4</t>
   </si>
@@ -1554,12 +1554,15 @@
   <si>
     <t>MexicanPepper</t>
   </si>
+  <si>
+    <t>RatGrey</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1661,46 +1664,8 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="2" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="22">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1787,12 +1752,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1818,12 +1777,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2142,7 +2095,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2221,7 +2174,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2233,7 +2186,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2261,10 +2214,10 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2288,7 +2241,7 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2300,10 +2253,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2333,7 +2286,7 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2431,21 +2384,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2484,7 +2422,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2508,13 +2446,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2535,11 +2473,11 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2549,49 +2487,7 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2603,7 +2499,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="115">
+  <dxfs count="117">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5067,58 +4977,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF139" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF139"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF140" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+  <autoFilter ref="A23:AF140"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="89"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
+    <tableColumn id="6" name="[category]" dataDxfId="87"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="86"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="85"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="84"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="83"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="82"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="81"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="80"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="79"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="78"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="77"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="76"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="75"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="74"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="73"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="72"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="71"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="70"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="69"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="68"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="67"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="66"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="65"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="62"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="61"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="60"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="59"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="53"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5131,50 +5041,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="[category]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="16" name="[size]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="17"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="6" name="[order]" dataDxfId="15"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="14"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="13"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="12"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="5"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="3"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="2" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5448,10 +5358,10 @@
   </sheetPr>
   <dimension ref="A1:AF173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="V1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="W50" sqref="W50"/>
+      <selection pane="topRight" activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5495,8 +5405,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
+      <c r="E3" s="155"/>
+      <c r="F3" s="155"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5660,8 +5570,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="174"/>
-      <c r="F22" s="174"/>
+      <c r="E22" s="155"/>
+      <c r="F22" s="155"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -5777,13 +5687,13 @@
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A24" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="124" t="s">
+      <c r="A24" s="119" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="119" t="s">
         <v>353</v>
       </c>
-      <c r="C24" s="125" t="s">
+      <c r="C24" s="120" t="s">
         <v>87</v>
       </c>
       <c r="D24" s="66">
@@ -5875,13 +5785,13 @@
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A25" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="124" t="s">
+      <c r="A25" s="119" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="119" t="s">
         <v>347</v>
       </c>
-      <c r="C25" s="125" t="s">
+      <c r="C25" s="120" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="66">
@@ -5973,13 +5883,13 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A26" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="124" t="s">
+      <c r="A26" s="119" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="119" t="s">
         <v>342</v>
       </c>
-      <c r="C26" s="125" t="s">
+      <c r="C26" s="120" t="s">
         <v>87</v>
       </c>
       <c r="D26" s="66">
@@ -6071,13 +5981,13 @@
       </c>
     </row>
     <row r="27" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="124" t="s">
+      <c r="A27" s="119" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="119" t="s">
         <v>339</v>
       </c>
-      <c r="C27" s="125" t="s">
+      <c r="C27" s="120" t="s">
         <v>82</v>
       </c>
       <c r="D27" s="66">
@@ -6555,13 +6465,13 @@
       <c r="AF31" s="79"/>
     </row>
     <row r="32" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="124" t="s">
+      <c r="A32" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="119" t="s">
         <v>321</v>
       </c>
-      <c r="C32" s="125" t="s">
+      <c r="C32" s="120" t="s">
         <v>87</v>
       </c>
       <c r="D32" s="66">
@@ -6649,13 +6559,13 @@
       <c r="AF32" s="71"/>
     </row>
     <row r="33" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="124" t="s">
+      <c r="A33" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="119" t="s">
         <v>320</v>
       </c>
-      <c r="C33" s="125" t="s">
+      <c r="C33" s="120" t="s">
         <v>68</v>
       </c>
       <c r="D33" s="66">
@@ -6748,13 +6658,13 @@
       </c>
     </row>
     <row r="34" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="126" t="s">
+      <c r="A34" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="121" t="s">
         <v>432</v>
       </c>
-      <c r="C34" s="127" t="s">
+      <c r="C34" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D34" s="66">
@@ -6842,13 +6752,13 @@
       <c r="AF34" s="71"/>
     </row>
     <row r="35" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="126" t="s">
+      <c r="A35" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="121" t="s">
         <v>441</v>
       </c>
-      <c r="C35" s="127" t="s">
+      <c r="C35" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D35" s="66">
@@ -7222,7 +7132,7 @@
       <c r="AF38" s="79"/>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A39" s="140" t="s">
+      <c r="A39" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="49" t="s">
@@ -7317,13 +7227,13 @@
       <c r="AF39" s="79"/>
     </row>
     <row r="40" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="124" t="s">
+      <c r="A40" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="125" t="s">
+      <c r="C40" s="120" t="s">
         <v>66</v>
       </c>
       <c r="D40" s="66">
@@ -7411,13 +7321,13 @@
       <c r="AF40" s="71"/>
     </row>
     <row r="41" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="124" t="s">
+      <c r="A41" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="119" t="s">
         <v>443</v>
       </c>
-      <c r="C41" s="125" t="s">
+      <c r="C41" s="120" t="s">
         <v>66</v>
       </c>
       <c r="D41" s="66">
@@ -7505,13 +7415,13 @@
       <c r="AF41" s="71"/>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A42" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="126" t="s">
+      <c r="A42" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="121" t="s">
         <v>302</v>
       </c>
-      <c r="C42" s="127" t="s">
+      <c r="C42" s="122" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="66">
@@ -7599,13 +7509,13 @@
       <c r="AF42" s="71"/>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A43" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="126" t="s">
+      <c r="A43" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="121" t="s">
         <v>434</v>
       </c>
-      <c r="C43" s="127" t="s">
+      <c r="C43" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D43" s="66">
@@ -7787,7 +7697,7 @@
       <c r="AE44" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF44" s="139" t="s">
+      <c r="AF44" s="134" t="s">
         <v>287</v>
       </c>
     </row>
@@ -7984,7 +7894,7 @@
       </c>
     </row>
     <row r="47" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="140" t="s">
+      <c r="A47" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="49" t="s">
@@ -8079,13 +7989,13 @@
       <c r="AF47" s="74"/>
     </row>
     <row r="48" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="124" t="s">
+      <c r="A48" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="119" t="s">
         <v>290</v>
       </c>
-      <c r="C48" s="125" t="s">
+      <c r="C48" s="120" t="s">
         <v>68</v>
       </c>
       <c r="D48" s="66">
@@ -8177,13 +8087,13 @@
       </c>
     </row>
     <row r="49" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="124" t="s">
+      <c r="A49" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="119" t="s">
         <v>286</v>
       </c>
-      <c r="C49" s="125" t="s">
+      <c r="C49" s="120" t="s">
         <v>87</v>
       </c>
       <c r="D49" s="66">
@@ -8271,13 +8181,13 @@
       <c r="AF49" s="71"/>
     </row>
     <row r="50" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" s="126" t="s">
+      <c r="A50" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="121" t="s">
         <v>282</v>
       </c>
-      <c r="C50" s="127" t="s">
+      <c r="C50" s="122" t="s">
         <v>273</v>
       </c>
       <c r="D50" s="66">
@@ -8369,13 +8279,13 @@
       </c>
     </row>
     <row r="51" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="126" t="s">
+      <c r="A51" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="121" t="s">
         <v>280</v>
       </c>
-      <c r="C51" s="127" t="s">
+      <c r="C51" s="122" t="s">
         <v>273</v>
       </c>
       <c r="D51" s="66">
@@ -8663,7 +8573,7 @@
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A54" s="140" t="s">
+      <c r="A54" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="49" t="s">
@@ -8761,7 +8671,7 @@
       </c>
     </row>
     <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="140" t="s">
+      <c r="A55" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="49" t="s">
@@ -8856,13 +8766,13 @@
       <c r="AF55" s="74"/>
     </row>
     <row r="56" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="124" t="s">
+      <c r="A56" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="C56" s="125" t="s">
+      <c r="C56" s="120" t="s">
         <v>82</v>
       </c>
       <c r="D56" s="66">
@@ -8950,14 +8860,14 @@
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
     </row>
-    <row r="57" spans="1:32" s="155" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="124" t="s">
+    <row r="57" spans="1:32" s="150" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="119" t="s">
         <v>448</v>
       </c>
-      <c r="C57" s="125" t="s">
+      <c r="C57" s="120" t="s">
         <v>449</v>
       </c>
       <c r="D57" s="66">
@@ -9039,13 +8949,13 @@
       <c r="AF57" s="71"/>
     </row>
     <row r="58" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" s="126" t="s">
+      <c r="A58" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="121" t="s">
         <v>431</v>
       </c>
-      <c r="C58" s="127" t="s">
+      <c r="C58" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D58" s="66">
@@ -9134,13 +9044,13 @@
       <c r="AF58" s="80"/>
     </row>
     <row r="59" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" s="126" t="s">
+      <c r="A59" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="121" t="s">
         <v>263</v>
       </c>
-      <c r="C59" s="127" t="s">
+      <c r="C59" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D59" s="66">
@@ -9418,7 +9328,7 @@
       <c r="AF61" s="74"/>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A62" s="140" t="s">
+      <c r="A62" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B62" s="49" t="s">
@@ -9513,7 +9423,7 @@
       <c r="AF62" s="74"/>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A63" s="140" t="s">
+      <c r="A63" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B63" s="49" t="s">
@@ -9608,13 +9518,13 @@
       <c r="AF63" s="74"/>
     </row>
     <row r="64" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B64" s="124" t="s">
+      <c r="A64" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="119" t="s">
         <v>253</v>
       </c>
-      <c r="C64" s="125" t="s">
+      <c r="C64" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D64" s="66">
@@ -9703,13 +9613,13 @@
       <c r="AF64" s="80"/>
     </row>
     <row r="65" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B65" s="124" t="s">
+      <c r="A65" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="119" t="s">
         <v>249</v>
       </c>
-      <c r="C65" s="125" t="s">
+      <c r="C65" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D65" s="66">
@@ -9793,16 +9703,16 @@
         <v>150</v>
       </c>
       <c r="AE65" s="63"/>
-      <c r="AF65" s="138"/>
+      <c r="AF65" s="133"/>
     </row>
     <row r="66" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="126" t="s">
+      <c r="A66" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="121" t="s">
         <v>244</v>
       </c>
-      <c r="C66" s="127" t="s">
+      <c r="C66" s="122" t="s">
         <v>66</v>
       </c>
       <c r="D66" s="66">
@@ -9895,13 +9805,13 @@
       </c>
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A67" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="126" t="s">
+      <c r="A67" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="121" t="s">
         <v>242</v>
       </c>
-      <c r="C67" s="127" t="s">
+      <c r="C67" s="122" t="s">
         <v>66</v>
       </c>
       <c r="D67" s="66">
@@ -10093,7 +10003,7 @@
       </c>
     </row>
     <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="140" t="s">
+      <c r="A69" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B69" s="49" t="s">
@@ -10191,7 +10101,7 @@
       </c>
     </row>
     <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="140" t="s">
+      <c r="A70" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B70" s="49" t="s">
@@ -10286,7 +10196,7 @@
       <c r="AF70" s="79"/>
     </row>
     <row r="71" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="140" t="s">
+      <c r="A71" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B71" s="49" t="s">
@@ -10381,13 +10291,13 @@
       <c r="AF71" s="79"/>
     </row>
     <row r="72" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" s="124" t="s">
+      <c r="A72" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="119" t="s">
         <v>230</v>
       </c>
-      <c r="C72" s="125" t="s">
+      <c r="C72" s="120" t="s">
         <v>229</v>
       </c>
       <c r="D72" s="66">
@@ -10474,18 +10384,18 @@
       <c r="AE72" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="AF72" s="138" t="s">
+      <c r="AF72" s="133" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="124" t="s">
+      <c r="A73" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="119" t="s">
         <v>225</v>
       </c>
-      <c r="C73" s="125" t="s">
+      <c r="C73" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D73" s="66">
@@ -10572,13 +10482,13 @@
       <c r="AF73" s="63"/>
     </row>
     <row r="74" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="126" t="s">
+      <c r="A74" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="121" t="s">
         <v>223</v>
       </c>
-      <c r="C74" s="127" t="s">
+      <c r="C74" s="122" t="s">
         <v>61</v>
       </c>
       <c r="D74" s="66">
@@ -10662,16 +10572,16 @@
         <v>58</v>
       </c>
       <c r="AE74" s="63"/>
-      <c r="AF74" s="138"/>
+      <c r="AF74" s="133"/>
     </row>
     <row r="75" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="126" t="s">
+      <c r="A75" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="121" t="s">
         <v>221</v>
       </c>
-      <c r="C75" s="127" t="s">
+      <c r="C75" s="122" t="s">
         <v>66</v>
       </c>
       <c r="D75" s="66">
@@ -10763,7 +10673,7 @@
       </c>
     </row>
     <row r="76" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="140" t="s">
+      <c r="A76" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B76" s="49" t="s">
@@ -10859,7 +10769,7 @@
       <c r="AF76" s="68"/>
     </row>
     <row r="77" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="140" t="s">
+      <c r="A77" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B77" s="49" t="s">
@@ -10952,7 +10862,7 @@
       <c r="AE77" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF77" s="158" t="s">
+      <c r="AF77" s="153" t="s">
         <v>213</v>
       </c>
     </row>
@@ -11051,7 +10961,7 @@
       <c r="AE78" s="68" t="s">
         <v>207</v>
       </c>
-      <c r="AF78" s="158" t="s">
+      <c r="AF78" s="153" t="s">
         <v>206</v>
       </c>
     </row>
@@ -11150,13 +11060,13 @@
       <c r="AF79" s="74"/>
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A80" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="124" t="s">
+      <c r="A80" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="119" t="s">
         <v>429</v>
       </c>
-      <c r="C80" s="125" t="s">
+      <c r="C80" s="120" t="s">
         <v>82</v>
       </c>
       <c r="D80" s="66">
@@ -11242,16 +11152,16 @@
         <v>98</v>
       </c>
       <c r="AE80" s="63"/>
-      <c r="AF80" s="123"/>
+      <c r="AF80" s="118"/>
     </row>
     <row r="81" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A81" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81" s="124" t="s">
+      <c r="A81" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="119" t="s">
         <v>430</v>
       </c>
-      <c r="C81" s="125" t="s">
+      <c r="C81" s="120" t="s">
         <v>82</v>
       </c>
       <c r="D81" s="66">
@@ -11340,13 +11250,13 @@
       <c r="AF81" s="71"/>
     </row>
     <row r="82" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A82" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82" s="126" t="s">
+      <c r="A82" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="121" t="s">
         <v>436</v>
       </c>
-      <c r="C82" s="127" t="s">
+      <c r="C82" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D82" s="66">
@@ -11433,18 +11343,18 @@
       <c r="AE82" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="AF82" s="123" t="s">
+      <c r="AF82" s="118" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A83" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" s="126" t="s">
+      <c r="A83" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="C83" s="127" t="s">
+      <c r="C83" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D83" s="66">
@@ -11529,10 +11439,10 @@
         <v>192</v>
       </c>
       <c r="AE83" s="63"/>
-      <c r="AF83" s="123"/>
+      <c r="AF83" s="118"/>
     </row>
     <row r="84" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="140" t="s">
+      <c r="A84" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B84" s="49" t="s">
@@ -11827,7 +11737,7 @@
       </c>
     </row>
     <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="140" t="s">
+      <c r="A87" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B87" s="49" t="s">
@@ -11925,13 +11835,13 @@
       </c>
     </row>
     <row r="88" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A88" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88" s="124" t="s">
+      <c r="A88" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="119" t="s">
         <v>191</v>
       </c>
-      <c r="C88" s="125" t="s">
+      <c r="C88" s="120" t="s">
         <v>24</v>
       </c>
       <c r="D88" s="66">
@@ -12019,18 +11929,18 @@
       <c r="AE88" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="AF88" s="131" t="s">
+      <c r="AF88" s="126" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="124" t="s">
+      <c r="A89" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="119" t="s">
         <v>189</v>
       </c>
-      <c r="C89" s="125" t="s">
+      <c r="C89" s="120" t="s">
         <v>24</v>
       </c>
       <c r="D89" s="66">
@@ -12069,7 +11979,7 @@
       <c r="O89" s="32">
         <v>5</v>
       </c>
-      <c r="P89" s="134">
+      <c r="P89" s="129">
         <v>5</v>
       </c>
       <c r="Q89" s="32">
@@ -12117,18 +12027,18 @@
       <c r="AE89" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="AF89" s="136" t="s">
+      <c r="AF89" s="131" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="90" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="126" t="s">
+      <c r="A90" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="C90" s="127" t="s">
+      <c r="C90" s="122" t="s">
         <v>24</v>
       </c>
       <c r="D90" s="66">
@@ -12167,7 +12077,7 @@
       <c r="O90" s="32">
         <v>5</v>
       </c>
-      <c r="P90" s="134">
+      <c r="P90" s="129">
         <v>4</v>
       </c>
       <c r="Q90" s="32">
@@ -12215,18 +12125,18 @@
       <c r="AE90" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="AF90" s="136" t="s">
+      <c r="AF90" s="131" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" s="126" t="s">
+      <c r="A91" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="127" t="s">
+      <c r="C91" s="122" t="s">
         <v>24</v>
       </c>
       <c r="D91" s="66">
@@ -12265,7 +12175,7 @@
       <c r="O91" s="32">
         <v>5</v>
       </c>
-      <c r="P91" s="134">
+      <c r="P91" s="129">
         <v>5</v>
       </c>
       <c r="Q91" s="32">
@@ -12313,7 +12223,7 @@
       <c r="AE91" s="34" t="s">
         <v>499</v>
       </c>
-      <c r="AF91" s="136" t="s">
+      <c r="AF91" s="131" t="s">
         <v>178</v>
       </c>
     </row>
@@ -12600,7 +12510,7 @@
       <c r="AF94" s="43"/>
     </row>
     <row r="95" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="140" t="s">
+      <c r="A95" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B95" s="49" t="s">
@@ -12645,14 +12555,14 @@
       <c r="O95" s="32">
         <v>5</v>
       </c>
-      <c r="P95" s="134">
+      <c r="P95" s="129">
         <v>0</v>
       </c>
       <c r="Q95" s="32">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>0</v>
       </c>
-      <c r="R95" s="146" t="b">
+      <c r="R95" s="141" t="b">
         <v>1</v>
       </c>
       <c r="S95" s="28" t="b">
@@ -12695,13 +12605,13 @@
       <c r="AF95" s="43"/>
     </row>
     <row r="96" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B96" s="124" t="s">
+      <c r="A96" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="119" t="s">
         <v>169</v>
       </c>
-      <c r="C96" s="125" t="s">
+      <c r="C96" s="120" t="s">
         <v>82</v>
       </c>
       <c r="D96" s="66">
@@ -12788,18 +12698,18 @@
       <c r="AE96" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="AF96" s="136" t="s">
+      <c r="AF96" s="131" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B97" s="124" t="s">
+      <c r="A97" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="119" t="s">
         <v>438</v>
       </c>
-      <c r="C97" s="125" t="s">
+      <c r="C97" s="120" t="s">
         <v>82</v>
       </c>
       <c r="D97" s="66">
@@ -12886,18 +12796,18 @@
       <c r="AE97" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="AF97" s="136" t="s">
+      <c r="AF97" s="131" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="98" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B98" s="126" t="s">
+      <c r="A98" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="121" t="s">
         <v>165</v>
       </c>
-      <c r="C98" s="127" t="s">
+      <c r="C98" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D98" s="66">
@@ -12985,13 +12895,13 @@
       <c r="AF98" s="62"/>
     </row>
     <row r="99" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A99" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B99" s="126" t="s">
+      <c r="A99" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="121" t="s">
         <v>161</v>
       </c>
-      <c r="C99" s="127" t="s">
+      <c r="C99" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D99" s="66">
@@ -13077,7 +12987,7 @@
         <v>158</v>
       </c>
       <c r="AE99" s="34"/>
-      <c r="AF99" s="131"/>
+      <c r="AF99" s="126"/>
     </row>
     <row r="100" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A100" s="49" t="s">
@@ -13224,7 +13134,7 @@
       <c r="O101" s="32">
         <v>5</v>
       </c>
-      <c r="P101" s="134">
+      <c r="P101" s="129">
         <v>0</v>
       </c>
       <c r="Q101" s="32">
@@ -13367,7 +13277,7 @@
       <c r="AF102" s="59"/>
     </row>
     <row r="103" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="140" t="s">
+      <c r="A103" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B103" s="49" t="s">
@@ -13406,13 +13316,13 @@
       <c r="M103" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="N103" s="137">
+      <c r="N103" s="132">
         <v>5</v>
       </c>
       <c r="O103" s="32">
         <v>5</v>
       </c>
-      <c r="P103" s="134">
+      <c r="P103" s="129">
         <v>2</v>
       </c>
       <c r="Q103" s="32">
@@ -13462,7 +13372,7 @@
       <c r="AF103" s="56"/>
     </row>
     <row r="104" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="140" t="s">
+      <c r="A104" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B104" s="49" t="s">
@@ -13556,13 +13466,13 @@
       <c r="AF104" s="59"/>
     </row>
     <row r="105" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A105" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="124" t="s">
+      <c r="A105" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="119" t="s">
         <v>151</v>
       </c>
-      <c r="C105" s="125" t="s">
+      <c r="C105" s="120" t="s">
         <v>66</v>
       </c>
       <c r="D105" s="66">
@@ -13649,18 +13559,18 @@
       <c r="AE105" s="34" t="s">
         <v>470</v>
       </c>
-      <c r="AF105" s="131" t="s">
+      <c r="AF105" s="126" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A106" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="124" t="s">
+      <c r="A106" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="119" t="s">
         <v>147</v>
       </c>
-      <c r="C106" s="125" t="s">
+      <c r="C106" s="120" t="s">
         <v>82</v>
       </c>
       <c r="D106" s="66">
@@ -13699,7 +13609,7 @@
       <c r="O106" s="32">
         <v>0</v>
       </c>
-      <c r="P106" s="134">
+      <c r="P106" s="129">
         <v>1</v>
       </c>
       <c r="Q106" s="32">
@@ -13711,7 +13621,7 @@
       <c r="S106" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="T106" s="135" t="b">
+      <c r="T106" s="130" t="b">
         <v>0</v>
       </c>
       <c r="U106" s="36">
@@ -13745,16 +13655,16 @@
         <v>144</v>
       </c>
       <c r="AE106" s="34"/>
-      <c r="AF106" s="136"/>
+      <c r="AF106" s="131"/>
     </row>
     <row r="107" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A107" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="126" t="s">
+      <c r="A107" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="121" t="s">
         <v>143</v>
       </c>
-      <c r="C107" s="127" t="s">
+      <c r="C107" s="122" t="s">
         <v>87</v>
       </c>
       <c r="D107" s="66">
@@ -13793,7 +13703,7 @@
       <c r="O107" s="32">
         <v>2</v>
       </c>
-      <c r="P107" s="134">
+      <c r="P107" s="129">
         <v>3</v>
       </c>
       <c r="Q107" s="32">
@@ -13805,7 +13715,7 @@
       <c r="S107" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="T107" s="135" t="b">
+      <c r="T107" s="130" t="b">
         <v>0</v>
       </c>
       <c r="U107" s="36">
@@ -13839,16 +13749,16 @@
         <v>71</v>
       </c>
       <c r="AE107" s="34"/>
-      <c r="AF107" s="131"/>
+      <c r="AF107" s="126"/>
     </row>
     <row r="108" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A108" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B108" s="126" t="s">
+      <c r="A108" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="121" t="s">
         <v>142</v>
       </c>
-      <c r="C108" s="127" t="s">
+      <c r="C108" s="122" t="s">
         <v>66</v>
       </c>
       <c r="D108" s="66">
@@ -13887,7 +13797,7 @@
       <c r="O108" s="32">
         <v>5</v>
       </c>
-      <c r="P108" s="134">
+      <c r="P108" s="129">
         <v>2</v>
       </c>
       <c r="Q108" s="32">
@@ -13934,7 +13844,7 @@
         <v>21</v>
       </c>
       <c r="AE108" s="34"/>
-      <c r="AF108" s="136"/>
+      <c r="AF108" s="131"/>
     </row>
     <row r="109" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A109" s="49" t="s">
@@ -14130,40 +14040,40 @@
       <c r="AF110" s="43"/>
     </row>
     <row r="111" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A111" s="141" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" s="143" t="s">
+      <c r="A111" s="136" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="138" t="s">
         <v>135</v>
       </c>
-      <c r="C111" s="144" t="s">
+      <c r="C111" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="D111" s="145">
+      <c r="D111" s="140">
         <v>120</v>
       </c>
-      <c r="E111" s="145">
+      <c r="E111" s="140">
         <v>17</v>
       </c>
-      <c r="F111" s="145">
-        <v>0</v>
-      </c>
-      <c r="G111" s="145">
+      <c r="F111" s="140">
+        <v>0</v>
+      </c>
+      <c r="G111" s="140">
         <v>50</v>
       </c>
-      <c r="H111" s="145">
-        <v>0</v>
-      </c>
-      <c r="I111" s="145">
+      <c r="H111" s="140">
+        <v>0</v>
+      </c>
+      <c r="I111" s="140">
         <v>70</v>
       </c>
-      <c r="J111" s="145">
+      <c r="J111" s="140">
         <v>0</v>
       </c>
       <c r="K111" s="42">
         <v>0.15</v>
       </c>
-      <c r="L111" s="145">
+      <c r="L111" s="140">
         <v>0</v>
       </c>
       <c r="M111" s="27" t="b">
@@ -14228,40 +14138,40 @@
       </c>
     </row>
     <row r="112" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A112" s="141" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="143" t="s">
+      <c r="A112" s="136" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="138" t="s">
         <v>129</v>
       </c>
-      <c r="C112" s="144" t="s">
+      <c r="C112" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="D112" s="145">
+      <c r="D112" s="140">
         <v>60</v>
       </c>
-      <c r="E112" s="145">
+      <c r="E112" s="140">
         <v>17</v>
       </c>
-      <c r="F112" s="145">
-        <v>0</v>
-      </c>
-      <c r="G112" s="145">
+      <c r="F112" s="140">
+        <v>0</v>
+      </c>
+      <c r="G112" s="140">
         <v>30</v>
       </c>
-      <c r="H112" s="145">
-        <v>0</v>
-      </c>
-      <c r="I112" s="145">
+      <c r="H112" s="140">
+        <v>0</v>
+      </c>
+      <c r="I112" s="140">
         <v>75</v>
       </c>
-      <c r="J112" s="145">
+      <c r="J112" s="140">
         <v>0</v>
       </c>
       <c r="K112" s="42">
         <v>0.15</v>
       </c>
-      <c r="L112" s="145">
+      <c r="L112" s="140">
         <v>0</v>
       </c>
       <c r="M112" s="27" t="b">
@@ -14326,13 +14236,13 @@
       </c>
     </row>
     <row r="113" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A113" s="129" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" s="142" t="s">
+      <c r="A113" s="124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C113" s="130" t="s">
+      <c r="C113" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D113" s="66">
@@ -14420,18 +14330,18 @@
       <c r="AE113" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="AF113" s="136" t="s">
+      <c r="AF113" s="131" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A114" s="129" t="s">
-        <v>2</v>
-      </c>
-      <c r="B114" s="142" t="s">
+      <c r="A114" s="124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="137" t="s">
         <v>118</v>
       </c>
-      <c r="C114" s="130" t="s">
+      <c r="C114" s="125" t="s">
         <v>82</v>
       </c>
       <c r="D114" s="38">
@@ -14519,18 +14429,18 @@
       <c r="AE114" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="AF114" s="136" t="s">
+      <c r="AF114" s="131" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A115" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" s="126" t="s">
+      <c r="A115" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="121" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="127" t="s">
+      <c r="C115" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D115" s="66">
@@ -14616,16 +14526,16 @@
         <v>109</v>
       </c>
       <c r="AE115" s="34"/>
-      <c r="AF115" s="136"/>
+      <c r="AF115" s="131"/>
     </row>
     <row r="116" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A116" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B116" s="126" t="s">
+      <c r="A116" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="121" t="s">
         <v>108</v>
       </c>
-      <c r="C116" s="127" t="s">
+      <c r="C116" s="122" t="s">
         <v>82</v>
       </c>
       <c r="D116" s="66">
@@ -14711,7 +14621,7 @@
         <v>105</v>
       </c>
       <c r="AE116" s="34"/>
-      <c r="AF116" s="136"/>
+      <c r="AF116" s="131"/>
     </row>
     <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" s="49" t="s">
@@ -14809,7 +14719,7 @@
       <c r="AF117" s="43"/>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A118" s="140" t="s">
+      <c r="A118" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B118" s="49" t="s">
@@ -14904,7 +14814,7 @@
       <c r="AF118" s="74"/>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A119" s="140" t="s">
+      <c r="A119" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B119" s="49" t="s">
@@ -14997,12 +14907,12 @@
       <c r="AE119" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="AF119" s="158" t="s">
+      <c r="AF119" s="153" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="120" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A120" s="140" t="s">
+      <c r="A120" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B120" s="49" t="s">
@@ -15096,13 +15006,13 @@
       <c r="AF120" s="74"/>
     </row>
     <row r="121" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A121" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B121" s="126" t="s">
+      <c r="A121" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="C121" s="125" t="s">
+      <c r="C121" s="120" t="s">
         <v>87</v>
       </c>
       <c r="D121" s="66">
@@ -15190,13 +15100,13 @@
       <c r="AF121" s="63"/>
     </row>
     <row r="122" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A122" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B122" s="126" t="s">
+      <c r="A122" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="C122" s="125" t="s">
+      <c r="C122" s="120" t="s">
         <v>82</v>
       </c>
       <c r="D122" s="66">
@@ -15285,13 +15195,13 @@
       <c r="AF122" s="72"/>
     </row>
     <row r="123" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A123" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B123" s="126" t="s">
+      <c r="A123" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="C123" s="125" t="s">
+      <c r="C123" s="120" t="s">
         <v>66</v>
       </c>
       <c r="D123" s="66">
@@ -15378,18 +15288,18 @@
       <c r="AE123" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="AF123" s="123" t="s">
+      <c r="AF123" s="118" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="124" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A124" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B124" s="126" t="s">
+      <c r="A124" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="C124" s="125" t="s">
+      <c r="C124" s="120" t="s">
         <v>68</v>
       </c>
       <c r="D124" s="66">
@@ -15452,16 +15362,16 @@
       <c r="W124" s="27">
         <v>0</v>
       </c>
-      <c r="X124" s="147">
+      <c r="X124" s="142">
         <v>0.25</v>
       </c>
-      <c r="Y124" s="147">
+      <c r="Y124" s="142">
         <v>0.25</v>
       </c>
-      <c r="Z124" s="147">
+      <c r="Z124" s="142">
         <v>0.8</v>
       </c>
-      <c r="AA124" s="147">
+      <c r="AA124" s="142">
         <v>0</v>
       </c>
       <c r="AB124" s="35" t="s">
@@ -15477,7 +15387,7 @@
       <c r="AF124" s="24"/>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A125" s="140" t="s">
+      <c r="A125" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B125" s="49" t="s">
@@ -15571,7 +15481,7 @@
       <c r="AF125" s="79"/>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A126" s="140" t="s">
+      <c r="A126" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B126" s="49" t="s">
@@ -15665,7 +15575,7 @@
       <c r="AF126" s="74"/>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A127" s="140" t="s">
+      <c r="A127" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B127" s="49" t="s">
@@ -15719,32 +15629,32 @@
       <c r="R127" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S127" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="T127" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="U127" s="148">
-        <v>1</v>
-      </c>
-      <c r="V127" s="148"/>
-      <c r="W127" s="148">
+      <c r="S127" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T127" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U127" s="143">
+        <v>1</v>
+      </c>
+      <c r="V127" s="143"/>
+      <c r="W127" s="143">
         <v>0</v>
       </c>
       <c r="X127" s="55">
         <v>0</v>
       </c>
-      <c r="Y127" s="149">
-        <v>0</v>
-      </c>
-      <c r="Z127" s="149">
+      <c r="Y127" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z127" s="144">
         <v>0</v>
       </c>
       <c r="AA127" s="55">
         <v>0</v>
       </c>
-      <c r="AB127" s="153" t="s">
+      <c r="AB127" s="148" t="s">
         <v>224</v>
       </c>
       <c r="AC127" s="72" t="s">
@@ -15753,11 +15663,11 @@
       <c r="AD127" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE127" s="150"/>
-      <c r="AF127" s="151"/>
+      <c r="AE127" s="145"/>
+      <c r="AF127" s="146"/>
     </row>
     <row r="128" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="140" t="s">
+      <c r="A128" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B128" s="49" t="s">
@@ -15811,32 +15721,32 @@
       <c r="R128" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S128" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="T128" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="U128" s="148">
-        <v>1</v>
-      </c>
-      <c r="V128" s="148"/>
-      <c r="W128" s="148">
+      <c r="S128" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T128" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U128" s="143">
+        <v>1</v>
+      </c>
+      <c r="V128" s="143"/>
+      <c r="W128" s="143">
         <v>0</v>
       </c>
       <c r="X128" s="55">
         <v>0</v>
       </c>
-      <c r="Y128" s="149">
-        <v>0</v>
-      </c>
-      <c r="Z128" s="149">
+      <c r="Y128" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z128" s="144">
         <v>0</v>
       </c>
       <c r="AA128" s="55">
         <v>0</v>
       </c>
-      <c r="AB128" s="153" t="s">
+      <c r="AB128" s="148" t="s">
         <v>224</v>
       </c>
       <c r="AC128" s="72" t="s">
@@ -15845,17 +15755,17 @@
       <c r="AD128" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE128" s="150"/>
-      <c r="AF128" s="151"/>
+      <c r="AE128" s="145"/>
+      <c r="AF128" s="146"/>
     </row>
     <row r="129" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A129" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B129" s="126" t="s">
+      <c r="A129" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="121" t="s">
         <v>491</v>
       </c>
-      <c r="C129" s="125" t="s">
+      <c r="C129" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D129" s="66">
@@ -15928,7 +15838,7 @@
       <c r="AA129" s="52">
         <v>0</v>
       </c>
-      <c r="AB129" s="156" t="s">
+      <c r="AB129" s="151" t="s">
         <v>224</v>
       </c>
       <c r="AC129" s="72" t="s">
@@ -15941,13 +15851,13 @@
       <c r="AF129" s="63"/>
     </row>
     <row r="130" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A130" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B130" s="126" t="s">
+      <c r="A130" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" s="121" t="s">
         <v>492</v>
       </c>
-      <c r="C130" s="125" t="s">
+      <c r="C130" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D130" s="66">
@@ -16020,7 +15930,7 @@
       <c r="AA130" s="52">
         <v>0</v>
       </c>
-      <c r="AB130" s="156" t="s">
+      <c r="AB130" s="151" t="s">
         <v>224</v>
       </c>
       <c r="AC130" s="72" t="s">
@@ -16033,13 +15943,13 @@
       <c r="AF130" s="72"/>
     </row>
     <row r="131" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A131" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B131" s="126" t="s">
+      <c r="A131" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="121" t="s">
         <v>493</v>
       </c>
-      <c r="C131" s="125" t="s">
+      <c r="C131" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D131" s="66">
@@ -16112,7 +16022,7 @@
       <c r="AA131" s="52">
         <v>0</v>
       </c>
-      <c r="AB131" s="156" t="s">
+      <c r="AB131" s="151" t="s">
         <v>224</v>
       </c>
       <c r="AC131" s="72" t="s">
@@ -16125,13 +16035,13 @@
       <c r="AF131" s="71"/>
     </row>
     <row r="132" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A132" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B132" s="126" t="s">
+      <c r="A132" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="121" t="s">
         <v>494</v>
       </c>
-      <c r="C132" s="125" t="s">
+      <c r="C132" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D132" s="66">
@@ -16192,19 +16102,19 @@
       <c r="W132" s="27">
         <v>0</v>
       </c>
-      <c r="X132" s="147">
-        <v>0</v>
-      </c>
-      <c r="Y132" s="147">
-        <v>0</v>
-      </c>
-      <c r="Z132" s="147">
-        <v>0</v>
-      </c>
-      <c r="AA132" s="147">
-        <v>0</v>
-      </c>
-      <c r="AB132" s="157" t="s">
+      <c r="X132" s="142">
+        <v>0</v>
+      </c>
+      <c r="Y132" s="142">
+        <v>0</v>
+      </c>
+      <c r="Z132" s="142">
+        <v>0</v>
+      </c>
+      <c r="AA132" s="142">
+        <v>0</v>
+      </c>
+      <c r="AB132" s="152" t="s">
         <v>224</v>
       </c>
       <c r="AC132" s="25" t="s">
@@ -16217,7 +16127,7 @@
       <c r="AF132" s="24"/>
     </row>
     <row r="133" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A133" s="140" t="s">
+      <c r="A133" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B133" s="49" t="s">
@@ -16271,32 +16181,32 @@
       <c r="R133" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S133" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="T133" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="U133" s="148">
-        <v>1</v>
-      </c>
-      <c r="V133" s="148"/>
-      <c r="W133" s="148">
+      <c r="S133" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T133" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U133" s="143">
+        <v>1</v>
+      </c>
+      <c r="V133" s="143"/>
+      <c r="W133" s="143">
         <v>0</v>
       </c>
       <c r="X133" s="55">
         <v>0</v>
       </c>
-      <c r="Y133" s="149">
-        <v>0</v>
-      </c>
-      <c r="Z133" s="149">
+      <c r="Y133" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z133" s="144">
         <v>0</v>
       </c>
       <c r="AA133" s="55">
         <v>0</v>
       </c>
-      <c r="AB133" s="153" t="s">
+      <c r="AB133" s="148" t="s">
         <v>224</v>
       </c>
       <c r="AC133" s="72" t="s">
@@ -16305,11 +16215,11 @@
       <c r="AD133" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE133" s="150"/>
-      <c r="AF133" s="151"/>
+      <c r="AE133" s="145"/>
+      <c r="AF133" s="146"/>
     </row>
     <row r="134" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A134" s="140" t="s">
+      <c r="A134" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B134" s="49" t="s">
@@ -16327,7 +16237,7 @@
       <c r="F134" s="76">
         <v>0</v>
       </c>
-      <c r="G134" s="154">
+      <c r="G134" s="149">
         <v>-20</v>
       </c>
       <c r="H134" s="76">
@@ -16364,34 +16274,34 @@
       <c r="R134" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S134" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="T134" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="U134" s="148">
-        <v>1</v>
-      </c>
-      <c r="V134" s="148">
-        <v>2</v>
-      </c>
-      <c r="W134" s="148">
+      <c r="S134" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T134" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U134" s="143">
+        <v>1</v>
+      </c>
+      <c r="V134" s="143">
+        <v>2</v>
+      </c>
+      <c r="W134" s="143">
         <v>0</v>
       </c>
       <c r="X134" s="55">
         <v>1</v>
       </c>
-      <c r="Y134" s="149">
-        <v>1</v>
-      </c>
-      <c r="Z134" s="149">
+      <c r="Y134" s="144">
+        <v>1</v>
+      </c>
+      <c r="Z134" s="144">
         <v>0</v>
       </c>
       <c r="AA134" s="55">
         <v>0</v>
       </c>
-      <c r="AB134" s="153" t="s">
+      <c r="AB134" s="148" t="s">
         <v>338</v>
       </c>
       <c r="AC134" s="72" t="s">
@@ -16400,11 +16310,11 @@
       <c r="AD134" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="AE134" s="150"/>
-      <c r="AF134" s="151"/>
+      <c r="AE134" s="145"/>
+      <c r="AF134" s="146"/>
     </row>
     <row r="135" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A135" s="140" t="s">
+      <c r="A135" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B135" s="49" t="s">
@@ -16422,7 +16332,7 @@
       <c r="F135" s="76">
         <v>1</v>
       </c>
-      <c r="G135" s="154">
+      <c r="G135" s="149">
         <v>0</v>
       </c>
       <c r="H135" s="76">
@@ -16458,32 +16368,32 @@
       <c r="R135" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S135" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="T135" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="U135" s="148">
-        <v>1</v>
-      </c>
-      <c r="V135" s="148"/>
-      <c r="W135" s="148">
+      <c r="S135" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T135" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U135" s="143">
+        <v>1</v>
+      </c>
+      <c r="V135" s="143"/>
+      <c r="W135" s="143">
         <v>0</v>
       </c>
       <c r="X135" s="55">
         <v>0</v>
       </c>
-      <c r="Y135" s="149">
-        <v>0</v>
-      </c>
-      <c r="Z135" s="149">
+      <c r="Y135" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z135" s="144">
         <v>0</v>
       </c>
       <c r="AA135" s="55">
         <v>0</v>
       </c>
-      <c r="AB135" s="153" t="s">
+      <c r="AB135" s="148" t="s">
         <v>224</v>
       </c>
       <c r="AC135" s="72" t="s">
@@ -16492,11 +16402,11 @@
       <c r="AD135" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE135" s="150"/>
-      <c r="AF135" s="151"/>
+      <c r="AE135" s="145"/>
+      <c r="AF135" s="146"/>
     </row>
     <row r="136" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A136" s="140" t="s">
+      <c r="A136" s="135" t="s">
         <v>2</v>
       </c>
       <c r="B136" s="49" t="s">
@@ -16514,7 +16424,7 @@
       <c r="F136" s="76">
         <v>0</v>
       </c>
-      <c r="G136" s="154">
+      <c r="G136" s="149">
         <v>0</v>
       </c>
       <c r="H136" s="76">
@@ -16550,32 +16460,32 @@
       <c r="R136" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S136" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="T136" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="U136" s="148">
-        <v>1</v>
-      </c>
-      <c r="V136" s="148"/>
-      <c r="W136" s="148">
+      <c r="S136" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T136" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U136" s="143">
+        <v>1</v>
+      </c>
+      <c r="V136" s="143"/>
+      <c r="W136" s="143">
         <v>0</v>
       </c>
       <c r="X136" s="55">
         <v>0</v>
       </c>
-      <c r="Y136" s="149">
-        <v>0</v>
-      </c>
-      <c r="Z136" s="149">
+      <c r="Y136" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z136" s="144">
         <v>0</v>
       </c>
       <c r="AA136" s="55">
         <v>0</v>
       </c>
-      <c r="AB136" s="153" t="s">
+      <c r="AB136" s="148" t="s">
         <v>224</v>
       </c>
       <c r="AC136" s="72" t="s">
@@ -16584,17 +16494,17 @@
       <c r="AD136" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AE136" s="150"/>
-      <c r="AF136" s="151"/>
+      <c r="AE136" s="145"/>
+      <c r="AF136" s="146"/>
     </row>
     <row r="137" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A137" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B137" s="126" t="s">
+      <c r="A137" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" s="121" t="s">
         <v>501</v>
       </c>
-      <c r="C137" s="125" t="s">
+      <c r="C137" s="120" t="s">
         <v>68</v>
       </c>
       <c r="D137" s="66">
@@ -16657,16 +16567,16 @@
       <c r="W137" s="27">
         <v>0</v>
       </c>
-      <c r="X137" s="147">
+      <c r="X137" s="142">
         <v>0.25</v>
       </c>
-      <c r="Y137" s="147">
+      <c r="Y137" s="142">
         <v>0.25</v>
       </c>
-      <c r="Z137" s="147">
+      <c r="Z137" s="142">
         <v>0.8</v>
       </c>
-      <c r="AA137" s="147">
+      <c r="AA137" s="142">
         <v>0</v>
       </c>
       <c r="AB137" s="35" t="s">
@@ -16682,13 +16592,13 @@
       <c r="AF137" s="24"/>
     </row>
     <row r="138" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B138" s="126" t="s">
+      <c r="A138" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="121" t="s">
         <v>502</v>
       </c>
-      <c r="C138" s="125" t="s">
+      <c r="C138" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D138" s="66">
@@ -16761,7 +16671,7 @@
       <c r="AA138" s="52">
         <v>0</v>
       </c>
-      <c r="AB138" s="156" t="s">
+      <c r="AB138" s="151" t="s">
         <v>224</v>
       </c>
       <c r="AC138" s="72" t="s">
@@ -16774,13 +16684,13 @@
       <c r="AF138" s="71"/>
     </row>
     <row r="139" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A139" s="128" t="s">
-        <v>2</v>
-      </c>
-      <c r="B139" s="126" t="s">
+      <c r="A139" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="121" t="s">
         <v>503</v>
       </c>
-      <c r="C139" s="125" t="s">
+      <c r="C139" s="120" t="s">
         <v>61</v>
       </c>
       <c r="D139" s="66">
@@ -16801,7 +16711,7 @@
       <c r="I139" s="65">
         <v>25</v>
       </c>
-      <c r="J139" s="173">
+      <c r="J139" s="154">
         <v>2500</v>
       </c>
       <c r="K139" s="53">
@@ -16855,7 +16765,7 @@
       <c r="AA139" s="52">
         <v>0</v>
       </c>
-      <c r="AB139" s="156" t="s">
+      <c r="AB139" s="151" t="s">
         <v>224</v>
       </c>
       <c r="AC139" s="72" t="s">
@@ -16868,38 +16778,99 @@
       <c r="AF139" s="71"/>
     </row>
     <row r="140" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A140" s="159"/>
-      <c r="B140" s="118"/>
-      <c r="C140" s="118"/>
-      <c r="D140" s="119"/>
-      <c r="E140" s="120"/>
-      <c r="F140" s="120"/>
-      <c r="G140" s="120"/>
-      <c r="H140" s="120"/>
-      <c r="I140" s="120"/>
-      <c r="J140" s="160"/>
-      <c r="K140" s="161"/>
-      <c r="L140" s="120"/>
-      <c r="M140" s="121"/>
-      <c r="N140" s="162"/>
-      <c r="O140" s="162"/>
-      <c r="P140" s="163"/>
-      <c r="Q140" s="162"/>
-      <c r="R140" s="164"/>
-      <c r="S140" s="165"/>
-      <c r="T140" s="165"/>
-      <c r="U140" s="164"/>
-      <c r="V140" s="122"/>
-      <c r="W140" s="121"/>
-      <c r="X140" s="166"/>
-      <c r="Y140" s="167"/>
-      <c r="Z140" s="167"/>
-      <c r="AA140" s="168"/>
-      <c r="AB140" s="169"/>
-      <c r="AC140" s="170"/>
-      <c r="AD140" s="171"/>
-      <c r="AE140" s="171"/>
-      <c r="AF140" s="172"/>
+      <c r="A140" s="123" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" s="121" t="s">
+        <v>504</v>
+      </c>
+      <c r="C140" s="120" t="s">
+        <v>82</v>
+      </c>
+      <c r="D140" s="66">
+        <v>30</v>
+      </c>
+      <c r="E140" s="65">
+        <v>20</v>
+      </c>
+      <c r="F140" s="65">
+        <v>0</v>
+      </c>
+      <c r="G140" s="65">
+        <v>5</v>
+      </c>
+      <c r="H140" s="65">
+        <v>0</v>
+      </c>
+      <c r="I140" s="65">
+        <v>40</v>
+      </c>
+      <c r="J140" s="154">
+        <v>0</v>
+      </c>
+      <c r="K140" s="53">
+        <v>0.15</v>
+      </c>
+      <c r="L140" s="65">
+        <v>0</v>
+      </c>
+      <c r="M140" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N140" s="40">
+        <v>5</v>
+      </c>
+      <c r="O140" s="37">
+        <v>5</v>
+      </c>
+      <c r="P140" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q140" s="40">
+        <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
+        <v>0</v>
+      </c>
+      <c r="R140" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S140" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="T140" s="73" t="b">
+        <v>0</v>
+      </c>
+      <c r="U140" s="36">
+        <v>1</v>
+      </c>
+      <c r="V140" s="36">
+        <v>2</v>
+      </c>
+      <c r="W140" s="36">
+        <v>0</v>
+      </c>
+      <c r="X140" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="Y140" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="Z140" s="52">
+        <v>0</v>
+      </c>
+      <c r="AA140" s="52">
+        <v>0</v>
+      </c>
+      <c r="AB140" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC140" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD140" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE140" s="72"/>
+      <c r="AF140" s="71"/>
     </row>
     <row r="141" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="142" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
@@ -16940,8 +16911,8 @@
       <c r="C143" s="22"/>
       <c r="D143" s="22"/>
       <c r="E143" s="22"/>
-      <c r="F143" s="174"/>
-      <c r="G143" s="174"/>
+      <c r="F143" s="155"/>
+      <c r="G143" s="155"/>
       <c r="H143" s="21" t="s">
         <v>56</v>
       </c>
@@ -17565,22 +17536,22 @@
       <c r="C156" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="D156" s="132" t="s">
+      <c r="D156" s="127" t="s">
         <v>30</v>
       </c>
       <c r="E156" s="14">
         <v>1</v>
       </c>
-      <c r="F156" s="133">
-        <v>0</v>
-      </c>
-      <c r="G156" s="133">
-        <v>0</v>
-      </c>
-      <c r="H156" s="133">
-        <v>0</v>
-      </c>
-      <c r="I156" s="133">
+      <c r="F156" s="128">
+        <v>0</v>
+      </c>
+      <c r="G156" s="128">
+        <v>0</v>
+      </c>
+      <c r="H156" s="128">
+        <v>0</v>
+      </c>
+      <c r="I156" s="128">
         <v>0</v>
       </c>
       <c r="J156" s="12">
@@ -17898,17 +17869,17 @@
     <mergeCell ref="F143:G143"/>
   </mergeCells>
   <conditionalFormatting sqref="M118:M124 R118:T124 M24:M56 R24:T56 S127:T127 M127 R58:T115 M58:M115">
-    <cfRule type="expression" dxfId="114" priority="65">
+    <cfRule type="expression" dxfId="116" priority="69">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="113" priority="58">
+    <cfRule type="expression" dxfId="115" priority="62">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116:Q116">
-    <cfRule type="colorScale" priority="57">
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17920,12 +17891,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="112" priority="52">
+    <cfRule type="expression" dxfId="114" priority="56">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N115:Q119">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17937,7 +17908,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N118:Q124 N24:Q56 N58:Q115">
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17949,11 +17920,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="111" priority="50">
+    <cfRule type="expression" dxfId="113" priority="54">
       <formula>M114=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N114:Q114">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M125:M126 R125:T126">
+    <cfRule type="expression" dxfId="112" priority="51">
+      <formula>M125=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M125 R125:T125">
+    <cfRule type="expression" dxfId="111" priority="50">
+      <formula>M125=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N125:Q125">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -17965,30 +17958,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="110" priority="47">
-      <formula>M125=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="109" priority="46">
-      <formula>M125=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N125:Q125">
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q127">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18000,17 +17971,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="108" priority="44">
+    <cfRule type="expression" dxfId="110" priority="48">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="107" priority="43">
+    <cfRule type="expression" dxfId="109" priority="47">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:Q128">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18022,21 +17993,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="106" priority="41">
+    <cfRule type="expression" dxfId="108" priority="45">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="105" priority="26">
+    <cfRule type="expression" dxfId="107" priority="30">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="104" priority="28">
+    <cfRule type="expression" dxfId="106" priority="32">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N133:Q133">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S134:T134 M134">
+    <cfRule type="expression" dxfId="105" priority="25">
+      <formula>M134=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M129:M132 R129:T132">
+    <cfRule type="expression" dxfId="104" priority="26">
+      <formula>M129=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N129:Q132">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -18048,30 +18041,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="103" priority="21">
-      <formula>M134=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="102" priority="22">
-      <formula>M129=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N129:Q132">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N134:Q134">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18083,17 +18054,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="101" priority="19">
+    <cfRule type="expression" dxfId="103" priority="23">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="100" priority="14">
+    <cfRule type="expression" dxfId="102" priority="18">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N135:Q135">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18105,16 +18076,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="99" priority="16">
+    <cfRule type="expression" dxfId="101" priority="20">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="98" priority="9">
+    <cfRule type="expression" dxfId="100" priority="13">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N136:Q136">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S136:T136 M136">
+    <cfRule type="expression" dxfId="99" priority="15">
+      <formula>M136=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M138 R138:T138">
+    <cfRule type="expression" dxfId="98" priority="11">
+      <formula>M138=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N138:Q138">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M57 R57:T57">
+    <cfRule type="expression" dxfId="97" priority="9">
+      <formula>M57=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N57:Q57">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -18126,17 +18136,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="97" priority="11">
-      <formula>M136=FALSE</formula>
+  <conditionalFormatting sqref="M137 R137:T137">
+    <cfRule type="expression" dxfId="96" priority="7">
+      <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="96" priority="7">
-      <formula>M138=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N138:Q138">
+  <conditionalFormatting sqref="N137:Q137">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -18148,12 +18153,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M57 R57:T57">
+  <conditionalFormatting sqref="M139 R139:T139">
     <cfRule type="expression" dxfId="95" priority="5">
-      <formula>M57=FALSE</formula>
+      <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57:Q57">
+  <conditionalFormatting sqref="N139:Q139">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -18165,29 +18170,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="94" priority="3">
-      <formula>M137=FALSE</formula>
+  <conditionalFormatting sqref="M140 R140:T140">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N137:Q137">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="93" priority="1">
-      <formula>M139=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N139:Q139">
+  <conditionalFormatting sqref="N140:Q140">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -18201,29 +18189,29 @@
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G134"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G133 J24:J138 H40:I140 G135:G140">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G133 J24:J138 G135:G140 H40:I140 J140">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D145:G156 M139:N140 P139:V140 N24:O138 Q24:W138">
+    <dataValidation type="decimal" allowBlank="1" sqref="D145:G156 P139:V139 Q24:W138 N24:O138 M139:N139 Q140:W140 N140:O140">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H145:L154 H155:I155 J156:L156 W139:Z140 X24:AA138">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H145:L154 H155:I155 J156:L156 X24:AA138 W139:Z139 X140:AA140">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C145:C156 C24:C140">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J155:L155 M145:O156 AB24:AB140 AC24:AC138 AA139:AC140 AD24:AF140"/>
-    <dataValidation type="list" sqref="O139:O140 P24:P138">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J155:L155 M145:O156 AA139:AC139 AC24:AC138 AD24:AF140 AB24:AB140 AC140"/>
+    <dataValidation type="list" sqref="P24:P138 O139 P140">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L138 K139:K140 J140">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L138 K139 K140:L140">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="L139:L140 M24:M138">
+    <dataValidation type="list" sqref="M24:M138 L139 M140">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F140">
@@ -18287,8 +18275,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="174"/>
-      <c r="G3" s="174"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
MexicanPepper FuryReward set to %
Former-commit-id: 55d9a0343440423a4e0e692e353c54dae68ee2e4
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5351,10 +5351,10 @@
   </sheetPr>
   <dimension ref="A1:AF173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A139" sqref="A139:XFD139"/>
+      <selection pane="topRight" activeCell="J105" sqref="J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13393,7 +13393,7 @@
         <v>25</v>
       </c>
       <c r="J104" s="76">
-        <v>2500</v>
+        <v>0.6</v>
       </c>
       <c r="K104" s="42">
         <v>0.22499999999999998</v>
@@ -16705,7 +16705,7 @@
         <v>25</v>
       </c>
       <c r="J139" s="154">
-        <v>2500</v>
+        <v>0.6</v>
       </c>
       <c r="K139" s="53">
         <v>0.23</v>

</xml_diff>

<commit_message>
Content - Jalapeno gives 30% and Fragile is now 80% dmg increased
Former-commit-id: ddf1e26db1d56d91065dc71a0e561c80ed36b808
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$144:$O$145</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5351,10 +5351,10 @@
   </sheetPr>
   <dimension ref="A1:AF173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="J105" sqref="J105"/>
+      <selection pane="topRight" activeCell="J130" sqref="J130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16705,7 +16705,7 @@
         <v>25</v>
       </c>
       <c r="J139" s="154">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="K139" s="53">
         <v>0.23</v>

</xml_diff>

<commit_message>
Miner has a different sku than Worker
Former-commit-id: 669b8c973eb20ef15396dbec9f7831ab0360b6df
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$144:$O$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$145:$O$146</definedName>
   </definedNames>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="506">
   <si>
     <t>tier_4</t>
   </si>
@@ -1556,6 +1556,9 @@
   </si>
   <si>
     <t>RatGrey</t>
+  </si>
+  <si>
+    <t>Miner</t>
   </si>
 </sst>
 </file>
@@ -2499,7 +2502,189 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="116">
+  <dxfs count="119">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4795,167 +4980,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4970,114 +4994,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF140" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF140"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF141" totalsRowShown="0" headerRowDxfId="118" dataDxfId="116" headerRowBorderDxfId="117" tableBorderDxfId="115" totalsRowBorderDxfId="114">
+  <autoFilter ref="A23:AF141"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="113"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="112"/>
+    <tableColumn id="6" name="[category]" dataDxfId="111"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="110"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="109"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="108"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="107"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="106"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="105"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="104"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="103"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="102"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="101"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="100"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="99"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="98"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="97"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="96"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="95"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="94"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="93"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="92"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="91"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="90"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="89"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="88"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="87"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="86"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="85"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="84"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="83"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="77"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A144:O156" totalsRowShown="0">
-  <autoFilter ref="A144:O156"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A145:O157" totalsRowShown="0">
+  <autoFilter ref="A145:O157"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="4" name="[category]" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="16" name="[size]" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="47" totalsRowDxfId="46"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="6" name="[order]" dataDxfId="39"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="38"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="37"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="36"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="29"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="27"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="26" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5349,12 +5373,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF173"/>
+  <dimension ref="A1:AF174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AC1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="J130" sqref="J130"/>
+      <selection pane="topRight" activeCell="AF141" sqref="AF141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16865,184 +16889,229 @@
       <c r="AE140" s="72"/>
       <c r="AF140" s="71"/>
     </row>
-    <row r="141" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="142" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A142" s="9" t="s">
+    <row r="141" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A141" s="135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="49" t="s">
+        <v>505</v>
+      </c>
+      <c r="C141" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="D141" s="61">
+        <v>80</v>
+      </c>
+      <c r="E141" s="76">
+        <v>4</v>
+      </c>
+      <c r="F141" s="76">
+        <v>0</v>
+      </c>
+      <c r="G141" s="149">
+        <v>12</v>
+      </c>
+      <c r="H141" s="76">
+        <v>0</v>
+      </c>
+      <c r="I141" s="76">
+        <v>90</v>
+      </c>
+      <c r="J141" s="76">
+        <v>0</v>
+      </c>
+      <c r="K141" s="42">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L141" s="76">
+        <v>0</v>
+      </c>
+      <c r="M141" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N141" s="40">
+        <v>5</v>
+      </c>
+      <c r="O141" s="40">
+        <v>0</v>
+      </c>
+      <c r="P141" s="81">
+        <v>1</v>
+      </c>
+      <c r="Q141" s="40">
+        <v>0</v>
+      </c>
+      <c r="R141" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S141" s="147" t="b">
+        <v>1</v>
+      </c>
+      <c r="T141" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U141" s="143">
+        <v>25</v>
+      </c>
+      <c r="V141" s="143">
+        <v>7</v>
+      </c>
+      <c r="W141" s="143">
+        <v>0</v>
+      </c>
+      <c r="X141" s="55">
+        <v>0.25</v>
+      </c>
+      <c r="Y141" s="144">
+        <v>0.25</v>
+      </c>
+      <c r="Z141" s="144">
+        <v>0.8</v>
+      </c>
+      <c r="AA141" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB141" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC141" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD141" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE141" s="145"/>
+      <c r="AF141" s="146"/>
+    </row>
+    <row r="142" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="143" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A143" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B142" s="9"/>
-      <c r="C142" s="9"/>
-      <c r="D142" s="9"/>
-      <c r="E142" s="9"/>
-      <c r="F142" s="9"/>
-      <c r="G142" s="9"/>
-      <c r="H142" s="9"/>
-      <c r="I142" s="9"/>
-      <c r="J142" s="9"/>
-      <c r="K142" s="9"/>
-      <c r="L142" s="9"/>
-      <c r="M142" s="9"/>
-      <c r="N142" s="9"/>
-      <c r="O142" s="9"/>
-      <c r="P142" s="9"/>
-      <c r="Q142" s="9"/>
-      <c r="R142" s="9"/>
-      <c r="S142" s="9"/>
-      <c r="T142" s="9"/>
-      <c r="U142" s="9"/>
-      <c r="V142" s="9"/>
-      <c r="W142" s="9"/>
-      <c r="X142" s="9"/>
-      <c r="Y142" s="9"/>
-      <c r="Z142" s="9"/>
-      <c r="AA142" s="9"/>
-      <c r="AF142" s="8"/>
-    </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A143" s="22"/>
-      <c r="B143" s="22"/>
-      <c r="C143" s="22"/>
-      <c r="D143" s="22"/>
-      <c r="E143" s="22"/>
-      <c r="F143" s="155"/>
-      <c r="G143" s="155"/>
-      <c r="H143" s="21" t="s">
+      <c r="B143" s="9"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+      <c r="H143" s="9"/>
+      <c r="I143" s="9"/>
+      <c r="J143" s="9"/>
+      <c r="K143" s="9"/>
+      <c r="L143" s="9"/>
+      <c r="M143" s="9"/>
+      <c r="N143" s="9"/>
+      <c r="O143" s="9"/>
+      <c r="P143" s="9"/>
+      <c r="Q143" s="9"/>
+      <c r="R143" s="9"/>
+      <c r="S143" s="9"/>
+      <c r="T143" s="9"/>
+      <c r="U143" s="9"/>
+      <c r="V143" s="9"/>
+      <c r="W143" s="9"/>
+      <c r="X143" s="9"/>
+      <c r="Y143" s="9"/>
+      <c r="Z143" s="9"/>
+      <c r="AA143" s="9"/>
+      <c r="AF143" s="8"/>
+    </row>
+    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A144" s="22"/>
+      <c r="B144" s="22"/>
+      <c r="C144" s="22"/>
+      <c r="D144" s="22"/>
+      <c r="E144" s="22"/>
+      <c r="F144" s="155"/>
+      <c r="G144" s="155"/>
+      <c r="H144" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I143" s="21"/>
-      <c r="J143" s="22"/>
-      <c r="K143" s="17"/>
-      <c r="L143" s="17"/>
-      <c r="M143" s="17" t="s">
+      <c r="I144" s="21"/>
+      <c r="J144" s="22"/>
+      <c r="K144" s="17"/>
+      <c r="L144" s="17"/>
+      <c r="M144" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N143" s="17"/>
-      <c r="O143" s="17"/>
-      <c r="P143" s="17"/>
-      <c r="Q143" s="17"/>
-      <c r="R143" s="17"/>
-      <c r="S143" s="17"/>
-      <c r="T143" s="17"/>
-      <c r="U143" s="17"/>
-      <c r="V143" s="17"/>
-      <c r="W143" s="17"/>
-      <c r="X143" s="17"/>
-      <c r="Y143" s="17"/>
-      <c r="Z143" s="17"/>
-      <c r="AA143" s="21"/>
-      <c r="AB143" s="21"/>
-      <c r="AC143" s="21"/>
-      <c r="AD143" s="21"/>
-      <c r="AE143" s="17"/>
-    </row>
-    <row r="144" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A144" s="7" t="s">
+      <c r="N144" s="17"/>
+      <c r="O144" s="17"/>
+      <c r="P144" s="17"/>
+      <c r="Q144" s="17"/>
+      <c r="R144" s="17"/>
+      <c r="S144" s="17"/>
+      <c r="T144" s="17"/>
+      <c r="U144" s="17"/>
+      <c r="V144" s="17"/>
+      <c r="W144" s="17"/>
+      <c r="X144" s="17"/>
+      <c r="Y144" s="17"/>
+      <c r="Z144" s="17"/>
+      <c r="AA144" s="21"/>
+      <c r="AB144" s="21"/>
+      <c r="AC144" s="21"/>
+      <c r="AD144" s="21"/>
+      <c r="AE144" s="17"/>
+    </row>
+    <row r="145" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B144" s="7" t="s">
+      <c r="B145" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C144" s="7" t="s">
+      <c r="C145" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D144" s="20" t="s">
+      <c r="D145" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E144" s="20" t="s">
+      <c r="E145" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F144" s="20" t="s">
+      <c r="F145" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G144" s="20" t="s">
+      <c r="G145" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H144" s="20" t="s">
+      <c r="H145" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I144" s="20" t="s">
+      <c r="I145" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J144" s="20" t="s">
+      <c r="J145" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K144" s="20" t="s">
+      <c r="K145" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="L144" s="20" t="s">
+      <c r="L145" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M144" s="19" t="s">
+      <c r="M145" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N144" s="19" t="s">
+      <c r="N145" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O144" s="19" t="s">
+      <c r="O145" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="145" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A145" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B145" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C145" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D145" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E145" s="14">
-        <v>3</v>
-      </c>
-      <c r="F145" s="18">
-        <v>0</v>
-      </c>
-      <c r="G145" s="18">
-        <v>0</v>
-      </c>
-      <c r="H145" s="18">
-        <v>0</v>
-      </c>
-      <c r="I145" s="18">
-        <v>0</v>
-      </c>
-      <c r="J145" s="12">
-        <v>2</v>
-      </c>
-      <c r="K145" s="12">
-        <v>0</v>
-      </c>
-      <c r="L145" s="12">
-        <v>0</v>
-      </c>
-      <c r="M145" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N145" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O145" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P145" s="17"/>
-      <c r="Q145" s="17"/>
     </row>
     <row r="146" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A146" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B146" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C146" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E146" s="14">
         <v>3</v>
@@ -17051,7 +17120,7 @@
         <v>0</v>
       </c>
       <c r="G146" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H146" s="18">
         <v>0</v>
@@ -17085,13 +17154,13 @@
         <v>2</v>
       </c>
       <c r="B147" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E147" s="14">
         <v>3</v>
@@ -17100,7 +17169,7 @@
         <v>0</v>
       </c>
       <c r="G147" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H147" s="18">
         <v>0</v>
@@ -17134,13 +17203,13 @@
         <v>2</v>
       </c>
       <c r="B148" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C148" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E148" s="14">
         <v>3</v>
@@ -17149,7 +17218,7 @@
         <v>0</v>
       </c>
       <c r="G148" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H148" s="18">
         <v>0</v>
@@ -17183,13 +17252,13 @@
         <v>2</v>
       </c>
       <c r="B149" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D149" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E149" s="14">
         <v>3</v>
@@ -17198,7 +17267,7 @@
         <v>0</v>
       </c>
       <c r="G149" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H149" s="18">
         <v>0</v>
@@ -17232,13 +17301,13 @@
         <v>2</v>
       </c>
       <c r="B150" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C150" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D150" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E150" s="14">
         <v>3</v>
@@ -17247,7 +17316,7 @@
         <v>0</v>
       </c>
       <c r="G150" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H150" s="18">
         <v>0</v>
@@ -17281,13 +17350,13 @@
         <v>2</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C151" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E151" s="14">
         <v>3</v>
@@ -17296,7 +17365,7 @@
         <v>0</v>
       </c>
       <c r="G151" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H151" s="18">
         <v>0</v>
@@ -17330,13 +17399,13 @@
         <v>2</v>
       </c>
       <c r="B152" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E152" s="14">
         <v>3</v>
@@ -17345,7 +17414,7 @@
         <v>0</v>
       </c>
       <c r="G152" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H152" s="18">
         <v>0</v>
@@ -17379,13 +17448,13 @@
         <v>2</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C153" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E153" s="14">
         <v>3</v>
@@ -17394,7 +17463,7 @@
         <v>0</v>
       </c>
       <c r="G153" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H153" s="18">
         <v>0</v>
@@ -17428,13 +17497,13 @@
         <v>2</v>
       </c>
       <c r="B154" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C154" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E154" s="14">
         <v>3</v>
@@ -17443,7 +17512,7 @@
         <v>0</v>
       </c>
       <c r="G154" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H154" s="18">
         <v>0</v>
@@ -17477,27 +17546,27 @@
         <v>2</v>
       </c>
       <c r="B155" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E155" s="14">
-        <v>1</v>
-      </c>
-      <c r="F155" s="13">
-        <v>0</v>
-      </c>
-      <c r="G155" s="13">
-        <v>1</v>
-      </c>
-      <c r="H155" s="13">
-        <v>0</v>
-      </c>
-      <c r="I155" s="13">
+        <v>3</v>
+      </c>
+      <c r="F155" s="18">
+        <v>0</v>
+      </c>
+      <c r="G155" s="18">
+        <v>2</v>
+      </c>
+      <c r="H155" s="18">
+        <v>0</v>
+      </c>
+      <c r="I155" s="18">
         <v>0</v>
       </c>
       <c r="J155" s="12">
@@ -17518,33 +17587,35 @@
       <c r="O155" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P155" s="17"/>
+      <c r="Q155" s="17"/>
     </row>
     <row r="156" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A156" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B156" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="C156" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="D156" s="127" t="s">
-        <v>30</v>
+      <c r="B156" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C156" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D156" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E156" s="14">
         <v>1</v>
       </c>
-      <c r="F156" s="128">
-        <v>0</v>
-      </c>
-      <c r="G156" s="128">
-        <v>0</v>
-      </c>
-      <c r="H156" s="128">
-        <v>0</v>
-      </c>
-      <c r="I156" s="128">
+      <c r="F156" s="13">
+        <v>0</v>
+      </c>
+      <c r="G156" s="13">
+        <v>1</v>
+      </c>
+      <c r="H156" s="13">
+        <v>0</v>
+      </c>
+      <c r="I156" s="13">
         <v>0</v>
       </c>
       <c r="J156" s="12">
@@ -17565,26 +17636,53 @@
       <c r="O156" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P156" s="8"/>
-      <c r="Q156" s="8"/>
-      <c r="R156" s="8"/>
-      <c r="S156" s="8"/>
-      <c r="T156" s="8"/>
-      <c r="U156" s="8"/>
-      <c r="V156" s="8"/>
-      <c r="W156" s="8"/>
-      <c r="X156" s="8"/>
-      <c r="Y156" s="8"/>
-      <c r="Z156" s="8"/>
-      <c r="AA156" s="8"/>
-      <c r="AB156" s="8"/>
-      <c r="AC156" s="8"/>
-      <c r="AD156" s="8"/>
-      <c r="AE156" s="8"/>
     </row>
     <row r="157" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N157" s="8"/>
-      <c r="O157" s="8"/>
+      <c r="A157" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B157" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="C157" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D157" s="127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E157" s="14">
+        <v>1</v>
+      </c>
+      <c r="F157" s="128">
+        <v>0</v>
+      </c>
+      <c r="G157" s="128">
+        <v>0</v>
+      </c>
+      <c r="H157" s="128">
+        <v>0</v>
+      </c>
+      <c r="I157" s="128">
+        <v>0</v>
+      </c>
+      <c r="J157" s="12">
+        <v>2</v>
+      </c>
+      <c r="K157" s="12">
+        <v>0</v>
+      </c>
+      <c r="L157" s="12">
+        <v>0</v>
+      </c>
+      <c r="M157" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N157" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O157" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="P157" s="8"/>
       <c r="Q157" s="8"/>
       <c r="R157" s="8"/>
@@ -17602,73 +17700,67 @@
       <c r="AD157" s="8"/>
       <c r="AE157" s="8"/>
     </row>
-    <row r="158" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="159" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A159" s="9" t="s">
+    <row r="158" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N158" s="8"/>
+      <c r="O158" s="8"/>
+      <c r="P158" s="8"/>
+      <c r="Q158" s="8"/>
+      <c r="R158" s="8"/>
+      <c r="S158" s="8"/>
+      <c r="T158" s="8"/>
+      <c r="U158" s="8"/>
+      <c r="V158" s="8"/>
+      <c r="W158" s="8"/>
+      <c r="X158" s="8"/>
+      <c r="Y158" s="8"/>
+      <c r="Z158" s="8"/>
+      <c r="AA158" s="8"/>
+      <c r="AB158" s="8"/>
+      <c r="AC158" s="8"/>
+      <c r="AD158" s="8"/>
+      <c r="AE158" s="8"/>
+    </row>
+    <row r="159" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="160" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A160" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B159" s="9"/>
-      <c r="C159" s="9"/>
-      <c r="D159" s="9"/>
-      <c r="E159" s="8"/>
-      <c r="F159" s="8"/>
-      <c r="G159" s="8"/>
-      <c r="H159" s="8"/>
-      <c r="I159" s="8"/>
-      <c r="J159" s="8"/>
-      <c r="K159" s="8"/>
-      <c r="L159" s="8"/>
-    </row>
-    <row r="161" spans="1:9" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="7" t="s">
+      <c r="B160" s="9"/>
+      <c r="C160" s="9"/>
+      <c r="D160" s="9"/>
+      <c r="E160" s="8"/>
+      <c r="F160" s="8"/>
+      <c r="G160" s="8"/>
+      <c r="H160" s="8"/>
+      <c r="I160" s="8"/>
+      <c r="J160" s="8"/>
+      <c r="K160" s="8"/>
+      <c r="L160" s="8"/>
+    </row>
+    <row r="162" spans="1:9" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B161" s="6" t="s">
+      <c r="B162" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C161" s="6" t="s">
+      <c r="C162" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D161" s="5" t="s">
+      <c r="D162" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E161" s="5" t="s">
+      <c r="E162" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F161" s="5" t="s">
+      <c r="F162" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G161" s="5" t="s">
+      <c r="G162" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H161" s="5" t="s">
+      <c r="H162" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A162" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D162" s="2">
-        <v>42</v>
-      </c>
-      <c r="E162" s="2">
-        <v>8</v>
-      </c>
-      <c r="F162" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G162" s="2">
-        <v>2</v>
-      </c>
-      <c r="H162" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -17676,19 +17768,19 @@
         <v>2</v>
       </c>
       <c r="B163" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D163" s="2">
+        <v>42</v>
+      </c>
+      <c r="E163" s="2">
         <v>8</v>
       </c>
-      <c r="C163" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D163" s="2">
-        <v>92</v>
-      </c>
-      <c r="E163" s="2">
-        <v>10</v>
-      </c>
       <c r="F163" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G163" s="2">
         <v>2</v>
@@ -17702,19 +17794,19 @@
         <v>2</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D164" s="2">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="E164" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F164" s="2">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G164" s="2">
         <v>2</v>
@@ -17728,19 +17820,19 @@
         <v>2</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D165" s="2">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="E165" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F165" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G165" s="2">
         <v>2</v>
@@ -17754,104 +17846,130 @@
         <v>2</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D166" s="2">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="E166" s="2">
         <v>14</v>
       </c>
       <c r="F166" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G166" s="2">
+        <v>2</v>
+      </c>
+      <c r="H166" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D167" s="2">
+        <v>1040</v>
+      </c>
+      <c r="E167" s="2">
+        <v>14</v>
+      </c>
+      <c r="F167" s="2">
         <v>0.5</v>
       </c>
-      <c r="G166" s="2">
-        <v>2</v>
-      </c>
-      <c r="H166" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D169" s="1">
-        <v>42</v>
-      </c>
-      <c r="F169" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G169">
-        <f>D162*F162</f>
-        <v>54.6</v>
-      </c>
-      <c r="I169">
-        <f>D169*F169</f>
-        <v>54.6</v>
+      <c r="G167" s="2">
+        <v>2</v>
+      </c>
+      <c r="H167" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D170" s="1">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="F170" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G170">
         <f>D163*F163</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
       <c r="I170">
         <f>D170*F170</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D171" s="1">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="F171" s="1">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G171">
         <f>D164*F164</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
       <c r="I171">
         <f>D171*F171</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D172" s="1">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="F172" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G172">
         <f>D165*F165</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
       <c r="I172">
         <f>D172*F172</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D173" s="1">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="F173" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G173">
         <f>D166*F166</f>
-        <v>520</v>
+        <v>480.2</v>
       </c>
       <c r="I173">
         <f>D173*F173</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D174" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F174" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G174">
+        <f>D167*F167</f>
+        <v>520</v>
+      </c>
+      <c r="I174">
+        <f>D174*F174</f>
         <v>520</v>
       </c>
     </row>
@@ -17859,20 +17977,20 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F143:G143"/>
+    <mergeCell ref="F144:G144"/>
   </mergeCells>
   <conditionalFormatting sqref="M118:M124 R118:T124 M24:M56 R24:T56 S127:T127 M127 R58:T115 M58:M115">
-    <cfRule type="expression" dxfId="115" priority="69">
+    <cfRule type="expression" dxfId="25" priority="74">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="114" priority="62">
+    <cfRule type="expression" dxfId="24" priority="67">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116:Q116">
-    <cfRule type="colorScale" priority="61">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17884,12 +18002,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="113" priority="56">
+    <cfRule type="expression" dxfId="23" priority="61">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N115:Q119">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17901,7 +18019,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N118:Q124 N24:Q56 N58:Q115">
-    <cfRule type="colorScale" priority="74">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17913,12 +18031,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="112" priority="54">
+    <cfRule type="expression" dxfId="22" priority="59">
       <formula>M114=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N114:Q114">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17930,17 +18048,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="111" priority="51">
+    <cfRule type="expression" dxfId="21" priority="56">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="110" priority="50">
+    <cfRule type="expression" dxfId="20" priority="55">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q125">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17952,7 +18070,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N125:Q127">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17964,17 +18082,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="109" priority="48">
+    <cfRule type="expression" dxfId="19" priority="53">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="108" priority="47">
+    <cfRule type="expression" dxfId="18" priority="52">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:Q128">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17986,22 +18104,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="107" priority="45">
+    <cfRule type="expression" dxfId="17" priority="50">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="106" priority="30">
+    <cfRule type="expression" dxfId="16" priority="35">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="105" priority="32">
+    <cfRule type="expression" dxfId="15" priority="37">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N133:Q133">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18013,17 +18131,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="104" priority="25">
+    <cfRule type="expression" dxfId="14" priority="30">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="103" priority="26">
+    <cfRule type="expression" dxfId="13" priority="31">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N129:Q132">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18035,6 +18153,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:Q134">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R134">
+    <cfRule type="expression" dxfId="12" priority="28">
+      <formula>R134=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R135">
+    <cfRule type="expression" dxfId="11" priority="23">
+      <formula>R135=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N135:Q135">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -18046,17 +18186,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="102" priority="23">
-      <formula>R134=FALSE</formula>
+  <conditionalFormatting sqref="S135:T135 M135">
+    <cfRule type="expression" dxfId="10" priority="25">
+      <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="101" priority="18">
-      <formula>R135=FALSE</formula>
+  <conditionalFormatting sqref="R136">
+    <cfRule type="expression" dxfId="9" priority="18">
+      <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N135:Q135">
+  <conditionalFormatting sqref="N136:Q136">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -18068,40 +18208,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="100" priority="20">
-      <formula>M135=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="99" priority="13">
-      <formula>R136=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N136:Q136">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="98" priority="15">
+    <cfRule type="expression" dxfId="8" priority="20">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="97" priority="11">
+    <cfRule type="expression" dxfId="7" priority="16">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N138:Q138">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18113,12 +18231,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="96" priority="9">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57:Q57">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18130,12 +18248,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="95" priority="7">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N137:Q137">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18147,12 +18265,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="94" priority="5">
+    <cfRule type="expression" dxfId="4" priority="10">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N139:Q139">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18164,11 +18282,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="93" priority="1">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N140:Q140">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R141">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>R141=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N141:Q141">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -18180,34 +18315,39 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S141:T141 M141">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>M141=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G134"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G133 J24:J138 G135:G140 H40:I140 J140">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G133 J24:J138 H40:I141 J140:J141 G135:G141">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D145:G156 P139:V139 Q24:W138 N24:O138 M139:N139 Q140:W140 N140:O140">
+    <dataValidation type="decimal" allowBlank="1" sqref="D146:G157 P139:V139 Q24:W138 N24:O138 M139:N139 N140:O141 Q140:W141">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H145:L154 H155:I155 J156:L156 X24:AA138 W139:Z139 X140:AA140">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H146:L155 H156:I156 J157:L157 X24:AA138 W139:Z139 X140:AA141">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C145:C156 C24:C140">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C146:C157 C24:C141">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J155:L155 M145:O156 AA139:AC139 AC24:AC138 AD24:AF140 AB24:AB140 AC140"/>
-    <dataValidation type="list" sqref="P24:P138 O139 P140">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J156:L156 M146:O157 AA139:AC139 AC24:AC138 AB24:AB141 AC140:AC141 AD24:AF141"/>
+    <dataValidation type="list" sqref="P24:P138 O139 P140:P141">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L138 K139 K140:L140">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L138 K139 K140:L141">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="M24:M138 L139 M140">
+    <dataValidation type="list" sqref="M24:M138 L139 M140:M141">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F140">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F141">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J139">

</xml_diff>

<commit_message>
GoodWitch02 should be edible by tier 2
Former-commit-id: 3ae81ddd3cff112aaa586fe71179138446bdf440
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -2502,189 +2502,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="119">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="118">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4980,6 +4798,181 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4994,58 +4987,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF141" totalsRowShown="0" headerRowDxfId="118" dataDxfId="116" headerRowBorderDxfId="117" tableBorderDxfId="115" totalsRowBorderDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF141" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF141"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="113"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="112"/>
-    <tableColumn id="6" name="[category]" dataDxfId="111"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="110"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="109"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="108"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="107"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="106"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="105"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="104"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="103"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="102"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="101"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="100"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="99"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="98"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="97"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="96"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="95"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="94"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="93"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="92"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="91"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="90"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="89"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="88"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="87"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="86"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="85"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="84"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="83"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="82"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="77"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5058,50 +5051,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="4" name="[category]" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="16" name="[size]" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="6" name="[order]" dataDxfId="39"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="38"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="37"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="36"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="35"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="29"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="27"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5375,10 +5368,10 @@
   </sheetPr>
   <dimension ref="A1:AF174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="AF141" sqref="AF141"/>
+      <selection pane="topRight" activeCell="P76" sqref="P76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10736,10 +10729,10 @@
         <v>5</v>
       </c>
       <c r="P76" s="46">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q76" s="48">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R76" s="36" t="b">
         <v>1</v>
@@ -17980,12 +17973,12 @@
     <mergeCell ref="F144:G144"/>
   </mergeCells>
   <conditionalFormatting sqref="M118:M124 R118:T124 M24:M56 R24:T56 S127:T127 M127 R58:T115 M58:M115">
-    <cfRule type="expression" dxfId="25" priority="74">
+    <cfRule type="expression" dxfId="117" priority="74">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116 R116:T116">
-    <cfRule type="expression" dxfId="24" priority="67">
+    <cfRule type="expression" dxfId="116" priority="67">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18002,7 +17995,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M119 R115:T119">
-    <cfRule type="expression" dxfId="23" priority="61">
+    <cfRule type="expression" dxfId="115" priority="61">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18031,7 +18024,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M114 R114:T114">
-    <cfRule type="expression" dxfId="22" priority="59">
+    <cfRule type="expression" dxfId="114" priority="59">
       <formula>M114=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18048,12 +18041,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125:M126 R125:T126">
-    <cfRule type="expression" dxfId="21" priority="56">
+    <cfRule type="expression" dxfId="113" priority="56">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M125 R125:T125">
-    <cfRule type="expression" dxfId="20" priority="55">
+    <cfRule type="expression" dxfId="112" priority="55">
       <formula>M125=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18082,12 +18075,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R127">
-    <cfRule type="expression" dxfId="19" priority="53">
+    <cfRule type="expression" dxfId="111" priority="53">
       <formula>R127=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S128:T128 M128">
-    <cfRule type="expression" dxfId="18" priority="52">
+    <cfRule type="expression" dxfId="110" priority="52">
       <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18104,17 +18097,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="17" priority="50">
+    <cfRule type="expression" dxfId="109" priority="50">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R133">
-    <cfRule type="expression" dxfId="16" priority="35">
+    <cfRule type="expression" dxfId="108" priority="35">
       <formula>R133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S133:T133 M133">
-    <cfRule type="expression" dxfId="15" priority="37">
+    <cfRule type="expression" dxfId="107" priority="37">
       <formula>M133=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18131,12 +18124,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="14" priority="30">
+    <cfRule type="expression" dxfId="106" priority="30">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M129:M132 R129:T132">
-    <cfRule type="expression" dxfId="13" priority="31">
+    <cfRule type="expression" dxfId="105" priority="31">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18165,12 +18158,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="12" priority="28">
+    <cfRule type="expression" dxfId="104" priority="28">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="11" priority="23">
+    <cfRule type="expression" dxfId="103" priority="23">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18187,12 +18180,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="10" priority="25">
+    <cfRule type="expression" dxfId="102" priority="25">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="9" priority="18">
+    <cfRule type="expression" dxfId="101" priority="18">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18209,12 +18202,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="8" priority="20">
+    <cfRule type="expression" dxfId="100" priority="20">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="7" priority="16">
+    <cfRule type="expression" dxfId="99" priority="16">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18231,7 +18224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="6" priority="14">
+    <cfRule type="expression" dxfId="98" priority="14">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18248,7 +18241,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M137 R137:T137">
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="97" priority="12">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18265,7 +18258,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="96" priority="10">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18282,7 +18275,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="95" priority="6">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18299,7 +18292,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R141">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="94" priority="1">
       <formula>R141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18316,7 +18309,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S141:T141 M141">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="93" priority="3">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Review HealthReward for some entities
Former-commit-id: 5e63cede9d6973edac5021c87ed36ecdabb2df8e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5368,10 +5368,10 @@
   </sheetPr>
   <dimension ref="A1:AF174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="P76" sqref="P76"/>
+      <selection pane="topRight" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6687,7 +6687,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="65">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H34" s="65">
         <v>0</v>
@@ -6781,7 +6781,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="65">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H35" s="65">
         <v>0</v>
@@ -7256,7 +7256,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="65">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H40" s="65">
         <v>0</v>
@@ -7350,7 +7350,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="65">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H41" s="65">
         <v>0</v>
@@ -7538,7 +7538,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="65">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H43" s="65">
         <v>0</v>
@@ -7633,7 +7633,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="76">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H44" s="76">
         <v>0</v>
@@ -8978,7 +8978,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="65">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H58" s="65">
         <v>0</v>
@@ -10995,7 +10995,7 @@
         <v>0</v>
       </c>
       <c r="G79" s="76">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H79" s="76">
         <v>0</v>
@@ -11089,7 +11089,7 @@
         <v>0</v>
       </c>
       <c r="G80" s="65">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H80" s="65">
         <v>0</v>
@@ -11184,7 +11184,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="65">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H81" s="65">
         <v>0</v>
@@ -11279,7 +11279,7 @@
         <v>0</v>
       </c>
       <c r="G82" s="65">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H82" s="65">
         <v>0</v>
@@ -12351,7 +12351,7 @@
         <v>0</v>
       </c>
       <c r="G93" s="76">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H93" s="76">
         <v>0</v>
@@ -12539,7 +12539,7 @@
         <v>0</v>
       </c>
       <c r="G95" s="76">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H95" s="76">
         <v>0</v>
@@ -12732,7 +12732,7 @@
         <v>0</v>
       </c>
       <c r="G97" s="65">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H97" s="65">
         <v>0</v>
@@ -13306,7 +13306,7 @@
         <v>0</v>
       </c>
       <c r="G103" s="76">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H103" s="76">
         <v>0</v>
@@ -13876,7 +13876,7 @@
         <v>0</v>
       </c>
       <c r="G109" s="76">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H109" s="76">
         <v>0</v>
@@ -13975,7 +13975,7 @@
         <v>0</v>
       </c>
       <c r="G110" s="76">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H110" s="76">
         <v>0</v>
@@ -16527,7 +16527,7 @@
         <v>0</v>
       </c>
       <c r="G137" s="65">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H137" s="65">
         <v>0</v>

</xml_diff>

<commit_message>
Drunken effect last 5 sec.
Former-commit-id: 7bfb6e1696b1b547311db7094a24cde94f51bebf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5368,10 +5368,10 @@
   </sheetPr>
   <dimension ref="A1:AF174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="G49" sqref="G49"/>
+      <selection pane="topRight" activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8107,10 +8107,10 @@
         <v>87</v>
       </c>
       <c r="D49" s="66">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E49" s="65">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F49" s="65">
         <v>0</v>
@@ -8122,7 +8122,7 @@
         <v>100</v>
       </c>
       <c r="I49" s="65">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="J49" s="65">
         <v>0</v>
@@ -8164,7 +8164,7 @@
         <v>9</v>
       </c>
       <c r="W49" s="36">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="X49" s="52">
         <v>0.25</v>

</xml_diff>

<commit_message>
Content - FIX CONTENT [CONTENT_MERGE] (Pets + UIType + Drunken + BetterEggs)
Former-commit-id: 2b84650742389718cda5e290c8454fc1d552af93
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$145:$O$146</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5368,10 +5368,10 @@
   </sheetPr>
   <dimension ref="A1:AF174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="L49" sqref="L49"/>
+      <selection pane="topRight" activeCell="V54" sqref="V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Castle scene review. Also, check some entities values
Former-commit-id: ab2d678ba76ba3352f4d69b33eb245b4fa561fff
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$145:$O$146</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5368,10 +5368,10 @@
   </sheetPr>
   <dimension ref="A1:AF174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="V54" sqref="V54"/>
+      <selection pane="topRight" activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6693,7 +6693,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="65">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="J34" s="65">
         <v>0</v>
@@ -8984,7 +8984,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="65">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J58" s="65">
         <v>0</v>
@@ -10136,7 +10136,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="76">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="J70" s="76">
         <v>0</v>
@@ -10231,7 +10231,7 @@
         <v>0</v>
       </c>
       <c r="I71" s="76">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J71" s="76">
         <v>0</v>
@@ -10804,7 +10804,7 @@
         <v>0</v>
       </c>
       <c r="I77" s="76">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="J77" s="76">
         <v>0</v>

</xml_diff>

<commit_message>
[CONTENT] [NEW] Added new skus in entityDefinitions for Halloween season (pumpkins)
Former-commit-id: 8c0172da4d1407ad3165f811e4efc35734f70fa7
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="511">
   <si>
     <t>tier_4</t>
   </si>
@@ -1561,23 +1561,26 @@
     <t>Miner</t>
   </si>
   <si>
+    <t>season_halloween_0</t>
+  </si>
+  <si>
     <t>season_halloween_1</t>
   </si>
   <si>
-    <t>season_halloween_0</t>
-  </si>
-  <si>
     <t>season_halloween_2</t>
   </si>
   <si>
-    <t>TID_EDIBLE_HALLOWEEN</t>
+    <t>TID_EDIBLE_SEASON_HALLOWEEN</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_KILL_ENT_GOODJUNK_01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1660,15 +1663,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1" tint="0.14999847407452621"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1790,7 +1806,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2088,12 +2104,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2453,13 +2480,26 @@
     <xf numFmtId="0" fontId="7" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2467,30 +2507,30 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="106">
+  <dxfs count="118">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4877,6 +4917,90 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5273,13 +5397,21 @@
   <dimension ref="A1:AF177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="B101" sqref="B101"/>
+      <selection pane="topRight" activeCell="V132" sqref="V132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="14" max="14" width="28.28515625" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="16" max="16" width="28.85546875" customWidth="1"/>
+    <col min="17" max="17" width="26.140625" customWidth="1"/>
+    <col min="18" max="18" width="28.5703125" customWidth="1"/>
+    <col min="19" max="19" width="26" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" customWidth="1"/>
     <col min="28" max="28" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5319,8 +5451,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5484,8 +5616,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="153"/>
-      <c r="F22" s="153"/>
+      <c r="E22" s="152"/>
+      <c r="F22" s="152"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -8774,7 +8906,7 @@
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
     </row>
-    <row r="57" spans="1:32" s="143" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" s="149" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="123" t="s">
         <v>2</v>
       </c>
@@ -10776,7 +10908,7 @@
       <c r="AE77" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="AF77" s="146" t="s">
+      <c r="AF77" s="150" t="s">
         <v>213</v>
       </c>
     </row>
@@ -10875,7 +11007,7 @@
       <c r="AE78" s="68" t="s">
         <v>207</v>
       </c>
-      <c r="AF78" s="146" t="s">
+      <c r="AF78" s="150" t="s">
         <v>206</v>
       </c>
     </row>
@@ -13367,24 +13499,24 @@
       <c r="AA104" s="55">
         <v>0</v>
       </c>
-      <c r="AB104" s="148" t="s">
+      <c r="AB104" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="AC104" s="26" t="s">
+      <c r="AC104" s="44" t="s">
         <v>247</v>
       </c>
-      <c r="AD104" s="26" t="s">
+      <c r="AD104" s="44" t="s">
         <v>150</v>
       </c>
       <c r="AE104" s="26"/>
       <c r="AF104" s="59"/>
     </row>
     <row r="105" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="151" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="152" t="s">
-        <v>507</v>
+      <c r="A105" s="135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="49" t="s">
+        <v>506</v>
       </c>
       <c r="C105" s="77" t="s">
         <v>61</v>
@@ -13461,24 +13593,24 @@
       <c r="AA105" s="55">
         <v>0</v>
       </c>
-      <c r="AB105" s="149" t="s">
+      <c r="AB105" s="45" t="s">
         <v>509</v>
       </c>
-      <c r="AC105" s="26" t="s">
+      <c r="AC105" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="AD105" s="26" t="s">
+      <c r="AD105" s="44" t="s">
         <v>150</v>
       </c>
       <c r="AE105" s="26"/>
       <c r="AF105" s="59"/>
     </row>
     <row r="106" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="151" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="152" t="s">
-        <v>506</v>
+      <c r="A106" s="135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="49" t="s">
+        <v>507</v>
       </c>
       <c r="C106" s="77" t="s">
         <v>61</v>
@@ -13555,31 +13687,29 @@
       <c r="AA106" s="55">
         <v>0</v>
       </c>
-      <c r="AB106" s="149" t="s">
+      <c r="AB106" s="45" t="s">
         <v>509</v>
       </c>
-      <c r="AC106" s="26" t="s">
+      <c r="AC106" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="AD106" s="26" t="s">
+      <c r="AD106" s="44" t="s">
         <v>150</v>
       </c>
       <c r="AE106" s="26"/>
       <c r="AF106" s="59"/>
     </row>
     <row r="107" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="151" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="152" t="s">
+      <c r="A107" s="135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="49" t="s">
         <v>508</v>
       </c>
       <c r="C107" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="D107" s="61">
-        <v>30</v>
-      </c>
+      <c r="D107" s="61"/>
       <c r="E107" s="76">
         <v>3</v>
       </c>
@@ -13649,13 +13779,13 @@
       <c r="AA107" s="55">
         <v>0</v>
       </c>
-      <c r="AB107" s="149" t="s">
+      <c r="AB107" s="45" t="s">
         <v>509</v>
       </c>
-      <c r="AC107" s="26" t="s">
+      <c r="AC107" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="AD107" s="26" t="s">
+      <c r="AD107" s="44" t="s">
         <v>150</v>
       </c>
       <c r="AE107" s="26"/>
@@ -13672,7 +13802,7 @@
         <v>66</v>
       </c>
       <c r="D108" s="66">
-        <v>540</v>
+        <v>0</v>
       </c>
       <c r="E108" s="65">
         <v>17</v>
@@ -15103,7 +15233,7 @@
       <c r="AE122" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="AF122" s="146" t="s">
+      <c r="AF122" s="150" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15619,7 +15749,7 @@
       <c r="L128" s="76">
         <v>0</v>
       </c>
-      <c r="M128" s="27" t="b">
+      <c r="M128" s="36" t="b">
         <v>1</v>
       </c>
       <c r="N128" s="37">
@@ -15628,7 +15758,7 @@
       <c r="O128" s="37">
         <v>0</v>
       </c>
-      <c r="P128" s="27">
+      <c r="P128" s="36">
         <v>1</v>
       </c>
       <c r="Q128" s="37">
@@ -15664,17 +15794,17 @@
       <c r="AA128" s="55">
         <v>0</v>
       </c>
-      <c r="AB128" s="149" t="s">
+      <c r="AB128" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="AC128" s="150" t="s">
+      <c r="AC128" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="AD128" s="150" t="s">
+      <c r="AD128" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="AE128" s="44"/>
-      <c r="AF128" s="43"/>
+      <c r="AE128" s="75"/>
+      <c r="AF128" s="79"/>
     </row>
     <row r="129" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A129" s="135" t="s">
@@ -15713,19 +15843,19 @@
       <c r="L129" s="76">
         <v>0</v>
       </c>
-      <c r="M129" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="N129" s="37">
+      <c r="M129" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N129" s="40">
         <v>5</v>
       </c>
       <c r="O129" s="37">
         <v>5</v>
       </c>
-      <c r="P129" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q129" s="37">
+      <c r="P129" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="40">
         <v>0</v>
       </c>
       <c r="R129" s="36" t="b">
@@ -15734,7 +15864,7 @@
       <c r="S129" s="36" t="b">
         <v>0</v>
       </c>
-      <c r="T129" s="36" t="b">
+      <c r="T129" s="73" t="b">
         <v>0</v>
       </c>
       <c r="U129" s="46">
@@ -15758,17 +15888,17 @@
       <c r="AA129" s="55">
         <v>0</v>
       </c>
-      <c r="AB129" s="149" t="s">
+      <c r="AB129" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="AC129" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD129" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE129" s="44"/>
-      <c r="AF129" s="43"/>
+      <c r="AC129" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD129" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE129" s="75"/>
+      <c r="AF129" s="74"/>
     </row>
     <row r="130" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A130" s="135" t="s">
@@ -15807,60 +15937,60 @@
       <c r="L130" s="76">
         <v>0</v>
       </c>
-      <c r="M130" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="N130" s="37">
-        <v>5</v>
-      </c>
-      <c r="O130" s="37">
-        <v>5</v>
-      </c>
-      <c r="P130" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q130" s="37">
+      <c r="M130" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N130" s="40">
+        <v>5</v>
+      </c>
+      <c r="O130" s="40">
+        <v>5</v>
+      </c>
+      <c r="P130" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="40">
         <v>0</v>
       </c>
       <c r="R130" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S130" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="T130" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="U130" s="46">
-        <v>1</v>
-      </c>
-      <c r="V130" s="46"/>
-      <c r="W130" s="46">
+      <c r="S130" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T130" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U130" s="143">
+        <v>1</v>
+      </c>
+      <c r="V130" s="143"/>
+      <c r="W130" s="143">
         <v>0</v>
       </c>
       <c r="X130" s="55">
         <v>0</v>
       </c>
-      <c r="Y130" s="55">
-        <v>0</v>
-      </c>
-      <c r="Z130" s="55">
+      <c r="Y130" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z130" s="144">
         <v>0</v>
       </c>
       <c r="AA130" s="55">
         <v>0</v>
       </c>
-      <c r="AB130" s="149" t="s">
+      <c r="AB130" s="153" t="s">
         <v>224</v>
       </c>
-      <c r="AC130" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD130" s="26" t="s">
+      <c r="AC130" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD130" s="154" t="s">
         <v>150</v>
       </c>
-      <c r="AE130" s="44"/>
-      <c r="AF130" s="43"/>
+      <c r="AE130" s="145"/>
+      <c r="AF130" s="146"/>
     </row>
     <row r="131" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="135" t="s">
@@ -15899,60 +16029,60 @@
       <c r="L131" s="76">
         <v>0</v>
       </c>
-      <c r="M131" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="N131" s="37">
-        <v>5</v>
-      </c>
-      <c r="O131" s="37">
-        <v>5</v>
-      </c>
-      <c r="P131" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q131" s="37">
+      <c r="M131" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N131" s="40">
+        <v>5</v>
+      </c>
+      <c r="O131" s="40">
+        <v>5</v>
+      </c>
+      <c r="P131" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q131" s="40">
         <v>0</v>
       </c>
       <c r="R131" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S131" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="T131" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="U131" s="46">
-        <v>1</v>
-      </c>
-      <c r="V131" s="46"/>
-      <c r="W131" s="46">
+      <c r="S131" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T131" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U131" s="143">
+        <v>1</v>
+      </c>
+      <c r="V131" s="143"/>
+      <c r="W131" s="143">
         <v>0</v>
       </c>
       <c r="X131" s="55">
         <v>0</v>
       </c>
-      <c r="Y131" s="55">
-        <v>0</v>
-      </c>
-      <c r="Z131" s="55">
+      <c r="Y131" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z131" s="144">
         <v>0</v>
       </c>
       <c r="AA131" s="55">
         <v>0</v>
       </c>
-      <c r="AB131" s="149" t="s">
+      <c r="AB131" s="153" t="s">
         <v>224</v>
       </c>
-      <c r="AC131" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD131" s="26" t="s">
+      <c r="AC131" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD131" s="154" t="s">
         <v>150</v>
       </c>
-      <c r="AE131" s="44"/>
-      <c r="AF131" s="43"/>
+      <c r="AE131" s="145"/>
+      <c r="AF131" s="146"/>
     </row>
     <row r="132" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A132" s="123" t="s">
@@ -16034,13 +16164,13 @@
       <c r="AA132" s="52">
         <v>0</v>
       </c>
-      <c r="AB132" s="144" t="s">
+      <c r="AB132" s="155" t="s">
         <v>224</v>
       </c>
-      <c r="AC132" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD132" s="72" t="s">
+      <c r="AC132" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD132" s="154" t="s">
         <v>150</v>
       </c>
       <c r="AE132" s="63"/>
@@ -16126,13 +16256,13 @@
       <c r="AA133" s="52">
         <v>0</v>
       </c>
-      <c r="AB133" s="144" t="s">
+      <c r="AB133" s="155" t="s">
         <v>224</v>
       </c>
-      <c r="AC133" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD133" s="72" t="s">
+      <c r="AC133" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD133" s="154" t="s">
         <v>150</v>
       </c>
       <c r="AE133" s="72"/>
@@ -16218,13 +16348,13 @@
       <c r="AA134" s="52">
         <v>0</v>
       </c>
-      <c r="AB134" s="144" t="s">
+      <c r="AB134" s="155" t="s">
         <v>224</v>
       </c>
-      <c r="AC134" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD134" s="72" t="s">
+      <c r="AC134" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD134" s="154" t="s">
         <v>150</v>
       </c>
       <c r="AE134" s="72"/>
@@ -16310,13 +16440,13 @@
       <c r="AA135" s="142">
         <v>0</v>
       </c>
-      <c r="AB135" s="145" t="s">
+      <c r="AB135" s="156" t="s">
         <v>224</v>
       </c>
-      <c r="AC135" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD135" s="72" t="s">
+      <c r="AC135" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD135" s="154" t="s">
         <v>150</v>
       </c>
       <c r="AE135" s="25"/>
@@ -16359,60 +16489,60 @@
       <c r="L136" s="76">
         <v>0</v>
       </c>
-      <c r="M136" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="N136" s="37">
-        <v>5</v>
-      </c>
-      <c r="O136" s="37">
-        <v>5</v>
-      </c>
-      <c r="P136" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q136" s="37">
+      <c r="M136" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N136" s="40">
+        <v>5</v>
+      </c>
+      <c r="O136" s="40">
+        <v>5</v>
+      </c>
+      <c r="P136" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q136" s="40">
         <v>0</v>
       </c>
       <c r="R136" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S136" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="T136" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="U136" s="46">
-        <v>1</v>
-      </c>
-      <c r="V136" s="46"/>
-      <c r="W136" s="46">
+      <c r="S136" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T136" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U136" s="143">
+        <v>1</v>
+      </c>
+      <c r="V136" s="143"/>
+      <c r="W136" s="143">
         <v>0</v>
       </c>
       <c r="X136" s="55">
         <v>0</v>
       </c>
-      <c r="Y136" s="55">
-        <v>0</v>
-      </c>
-      <c r="Z136" s="55">
+      <c r="Y136" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z136" s="144">
         <v>0</v>
       </c>
       <c r="AA136" s="55">
         <v>0</v>
       </c>
-      <c r="AB136" s="148" t="s">
+      <c r="AB136" s="153" t="s">
         <v>224</v>
       </c>
-      <c r="AC136" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD136" s="26" t="s">
+      <c r="AC136" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD136" s="154" t="s">
         <v>150</v>
       </c>
-      <c r="AE136" s="44"/>
-      <c r="AF136" s="43"/>
+      <c r="AE136" s="145"/>
+      <c r="AF136" s="146"/>
     </row>
     <row r="137" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A137" s="135" t="s">
@@ -16433,7 +16563,7 @@
       <c r="F137" s="76">
         <v>0</v>
       </c>
-      <c r="G137" s="76">
+      <c r="G137" s="148">
         <v>-20</v>
       </c>
       <c r="H137" s="76">
@@ -16451,67 +16581,63 @@
       <c r="L137" s="76">
         <v>0</v>
       </c>
-      <c r="M137" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="N137" s="37">
-        <v>5</v>
-      </c>
-      <c r="O137" s="37">
-        <v>5</v>
-      </c>
-      <c r="P137" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q137" s="37">
+      <c r="M137" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N137" s="40">
+        <v>5</v>
+      </c>
+      <c r="O137" s="40">
+        <v>5</v>
+      </c>
+      <c r="P137" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q137" s="40">
         <f>entityDefinitions[[#This Row],['[edibleFromTier']]]</f>
         <v>0</v>
       </c>
       <c r="R137" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S137" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="T137" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="U137" s="46">
-        <v>1</v>
-      </c>
-      <c r="V137" s="46">
-        <v>2</v>
-      </c>
-      <c r="W137" s="46">
+      <c r="S137" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T137" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U137" s="143">
+        <v>1</v>
+      </c>
+      <c r="V137" s="143">
+        <v>2</v>
+      </c>
+      <c r="W137" s="143">
         <v>0</v>
       </c>
       <c r="X137" s="55">
         <v>1</v>
       </c>
-      <c r="Y137" s="55">
-        <v>1</v>
-      </c>
-      <c r="Z137" s="55">
-        <v>0.5</v>
+      <c r="Y137" s="144">
+        <v>1</v>
+      </c>
+      <c r="Z137" s="144">
+        <v>0</v>
       </c>
       <c r="AA137" s="55">
-        <v>1</v>
-      </c>
-      <c r="AB137" s="148" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB137" s="153" t="s">
         <v>338</v>
       </c>
-      <c r="AC137" s="26" t="s">
+      <c r="AC137" s="154" t="s">
         <v>337</v>
       </c>
-      <c r="AD137" s="26" t="s">
+      <c r="AD137" s="154" t="s">
         <v>137</v>
       </c>
-      <c r="AE137" s="44" t="s">
-        <v>337</v>
-      </c>
-      <c r="AF137" s="43" t="s">
-        <v>337</v>
-      </c>
+      <c r="AE137" s="145"/>
+      <c r="AF137" s="146"/>
     </row>
     <row r="138" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A138" s="135" t="s">
@@ -16532,7 +16658,7 @@
       <c r="F138" s="76">
         <v>1</v>
       </c>
-      <c r="G138" s="76">
+      <c r="G138" s="148">
         <v>0</v>
       </c>
       <c r="H138" s="76">
@@ -16550,60 +16676,60 @@
       <c r="L138" s="76">
         <v>1</v>
       </c>
-      <c r="M138" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="N138" s="37">
-        <v>5</v>
-      </c>
-      <c r="O138" s="37">
-        <v>5</v>
-      </c>
-      <c r="P138" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q138" s="37">
+      <c r="M138" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N138" s="40">
+        <v>5</v>
+      </c>
+      <c r="O138" s="40">
+        <v>5</v>
+      </c>
+      <c r="P138" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="40">
         <v>0</v>
       </c>
       <c r="R138" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S138" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="T138" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="U138" s="46">
-        <v>1</v>
-      </c>
-      <c r="V138" s="46"/>
-      <c r="W138" s="46">
+      <c r="S138" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T138" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U138" s="143">
+        <v>1</v>
+      </c>
+      <c r="V138" s="143"/>
+      <c r="W138" s="143">
         <v>0</v>
       </c>
       <c r="X138" s="55">
         <v>0</v>
       </c>
-      <c r="Y138" s="55">
-        <v>0</v>
-      </c>
-      <c r="Z138" s="55">
+      <c r="Y138" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z138" s="144">
         <v>0</v>
       </c>
       <c r="AA138" s="55">
         <v>0</v>
       </c>
-      <c r="AB138" s="148" t="s">
+      <c r="AB138" s="153" t="s">
         <v>224</v>
       </c>
-      <c r="AC138" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD138" s="26" t="s">
+      <c r="AC138" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD138" s="154" t="s">
         <v>150</v>
       </c>
-      <c r="AE138" s="44"/>
-      <c r="AF138" s="43"/>
+      <c r="AE138" s="145"/>
+      <c r="AF138" s="146"/>
     </row>
     <row r="139" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A139" s="135" t="s">
@@ -16624,7 +16750,7 @@
       <c r="F139" s="76">
         <v>0</v>
       </c>
-      <c r="G139" s="76">
+      <c r="G139" s="148">
         <v>0</v>
       </c>
       <c r="H139" s="76">
@@ -16642,60 +16768,60 @@
       <c r="L139" s="76">
         <v>0</v>
       </c>
-      <c r="M139" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="N139" s="37">
-        <v>5</v>
-      </c>
-      <c r="O139" s="37">
-        <v>5</v>
-      </c>
-      <c r="P139" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q139" s="37">
+      <c r="M139" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N139" s="40">
+        <v>5</v>
+      </c>
+      <c r="O139" s="40">
+        <v>5</v>
+      </c>
+      <c r="P139" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="40">
         <v>0</v>
       </c>
       <c r="R139" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S139" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="T139" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="U139" s="46">
-        <v>1</v>
-      </c>
-      <c r="V139" s="46"/>
-      <c r="W139" s="46">
+      <c r="S139" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T139" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U139" s="143">
+        <v>1</v>
+      </c>
+      <c r="V139" s="143"/>
+      <c r="W139" s="143">
         <v>0</v>
       </c>
       <c r="X139" s="55">
         <v>0</v>
       </c>
-      <c r="Y139" s="55">
-        <v>0</v>
-      </c>
-      <c r="Z139" s="55">
+      <c r="Y139" s="144">
+        <v>0</v>
+      </c>
+      <c r="Z139" s="144">
         <v>0</v>
       </c>
       <c r="AA139" s="55">
         <v>0</v>
       </c>
-      <c r="AB139" s="148" t="s">
+      <c r="AB139" s="153" t="s">
         <v>224</v>
       </c>
-      <c r="AC139" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD139" s="26" t="s">
+      <c r="AC139" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD139" s="154" t="s">
         <v>150</v>
       </c>
-      <c r="AE139" s="44"/>
-      <c r="AF139" s="43"/>
+      <c r="AE139" s="145"/>
+      <c r="AF139" s="146"/>
     </row>
     <row r="140" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A140" s="123" t="s">
@@ -16779,13 +16905,13 @@
       <c r="AA140" s="142">
         <v>0</v>
       </c>
-      <c r="AB140" s="35" t="s">
+      <c r="AB140" s="156" t="s">
         <v>65</v>
       </c>
-      <c r="AC140" s="34" t="s">
+      <c r="AC140" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="AD140" s="34" t="s">
+      <c r="AD140" s="157" t="s">
         <v>63</v>
       </c>
       <c r="AE140" s="25"/>
@@ -16871,13 +16997,13 @@
       <c r="AA141" s="52">
         <v>0</v>
       </c>
-      <c r="AB141" s="144" t="s">
+      <c r="AB141" s="155" t="s">
         <v>224</v>
       </c>
-      <c r="AC141" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD141" s="72" t="s">
+      <c r="AC141" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD141" s="154" t="s">
         <v>150</v>
       </c>
       <c r="AE141" s="72"/>
@@ -16911,7 +17037,7 @@
       <c r="I142" s="65">
         <v>25</v>
       </c>
-      <c r="J142" s="147">
+      <c r="J142" s="151">
         <v>0.3</v>
       </c>
       <c r="K142" s="53">
@@ -16965,13 +17091,13 @@
       <c r="AA142" s="52">
         <v>0</v>
       </c>
-      <c r="AB142" s="144" t="s">
+      <c r="AB142" s="155" t="s">
         <v>224</v>
       </c>
-      <c r="AC142" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD142" s="72" t="s">
+      <c r="AC142" s="154" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD142" s="154" t="s">
         <v>150</v>
       </c>
       <c r="AE142" s="72"/>
@@ -17005,7 +17131,7 @@
       <c r="I143" s="65">
         <v>40</v>
       </c>
-      <c r="J143" s="147">
+      <c r="J143" s="151">
         <v>0</v>
       </c>
       <c r="K143" s="53">
@@ -17091,7 +17217,7 @@
       <c r="F144" s="76">
         <v>0</v>
       </c>
-      <c r="G144" s="76">
+      <c r="G144" s="148">
         <v>12</v>
       </c>
       <c r="H144" s="76">
@@ -17109,62 +17235,62 @@
       <c r="L144" s="76">
         <v>0</v>
       </c>
-      <c r="M144" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="N144" s="37">
-        <v>5</v>
-      </c>
-      <c r="O144" s="37">
-        <v>0</v>
-      </c>
-      <c r="P144" s="27">
-        <v>1</v>
-      </c>
-      <c r="Q144" s="37">
+      <c r="M144" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N144" s="40">
+        <v>5</v>
+      </c>
+      <c r="O144" s="40">
+        <v>0</v>
+      </c>
+      <c r="P144" s="81">
+        <v>1</v>
+      </c>
+      <c r="Q144" s="40">
         <v>0</v>
       </c>
       <c r="R144" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S144" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="T144" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="U144" s="46">
+      <c r="S144" s="147" t="b">
+        <v>1</v>
+      </c>
+      <c r="T144" s="147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U144" s="143">
         <v>25</v>
       </c>
-      <c r="V144" s="46">
+      <c r="V144" s="143">
         <v>7</v>
       </c>
-      <c r="W144" s="46">
+      <c r="W144" s="143">
         <v>0</v>
       </c>
       <c r="X144" s="55">
         <v>0.25</v>
       </c>
-      <c r="Y144" s="55">
+      <c r="Y144" s="144">
         <v>0.25</v>
       </c>
-      <c r="Z144" s="55">
+      <c r="Z144" s="144">
         <v>0.8</v>
       </c>
       <c r="AA144" s="55">
         <v>0</v>
       </c>
-      <c r="AB144" s="148" t="s">
+      <c r="AB144" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="AC144" s="26" t="s">
+      <c r="AC144" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="AD144" s="26" t="s">
+      <c r="AD144" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="AE144" s="44"/>
-      <c r="AF144" s="43"/>
+      <c r="AE144" s="145"/>
+      <c r="AF144" s="146"/>
     </row>
     <row r="145" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="146" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
@@ -17205,8 +17331,8 @@
       <c r="C147" s="22"/>
       <c r="D147" s="22"/>
       <c r="E147" s="22"/>
-      <c r="F147" s="153"/>
-      <c r="G147" s="153"/>
+      <c r="F147" s="152"/>
+      <c r="G147" s="152"/>
       <c r="H147" s="21" t="s">
         <v>56</v>
       </c>
@@ -18162,18 +18288,18 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="F147:G147"/>
   </mergeCells>
-  <conditionalFormatting sqref="M121:M127 R121:T127 M24:M56 R24:T56 R58:T118 M58:M118">
-    <cfRule type="expression" dxfId="105" priority="82">
+  <conditionalFormatting sqref="M121:M127 R121:T127 M24:M56 R24:T56 S130:T130 M130 M58:M118 R58:T118">
+    <cfRule type="expression" dxfId="117" priority="76">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M119 R119:T119">
-    <cfRule type="expression" dxfId="104" priority="75">
+    <cfRule type="expression" dxfId="116" priority="69">
       <formula>M119=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N119:Q119">
-    <cfRule type="colorScale" priority="74">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18185,12 +18311,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M118:M122 R118:T122">
-    <cfRule type="expression" dxfId="103" priority="69">
+    <cfRule type="expression" dxfId="115" priority="63">
       <formula>M118=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N118:Q122">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18202,7 +18328,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N121:Q127 N24:Q56 N58:Q118">
-    <cfRule type="colorScale" priority="87">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18214,12 +18340,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="102" priority="67">
+    <cfRule type="expression" dxfId="114" priority="61">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N117:Q117">
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18230,13 +18356,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M132:M135 R132:T135">
-    <cfRule type="expression" dxfId="101" priority="39">
-      <formula>M132=FALSE</formula>
+  <conditionalFormatting sqref="M128:M129 R128:T129">
+    <cfRule type="expression" dxfId="113" priority="58">
+      <formula>M128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N132:Q135">
-    <cfRule type="colorScale" priority="40">
+  <conditionalFormatting sqref="M128 R128:T128">
+    <cfRule type="expression" dxfId="112" priority="57">
+      <formula>M128=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N128:Q128">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18247,13 +18378,157 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N128:Q130">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R130">
+    <cfRule type="expression" dxfId="111" priority="55">
+      <formula>R130=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S131:T131 M131">
+    <cfRule type="expression" dxfId="110" priority="54">
+      <formula>M131=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N131:Q131">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R131">
+    <cfRule type="expression" dxfId="109" priority="52">
+      <formula>R131=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R136">
+    <cfRule type="expression" dxfId="108" priority="37">
+      <formula>R136=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S136:T136 M136">
+    <cfRule type="expression" dxfId="107" priority="39">
+      <formula>M136=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N136:Q136">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S137:T137 M137">
+    <cfRule type="expression" dxfId="106" priority="32">
+      <formula>M137=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M132:M135 R132:T135">
+    <cfRule type="expression" dxfId="105" priority="33">
+      <formula>M132=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N132:Q135">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N137:Q137">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R137">
+    <cfRule type="expression" dxfId="104" priority="30">
+      <formula>R137=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R138">
+    <cfRule type="expression" dxfId="103" priority="25">
+      <formula>R138=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N138:Q138">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S138:T138 M138">
+    <cfRule type="expression" dxfId="102" priority="27">
+      <formula>M138=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R139">
+    <cfRule type="expression" dxfId="101" priority="20">
+      <formula>R139=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N139:Q139">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S139:T139 M139">
+    <cfRule type="expression" dxfId="100" priority="22">
+      <formula>M139=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="100" priority="24">
+    <cfRule type="expression" dxfId="99" priority="18">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N141:Q141">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18265,12 +18540,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="99" priority="22">
+    <cfRule type="expression" dxfId="98" priority="16">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57:Q57">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18282,12 +18557,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="98" priority="20">
+    <cfRule type="expression" dxfId="97" priority="14">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N140:Q140">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18299,12 +18574,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M142 R142:T142">
-    <cfRule type="expression" dxfId="97" priority="18">
+    <cfRule type="expression" dxfId="96" priority="12">
       <formula>M142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N142:Q142">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18316,12 +18591,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M143 R143:T143">
-    <cfRule type="expression" dxfId="96" priority="14">
+    <cfRule type="expression" dxfId="95" priority="8">
       <formula>M143=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N143:Q143">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18332,29 +18607,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R144:T144 M144">
-    <cfRule type="expression" dxfId="95" priority="5">
-      <formula>M144=FALSE</formula>
+  <conditionalFormatting sqref="R144">
+    <cfRule type="expression" dxfId="94" priority="3">
+      <formula>R144=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N144:Q144">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R136:T139 M136:M139">
-    <cfRule type="expression" dxfId="94" priority="3">
-      <formula>M136=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N136:Q139">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -18366,29 +18624,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R128:T131 M128:M131">
-    <cfRule type="expression" dxfId="93" priority="1">
-      <formula>M128=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N128:Q131">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+  <conditionalFormatting sqref="S144:T144 M144">
+    <cfRule type="expression" dxfId="93" priority="5">
+      <formula>M144=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G137"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G138:G144 J143:J144 G42:G136 J24:J141 H40:I144">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G136 J24:J141 H40:I144 J143:J144 G138:G144">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D149:G160 P142:V142 Q143:W144 M142:N142 N143:O144 Q24:W141 N24:O141">
+    <dataValidation type="decimal" allowBlank="1" sqref="D149:G160 P142:V142 N24:O141 Q143:W144 M142:N142 N143:O144 Q24:W141">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -18399,7 +18645,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C149:C160 C24:C144">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J159:L159 M149:O160 AA142:AC142 AC143:AC144 AB24:AB144 AC24:AC141 AD24:AF144"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J159:L159 M149:O160 AB24:AF144 AA142:AB142"/>
     <dataValidation type="list" sqref="P143:P144 O142 P24:P141">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
@@ -18435,7 +18681,7 @@
   </sheetPr>
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
@@ -18471,8 +18717,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
[FIX] golden chance and fury = 0 for moonCake. increased HP
Former-commit-id: 2d0b039c2043622b852c7859b784d2884c95d351
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2104,7 +2104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2503,6 +2503,52 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5381,10 +5427,10 @@
   </sheetPr>
   <dimension ref="A1:AF175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="AB105" sqref="AB105"/>
+      <selection pane="topRight" activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13408,7 +13454,7 @@
         <v>20</v>
       </c>
       <c r="E104" s="76">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F104" s="76">
         <v>0</v>
@@ -13423,10 +13469,10 @@
         <v>25</v>
       </c>
       <c r="J104" s="76">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K104" s="42">
-        <v>0.22499999999999998</v>
+        <v>0</v>
       </c>
       <c r="L104" s="76">
         <v>0</v>
@@ -13488,74 +13534,74 @@
       <c r="AE104" s="26"/>
       <c r="AF104" s="59"/>
     </row>
-    <row r="105" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="135" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="49" t="s">
+    <row r="105" spans="1:32" s="171" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="159" t="s">
         <v>506</v>
       </c>
-      <c r="C105" s="77" t="s">
+      <c r="C105" s="160" t="s">
         <v>61</v>
       </c>
-      <c r="D105" s="61">
+      <c r="D105" s="161">
         <v>20</v>
       </c>
-      <c r="E105" s="76">
-        <v>3</v>
-      </c>
-      <c r="F105" s="76">
-        <v>0</v>
-      </c>
-      <c r="G105" s="76">
-        <v>5</v>
-      </c>
-      <c r="H105" s="76">
-        <v>0</v>
-      </c>
-      <c r="I105" s="76">
+      <c r="E105" s="162">
+        <v>0</v>
+      </c>
+      <c r="F105" s="162">
+        <v>0</v>
+      </c>
+      <c r="G105" s="162">
+        <v>30</v>
+      </c>
+      <c r="H105" s="162">
+        <v>0</v>
+      </c>
+      <c r="I105" s="162">
         <v>25</v>
       </c>
-      <c r="J105" s="76">
-        <v>0.6</v>
-      </c>
-      <c r="K105" s="42">
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="L105" s="76">
-        <v>0</v>
-      </c>
-      <c r="M105" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="N105" s="47">
-        <v>5</v>
-      </c>
-      <c r="O105" s="47">
-        <v>5</v>
-      </c>
-      <c r="P105" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q105" s="47">
-        <v>0</v>
-      </c>
-      <c r="R105" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="S105" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="T105" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="U105" s="46">
-        <v>1</v>
-      </c>
-      <c r="V105" s="46">
-        <v>1</v>
-      </c>
-      <c r="W105" s="46">
+      <c r="J105" s="162">
+        <v>0</v>
+      </c>
+      <c r="K105" s="163">
+        <v>0</v>
+      </c>
+      <c r="L105" s="162">
+        <v>0</v>
+      </c>
+      <c r="M105" s="164" t="b">
+        <v>1</v>
+      </c>
+      <c r="N105" s="156">
+        <v>5</v>
+      </c>
+      <c r="O105" s="156">
+        <v>5</v>
+      </c>
+      <c r="P105" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="156">
+        <v>0</v>
+      </c>
+      <c r="R105" s="165" t="b">
+        <v>1</v>
+      </c>
+      <c r="S105" s="166" t="b">
+        <v>0</v>
+      </c>
+      <c r="T105" s="167" t="b">
+        <v>0</v>
+      </c>
+      <c r="U105" s="168">
+        <v>1</v>
+      </c>
+      <c r="V105" s="168">
+        <v>1</v>
+      </c>
+      <c r="W105" s="168">
         <v>0</v>
       </c>
       <c r="X105" s="55">
@@ -13570,17 +13616,17 @@
       <c r="AA105" s="55">
         <v>0</v>
       </c>
-      <c r="AB105" s="45" t="s">
+      <c r="AB105" s="169" t="s">
         <v>507</v>
       </c>
-      <c r="AC105" s="44" t="s">
+      <c r="AC105" s="170" t="s">
         <v>59</v>
       </c>
-      <c r="AD105" s="44" t="s">
+      <c r="AD105" s="170" t="s">
         <v>58</v>
       </c>
-      <c r="AE105" s="26"/>
-      <c r="AF105" s="59"/>
+      <c r="AE105" s="170"/>
+      <c r="AF105" s="157"/>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A106" s="123" t="s">
@@ -16832,7 +16878,7 @@
         <v>0.3</v>
       </c>
       <c r="K140" s="53">
-        <v>0.23</v>
+        <v>0.08</v>
       </c>
       <c r="L140" s="65">
         <v>0</v>

</xml_diff>

<commit_message>
[CHANGE] Tweaking numbers for collectible item pumpkin
Former-commit-id: 9aef84fe14729c1cac6d20dc86e942242401fcd8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -2507,9 +2507,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2524,6 +2521,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5396,10 +5396,10 @@
   </sheetPr>
   <dimension ref="A1:AF177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="V132" sqref="V132"/>
+      <selection pane="topRight" activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5451,8 +5451,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5616,8 +5616,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="152"/>
-      <c r="F22" s="152"/>
+      <c r="E22" s="157"/>
+      <c r="F22" s="157"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -13525,7 +13525,7 @@
         <v>120</v>
       </c>
       <c r="E105" s="76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F105" s="76">
         <v>0</v>
@@ -13534,16 +13534,16 @@
         <v>20</v>
       </c>
       <c r="H105" s="76">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I105" s="76">
         <v>32</v>
       </c>
       <c r="J105" s="76">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K105" s="42">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="L105" s="76">
         <v>0</v>
@@ -13619,7 +13619,7 @@
         <v>40</v>
       </c>
       <c r="E106" s="76">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F106" s="76">
         <v>0</v>
@@ -13628,16 +13628,16 @@
         <v>5</v>
       </c>
       <c r="H106" s="76">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I106" s="76">
         <v>24</v>
       </c>
       <c r="J106" s="76">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K106" s="42">
-        <v>0.23</v>
+        <v>0.15</v>
       </c>
       <c r="L106" s="76">
         <v>0</v>
@@ -13709,9 +13709,11 @@
       <c r="C107" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="D107" s="61"/>
+      <c r="D107" s="61">
+        <v>30</v>
+      </c>
       <c r="E107" s="76">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F107" s="76">
         <v>0</v>
@@ -13720,16 +13722,16 @@
         <v>5</v>
       </c>
       <c r="H107" s="76">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I107" s="76">
         <v>95</v>
       </c>
       <c r="J107" s="76">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="K107" s="42">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="L107" s="76">
         <v>0</v>
@@ -15980,13 +15982,13 @@
       <c r="AA130" s="55">
         <v>0</v>
       </c>
-      <c r="AB130" s="153" t="s">
+      <c r="AB130" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="AC130" s="154" t="s">
+      <c r="AC130" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD130" s="154" t="s">
+      <c r="AD130" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE130" s="145"/>
@@ -16072,13 +16074,13 @@
       <c r="AA131" s="55">
         <v>0</v>
       </c>
-      <c r="AB131" s="153" t="s">
+      <c r="AB131" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="AC131" s="154" t="s">
+      <c r="AC131" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD131" s="154" t="s">
+      <c r="AD131" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE131" s="145"/>
@@ -16164,13 +16166,13 @@
       <c r="AA132" s="52">
         <v>0</v>
       </c>
-      <c r="AB132" s="155" t="s">
+      <c r="AB132" s="154" t="s">
         <v>224</v>
       </c>
-      <c r="AC132" s="154" t="s">
+      <c r="AC132" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD132" s="154" t="s">
+      <c r="AD132" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE132" s="63"/>
@@ -16256,13 +16258,13 @@
       <c r="AA133" s="52">
         <v>0</v>
       </c>
-      <c r="AB133" s="155" t="s">
+      <c r="AB133" s="154" t="s">
         <v>224</v>
       </c>
-      <c r="AC133" s="154" t="s">
+      <c r="AC133" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD133" s="154" t="s">
+      <c r="AD133" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE133" s="72"/>
@@ -16348,13 +16350,13 @@
       <c r="AA134" s="52">
         <v>0</v>
       </c>
-      <c r="AB134" s="155" t="s">
+      <c r="AB134" s="154" t="s">
         <v>224</v>
       </c>
-      <c r="AC134" s="154" t="s">
+      <c r="AC134" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD134" s="154" t="s">
+      <c r="AD134" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE134" s="72"/>
@@ -16440,13 +16442,13 @@
       <c r="AA135" s="142">
         <v>0</v>
       </c>
-      <c r="AB135" s="156" t="s">
+      <c r="AB135" s="155" t="s">
         <v>224</v>
       </c>
-      <c r="AC135" s="154" t="s">
+      <c r="AC135" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD135" s="154" t="s">
+      <c r="AD135" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE135" s="25"/>
@@ -16532,13 +16534,13 @@
       <c r="AA136" s="55">
         <v>0</v>
       </c>
-      <c r="AB136" s="153" t="s">
+      <c r="AB136" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="AC136" s="154" t="s">
+      <c r="AC136" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD136" s="154" t="s">
+      <c r="AD136" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE136" s="145"/>
@@ -16627,13 +16629,13 @@
       <c r="AA137" s="55">
         <v>0</v>
       </c>
-      <c r="AB137" s="153" t="s">
+      <c r="AB137" s="152" t="s">
         <v>338</v>
       </c>
-      <c r="AC137" s="154" t="s">
+      <c r="AC137" s="153" t="s">
         <v>337</v>
       </c>
-      <c r="AD137" s="154" t="s">
+      <c r="AD137" s="153" t="s">
         <v>137</v>
       </c>
       <c r="AE137" s="145"/>
@@ -16719,13 +16721,13 @@
       <c r="AA138" s="55">
         <v>0</v>
       </c>
-      <c r="AB138" s="153" t="s">
+      <c r="AB138" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="AC138" s="154" t="s">
+      <c r="AC138" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD138" s="154" t="s">
+      <c r="AD138" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE138" s="145"/>
@@ -16811,13 +16813,13 @@
       <c r="AA139" s="55">
         <v>0</v>
       </c>
-      <c r="AB139" s="153" t="s">
+      <c r="AB139" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="AC139" s="154" t="s">
+      <c r="AC139" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD139" s="154" t="s">
+      <c r="AD139" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE139" s="145"/>
@@ -16905,13 +16907,13 @@
       <c r="AA140" s="142">
         <v>0</v>
       </c>
-      <c r="AB140" s="156" t="s">
+      <c r="AB140" s="155" t="s">
         <v>65</v>
       </c>
-      <c r="AC140" s="157" t="s">
+      <c r="AC140" s="156" t="s">
         <v>64</v>
       </c>
-      <c r="AD140" s="157" t="s">
+      <c r="AD140" s="156" t="s">
         <v>63</v>
       </c>
       <c r="AE140" s="25"/>
@@ -16997,13 +16999,13 @@
       <c r="AA141" s="52">
         <v>0</v>
       </c>
-      <c r="AB141" s="155" t="s">
+      <c r="AB141" s="154" t="s">
         <v>224</v>
       </c>
-      <c r="AC141" s="154" t="s">
+      <c r="AC141" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD141" s="154" t="s">
+      <c r="AD141" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE141" s="72"/>
@@ -17091,13 +17093,13 @@
       <c r="AA142" s="52">
         <v>0</v>
       </c>
-      <c r="AB142" s="155" t="s">
+      <c r="AB142" s="154" t="s">
         <v>224</v>
       </c>
-      <c r="AC142" s="154" t="s">
+      <c r="AC142" s="153" t="s">
         <v>510</v>
       </c>
-      <c r="AD142" s="154" t="s">
+      <c r="AD142" s="153" t="s">
         <v>150</v>
       </c>
       <c r="AE142" s="72"/>
@@ -17331,8 +17333,8 @@
       <c r="C147" s="22"/>
       <c r="D147" s="22"/>
       <c r="E147" s="22"/>
-      <c r="F147" s="152"/>
-      <c r="G147" s="152"/>
+      <c r="F147" s="157"/>
+      <c r="G147" s="157"/>
       <c r="H147" s="21" t="s">
         <v>56</v>
       </c>
@@ -18717,8 +18719,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
Added Halloween entities manually (merge conflicts)
Former-commit-id: a505f0710fa59187824eee942dcc0879e3f4c844
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$146:$O$147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$149:$O$150</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="512">
   <si>
     <t>tier_4</t>
   </si>
@@ -1565,6 +1565,18 @@
   </si>
   <si>
     <t>TID_EDIBLE_MOONCAKE</t>
+  </si>
+  <si>
+    <t>season_halloween_0</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SEASON_HALLOWEEN</t>
+  </si>
+  <si>
+    <t>season_halloween_1</t>
+  </si>
+  <si>
+    <t>season_halloween_2</t>
   </si>
 </sst>
 </file>
@@ -2500,9 +2512,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2549,12 +2558,204 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="119">
+  <dxfs count="120">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4850,188 +5051,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5046,114 +5065,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF142" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF142"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF145" totalsRowShown="0" headerRowDxfId="119" dataDxfId="117" headerRowBorderDxfId="118" tableBorderDxfId="116" totalsRowBorderDxfId="115">
+  <autoFilter ref="A23:AF145"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="114"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="113"/>
+    <tableColumn id="6" name="[category]" dataDxfId="112"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="111"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="110"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="109"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="108"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="107"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="106"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="105"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="104"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="103"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="102"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="101"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="100"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="99"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="98"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="97"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="96"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="95"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="94"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="93"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="92"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="91"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="90"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="89"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="88"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="87"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="86"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="85"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="84"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="78"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A146:O158" totalsRowShown="0">
-  <autoFilter ref="A146:O158"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A149:O161" totalsRowShown="0">
+  <autoFilter ref="A149:O161"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="4" name="[category]" dataDxfId="72" totalsRowDxfId="71"/>
+    <tableColumn id="16" name="[size]" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="48" totalsRowDxfId="47"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="6" name="[order]" dataDxfId="40"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="39"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="38"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="37"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="30"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="28"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="27" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5425,12 +5444,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF175"/>
+  <dimension ref="A1:AF178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="G105" sqref="G105"/>
+      <selection pane="topRight" activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5474,8 +5493,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="155"/>
-      <c r="F3" s="155"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5639,8 +5658,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="155"/>
-      <c r="F22" s="155"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="171"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -13534,74 +13553,74 @@
       <c r="AE104" s="26"/>
       <c r="AF104" s="59"/>
     </row>
-    <row r="105" spans="1:32" s="171" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="158" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="159" t="s">
+    <row r="105" spans="1:32" s="170" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="157" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="158" t="s">
         <v>506</v>
       </c>
-      <c r="C105" s="160" t="s">
+      <c r="C105" s="159" t="s">
         <v>61</v>
       </c>
-      <c r="D105" s="161">
+      <c r="D105" s="160">
         <v>20</v>
       </c>
-      <c r="E105" s="162">
-        <v>0</v>
-      </c>
-      <c r="F105" s="162">
-        <v>0</v>
-      </c>
-      <c r="G105" s="162">
+      <c r="E105" s="161">
+        <v>0</v>
+      </c>
+      <c r="F105" s="161">
+        <v>0</v>
+      </c>
+      <c r="G105" s="161">
         <v>30</v>
       </c>
-      <c r="H105" s="162">
-        <v>0</v>
-      </c>
-      <c r="I105" s="162">
+      <c r="H105" s="161">
+        <v>0</v>
+      </c>
+      <c r="I105" s="161">
         <v>25</v>
       </c>
-      <c r="J105" s="162">
-        <v>0</v>
-      </c>
-      <c r="K105" s="163">
-        <v>0</v>
-      </c>
-      <c r="L105" s="162">
-        <v>0</v>
-      </c>
-      <c r="M105" s="164" t="b">
-        <v>1</v>
-      </c>
-      <c r="N105" s="156">
-        <v>5</v>
-      </c>
-      <c r="O105" s="156">
-        <v>5</v>
-      </c>
-      <c r="P105" s="156">
-        <v>0</v>
-      </c>
-      <c r="Q105" s="156">
-        <v>0</v>
-      </c>
-      <c r="R105" s="165" t="b">
-        <v>1</v>
-      </c>
-      <c r="S105" s="166" t="b">
-        <v>0</v>
-      </c>
-      <c r="T105" s="167" t="b">
-        <v>0</v>
-      </c>
-      <c r="U105" s="168">
-        <v>1</v>
-      </c>
-      <c r="V105" s="168">
-        <v>1</v>
-      </c>
-      <c r="W105" s="168">
+      <c r="J105" s="161">
+        <v>0</v>
+      </c>
+      <c r="K105" s="162">
+        <v>0</v>
+      </c>
+      <c r="L105" s="161">
+        <v>0</v>
+      </c>
+      <c r="M105" s="163" t="b">
+        <v>1</v>
+      </c>
+      <c r="N105" s="155">
+        <v>5</v>
+      </c>
+      <c r="O105" s="155">
+        <v>5</v>
+      </c>
+      <c r="P105" s="155">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="155">
+        <v>0</v>
+      </c>
+      <c r="R105" s="164" t="b">
+        <v>1</v>
+      </c>
+      <c r="S105" s="165" t="b">
+        <v>0</v>
+      </c>
+      <c r="T105" s="166" t="b">
+        <v>0</v>
+      </c>
+      <c r="U105" s="167">
+        <v>1</v>
+      </c>
+      <c r="V105" s="167">
+        <v>1</v>
+      </c>
+      <c r="W105" s="167">
         <v>0</v>
       </c>
       <c r="X105" s="55">
@@ -13616,17 +13635,17 @@
       <c r="AA105" s="55">
         <v>0</v>
       </c>
-      <c r="AB105" s="169" t="s">
+      <c r="AB105" s="168" t="s">
         <v>507</v>
       </c>
-      <c r="AC105" s="170" t="s">
+      <c r="AC105" s="169" t="s">
         <v>59</v>
       </c>
-      <c r="AD105" s="170" t="s">
+      <c r="AD105" s="169" t="s">
         <v>58</v>
       </c>
-      <c r="AE105" s="170"/>
-      <c r="AF105" s="157"/>
+      <c r="AE105" s="169"/>
+      <c r="AF105" s="156"/>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A106" s="123" t="s">
@@ -17129,282 +17148,417 @@
       <c r="AE142" s="145"/>
       <c r="AF142" s="146"/>
     </row>
-    <row r="143" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="144" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A144" s="9" t="s">
+    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A143" s="135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B143" s="49" t="s">
+        <v>508</v>
+      </c>
+      <c r="C143" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D143" s="61">
+        <v>120</v>
+      </c>
+      <c r="E143" s="76">
+        <v>2</v>
+      </c>
+      <c r="F143" s="76">
+        <v>0</v>
+      </c>
+      <c r="G143" s="76">
+        <v>20</v>
+      </c>
+      <c r="H143" s="76">
+        <v>15</v>
+      </c>
+      <c r="I143" s="76">
+        <v>32</v>
+      </c>
+      <c r="J143" s="76">
+        <v>0.2</v>
+      </c>
+      <c r="K143" s="42">
+        <v>0.05</v>
+      </c>
+      <c r="L143" s="76">
+        <v>0</v>
+      </c>
+      <c r="M143" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N143" s="47">
+        <v>5</v>
+      </c>
+      <c r="O143" s="47">
+        <v>5</v>
+      </c>
+      <c r="P143" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q143" s="47">
+        <v>0</v>
+      </c>
+      <c r="R143" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S143" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T143" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U143" s="46">
+        <v>1</v>
+      </c>
+      <c r="V143" s="46">
+        <v>1</v>
+      </c>
+      <c r="W143" s="46">
+        <v>0</v>
+      </c>
+      <c r="X143" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y143" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z143" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA143" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB143" s="45" t="s">
+        <v>509</v>
+      </c>
+      <c r="AC143" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD143" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE143" s="26"/>
+      <c r="AF143" s="59"/>
+    </row>
+    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A144" s="135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B144" s="49" t="s">
+        <v>510</v>
+      </c>
+      <c r="C144" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D144" s="61">
+        <v>40</v>
+      </c>
+      <c r="E144" s="76">
+        <v>10</v>
+      </c>
+      <c r="F144" s="76">
+        <v>0</v>
+      </c>
+      <c r="G144" s="76">
+        <v>5</v>
+      </c>
+      <c r="H144" s="76">
+        <v>60</v>
+      </c>
+      <c r="I144" s="76">
+        <v>24</v>
+      </c>
+      <c r="J144" s="76">
+        <v>0.2</v>
+      </c>
+      <c r="K144" s="42">
+        <v>0.15</v>
+      </c>
+      <c r="L144" s="76">
+        <v>0</v>
+      </c>
+      <c r="M144" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N144" s="47">
+        <v>5</v>
+      </c>
+      <c r="O144" s="47">
+        <v>5</v>
+      </c>
+      <c r="P144" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q144" s="47">
+        <v>0</v>
+      </c>
+      <c r="R144" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S144" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T144" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U144" s="46">
+        <v>1</v>
+      </c>
+      <c r="V144" s="46">
+        <v>1</v>
+      </c>
+      <c r="W144" s="46">
+        <v>0</v>
+      </c>
+      <c r="X144" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y144" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z144" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA144" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB144" s="45" t="s">
+        <v>509</v>
+      </c>
+      <c r="AC144" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD144" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE144" s="26"/>
+      <c r="AF144" s="59"/>
+    </row>
+    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A145" s="135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145" s="49" t="s">
+        <v>511</v>
+      </c>
+      <c r="C145" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D145" s="61">
+        <v>30</v>
+      </c>
+      <c r="E145" s="76">
+        <v>4</v>
+      </c>
+      <c r="F145" s="76">
+        <v>0</v>
+      </c>
+      <c r="G145" s="76">
+        <v>5</v>
+      </c>
+      <c r="H145" s="76">
+        <v>20</v>
+      </c>
+      <c r="I145" s="76">
+        <v>95</v>
+      </c>
+      <c r="J145" s="76">
+        <v>0.6</v>
+      </c>
+      <c r="K145" s="42">
+        <v>0.03</v>
+      </c>
+      <c r="L145" s="76">
+        <v>0</v>
+      </c>
+      <c r="M145" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N145" s="47">
+        <v>5</v>
+      </c>
+      <c r="O145" s="47">
+        <v>5</v>
+      </c>
+      <c r="P145" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q145" s="47">
+        <v>0</v>
+      </c>
+      <c r="R145" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S145" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T145" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U145" s="46">
+        <v>1</v>
+      </c>
+      <c r="V145" s="46">
+        <v>1</v>
+      </c>
+      <c r="W145" s="46">
+        <v>0</v>
+      </c>
+      <c r="X145" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y145" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z145" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA145" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB145" s="45" t="s">
+        <v>509</v>
+      </c>
+      <c r="AC145" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD145" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE145" s="26"/>
+      <c r="AF145" s="59"/>
+    </row>
+    <row r="146" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="147" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A147" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B144" s="9"/>
-      <c r="C144" s="9"/>
-      <c r="D144" s="9"/>
-      <c r="E144" s="9"/>
-      <c r="F144" s="9"/>
-      <c r="G144" s="9"/>
-      <c r="H144" s="9"/>
-      <c r="I144" s="9"/>
-      <c r="J144" s="9"/>
-      <c r="K144" s="9"/>
-      <c r="L144" s="9"/>
-      <c r="M144" s="9"/>
-      <c r="N144" s="9"/>
-      <c r="O144" s="9"/>
-      <c r="P144" s="9"/>
-      <c r="Q144" s="9"/>
-      <c r="R144" s="9"/>
-      <c r="S144" s="9"/>
-      <c r="T144" s="9"/>
-      <c r="U144" s="9"/>
-      <c r="V144" s="9"/>
-      <c r="W144" s="9"/>
-      <c r="X144" s="9"/>
-      <c r="Y144" s="9"/>
-      <c r="Z144" s="9"/>
-      <c r="AA144" s="9"/>
-      <c r="AF144" s="8"/>
-    </row>
-    <row r="145" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A145" s="22"/>
-      <c r="B145" s="22"/>
-      <c r="C145" s="22"/>
-      <c r="D145" s="22"/>
-      <c r="E145" s="22"/>
-      <c r="F145" s="155"/>
-      <c r="G145" s="155"/>
-      <c r="H145" s="21" t="s">
+      <c r="B147" s="9"/>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="9"/>
+      <c r="I147" s="9"/>
+      <c r="J147" s="9"/>
+      <c r="K147" s="9"/>
+      <c r="L147" s="9"/>
+      <c r="M147" s="9"/>
+      <c r="N147" s="9"/>
+      <c r="O147" s="9"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="9"/>
+      <c r="R147" s="9"/>
+      <c r="S147" s="9"/>
+      <c r="T147" s="9"/>
+      <c r="U147" s="9"/>
+      <c r="V147" s="9"/>
+      <c r="W147" s="9"/>
+      <c r="X147" s="9"/>
+      <c r="Y147" s="9"/>
+      <c r="Z147" s="9"/>
+      <c r="AA147" s="9"/>
+      <c r="AF147" s="8"/>
+    </row>
+    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A148" s="22"/>
+      <c r="B148" s="22"/>
+      <c r="C148" s="22"/>
+      <c r="D148" s="22"/>
+      <c r="E148" s="22"/>
+      <c r="F148" s="171"/>
+      <c r="G148" s="171"/>
+      <c r="H148" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I145" s="21"/>
-      <c r="J145" s="22"/>
-      <c r="K145" s="17"/>
-      <c r="L145" s="17"/>
-      <c r="M145" s="17" t="s">
+      <c r="I148" s="21"/>
+      <c r="J148" s="22"/>
+      <c r="K148" s="17"/>
+      <c r="L148" s="17"/>
+      <c r="M148" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N145" s="17"/>
-      <c r="O145" s="17"/>
-      <c r="P145" s="17"/>
-      <c r="Q145" s="17"/>
-      <c r="R145" s="17"/>
-      <c r="S145" s="17"/>
-      <c r="T145" s="17"/>
-      <c r="U145" s="17"/>
-      <c r="V145" s="17"/>
-      <c r="W145" s="17"/>
-      <c r="X145" s="17"/>
-      <c r="Y145" s="17"/>
-      <c r="Z145" s="17"/>
-      <c r="AA145" s="21"/>
-      <c r="AB145" s="21"/>
-      <c r="AC145" s="21"/>
-      <c r="AD145" s="21"/>
-      <c r="AE145" s="17"/>
-    </row>
-    <row r="146" spans="1:31" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A146" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D146" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E146" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F146" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G146" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H146" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I146" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="J146" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="K146" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="L146" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="M146" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="N146" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O146" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="147" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A147" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B147" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C147" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D147" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E147" s="14">
-        <v>3</v>
-      </c>
-      <c r="F147" s="18">
-        <v>0</v>
-      </c>
-      <c r="G147" s="18">
-        <v>0</v>
-      </c>
-      <c r="H147" s="18">
-        <v>0</v>
-      </c>
-      <c r="I147" s="18">
-        <v>0</v>
-      </c>
-      <c r="J147" s="12">
-        <v>2</v>
-      </c>
-      <c r="K147" s="12">
-        <v>0</v>
-      </c>
-      <c r="L147" s="12">
-        <v>0</v>
-      </c>
-      <c r="M147" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N147" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O147" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P147" s="17"/>
-      <c r="Q147" s="17"/>
-    </row>
-    <row r="148" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A148" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B148" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C148" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D148" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E148" s="14">
-        <v>3</v>
-      </c>
-      <c r="F148" s="18">
-        <v>0</v>
-      </c>
-      <c r="G148" s="18">
-        <v>1</v>
-      </c>
-      <c r="H148" s="18">
-        <v>0</v>
-      </c>
-      <c r="I148" s="18">
-        <v>0</v>
-      </c>
-      <c r="J148" s="12">
-        <v>2</v>
-      </c>
-      <c r="K148" s="12">
-        <v>0</v>
-      </c>
-      <c r="L148" s="12">
-        <v>0</v>
-      </c>
-      <c r="M148" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N148" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O148" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N148" s="17"/>
+      <c r="O148" s="17"/>
       <c r="P148" s="17"/>
       <c r="Q148" s="17"/>
-    </row>
-    <row r="149" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A149" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B149" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C149" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D149" s="14" t="s">
+      <c r="R148" s="17"/>
+      <c r="S148" s="17"/>
+      <c r="T148" s="17"/>
+      <c r="U148" s="17"/>
+      <c r="V148" s="17"/>
+      <c r="W148" s="17"/>
+      <c r="X148" s="17"/>
+      <c r="Y148" s="17"/>
+      <c r="Z148" s="17"/>
+      <c r="AA148" s="21"/>
+      <c r="AB148" s="21"/>
+      <c r="AC148" s="21"/>
+      <c r="AD148" s="21"/>
+      <c r="AE148" s="17"/>
+    </row>
+    <row r="149" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A149" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D149" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E149" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F149" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G149" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H149" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I149" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J149" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="K149" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L149" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M149" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N149" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="O149" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A150" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C150" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D150" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="E149" s="14">
-        <v>3</v>
-      </c>
-      <c r="F149" s="18">
-        <v>0</v>
-      </c>
-      <c r="G149" s="18">
-        <v>0</v>
-      </c>
-      <c r="H149" s="18">
-        <v>0</v>
-      </c>
-      <c r="I149" s="18">
-        <v>0</v>
-      </c>
-      <c r="J149" s="12">
-        <v>2</v>
-      </c>
-      <c r="K149" s="12">
-        <v>0</v>
-      </c>
-      <c r="L149" s="12">
-        <v>0</v>
-      </c>
-      <c r="M149" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N149" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O149" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P149" s="17"/>
-      <c r="Q149" s="17"/>
-    </row>
-    <row r="150" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A150" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B150" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C150" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D150" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="E150" s="14">
         <v>3</v>
@@ -17413,7 +17567,7 @@
         <v>0</v>
       </c>
       <c r="G150" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H150" s="18">
         <v>0</v>
@@ -17442,18 +17596,18 @@
       <c r="P150" s="17"/>
       <c r="Q150" s="17"/>
     </row>
-    <row r="151" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A151" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E151" s="14">
         <v>3</v>
@@ -17462,7 +17616,7 @@
         <v>0</v>
       </c>
       <c r="G151" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H151" s="18">
         <v>0</v>
@@ -17491,18 +17645,18 @@
       <c r="P151" s="17"/>
       <c r="Q151" s="17"/>
     </row>
-    <row r="152" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A152" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B152" s="15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E152" s="14">
         <v>3</v>
@@ -17511,7 +17665,7 @@
         <v>0</v>
       </c>
       <c r="G152" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H152" s="18">
         <v>0</v>
@@ -17540,18 +17694,18 @@
       <c r="P152" s="17"/>
       <c r="Q152" s="17"/>
     </row>
-    <row r="153" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A153" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E153" s="14">
         <v>3</v>
@@ -17560,7 +17714,7 @@
         <v>0</v>
       </c>
       <c r="G153" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H153" s="18">
         <v>0</v>
@@ -17589,15 +17743,15 @@
       <c r="P153" s="17"/>
       <c r="Q153" s="17"/>
     </row>
-    <row r="154" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A154" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B154" s="15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D154" s="14" t="s">
         <v>30</v>
@@ -17638,15 +17792,15 @@
       <c r="P154" s="17"/>
       <c r="Q154" s="17"/>
     </row>
-    <row r="155" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B155" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D155" s="14" t="s">
         <v>23</v>
@@ -17687,15 +17841,15 @@
       <c r="P155" s="17"/>
       <c r="Q155" s="17"/>
     </row>
-    <row r="156" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A156" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B156" s="15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D156" s="14" t="s">
         <v>26</v>
@@ -17736,32 +17890,32 @@
       <c r="P156" s="17"/>
       <c r="Q156" s="17"/>
     </row>
-    <row r="157" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A157" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E157" s="14">
-        <v>1</v>
-      </c>
-      <c r="F157" s="13">
-        <v>0</v>
-      </c>
-      <c r="G157" s="13">
-        <v>1</v>
-      </c>
-      <c r="H157" s="13">
-        <v>0</v>
-      </c>
-      <c r="I157" s="13">
+        <v>3</v>
+      </c>
+      <c r="F157" s="18">
+        <v>0</v>
+      </c>
+      <c r="G157" s="18">
+        <v>0</v>
+      </c>
+      <c r="H157" s="18">
+        <v>0</v>
+      </c>
+      <c r="I157" s="18">
         <v>0</v>
       </c>
       <c r="J157" s="12">
@@ -17782,33 +17936,35 @@
       <c r="O157" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="158" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P157" s="17"/>
+      <c r="Q157" s="17"/>
+    </row>
+    <row r="158" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A158" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B158" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="C158" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="D158" s="127" t="s">
-        <v>30</v>
+      <c r="B158" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C158" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D158" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E158" s="14">
-        <v>1</v>
-      </c>
-      <c r="F158" s="128">
-        <v>0</v>
-      </c>
-      <c r="G158" s="128">
-        <v>0</v>
-      </c>
-      <c r="H158" s="128">
-        <v>0</v>
-      </c>
-      <c r="I158" s="128">
+        <v>3</v>
+      </c>
+      <c r="F158" s="18">
+        <v>0</v>
+      </c>
+      <c r="G158" s="18">
+        <v>1</v>
+      </c>
+      <c r="H158" s="18">
+        <v>0</v>
+      </c>
+      <c r="I158" s="18">
         <v>0</v>
       </c>
       <c r="J158" s="12">
@@ -17829,293 +17985,438 @@
       <c r="O158" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P158" s="8"/>
-      <c r="Q158" s="8"/>
-      <c r="R158" s="8"/>
-      <c r="S158" s="8"/>
-      <c r="T158" s="8"/>
-      <c r="U158" s="8"/>
-      <c r="V158" s="8"/>
-      <c r="W158" s="8"/>
-      <c r="X158" s="8"/>
-      <c r="Y158" s="8"/>
-      <c r="Z158" s="8"/>
-      <c r="AA158" s="8"/>
-      <c r="AB158" s="8"/>
-      <c r="AC158" s="8"/>
-      <c r="AD158" s="8"/>
-      <c r="AE158" s="8"/>
-    </row>
-    <row r="159" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N159" s="8"/>
-      <c r="O159" s="8"/>
-      <c r="P159" s="8"/>
-      <c r="Q159" s="8"/>
-      <c r="R159" s="8"/>
-      <c r="S159" s="8"/>
-      <c r="T159" s="8"/>
-      <c r="U159" s="8"/>
-      <c r="V159" s="8"/>
-      <c r="W159" s="8"/>
-      <c r="X159" s="8"/>
-      <c r="Y159" s="8"/>
-      <c r="Z159" s="8"/>
-      <c r="AA159" s="8"/>
-      <c r="AB159" s="8"/>
-      <c r="AC159" s="8"/>
-      <c r="AD159" s="8"/>
-      <c r="AE159" s="8"/>
-    </row>
-    <row r="160" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="161" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A161" s="9" t="s">
+      <c r="P158" s="17"/>
+      <c r="Q158" s="17"/>
+    </row>
+    <row r="159" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B159" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C159" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D159" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E159" s="14">
+        <v>3</v>
+      </c>
+      <c r="F159" s="18">
+        <v>0</v>
+      </c>
+      <c r="G159" s="18">
+        <v>2</v>
+      </c>
+      <c r="H159" s="18">
+        <v>0</v>
+      </c>
+      <c r="I159" s="18">
+        <v>0</v>
+      </c>
+      <c r="J159" s="12">
+        <v>2</v>
+      </c>
+      <c r="K159" s="12">
+        <v>0</v>
+      </c>
+      <c r="L159" s="12">
+        <v>0</v>
+      </c>
+      <c r="M159" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N159" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O159" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P159" s="17"/>
+      <c r="Q159" s="17"/>
+    </row>
+    <row r="160" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B160" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C160" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D160" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E160" s="14">
+        <v>1</v>
+      </c>
+      <c r="F160" s="13">
+        <v>0</v>
+      </c>
+      <c r="G160" s="13">
+        <v>1</v>
+      </c>
+      <c r="H160" s="13">
+        <v>0</v>
+      </c>
+      <c r="I160" s="13">
+        <v>0</v>
+      </c>
+      <c r="J160" s="12">
+        <v>2</v>
+      </c>
+      <c r="K160" s="12">
+        <v>0</v>
+      </c>
+      <c r="L160" s="12">
+        <v>0</v>
+      </c>
+      <c r="M160" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N160" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O160" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A161" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B161" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="C161" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D161" s="127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E161" s="14">
+        <v>1</v>
+      </c>
+      <c r="F161" s="128">
+        <v>0</v>
+      </c>
+      <c r="G161" s="128">
+        <v>0</v>
+      </c>
+      <c r="H161" s="128">
+        <v>0</v>
+      </c>
+      <c r="I161" s="128">
+        <v>0</v>
+      </c>
+      <c r="J161" s="12">
+        <v>2</v>
+      </c>
+      <c r="K161" s="12">
+        <v>0</v>
+      </c>
+      <c r="L161" s="12">
+        <v>0</v>
+      </c>
+      <c r="M161" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N161" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O161" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P161" s="8"/>
+      <c r="Q161" s="8"/>
+      <c r="R161" s="8"/>
+      <c r="S161" s="8"/>
+      <c r="T161" s="8"/>
+      <c r="U161" s="8"/>
+      <c r="V161" s="8"/>
+      <c r="W161" s="8"/>
+      <c r="X161" s="8"/>
+      <c r="Y161" s="8"/>
+      <c r="Z161" s="8"/>
+      <c r="AA161" s="8"/>
+      <c r="AB161" s="8"/>
+      <c r="AC161" s="8"/>
+      <c r="AD161" s="8"/>
+      <c r="AE161" s="8"/>
+    </row>
+    <row r="162" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N162" s="8"/>
+      <c r="O162" s="8"/>
+      <c r="P162" s="8"/>
+      <c r="Q162" s="8"/>
+      <c r="R162" s="8"/>
+      <c r="S162" s="8"/>
+      <c r="T162" s="8"/>
+      <c r="U162" s="8"/>
+      <c r="V162" s="8"/>
+      <c r="W162" s="8"/>
+      <c r="X162" s="8"/>
+      <c r="Y162" s="8"/>
+      <c r="Z162" s="8"/>
+      <c r="AA162" s="8"/>
+      <c r="AB162" s="8"/>
+      <c r="AC162" s="8"/>
+      <c r="AD162" s="8"/>
+      <c r="AE162" s="8"/>
+    </row>
+    <row r="163" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="164" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A164" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B161" s="9"/>
-      <c r="C161" s="9"/>
-      <c r="D161" s="9"/>
-      <c r="E161" s="8"/>
-      <c r="F161" s="8"/>
-      <c r="G161" s="8"/>
-      <c r="H161" s="8"/>
-      <c r="I161" s="8"/>
-      <c r="J161" s="8"/>
-      <c r="K161" s="8"/>
-      <c r="L161" s="8"/>
-    </row>
-    <row r="163" spans="1:12" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="7" t="s">
+      <c r="B164" s="9"/>
+      <c r="C164" s="9"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="8"/>
+      <c r="F164" s="8"/>
+      <c r="G164" s="8"/>
+      <c r="H164" s="8"/>
+      <c r="I164" s="8"/>
+      <c r="J164" s="8"/>
+      <c r="K164" s="8"/>
+      <c r="L164" s="8"/>
+    </row>
+    <row r="166" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B163" s="6" t="s">
+      <c r="B166" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C163" s="6" t="s">
+      <c r="C166" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D163" s="5" t="s">
+      <c r="D166" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E163" s="5" t="s">
+      <c r="E166" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F163" s="5" t="s">
+      <c r="F166" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G163" s="5" t="s">
+      <c r="G166" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H163" s="5" t="s">
+      <c r="H166" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A164" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B164" s="3" t="s">
+    <row r="167" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B167" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C164" s="3" t="s">
+      <c r="C167" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D164" s="2">
+      <c r="D167" s="2">
         <v>42</v>
       </c>
-      <c r="E164" s="2">
+      <c r="E167" s="2">
         <v>8</v>
       </c>
-      <c r="F164" s="2">
+      <c r="F167" s="2">
         <v>1.3</v>
       </c>
-      <c r="G164" s="2">
-        <v>2</v>
-      </c>
-      <c r="H164" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A165" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B165" s="3" t="s">
+      <c r="G167" s="2">
+        <v>2</v>
+      </c>
+      <c r="H167" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A168" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B168" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C165" s="3" t="s">
+      <c r="C168" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D165" s="2">
+      <c r="D168" s="2">
         <v>92</v>
       </c>
-      <c r="E165" s="2">
+      <c r="E168" s="2">
         <v>10</v>
       </c>
-      <c r="F165" s="2">
+      <c r="F168" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G165" s="2">
-        <v>2</v>
-      </c>
-      <c r="H165" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A166" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B166" s="3" t="s">
+      <c r="G168" s="2">
+        <v>2</v>
+      </c>
+      <c r="H168" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A169" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B169" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C166" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D166" s="2">
+      <c r="C169" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D169" s="2">
         <v>235</v>
       </c>
-      <c r="E166" s="2">
+      <c r="E169" s="2">
         <v>12</v>
       </c>
-      <c r="F166" s="2">
+      <c r="F169" s="2">
         <v>0.9</v>
       </c>
-      <c r="G166" s="2">
-        <v>2</v>
-      </c>
-      <c r="H166" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A167" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B167" s="3" t="s">
+      <c r="G169" s="2">
+        <v>2</v>
+      </c>
+      <c r="H169" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A170" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B170" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="C170" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D167" s="2">
+      <c r="D170" s="2">
         <v>686</v>
       </c>
-      <c r="E167" s="2">
+      <c r="E170" s="2">
         <v>14</v>
       </c>
-      <c r="F167" s="2">
+      <c r="F170" s="2">
         <v>0.7</v>
       </c>
-      <c r="G167" s="2">
-        <v>2</v>
-      </c>
-      <c r="H167" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D168" s="2">
+      <c r="G170" s="2">
+        <v>2</v>
+      </c>
+      <c r="H170" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A171" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D171" s="2">
         <v>1040</v>
       </c>
-      <c r="E168" s="2">
+      <c r="E171" s="2">
         <v>14</v>
       </c>
-      <c r="F168" s="2">
+      <c r="F171" s="2">
         <v>0.5</v>
       </c>
-      <c r="G168" s="2">
-        <v>2</v>
-      </c>
-      <c r="H168" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D171" s="1">
+      <c r="G171" s="2">
+        <v>2</v>
+      </c>
+      <c r="H171" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D174" s="1">
         <v>42</v>
       </c>
-      <c r="F171" s="1">
+      <c r="F174" s="1">
         <v>1.3</v>
-      </c>
-      <c r="G171">
-        <f>D164*F164</f>
-        <v>54.6</v>
-      </c>
-      <c r="I171">
-        <f>D171*F171</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D172" s="1">
-        <v>92</v>
-      </c>
-      <c r="F172" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G172">
-        <f>D165*F165</f>
-        <v>101.2</v>
-      </c>
-      <c r="I172">
-        <f>D172*F172</f>
-        <v>101.2</v>
-      </c>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D173" s="1">
-        <v>235</v>
-      </c>
-      <c r="F173" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="G173">
-        <f>D166*F166</f>
-        <v>211.5</v>
-      </c>
-      <c r="I173">
-        <f>D173*F173</f>
-        <v>211.5</v>
-      </c>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D174" s="1">
-        <v>686</v>
-      </c>
-      <c r="F174" s="1">
-        <v>0.7</v>
       </c>
       <c r="G174">
         <f>D167*F167</f>
-        <v>480.2</v>
+        <v>54.6</v>
       </c>
       <c r="I174">
         <f>D174*F174</f>
-        <v>480.2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D175" s="1">
-        <v>1040</v>
+        <v>92</v>
       </c>
       <c r="F175" s="1">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G175">
         <f>D168*F168</f>
-        <v>520</v>
+        <v>101.2</v>
       </c>
       <c r="I175">
         <f>D175*F175</f>
+        <v>101.2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D176" s="1">
+        <v>235</v>
+      </c>
+      <c r="F176" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G176">
+        <f>D169*F169</f>
+        <v>211.5</v>
+      </c>
+      <c r="I176">
+        <f>D176*F176</f>
+        <v>211.5</v>
+      </c>
+    </row>
+    <row r="177" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D177" s="1">
+        <v>686</v>
+      </c>
+      <c r="F177" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G177">
+        <f>D170*F170</f>
+        <v>480.2</v>
+      </c>
+      <c r="I177">
+        <f>D177*F177</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="178" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D178" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F178" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G178">
+        <f>D171*F171</f>
+        <v>520</v>
+      </c>
+      <c r="I178">
+        <f>D178*F178</f>
         <v>520</v>
       </c>
     </row>
@@ -18123,20 +18424,20 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F145:G145"/>
+    <mergeCell ref="F148:G148"/>
   </mergeCells>
   <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116">
-    <cfRule type="expression" dxfId="118" priority="76">
+    <cfRule type="expression" dxfId="26" priority="78">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="117" priority="69">
+    <cfRule type="expression" dxfId="25" priority="71">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N117:Q117">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18148,11 +18449,40 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:M120 R116:T120">
-    <cfRule type="expression" dxfId="116" priority="63">
+    <cfRule type="expression" dxfId="24" priority="65">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116:Q120">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N119:Q125 N24:Q56 N58:Q104 N106:Q116">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M115 R115:T115">
+    <cfRule type="expression" dxfId="23" priority="63">
+      <formula>M115=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N115:Q115">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -18164,47 +18494,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N119:Q125 N24:Q56 N58:Q104 N106:Q116">
-    <cfRule type="colorScale" priority="81">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M115 R115:T115">
-    <cfRule type="expression" dxfId="115" priority="61">
-      <formula>M115=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N115:Q115">
-    <cfRule type="colorScale" priority="60">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M126:M127 R126:T127">
-    <cfRule type="expression" dxfId="114" priority="58">
+    <cfRule type="expression" dxfId="22" priority="60">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126 R126:T126">
-    <cfRule type="expression" dxfId="113" priority="57">
+    <cfRule type="expression" dxfId="21" priority="59">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N126:Q126">
-    <cfRule type="colorScale" priority="56">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18216,7 +18517,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N126:Q128">
-    <cfRule type="colorScale" priority="59">
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18228,17 +18529,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="112" priority="55">
+    <cfRule type="expression" dxfId="20" priority="57">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S129:T129 M129">
-    <cfRule type="expression" dxfId="111" priority="54">
+    <cfRule type="expression" dxfId="19" priority="56">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N129:Q129">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18250,22 +18551,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R129">
-    <cfRule type="expression" dxfId="110" priority="52">
+    <cfRule type="expression" dxfId="18" priority="54">
       <formula>R129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="109" priority="37">
+    <cfRule type="expression" dxfId="17" priority="39">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="108" priority="39">
+    <cfRule type="expression" dxfId="16" priority="41">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:Q134">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18277,17 +18578,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="107" priority="32">
+    <cfRule type="expression" dxfId="15" priority="34">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M133 R130:T133">
-    <cfRule type="expression" dxfId="106" priority="33">
+    <cfRule type="expression" dxfId="14" priority="35">
       <formula>M130=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N130:Q133">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18299,7 +18600,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N135:Q135">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18311,17 +18612,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="105" priority="30">
+    <cfRule type="expression" dxfId="13" priority="32">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="104" priority="25">
+    <cfRule type="expression" dxfId="12" priority="27">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N136:Q136">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18333,16 +18634,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="103" priority="27">
+    <cfRule type="expression" dxfId="11" priority="29">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R137">
-    <cfRule type="expression" dxfId="102" priority="20">
+    <cfRule type="expression" dxfId="10" priority="22">
       <formula>R137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N137:Q137">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S137:T137 M137">
+    <cfRule type="expression" dxfId="9" priority="24">
+      <formula>M137=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M139 R139:T139">
+    <cfRule type="expression" dxfId="8" priority="20">
+      <formula>M139=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N139:Q139">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -18354,17 +18677,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S137:T137 M137">
-    <cfRule type="expression" dxfId="101" priority="22">
-      <formula>M137=FALSE</formula>
+  <conditionalFormatting sqref="M57 R57:T57">
+    <cfRule type="expression" dxfId="7" priority="18">
+      <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="100" priority="18">
-      <formula>M139=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N139:Q139">
+  <conditionalFormatting sqref="N57:Q57">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -18376,12 +18694,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="99" priority="16">
-      <formula>M57=FALSE</formula>
+  <conditionalFormatting sqref="M138 R138:T138">
+    <cfRule type="expression" dxfId="6" priority="16">
+      <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57:Q57">
+  <conditionalFormatting sqref="N138:Q138">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -18393,12 +18711,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="98" priority="14">
-      <formula>M138=FALSE</formula>
+  <conditionalFormatting sqref="M140 R140:T140">
+    <cfRule type="expression" dxfId="5" priority="14">
+      <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N138:Q138">
+  <conditionalFormatting sqref="N140:Q140">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -18410,30 +18728,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="97" priority="12">
-      <formula>M140=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N140:Q140">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="96" priority="8">
+    <cfRule type="expression" dxfId="4" priority="10">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N141:Q141">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18445,11 +18746,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R142">
-    <cfRule type="expression" dxfId="95" priority="3">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>R142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N142:Q142">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S142:T142 M142">
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>M142=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R105:T105 M105">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>M105=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N105:Q105">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -18461,17 +18784,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S142:T142 M142">
-    <cfRule type="expression" dxfId="94" priority="5">
-      <formula>M142=FALSE</formula>
+  <conditionalFormatting sqref="M143:M145 R143:T145">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>M143=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R105:T105 M105">
-    <cfRule type="expression" dxfId="93" priority="1">
-      <formula>M105=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N105:Q105">
+  <conditionalFormatting sqref="N143:Q145">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -18485,32 +18803,32 @@
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G135"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G136:G142 J141:J142 H40:I142 J24:J139 G42:G134">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 J141:J145 H40:I145 G42:G134 J24:J139 G136:G145">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D147:G158 P140:V140 Q141:W142 M140:N140 N141:O142 N24:O139 Q24:W139">
+    <dataValidation type="decimal" allowBlank="1" sqref="D150:G161 P140:V140 N141:O145 M140:N140 Q24:W139 N24:O139 Q141:W145">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H147:L156 H157:I157 J158:L158 X141:AA142 W140:Z140 X24:AA139">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H150:L159 H160:I160 J161:L161 X24:AA139 W140:Z140 X141:AA145">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C147:C158 C24:C142">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C150:C161 C24:C145">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J157:L157 M147:O158 AA140:AC140 AC141:AC142 AD24:AF142 AB24:AB142 AC24:AC139"/>
-    <dataValidation type="list" sqref="P141:P142 O140 P24:P139">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J160:L160 M150:O161 AA140:AC140 AD24:AF142 AB24:AB142 AC24:AC139 AC141:AC142 AB143:AF145"/>
+    <dataValidation type="list" sqref="P24:P139 O140 P141:P145">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K141:L142 K140 K24:L139">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L145">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="M141:M142 L140 M24:M139">
+    <dataValidation type="list" sqref="M24:M139 L140 M141:M145">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F142">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F145">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J140">
@@ -18571,8 +18889,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
[CHANGE] [CONTENT] changed color text for the new pets entry in metagame. Gameplay, nerfed stats for pumpkins because firerush is activated very fast and runs were too long
Former-commit-id: 52edece4368f3f48e2ac61844aea0fed49910ee9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2567,195 +2567,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="120">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5051,6 +4862,195 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5065,58 +5065,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF145" totalsRowShown="0" headerRowDxfId="119" dataDxfId="117" headerRowBorderDxfId="118" tableBorderDxfId="116" totalsRowBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF145" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF145"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="114"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="113"/>
-    <tableColumn id="6" name="[category]" dataDxfId="112"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="111"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="110"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="109"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="108"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="107"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="106"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="105"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="104"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="103"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="102"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="101"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="100"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="99"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="98"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="97"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="96"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="95"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="94"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="93"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="92"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="91"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="90"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="89"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="88"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="87"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="86"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="85"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="84"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="83"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="78"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="77"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5129,50 +5129,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="4" name="[category]" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="16" name="[size]" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="6" name="[order]" dataDxfId="40"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="39"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="38"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="37"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="36"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="30"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="28"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5446,10 +5446,10 @@
   </sheetPr>
   <dimension ref="A1:AF178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="B104" sqref="B104"/>
+      <selection pane="topRight" activeCell="A145" sqref="A145:XFD145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17159,7 +17159,7 @@
         <v>61</v>
       </c>
       <c r="D143" s="61">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="E143" s="76">
         <v>2</v>
@@ -17171,13 +17171,13 @@
         <v>20</v>
       </c>
       <c r="H143" s="76">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I143" s="76">
         <v>32</v>
       </c>
       <c r="J143" s="76">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K143" s="42">
         <v>0.05</v>
@@ -17253,28 +17253,28 @@
         <v>61</v>
       </c>
       <c r="D144" s="61">
+        <v>23</v>
+      </c>
+      <c r="E144" s="76">
+        <v>9</v>
+      </c>
+      <c r="F144" s="76">
+        <v>0</v>
+      </c>
+      <c r="G144" s="76">
+        <v>5</v>
+      </c>
+      <c r="H144" s="76">
         <v>40</v>
-      </c>
-      <c r="E144" s="76">
-        <v>10</v>
-      </c>
-      <c r="F144" s="76">
-        <v>0</v>
-      </c>
-      <c r="G144" s="76">
-        <v>5</v>
-      </c>
-      <c r="H144" s="76">
-        <v>60</v>
       </c>
       <c r="I144" s="76">
         <v>24</v>
       </c>
       <c r="J144" s="76">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K144" s="42">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="L144" s="76">
         <v>0</v>
@@ -17347,10 +17347,10 @@
         <v>61</v>
       </c>
       <c r="D145" s="61">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E145" s="76">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F145" s="76">
         <v>0</v>
@@ -17359,16 +17359,16 @@
         <v>5</v>
       </c>
       <c r="H145" s="76">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I145" s="76">
         <v>95</v>
       </c>
       <c r="J145" s="76">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K145" s="42">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="L145" s="76">
         <v>0</v>
@@ -18427,12 +18427,12 @@
     <mergeCell ref="F148:G148"/>
   </mergeCells>
   <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116">
-    <cfRule type="expression" dxfId="26" priority="78">
+    <cfRule type="expression" dxfId="119" priority="78">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="25" priority="71">
+    <cfRule type="expression" dxfId="118" priority="71">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18449,7 +18449,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:M120 R116:T120">
-    <cfRule type="expression" dxfId="24" priority="65">
+    <cfRule type="expression" dxfId="117" priority="65">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18478,7 +18478,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115 R115:T115">
-    <cfRule type="expression" dxfId="23" priority="63">
+    <cfRule type="expression" dxfId="116" priority="63">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18495,12 +18495,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126:M127 R126:T127">
-    <cfRule type="expression" dxfId="22" priority="60">
+    <cfRule type="expression" dxfId="115" priority="60">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126 R126:T126">
-    <cfRule type="expression" dxfId="21" priority="59">
+    <cfRule type="expression" dxfId="114" priority="59">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18529,12 +18529,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="20" priority="57">
+    <cfRule type="expression" dxfId="113" priority="57">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S129:T129 M129">
-    <cfRule type="expression" dxfId="19" priority="56">
+    <cfRule type="expression" dxfId="112" priority="56">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18551,17 +18551,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R129">
-    <cfRule type="expression" dxfId="18" priority="54">
+    <cfRule type="expression" dxfId="111" priority="54">
       <formula>R129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="17" priority="39">
+    <cfRule type="expression" dxfId="110" priority="39">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="16" priority="41">
+    <cfRule type="expression" dxfId="109" priority="41">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18578,12 +18578,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="15" priority="34">
+    <cfRule type="expression" dxfId="108" priority="34">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M133 R130:T133">
-    <cfRule type="expression" dxfId="14" priority="35">
+    <cfRule type="expression" dxfId="107" priority="35">
       <formula>M130=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18612,12 +18612,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="13" priority="32">
+    <cfRule type="expression" dxfId="106" priority="32">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="12" priority="27">
+    <cfRule type="expression" dxfId="105" priority="27">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18634,12 +18634,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="11" priority="29">
+    <cfRule type="expression" dxfId="104" priority="29">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R137">
-    <cfRule type="expression" dxfId="10" priority="22">
+    <cfRule type="expression" dxfId="103" priority="22">
       <formula>R137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18656,12 +18656,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S137:T137 M137">
-    <cfRule type="expression" dxfId="9" priority="24">
+    <cfRule type="expression" dxfId="102" priority="24">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="8" priority="20">
+    <cfRule type="expression" dxfId="101" priority="20">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18678,7 +18678,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="7" priority="18">
+    <cfRule type="expression" dxfId="100" priority="18">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18695,7 +18695,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="6" priority="16">
+    <cfRule type="expression" dxfId="99" priority="16">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18712,7 +18712,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="5" priority="14">
+    <cfRule type="expression" dxfId="98" priority="14">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18729,7 +18729,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="97" priority="10">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18746,7 +18746,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R142">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="96" priority="5">
       <formula>R142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18763,12 +18763,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S142:T142 M142">
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="95" priority="7">
       <formula>M142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105:T105 M105">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="94" priority="3">
       <formula>M105=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18785,7 +18785,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M143:M145 R143:T145">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="93" priority="1">
       <formula>M143=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Tier S should burn Trolls (as they can kill them)
Former-commit-id: 96d9720222adfd7eb135261285b1222d39462c3c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5446,10 +5446,10 @@
   </sheetPr>
   <dimension ref="A1:AF178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="A145" sqref="A145:XFD145"/>
+      <selection pane="topRight" activeCell="Q120" sqref="Q120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15045,7 +15045,7 @@
         <v>1</v>
       </c>
       <c r="Q120" s="37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R120" s="36" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Content - Add Xmas gift in content
Former-commit-id: 9091c0b42ef25701b2db70cb2d7461abfbdb7b20
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$149:$O$150</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$150:$O$151</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="514">
   <si>
     <t>tier_4</t>
   </si>
@@ -1578,12 +1578,18 @@
   <si>
     <t>season_halloween_2</t>
   </si>
+  <si>
+    <t>XmasPresent</t>
+  </si>
+  <si>
+    <t>TID_SEASON_XMAS_NAME</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1685,8 +1691,27 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1798,6 +1823,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2116,7 +2153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2561,12 +2598,203 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="119">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4862,195 +5090,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5065,114 +5104,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF145" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF145"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF146" totalsRowShown="0" headerRowDxfId="118" dataDxfId="116" headerRowBorderDxfId="117" tableBorderDxfId="115" totalsRowBorderDxfId="114">
+  <autoFilter ref="A23:AF146"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="113"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="112"/>
+    <tableColumn id="6" name="[category]" dataDxfId="111"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="110"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="109"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="108"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="107"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="106"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="105"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="104"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="103"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="102"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="101"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="100"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="99"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="98"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="97"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="96"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="95"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="94"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="93"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="92"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="91"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="90"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="89"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="88"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="87"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="86"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="85"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="84"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="83"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="77"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A149:O161" totalsRowShown="0">
-  <autoFilter ref="A149:O161"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A150:O162" totalsRowShown="0">
+  <autoFilter ref="A150:O162"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="4" name="[category]" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="16" name="[size]" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="47" totalsRowDxfId="46"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="6" name="[order]" dataDxfId="39"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="38"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="37"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="36"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="29"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="27"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="26" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5444,17 +5483,19 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF178"/>
+  <dimension ref="A1:AF179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AD1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="Q120" sqref="Q120"/>
+      <selection pane="topRight" activeCell="AE147" sqref="AE147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="28" max="28" width="40.7109375" customWidth="1"/>
+    <col min="29" max="29" width="162.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="107.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -17430,184 +17471,227 @@
       <c r="AE145" s="26"/>
       <c r="AF145" s="59"/>
     </row>
-    <row r="146" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="147" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A147" s="9" t="s">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A146" s="172" t="s">
+        <v>2</v>
+      </c>
+      <c r="B146" s="49" t="s">
+        <v>512</v>
+      </c>
+      <c r="C146" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D146" s="61">
+        <v>40</v>
+      </c>
+      <c r="E146" s="76">
+        <v>6</v>
+      </c>
+      <c r="F146" s="76">
+        <v>1</v>
+      </c>
+      <c r="G146" s="76">
+        <v>5</v>
+      </c>
+      <c r="H146" s="76">
+        <v>0</v>
+      </c>
+      <c r="I146" s="76">
+        <v>0</v>
+      </c>
+      <c r="J146" s="173">
+        <v>0</v>
+      </c>
+      <c r="K146" s="174">
+        <v>0</v>
+      </c>
+      <c r="L146" s="76">
+        <v>0</v>
+      </c>
+      <c r="M146" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N146" s="47">
+        <v>5</v>
+      </c>
+      <c r="O146" s="47">
+        <v>5</v>
+      </c>
+      <c r="P146" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q146" s="47">
+        <v>0</v>
+      </c>
+      <c r="R146" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S146" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T146" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U146" s="46">
+        <v>1</v>
+      </c>
+      <c r="V146" s="46"/>
+      <c r="W146" s="46">
+        <v>0</v>
+      </c>
+      <c r="X146" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y146" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z146" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA146" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB146" s="45" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC146" s="44" t="s">
+        <v>513</v>
+      </c>
+      <c r="AD146" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE146" s="26"/>
+      <c r="AF146" s="59"/>
+    </row>
+    <row r="147" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="148" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A148" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B147" s="9"/>
-      <c r="C147" s="9"/>
-      <c r="D147" s="9"/>
-      <c r="E147" s="9"/>
-      <c r="F147" s="9"/>
-      <c r="G147" s="9"/>
-      <c r="H147" s="9"/>
-      <c r="I147" s="9"/>
-      <c r="J147" s="9"/>
-      <c r="K147" s="9"/>
-      <c r="L147" s="9"/>
-      <c r="M147" s="9"/>
-      <c r="N147" s="9"/>
-      <c r="O147" s="9"/>
-      <c r="P147" s="9"/>
-      <c r="Q147" s="9"/>
-      <c r="R147" s="9"/>
-      <c r="S147" s="9"/>
-      <c r="T147" s="9"/>
-      <c r="U147" s="9"/>
-      <c r="V147" s="9"/>
-      <c r="W147" s="9"/>
-      <c r="X147" s="9"/>
-      <c r="Y147" s="9"/>
-      <c r="Z147" s="9"/>
-      <c r="AA147" s="9"/>
-      <c r="AF147" s="8"/>
-    </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A148" s="22"/>
-      <c r="B148" s="22"/>
-      <c r="C148" s="22"/>
-      <c r="D148" s="22"/>
-      <c r="E148" s="22"/>
-      <c r="F148" s="171"/>
-      <c r="G148" s="171"/>
-      <c r="H148" s="21" t="s">
+      <c r="B148" s="9"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="9"/>
+      <c r="J148" s="9"/>
+      <c r="K148" s="9"/>
+      <c r="L148" s="9"/>
+      <c r="M148" s="9"/>
+      <c r="N148" s="9"/>
+      <c r="O148" s="9"/>
+      <c r="P148" s="9"/>
+      <c r="Q148" s="9"/>
+      <c r="R148" s="9"/>
+      <c r="S148" s="9"/>
+      <c r="T148" s="9"/>
+      <c r="U148" s="9"/>
+      <c r="V148" s="9"/>
+      <c r="W148" s="9"/>
+      <c r="X148" s="9"/>
+      <c r="Y148" s="9"/>
+      <c r="Z148" s="9"/>
+      <c r="AA148" s="9"/>
+      <c r="AF148" s="8"/>
+    </row>
+    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A149" s="22"/>
+      <c r="B149" s="22"/>
+      <c r="C149" s="22"/>
+      <c r="D149" s="22"/>
+      <c r="E149" s="22"/>
+      <c r="F149" s="171"/>
+      <c r="G149" s="171"/>
+      <c r="H149" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I148" s="21"/>
-      <c r="J148" s="22"/>
-      <c r="K148" s="17"/>
-      <c r="L148" s="17"/>
-      <c r="M148" s="17" t="s">
+      <c r="I149" s="21"/>
+      <c r="J149" s="22"/>
+      <c r="K149" s="17"/>
+      <c r="L149" s="17"/>
+      <c r="M149" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N148" s="17"/>
-      <c r="O148" s="17"/>
-      <c r="P148" s="17"/>
-      <c r="Q148" s="17"/>
-      <c r="R148" s="17"/>
-      <c r="S148" s="17"/>
-      <c r="T148" s="17"/>
-      <c r="U148" s="17"/>
-      <c r="V148" s="17"/>
-      <c r="W148" s="17"/>
-      <c r="X148" s="17"/>
-      <c r="Y148" s="17"/>
-      <c r="Z148" s="17"/>
-      <c r="AA148" s="21"/>
-      <c r="AB148" s="21"/>
-      <c r="AC148" s="21"/>
-      <c r="AD148" s="21"/>
-      <c r="AE148" s="17"/>
-    </row>
-    <row r="149" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A149" s="7" t="s">
+      <c r="N149" s="17"/>
+      <c r="O149" s="17"/>
+      <c r="P149" s="17"/>
+      <c r="Q149" s="17"/>
+      <c r="R149" s="17"/>
+      <c r="S149" s="17"/>
+      <c r="T149" s="17"/>
+      <c r="U149" s="17"/>
+      <c r="V149" s="17"/>
+      <c r="W149" s="17"/>
+      <c r="X149" s="17"/>
+      <c r="Y149" s="17"/>
+      <c r="Z149" s="17"/>
+      <c r="AA149" s="21"/>
+      <c r="AB149" s="21"/>
+      <c r="AC149" s="21"/>
+      <c r="AD149" s="21"/>
+      <c r="AE149" s="17"/>
+    </row>
+    <row r="150" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B149" s="7" t="s">
+      <c r="B150" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C149" s="7" t="s">
+      <c r="C150" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D149" s="20" t="s">
+      <c r="D150" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E149" s="20" t="s">
+      <c r="E150" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F149" s="20" t="s">
+      <c r="F150" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G149" s="20" t="s">
+      <c r="G150" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H149" s="20" t="s">
+      <c r="H150" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I149" s="20" t="s">
+      <c r="I150" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J149" s="20" t="s">
+      <c r="J150" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K149" s="20" t="s">
+      <c r="K150" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="L149" s="20" t="s">
+      <c r="L150" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M149" s="19" t="s">
+      <c r="M150" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N149" s="19" t="s">
+      <c r="N150" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O149" s="19" t="s">
+      <c r="O150" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A150" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B150" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C150" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D150" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E150" s="14">
-        <v>3</v>
-      </c>
-      <c r="F150" s="18">
-        <v>0</v>
-      </c>
-      <c r="G150" s="18">
-        <v>0</v>
-      </c>
-      <c r="H150" s="18">
-        <v>0</v>
-      </c>
-      <c r="I150" s="18">
-        <v>0</v>
-      </c>
-      <c r="J150" s="12">
-        <v>2</v>
-      </c>
-      <c r="K150" s="12">
-        <v>0</v>
-      </c>
-      <c r="L150" s="12">
-        <v>0</v>
-      </c>
-      <c r="M150" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N150" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O150" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P150" s="17"/>
-      <c r="Q150" s="17"/>
     </row>
     <row r="151" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A151" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C151" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E151" s="14">
         <v>3</v>
@@ -17616,7 +17700,7 @@
         <v>0</v>
       </c>
       <c r="G151" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H151" s="18">
         <v>0</v>
@@ -17650,13 +17734,13 @@
         <v>2</v>
       </c>
       <c r="B152" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E152" s="14">
         <v>3</v>
@@ -17665,7 +17749,7 @@
         <v>0</v>
       </c>
       <c r="G152" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H152" s="18">
         <v>0</v>
@@ -17699,13 +17783,13 @@
         <v>2</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C153" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E153" s="14">
         <v>3</v>
@@ -17714,7 +17798,7 @@
         <v>0</v>
       </c>
       <c r="G153" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H153" s="18">
         <v>0</v>
@@ -17748,13 +17832,13 @@
         <v>2</v>
       </c>
       <c r="B154" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E154" s="14">
         <v>3</v>
@@ -17763,7 +17847,7 @@
         <v>0</v>
       </c>
       <c r="G154" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H154" s="18">
         <v>0</v>
@@ -17797,13 +17881,13 @@
         <v>2</v>
       </c>
       <c r="B155" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C155" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E155" s="14">
         <v>3</v>
@@ -17812,7 +17896,7 @@
         <v>0</v>
       </c>
       <c r="G155" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H155" s="18">
         <v>0</v>
@@ -17846,13 +17930,13 @@
         <v>2</v>
       </c>
       <c r="B156" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C156" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E156" s="14">
         <v>3</v>
@@ -17861,7 +17945,7 @@
         <v>0</v>
       </c>
       <c r="G156" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H156" s="18">
         <v>0</v>
@@ -17895,13 +17979,13 @@
         <v>2</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E157" s="14">
         <v>3</v>
@@ -17910,7 +17994,7 @@
         <v>0</v>
       </c>
       <c r="G157" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H157" s="18">
         <v>0</v>
@@ -17944,13 +18028,13 @@
         <v>2</v>
       </c>
       <c r="B158" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C158" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E158" s="14">
         <v>3</v>
@@ -17959,7 +18043,7 @@
         <v>0</v>
       </c>
       <c r="G158" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H158" s="18">
         <v>0</v>
@@ -17993,13 +18077,13 @@
         <v>2</v>
       </c>
       <c r="B159" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C159" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E159" s="14">
         <v>3</v>
@@ -18008,7 +18092,7 @@
         <v>0</v>
       </c>
       <c r="G159" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H159" s="18">
         <v>0</v>
@@ -18042,27 +18126,27 @@
         <v>2</v>
       </c>
       <c r="B160" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E160" s="14">
-        <v>1</v>
-      </c>
-      <c r="F160" s="13">
-        <v>0</v>
-      </c>
-      <c r="G160" s="13">
-        <v>1</v>
-      </c>
-      <c r="H160" s="13">
-        <v>0</v>
-      </c>
-      <c r="I160" s="13">
+        <v>3</v>
+      </c>
+      <c r="F160" s="18">
+        <v>0</v>
+      </c>
+      <c r="G160" s="18">
+        <v>2</v>
+      </c>
+      <c r="H160" s="18">
+        <v>0</v>
+      </c>
+      <c r="I160" s="18">
         <v>0</v>
       </c>
       <c r="J160" s="12">
@@ -18083,33 +18167,35 @@
       <c r="O160" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P160" s="17"/>
+      <c r="Q160" s="17"/>
     </row>
     <row r="161" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A161" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B161" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="C161" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="D161" s="127" t="s">
-        <v>30</v>
+      <c r="B161" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C161" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D161" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E161" s="14">
         <v>1</v>
       </c>
-      <c r="F161" s="128">
-        <v>0</v>
-      </c>
-      <c r="G161" s="128">
-        <v>0</v>
-      </c>
-      <c r="H161" s="128">
-        <v>0</v>
-      </c>
-      <c r="I161" s="128">
+      <c r="F161" s="13">
+        <v>0</v>
+      </c>
+      <c r="G161" s="13">
+        <v>1</v>
+      </c>
+      <c r="H161" s="13">
+        <v>0</v>
+      </c>
+      <c r="I161" s="13">
         <v>0</v>
       </c>
       <c r="J161" s="12">
@@ -18130,26 +18216,53 @@
       <c r="O161" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P161" s="8"/>
-      <c r="Q161" s="8"/>
-      <c r="R161" s="8"/>
-      <c r="S161" s="8"/>
-      <c r="T161" s="8"/>
-      <c r="U161" s="8"/>
-      <c r="V161" s="8"/>
-      <c r="W161" s="8"/>
-      <c r="X161" s="8"/>
-      <c r="Y161" s="8"/>
-      <c r="Z161" s="8"/>
-      <c r="AA161" s="8"/>
-      <c r="AB161" s="8"/>
-      <c r="AC161" s="8"/>
-      <c r="AD161" s="8"/>
-      <c r="AE161" s="8"/>
     </row>
     <row r="162" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N162" s="8"/>
-      <c r="O162" s="8"/>
+      <c r="A162" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B162" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="C162" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D162" s="127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E162" s="14">
+        <v>1</v>
+      </c>
+      <c r="F162" s="128">
+        <v>0</v>
+      </c>
+      <c r="G162" s="128">
+        <v>0</v>
+      </c>
+      <c r="H162" s="128">
+        <v>0</v>
+      </c>
+      <c r="I162" s="128">
+        <v>0</v>
+      </c>
+      <c r="J162" s="12">
+        <v>2</v>
+      </c>
+      <c r="K162" s="12">
+        <v>0</v>
+      </c>
+      <c r="L162" s="12">
+        <v>0</v>
+      </c>
+      <c r="M162" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N162" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O162" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="P162" s="8"/>
       <c r="Q162" s="8"/>
       <c r="R162" s="8"/>
@@ -18167,73 +18280,67 @@
       <c r="AD162" s="8"/>
       <c r="AE162" s="8"/>
     </row>
-    <row r="163" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="164" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A164" s="9" t="s">
+    <row r="163" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N163" s="8"/>
+      <c r="O163" s="8"/>
+      <c r="P163" s="8"/>
+      <c r="Q163" s="8"/>
+      <c r="R163" s="8"/>
+      <c r="S163" s="8"/>
+      <c r="T163" s="8"/>
+      <c r="U163" s="8"/>
+      <c r="V163" s="8"/>
+      <c r="W163" s="8"/>
+      <c r="X163" s="8"/>
+      <c r="Y163" s="8"/>
+      <c r="Z163" s="8"/>
+      <c r="AA163" s="8"/>
+      <c r="AB163" s="8"/>
+      <c r="AC163" s="8"/>
+      <c r="AD163" s="8"/>
+      <c r="AE163" s="8"/>
+    </row>
+    <row r="164" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="165" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A165" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B164" s="9"/>
-      <c r="C164" s="9"/>
-      <c r="D164" s="9"/>
-      <c r="E164" s="8"/>
-      <c r="F164" s="8"/>
-      <c r="G164" s="8"/>
-      <c r="H164" s="8"/>
-      <c r="I164" s="8"/>
-      <c r="J164" s="8"/>
-      <c r="K164" s="8"/>
-      <c r="L164" s="8"/>
-    </row>
-    <row r="166" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A166" s="7" t="s">
+      <c r="B165" s="9"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="9"/>
+      <c r="E165" s="8"/>
+      <c r="F165" s="8"/>
+      <c r="G165" s="8"/>
+      <c r="H165" s="8"/>
+      <c r="I165" s="8"/>
+      <c r="J165" s="8"/>
+      <c r="K165" s="8"/>
+      <c r="L165" s="8"/>
+    </row>
+    <row r="167" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A167" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B166" s="6" t="s">
+      <c r="B167" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C166" s="6" t="s">
+      <c r="C167" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D166" s="5" t="s">
+      <c r="D167" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E166" s="5" t="s">
+      <c r="E167" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F166" s="5" t="s">
+      <c r="F167" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G166" s="5" t="s">
+      <c r="G167" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H166" s="5" t="s">
+      <c r="H167" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="167" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A167" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D167" s="2">
-        <v>42</v>
-      </c>
-      <c r="E167" s="2">
-        <v>8</v>
-      </c>
-      <c r="F167" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G167" s="2">
-        <v>2</v>
-      </c>
-      <c r="H167" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:31" x14ac:dyDescent="0.25">
@@ -18241,19 +18348,19 @@
         <v>2</v>
       </c>
       <c r="B168" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D168" s="2">
+        <v>42</v>
+      </c>
+      <c r="E168" s="2">
         <v>8</v>
       </c>
-      <c r="C168" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D168" s="2">
-        <v>92</v>
-      </c>
-      <c r="E168" s="2">
-        <v>10</v>
-      </c>
       <c r="F168" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G168" s="2">
         <v>2</v>
@@ -18267,19 +18374,19 @@
         <v>2</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D169" s="2">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="E169" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F169" s="2">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G169" s="2">
         <v>2</v>
@@ -18293,19 +18400,19 @@
         <v>2</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D170" s="2">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="E170" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F170" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G170" s="2">
         <v>2</v>
@@ -18319,104 +18426,130 @@
         <v>2</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D171" s="2">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="E171" s="2">
         <v>14</v>
       </c>
       <c r="F171" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G171" s="2">
+        <v>2</v>
+      </c>
+      <c r="H171" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A172" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D172" s="2">
+        <v>1040</v>
+      </c>
+      <c r="E172" s="2">
+        <v>14</v>
+      </c>
+      <c r="F172" s="2">
         <v>0.5</v>
       </c>
-      <c r="G171" s="2">
-        <v>2</v>
-      </c>
-      <c r="H171" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D174" s="1">
-        <v>42</v>
-      </c>
-      <c r="F174" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G174">
-        <f>D167*F167</f>
-        <v>54.6</v>
-      </c>
-      <c r="I174">
-        <f>D174*F174</f>
-        <v>54.6</v>
+      <c r="G172" s="2">
+        <v>2</v>
+      </c>
+      <c r="H172" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D175" s="1">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="F175" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G175">
         <f>D168*F168</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
       <c r="I175">
         <f>D175*F175</f>
-        <v>101.2</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="176" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D176" s="1">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="F176" s="1">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G176">
         <f>D169*F169</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
       <c r="I176">
         <f>D176*F176</f>
-        <v>211.5</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="177" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D177" s="1">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="F177" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G177">
         <f>D170*F170</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
       <c r="I177">
         <f>D177*F177</f>
-        <v>480.2</v>
+        <v>211.5</v>
       </c>
     </row>
     <row r="178" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D178" s="1">
-        <v>1040</v>
+        <v>686</v>
       </c>
       <c r="F178" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G178">
         <f>D171*F171</f>
-        <v>520</v>
+        <v>480.2</v>
       </c>
       <c r="I178">
         <f>D178*F178</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="179" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D179" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F179" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G179">
+        <f>D172*F172</f>
+        <v>520</v>
+      </c>
+      <c r="I179">
+        <f>D179*F179</f>
         <v>520</v>
       </c>
     </row>
@@ -18424,15 +18557,15 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F148:G148"/>
+    <mergeCell ref="F149:G149"/>
   </mergeCells>
-  <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116">
-    <cfRule type="expression" dxfId="119" priority="78">
+  <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M146 R143:T146">
+    <cfRule type="expression" dxfId="25" priority="78">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="118" priority="71">
+    <cfRule type="expression" dxfId="24" priority="71">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18449,7 +18582,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:M120 R116:T120">
-    <cfRule type="expression" dxfId="117" priority="65">
+    <cfRule type="expression" dxfId="23" priority="65">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18478,7 +18611,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115 R115:T115">
-    <cfRule type="expression" dxfId="116" priority="63">
+    <cfRule type="expression" dxfId="22" priority="63">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18495,12 +18628,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126:M127 R126:T127">
-    <cfRule type="expression" dxfId="115" priority="60">
+    <cfRule type="expression" dxfId="21" priority="60">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126 R126:T126">
-    <cfRule type="expression" dxfId="114" priority="59">
+    <cfRule type="expression" dxfId="20" priority="59">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18529,12 +18662,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="113" priority="57">
+    <cfRule type="expression" dxfId="19" priority="57">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S129:T129 M129">
-    <cfRule type="expression" dxfId="112" priority="56">
+    <cfRule type="expression" dxfId="18" priority="56">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18551,17 +18684,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R129">
-    <cfRule type="expression" dxfId="111" priority="54">
+    <cfRule type="expression" dxfId="17" priority="54">
       <formula>R129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="110" priority="39">
+    <cfRule type="expression" dxfId="16" priority="39">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="109" priority="41">
+    <cfRule type="expression" dxfId="15" priority="41">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18578,12 +18711,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="108" priority="34">
+    <cfRule type="expression" dxfId="14" priority="34">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M133 R130:T133">
-    <cfRule type="expression" dxfId="107" priority="35">
+    <cfRule type="expression" dxfId="13" priority="35">
       <formula>M130=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18612,12 +18745,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="106" priority="32">
+    <cfRule type="expression" dxfId="12" priority="32">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="105" priority="27">
+    <cfRule type="expression" dxfId="11" priority="27">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18634,12 +18767,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="104" priority="29">
+    <cfRule type="expression" dxfId="10" priority="29">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R137">
-    <cfRule type="expression" dxfId="103" priority="22">
+    <cfRule type="expression" dxfId="9" priority="22">
       <formula>R137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18656,12 +18789,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S137:T137 M137">
-    <cfRule type="expression" dxfId="102" priority="24">
+    <cfRule type="expression" dxfId="8" priority="24">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="101" priority="20">
+    <cfRule type="expression" dxfId="7" priority="20">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18678,7 +18811,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="100" priority="18">
+    <cfRule type="expression" dxfId="6" priority="18">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18695,7 +18828,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="99" priority="16">
+    <cfRule type="expression" dxfId="5" priority="16">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18712,7 +18845,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="98" priority="14">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18729,7 +18862,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="97" priority="10">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18746,7 +18879,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R142">
-    <cfRule type="expression" dxfId="96" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>R142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18763,12 +18896,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S142:T142 M142">
-    <cfRule type="expression" dxfId="95" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>M142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105:T105 M105">
-    <cfRule type="expression" dxfId="94" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>M105=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18784,13 +18917,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M143:M145 R143:T145">
-    <cfRule type="expression" dxfId="93" priority="1">
-      <formula>M143=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N143:Q145">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="N143:Q146">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18803,37 +18931,37 @@
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G135"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 J141:J145 H40:I145 G42:G134 J24:J139 G136:G145">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 G136:G146 H40:I146 J141:J146">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D150:G161 P140:V140 N141:O145 M140:N140 Q24:W139 N24:O139 Q141:W145">
+    <dataValidation type="decimal" allowBlank="1" sqref="D151:G162 P140:V140 M140:N140 Q141:W146 N141:O146 N24:O139 Q24:W139">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H150:L159 H160:I160 J161:L161 X24:AA139 W140:Z140 X141:AA145">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H151:L160 H161:I161 J162:L162 X141:AA146 W140:Z140 X24:AA139">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C150:C161 C24:C145">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C151:C162 C24:C146">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J160:L160 M150:O161 AA140:AC140 AD24:AF142 AB24:AB142 AC24:AC139 AC141:AC142 AB143:AF145"/>
-    <dataValidation type="list" sqref="P24:P139 O140 P141:P145">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J161:L161 M151:O162 AA140:AC140 AB131:AB142 AC131:AC139 AB143:AF146 AC141:AC142 AB24:AC130 AD24:AF142"/>
+    <dataValidation type="list" sqref="P141:P146 O140 P24:P139">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L145">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L146">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="M24:M139 L140 M141:M145">
+    <dataValidation type="list" sqref="M141:M146 L140 M24:M139">
       <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F145">
-      <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J140">
       <formula1>0</formula1>
       <formula2>10000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F146">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added feedback when dragon eats Christmas event spawner: Content + texts
Former-commit-id: b0c8e01cedbf6f937949696ce950cfa0cfb6c684
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1582,7 +1582,7 @@
     <t>XmasPresent</t>
   </si>
   <si>
-    <t>TID_SEASON_XMAS_NAME</t>
+    <t>TID_QUIP_DRG_KILL_XMAS_01</t>
   </si>
 </sst>
 </file>
@@ -2595,9 +2595,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2607,194 +2604,15 @@
     <xf numFmtId="2" fontId="16" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="119">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5090,6 +4908,188 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5104,58 +5104,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF146" totalsRowShown="0" headerRowDxfId="118" dataDxfId="116" headerRowBorderDxfId="117" tableBorderDxfId="115" totalsRowBorderDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF146" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF146"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="113"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="112"/>
-    <tableColumn id="6" name="[category]" dataDxfId="111"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="110"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="109"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="108"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="107"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="106"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="105"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="104"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="103"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="102"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="101"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="100"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="99"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="98"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="97"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="96"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="95"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="94"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="93"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="92"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="91"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="90"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="89"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="88"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="87"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="86"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="85"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="84"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="83"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="82"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="77"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5168,50 +5168,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="4" name="[category]" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="16" name="[size]" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="6" name="[order]" dataDxfId="39"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="38"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="37"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="36"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="35"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="29"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="27"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5486,9 +5486,9 @@
   <dimension ref="A1:AF179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="AE147" sqref="AE147"/>
+      <selection pane="topRight" activeCell="AC146" sqref="AC146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5534,8 +5534,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5699,8 +5699,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="171"/>
-      <c r="F22" s="171"/>
+      <c r="E22" s="174"/>
+      <c r="F22" s="174"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -17472,7 +17472,7 @@
       <c r="AF145" s="59"/>
     </row>
     <row r="146" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A146" s="172" t="s">
+      <c r="A146" s="171" t="s">
         <v>2</v>
       </c>
       <c r="B146" s="49" t="s">
@@ -17499,10 +17499,10 @@
       <c r="I146" s="76">
         <v>0</v>
       </c>
-      <c r="J146" s="173">
-        <v>0</v>
-      </c>
-      <c r="K146" s="174">
+      <c r="J146" s="172">
+        <v>0</v>
+      </c>
+      <c r="K146" s="173">
         <v>0</v>
       </c>
       <c r="L146" s="76">
@@ -17602,8 +17602,8 @@
       <c r="C149" s="22"/>
       <c r="D149" s="22"/>
       <c r="E149" s="22"/>
-      <c r="F149" s="171"/>
-      <c r="G149" s="171"/>
+      <c r="F149" s="174"/>
+      <c r="G149" s="174"/>
       <c r="H149" s="21" t="s">
         <v>56</v>
       </c>
@@ -18560,12 +18560,12 @@
     <mergeCell ref="F149:G149"/>
   </mergeCells>
   <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M146 R143:T146">
-    <cfRule type="expression" dxfId="25" priority="78">
+    <cfRule type="expression" dxfId="118" priority="78">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="24" priority="71">
+    <cfRule type="expression" dxfId="117" priority="71">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18582,7 +18582,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:M120 R116:T120">
-    <cfRule type="expression" dxfId="23" priority="65">
+    <cfRule type="expression" dxfId="116" priority="65">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18611,7 +18611,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115 R115:T115">
-    <cfRule type="expression" dxfId="22" priority="63">
+    <cfRule type="expression" dxfId="115" priority="63">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18628,12 +18628,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126:M127 R126:T127">
-    <cfRule type="expression" dxfId="21" priority="60">
+    <cfRule type="expression" dxfId="114" priority="60">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126 R126:T126">
-    <cfRule type="expression" dxfId="20" priority="59">
+    <cfRule type="expression" dxfId="113" priority="59">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18662,12 +18662,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="19" priority="57">
+    <cfRule type="expression" dxfId="112" priority="57">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S129:T129 M129">
-    <cfRule type="expression" dxfId="18" priority="56">
+    <cfRule type="expression" dxfId="111" priority="56">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18684,17 +18684,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R129">
-    <cfRule type="expression" dxfId="17" priority="54">
+    <cfRule type="expression" dxfId="110" priority="54">
       <formula>R129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="16" priority="39">
+    <cfRule type="expression" dxfId="109" priority="39">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="15" priority="41">
+    <cfRule type="expression" dxfId="108" priority="41">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18711,12 +18711,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="14" priority="34">
+    <cfRule type="expression" dxfId="107" priority="34">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M133 R130:T133">
-    <cfRule type="expression" dxfId="13" priority="35">
+    <cfRule type="expression" dxfId="106" priority="35">
       <formula>M130=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18745,12 +18745,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="12" priority="32">
+    <cfRule type="expression" dxfId="105" priority="32">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="11" priority="27">
+    <cfRule type="expression" dxfId="104" priority="27">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18767,12 +18767,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="10" priority="29">
+    <cfRule type="expression" dxfId="103" priority="29">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R137">
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="102" priority="22">
       <formula>R137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18789,12 +18789,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S137:T137 M137">
-    <cfRule type="expression" dxfId="8" priority="24">
+    <cfRule type="expression" dxfId="101" priority="24">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="7" priority="20">
+    <cfRule type="expression" dxfId="100" priority="20">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18811,7 +18811,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="6" priority="18">
+    <cfRule type="expression" dxfId="99" priority="18">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18828,7 +18828,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="5" priority="16">
+    <cfRule type="expression" dxfId="98" priority="16">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18845,7 +18845,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="97" priority="14">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18862,7 +18862,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="96" priority="10">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18879,7 +18879,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R142">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="95" priority="5">
       <formula>R142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18896,12 +18896,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S142:T142 M142">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="94" priority="7">
       <formula>M142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105:T105 M105">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="93" priority="3">
       <formula>M105=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19017,8 +19017,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
kwwbk prefab added to content with TIDS, fixed collision space gap castle, fixed level_0
Former-commit-id: 6554e1de0abd9de3fbf8a6948621ab90a22a2577
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$150:$O$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$152:$O$153</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="519">
   <si>
     <t>tier_4</t>
   </si>
@@ -1583,6 +1583,21 @@
   </si>
   <si>
     <t>TID_QUIP_DRG_KILL_XMAS_01</t>
+  </si>
+  <si>
+    <t>armour_pieces</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SEASON_MOVIE_KWWBK</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_KILL_ENT_ARMOUR_PIECES_01;TID_QUIP_DRG_KILL_ENT_ARMOUR_PIECES_02</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_BURN_ENT_05;TID_QUIP_DRG_BURN_ENT_03</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SEASON_XMAS</t>
   </si>
 </sst>
 </file>
@@ -2153,7 +2168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2607,12 +2622,243 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="119">
+  <dxfs count="120">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4908,188 +5154,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5104,114 +5168,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF146" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF146"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF147" totalsRowShown="0" headerRowDxfId="119" dataDxfId="117" headerRowBorderDxfId="118" tableBorderDxfId="116" totalsRowBorderDxfId="115">
+  <autoFilter ref="A23:AF147"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="114"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="113"/>
+    <tableColumn id="6" name="[category]" dataDxfId="112"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="111"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="110"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="109"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="108"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="107"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="106"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="105"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="104"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="103"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="102"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="101"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="100"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="99"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="98"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="97"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="96"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="95"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="94"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="93"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="92"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="91"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="90"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="89"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="88"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="87"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="86"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="85"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="84"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="78"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A150:O162" totalsRowShown="0">
-  <autoFilter ref="A150:O162"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A152:O164" totalsRowShown="0">
+  <autoFilter ref="A152:O164"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="4" name="[category]" dataDxfId="72" totalsRowDxfId="71"/>
+    <tableColumn id="16" name="[size]" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="48" totalsRowDxfId="47"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="6" name="[order]" dataDxfId="40"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="39"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="38"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="37"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="30"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="28"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="27" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5483,12 +5547,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF179"/>
+  <dimension ref="A1:AF181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="AC146" sqref="AC146"/>
+      <selection pane="topRight" activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17552,7 +17616,7 @@
         <v>0</v>
       </c>
       <c r="AB146" s="45" t="s">
-        <v>224</v>
+        <v>518</v>
       </c>
       <c r="AC146" s="44" t="s">
         <v>513</v>
@@ -17563,230 +17627,258 @@
       <c r="AE146" s="26"/>
       <c r="AF146" s="59"/>
     </row>
-    <row r="147" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="148" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A148" s="9" t="s">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A147" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" s="49" t="s">
+        <v>514</v>
+      </c>
+      <c r="C147" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D147" s="61">
+        <v>20</v>
+      </c>
+      <c r="E147" s="76">
+        <v>0</v>
+      </c>
+      <c r="F147" s="76">
+        <v>0</v>
+      </c>
+      <c r="G147" s="76">
+        <v>7</v>
+      </c>
+      <c r="H147" s="76">
+        <v>0</v>
+      </c>
+      <c r="I147" s="76">
+        <v>25</v>
+      </c>
+      <c r="J147" s="172">
+        <v>0</v>
+      </c>
+      <c r="K147" s="173">
+        <v>0</v>
+      </c>
+      <c r="L147" s="76">
+        <v>0</v>
+      </c>
+      <c r="M147" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N147" s="47">
+        <v>5</v>
+      </c>
+      <c r="O147" s="47">
+        <v>5</v>
+      </c>
+      <c r="P147" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q147" s="47">
+        <v>0</v>
+      </c>
+      <c r="R147" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S147" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T147" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U147" s="46">
+        <v>1</v>
+      </c>
+      <c r="V147" s="46"/>
+      <c r="W147" s="46">
+        <v>0</v>
+      </c>
+      <c r="X147" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y147" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z147" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA147" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB147" s="45" t="s">
+        <v>515</v>
+      </c>
+      <c r="AC147" s="44" t="s">
+        <v>516</v>
+      </c>
+      <c r="AD147" s="44" t="s">
+        <v>517</v>
+      </c>
+      <c r="AE147" s="26"/>
+      <c r="AF147" s="146"/>
+    </row>
+    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A148" s="175"/>
+      <c r="B148" s="176"/>
+      <c r="C148" s="176"/>
+      <c r="D148" s="177"/>
+      <c r="E148" s="177"/>
+      <c r="F148" s="177"/>
+      <c r="G148" s="177"/>
+      <c r="H148" s="177"/>
+      <c r="I148" s="177"/>
+      <c r="J148" s="178"/>
+      <c r="K148" s="179"/>
+      <c r="L148" s="177"/>
+      <c r="M148" s="180"/>
+      <c r="N148" s="181"/>
+      <c r="O148" s="181"/>
+      <c r="P148" s="182"/>
+      <c r="Q148" s="181"/>
+      <c r="R148" s="180"/>
+      <c r="S148" s="180"/>
+      <c r="T148" s="183"/>
+      <c r="U148" s="182"/>
+      <c r="V148" s="182"/>
+      <c r="W148" s="182"/>
+      <c r="X148" s="184"/>
+      <c r="Y148" s="184"/>
+      <c r="Z148" s="184"/>
+      <c r="AA148" s="184"/>
+      <c r="AB148" s="185"/>
+      <c r="AC148" s="186"/>
+      <c r="AD148" s="186"/>
+      <c r="AE148" s="187"/>
+      <c r="AF148" s="188"/>
+    </row>
+    <row r="149" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="150" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A150" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B148" s="9"/>
-      <c r="C148" s="9"/>
-      <c r="D148" s="9"/>
-      <c r="E148" s="9"/>
-      <c r="F148" s="9"/>
-      <c r="G148" s="9"/>
-      <c r="H148" s="9"/>
-      <c r="I148" s="9"/>
-      <c r="J148" s="9"/>
-      <c r="K148" s="9"/>
-      <c r="L148" s="9"/>
-      <c r="M148" s="9"/>
-      <c r="N148" s="9"/>
-      <c r="O148" s="9"/>
-      <c r="P148" s="9"/>
-      <c r="Q148" s="9"/>
-      <c r="R148" s="9"/>
-      <c r="S148" s="9"/>
-      <c r="T148" s="9"/>
-      <c r="U148" s="9"/>
-      <c r="V148" s="9"/>
-      <c r="W148" s="9"/>
-      <c r="X148" s="9"/>
-      <c r="Y148" s="9"/>
-      <c r="Z148" s="9"/>
-      <c r="AA148" s="9"/>
-      <c r="AF148" s="8"/>
-    </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A149" s="22"/>
-      <c r="B149" s="22"/>
-      <c r="C149" s="22"/>
-      <c r="D149" s="22"/>
-      <c r="E149" s="22"/>
-      <c r="F149" s="174"/>
-      <c r="G149" s="174"/>
-      <c r="H149" s="21" t="s">
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+      <c r="K150" s="9"/>
+      <c r="L150" s="9"/>
+      <c r="M150" s="9"/>
+      <c r="N150" s="9"/>
+      <c r="O150" s="9"/>
+      <c r="P150" s="9"/>
+      <c r="Q150" s="9"/>
+      <c r="R150" s="9"/>
+      <c r="S150" s="9"/>
+      <c r="T150" s="9"/>
+      <c r="U150" s="9"/>
+      <c r="V150" s="9"/>
+      <c r="W150" s="9"/>
+      <c r="X150" s="9"/>
+      <c r="Y150" s="9"/>
+      <c r="Z150" s="9"/>
+      <c r="AA150" s="9"/>
+      <c r="AF150" s="8"/>
+    </row>
+    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A151" s="22"/>
+      <c r="B151" s="22"/>
+      <c r="C151" s="22"/>
+      <c r="D151" s="22"/>
+      <c r="E151" s="22"/>
+      <c r="F151" s="174"/>
+      <c r="G151" s="174"/>
+      <c r="H151" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I149" s="21"/>
-      <c r="J149" s="22"/>
-      <c r="K149" s="17"/>
-      <c r="L149" s="17"/>
-      <c r="M149" s="17" t="s">
+      <c r="I151" s="21"/>
+      <c r="J151" s="22"/>
+      <c r="K151" s="17"/>
+      <c r="L151" s="17"/>
+      <c r="M151" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N149" s="17"/>
-      <c r="O149" s="17"/>
-      <c r="P149" s="17"/>
-      <c r="Q149" s="17"/>
-      <c r="R149" s="17"/>
-      <c r="S149" s="17"/>
-      <c r="T149" s="17"/>
-      <c r="U149" s="17"/>
-      <c r="V149" s="17"/>
-      <c r="W149" s="17"/>
-      <c r="X149" s="17"/>
-      <c r="Y149" s="17"/>
-      <c r="Z149" s="17"/>
-      <c r="AA149" s="21"/>
-      <c r="AB149" s="21"/>
-      <c r="AC149" s="21"/>
-      <c r="AD149" s="21"/>
-      <c r="AE149" s="17"/>
-    </row>
-    <row r="150" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A150" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B150" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C150" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D150" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E150" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F150" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G150" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H150" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I150" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="J150" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="K150" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="L150" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="M150" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="N150" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O150" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A151" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B151" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C151" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D151" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E151" s="14">
-        <v>3</v>
-      </c>
-      <c r="F151" s="18">
-        <v>0</v>
-      </c>
-      <c r="G151" s="18">
-        <v>0</v>
-      </c>
-      <c r="H151" s="18">
-        <v>0</v>
-      </c>
-      <c r="I151" s="18">
-        <v>0</v>
-      </c>
-      <c r="J151" s="12">
-        <v>2</v>
-      </c>
-      <c r="K151" s="12">
-        <v>0</v>
-      </c>
-      <c r="L151" s="12">
-        <v>0</v>
-      </c>
-      <c r="M151" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N151" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O151" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N151" s="17"/>
+      <c r="O151" s="17"/>
       <c r="P151" s="17"/>
       <c r="Q151" s="17"/>
-    </row>
-    <row r="152" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A152" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B152" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C152" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D152" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E152" s="14">
-        <v>3</v>
-      </c>
-      <c r="F152" s="18">
-        <v>0</v>
-      </c>
-      <c r="G152" s="18">
-        <v>1</v>
-      </c>
-      <c r="H152" s="18">
-        <v>0</v>
-      </c>
-      <c r="I152" s="18">
-        <v>0</v>
-      </c>
-      <c r="J152" s="12">
-        <v>2</v>
-      </c>
-      <c r="K152" s="12">
-        <v>0</v>
-      </c>
-      <c r="L152" s="12">
-        <v>0</v>
-      </c>
-      <c r="M152" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N152" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O152" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P152" s="17"/>
-      <c r="Q152" s="17"/>
+      <c r="R151" s="17"/>
+      <c r="S151" s="17"/>
+      <c r="T151" s="17"/>
+      <c r="U151" s="17"/>
+      <c r="V151" s="17"/>
+      <c r="W151" s="17"/>
+      <c r="X151" s="17"/>
+      <c r="Y151" s="17"/>
+      <c r="Z151" s="17"/>
+      <c r="AA151" s="21"/>
+      <c r="AB151" s="21"/>
+      <c r="AC151" s="21"/>
+      <c r="AD151" s="21"/>
+      <c r="AE151" s="17"/>
+    </row>
+    <row r="152" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A152" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D152" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E152" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F152" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G152" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H152" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I152" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J152" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="K152" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L152" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M152" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N152" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="O152" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="153" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A153" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D153" s="14" t="s">
         <v>30</v>
@@ -17832,10 +17924,10 @@
         <v>2</v>
       </c>
       <c r="B154" s="15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D154" s="14" t="s">
         <v>23</v>
@@ -17881,10 +17973,10 @@
         <v>2</v>
       </c>
       <c r="B155" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D155" s="14" t="s">
         <v>30</v>
@@ -17930,10 +18022,10 @@
         <v>2</v>
       </c>
       <c r="B156" s="15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D156" s="14" t="s">
         <v>23</v>
@@ -17979,13 +18071,13 @@
         <v>2</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C157" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E157" s="14">
         <v>3</v>
@@ -17994,7 +18086,7 @@
         <v>0</v>
       </c>
       <c r="G157" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H157" s="18">
         <v>0</v>
@@ -18028,13 +18120,13 @@
         <v>2</v>
       </c>
       <c r="B158" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E158" s="14">
         <v>3</v>
@@ -18043,7 +18135,7 @@
         <v>0</v>
       </c>
       <c r="G158" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H158" s="18">
         <v>0</v>
@@ -18077,13 +18169,13 @@
         <v>2</v>
       </c>
       <c r="B159" s="15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E159" s="14">
         <v>3</v>
@@ -18092,7 +18184,7 @@
         <v>0</v>
       </c>
       <c r="G159" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H159" s="18">
         <v>0</v>
@@ -18126,13 +18218,13 @@
         <v>2</v>
       </c>
       <c r="B160" s="15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C160" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E160" s="14">
         <v>3</v>
@@ -18141,7 +18233,7 @@
         <v>0</v>
       </c>
       <c r="G160" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H160" s="18">
         <v>0</v>
@@ -18175,27 +18267,27 @@
         <v>2</v>
       </c>
       <c r="B161" s="15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D161" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E161" s="14">
-        <v>1</v>
-      </c>
-      <c r="F161" s="13">
-        <v>0</v>
-      </c>
-      <c r="G161" s="13">
-        <v>1</v>
-      </c>
-      <c r="H161" s="13">
-        <v>0</v>
-      </c>
-      <c r="I161" s="13">
+        <v>3</v>
+      </c>
+      <c r="F161" s="18">
+        <v>0</v>
+      </c>
+      <c r="G161" s="18">
+        <v>1</v>
+      </c>
+      <c r="H161" s="18">
+        <v>0</v>
+      </c>
+      <c r="I161" s="18">
         <v>0</v>
       </c>
       <c r="J161" s="12">
@@ -18216,33 +18308,35 @@
       <c r="O161" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P161" s="17"/>
+      <c r="Q161" s="17"/>
     </row>
     <row r="162" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A162" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B162" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="C162" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="D162" s="127" t="s">
-        <v>30</v>
+      <c r="B162" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C162" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D162" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E162" s="14">
-        <v>1</v>
-      </c>
-      <c r="F162" s="128">
-        <v>0</v>
-      </c>
-      <c r="G162" s="128">
-        <v>0</v>
-      </c>
-      <c r="H162" s="128">
-        <v>0</v>
-      </c>
-      <c r="I162" s="128">
+        <v>3</v>
+      </c>
+      <c r="F162" s="18">
+        <v>0</v>
+      </c>
+      <c r="G162" s="18">
+        <v>2</v>
+      </c>
+      <c r="H162" s="18">
+        <v>0</v>
+      </c>
+      <c r="I162" s="18">
         <v>0</v>
       </c>
       <c r="J162" s="12">
@@ -18263,136 +18357,180 @@
       <c r="O162" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P162" s="8"/>
-      <c r="Q162" s="8"/>
-      <c r="R162" s="8"/>
-      <c r="S162" s="8"/>
-      <c r="T162" s="8"/>
-      <c r="U162" s="8"/>
-      <c r="V162" s="8"/>
-      <c r="W162" s="8"/>
-      <c r="X162" s="8"/>
-      <c r="Y162" s="8"/>
-      <c r="Z162" s="8"/>
-      <c r="AA162" s="8"/>
-      <c r="AB162" s="8"/>
-      <c r="AC162" s="8"/>
-      <c r="AD162" s="8"/>
-      <c r="AE162" s="8"/>
+      <c r="P162" s="17"/>
+      <c r="Q162" s="17"/>
     </row>
     <row r="163" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N163" s="8"/>
-      <c r="O163" s="8"/>
-      <c r="P163" s="8"/>
-      <c r="Q163" s="8"/>
-      <c r="R163" s="8"/>
-      <c r="S163" s="8"/>
-      <c r="T163" s="8"/>
-      <c r="U163" s="8"/>
-      <c r="V163" s="8"/>
-      <c r="W163" s="8"/>
-      <c r="X163" s="8"/>
-      <c r="Y163" s="8"/>
-      <c r="Z163" s="8"/>
-      <c r="AA163" s="8"/>
-      <c r="AB163" s="8"/>
-      <c r="AC163" s="8"/>
-      <c r="AD163" s="8"/>
-      <c r="AE163" s="8"/>
-    </row>
-    <row r="164" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="165" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A165" s="9" t="s">
+      <c r="A163" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B163" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C163" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D163" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E163" s="14">
+        <v>1</v>
+      </c>
+      <c r="F163" s="13">
+        <v>0</v>
+      </c>
+      <c r="G163" s="13">
+        <v>1</v>
+      </c>
+      <c r="H163" s="13">
+        <v>0</v>
+      </c>
+      <c r="I163" s="13">
+        <v>0</v>
+      </c>
+      <c r="J163" s="12">
+        <v>2</v>
+      </c>
+      <c r="K163" s="12">
+        <v>0</v>
+      </c>
+      <c r="L163" s="12">
+        <v>0</v>
+      </c>
+      <c r="M163" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N163" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O163" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="164" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A164" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B164" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="C164" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D164" s="127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E164" s="14">
+        <v>1</v>
+      </c>
+      <c r="F164" s="128">
+        <v>0</v>
+      </c>
+      <c r="G164" s="128">
+        <v>0</v>
+      </c>
+      <c r="H164" s="128">
+        <v>0</v>
+      </c>
+      <c r="I164" s="128">
+        <v>0</v>
+      </c>
+      <c r="J164" s="12">
+        <v>2</v>
+      </c>
+      <c r="K164" s="12">
+        <v>0</v>
+      </c>
+      <c r="L164" s="12">
+        <v>0</v>
+      </c>
+      <c r="M164" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N164" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O164" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P164" s="8"/>
+      <c r="Q164" s="8"/>
+      <c r="R164" s="8"/>
+      <c r="S164" s="8"/>
+      <c r="T164" s="8"/>
+      <c r="U164" s="8"/>
+      <c r="V164" s="8"/>
+      <c r="W164" s="8"/>
+      <c r="X164" s="8"/>
+      <c r="Y164" s="8"/>
+      <c r="Z164" s="8"/>
+      <c r="AA164" s="8"/>
+      <c r="AB164" s="8"/>
+      <c r="AC164" s="8"/>
+      <c r="AD164" s="8"/>
+      <c r="AE164" s="8"/>
+    </row>
+    <row r="165" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N165" s="8"/>
+      <c r="O165" s="8"/>
+      <c r="P165" s="8"/>
+      <c r="Q165" s="8"/>
+      <c r="R165" s="8"/>
+      <c r="S165" s="8"/>
+      <c r="T165" s="8"/>
+      <c r="U165" s="8"/>
+      <c r="V165" s="8"/>
+      <c r="W165" s="8"/>
+      <c r="X165" s="8"/>
+      <c r="Y165" s="8"/>
+      <c r="Z165" s="8"/>
+      <c r="AA165" s="8"/>
+      <c r="AB165" s="8"/>
+      <c r="AC165" s="8"/>
+      <c r="AD165" s="8"/>
+      <c r="AE165" s="8"/>
+    </row>
+    <row r="166" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="167" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A167" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B165" s="9"/>
-      <c r="C165" s="9"/>
-      <c r="D165" s="9"/>
-      <c r="E165" s="8"/>
-      <c r="F165" s="8"/>
-      <c r="G165" s="8"/>
-      <c r="H165" s="8"/>
-      <c r="I165" s="8"/>
-      <c r="J165" s="8"/>
-      <c r="K165" s="8"/>
-      <c r="L165" s="8"/>
-    </row>
-    <row r="167" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="7" t="s">
+      <c r="B167" s="9"/>
+      <c r="C167" s="9"/>
+      <c r="D167" s="9"/>
+      <c r="E167" s="8"/>
+      <c r="F167" s="8"/>
+      <c r="G167" s="8"/>
+      <c r="H167" s="8"/>
+      <c r="I167" s="8"/>
+      <c r="J167" s="8"/>
+      <c r="K167" s="8"/>
+      <c r="L167" s="8"/>
+    </row>
+    <row r="169" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A169" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B167" s="6" t="s">
+      <c r="B169" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C167" s="6" t="s">
+      <c r="C169" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D167" s="5" t="s">
+      <c r="D169" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E167" s="5" t="s">
+      <c r="E169" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F167" s="5" t="s">
+      <c r="F169" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G167" s="5" t="s">
+      <c r="G169" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H167" s="5" t="s">
+      <c r="H169" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="168" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D168" s="2">
-        <v>42</v>
-      </c>
-      <c r="E168" s="2">
-        <v>8</v>
-      </c>
-      <c r="F168" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G168" s="2">
-        <v>2</v>
-      </c>
-      <c r="H168" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A169" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D169" s="2">
-        <v>92</v>
-      </c>
-      <c r="E169" s="2">
-        <v>10</v>
-      </c>
-      <c r="F169" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G169" s="2">
-        <v>2</v>
-      </c>
-      <c r="H169" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:31" x14ac:dyDescent="0.25">
@@ -18400,19 +18538,19 @@
         <v>2</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D170" s="2">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="E170" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F170" s="2">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="G170" s="2">
         <v>2</v>
@@ -18426,19 +18564,19 @@
         <v>2</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D171" s="2">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="E171" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F171" s="2">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G171" s="2">
         <v>2</v>
@@ -18452,104 +18590,156 @@
         <v>2</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D172" s="2">
+        <v>235</v>
+      </c>
+      <c r="E172" s="2">
+        <v>12</v>
+      </c>
+      <c r="F172" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G172" s="2">
+        <v>2</v>
+      </c>
+      <c r="H172" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A173" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D173" s="2">
+        <v>686</v>
+      </c>
+      <c r="E173" s="2">
+        <v>14</v>
+      </c>
+      <c r="F173" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G173" s="2">
+        <v>2</v>
+      </c>
+      <c r="H173" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A174" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D174" s="2">
         <v>1040</v>
       </c>
-      <c r="E172" s="2">
+      <c r="E174" s="2">
         <v>14</v>
       </c>
-      <c r="F172" s="2">
+      <c r="F174" s="2">
         <v>0.5</v>
       </c>
-      <c r="G172" s="2">
-        <v>2</v>
-      </c>
-      <c r="H172" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D175" s="1">
-        <v>42</v>
-      </c>
-      <c r="F175" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G175">
-        <f>D168*F168</f>
-        <v>54.6</v>
-      </c>
-      <c r="I175">
-        <f>D175*F175</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="176" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D176" s="1">
-        <v>92</v>
-      </c>
-      <c r="F176" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G176">
-        <f>D169*F169</f>
-        <v>101.2</v>
-      </c>
-      <c r="I176">
-        <f>D176*F176</f>
-        <v>101.2</v>
+      <c r="G174" s="2">
+        <v>2</v>
+      </c>
+      <c r="H174" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D177" s="1">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="F177" s="1">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="G177">
         <f>D170*F170</f>
-        <v>211.5</v>
+        <v>54.6</v>
       </c>
       <c r="I177">
         <f>D177*F177</f>
-        <v>211.5</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="178" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D178" s="1">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="F178" s="1">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G178">
         <f>D171*F171</f>
-        <v>480.2</v>
+        <v>101.2</v>
       </c>
       <c r="I178">
         <f>D178*F178</f>
-        <v>480.2</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="179" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D179" s="1">
-        <v>1040</v>
+        <v>235</v>
       </c>
       <c r="F179" s="1">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G179">
         <f>D172*F172</f>
-        <v>520</v>
+        <v>211.5</v>
       </c>
       <c r="I179">
         <f>D179*F179</f>
+        <v>211.5</v>
+      </c>
+    </row>
+    <row r="180" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D180" s="1">
+        <v>686</v>
+      </c>
+      <c r="F180" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G180">
+        <f>D173*F173</f>
+        <v>480.2</v>
+      </c>
+      <c r="I180">
+        <f>D180*F180</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="181" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D181" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F181" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G181">
+        <f>D174*F174</f>
+        <v>520</v>
+      </c>
+      <c r="I181">
+        <f>D181*F181</f>
         <v>520</v>
       </c>
     </row>
@@ -18557,15 +18747,15 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F149:G149"/>
+    <mergeCell ref="F151:G151"/>
   </mergeCells>
-  <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M146 R143:T146">
-    <cfRule type="expression" dxfId="118" priority="78">
+  <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M148 R143:T148">
+    <cfRule type="expression" dxfId="26" priority="78">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="117" priority="71">
+    <cfRule type="expression" dxfId="24" priority="71">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18582,7 +18772,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:M120 R116:T120">
-    <cfRule type="expression" dxfId="116" priority="65">
+    <cfRule type="expression" dxfId="23" priority="65">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18611,7 +18801,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115 R115:T115">
-    <cfRule type="expression" dxfId="115" priority="63">
+    <cfRule type="expression" dxfId="22" priority="63">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18628,12 +18818,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126:M127 R126:T127">
-    <cfRule type="expression" dxfId="114" priority="60">
+    <cfRule type="expression" dxfId="21" priority="60">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126 R126:T126">
-    <cfRule type="expression" dxfId="113" priority="59">
+    <cfRule type="expression" dxfId="20" priority="59">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18662,12 +18852,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="112" priority="57">
+    <cfRule type="expression" dxfId="19" priority="57">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S129:T129 M129">
-    <cfRule type="expression" dxfId="111" priority="56">
+    <cfRule type="expression" dxfId="18" priority="56">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18684,17 +18874,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R129">
-    <cfRule type="expression" dxfId="110" priority="54">
+    <cfRule type="expression" dxfId="17" priority="54">
       <formula>R129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="109" priority="39">
+    <cfRule type="expression" dxfId="16" priority="39">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="108" priority="41">
+    <cfRule type="expression" dxfId="15" priority="41">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18711,12 +18901,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="107" priority="34">
+    <cfRule type="expression" dxfId="14" priority="34">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M133 R130:T133">
-    <cfRule type="expression" dxfId="106" priority="35">
+    <cfRule type="expression" dxfId="13" priority="35">
       <formula>M130=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18745,12 +18935,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="105" priority="32">
+    <cfRule type="expression" dxfId="12" priority="32">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="104" priority="27">
+    <cfRule type="expression" dxfId="11" priority="27">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18767,12 +18957,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="103" priority="29">
+    <cfRule type="expression" dxfId="10" priority="29">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R137">
-    <cfRule type="expression" dxfId="102" priority="22">
+    <cfRule type="expression" dxfId="9" priority="22">
       <formula>R137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18789,12 +18979,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S137:T137 M137">
-    <cfRule type="expression" dxfId="101" priority="24">
+    <cfRule type="expression" dxfId="8" priority="24">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="100" priority="20">
+    <cfRule type="expression" dxfId="7" priority="20">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18811,7 +19001,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="99" priority="18">
+    <cfRule type="expression" dxfId="6" priority="18">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18828,7 +19018,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="98" priority="16">
+    <cfRule type="expression" dxfId="5" priority="16">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18845,7 +19035,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="97" priority="14">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18862,7 +19052,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="96" priority="10">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18879,7 +19069,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R142">
-    <cfRule type="expression" dxfId="95" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>R142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18896,12 +19086,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S142:T142 M142">
-    <cfRule type="expression" dxfId="94" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>M142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105:T105 M105">
-    <cfRule type="expression" dxfId="93" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>M105=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18917,8 +19107,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N143:Q146">
-    <cfRule type="colorScale" priority="89">
+  <conditionalFormatting sqref="N143:Q148">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18931,36 +19121,36 @@
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G135"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 G136:G146 H40:I146 J141:J146">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 G136:G148 H40:I148 J141:J148">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D151:G162 P140:V140 M140:N140 Q141:W146 N141:O146 N24:O139 Q24:W139">
+    <dataValidation type="decimal" allowBlank="1" sqref="D153:G164 P140:V140 M140:N140 N24:O139 Q24:W139 Q141:W148 N141:O148">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H151:L160 H161:I161 J162:L162 X141:AA146 W140:Z140 X24:AA139">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H153:L162 H163:I163 J164:L164 W140:Z140 X24:AA139 X141:AA148">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C151:C162 C24:C146">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C153:C164 C24:C148">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J161:L161 M151:O162 AA140:AC140 AB131:AB142 AC131:AC139 AB143:AF146 AC141:AC142 AB24:AC130 AD24:AF142"/>
-    <dataValidation type="list" sqref="P141:P146 O140 P24:P139">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J163:L163 M153:O164 AA140:AC140 AB131:AB142 AC131:AC139 AC141:AC142 AB24:AC130 AD24:AF142 AB143:AF148"/>
+    <dataValidation type="list" sqref="O140 P24:P139 P141:P148">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L146">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L148">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="M141:M146 L140 M24:M139">
+    <dataValidation type="list" sqref="L140 M24:M139 M141:M148">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J140">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F146">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F148">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added to content red envelop and heart
Former-commit-id: 1e8e6657d31a4c205a54b48d2e25f0ee87ee14c1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$152:$O$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$154:$O$155</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="525">
   <si>
     <t>tier_4</t>
   </si>
@@ -1598,6 +1598,24 @@
   </si>
   <si>
     <t>TID_EDIBLE_SEASON_XMAS</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_KILL_ENT_ARMOUR_PIECES_01;TID_QUIP_DRG_KILL_ENT_ARMOUR_PIECES_03</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_BURN_ENT_05;TID_QUIP_DRG_BURN_ENT_04</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_KILL_ENT_ARMOUR_PIECES_01;TID_QUIP_DRG_KILL_ENT_ARMOUR_PIECES_04</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_BURN_ENT_05;TID_QUIP_DRG_BURN_ENT_05</t>
+  </si>
+  <si>
+    <t>red_envelop</t>
+  </si>
+  <si>
+    <t>valentines_heart</t>
   </si>
 </sst>
 </file>
@@ -2619,9 +2637,6 @@
     <xf numFmtId="2" fontId="16" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2664,19 +2679,15 @@
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="120">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="119">
     <dxf>
       <fill>
         <patternFill>
@@ -5168,114 +5179,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF147" totalsRowShown="0" headerRowDxfId="119" dataDxfId="117" headerRowBorderDxfId="118" tableBorderDxfId="116" totalsRowBorderDxfId="115">
-  <autoFilter ref="A23:AF147"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="118" dataDxfId="116" headerRowBorderDxfId="117" tableBorderDxfId="115" totalsRowBorderDxfId="114">
+  <autoFilter ref="A23:AF149"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="114"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="113"/>
-    <tableColumn id="6" name="[category]" dataDxfId="112"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="111"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="110"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="109"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="108"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="107"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="106"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="105"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="104"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="103"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="102"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="101"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="100"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="99"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="98"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="97"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="96"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="95"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="94"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="93"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="92"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="91"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="90"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="89"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="88"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="87"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="86"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="85"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="84"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="83"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="113"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="112"/>
+    <tableColumn id="6" name="[category]" dataDxfId="111"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="110"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="109"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="108"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="107"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="106"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="105"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="104"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="103"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="102"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="101"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="100"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="99"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="98"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="97"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="96"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="95"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="94"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="93"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="92"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="91"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="90"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="89"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="88"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="87"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="86"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="85"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="84"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="83"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="78"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="77"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="77"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A152:O164" totalsRowShown="0">
-  <autoFilter ref="A152:O164"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A154:O166" totalsRowShown="0">
+  <autoFilter ref="A154:O166"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="4" name="[category]" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="16" name="[size]" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="4" name="[category]" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="16" name="[size]" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="47" totalsRowDxfId="46"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="6" name="[order]" dataDxfId="40"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="39"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="38"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="37"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="36"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="6" name="[order]" dataDxfId="39"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="38"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="37"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="36"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="30"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="28"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="29"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="27"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="26" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5547,12 +5558,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF181"/>
+  <dimension ref="A1:AF183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="G142" sqref="G142"/>
+      <selection pane="topRight" activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5598,8 +5609,8 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
@@ -5763,8 +5774,8 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="174"/>
-      <c r="F22" s="174"/>
+      <c r="E22" s="188"/>
+      <c r="F22" s="188"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -17720,263 +17731,349 @@
       <c r="AF147" s="146"/>
     </row>
     <row r="148" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A148" s="175"/>
-      <c r="B148" s="176"/>
-      <c r="C148" s="176"/>
-      <c r="D148" s="177"/>
-      <c r="E148" s="177"/>
-      <c r="F148" s="177"/>
-      <c r="G148" s="177"/>
-      <c r="H148" s="177"/>
-      <c r="I148" s="177"/>
-      <c r="J148" s="178"/>
-      <c r="K148" s="179"/>
-      <c r="L148" s="177"/>
-      <c r="M148" s="180"/>
-      <c r="N148" s="181"/>
-      <c r="O148" s="181"/>
-      <c r="P148" s="182"/>
-      <c r="Q148" s="181"/>
-      <c r="R148" s="180"/>
-      <c r="S148" s="180"/>
-      <c r="T148" s="183"/>
-      <c r="U148" s="182"/>
-      <c r="V148" s="182"/>
-      <c r="W148" s="182"/>
-      <c r="X148" s="184"/>
-      <c r="Y148" s="184"/>
-      <c r="Z148" s="184"/>
-      <c r="AA148" s="184"/>
-      <c r="AB148" s="185"/>
-      <c r="AC148" s="186"/>
-      <c r="AD148" s="186"/>
-      <c r="AE148" s="187"/>
-      <c r="AF148" s="188"/>
-    </row>
-    <row r="149" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="150" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A150" s="9" t="s">
+      <c r="A148" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="B148" s="49" t="s">
+        <v>523</v>
+      </c>
+      <c r="C148" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D148" s="61">
+        <v>20</v>
+      </c>
+      <c r="E148" s="76">
+        <v>6</v>
+      </c>
+      <c r="F148" s="76">
+        <v>0</v>
+      </c>
+      <c r="G148" s="76">
+        <v>7</v>
+      </c>
+      <c r="H148" s="76">
+        <v>0</v>
+      </c>
+      <c r="I148" s="76">
+        <v>25</v>
+      </c>
+      <c r="J148" s="172">
+        <v>0</v>
+      </c>
+      <c r="K148" s="173">
+        <v>0</v>
+      </c>
+      <c r="L148" s="76">
+        <v>0</v>
+      </c>
+      <c r="M148" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N148" s="47">
+        <v>5</v>
+      </c>
+      <c r="O148" s="47">
+        <v>5</v>
+      </c>
+      <c r="P148" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q148" s="47">
+        <v>0</v>
+      </c>
+      <c r="R148" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S148" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T148" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U148" s="46">
+        <v>1</v>
+      </c>
+      <c r="V148" s="46"/>
+      <c r="W148" s="46">
+        <v>0</v>
+      </c>
+      <c r="X148" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y148" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z148" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA148" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB148" s="45" t="s">
+        <v>515</v>
+      </c>
+      <c r="AC148" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="AD148" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="AE148" s="26"/>
+      <c r="AF148" s="146"/>
+    </row>
+    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A149" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="B149" s="49" t="s">
+        <v>524</v>
+      </c>
+      <c r="C149" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D149" s="61">
+        <v>20</v>
+      </c>
+      <c r="E149" s="76">
+        <v>0</v>
+      </c>
+      <c r="F149" s="76">
+        <v>0</v>
+      </c>
+      <c r="G149" s="76">
+        <v>7</v>
+      </c>
+      <c r="H149" s="76">
+        <v>0</v>
+      </c>
+      <c r="I149" s="76">
+        <v>25</v>
+      </c>
+      <c r="J149" s="172">
+        <v>0</v>
+      </c>
+      <c r="K149" s="173">
+        <v>0</v>
+      </c>
+      <c r="L149" s="76">
+        <v>0</v>
+      </c>
+      <c r="M149" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N149" s="47">
+        <v>5</v>
+      </c>
+      <c r="O149" s="47">
+        <v>5</v>
+      </c>
+      <c r="P149" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q149" s="47">
+        <v>0</v>
+      </c>
+      <c r="R149" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S149" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T149" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U149" s="46">
+        <v>1</v>
+      </c>
+      <c r="V149" s="46"/>
+      <c r="W149" s="46">
+        <v>0</v>
+      </c>
+      <c r="X149" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y149" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z149" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA149" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB149" s="45" t="s">
+        <v>515</v>
+      </c>
+      <c r="AC149" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="AD149" s="44" t="s">
+        <v>522</v>
+      </c>
+      <c r="AE149" s="26"/>
+      <c r="AF149" s="146"/>
+    </row>
+    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A150" s="174"/>
+      <c r="B150" s="175"/>
+      <c r="C150" s="175"/>
+      <c r="D150" s="176"/>
+      <c r="E150" s="176"/>
+      <c r="F150" s="176"/>
+      <c r="G150" s="176"/>
+      <c r="H150" s="176"/>
+      <c r="I150" s="176"/>
+      <c r="J150" s="177"/>
+      <c r="K150" s="178"/>
+      <c r="L150" s="176"/>
+      <c r="M150" s="179"/>
+      <c r="N150" s="180"/>
+      <c r="O150" s="180"/>
+      <c r="P150" s="181"/>
+      <c r="Q150" s="180"/>
+      <c r="R150" s="179"/>
+      <c r="S150" s="179"/>
+      <c r="T150" s="182"/>
+      <c r="U150" s="181"/>
+      <c r="V150" s="181"/>
+      <c r="W150" s="181"/>
+      <c r="X150" s="183"/>
+      <c r="Y150" s="183"/>
+      <c r="Z150" s="183"/>
+      <c r="AA150" s="183"/>
+      <c r="AB150" s="184"/>
+      <c r="AC150" s="185"/>
+      <c r="AD150" s="185"/>
+      <c r="AE150" s="186"/>
+      <c r="AF150" s="187"/>
+    </row>
+    <row r="151" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A152" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B150" s="9"/>
-      <c r="C150" s="9"/>
-      <c r="D150" s="9"/>
-      <c r="E150" s="9"/>
-      <c r="F150" s="9"/>
-      <c r="G150" s="9"/>
-      <c r="H150" s="9"/>
-      <c r="I150" s="9"/>
-      <c r="J150" s="9"/>
-      <c r="K150" s="9"/>
-      <c r="L150" s="9"/>
-      <c r="M150" s="9"/>
-      <c r="N150" s="9"/>
-      <c r="O150" s="9"/>
-      <c r="P150" s="9"/>
-      <c r="Q150" s="9"/>
-      <c r="R150" s="9"/>
-      <c r="S150" s="9"/>
-      <c r="T150" s="9"/>
-      <c r="U150" s="9"/>
-      <c r="V150" s="9"/>
-      <c r="W150" s="9"/>
-      <c r="X150" s="9"/>
-      <c r="Y150" s="9"/>
-      <c r="Z150" s="9"/>
-      <c r="AA150" s="9"/>
-      <c r="AF150" s="8"/>
-    </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A151" s="22"/>
-      <c r="B151" s="22"/>
-      <c r="C151" s="22"/>
-      <c r="D151" s="22"/>
-      <c r="E151" s="22"/>
-      <c r="F151" s="174"/>
-      <c r="G151" s="174"/>
-      <c r="H151" s="21" t="s">
+      <c r="B152" s="9"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="9"/>
+      <c r="H152" s="9"/>
+      <c r="I152" s="9"/>
+      <c r="J152" s="9"/>
+      <c r="K152" s="9"/>
+      <c r="L152" s="9"/>
+      <c r="M152" s="9"/>
+      <c r="N152" s="9"/>
+      <c r="O152" s="9"/>
+      <c r="P152" s="9"/>
+      <c r="Q152" s="9"/>
+      <c r="R152" s="9"/>
+      <c r="S152" s="9"/>
+      <c r="T152" s="9"/>
+      <c r="U152" s="9"/>
+      <c r="V152" s="9"/>
+      <c r="W152" s="9"/>
+      <c r="X152" s="9"/>
+      <c r="Y152" s="9"/>
+      <c r="Z152" s="9"/>
+      <c r="AA152" s="9"/>
+      <c r="AF152" s="8"/>
+    </row>
+    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A153" s="22"/>
+      <c r="B153" s="22"/>
+      <c r="C153" s="22"/>
+      <c r="D153" s="22"/>
+      <c r="E153" s="22"/>
+      <c r="F153" s="188"/>
+      <c r="G153" s="188"/>
+      <c r="H153" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I151" s="21"/>
-      <c r="J151" s="22"/>
-      <c r="K151" s="17"/>
-      <c r="L151" s="17"/>
-      <c r="M151" s="17" t="s">
+      <c r="I153" s="21"/>
+      <c r="J153" s="22"/>
+      <c r="K153" s="17"/>
+      <c r="L153" s="17"/>
+      <c r="M153" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N151" s="17"/>
-      <c r="O151" s="17"/>
-      <c r="P151" s="17"/>
-      <c r="Q151" s="17"/>
-      <c r="R151" s="17"/>
-      <c r="S151" s="17"/>
-      <c r="T151" s="17"/>
-      <c r="U151" s="17"/>
-      <c r="V151" s="17"/>
-      <c r="W151" s="17"/>
-      <c r="X151" s="17"/>
-      <c r="Y151" s="17"/>
-      <c r="Z151" s="17"/>
-      <c r="AA151" s="21"/>
-      <c r="AB151" s="21"/>
-      <c r="AC151" s="21"/>
-      <c r="AD151" s="21"/>
-      <c r="AE151" s="17"/>
-    </row>
-    <row r="152" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A152" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B152" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D152" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E152" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F152" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G152" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H152" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I152" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="J152" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="K152" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="L152" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="M152" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="N152" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O152" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A153" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B153" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C153" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D153" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E153" s="14">
-        <v>3</v>
-      </c>
-      <c r="F153" s="18">
-        <v>0</v>
-      </c>
-      <c r="G153" s="18">
-        <v>0</v>
-      </c>
-      <c r="H153" s="18">
-        <v>0</v>
-      </c>
-      <c r="I153" s="18">
-        <v>0</v>
-      </c>
-      <c r="J153" s="12">
-        <v>2</v>
-      </c>
-      <c r="K153" s="12">
-        <v>0</v>
-      </c>
-      <c r="L153" s="12">
-        <v>0</v>
-      </c>
-      <c r="M153" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N153" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O153" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N153" s="17"/>
+      <c r="O153" s="17"/>
       <c r="P153" s="17"/>
       <c r="Q153" s="17"/>
-    </row>
-    <row r="154" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A154" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B154" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C154" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D154" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E154" s="14">
-        <v>3</v>
-      </c>
-      <c r="F154" s="18">
-        <v>0</v>
-      </c>
-      <c r="G154" s="18">
-        <v>1</v>
-      </c>
-      <c r="H154" s="18">
-        <v>0</v>
-      </c>
-      <c r="I154" s="18">
-        <v>0</v>
-      </c>
-      <c r="J154" s="12">
-        <v>2</v>
-      </c>
-      <c r="K154" s="12">
-        <v>0</v>
-      </c>
-      <c r="L154" s="12">
-        <v>0</v>
-      </c>
-      <c r="M154" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N154" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O154" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P154" s="17"/>
-      <c r="Q154" s="17"/>
+      <c r="R153" s="17"/>
+      <c r="S153" s="17"/>
+      <c r="T153" s="17"/>
+      <c r="U153" s="17"/>
+      <c r="V153" s="17"/>
+      <c r="W153" s="17"/>
+      <c r="X153" s="17"/>
+      <c r="Y153" s="17"/>
+      <c r="Z153" s="17"/>
+      <c r="AA153" s="21"/>
+      <c r="AB153" s="21"/>
+      <c r="AC153" s="21"/>
+      <c r="AD153" s="21"/>
+      <c r="AE153" s="17"/>
+    </row>
+    <row r="154" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A154" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D154" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E154" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F154" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G154" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H154" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I154" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J154" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="K154" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L154" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M154" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N154" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="O154" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="155" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B155" s="15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D155" s="14" t="s">
         <v>30</v>
@@ -18022,10 +18119,10 @@
         <v>2</v>
       </c>
       <c r="B156" s="15" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D156" s="14" t="s">
         <v>23</v>
@@ -18071,10 +18168,10 @@
         <v>2</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D157" s="14" t="s">
         <v>30</v>
@@ -18120,10 +18217,10 @@
         <v>2</v>
       </c>
       <c r="B158" s="15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D158" s="14" t="s">
         <v>23</v>
@@ -18169,13 +18266,13 @@
         <v>2</v>
       </c>
       <c r="B159" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C159" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E159" s="14">
         <v>3</v>
@@ -18184,7 +18281,7 @@
         <v>0</v>
       </c>
       <c r="G159" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H159" s="18">
         <v>0</v>
@@ -18218,13 +18315,13 @@
         <v>2</v>
       </c>
       <c r="B160" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E160" s="14">
         <v>3</v>
@@ -18233,7 +18330,7 @@
         <v>0</v>
       </c>
       <c r="G160" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H160" s="18">
         <v>0</v>
@@ -18267,13 +18364,13 @@
         <v>2</v>
       </c>
       <c r="B161" s="15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E161" s="14">
         <v>3</v>
@@ -18282,7 +18379,7 @@
         <v>0</v>
       </c>
       <c r="G161" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H161" s="18">
         <v>0</v>
@@ -18316,13 +18413,13 @@
         <v>2</v>
       </c>
       <c r="B162" s="15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C162" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E162" s="14">
         <v>3</v>
@@ -18331,7 +18428,7 @@
         <v>0</v>
       </c>
       <c r="G162" s="18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H162" s="18">
         <v>0</v>
@@ -18365,27 +18462,27 @@
         <v>2</v>
       </c>
       <c r="B163" s="15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D163" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E163" s="14">
-        <v>1</v>
-      </c>
-      <c r="F163" s="13">
-        <v>0</v>
-      </c>
-      <c r="G163" s="13">
-        <v>1</v>
-      </c>
-      <c r="H163" s="13">
-        <v>0</v>
-      </c>
-      <c r="I163" s="13">
+        <v>3</v>
+      </c>
+      <c r="F163" s="18">
+        <v>0</v>
+      </c>
+      <c r="G163" s="18">
+        <v>1</v>
+      </c>
+      <c r="H163" s="18">
+        <v>0</v>
+      </c>
+      <c r="I163" s="18">
         <v>0</v>
       </c>
       <c r="J163" s="12">
@@ -18406,33 +18503,35 @@
       <c r="O163" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P163" s="17"/>
+      <c r="Q163" s="17"/>
     </row>
     <row r="164" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A164" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B164" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="C164" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="D164" s="127" t="s">
-        <v>30</v>
+      <c r="B164" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C164" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D164" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E164" s="14">
-        <v>1</v>
-      </c>
-      <c r="F164" s="128">
-        <v>0</v>
-      </c>
-      <c r="G164" s="128">
-        <v>0</v>
-      </c>
-      <c r="H164" s="128">
-        <v>0</v>
-      </c>
-      <c r="I164" s="128">
+        <v>3</v>
+      </c>
+      <c r="F164" s="18">
+        <v>0</v>
+      </c>
+      <c r="G164" s="18">
+        <v>2</v>
+      </c>
+      <c r="H164" s="18">
+        <v>0</v>
+      </c>
+      <c r="I164" s="18">
         <v>0</v>
       </c>
       <c r="J164" s="12">
@@ -18453,136 +18552,180 @@
       <c r="O164" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P164" s="8"/>
-      <c r="Q164" s="8"/>
-      <c r="R164" s="8"/>
-      <c r="S164" s="8"/>
-      <c r="T164" s="8"/>
-      <c r="U164" s="8"/>
-      <c r="V164" s="8"/>
-      <c r="W164" s="8"/>
-      <c r="X164" s="8"/>
-      <c r="Y164" s="8"/>
-      <c r="Z164" s="8"/>
-      <c r="AA164" s="8"/>
-      <c r="AB164" s="8"/>
-      <c r="AC164" s="8"/>
-      <c r="AD164" s="8"/>
-      <c r="AE164" s="8"/>
+      <c r="P164" s="17"/>
+      <c r="Q164" s="17"/>
     </row>
     <row r="165" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N165" s="8"/>
-      <c r="O165" s="8"/>
-      <c r="P165" s="8"/>
-      <c r="Q165" s="8"/>
-      <c r="R165" s="8"/>
-      <c r="S165" s="8"/>
-      <c r="T165" s="8"/>
-      <c r="U165" s="8"/>
-      <c r="V165" s="8"/>
-      <c r="W165" s="8"/>
-      <c r="X165" s="8"/>
-      <c r="Y165" s="8"/>
-      <c r="Z165" s="8"/>
-      <c r="AA165" s="8"/>
-      <c r="AB165" s="8"/>
-      <c r="AC165" s="8"/>
-      <c r="AD165" s="8"/>
-      <c r="AE165" s="8"/>
-    </row>
-    <row r="166" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="167" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A167" s="9" t="s">
+      <c r="A165" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B165" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C165" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D165" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E165" s="14">
+        <v>1</v>
+      </c>
+      <c r="F165" s="13">
+        <v>0</v>
+      </c>
+      <c r="G165" s="13">
+        <v>1</v>
+      </c>
+      <c r="H165" s="13">
+        <v>0</v>
+      </c>
+      <c r="I165" s="13">
+        <v>0</v>
+      </c>
+      <c r="J165" s="12">
+        <v>2</v>
+      </c>
+      <c r="K165" s="12">
+        <v>0</v>
+      </c>
+      <c r="L165" s="12">
+        <v>0</v>
+      </c>
+      <c r="M165" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N165" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O165" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A166" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B166" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="C166" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D166" s="127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E166" s="14">
+        <v>1</v>
+      </c>
+      <c r="F166" s="128">
+        <v>0</v>
+      </c>
+      <c r="G166" s="128">
+        <v>0</v>
+      </c>
+      <c r="H166" s="128">
+        <v>0</v>
+      </c>
+      <c r="I166" s="128">
+        <v>0</v>
+      </c>
+      <c r="J166" s="12">
+        <v>2</v>
+      </c>
+      <c r="K166" s="12">
+        <v>0</v>
+      </c>
+      <c r="L166" s="12">
+        <v>0</v>
+      </c>
+      <c r="M166" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N166" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O166" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P166" s="8"/>
+      <c r="Q166" s="8"/>
+      <c r="R166" s="8"/>
+      <c r="S166" s="8"/>
+      <c r="T166" s="8"/>
+      <c r="U166" s="8"/>
+      <c r="V166" s="8"/>
+      <c r="W166" s="8"/>
+      <c r="X166" s="8"/>
+      <c r="Y166" s="8"/>
+      <c r="Z166" s="8"/>
+      <c r="AA166" s="8"/>
+      <c r="AB166" s="8"/>
+      <c r="AC166" s="8"/>
+      <c r="AD166" s="8"/>
+      <c r="AE166" s="8"/>
+    </row>
+    <row r="167" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N167" s="8"/>
+      <c r="O167" s="8"/>
+      <c r="P167" s="8"/>
+      <c r="Q167" s="8"/>
+      <c r="R167" s="8"/>
+      <c r="S167" s="8"/>
+      <c r="T167" s="8"/>
+      <c r="U167" s="8"/>
+      <c r="V167" s="8"/>
+      <c r="W167" s="8"/>
+      <c r="X167" s="8"/>
+      <c r="Y167" s="8"/>
+      <c r="Z167" s="8"/>
+      <c r="AA167" s="8"/>
+      <c r="AB167" s="8"/>
+      <c r="AC167" s="8"/>
+      <c r="AD167" s="8"/>
+      <c r="AE167" s="8"/>
+    </row>
+    <row r="168" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="169" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A169" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B167" s="9"/>
-      <c r="C167" s="9"/>
-      <c r="D167" s="9"/>
-      <c r="E167" s="8"/>
-      <c r="F167" s="8"/>
-      <c r="G167" s="8"/>
-      <c r="H167" s="8"/>
-      <c r="I167" s="8"/>
-      <c r="J167" s="8"/>
-      <c r="K167" s="8"/>
-      <c r="L167" s="8"/>
-    </row>
-    <row r="169" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A169" s="7" t="s">
+      <c r="B169" s="9"/>
+      <c r="C169" s="9"/>
+      <c r="D169" s="9"/>
+      <c r="E169" s="8"/>
+      <c r="F169" s="8"/>
+      <c r="G169" s="8"/>
+      <c r="H169" s="8"/>
+      <c r="I169" s="8"/>
+      <c r="J169" s="8"/>
+      <c r="K169" s="8"/>
+      <c r="L169" s="8"/>
+    </row>
+    <row r="171" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A171" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B169" s="6" t="s">
+      <c r="B171" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C169" s="6" t="s">
+      <c r="C171" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D169" s="5" t="s">
+      <c r="D171" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E169" s="5" t="s">
+      <c r="E171" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F169" s="5" t="s">
+      <c r="F171" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G169" s="5" t="s">
+      <c r="G171" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H169" s="5" t="s">
+      <c r="H171" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="170" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A170" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D170" s="2">
-        <v>42</v>
-      </c>
-      <c r="E170" s="2">
-        <v>8</v>
-      </c>
-      <c r="F170" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G170" s="2">
-        <v>2</v>
-      </c>
-      <c r="H170" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A171" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D171" s="2">
-        <v>92</v>
-      </c>
-      <c r="E171" s="2">
-        <v>10</v>
-      </c>
-      <c r="F171" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G171" s="2">
-        <v>2</v>
-      </c>
-      <c r="H171" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:31" x14ac:dyDescent="0.25">
@@ -18590,19 +18733,19 @@
         <v>2</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D172" s="2">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="E172" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F172" s="2">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="G172" s="2">
         <v>2</v>
@@ -18616,19 +18759,19 @@
         <v>2</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D173" s="2">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="E173" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F173" s="2">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G173" s="2">
         <v>2</v>
@@ -18642,104 +18785,156 @@
         <v>2</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D174" s="2">
+        <v>235</v>
+      </c>
+      <c r="E174" s="2">
+        <v>12</v>
+      </c>
+      <c r="F174" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G174" s="2">
+        <v>2</v>
+      </c>
+      <c r="H174" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A175" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D175" s="2">
+        <v>686</v>
+      </c>
+      <c r="E175" s="2">
+        <v>14</v>
+      </c>
+      <c r="F175" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G175" s="2">
+        <v>2</v>
+      </c>
+      <c r="H175" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A176" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D176" s="2">
         <v>1040</v>
       </c>
-      <c r="E174" s="2">
+      <c r="E176" s="2">
         <v>14</v>
       </c>
-      <c r="F174" s="2">
+      <c r="F176" s="2">
         <v>0.5</v>
       </c>
-      <c r="G174" s="2">
-        <v>2</v>
-      </c>
-      <c r="H174" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D177" s="1">
-        <v>42</v>
-      </c>
-      <c r="F177" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G177">
-        <f>D170*F170</f>
-        <v>54.6</v>
-      </c>
-      <c r="I177">
-        <f>D177*F177</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="178" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D178" s="1">
-        <v>92</v>
-      </c>
-      <c r="F178" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G178">
-        <f>D171*F171</f>
-        <v>101.2</v>
-      </c>
-      <c r="I178">
-        <f>D178*F178</f>
-        <v>101.2</v>
+      <c r="G176" s="2">
+        <v>2</v>
+      </c>
+      <c r="H176" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D179" s="1">
-        <v>235</v>
+        <v>42</v>
       </c>
       <c r="F179" s="1">
-        <v>0.9</v>
+        <v>1.3</v>
       </c>
       <c r="G179">
         <f>D172*F172</f>
-        <v>211.5</v>
+        <v>54.6</v>
       </c>
       <c r="I179">
         <f>D179*F179</f>
-        <v>211.5</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="180" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D180" s="1">
-        <v>686</v>
+        <v>92</v>
       </c>
       <c r="F180" s="1">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G180">
         <f>D173*F173</f>
-        <v>480.2</v>
+        <v>101.2</v>
       </c>
       <c r="I180">
         <f>D180*F180</f>
-        <v>480.2</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="181" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D181" s="1">
-        <v>1040</v>
+        <v>235</v>
       </c>
       <c r="F181" s="1">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G181">
         <f>D174*F174</f>
-        <v>520</v>
+        <v>211.5</v>
       </c>
       <c r="I181">
         <f>D181*F181</f>
+        <v>211.5</v>
+      </c>
+    </row>
+    <row r="182" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D182" s="1">
+        <v>686</v>
+      </c>
+      <c r="F182" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G182">
+        <f>D175*F175</f>
+        <v>480.2</v>
+      </c>
+      <c r="I182">
+        <f>D182*F182</f>
+        <v>480.2</v>
+      </c>
+    </row>
+    <row r="183" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D183" s="1">
+        <v>1040</v>
+      </c>
+      <c r="F183" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G183">
+        <f>D176*F176</f>
+        <v>520</v>
+      </c>
+      <c r="I183">
+        <f>D183*F183</f>
         <v>520</v>
       </c>
     </row>
@@ -18747,10 +18942,10 @@
   <mergeCells count="3">
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F151:G151"/>
+    <mergeCell ref="F153:G153"/>
   </mergeCells>
-  <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M148 R143:T148">
-    <cfRule type="expression" dxfId="26" priority="78">
+  <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M150 R143:T150">
+    <cfRule type="expression" dxfId="25" priority="78">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19107,8 +19302,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N143:Q148">
-    <cfRule type="colorScale" priority="94">
+  <conditionalFormatting sqref="N143:Q150">
+    <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19121,36 +19316,36 @@
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G135"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 G136:G148 H40:I148 J141:J148">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 G136:G150 H40:I150 J141:J150">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D153:G164 P140:V140 M140:N140 N24:O139 Q24:W139 Q141:W148 N141:O148">
+    <dataValidation type="decimal" allowBlank="1" sqref="D155:G166 P140:V140 M140:N140 N24:O139 Q24:W139 Q141:W150 N141:O150">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H153:L162 H163:I163 J164:L164 W140:Z140 X24:AA139 X141:AA148">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H155:L164 H165:I165 J166:L166 W140:Z140 X24:AA139 X141:AA150">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C153:C164 C24:C148">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C155:C166 C24:C150">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J163:L163 M153:O164 AA140:AC140 AB131:AB142 AC131:AC139 AC141:AC142 AB24:AC130 AD24:AF142 AB143:AF148"/>
-    <dataValidation type="list" sqref="O140 P24:P139 P141:P148">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J165:L165 M155:O166 AA140:AC140 AB131:AB142 AC131:AC139 AC141:AC142 AB24:AC130 AD24:AF142 AB143:AF150"/>
+    <dataValidation type="list" sqref="O140 P24:P139 P141:P150">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L148">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L150">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="L140 M24:M139 M141:M148">
+    <dataValidation type="list" sqref="L140 M24:M139 M141:M150">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J140">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F148">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F150">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -19207,8 +19402,8 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="174"/>
-      <c r="G3" s="174"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>

</xml_diff>

<commit_message>
Added a new Tracker to track how many equipped npcs are killed.
Former-commit-id: 5f4a05b693ef362a339c4a478ff9dbc64639a330
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msana/Workspace/Dragon/client_ios/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C071106B-1B35-B74E-AE66-F142B34F38A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="2" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$154:$O$155</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="530">
   <si>
     <t>tier_4</t>
   </si>
@@ -1617,11 +1618,26 @@
   <si>
     <t>valentines_heart</t>
   </si>
+  <si>
+    <t>EQUIPABLE DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{equipableDefinitions}</t>
+  </si>
+  <si>
+    <t>leprechaun_hat</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>TID_LEPRECHAUN_HAT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1709,6 +1725,7 @@
       <sz val="11"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1716,24 +1733,28 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2186,7 +2207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2682,194 +2703,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="119">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5165,6 +5007,188 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5179,114 +5203,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="118" dataDxfId="116" headerRowBorderDxfId="117" tableBorderDxfId="115" totalsRowBorderDxfId="114">
-  <autoFilter ref="A23:AF149"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+  <autoFilter ref="A23:AF149" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="113"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="112"/>
-    <tableColumn id="6" name="[category]" dataDxfId="111"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="110"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="109"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="108"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="107"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="106"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="105"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="104"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="103"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="102"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="101"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="100"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="99"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="98"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="97"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="96"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="95"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="94"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="93"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="92"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="91"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="90"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="89"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="88"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="87"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="86"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="85"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="84"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="83"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
-  <autoFilter ref="A4:B18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="A4:B18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="77"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A154:O166" totalsRowShown="0">
-  <autoFilter ref="A154:O166"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A154:O166" totalsRowShown="0">
+  <autoFilter ref="A154:O166" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="4" name="[category]" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="16" name="[size]" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0200-00001E000000}" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0200-00001F000000}" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0200-000021000000}" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0200-000022000000}" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B4:H29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="B4:H29" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="6" name="[order]" dataDxfId="39"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="38"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="37"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="36"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
-  <autoFilter ref="B35:E45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B35:E45" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="29"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="27"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5554,27 +5578,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF183"/>
+  <dimension ref="A1:AF189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="D148" sqref="D148"/>
+      <selection pane="topRight" activeCell="F197" sqref="F197"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="28" max="28" width="40.7109375" customWidth="1"/>
-    <col min="29" max="29" width="162.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="107.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="40.6640625" customWidth="1"/>
+    <col min="29" max="29" width="162.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="107.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:24" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>386</v>
       </c>
@@ -5602,20 +5626,20 @@
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
     </row>
-    <row r="3" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="98" t="s">
         <v>385</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="188"/>
-      <c r="F3" s="188"/>
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
     </row>
-    <row r="4" spans="1:24" ht="134.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="131" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>384</v>
       </c>
@@ -5623,7 +5647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="94" t="s">
         <v>2</v>
       </c>
@@ -5631,7 +5655,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="94" t="s">
         <v>2</v>
       </c>
@@ -5639,7 +5663,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="94" t="s">
         <v>2</v>
       </c>
@@ -5647,7 +5671,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="94" t="s">
         <v>2</v>
       </c>
@@ -5655,7 +5679,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
         <v>2</v>
       </c>
@@ -5663,7 +5687,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="94" t="s">
         <v>2</v>
       </c>
@@ -5671,7 +5695,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="94" t="s">
         <v>2</v>
       </c>
@@ -5679,7 +5703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="94" t="s">
         <v>2</v>
       </c>
@@ -5687,7 +5711,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="96" t="s">
         <v>2</v>
       </c>
@@ -5695,7 +5719,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="94" t="s">
         <v>2</v>
       </c>
@@ -5703,7 +5727,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
         <v>2</v>
       </c>
@@ -5711,7 +5735,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="94" t="s">
         <v>2</v>
       </c>
@@ -5719,7 +5743,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="94" t="s">
         <v>2</v>
       </c>
@@ -5727,7 +5751,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="94" t="s">
         <v>2</v>
       </c>
@@ -5735,8 +5759,8 @@
         <v>449</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:32" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:32" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>381</v>
       </c>
@@ -5767,15 +5791,15 @@
       <c r="Z21" s="9"/>
       <c r="AA21" s="9"/>
     </row>
-    <row r="22" spans="1:32" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" s="17" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="21" t="s">
         <v>380</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="188"/>
-      <c r="F22" s="188"/>
+      <c r="E22" s="189"/>
+      <c r="F22" s="189"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -5792,7 +5816,7 @@
       <c r="Z22" s="21"/>
       <c r="AA22" s="21"/>
     </row>
-    <row r="23" spans="1:32" ht="126" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" ht="127" x14ac:dyDescent="0.2">
       <c r="A23" s="93" t="s">
         <v>378</v>
       </c>
@@ -5890,7 +5914,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="119" t="s">
         <v>2</v>
       </c>
@@ -5988,7 +6012,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="119" t="s">
         <v>2</v>
       </c>
@@ -6086,7 +6110,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="119" t="s">
         <v>2</v>
       </c>
@@ -6184,7 +6208,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="119" t="s">
         <v>2</v>
       </c>
@@ -6279,7 +6303,7 @@
       <c r="AE27" s="72"/>
       <c r="AF27" s="80"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="49" t="s">
         <v>2</v>
       </c>
@@ -6377,7 +6401,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="49" t="s">
         <v>2</v>
       </c>
@@ -6475,7 +6499,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="30" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="49" t="s">
         <v>2</v>
       </c>
@@ -6573,7 +6597,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="49" t="s">
         <v>2</v>
       </c>
@@ -6668,7 +6692,7 @@
       <c r="AE31" s="75"/>
       <c r="AF31" s="79"/>
     </row>
-    <row r="32" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="123" t="s">
         <v>2</v>
       </c>
@@ -6762,7 +6786,7 @@
       <c r="AE32" s="72"/>
       <c r="AF32" s="71"/>
     </row>
-    <row r="33" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="123" t="s">
         <v>2</v>
       </c>
@@ -6861,7 +6885,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="123" t="s">
         <v>2</v>
       </c>
@@ -6955,7 +6979,7 @@
       <c r="AE34" s="72"/>
       <c r="AF34" s="71"/>
     </row>
-    <row r="35" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="121" t="s">
         <v>2</v>
       </c>
@@ -7050,7 +7074,7 @@
       <c r="AE35" s="72"/>
       <c r="AF35" s="71"/>
     </row>
-    <row r="36" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="49" t="s">
         <v>2</v>
       </c>
@@ -7145,7 +7169,7 @@
       <c r="AE36" s="75"/>
       <c r="AF36" s="74"/>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="49" t="s">
         <v>2</v>
       </c>
@@ -7240,7 +7264,7 @@
       <c r="AE37" s="75"/>
       <c r="AF37" s="79"/>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="49" t="s">
         <v>2</v>
       </c>
@@ -7335,7 +7359,7 @@
       <c r="AE38" s="75"/>
       <c r="AF38" s="79"/>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="135" t="s">
         <v>2</v>
       </c>
@@ -7430,7 +7454,7 @@
       <c r="AE39" s="75"/>
       <c r="AF39" s="79"/>
     </row>
-    <row r="40" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="123" t="s">
         <v>2</v>
       </c>
@@ -7524,7 +7548,7 @@
       <c r="AE40" s="72"/>
       <c r="AF40" s="71"/>
     </row>
-    <row r="41" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="123" t="s">
         <v>2</v>
       </c>
@@ -7618,7 +7642,7 @@
       <c r="AE41" s="72"/>
       <c r="AF41" s="71"/>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" s="123" t="s">
         <v>2</v>
       </c>
@@ -7712,7 +7736,7 @@
       <c r="AE42" s="72"/>
       <c r="AF42" s="71"/>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="121" t="s">
         <v>2</v>
       </c>
@@ -7807,7 +7831,7 @@
       <c r="AE43" s="72"/>
       <c r="AF43" s="71"/>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" s="49" t="s">
         <v>2</v>
       </c>
@@ -7905,7 +7929,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="49" t="s">
         <v>2</v>
       </c>
@@ -7999,7 +8023,7 @@
       <c r="AE45" s="75"/>
       <c r="AF45" s="74"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="49" t="s">
         <v>2</v>
       </c>
@@ -8097,7 +8121,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="135" t="s">
         <v>2</v>
       </c>
@@ -8192,7 +8216,7 @@
       <c r="AE47" s="75"/>
       <c r="AF47" s="74"/>
     </row>
-    <row r="48" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="123" t="s">
         <v>2</v>
       </c>
@@ -8290,7 +8314,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="49" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="123" t="s">
         <v>2</v>
       </c>
@@ -8384,7 +8408,7 @@
       <c r="AE49" s="72"/>
       <c r="AF49" s="71"/>
     </row>
-    <row r="50" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="121" t="s">
         <v>2</v>
       </c>
@@ -8482,7 +8506,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="121" t="s">
         <v>2</v>
       </c>
@@ -8580,7 +8604,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="49" t="s">
         <v>2</v>
       </c>
@@ -8678,7 +8702,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A53" s="49" t="s">
         <v>2</v>
       </c>
@@ -8776,7 +8800,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A54" s="135" t="s">
         <v>2</v>
       </c>
@@ -8874,7 +8898,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="135" t="s">
         <v>2</v>
       </c>
@@ -8969,7 +8993,7 @@
       <c r="AE55" s="75"/>
       <c r="AF55" s="74"/>
     </row>
-    <row r="56" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="123" t="s">
         <v>2</v>
       </c>
@@ -9064,7 +9088,7 @@
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
     </row>
-    <row r="57" spans="1:32" s="150" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" s="150" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="123" t="s">
         <v>2</v>
       </c>
@@ -9152,7 +9176,7 @@
       <c r="AE57" s="72"/>
       <c r="AF57" s="71"/>
     </row>
-    <row r="58" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="121" t="s">
         <v>2</v>
       </c>
@@ -9247,7 +9271,7 @@
       <c r="AE58" s="72"/>
       <c r="AF58" s="80"/>
     </row>
-    <row r="59" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="121" t="s">
         <v>2</v>
       </c>
@@ -9342,7 +9366,7 @@
       <c r="AE59" s="72"/>
       <c r="AF59" s="80"/>
     </row>
-    <row r="60" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="49" t="s">
         <v>2</v>
       </c>
@@ -9437,7 +9461,7 @@
       <c r="AE60" s="75"/>
       <c r="AF60" s="79"/>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A61" s="49" t="s">
         <v>2</v>
       </c>
@@ -9531,7 +9555,7 @@
       <c r="AE61" s="75"/>
       <c r="AF61" s="74"/>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A62" s="135" t="s">
         <v>2</v>
       </c>
@@ -9626,7 +9650,7 @@
       <c r="AE62" s="75"/>
       <c r="AF62" s="74"/>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A63" s="135" t="s">
         <v>2</v>
       </c>
@@ -9721,7 +9745,7 @@
       <c r="AE63" s="75"/>
       <c r="AF63" s="74"/>
     </row>
-    <row r="64" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="123" t="s">
         <v>2</v>
       </c>
@@ -9816,7 +9840,7 @@
       <c r="AE64" s="72"/>
       <c r="AF64" s="80"/>
     </row>
-    <row r="65" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="123" t="s">
         <v>2</v>
       </c>
@@ -9909,7 +9933,7 @@
       <c r="AE65" s="63"/>
       <c r="AF65" s="133"/>
     </row>
-    <row r="66" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="121" t="s">
         <v>2</v>
       </c>
@@ -10008,7 +10032,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A67" s="121" t="s">
         <v>2</v>
       </c>
@@ -10107,7 +10131,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A68" s="49" t="s">
         <v>2</v>
       </c>
@@ -10206,7 +10230,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="135" t="s">
         <v>2</v>
       </c>
@@ -10304,7 +10328,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="135" t="s">
         <v>2</v>
       </c>
@@ -10399,7 +10423,7 @@
       <c r="AE70" s="75"/>
       <c r="AF70" s="79"/>
     </row>
-    <row r="71" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="135" t="s">
         <v>2</v>
       </c>
@@ -10494,7 +10518,7 @@
       <c r="AE71" s="75"/>
       <c r="AF71" s="79"/>
     </row>
-    <row r="72" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="121" t="s">
         <v>2</v>
       </c>
@@ -10592,7 +10616,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="121" t="s">
         <v>2</v>
       </c>
@@ -10685,7 +10709,7 @@
       <c r="AE73" s="63"/>
       <c r="AF73" s="63"/>
     </row>
-    <row r="74" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="121" t="s">
         <v>2</v>
       </c>
@@ -10778,7 +10802,7 @@
       <c r="AE74" s="63"/>
       <c r="AF74" s="133"/>
     </row>
-    <row r="75" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="123" t="s">
         <v>2</v>
       </c>
@@ -10876,7 +10900,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="135" t="s">
         <v>2</v>
       </c>
@@ -10972,7 +10996,7 @@
       </c>
       <c r="AF76" s="68"/>
     </row>
-    <row r="77" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="135" t="s">
         <v>2</v>
       </c>
@@ -11070,7 +11094,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A78" s="49" t="s">
         <v>2</v>
       </c>
@@ -11169,7 +11193,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A79" s="49" t="s">
         <v>2</v>
       </c>
@@ -11263,7 +11287,7 @@
       <c r="AE79" s="75"/>
       <c r="AF79" s="74"/>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A80" s="121" t="s">
         <v>2</v>
       </c>
@@ -11358,7 +11382,7 @@
       <c r="AE80" s="63"/>
       <c r="AF80" s="118"/>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A81" s="121" t="s">
         <v>2</v>
       </c>
@@ -11453,7 +11477,7 @@
       <c r="AE81" s="72"/>
       <c r="AF81" s="71"/>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A82" s="123" t="s">
         <v>2</v>
       </c>
@@ -11551,7 +11575,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A83" s="123" t="s">
         <v>2</v>
       </c>
@@ -11645,7 +11669,7 @@
       <c r="AE83" s="63"/>
       <c r="AF83" s="118"/>
     </row>
-    <row r="84" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="135" t="s">
         <v>2</v>
       </c>
@@ -11743,7 +11767,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A85" s="49" t="s">
         <v>2</v>
       </c>
@@ -11841,7 +11865,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A86" s="49" t="s">
         <v>2</v>
       </c>
@@ -11940,7 +11964,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="135" t="s">
         <v>2</v>
       </c>
@@ -12038,7 +12062,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A88" s="123" t="s">
         <v>2</v>
       </c>
@@ -12137,7 +12161,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="89" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="123" t="s">
         <v>2</v>
       </c>
@@ -12235,7 +12259,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="90" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="123" t="s">
         <v>2</v>
       </c>
@@ -12333,7 +12357,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="121" t="s">
         <v>2</v>
       </c>
@@ -12431,7 +12455,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A92" s="49" t="s">
         <v>2</v>
       </c>
@@ -12525,7 +12549,7 @@
       <c r="AE92" s="44"/>
       <c r="AF92" s="56"/>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A93" s="49" t="s">
         <v>2</v>
       </c>
@@ -12619,7 +12643,7 @@
       <c r="AE93" s="44"/>
       <c r="AF93" s="56"/>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A94" s="49" t="s">
         <v>2</v>
       </c>
@@ -12713,7 +12737,7 @@
       <c r="AE94" s="44"/>
       <c r="AF94" s="43"/>
     </row>
-    <row r="95" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="135" t="s">
         <v>2</v>
       </c>
@@ -12808,7 +12832,7 @@
       <c r="AE95" s="44"/>
       <c r="AF95" s="43"/>
     </row>
-    <row r="96" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="123" t="s">
         <v>2</v>
       </c>
@@ -12906,7 +12930,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="123" t="s">
         <v>2</v>
       </c>
@@ -13004,7 +13028,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="123" t="s">
         <v>2</v>
       </c>
@@ -13098,7 +13122,7 @@
       <c r="AE98" s="63"/>
       <c r="AF98" s="62"/>
     </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A99" s="121" t="s">
         <v>2</v>
       </c>
@@ -13193,7 +13217,7 @@
       <c r="AE99" s="34"/>
       <c r="AF99" s="126"/>
     </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A100" s="49" t="s">
         <v>2</v>
       </c>
@@ -13292,7 +13316,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A101" s="49" t="s">
         <v>2</v>
       </c>
@@ -13386,7 +13410,7 @@
       <c r="AE101" s="26"/>
       <c r="AF101" s="59"/>
     </row>
-    <row r="102" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="49" t="s">
         <v>2</v>
       </c>
@@ -13480,7 +13504,7 @@
       <c r="AE102" s="26"/>
       <c r="AF102" s="59"/>
     </row>
-    <row r="103" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="135" t="s">
         <v>2</v>
       </c>
@@ -13575,7 +13599,7 @@
       <c r="AE103" s="44"/>
       <c r="AF103" s="56"/>
     </row>
-    <row r="104" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="135" t="s">
         <v>2</v>
       </c>
@@ -13669,7 +13693,7 @@
       <c r="AE104" s="26"/>
       <c r="AF104" s="59"/>
     </row>
-    <row r="105" spans="1:32" s="170" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:32" s="170" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="157" t="s">
         <v>2</v>
       </c>
@@ -13763,7 +13787,7 @@
       <c r="AE105" s="169"/>
       <c r="AF105" s="156"/>
     </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A106" s="123" t="s">
         <v>2</v>
       </c>
@@ -13861,7 +13885,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A107" s="123" t="s">
         <v>2</v>
       </c>
@@ -13955,7 +13979,7 @@
       <c r="AE107" s="34"/>
       <c r="AF107" s="131"/>
     </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A108" s="121" t="s">
         <v>2</v>
       </c>
@@ -14049,7 +14073,7 @@
       <c r="AE108" s="34"/>
       <c r="AF108" s="126"/>
     </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A109" s="121" t="s">
         <v>2</v>
       </c>
@@ -14144,7 +14168,7 @@
       <c r="AE109" s="34"/>
       <c r="AF109" s="131"/>
     </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A110" s="49" t="s">
         <v>2</v>
       </c>
@@ -14243,7 +14267,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A111" s="49" t="s">
         <v>2</v>
       </c>
@@ -14337,7 +14361,7 @@
       <c r="AE111" s="44"/>
       <c r="AF111" s="43"/>
     </row>
-    <row r="112" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A112" s="136" t="s">
         <v>2</v>
       </c>
@@ -14435,7 +14459,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A113" s="136" t="s">
         <v>2</v>
       </c>
@@ -14533,7 +14557,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A114" s="124" t="s">
         <v>2</v>
       </c>
@@ -14632,7 +14656,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A115" s="124" t="s">
         <v>2</v>
       </c>
@@ -14731,7 +14755,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A116" s="121" t="s">
         <v>2</v>
       </c>
@@ -14826,7 +14850,7 @@
       <c r="AE116" s="34"/>
       <c r="AF116" s="131"/>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A117" s="121" t="s">
         <v>2</v>
       </c>
@@ -14921,7 +14945,7 @@
       <c r="AE117" s="34"/>
       <c r="AF117" s="131"/>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A118" s="49" t="s">
         <v>2</v>
       </c>
@@ -15016,7 +15040,7 @@
       <c r="AE118" s="44"/>
       <c r="AF118" s="43"/>
     </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A119" s="135" t="s">
         <v>2</v>
       </c>
@@ -15111,7 +15135,7 @@
       <c r="AE119" s="75"/>
       <c r="AF119" s="74"/>
     </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A120" s="135" t="s">
         <v>2</v>
       </c>
@@ -15209,7 +15233,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A121" s="135" t="s">
         <v>2</v>
       </c>
@@ -15303,7 +15327,7 @@
       <c r="AE121" s="75"/>
       <c r="AF121" s="74"/>
     </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A122" s="123" t="s">
         <v>2</v>
       </c>
@@ -15397,7 +15421,7 @@
       <c r="AE122" s="63"/>
       <c r="AF122" s="63"/>
     </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A123" s="123" t="s">
         <v>2</v>
       </c>
@@ -15492,7 +15516,7 @@
       <c r="AE123" s="72"/>
       <c r="AF123" s="72"/>
     </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A124" s="123" t="s">
         <v>2</v>
       </c>
@@ -15590,7 +15614,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A125" s="123" t="s">
         <v>2</v>
       </c>
@@ -15684,7 +15708,7 @@
       <c r="AE125" s="25"/>
       <c r="AF125" s="24"/>
     </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A126" s="135" t="s">
         <v>2</v>
       </c>
@@ -15778,7 +15802,7 @@
       <c r="AE126" s="75"/>
       <c r="AF126" s="79"/>
     </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A127" s="135" t="s">
         <v>2</v>
       </c>
@@ -15872,7 +15896,7 @@
       <c r="AE127" s="75"/>
       <c r="AF127" s="74"/>
     </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A128" s="135" t="s">
         <v>2</v>
       </c>
@@ -15964,7 +15988,7 @@
       <c r="AE128" s="145"/>
       <c r="AF128" s="146"/>
     </row>
-    <row r="129" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="135" t="s">
         <v>2</v>
       </c>
@@ -16056,7 +16080,7 @@
       <c r="AE129" s="145"/>
       <c r="AF129" s="146"/>
     </row>
-    <row r="130" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A130" s="123" t="s">
         <v>2</v>
       </c>
@@ -16148,7 +16172,7 @@
       <c r="AE130" s="63"/>
       <c r="AF130" s="63"/>
     </row>
-    <row r="131" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A131" s="123" t="s">
         <v>2</v>
       </c>
@@ -16240,7 +16264,7 @@
       <c r="AE131" s="72"/>
       <c r="AF131" s="72"/>
     </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A132" s="123" t="s">
         <v>2</v>
       </c>
@@ -16332,7 +16356,7 @@
       <c r="AE132" s="72"/>
       <c r="AF132" s="71"/>
     </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A133" s="123" t="s">
         <v>2</v>
       </c>
@@ -16424,7 +16448,7 @@
       <c r="AE133" s="25"/>
       <c r="AF133" s="24"/>
     </row>
-    <row r="134" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A134" s="135" t="s">
         <v>2</v>
       </c>
@@ -16516,7 +16540,7 @@
       <c r="AE134" s="145"/>
       <c r="AF134" s="146"/>
     </row>
-    <row r="135" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A135" s="135" t="s">
         <v>2</v>
       </c>
@@ -16611,7 +16635,7 @@
       <c r="AE135" s="145"/>
       <c r="AF135" s="146"/>
     </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A136" s="135" t="s">
         <v>2</v>
       </c>
@@ -16703,7 +16727,7 @@
       <c r="AE136" s="145"/>
       <c r="AF136" s="146"/>
     </row>
-    <row r="137" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A137" s="135" t="s">
         <v>2</v>
       </c>
@@ -16795,7 +16819,7 @@
       <c r="AE137" s="145"/>
       <c r="AF137" s="146"/>
     </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A138" s="123" t="s">
         <v>2</v>
       </c>
@@ -16889,7 +16913,7 @@
       <c r="AE138" s="25"/>
       <c r="AF138" s="24"/>
     </row>
-    <row r="139" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="123" t="s">
         <v>2</v>
       </c>
@@ -16981,7 +17005,7 @@
       <c r="AE139" s="72"/>
       <c r="AF139" s="71"/>
     </row>
-    <row r="140" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A140" s="123" t="s">
         <v>2</v>
       </c>
@@ -17075,7 +17099,7 @@
       <c r="AE140" s="72"/>
       <c r="AF140" s="71"/>
     </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A141" s="123" t="s">
         <v>2</v>
       </c>
@@ -17170,7 +17194,7 @@
       <c r="AE141" s="72"/>
       <c r="AF141" s="71"/>
     </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A142" s="135" t="s">
         <v>2</v>
       </c>
@@ -17264,7 +17288,7 @@
       <c r="AE142" s="145"/>
       <c r="AF142" s="146"/>
     </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A143" s="135" t="s">
         <v>2</v>
       </c>
@@ -17358,7 +17382,7 @@
       <c r="AE143" s="26"/>
       <c r="AF143" s="59"/>
     </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A144" s="135" t="s">
         <v>2</v>
       </c>
@@ -17452,7 +17476,7 @@
       <c r="AE144" s="26"/>
       <c r="AF144" s="59"/>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A145" s="135" t="s">
         <v>2</v>
       </c>
@@ -17546,7 +17570,7 @@
       <c r="AE145" s="26"/>
       <c r="AF145" s="59"/>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A146" s="171" t="s">
         <v>2</v>
       </c>
@@ -17638,7 +17662,7 @@
       <c r="AE146" s="26"/>
       <c r="AF146" s="59"/>
     </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A147" s="171" t="s">
         <v>2</v>
       </c>
@@ -17730,7 +17754,7 @@
       <c r="AE147" s="26"/>
       <c r="AF147" s="146"/>
     </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A148" s="171" t="s">
         <v>2</v>
       </c>
@@ -17822,7 +17846,7 @@
       <c r="AE148" s="26"/>
       <c r="AF148" s="146"/>
     </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A149" s="171" t="s">
         <v>2</v>
       </c>
@@ -17914,7 +17938,7 @@
       <c r="AE149" s="26"/>
       <c r="AF149" s="146"/>
     </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A150" s="174"/>
       <c r="B150" s="175"/>
       <c r="C150" s="175"/>
@@ -17948,8 +17972,8 @@
       <c r="AE150" s="186"/>
       <c r="AF150" s="187"/>
     </row>
-    <row r="151" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="152" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:32" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:32" ht="24" x14ac:dyDescent="0.3">
       <c r="A152" s="9" t="s">
         <v>57</v>
       </c>
@@ -17981,14 +18005,14 @@
       <c r="AA152" s="9"/>
       <c r="AF152" s="8"/>
     </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A153" s="22"/>
       <c r="B153" s="22"/>
       <c r="C153" s="22"/>
       <c r="D153" s="22"/>
       <c r="E153" s="22"/>
-      <c r="F153" s="188"/>
-      <c r="G153" s="188"/>
+      <c r="F153" s="189"/>
+      <c r="G153" s="189"/>
       <c r="H153" s="21" t="s">
         <v>56</v>
       </c>
@@ -18018,7 +18042,7 @@
       <c r="AD153" s="21"/>
       <c r="AE153" s="17"/>
     </row>
-    <row r="154" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:32" ht="144" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>54</v>
       </c>
@@ -18065,7 +18089,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A155" s="16" t="s">
         <v>2</v>
       </c>
@@ -18114,7 +18138,7 @@
       <c r="P155" s="17"/>
       <c r="Q155" s="17"/>
     </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A156" s="16" t="s">
         <v>2</v>
       </c>
@@ -18163,7 +18187,7 @@
       <c r="P156" s="17"/>
       <c r="Q156" s="17"/>
     </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A157" s="16" t="s">
         <v>2</v>
       </c>
@@ -18212,7 +18236,7 @@
       <c r="P157" s="17"/>
       <c r="Q157" s="17"/>
     </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A158" s="16" t="s">
         <v>2</v>
       </c>
@@ -18261,7 +18285,7 @@
       <c r="P158" s="17"/>
       <c r="Q158" s="17"/>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A159" s="16" t="s">
         <v>2</v>
       </c>
@@ -18310,7 +18334,7 @@
       <c r="P159" s="17"/>
       <c r="Q159" s="17"/>
     </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A160" s="16" t="s">
         <v>2</v>
       </c>
@@ -18359,7 +18383,7 @@
       <c r="P160" s="17"/>
       <c r="Q160" s="17"/>
     </row>
-    <row r="161" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A161" s="16" t="s">
         <v>2</v>
       </c>
@@ -18408,7 +18432,7 @@
       <c r="P161" s="17"/>
       <c r="Q161" s="17"/>
     </row>
-    <row r="162" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A162" s="16" t="s">
         <v>2</v>
       </c>
@@ -18457,7 +18481,7 @@
       <c r="P162" s="17"/>
       <c r="Q162" s="17"/>
     </row>
-    <row r="163" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A163" s="16" t="s">
         <v>2</v>
       </c>
@@ -18506,7 +18530,7 @@
       <c r="P163" s="17"/>
       <c r="Q163" s="17"/>
     </row>
-    <row r="164" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A164" s="16" t="s">
         <v>2</v>
       </c>
@@ -18555,7 +18579,7 @@
       <c r="P164" s="17"/>
       <c r="Q164" s="17"/>
     </row>
-    <row r="165" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A165" s="16" t="s">
         <v>2</v>
       </c>
@@ -18602,7 +18626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A166" s="16" t="s">
         <v>2</v>
       </c>
@@ -18665,7 +18689,7 @@
       <c r="AD166" s="8"/>
       <c r="AE166" s="8"/>
     </row>
-    <row r="167" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:31" x14ac:dyDescent="0.2">
       <c r="N167" s="8"/>
       <c r="O167" s="8"/>
       <c r="P167" s="8"/>
@@ -18685,8 +18709,8 @@
       <c r="AD167" s="8"/>
       <c r="AE167" s="8"/>
     </row>
-    <row r="168" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="169" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:31" ht="24" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
         <v>19</v>
       </c>
@@ -18702,7 +18726,7 @@
       <c r="K169" s="8"/>
       <c r="L169" s="8"/>
     </row>
-    <row r="171" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:31" ht="156" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="s">
         <v>18</v>
       </c>
@@ -18728,7 +18752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>2</v>
       </c>
@@ -18754,7 +18778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>2</v>
       </c>
@@ -18780,7 +18804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>2</v>
       </c>
@@ -18806,7 +18830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>2</v>
       </c>
@@ -18832,7 +18856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>2</v>
       </c>
@@ -18858,7 +18882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D179" s="1">
         <v>42</v>
       </c>
@@ -18874,7 +18898,7 @@
         <v>54.6</v>
       </c>
     </row>
-    <row r="180" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D180" s="1">
         <v>92</v>
       </c>
@@ -18890,7 +18914,7 @@
         <v>101.2</v>
       </c>
     </row>
-    <row r="181" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D181" s="1">
         <v>235</v>
       </c>
@@ -18906,7 +18930,7 @@
         <v>211.5</v>
       </c>
     </row>
-    <row r="182" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D182" s="1">
         <v>686</v>
       </c>
@@ -18922,7 +18946,7 @@
         <v>480.2</v>
       </c>
     </row>
-    <row r="183" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D183" s="1">
         <v>1040</v>
       </c>
@@ -18936,6 +18960,51 @@
       <c r="I183">
         <f>D183*F183</f>
         <v>520</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A186" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="B186" s="9"/>
+      <c r="C186" s="9"/>
+      <c r="D186" s="9"/>
+      <c r="E186" s="9"/>
+      <c r="F186" s="9"/>
+      <c r="G186" s="9"/>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A187" s="188"/>
+      <c r="B187" s="188"/>
+      <c r="C187" s="188"/>
+    </row>
+    <row r="188" spans="1:9" ht="110" x14ac:dyDescent="0.2">
+      <c r="A188" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C188" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D188" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A189" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B189" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="C189" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="D189" s="15" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -18945,12 +19014,12 @@
     <mergeCell ref="F153:G153"/>
   </mergeCells>
   <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M150 R143:T150">
-    <cfRule type="expression" dxfId="25" priority="78">
+    <cfRule type="expression" dxfId="118" priority="78">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="24" priority="71">
+    <cfRule type="expression" dxfId="117" priority="71">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18967,7 +19036,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:M120 R116:T120">
-    <cfRule type="expression" dxfId="23" priority="65">
+    <cfRule type="expression" dxfId="116" priority="65">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18996,7 +19065,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115 R115:T115">
-    <cfRule type="expression" dxfId="22" priority="63">
+    <cfRule type="expression" dxfId="115" priority="63">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19013,12 +19082,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126:M127 R126:T127">
-    <cfRule type="expression" dxfId="21" priority="60">
+    <cfRule type="expression" dxfId="114" priority="60">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126 R126:T126">
-    <cfRule type="expression" dxfId="20" priority="59">
+    <cfRule type="expression" dxfId="113" priority="59">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19047,12 +19116,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="19" priority="57">
+    <cfRule type="expression" dxfId="112" priority="57">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S129:T129 M129">
-    <cfRule type="expression" dxfId="18" priority="56">
+    <cfRule type="expression" dxfId="111" priority="56">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19069,17 +19138,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R129">
-    <cfRule type="expression" dxfId="17" priority="54">
+    <cfRule type="expression" dxfId="110" priority="54">
       <formula>R129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="16" priority="39">
+    <cfRule type="expression" dxfId="109" priority="39">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="15" priority="41">
+    <cfRule type="expression" dxfId="108" priority="41">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19096,12 +19165,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="14" priority="34">
+    <cfRule type="expression" dxfId="107" priority="34">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M133 R130:T133">
-    <cfRule type="expression" dxfId="13" priority="35">
+    <cfRule type="expression" dxfId="106" priority="35">
       <formula>M130=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19130,12 +19199,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="12" priority="32">
+    <cfRule type="expression" dxfId="105" priority="32">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="11" priority="27">
+    <cfRule type="expression" dxfId="104" priority="27">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19152,12 +19221,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="10" priority="29">
+    <cfRule type="expression" dxfId="103" priority="29">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R137">
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="102" priority="22">
       <formula>R137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19174,12 +19243,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S137:T137 M137">
-    <cfRule type="expression" dxfId="8" priority="24">
+    <cfRule type="expression" dxfId="101" priority="24">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="7" priority="20">
+    <cfRule type="expression" dxfId="100" priority="20">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19196,7 +19265,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="6" priority="18">
+    <cfRule type="expression" dxfId="99" priority="18">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19213,7 +19282,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="5" priority="16">
+    <cfRule type="expression" dxfId="98" priority="16">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19230,7 +19299,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="97" priority="14">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19247,7 +19316,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="96" priority="10">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19264,7 +19333,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R142">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="95" priority="5">
       <formula>R142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19281,12 +19350,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S142:T142 M142">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="94" priority="7">
       <formula>M142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105:T105 M105">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="93" priority="3">
       <formula>M105=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19315,37 +19384,37 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G135"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 G136:G150 H40:I150 J141:J150">
+    <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G135" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 G136:G150 H40:I150 J141:J150" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D155:G166 P140:V140 M140:N140 N24:O139 Q24:W139 Q141:W150 N141:O150">
+    <dataValidation type="decimal" allowBlank="1" sqref="D155:G166 P140:V140 M140:N140 N24:O139 Q24:W139 Q141:W150 N141:O150" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H155:L164 H165:I165 J166:L166 W140:Z140 X24:AA139 X141:AA150">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H155:L164 H165:I165 J166:L166 W140:Z140 X24:AA139 X141:AA150" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C155:C166 C24:C150">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C155:C166 C24:C150" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J165:L165 M155:O166 AA140:AC140 AB131:AB142 AC131:AC139 AC141:AC142 AB24:AC130 AD24:AF142 AB143:AF150"/>
-    <dataValidation type="list" sqref="O140 P24:P139 P141:P150">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J165:L165 M155:O166 AA140:AC140 AB131:AB142 AC131:AC139 AC141:AC142 AB24:AC130 AD24:AF142 AB143:AF150" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation type="list" sqref="O140 P24:P139 P141:P150" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L150">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L150" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="L140 M24:M139 M141:M150">
+    <dataValidation type="list" sqref="L140 M24:M139 M141:M150" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J140">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J140" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F150">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F150" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -19360,7 +19429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -19370,20 +19439,20 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" customWidth="1"/>
     <col min="9" max="28" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>426</v>
       </c>
@@ -19397,19 +19466,19 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="98"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="188"/>
-      <c r="G3" s="188"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="189"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>
       <c r="K3" s="97"/>
     </row>
-    <row r="4" spans="2:11" ht="136.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="132" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>425</v>
       </c>
@@ -19432,7 +19501,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="116" t="s">
         <v>2</v>
       </c>
@@ -19453,7 +19522,7 @@
       </c>
       <c r="H5" s="113"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="116" t="s">
         <v>2</v>
       </c>
@@ -19474,7 +19543,7 @@
       </c>
       <c r="H6" s="113"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="112" t="s">
         <v>411</v>
       </c>
@@ -19487,7 +19556,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="112" t="s">
         <v>411</v>
       </c>
@@ -19500,7 +19569,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="112" t="s">
         <v>411</v>
       </c>
@@ -19513,7 +19582,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="116" t="s">
         <v>2</v>
       </c>
@@ -19534,7 +19603,7 @@
       </c>
       <c r="H10" s="113"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="112" t="s">
         <v>411</v>
       </c>
@@ -19547,7 +19616,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="112" t="s">
         <v>411</v>
       </c>
@@ -19560,7 +19629,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="112" t="s">
         <v>411</v>
       </c>
@@ -19573,7 +19642,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="116" t="s">
         <v>2</v>
       </c>
@@ -19594,7 +19663,7 @@
       </c>
       <c r="H14" s="113"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="112" t="s">
         <v>411</v>
       </c>
@@ -19607,7 +19676,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="112" t="s">
         <v>411</v>
       </c>
@@ -19620,7 +19689,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="112" t="s">
         <v>411</v>
       </c>
@@ -19633,7 +19702,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="116" t="s">
         <v>2</v>
       </c>
@@ -19654,7 +19723,7 @@
       </c>
       <c r="H18" s="113"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="112" t="s">
         <v>411</v>
       </c>
@@ -19667,7 +19736,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="112" t="s">
         <v>411</v>
       </c>
@@ -19680,7 +19749,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="112" t="s">
         <v>411</v>
       </c>
@@ -19693,7 +19762,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="112" t="s">
         <v>2</v>
       </c>
@@ -19714,7 +19783,7 @@
       </c>
       <c r="H22" s="109"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="112" t="s">
         <v>411</v>
       </c>
@@ -19727,7 +19796,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="112" t="s">
         <v>2</v>
       </c>
@@ -19748,7 +19817,7 @@
       </c>
       <c r="H24" s="109"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="112" t="s">
         <v>411</v>
       </c>
@@ -19761,7 +19830,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="112" t="s">
         <v>2</v>
       </c>
@@ -19782,7 +19851,7 @@
       </c>
       <c r="H26" s="109"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="112" t="s">
         <v>411</v>
       </c>
@@ -19795,7 +19864,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="112" t="s">
         <v>2</v>
       </c>
@@ -19816,7 +19885,7 @@
       </c>
       <c r="H28" s="109"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="112" t="s">
         <v>411</v>
       </c>
@@ -19829,8 +19898,8 @@
         <v>465</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:8" ht="24" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
         <v>410</v>
       </c>
@@ -19841,7 +19910,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="35" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="128" x14ac:dyDescent="0.2">
       <c r="B35" s="108" t="s">
         <v>409</v>
       </c>
@@ -19855,7 +19924,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="106" t="s">
         <v>2</v>
       </c>
@@ -19869,7 +19938,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="106" t="s">
         <v>2</v>
       </c>
@@ -19883,7 +19952,7 @@
         <v>8.7055056329612412E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="106" t="s">
         <v>2</v>
       </c>
@@ -19897,7 +19966,7 @@
         <v>8.027415617602307E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="106" t="s">
         <v>2</v>
       </c>
@@ -19911,7 +19980,7 @@
         <v>7.5785828325519916E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="106" t="s">
         <v>2</v>
       </c>
@@ -19925,7 +19994,7 @@
         <v>7.2477966367769556E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="106" t="s">
         <v>2</v>
       </c>
@@ -19939,7 +20008,7 @@
         <v>6.988271187715793E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" s="106" t="s">
         <v>2</v>
       </c>
@@ -19953,7 +20022,7 @@
         <v>6.776109134004811E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" s="106" t="s">
         <v>2</v>
       </c>
@@ -19967,7 +20036,7 @@
         <v>6.5975395538644718E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" s="106" t="s">
         <v>2</v>
       </c>
@@ -19981,7 +20050,7 @@
         <v>6.4439401497725424E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" s="106" t="s">
         <v>2</v>
       </c>
@@ -19995,8 +20064,8 @@
         <v>6.3095734448019331E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:8" ht="24" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
         <v>396</v>
       </c>
@@ -20007,7 +20076,7 @@
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
     </row>
-    <row r="49" spans="2:8" ht="130.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" ht="128" x14ac:dyDescent="0.2">
       <c r="B49" s="103" t="s">
         <v>395</v>
       </c>
@@ -20030,7 +20099,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="101" t="s">
         <v>2</v>
       </c>
@@ -20058,8 +20127,8 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="H5:H29"/>
-    <dataValidation allowBlank="1" sqref="E36:F45 E5:G29"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="H5:H29" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" sqref="E36:F45 E5:G29" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
pf seasonal ready. NOT THE STATS of the collectable
Former-commit-id: 5feff0c819c161190e7b6f46975021ecb1d1e32d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msana/Workspace/Dragon/client_ios/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C071106B-1B35-B74E-AE66-F142B34F38A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="37395" windowHeight="21135"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="2" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$154:$O$155</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="531">
   <si>
     <t>tier_4</t>
   </si>
@@ -1633,11 +1632,14 @@
   <si>
     <t>TID_LEPRECHAUN_HAT</t>
   </si>
+  <si>
+    <t>patricks_balloon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2207,7 +2209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2658,48 +2660,6 @@
     <xf numFmtId="2" fontId="16" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2711,7 +2671,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="119">
+  <dxfs count="121">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5203,114 +5177,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A23:AF149" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+  <autoFilter ref="A23:AF149"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="89"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="88"/>
+    <tableColumn id="6" name="[category]" dataDxfId="87"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="86"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="85"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="84"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="83"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="82"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="81"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="80"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="79"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="78"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="77"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="76"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="75"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="74"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="73"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="72"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="71"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="70"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="69"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="68"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="67"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="66"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="65"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="62"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="61"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="60"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="59"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
-  <autoFilter ref="A4:B18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+  <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="53"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A154:O166" totalsRowShown="0">
-  <autoFilter ref="A154:O166" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A154:O166" totalsRowShown="0">
+  <autoFilter ref="A154:O166"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0200-00001E000000}" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0200-00001F000000}" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0200-000021000000}" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0200-000022000000}" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="[category]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="16" name="[size]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="B4:H29" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="17"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="6" name="[order]" dataDxfId="15"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="14"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="13"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="12"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B35:E45" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="5"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="4"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="3"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="2" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5578,27 +5552,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:AF189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="F197" sqref="F197"/>
+      <selection pane="topRight" activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="28" max="28" width="40.6640625" customWidth="1"/>
-    <col min="29" max="29" width="162.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="107.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="40.7109375" customWidth="1"/>
+    <col min="29" max="29" width="162.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="107.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:24" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>386</v>
       </c>
@@ -5626,20 +5600,20 @@
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
     </row>
-    <row r="3" spans="1:24" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="98" t="s">
         <v>385</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
-      <c r="E3" s="189"/>
-      <c r="F3" s="189"/>
+      <c r="E3" s="175"/>
+      <c r="F3" s="175"/>
       <c r="G3" s="22"/>
       <c r="H3" s="21"/>
       <c r="I3" s="97"/>
     </row>
-    <row r="4" spans="1:24" ht="131" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="134.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>384</v>
       </c>
@@ -5647,7 +5621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="94" t="s">
         <v>2</v>
       </c>
@@ -5655,7 +5629,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="94" t="s">
         <v>2</v>
       </c>
@@ -5663,7 +5637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="94" t="s">
         <v>2</v>
       </c>
@@ -5671,7 +5645,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="94" t="s">
         <v>2</v>
       </c>
@@ -5679,7 +5653,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="94" t="s">
         <v>2</v>
       </c>
@@ -5687,7 +5661,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="94" t="s">
         <v>2</v>
       </c>
@@ -5695,7 +5669,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="94" t="s">
         <v>2</v>
       </c>
@@ -5703,7 +5677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="94" t="s">
         <v>2</v>
       </c>
@@ -5711,7 +5685,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="96" t="s">
         <v>2</v>
       </c>
@@ -5719,7 +5693,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="94" t="s">
         <v>2</v>
       </c>
@@ -5727,7 +5701,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="94" t="s">
         <v>2</v>
       </c>
@@ -5735,7 +5709,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="94" t="s">
         <v>2</v>
       </c>
@@ -5743,7 +5717,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="94" t="s">
         <v>2</v>
       </c>
@@ -5751,7 +5725,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="94" t="s">
         <v>2</v>
       </c>
@@ -5759,8 +5733,8 @@
         <v>449</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:32" ht="24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>381</v>
       </c>
@@ -5791,15 +5765,15 @@
       <c r="Z21" s="9"/>
       <c r="AA21" s="9"/>
     </row>
-    <row r="22" spans="1:32" s="17" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="21" t="s">
         <v>380</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="189"/>
-      <c r="F22" s="189"/>
+      <c r="E22" s="175"/>
+      <c r="F22" s="175"/>
       <c r="G22" s="22"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22"/>
@@ -5816,7 +5790,7 @@
       <c r="Z22" s="21"/>
       <c r="AA22" s="21"/>
     </row>
-    <row r="23" spans="1:32" ht="127" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" ht="126" x14ac:dyDescent="0.25">
       <c r="A23" s="93" t="s">
         <v>378</v>
       </c>
@@ -5914,7 +5888,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="119" t="s">
         <v>2</v>
       </c>
@@ -6012,7 +5986,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="119" t="s">
         <v>2</v>
       </c>
@@ -6110,7 +6084,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="119" t="s">
         <v>2</v>
       </c>
@@ -6208,7 +6182,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="119" t="s">
         <v>2</v>
       </c>
@@ -6303,7 +6277,7 @@
       <c r="AE27" s="72"/>
       <c r="AF27" s="80"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
         <v>2</v>
       </c>
@@ -6401,7 +6375,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
         <v>2</v>
       </c>
@@ -6499,7 +6473,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="30" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
         <v>2</v>
       </c>
@@ -6597,7 +6571,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
         <v>2</v>
       </c>
@@ -6692,7 +6666,7 @@
       <c r="AE31" s="75"/>
       <c r="AF31" s="79"/>
     </row>
-    <row r="32" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="123" t="s">
         <v>2</v>
       </c>
@@ -6786,7 +6760,7 @@
       <c r="AE32" s="72"/>
       <c r="AF32" s="71"/>
     </row>
-    <row r="33" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="123" t="s">
         <v>2</v>
       </c>
@@ -6885,7 +6859,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="123" t="s">
         <v>2</v>
       </c>
@@ -6979,7 +6953,7 @@
       <c r="AE34" s="72"/>
       <c r="AF34" s="71"/>
     </row>
-    <row r="35" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="121" t="s">
         <v>2</v>
       </c>
@@ -7074,7 +7048,7 @@
       <c r="AE35" s="72"/>
       <c r="AF35" s="71"/>
     </row>
-    <row r="36" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="49" t="s">
         <v>2</v>
       </c>
@@ -7169,7 +7143,7 @@
       <c r="AE36" s="75"/>
       <c r="AF36" s="74"/>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
         <v>2</v>
       </c>
@@ -7264,7 +7238,7 @@
       <c r="AE37" s="75"/>
       <c r="AF37" s="79"/>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="49" t="s">
         <v>2</v>
       </c>
@@ -7359,7 +7333,7 @@
       <c r="AE38" s="75"/>
       <c r="AF38" s="79"/>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="135" t="s">
         <v>2</v>
       </c>
@@ -7454,7 +7428,7 @@
       <c r="AE39" s="75"/>
       <c r="AF39" s="79"/>
     </row>
-    <row r="40" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="123" t="s">
         <v>2</v>
       </c>
@@ -7548,7 +7522,7 @@
       <c r="AE40" s="72"/>
       <c r="AF40" s="71"/>
     </row>
-    <row r="41" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="123" t="s">
         <v>2</v>
       </c>
@@ -7642,7 +7616,7 @@
       <c r="AE41" s="72"/>
       <c r="AF41" s="71"/>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="123" t="s">
         <v>2</v>
       </c>
@@ -7736,7 +7710,7 @@
       <c r="AE42" s="72"/>
       <c r="AF42" s="71"/>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="121" t="s">
         <v>2</v>
       </c>
@@ -7831,7 +7805,7 @@
       <c r="AE43" s="72"/>
       <c r="AF43" s="71"/>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
         <v>2</v>
       </c>
@@ -7929,7 +7903,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="49" t="s">
         <v>2</v>
       </c>
@@ -8023,7 +7997,7 @@
       <c r="AE45" s="75"/>
       <c r="AF45" s="74"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="49" t="s">
         <v>2</v>
       </c>
@@ -8121,7 +8095,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="135" t="s">
         <v>2</v>
       </c>
@@ -8216,7 +8190,7 @@
       <c r="AE47" s="75"/>
       <c r="AF47" s="74"/>
     </row>
-    <row r="48" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="123" t="s">
         <v>2</v>
       </c>
@@ -8314,7 +8288,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="49" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="123" t="s">
         <v>2</v>
       </c>
@@ -8408,7 +8382,7 @@
       <c r="AE49" s="72"/>
       <c r="AF49" s="71"/>
     </row>
-    <row r="50" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="121" t="s">
         <v>2</v>
       </c>
@@ -8506,7 +8480,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="121" t="s">
         <v>2</v>
       </c>
@@ -8604,7 +8578,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="49" t="s">
         <v>2</v>
       </c>
@@ -8702,7 +8676,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" s="49" t="s">
         <v>2</v>
       </c>
@@ -8800,7 +8774,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" s="135" t="s">
         <v>2</v>
       </c>
@@ -8898,7 +8872,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="135" t="s">
         <v>2</v>
       </c>
@@ -8993,7 +8967,7 @@
       <c r="AE55" s="75"/>
       <c r="AF55" s="74"/>
     </row>
-    <row r="56" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="123" t="s">
         <v>2</v>
       </c>
@@ -9088,7 +9062,7 @@
       <c r="AE56" s="72"/>
       <c r="AF56" s="71"/>
     </row>
-    <row r="57" spans="1:32" s="150" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:32" s="150" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="123" t="s">
         <v>2</v>
       </c>
@@ -9176,7 +9150,7 @@
       <c r="AE57" s="72"/>
       <c r="AF57" s="71"/>
     </row>
-    <row r="58" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="121" t="s">
         <v>2</v>
       </c>
@@ -9271,7 +9245,7 @@
       <c r="AE58" s="72"/>
       <c r="AF58" s="80"/>
     </row>
-    <row r="59" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="121" t="s">
         <v>2</v>
       </c>
@@ -9366,7 +9340,7 @@
       <c r="AE59" s="72"/>
       <c r="AF59" s="80"/>
     </row>
-    <row r="60" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="49" t="s">
         <v>2</v>
       </c>
@@ -9461,7 +9435,7 @@
       <c r="AE60" s="75"/>
       <c r="AF60" s="79"/>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="49" t="s">
         <v>2</v>
       </c>
@@ -9555,7 +9529,7 @@
       <c r="AE61" s="75"/>
       <c r="AF61" s="74"/>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" s="135" t="s">
         <v>2</v>
       </c>
@@ -9650,7 +9624,7 @@
       <c r="AE62" s="75"/>
       <c r="AF62" s="74"/>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63" s="135" t="s">
         <v>2</v>
       </c>
@@ -9745,7 +9719,7 @@
       <c r="AE63" s="75"/>
       <c r="AF63" s="74"/>
     </row>
-    <row r="64" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="123" t="s">
         <v>2</v>
       </c>
@@ -9840,7 +9814,7 @@
       <c r="AE64" s="72"/>
       <c r="AF64" s="80"/>
     </row>
-    <row r="65" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="123" t="s">
         <v>2</v>
       </c>
@@ -9933,7 +9907,7 @@
       <c r="AE65" s="63"/>
       <c r="AF65" s="133"/>
     </row>
-    <row r="66" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="121" t="s">
         <v>2</v>
       </c>
@@ -10032,7 +10006,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" s="121" t="s">
         <v>2</v>
       </c>
@@ -10131,7 +10105,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="49" t="s">
         <v>2</v>
       </c>
@@ -10230,7 +10204,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="135" t="s">
         <v>2</v>
       </c>
@@ -10328,7 +10302,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="135" t="s">
         <v>2</v>
       </c>
@@ -10423,7 +10397,7 @@
       <c r="AE70" s="75"/>
       <c r="AF70" s="79"/>
     </row>
-    <row r="71" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="135" t="s">
         <v>2</v>
       </c>
@@ -10518,7 +10492,7 @@
       <c r="AE71" s="75"/>
       <c r="AF71" s="79"/>
     </row>
-    <row r="72" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="121" t="s">
         <v>2</v>
       </c>
@@ -10616,7 +10590,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="121" t="s">
         <v>2</v>
       </c>
@@ -10709,7 +10683,7 @@
       <c r="AE73" s="63"/>
       <c r="AF73" s="63"/>
     </row>
-    <row r="74" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="121" t="s">
         <v>2</v>
       </c>
@@ -10802,7 +10776,7 @@
       <c r="AE74" s="63"/>
       <c r="AF74" s="133"/>
     </row>
-    <row r="75" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="123" t="s">
         <v>2</v>
       </c>
@@ -10900,7 +10874,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="135" t="s">
         <v>2</v>
       </c>
@@ -10996,7 +10970,7 @@
       </c>
       <c r="AF76" s="68"/>
     </row>
-    <row r="77" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="135" t="s">
         <v>2</v>
       </c>
@@ -11094,7 +11068,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
         <v>2</v>
       </c>
@@ -11193,7 +11167,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
         <v>2</v>
       </c>
@@ -11287,7 +11261,7 @@
       <c r="AE79" s="75"/>
       <c r="AF79" s="74"/>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80" s="121" t="s">
         <v>2</v>
       </c>
@@ -11382,7 +11356,7 @@
       <c r="AE80" s="63"/>
       <c r="AF80" s="118"/>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81" s="121" t="s">
         <v>2</v>
       </c>
@@ -11477,7 +11451,7 @@
       <c r="AE81" s="72"/>
       <c r="AF81" s="71"/>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" s="123" t="s">
         <v>2</v>
       </c>
@@ -11575,7 +11549,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" s="123" t="s">
         <v>2</v>
       </c>
@@ -11669,7 +11643,7 @@
       <c r="AE83" s="63"/>
       <c r="AF83" s="118"/>
     </row>
-    <row r="84" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="135" t="s">
         <v>2</v>
       </c>
@@ -11767,7 +11741,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85" s="49" t="s">
         <v>2</v>
       </c>
@@ -11865,7 +11839,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A86" s="49" t="s">
         <v>2</v>
       </c>
@@ -11964,7 +11938,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="135" t="s">
         <v>2</v>
       </c>
@@ -12062,7 +12036,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A88" s="123" t="s">
         <v>2</v>
       </c>
@@ -12161,7 +12135,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="89" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="123" t="s">
         <v>2</v>
       </c>
@@ -12259,7 +12233,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="90" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="123" t="s">
         <v>2</v>
       </c>
@@ -12357,7 +12331,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="121" t="s">
         <v>2</v>
       </c>
@@ -12455,7 +12429,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A92" s="49" t="s">
         <v>2</v>
       </c>
@@ -12549,7 +12523,7 @@
       <c r="AE92" s="44"/>
       <c r="AF92" s="56"/>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" s="49" t="s">
         <v>2</v>
       </c>
@@ -12643,7 +12617,7 @@
       <c r="AE93" s="44"/>
       <c r="AF93" s="56"/>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94" s="49" t="s">
         <v>2</v>
       </c>
@@ -12737,7 +12711,7 @@
       <c r="AE94" s="44"/>
       <c r="AF94" s="43"/>
     </row>
-    <row r="95" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="135" t="s">
         <v>2</v>
       </c>
@@ -12832,7 +12806,7 @@
       <c r="AE95" s="44"/>
       <c r="AF95" s="43"/>
     </row>
-    <row r="96" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="123" t="s">
         <v>2</v>
       </c>
@@ -12930,7 +12904,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="123" t="s">
         <v>2</v>
       </c>
@@ -13028,7 +13002,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="123" t="s">
         <v>2</v>
       </c>
@@ -13122,7 +13096,7 @@
       <c r="AE98" s="63"/>
       <c r="AF98" s="62"/>
     </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A99" s="121" t="s">
         <v>2</v>
       </c>
@@ -13217,7 +13191,7 @@
       <c r="AE99" s="34"/>
       <c r="AF99" s="126"/>
     </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A100" s="49" t="s">
         <v>2</v>
       </c>
@@ -13316,7 +13290,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A101" s="49" t="s">
         <v>2</v>
       </c>
@@ -13410,7 +13384,7 @@
       <c r="AE101" s="26"/>
       <c r="AF101" s="59"/>
     </row>
-    <row r="102" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="49" t="s">
         <v>2</v>
       </c>
@@ -13504,7 +13478,7 @@
       <c r="AE102" s="26"/>
       <c r="AF102" s="59"/>
     </row>
-    <row r="103" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="135" t="s">
         <v>2</v>
       </c>
@@ -13599,7 +13573,7 @@
       <c r="AE103" s="44"/>
       <c r="AF103" s="56"/>
     </row>
-    <row r="104" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:32" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="135" t="s">
         <v>2</v>
       </c>
@@ -13693,7 +13667,7 @@
       <c r="AE104" s="26"/>
       <c r="AF104" s="59"/>
     </row>
-    <row r="105" spans="1:32" s="170" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:32" s="170" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="157" t="s">
         <v>2</v>
       </c>
@@ -13787,7 +13761,7 @@
       <c r="AE105" s="169"/>
       <c r="AF105" s="156"/>
     </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A106" s="123" t="s">
         <v>2</v>
       </c>
@@ -13885,7 +13859,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A107" s="123" t="s">
         <v>2</v>
       </c>
@@ -13979,7 +13953,7 @@
       <c r="AE107" s="34"/>
       <c r="AF107" s="131"/>
     </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A108" s="121" t="s">
         <v>2</v>
       </c>
@@ -14073,7 +14047,7 @@
       <c r="AE108" s="34"/>
       <c r="AF108" s="126"/>
     </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A109" s="121" t="s">
         <v>2</v>
       </c>
@@ -14168,7 +14142,7 @@
       <c r="AE109" s="34"/>
       <c r="AF109" s="131"/>
     </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A110" s="49" t="s">
         <v>2</v>
       </c>
@@ -14267,7 +14241,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A111" s="49" t="s">
         <v>2</v>
       </c>
@@ -14361,7 +14335,7 @@
       <c r="AE111" s="44"/>
       <c r="AF111" s="43"/>
     </row>
-    <row r="112" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A112" s="136" t="s">
         <v>2</v>
       </c>
@@ -14459,7 +14433,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A113" s="136" t="s">
         <v>2</v>
       </c>
@@ -14557,7 +14531,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A114" s="124" t="s">
         <v>2</v>
       </c>
@@ -14656,7 +14630,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A115" s="124" t="s">
         <v>2</v>
       </c>
@@ -14755,7 +14729,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A116" s="121" t="s">
         <v>2</v>
       </c>
@@ -14850,7 +14824,7 @@
       <c r="AE116" s="34"/>
       <c r="AF116" s="131"/>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" s="121" t="s">
         <v>2</v>
       </c>
@@ -14945,7 +14919,7 @@
       <c r="AE117" s="34"/>
       <c r="AF117" s="131"/>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A118" s="49" t="s">
         <v>2</v>
       </c>
@@ -15040,7 +15014,7 @@
       <c r="AE118" s="44"/>
       <c r="AF118" s="43"/>
     </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A119" s="135" t="s">
         <v>2</v>
       </c>
@@ -15135,7 +15109,7 @@
       <c r="AE119" s="75"/>
       <c r="AF119" s="74"/>
     </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A120" s="135" t="s">
         <v>2</v>
       </c>
@@ -15233,7 +15207,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A121" s="135" t="s">
         <v>2</v>
       </c>
@@ -15327,7 +15301,7 @@
       <c r="AE121" s="75"/>
       <c r="AF121" s="74"/>
     </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A122" s="123" t="s">
         <v>2</v>
       </c>
@@ -15421,7 +15395,7 @@
       <c r="AE122" s="63"/>
       <c r="AF122" s="63"/>
     </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A123" s="123" t="s">
         <v>2</v>
       </c>
@@ -15516,7 +15490,7 @@
       <c r="AE123" s="72"/>
       <c r="AF123" s="72"/>
     </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A124" s="123" t="s">
         <v>2</v>
       </c>
@@ -15614,7 +15588,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A125" s="123" t="s">
         <v>2</v>
       </c>
@@ -15708,7 +15682,7 @@
       <c r="AE125" s="25"/>
       <c r="AF125" s="24"/>
     </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A126" s="135" t="s">
         <v>2</v>
       </c>
@@ -15802,7 +15776,7 @@
       <c r="AE126" s="75"/>
       <c r="AF126" s="79"/>
     </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A127" s="135" t="s">
         <v>2</v>
       </c>
@@ -15896,7 +15870,7 @@
       <c r="AE127" s="75"/>
       <c r="AF127" s="74"/>
     </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A128" s="135" t="s">
         <v>2</v>
       </c>
@@ -15988,7 +15962,7 @@
       <c r="AE128" s="145"/>
       <c r="AF128" s="146"/>
     </row>
-    <row r="129" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:32" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="135" t="s">
         <v>2</v>
       </c>
@@ -16080,7 +16054,7 @@
       <c r="AE129" s="145"/>
       <c r="AF129" s="146"/>
     </row>
-    <row r="130" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A130" s="123" t="s">
         <v>2</v>
       </c>
@@ -16172,7 +16146,7 @@
       <c r="AE130" s="63"/>
       <c r="AF130" s="63"/>
     </row>
-    <row r="131" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A131" s="123" t="s">
         <v>2</v>
       </c>
@@ -16264,7 +16238,7 @@
       <c r="AE131" s="72"/>
       <c r="AF131" s="72"/>
     </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A132" s="123" t="s">
         <v>2</v>
       </c>
@@ -16356,7 +16330,7 @@
       <c r="AE132" s="72"/>
       <c r="AF132" s="71"/>
     </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A133" s="123" t="s">
         <v>2</v>
       </c>
@@ -16448,7 +16422,7 @@
       <c r="AE133" s="25"/>
       <c r="AF133" s="24"/>
     </row>
-    <row r="134" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A134" s="135" t="s">
         <v>2</v>
       </c>
@@ -16540,7 +16514,7 @@
       <c r="AE134" s="145"/>
       <c r="AF134" s="146"/>
     </row>
-    <row r="135" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A135" s="135" t="s">
         <v>2</v>
       </c>
@@ -16635,7 +16609,7 @@
       <c r="AE135" s="145"/>
       <c r="AF135" s="146"/>
     </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A136" s="135" t="s">
         <v>2</v>
       </c>
@@ -16727,7 +16701,7 @@
       <c r="AE136" s="145"/>
       <c r="AF136" s="146"/>
     </row>
-    <row r="137" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A137" s="135" t="s">
         <v>2</v>
       </c>
@@ -16819,7 +16793,7 @@
       <c r="AE137" s="145"/>
       <c r="AF137" s="146"/>
     </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A138" s="123" t="s">
         <v>2</v>
       </c>
@@ -16913,7 +16887,7 @@
       <c r="AE138" s="25"/>
       <c r="AF138" s="24"/>
     </row>
-    <row r="139" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="123" t="s">
         <v>2</v>
       </c>
@@ -17005,7 +16979,7 @@
       <c r="AE139" s="72"/>
       <c r="AF139" s="71"/>
     </row>
-    <row r="140" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A140" s="123" t="s">
         <v>2</v>
       </c>
@@ -17099,7 +17073,7 @@
       <c r="AE140" s="72"/>
       <c r="AF140" s="71"/>
     </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A141" s="123" t="s">
         <v>2</v>
       </c>
@@ -17194,7 +17168,7 @@
       <c r="AE141" s="72"/>
       <c r="AF141" s="71"/>
     </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A142" s="135" t="s">
         <v>2</v>
       </c>
@@ -17288,7 +17262,7 @@
       <c r="AE142" s="145"/>
       <c r="AF142" s="146"/>
     </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A143" s="135" t="s">
         <v>2</v>
       </c>
@@ -17382,7 +17356,7 @@
       <c r="AE143" s="26"/>
       <c r="AF143" s="59"/>
     </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A144" s="135" t="s">
         <v>2</v>
       </c>
@@ -17476,7 +17450,7 @@
       <c r="AE144" s="26"/>
       <c r="AF144" s="59"/>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A145" s="135" t="s">
         <v>2</v>
       </c>
@@ -17570,7 +17544,7 @@
       <c r="AE145" s="26"/>
       <c r="AF145" s="59"/>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A146" s="171" t="s">
         <v>2</v>
       </c>
@@ -17662,7 +17636,7 @@
       <c r="AE146" s="26"/>
       <c r="AF146" s="59"/>
     </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A147" s="171" t="s">
         <v>2</v>
       </c>
@@ -17754,7 +17728,7 @@
       <c r="AE147" s="26"/>
       <c r="AF147" s="146"/>
     </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A148" s="171" t="s">
         <v>2</v>
       </c>
@@ -17846,7 +17820,7 @@
       <c r="AE148" s="26"/>
       <c r="AF148" s="146"/>
     </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A149" s="171" t="s">
         <v>2</v>
       </c>
@@ -17938,42 +17912,100 @@
       <c r="AE149" s="26"/>
       <c r="AF149" s="146"/>
     </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A150" s="174"/>
-      <c r="B150" s="175"/>
-      <c r="C150" s="175"/>
-      <c r="D150" s="176"/>
-      <c r="E150" s="176"/>
-      <c r="F150" s="176"/>
-      <c r="G150" s="176"/>
-      <c r="H150" s="176"/>
-      <c r="I150" s="176"/>
-      <c r="J150" s="177"/>
-      <c r="K150" s="178"/>
-      <c r="L150" s="176"/>
-      <c r="M150" s="179"/>
-      <c r="N150" s="180"/>
-      <c r="O150" s="180"/>
-      <c r="P150" s="181"/>
-      <c r="Q150" s="180"/>
-      <c r="R150" s="179"/>
-      <c r="S150" s="179"/>
-      <c r="T150" s="182"/>
-      <c r="U150" s="181"/>
-      <c r="V150" s="181"/>
-      <c r="W150" s="181"/>
-      <c r="X150" s="183"/>
-      <c r="Y150" s="183"/>
-      <c r="Z150" s="183"/>
-      <c r="AA150" s="183"/>
-      <c r="AB150" s="184"/>
-      <c r="AC150" s="185"/>
-      <c r="AD150" s="185"/>
-      <c r="AE150" s="186"/>
-      <c r="AF150" s="187"/>
-    </row>
-    <row r="151" spans="1:32" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="152" spans="1:32" ht="24" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A150" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" s="49" t="s">
+        <v>530</v>
+      </c>
+      <c r="C150" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D150" s="61">
+        <v>40</v>
+      </c>
+      <c r="E150" s="76">
+        <v>6</v>
+      </c>
+      <c r="F150" s="76">
+        <v>1</v>
+      </c>
+      <c r="G150" s="76">
+        <v>5</v>
+      </c>
+      <c r="H150" s="76">
+        <v>0</v>
+      </c>
+      <c r="I150" s="76">
+        <v>0</v>
+      </c>
+      <c r="J150" s="172">
+        <v>0</v>
+      </c>
+      <c r="K150" s="173">
+        <v>0</v>
+      </c>
+      <c r="L150" s="76">
+        <v>0</v>
+      </c>
+      <c r="M150" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N150" s="47">
+        <v>5</v>
+      </c>
+      <c r="O150" s="47">
+        <v>5</v>
+      </c>
+      <c r="P150" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q150" s="47">
+        <v>0</v>
+      </c>
+      <c r="R150" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S150" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T150" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U150" s="46">
+        <v>1</v>
+      </c>
+      <c r="V150" s="46"/>
+      <c r="W150" s="46">
+        <v>0</v>
+      </c>
+      <c r="X150" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y150" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z150" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA150" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB150" s="45" t="s">
+        <v>518</v>
+      </c>
+      <c r="AC150" s="44" t="s">
+        <v>513</v>
+      </c>
+      <c r="AD150" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE150" s="26"/>
+      <c r="AF150" s="59"/>
+    </row>
+    <row r="151" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A152" s="9" t="s">
         <v>57</v>
       </c>
@@ -18005,14 +18037,14 @@
       <c r="AA152" s="9"/>
       <c r="AF152" s="8"/>
     </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A153" s="22"/>
       <c r="B153" s="22"/>
       <c r="C153" s="22"/>
       <c r="D153" s="22"/>
       <c r="E153" s="22"/>
-      <c r="F153" s="189"/>
-      <c r="G153" s="189"/>
+      <c r="F153" s="175"/>
+      <c r="G153" s="175"/>
       <c r="H153" s="21" t="s">
         <v>56</v>
       </c>
@@ -18042,7 +18074,7 @@
       <c r="AD153" s="21"/>
       <c r="AE153" s="17"/>
     </row>
-    <row r="154" spans="1:32" ht="144" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>54</v>
       </c>
@@ -18089,7 +18121,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
         <v>2</v>
       </c>
@@ -18138,7 +18170,7 @@
       <c r="P155" s="17"/>
       <c r="Q155" s="17"/>
     </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A156" s="16" t="s">
         <v>2</v>
       </c>
@@ -18187,7 +18219,7 @@
       <c r="P156" s="17"/>
       <c r="Q156" s="17"/>
     </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A157" s="16" t="s">
         <v>2</v>
       </c>
@@ -18236,7 +18268,7 @@
       <c r="P157" s="17"/>
       <c r="Q157" s="17"/>
     </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A158" s="16" t="s">
         <v>2</v>
       </c>
@@ -18285,7 +18317,7 @@
       <c r="P158" s="17"/>
       <c r="Q158" s="17"/>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A159" s="16" t="s">
         <v>2</v>
       </c>
@@ -18334,7 +18366,7 @@
       <c r="P159" s="17"/>
       <c r="Q159" s="17"/>
     </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A160" s="16" t="s">
         <v>2</v>
       </c>
@@ -18383,7 +18415,7 @@
       <c r="P160" s="17"/>
       <c r="Q160" s="17"/>
     </row>
-    <row r="161" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A161" s="16" t="s">
         <v>2</v>
       </c>
@@ -18432,7 +18464,7 @@
       <c r="P161" s="17"/>
       <c r="Q161" s="17"/>
     </row>
-    <row r="162" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A162" s="16" t="s">
         <v>2</v>
       </c>
@@ -18481,7 +18513,7 @@
       <c r="P162" s="17"/>
       <c r="Q162" s="17"/>
     </row>
-    <row r="163" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A163" s="16" t="s">
         <v>2</v>
       </c>
@@ -18530,7 +18562,7 @@
       <c r="P163" s="17"/>
       <c r="Q163" s="17"/>
     </row>
-    <row r="164" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A164" s="16" t="s">
         <v>2</v>
       </c>
@@ -18579,7 +18611,7 @@
       <c r="P164" s="17"/>
       <c r="Q164" s="17"/>
     </row>
-    <row r="165" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A165" s="16" t="s">
         <v>2</v>
       </c>
@@ -18626,7 +18658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A166" s="16" t="s">
         <v>2</v>
       </c>
@@ -18689,7 +18721,7 @@
       <c r="AD166" s="8"/>
       <c r="AE166" s="8"/>
     </row>
-    <row r="167" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N167" s="8"/>
       <c r="O167" s="8"/>
       <c r="P167" s="8"/>
@@ -18709,8 +18741,8 @@
       <c r="AD167" s="8"/>
       <c r="AE167" s="8"/>
     </row>
-    <row r="168" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="1:31" ht="24" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="169" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A169" s="9" t="s">
         <v>19</v>
       </c>
@@ -18726,7 +18758,7 @@
       <c r="K169" s="8"/>
       <c r="L169" s="8"/>
     </row>
-    <row r="171" spans="1:31" ht="156" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>18</v>
       </c>
@@ -18752,7 +18784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>2</v>
       </c>
@@ -18778,7 +18810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>2</v>
       </c>
@@ -18804,7 +18836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>2</v>
       </c>
@@ -18830,7 +18862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>2</v>
       </c>
@@ -18856,7 +18888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>2</v>
       </c>
@@ -18882,7 +18914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D179" s="1">
         <v>42</v>
       </c>
@@ -18898,7 +18930,7 @@
         <v>54.6</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D180" s="1">
         <v>92</v>
       </c>
@@ -18914,7 +18946,7 @@
         <v>101.2</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D181" s="1">
         <v>235</v>
       </c>
@@ -18930,7 +18962,7 @@
         <v>211.5</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D182" s="1">
         <v>686</v>
       </c>
@@ -18946,7 +18978,7 @@
         <v>480.2</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D183" s="1">
         <v>1040</v>
       </c>
@@ -18962,8 +18994,8 @@
         <v>520</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="186" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="186" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A186" s="9" t="s">
         <v>525</v>
       </c>
@@ -18974,12 +19006,12 @@
       <c r="F186" s="9"/>
       <c r="G186" s="9"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A187" s="188"/>
-      <c r="B187" s="188"/>
-      <c r="C187" s="188"/>
-    </row>
-    <row r="188" spans="1:9" ht="110" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187" s="174"/>
+      <c r="B187" s="174"/>
+      <c r="C187" s="174"/>
+    </row>
+    <row r="188" spans="1:9" ht="113.25" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
         <v>526</v>
       </c>
@@ -18993,7 +19025,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="16" t="s">
         <v>2</v>
       </c>
@@ -19013,18 +19045,18 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="F153:G153"/>
   </mergeCells>
-  <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M150 R143:T150">
-    <cfRule type="expression" dxfId="118" priority="78">
+  <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M149 R143:T149">
+    <cfRule type="expression" dxfId="120" priority="80">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="117" priority="71">
+    <cfRule type="expression" dxfId="119" priority="73">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N117:Q117">
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19036,11 +19068,40 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:M120 R116:T120">
-    <cfRule type="expression" dxfId="116" priority="65">
+    <cfRule type="expression" dxfId="118" priority="67">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116:Q120">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N119:Q125 N24:Q56 N58:Q104 N106:Q116">
+    <cfRule type="colorScale" priority="85">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M115 R115:T115">
+    <cfRule type="expression" dxfId="117" priority="65">
+      <formula>M115=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N115:Q115">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -19052,47 +19113,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N119:Q125 N24:Q56 N58:Q104 N106:Q116">
-    <cfRule type="colorScale" priority="83">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M115 R115:T115">
-    <cfRule type="expression" dxfId="115" priority="63">
-      <formula>M115=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N115:Q115">
-    <cfRule type="colorScale" priority="62">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M126:M127 R126:T127">
-    <cfRule type="expression" dxfId="114" priority="60">
+    <cfRule type="expression" dxfId="116" priority="62">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126 R126:T126">
-    <cfRule type="expression" dxfId="113" priority="59">
+    <cfRule type="expression" dxfId="115" priority="61">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N126:Q126">
-    <cfRule type="colorScale" priority="58">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19104,7 +19136,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N126:Q128">
-    <cfRule type="colorScale" priority="61">
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19116,17 +19148,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="112" priority="57">
+    <cfRule type="expression" dxfId="114" priority="59">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S129:T129 M129">
-    <cfRule type="expression" dxfId="111" priority="56">
+    <cfRule type="expression" dxfId="113" priority="58">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N129:Q129">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19138,22 +19170,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R129">
-    <cfRule type="expression" dxfId="110" priority="54">
+    <cfRule type="expression" dxfId="112" priority="56">
       <formula>R129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="109" priority="39">
+    <cfRule type="expression" dxfId="111" priority="41">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="108" priority="41">
+    <cfRule type="expression" dxfId="110" priority="43">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:Q134">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19165,17 +19197,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="107" priority="34">
+    <cfRule type="expression" dxfId="109" priority="36">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M133 R130:T133">
-    <cfRule type="expression" dxfId="106" priority="35">
+    <cfRule type="expression" dxfId="108" priority="37">
       <formula>M130=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N130:Q133">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19187,7 +19219,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N135:Q135">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19199,17 +19231,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="105" priority="32">
+    <cfRule type="expression" dxfId="107" priority="34">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="104" priority="27">
+    <cfRule type="expression" dxfId="106" priority="29">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N136:Q136">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19221,16 +19253,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="103" priority="29">
+    <cfRule type="expression" dxfId="105" priority="31">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R137">
-    <cfRule type="expression" dxfId="102" priority="22">
+    <cfRule type="expression" dxfId="104" priority="24">
       <formula>R137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N137:Q137">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S137:T137 M137">
+    <cfRule type="expression" dxfId="103" priority="26">
+      <formula>M137=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M139 R139:T139">
+    <cfRule type="expression" dxfId="102" priority="22">
+      <formula>M139=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N139:Q139">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -19242,17 +19296,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S137:T137 M137">
-    <cfRule type="expression" dxfId="101" priority="24">
-      <formula>M137=FALSE</formula>
+  <conditionalFormatting sqref="M57 R57:T57">
+    <cfRule type="expression" dxfId="101" priority="20">
+      <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="100" priority="20">
-      <formula>M139=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N139:Q139">
+  <conditionalFormatting sqref="N57:Q57">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -19264,12 +19313,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="99" priority="18">
-      <formula>M57=FALSE</formula>
+  <conditionalFormatting sqref="M138 R138:T138">
+    <cfRule type="expression" dxfId="100" priority="18">
+      <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57:Q57">
+  <conditionalFormatting sqref="N138:Q138">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -19281,12 +19330,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="98" priority="16">
-      <formula>M138=FALSE</formula>
+  <conditionalFormatting sqref="M140 R140:T140">
+    <cfRule type="expression" dxfId="99" priority="16">
+      <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N138:Q138">
+  <conditionalFormatting sqref="N140:Q140">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -19298,30 +19347,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="97" priority="14">
-      <formula>M140=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N140:Q140">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="96" priority="10">
+    <cfRule type="expression" dxfId="98" priority="12">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N141:Q141">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19333,11 +19365,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R142">
-    <cfRule type="expression" dxfId="95" priority="5">
+    <cfRule type="expression" dxfId="97" priority="7">
       <formula>R142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N142:Q142">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S142:T142 M142">
+    <cfRule type="expression" dxfId="96" priority="9">
+      <formula>M142=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R105:T105 M105">
+    <cfRule type="expression" dxfId="95" priority="5">
+      <formula>M105=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N105:Q105">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -19349,18 +19403,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S142:T142 M142">
-    <cfRule type="expression" dxfId="94" priority="7">
-      <formula>M142=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R105:T105 M105">
-    <cfRule type="expression" dxfId="93" priority="3">
-      <formula>M105=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N105:Q105">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="N143:Q149">
+    <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19371,8 +19415,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N143:Q150">
-    <cfRule type="colorScale" priority="104">
+  <conditionalFormatting sqref="M150 R150:T150">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>M150=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N150:Q150">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19384,37 +19433,37 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G135" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 G136:G150 H40:I150 J141:J150" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G41 G135"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G40 G24:I39 G42:G134 J24:J139 H40:I150 J141:J150 G136:G150">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="D155:G166 P140:V140 M140:N140 N24:O139 Q24:W139 Q141:W150 N141:O150" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="decimal" allowBlank="1" sqref="D155:G166 P140:V140 M140:N140 N24:O139 Q24:W139 N141:O150 Q141:W150">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H155:L164 H165:I165 J166:L166 W140:Z140 X24:AA139 X141:AA150" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="probability [0..1]" sqref="H155:L164 H165:I165 J166:L166 W140:Z140 X24:AA139 X141:AA150">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C155:C166 C24:C150" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C155:C166 C24:C150">
       <formula1>INDIRECT("entityCategoryDefinitions['[sku']]")</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J165:L165 M155:O166 AA140:AC140 AB131:AB142 AC131:AC139 AC141:AC142 AB24:AC130 AD24:AF142 AB143:AF150" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation type="list" sqref="O140 P24:P139 P141:P150" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="J165:L165 M155:O166 AA140:AC140 AB131:AB142 AC131:AC139 AC141:AC142 AB24:AC130 AD24:AF142 AB143:AF150"/>
+    <dataValidation type="list" sqref="O140 P24:P139 P141:P150">
       <formula1>INDIRECT("dragonTierDefinitions['[order']]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L150" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="K24:L139 K140 K141:L150">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="L140 M24:M139 M141:M150" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" sqref="L140 M24:M139 M141:M150">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J140" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" prompt="probability [0..1]" sqref="J140">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F150" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D24:F150">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -19429,7 +19478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -19439,20 +19488,20 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" customWidth="1"/>
     <col min="9" max="28" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>426</v>
       </c>
@@ -19466,19 +19515,19 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="98"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="189"/>
-      <c r="G3" s="189"/>
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
       <c r="H3" s="22"/>
       <c r="I3" s="21"/>
       <c r="J3" s="97"/>
       <c r="K3" s="97"/>
     </row>
-    <row r="4" spans="2:11" ht="132" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>425</v>
       </c>
@@ -19501,7 +19550,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="116" t="s">
         <v>2</v>
       </c>
@@ -19522,7 +19571,7 @@
       </c>
       <c r="H5" s="113"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="116" t="s">
         <v>2</v>
       </c>
@@ -19543,7 +19592,7 @@
       </c>
       <c r="H6" s="113"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="112" t="s">
         <v>411</v>
       </c>
@@ -19556,7 +19605,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="112" t="s">
         <v>411</v>
       </c>
@@ -19569,7 +19618,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="112" t="s">
         <v>411</v>
       </c>
@@ -19582,7 +19631,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="116" t="s">
         <v>2</v>
       </c>
@@ -19603,7 +19652,7 @@
       </c>
       <c r="H10" s="113"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="112" t="s">
         <v>411</v>
       </c>
@@ -19616,7 +19665,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="112" t="s">
         <v>411</v>
       </c>
@@ -19629,7 +19678,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="112" t="s">
         <v>411</v>
       </c>
@@ -19642,7 +19691,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="116" t="s">
         <v>2</v>
       </c>
@@ -19663,7 +19712,7 @@
       </c>
       <c r="H14" s="113"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="112" t="s">
         <v>411</v>
       </c>
@@ -19676,7 +19725,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="112" t="s">
         <v>411</v>
       </c>
@@ -19689,7 +19738,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="112" t="s">
         <v>411</v>
       </c>
@@ -19702,7 +19751,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="116" t="s">
         <v>2</v>
       </c>
@@ -19723,7 +19772,7 @@
       </c>
       <c r="H18" s="113"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="112" t="s">
         <v>411</v>
       </c>
@@ -19736,7 +19785,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="112" t="s">
         <v>411</v>
       </c>
@@ -19749,7 +19798,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="112" t="s">
         <v>411</v>
       </c>
@@ -19762,7 +19811,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="112" t="s">
         <v>2</v>
       </c>
@@ -19783,7 +19832,7 @@
       </c>
       <c r="H22" s="109"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="112" t="s">
         <v>411</v>
       </c>
@@ -19796,7 +19845,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="112" t="s">
         <v>2</v>
       </c>
@@ -19817,7 +19866,7 @@
       </c>
       <c r="H24" s="109"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="112" t="s">
         <v>411</v>
       </c>
@@ -19830,7 +19879,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="112" t="s">
         <v>2</v>
       </c>
@@ -19851,7 +19900,7 @@
       </c>
       <c r="H26" s="109"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="112" t="s">
         <v>411</v>
       </c>
@@ -19864,7 +19913,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="112" t="s">
         <v>2</v>
       </c>
@@ -19885,7 +19934,7 @@
       </c>
       <c r="H28" s="109"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="112" t="s">
         <v>411</v>
       </c>
@@ -19898,8 +19947,8 @@
         <v>465</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B33" s="9" t="s">
         <v>410</v>
       </c>
@@ -19910,7 +19959,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="35" spans="2:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="129.75" x14ac:dyDescent="0.25">
       <c r="B35" s="108" t="s">
         <v>409</v>
       </c>
@@ -19924,7 +19973,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="106" t="s">
         <v>2</v>
       </c>
@@ -19938,7 +19987,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="106" t="s">
         <v>2</v>
       </c>
@@ -19952,7 +20001,7 @@
         <v>8.7055056329612412E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="106" t="s">
         <v>2</v>
       </c>
@@ -19966,7 +20015,7 @@
         <v>8.027415617602307E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="106" t="s">
         <v>2</v>
       </c>
@@ -19980,7 +20029,7 @@
         <v>7.5785828325519916E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="106" t="s">
         <v>2</v>
       </c>
@@ -19994,7 +20043,7 @@
         <v>7.2477966367769556E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="106" t="s">
         <v>2</v>
       </c>
@@ -20008,7 +20057,7 @@
         <v>6.988271187715793E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="106" t="s">
         <v>2</v>
       </c>
@@ -20022,7 +20071,7 @@
         <v>6.776109134004811E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="106" t="s">
         <v>2</v>
       </c>
@@ -20036,7 +20085,7 @@
         <v>6.5975395538644718E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="106" t="s">
         <v>2</v>
       </c>
@@ -20050,7 +20099,7 @@
         <v>6.4439401497725424E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="106" t="s">
         <v>2</v>
       </c>
@@ -20064,8 +20113,8 @@
         <v>6.3095734448019331E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B47" s="9" t="s">
         <v>396</v>
       </c>
@@ -20076,7 +20125,7 @@
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
     </row>
-    <row r="49" spans="2:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="130.5" x14ac:dyDescent="0.25">
       <c r="B49" s="103" t="s">
         <v>395</v>
       </c>
@@ -20099,7 +20148,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="101" t="s">
         <v>2</v>
       </c>
@@ -20127,8 +20176,8 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="H5:H29" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" sqref="E36:F45 E5:G29" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="H5:H29"/>
+    <dataValidation allowBlank="1" sqref="E36:F45 E5:G29"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
Increased Rings score reward from 10 to 50
Former-commit-id: 58d0814e9d25ff6bfc6a461df3cbb33bd52cc238
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -2688,188 +2688,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="119">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5165,6 +4983,188 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5179,58 +5179,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="118" dataDxfId="116" headerRowBorderDxfId="117" tableBorderDxfId="115" totalsRowBorderDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A23:AF149"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="113"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="112"/>
-    <tableColumn id="6" name="[category]" dataDxfId="111"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="110"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="109"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="108"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="107"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="106"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="105"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="104"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="103"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="102"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="101"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="100"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="99"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="98"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="97"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="96"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="95"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="94"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="93"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="92"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="91"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="90"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="89"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="88"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="87"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="86"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="85"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="84"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="83"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="82"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
+    <tableColumn id="6" name="[category]" dataDxfId="85"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="77"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="76"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5243,50 +5243,50 @@
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="4" name="[category]" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="16" name="[size]" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="6" name="[order]" dataDxfId="39"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="38"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="37"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="36"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="35"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="6" name="[order]" dataDxfId="13"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="29"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="28"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="27"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5563,7 +5563,7 @@
     <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="D148" sqref="D148"/>
+      <selection pane="topRight" activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16343,7 +16343,7 @@
         <v>61</v>
       </c>
       <c r="D133" s="66">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E133" s="65">
         <v>1</v>
@@ -18945,12 +18945,12 @@
     <mergeCell ref="F153:G153"/>
   </mergeCells>
   <conditionalFormatting sqref="M119:M125 R119:T125 M24:M56 R24:T56 S128:T128 M128 R58:T104 M58:M104 M106:M116 R106:T116 M143:M150 R143:T150">
-    <cfRule type="expression" dxfId="25" priority="78">
+    <cfRule type="expression" dxfId="118" priority="78">
       <formula>M24=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117 R117:T117">
-    <cfRule type="expression" dxfId="24" priority="71">
+    <cfRule type="expression" dxfId="117" priority="71">
       <formula>M117=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18967,7 +18967,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M116:M120 R116:T120">
-    <cfRule type="expression" dxfId="23" priority="65">
+    <cfRule type="expression" dxfId="116" priority="65">
       <formula>M116=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18996,7 +18996,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115 R115:T115">
-    <cfRule type="expression" dxfId="22" priority="63">
+    <cfRule type="expression" dxfId="115" priority="63">
       <formula>M115=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19013,12 +19013,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126:M127 R126:T127">
-    <cfRule type="expression" dxfId="21" priority="60">
+    <cfRule type="expression" dxfId="114" priority="60">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M126 R126:T126">
-    <cfRule type="expression" dxfId="20" priority="59">
+    <cfRule type="expression" dxfId="113" priority="59">
       <formula>M126=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19047,12 +19047,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R128">
-    <cfRule type="expression" dxfId="19" priority="57">
+    <cfRule type="expression" dxfId="112" priority="57">
       <formula>R128=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S129:T129 M129">
-    <cfRule type="expression" dxfId="18" priority="56">
+    <cfRule type="expression" dxfId="111" priority="56">
       <formula>M129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19069,17 +19069,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R129">
-    <cfRule type="expression" dxfId="17" priority="54">
+    <cfRule type="expression" dxfId="110" priority="54">
       <formula>R129=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R134">
-    <cfRule type="expression" dxfId="16" priority="39">
+    <cfRule type="expression" dxfId="109" priority="39">
       <formula>R134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S134:T134 M134">
-    <cfRule type="expression" dxfId="15" priority="41">
+    <cfRule type="expression" dxfId="108" priority="41">
       <formula>M134=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19096,12 +19096,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:T135 M135">
-    <cfRule type="expression" dxfId="14" priority="34">
+    <cfRule type="expression" dxfId="107" priority="34">
       <formula>M135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M133 R130:T133">
-    <cfRule type="expression" dxfId="13" priority="35">
+    <cfRule type="expression" dxfId="106" priority="35">
       <formula>M130=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19130,12 +19130,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R135">
-    <cfRule type="expression" dxfId="12" priority="32">
+    <cfRule type="expression" dxfId="105" priority="32">
       <formula>R135=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R136">
-    <cfRule type="expression" dxfId="11" priority="27">
+    <cfRule type="expression" dxfId="104" priority="27">
       <formula>R136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19152,12 +19152,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:T136 M136">
-    <cfRule type="expression" dxfId="10" priority="29">
+    <cfRule type="expression" dxfId="103" priority="29">
       <formula>M136=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R137">
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="102" priority="22">
       <formula>R137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19174,12 +19174,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S137:T137 M137">
-    <cfRule type="expression" dxfId="8" priority="24">
+    <cfRule type="expression" dxfId="101" priority="24">
       <formula>M137=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M139 R139:T139">
-    <cfRule type="expression" dxfId="7" priority="20">
+    <cfRule type="expression" dxfId="100" priority="20">
       <formula>M139=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19196,7 +19196,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57 R57:T57">
-    <cfRule type="expression" dxfId="6" priority="18">
+    <cfRule type="expression" dxfId="99" priority="18">
       <formula>M57=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19213,7 +19213,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138 R138:T138">
-    <cfRule type="expression" dxfId="5" priority="16">
+    <cfRule type="expression" dxfId="98" priority="16">
       <formula>M138=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19230,7 +19230,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M140 R140:T140">
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="97" priority="14">
       <formula>M140=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19247,7 +19247,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M141 R141:T141">
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="96" priority="10">
       <formula>M141=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19264,7 +19264,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R142">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="95" priority="5">
       <formula>R142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19281,12 +19281,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S142:T142 M142">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="94" priority="7">
       <formula>M142=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105:T105 M105">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="93" priority="3">
       <formula>M105=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added the st patricks collectable to the excel
Former-commit-id: 9dd04e44134cf396d9ec1c0da428134a5a3c4c93
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Gameplay.xlsx
+++ b/Docs/Content/HungryDragonContent_Gameplay.xlsx
@@ -16,7 +16,7 @@
     <sheet name="score" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$154:$O$155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entities!$A$155:$O$156</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="529">
   <si>
     <t>tier_4</t>
   </si>
@@ -1616,6 +1616,18 @@
   </si>
   <si>
     <t>valentines_heart</t>
+  </si>
+  <si>
+    <t>st_patrick</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_KILL_ENT_PATRICK_01;TID_QUIP_DRG_KILL_ENT_PATRICK_02;TID_QUIP_DRG_KILL_ENT_PATRICK_03</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SEASON_ST_PATRICKS_BALLOON</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_BURN_ENT_05;TID_QUIP_DRG_BURN_ENT_06</t>
   </si>
 </sst>
 </file>
@@ -1872,7 +1884,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -2181,12 +2193,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2682,12 +2709,218 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="119">
+  <dxfs count="122">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4983,188 +5216,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5179,114 +5230,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="entityDefinitions" displayName="entityDefinitions" ref="A23:AF149" totalsRowShown="0" headerRowDxfId="121" dataDxfId="119" headerRowBorderDxfId="120" tableBorderDxfId="118" totalsRowBorderDxfId="117">
   <autoFilter ref="A23:AF149"/>
   <sortState ref="A24:AF134">
     <sortCondition ref="B23:B134"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="87"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="86"/>
-    <tableColumn id="6" name="[category]" dataDxfId="85"/>
-    <tableColumn id="10" name="[rewardScore]" dataDxfId="84"/>
-    <tableColumn id="11" name="[rewardCoins]" dataDxfId="83"/>
-    <tableColumn id="12" name="[rewardPC]" dataDxfId="82"/>
-    <tableColumn id="13" name="[rewardHealth]" dataDxfId="81"/>
-    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="80"/>
-    <tableColumn id="16" name="[rewardXp]" dataDxfId="79"/>
-    <tableColumn id="26" name="[rewardFury]" dataDxfId="78"/>
-    <tableColumn id="17" name="[goldenChance]" dataDxfId="77"/>
-    <tableColumn id="18" name="[pcChance]" dataDxfId="76"/>
-    <tableColumn id="3" name="[isEdible]" dataDxfId="75"/>
-    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="74"/>
-    <tableColumn id="31" name="[grabFromTier]" dataDxfId="73"/>
-    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="72"/>
-    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="71"/>
-    <tableColumn id="35" name="[isBurnable]" dataDxfId="70"/>
-    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="69"/>
-    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="68"/>
-    <tableColumn id="28" name="[maxHealth]" dataDxfId="67"/>
-    <tableColumn id="5" name="[biteResistance]" dataDxfId="66"/>
-    <tableColumn id="8" name="[alcohol]" dataDxfId="65"/>
-    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="64"/>
-    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="63"/>
-    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="62"/>
-    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="61"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="60"/>
-    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="59"/>
-    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="58"/>
-    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="57"/>
-    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="56"/>
+    <tableColumn id="1" name="{entityDefinitions}" dataDxfId="116"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="115"/>
+    <tableColumn id="6" name="[category]" dataDxfId="114"/>
+    <tableColumn id="10" name="[rewardScore]" dataDxfId="113"/>
+    <tableColumn id="11" name="[rewardCoins]" dataDxfId="112"/>
+    <tableColumn id="12" name="[rewardPC]" dataDxfId="111"/>
+    <tableColumn id="13" name="[rewardHealth]" dataDxfId="110"/>
+    <tableColumn id="14" name="[rewardEnergy]" dataDxfId="109"/>
+    <tableColumn id="16" name="[rewardXp]" dataDxfId="108"/>
+    <tableColumn id="26" name="[rewardFury]" dataDxfId="107"/>
+    <tableColumn id="17" name="[goldenChance]" dataDxfId="106"/>
+    <tableColumn id="18" name="[pcChance]" dataDxfId="105"/>
+    <tableColumn id="3" name="[isEdible]" dataDxfId="104"/>
+    <tableColumn id="15" name="[latchOnFromTier]" dataDxfId="103"/>
+    <tableColumn id="31" name="[grabFromTier]" dataDxfId="102"/>
+    <tableColumn id="4" name="[edibleFromTier]" dataDxfId="101"/>
+    <tableColumn id="34" name="[burnableFromTier]" dataDxfId="100"/>
+    <tableColumn id="35" name="[isBurnable]" dataDxfId="99"/>
+    <tableColumn id="30" name="[canBeGrabed]" dataDxfId="98"/>
+    <tableColumn id="29" name="[canBeLatchedOn]" dataDxfId="97"/>
+    <tableColumn id="28" name="[maxHealth]" dataDxfId="96"/>
+    <tableColumn id="5" name="[biteResistance]" dataDxfId="95"/>
+    <tableColumn id="8" name="[alcohol]" dataDxfId="94"/>
+    <tableColumn id="19" name="[eatFeedbackChance]" dataDxfId="93"/>
+    <tableColumn id="20" name="[burnFeedbackChance]" dataDxfId="92"/>
+    <tableColumn id="21" name="[damageFeedbackChance]" dataDxfId="91"/>
+    <tableColumn id="22" name="[deathFeedbackChance]" dataDxfId="90"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="89"/>
+    <tableColumn id="9" name="[tidEatFeedback]" dataDxfId="88"/>
+    <tableColumn id="23" name="[tidBurnFeedback]" dataDxfId="87"/>
+    <tableColumn id="24" name="[tidDamageFeedback]" dataDxfId="86"/>
+    <tableColumn id="25" name="[tidDeathFeedback]" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="entityCategoryDefinitions" displayName="entityCategoryDefinitions" ref="A4:B18" totalsRowShown="0" headerRowDxfId="84" headerRowBorderDxfId="83" tableBorderDxfId="82" totalsRowBorderDxfId="81">
   <autoFilter ref="A4:B18"/>
   <sortState ref="A5:B14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="1" name="{entityCategoryDefinitions}" dataDxfId="80"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A154:O166" totalsRowShown="0">
-  <autoFilter ref="A154:O166"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table4" displayName="Table4" ref="A155:O167" totalsRowShown="0">
+  <autoFilter ref="A155:O167"/>
   <sortState ref="A51:L77">
     <sortCondition ref="C50:C77"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" name="[category]" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="16" name="[size]" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="18" name="[minTierBurn]" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" name="[rewardScore]" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="31" name="[tidName]" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" name="{decorationDefinitions}" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="4" name="[category]" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="16" name="[size]" dataDxfId="72" totalsRowDxfId="71"/>
+    <tableColumn id="5" name="[minTierDisintegrate]" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="17" name="[minTierBurnFeedback]" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="18" name="[minTierBurn]" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="28" name="[burnFeedbackChance]" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="30" name="[destroyFeedbackChance]" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="11" name="[minTierDestruction]" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="10" name="[minTierDestructionFeedback]" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="6" name="[rewardScore]" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="31" name="[tidName]" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="33" name="[tidBurnFeedback]" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="34" name="[tidDestroyFeedback]" dataDxfId="50" totalsRowDxfId="49"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="scoreMultiplierDefinitions" displayName="scoreMultiplierDefinitions" ref="B4:H29" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="B4:H29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="6" name="[order]" dataDxfId="13"/>
-    <tableColumn id="3" name="[multiplier]" dataDxfId="12"/>
-    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="11"/>
-    <tableColumn id="5" name="[duration]" dataDxfId="10"/>
-    <tableColumn id="7" name="[tidMessage]" dataDxfId="9"/>
+    <tableColumn id="1" name="{scoreMultiplierDefinitions}" dataDxfId="44"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
+    <tableColumn id="6" name="[order]" dataDxfId="42"/>
+    <tableColumn id="3" name="[multiplier]" dataDxfId="41"/>
+    <tableColumn id="4" name="[requiredKillStreak]" dataDxfId="40"/>
+    <tableColumn id="5" name="[duration]" dataDxfId="39"/>
+    <tableColumn id="7" name="[tidMessage]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="scoreMultiplierDefinitions1928" displayName="scoreMultiplierDefinitions1928" ref="B35:E45" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B35:E45"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="3"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="2"/>
-    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="1"/>
-    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="{survivalBonusDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="5" name="[survivedMinutes]" dataDxfId="30"/>
+    <tableColumn id="6" name="[bonusPerMinute]" dataDxfId="29" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5558,12 +5609,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF183"/>
+  <dimension ref="A1:AF184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AD1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="D133" sqref="D133"/>
+      <selection pane="topRight" activeCell="AE150" sqref="AE150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17915,217 +17966,260 @@
       <c r="AF149" s="146"/>
     </row>
     <row r="150" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A150" s="174"/>
-      <c r="B150" s="175"/>
-      <c r="C150" s="175"/>
-      <c r="D150" s="176"/>
-      <c r="E150" s="176"/>
-      <c r="F150" s="176"/>
-      <c r="G150" s="176"/>
-      <c r="H150" s="176"/>
-      <c r="I150" s="176"/>
-      <c r="J150" s="177"/>
-      <c r="K150" s="178"/>
-      <c r="L150" s="176"/>
-      <c r="M150" s="179"/>
-      <c r="N150" s="180"/>
-      <c r="O150" s="180"/>
-      <c r="P150" s="181"/>
-      <c r="Q150" s="180"/>
-      <c r="R150" s="179"/>
-      <c r="S150" s="179"/>
-      <c r="T150" s="182"/>
-      <c r="U150" s="181"/>
-      <c r="V150" s="181"/>
-      <c r="W150" s="181"/>
-      <c r="X150" s="183"/>
-      <c r="Y150" s="183"/>
-      <c r="Z150" s="183"/>
-      <c r="AA150" s="183"/>
-      <c r="AB150" s="184"/>
-      <c r="AC150" s="185"/>
-      <c r="AD150" s="185"/>
-      <c r="AE150" s="186"/>
-      <c r="AF150" s="187"/>
-    </row>
-    <row r="151" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="152" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A152" s="9" t="s">
+      <c r="A150" s="171" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" s="49" t="s">
+        <v>525</v>
+      </c>
+      <c r="C150" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D150" s="61">
+        <v>40</v>
+      </c>
+      <c r="E150" s="76">
+        <v>6</v>
+      </c>
+      <c r="F150" s="76">
+        <v>1</v>
+      </c>
+      <c r="G150" s="76">
+        <v>5</v>
+      </c>
+      <c r="H150" s="76">
+        <v>0</v>
+      </c>
+      <c r="I150" s="76">
+        <v>0</v>
+      </c>
+      <c r="J150" s="172">
+        <v>0</v>
+      </c>
+      <c r="K150" s="173">
+        <v>0</v>
+      </c>
+      <c r="L150" s="76">
+        <v>0</v>
+      </c>
+      <c r="M150" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N150" s="47">
+        <v>5</v>
+      </c>
+      <c r="O150" s="47">
+        <v>5</v>
+      </c>
+      <c r="P150" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q150" s="47">
+        <v>0</v>
+      </c>
+      <c r="R150" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="S150" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T150" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U150" s="46">
+        <v>1</v>
+      </c>
+      <c r="V150" s="46"/>
+      <c r="W150" s="46">
+        <v>0</v>
+      </c>
+      <c r="X150" s="55">
+        <v>0</v>
+      </c>
+      <c r="Y150" s="55">
+        <v>0</v>
+      </c>
+      <c r="Z150" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA150" s="55">
+        <v>0</v>
+      </c>
+      <c r="AB150" s="45" t="s">
+        <v>527</v>
+      </c>
+      <c r="AC150" s="189" t="s">
+        <v>526</v>
+      </c>
+      <c r="AD150" s="44" t="s">
+        <v>528</v>
+      </c>
+      <c r="AE150" s="26"/>
+      <c r="AF150" s="59"/>
+    </row>
+    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A151" s="174"/>
+      <c r="B151" s="175"/>
+      <c r="C151" s="175"/>
+      <c r="D151" s="176"/>
+      <c r="E151" s="176"/>
+      <c r="F151" s="176"/>
+      <c r="G151" s="176"/>
+      <c r="H151" s="176"/>
+      <c r="I151" s="176"/>
+      <c r="J151" s="177"/>
+      <c r="K151" s="178"/>
+      <c r="L151" s="176"/>
+      <c r="M151" s="179"/>
+      <c r="N151" s="180"/>
+      <c r="O151" s="180"/>
+      <c r="P151" s="181"/>
+      <c r="Q151" s="180"/>
+      <c r="R151" s="179"/>
+      <c r="S151" s="179"/>
+      <c r="T151" s="182"/>
+      <c r="U151" s="181"/>
+      <c r="V151" s="181"/>
+      <c r="W151" s="181"/>
+      <c r="X151" s="183"/>
+      <c r="Y151" s="183"/>
+      <c r="Z151" s="183"/>
+      <c r="AA151" s="183"/>
+      <c r="AB151" s="184"/>
+      <c r="AC151" s="185"/>
+      <c r="AD151" s="185"/>
+      <c r="AE151" s="186"/>
+      <c r="AF151" s="187"/>
+    </row>
+    <row r="152" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="153" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A153" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B152" s="9"/>
-      <c r="C152" s="9"/>
-      <c r="D152" s="9"/>
-      <c r="E152" s="9"/>
-      <c r="F152" s="9"/>
-      <c r="G152" s="9"/>
-      <c r="H152" s="9"/>
-      <c r="I152" s="9"/>
-      <c r="J152" s="9"/>
-      <c r="K152" s="9"/>
-      <c r="L152" s="9"/>
-      <c r="M152" s="9"/>
-      <c r="N152" s="9"/>
-      <c r="O152" s="9"/>
-      <c r="P152" s="9"/>
-      <c r="Q152" s="9"/>
-      <c r="R152" s="9"/>
-      <c r="S152" s="9"/>
-      <c r="T152" s="9"/>
-      <c r="U152" s="9"/>
-      <c r="V152" s="9"/>
-      <c r="W152" s="9"/>
-      <c r="X152" s="9"/>
-      <c r="Y152" s="9"/>
-      <c r="Z152" s="9"/>
-      <c r="AA152" s="9"/>
-      <c r="AF152" s="8"/>
-    </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A153" s="22"/>
-      <c r="B153" s="22"/>
-      <c r="C153" s="22"/>
-      <c r="D153" s="22"/>
-      <c r="E153" s="22"/>
-      <c r="F153" s="188"/>
-      <c r="G153" s="188"/>
-      <c r="H153" s="21" t="s">
+      <c r="B153" s="9"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
+      <c r="K153" s="9"/>
+      <c r="L153" s="9"/>
+      <c r="M153" s="9"/>
+      <c r="N153" s="9"/>
+      <c r="O153" s="9"/>
+      <c r="P153" s="9"/>
+      <c r="Q153" s="9"/>
+      <c r="R153" s="9"/>
+      <c r="S153" s="9"/>
+      <c r="T153" s="9"/>
+      <c r="U153" s="9"/>
+      <c r="V153" s="9"/>
+      <c r="W153" s="9"/>
+      <c r="X153" s="9"/>
+      <c r="Y153" s="9"/>
+      <c r="Z153" s="9"/>
+      <c r="AA153" s="9"/>
+      <c r="AF153" s="8"/>
+    </row>
+    <row r="154" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A154" s="22"/>
+      <c r="B154" s="22"/>
+      <c r="C154" s="22"/>
+      <c r="D154" s="22"/>
+      <c r="E154" s="22"/>
+      <c r="F154" s="188"/>
+      <c r="G154" s="188"/>
+      <c r="H154" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I153" s="21"/>
-      <c r="J153" s="22"/>
-      <c r="K153" s="17"/>
-      <c r="L153" s="17"/>
-      <c r="M153" s="17" t="s">
+      <c r="I154" s="21"/>
+      <c r="J154" s="22"/>
+      <c r="K154" s="17"/>
+      <c r="L154" s="17"/>
+      <c r="M154" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N153" s="17"/>
-      <c r="O153" s="17"/>
-      <c r="P153" s="17"/>
-      <c r="Q153" s="17"/>
-      <c r="R153" s="17"/>
-      <c r="S153" s="17"/>
-      <c r="T153" s="17"/>
-      <c r="U153" s="17"/>
-      <c r="V153" s="17"/>
-      <c r="W153" s="17"/>
-      <c r="X153" s="17"/>
-      <c r="Y153" s="17"/>
-      <c r="Z153" s="17"/>
-      <c r="AA153" s="21"/>
-      <c r="AB153" s="21"/>
-      <c r="AC153" s="21"/>
-      <c r="AD153" s="21"/>
-      <c r="AE153" s="17"/>
-    </row>
-    <row r="154" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
-      <c r="A154" s="7" t="s">
+      <c r="N154" s="17"/>
+      <c r="O154" s="17"/>
+      <c r="P154" s="17"/>
+      <c r="Q154" s="17"/>
+      <c r="R154" s="17"/>
+      <c r="S154" s="17"/>
+      <c r="T154" s="17"/>
+      <c r="U154" s="17"/>
+      <c r="V154" s="17"/>
+      <c r="W154" s="17"/>
+      <c r="X154" s="17"/>
+      <c r="Y154" s="17"/>
+      <c r="Z154" s="17"/>
+      <c r="AA154" s="21"/>
+      <c r="AB154" s="21"/>
+      <c r="AC154" s="21"/>
+      <c r="AD154" s="21"/>
+      <c r="AE154" s="17"/>
+    </row>
+    <row r="155" spans="1:32" ht="145.5" x14ac:dyDescent="0.25">
+      <c r="A155" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B154" s="7" t="s">
+      <c r="B155" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C154" s="7" t="s">
+      <c r="C155" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D154" s="20" t="s">
+      <c r="D155" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E154" s="20" t="s">
+      <c r="E155" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F154" s="20" t="s">
+      <c r="F155" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G154" s="20" t="s">
+      <c r="G155" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H154" s="20" t="s">
+      <c r="H155" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I154" s="20" t="s">
+      <c r="I155" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J154" s="20" t="s">
+      <c r="J155" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K154" s="20" t="s">
+      <c r="K155" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="L154" s="20" t="s">
+      <c r="L155" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M154" s="19" t="s">
+      <c r="M155" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N154" s="19" t="s">
+      <c r="N155" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="O154" s="19" t="s">
+      <c r="O155" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A155" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B155" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C155" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D155" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E155" s="14">
-        <v>3</v>
-      </c>
-      <c r="F155" s="18">
-        <v>0</v>
-      </c>
-      <c r="G155" s="18">
-        <v>0</v>
-      </c>
-      <c r="H155" s="18">
-        <v>0</v>
-      </c>
-      <c r="I155" s="18">
-        <v>0</v>
-      </c>
-      <c r="J155" s="12">
-        <v>2</v>
-      </c>
-      <c r="K155" s="12">
-        <v>0</v>
-      </c>
-      <c r="L155" s="12">
-        <v>0</v>
-      </c>
-      <c r="M155" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N155" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O155" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P155" s="17"/>
-      <c r="Q155" s="17"/>
     </row>
     <row r="156" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A156" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B156" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C156" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E156" s="14">
         <v>3</v>
@@ -18134,7 +18228,7 @@
         <v>0</v>
       </c>
       <c r="G156" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H156" s="18">
         <v>0</v>
@@ -18168,13 +18262,13 @@
         <v>2</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E157" s="14">
         <v>3</v>
@@ -18183,7 +18277,7 @@
         <v>0</v>
       </c>
       <c r="G157" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H157" s="18">
         <v>0</v>
@@ -18217,13 +18311,13 @@
         <v>2</v>
       </c>
       <c r="B158" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C158" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E158" s="14">
         <v>3</v>
@@ -18232,7 +18326,7 @@
         <v>0</v>
       </c>
       <c r="G158" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H158" s="18">
         <v>0</v>
@@ -18266,13 +18360,13 @@
         <v>2</v>
       </c>
       <c r="B159" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E159" s="14">
         <v>3</v>
@@ -18281,7 +18375,7 @@
         <v>0</v>
       </c>
       <c r="G159" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H159" s="18">
         <v>0</v>
@@ -18315,13 +18409,13 @@
         <v>2</v>
       </c>
       <c r="B160" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C160" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E160" s="14">
         <v>3</v>
@@ -18330,7 +18424,7 @@
         <v>0</v>
       </c>
       <c r="G160" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H160" s="18">
         <v>0</v>
@@ -18364,13 +18458,13 @@
         <v>2</v>
       </c>
       <c r="B161" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C161" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E161" s="14">
         <v>3</v>
@@ -18379,7 +18473,7 @@
         <v>0</v>
       </c>
       <c r="G161" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H161" s="18">
         <v>0</v>
@@ -18413,13 +18507,13 @@
         <v>2</v>
       </c>
       <c r="B162" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E162" s="14">
         <v>3</v>
@@ -18428,7 +18522,7 @@
         <v>0</v>
       </c>
       <c r="G162" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H162" s="18">
         <v>0</v>
@@ -18462,13 +18556,13 @@
         <v>2</v>
       </c>
       <c r="B163" s="15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C163" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E163" s="14">
         <v>3</v>
@@ -18477,7 +18571,7 @@
         <v>0</v>
       </c>
       <c r="G163" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H163" s="18">
         <v>0</v>
@@ -18511,13 +18605,13 @@
         <v>2</v>
       </c>
       <c r="B164" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C164" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E164" s="14">
         <v>3</v>
@@ -18526,7 +18620,7 @@
         <v>0</v>
       </c>
       <c r="G164" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H164" s="18">
         <v>0</v>
@@ -18560,27 +18654,27 @@
         <v>2</v>
       </c>
       <c r="B165" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E165" s="14">
-        <v>1</v>
-      </c>
-      <c r="F165" s="13">
-        <v>0</v>
-      </c>
-      <c r="G165" s="13">
-        <v>1</v>
-      </c>
-      <c r="H165" s="13">
-        <v>0</v>
-      </c>
-      <c r="I165" s="13">
+        <v>3</v>
+      </c>
+      <c r="F165" s="18">
+        <v>0</v>
+      </c>
+      <c r="G165" s="18">
+        <v>2</v>
+      </c>
+      <c r="H165" s="18">
+        <v>0</v>
+      </c>
+      <c r="I165" s="18">
         <v>0</v>
       </c>
       <c r="J165" s="12">
@@ -18601,33 +18695,35 @@
       <c r="O165" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="P165" s="17"/>
+      <c r="Q165" s="17"/>
     </row>
     <row r="166" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A166" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B166" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="C166" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="D166" s="127" t="s">
-        <v>30</v>
+      <c r="B166" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C166" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D166" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="E166" s="14">
         <v>1</v>
       </c>
-      <c r="F166" s="128">
-        <v>0</v>
-      </c>
-      <c r="G166" s="128">
-        <v>0</v>
-      </c>
-      <c r="H166" s="128">
-        <v>0</v>
-      </c>
-      <c r="I166" s="128">
+      <c r="F166" s="13">
+        <v>0</v>
+      </c>
+      <c r="G166" s="13">
+        <v>1</v>
+      </c>
+      <c r="H166" s="13">
+        <v>0</v>
+      </c>
+      <c r="I166" s="13">
         <v>0</v>
       </c>
       <c r="J166" s="12">
@@ -18648,26 +18744,53 @@
       <c r="O166" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P166" s="8"/>
-      <c r="Q166" s="8"/>
-      <c r="R166" s="8"/>
-      <c r="S166" s="8"/>
-      <c r="T166" s="8"/>
-      <c r="U166" s="8"/>
-      <c r="V166" s="8"/>
-      <c r="W166" s="8"/>
-      <c r="X166" s="8"/>
-      <c r="Y166" s="8"/>
-      <c r="Z166" s="8"/>
-      <c r="AA166" s="8"/>
-      <c r="AB166" s="8"/>
-      <c r="AC166" s="8"/>
-      <c r="AD166" s="8"/>
-      <c r="AE166" s="8"/>
     </row>
     <row r="167" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="N167" s="8"/>
-      <c r="O167" s="8"/>
+      <c r="A167" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B167" s="95" t="s">
+        <v>447</v>
+      </c>
+      <c r="C167" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D167" s="127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E167" s="14">
+        <v>1</v>
+      </c>
+      <c r="F167" s="128">
+        <v>0</v>
+      </c>
+      <c r="G167" s="128">
+        <v>0</v>
+      </c>
+      <c r="H167" s="128">
+        <v>0</v>
+      </c>
+      <c r="I167" s="128">
+        <v>0</v>
+      </c>
+      <c r="J167" s="12">
+        <v>2</v>
+      </c>
+      <c r="K167" s="12">
+        <v>0</v>
+      </c>
+      <c r="L167" s="12">
+        <v>0</v>
+      </c>
+      <c r="M167" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N167" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O167" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="P167" s="8"/>
       <c r="Q167" s="8"/>
       <c r="R167" s="8"/>
@@ -18685,73 +18808,67 @@
       <c r="AD167" s="8"/>
       <c r="AE167" s="8"/>
     </row>
-    <row r="168" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="169" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A169" s="9" t="s">
+    <row r="168" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N168" s="8"/>
+      <c r="O168" s="8"/>
+      <c r="P168" s="8"/>
+      <c r="Q168" s="8"/>
+      <c r="R168" s="8"/>
+      <c r="S168" s="8"/>
+      <c r="T168" s="8"/>
+      <c r="U168" s="8"/>
+      <c r="V168" s="8"/>
+      <c r="W168" s="8"/>
+      <c r="X168" s="8"/>
+      <c r="Y168" s="8"/>
+      <c r="Z168" s="8"/>
+      <c r="AA168" s="8"/>
+      <c r="AB168" s="8"/>
+      <c r="AC168" s="8"/>
+      <c r="AD168" s="8"/>
+      <c r="AE168" s="8"/>
+    </row>
+    <row r="169" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A170" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B169" s="9"/>
-      <c r="C169" s="9"/>
-      <c r="D169" s="9"/>
-      <c r="E169" s="8"/>
-      <c r="F169" s="8"/>
-      <c r="G169" s="8"/>
-      <c r="H169" s="8"/>
-      <c r="I169" s="8"/>
-      <c r="J169" s="8"/>
-      <c r="K169" s="8"/>
-      <c r="L169" s="8"/>
-    </row>
-    <row r="171" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
-      <c r="A171" s="7" t="s">
+      <c r="B170" s="9"/>
+      <c r="C170" s="9"/>
+      <c r="D170" s="9"/>
+      <c r="E170" s="8"/>
+      <c r="F170" s="8"/>
+      <c r="G170" s="8"/>
+      <c r="H170" s="8"/>
+      <c r="I170" s="8"/>
+      <c r="J170" s="8"/>
+      <c r="K170" s="8"/>
+      <c r="L170" s="8"/>
+    </row>
+    <row r="172" spans="1:31" ht="159.75" x14ac:dyDescent="0.25">
+      <c r="A172" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B171" s="6" t="s">
+      <c r="B172" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C171" s="6" t="s">
+      <c r="C172" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D171" s="5" t="s">
+      <c r="D172" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E171" s="5" t="s">
+      <c r="E172" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F171" s="5" t="s">
+      <c r="F172" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G171" s="5" t="s">
+      <c r="G172" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H171" s="5" t="s">
+      <c r="H172" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="172" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A172" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D172" s="2">
-        <v>42</v>
-      </c>
-      <c r="E172" s="2">
-        <v>8</v>
-      </c>
-      <c r="F172" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="G172" s="2">
-        <v>2</v>
-      </c>
-      <c r="H172" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:31" x14ac:dyDescent="0.25">
@@ -18759,19 +18876,19 @@
         <v>2</v>
       </c>
       <c r="B173" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D173" s="2">
+        <v>42</v>
+      </c>
+      <c r="E173" s="2">
         <v>8</v>
       </c>
-      <c r="C173" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D173" s="2">
-        <v>92</v>
-      </c>
-      <c r="E173" s="2">
-        <v>10</v>
-      </c>
       <c r="F173" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G173" s="2">
         <v>2</v>
@@ -18785,19 +18902,19 @@
         <v>2</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D174" s="2">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="E174" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F174" s="2">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G174" s="2">
         <v>2</v>
@@ -18811,19 +18928,19 @@
         <v>2</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D175" s="2">
-        <v>686</v>
+        <v>235</v>
       </c>
       <c r="E175" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F175" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G175" s="2">
         <v>2</v>
@@ -18837,104 +18954,130 @@
         <v>2</v>
       </c>
       <c r="